<commit_message>
Data listing with relations implemented
</commit_message>
<xml_diff>
--- a/Helper.xlsx
+++ b/Helper.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2959" uniqueCount="625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3000" uniqueCount="625">
   <si>
     <t>resource_scopes</t>
   </si>
@@ -4007,8 +4007,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R233" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
-  <autoFilter ref="A1:R233">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R245" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
+  <autoFilter ref="A1:R245">
     <filterColumn colId="1">
       <filters>
         <filter val="Resource Relations"/>
@@ -4044,8 +4044,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SeedMap" displayName="SeedMap" ref="A1:E22" totalsRowShown="0" dataDxfId="63">
-  <autoFilter ref="A1:E22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SeedMap" displayName="SeedMap" ref="A1:E24" totalsRowShown="0" dataDxfId="63">
+  <autoFilter ref="A1:E24"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Name" dataDxfId="62"/>
     <tableColumn id="3" name="FW Table Name" dataDxfId="61"/>
@@ -23455,10 +23455,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R233"/>
+  <dimension ref="A1:R245"/>
   <sheetViews>
-    <sheetView topLeftCell="B158" workbookViewId="0">
-      <selection activeCell="B233" sqref="B233"/>
+    <sheetView topLeftCell="B218" workbookViewId="0">
+      <selection activeCell="B246" sqref="B246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -32075,6 +32075,422 @@
       <c r="Q233" s="40"/>
       <c r="R233" s="40"/>
     </row>
+    <row r="234" spans="1:18">
+      <c r="A234" s="22" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Data View Section-0</v>
+      </c>
+      <c r="B234" s="40" t="s">
+        <v>612</v>
+      </c>
+      <c r="C234" s="22">
+        <f>COUNTIF($B$1:$B233,[Table Name])</f>
+        <v>0</v>
+      </c>
+      <c r="D234" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="E234" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="F234" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="G234" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="H234" s="40" t="s">
+        <v>596</v>
+      </c>
+      <c r="I234" s="40"/>
+      <c r="J234" s="40"/>
+      <c r="K234" s="40"/>
+      <c r="L234" s="40"/>
+      <c r="M234" s="40"/>
+      <c r="N234" s="40"/>
+      <c r="O234" s="40"/>
+      <c r="P234" s="40"/>
+      <c r="Q234" s="40"/>
+      <c r="R234" s="40"/>
+    </row>
+    <row r="235" spans="1:18">
+      <c r="A235" s="22" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Data View Section-1</v>
+      </c>
+      <c r="B235" s="40" t="s">
+        <v>612</v>
+      </c>
+      <c r="C235" s="22">
+        <f>COUNTIF($B$1:$B234,[Table Name])</f>
+        <v>1</v>
+      </c>
+      <c r="D235" s="40">
+        <v>1</v>
+      </c>
+      <c r="E235" s="40"/>
+      <c r="F235" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="G235" s="40"/>
+      <c r="H235" s="40">
+        <v>12</v>
+      </c>
+      <c r="I235" s="40"/>
+      <c r="J235" s="40"/>
+      <c r="K235" s="40"/>
+      <c r="L235" s="40"/>
+      <c r="M235" s="40"/>
+      <c r="N235" s="40"/>
+      <c r="O235" s="40"/>
+      <c r="P235" s="40"/>
+      <c r="Q235" s="40"/>
+      <c r="R235" s="40"/>
+    </row>
+    <row r="236" spans="1:18">
+      <c r="A236" s="22" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Data View Section-2</v>
+      </c>
+      <c r="B236" s="40" t="s">
+        <v>612</v>
+      </c>
+      <c r="C236" s="22">
+        <f>COUNTIF($B$1:$B235,[Table Name])</f>
+        <v>2</v>
+      </c>
+      <c r="D236" s="40">
+        <v>2</v>
+      </c>
+      <c r="E236" s="40"/>
+      <c r="F236" s="40"/>
+      <c r="G236" s="40"/>
+      <c r="H236" s="40">
+        <v>4</v>
+      </c>
+      <c r="I236" s="40"/>
+      <c r="J236" s="40"/>
+      <c r="K236" s="40"/>
+      <c r="L236" s="40"/>
+      <c r="M236" s="40"/>
+      <c r="N236" s="40"/>
+      <c r="O236" s="40"/>
+      <c r="P236" s="40"/>
+      <c r="Q236" s="40"/>
+      <c r="R236" s="40"/>
+    </row>
+    <row r="237" spans="1:18">
+      <c r="A237" s="22" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Data View Section-3</v>
+      </c>
+      <c r="B237" s="40" t="s">
+        <v>612</v>
+      </c>
+      <c r="C237" s="22">
+        <f>COUNTIF($B$1:$B236,[Table Name])</f>
+        <v>3</v>
+      </c>
+      <c r="D237" s="40">
+        <v>2</v>
+      </c>
+      <c r="E237" s="40" t="s">
+        <v>180</v>
+      </c>
+      <c r="F237" s="40"/>
+      <c r="G237" s="40">
+        <v>1</v>
+      </c>
+      <c r="H237" s="40">
+        <v>8</v>
+      </c>
+      <c r="I237" s="40"/>
+      <c r="J237" s="40"/>
+      <c r="K237" s="40"/>
+      <c r="L237" s="40"/>
+      <c r="M237" s="40"/>
+      <c r="N237" s="40"/>
+      <c r="O237" s="40"/>
+      <c r="P237" s="40"/>
+      <c r="Q237" s="40"/>
+      <c r="R237" s="40"/>
+    </row>
+    <row r="238" spans="1:18">
+      <c r="A238" s="22" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Data View Section Items-0</v>
+      </c>
+      <c r="B238" s="40" t="s">
+        <v>619</v>
+      </c>
+      <c r="C238" s="22">
+        <f>COUNTIF($B$1:$B237,[Table Name])</f>
+        <v>0</v>
+      </c>
+      <c r="D238" s="40" t="s">
+        <v>607</v>
+      </c>
+      <c r="E238" s="40" t="s">
+        <v>269</v>
+      </c>
+      <c r="F238" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="G238" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="H238" s="40"/>
+      <c r="I238" s="40"/>
+      <c r="J238" s="40"/>
+      <c r="K238" s="40"/>
+      <c r="L238" s="40"/>
+      <c r="M238" s="40"/>
+      <c r="N238" s="40"/>
+      <c r="O238" s="40"/>
+      <c r="P238" s="40"/>
+      <c r="Q238" s="40"/>
+      <c r="R238" s="40"/>
+    </row>
+    <row r="239" spans="1:18">
+      <c r="A239" s="22" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Data View Section Items-1</v>
+      </c>
+      <c r="B239" s="40" t="s">
+        <v>619</v>
+      </c>
+      <c r="C239" s="22">
+        <f>COUNTIF($B$1:$B238,[Table Name])</f>
+        <v>1</v>
+      </c>
+      <c r="D239" s="40">
+        <v>1</v>
+      </c>
+      <c r="E239" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="F239" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="G239" s="40"/>
+      <c r="H239" s="40"/>
+      <c r="I239" s="40"/>
+      <c r="J239" s="40"/>
+      <c r="K239" s="40"/>
+      <c r="L239" s="40"/>
+      <c r="M239" s="40"/>
+      <c r="N239" s="40"/>
+      <c r="O239" s="40"/>
+      <c r="P239" s="40"/>
+      <c r="Q239" s="40"/>
+      <c r="R239" s="40"/>
+    </row>
+    <row r="240" spans="1:18">
+      <c r="A240" s="22" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Data View Section Items-2</v>
+      </c>
+      <c r="B240" s="40" t="s">
+        <v>619</v>
+      </c>
+      <c r="C240" s="22">
+        <f>COUNTIF($B$1:$B239,[Table Name])</f>
+        <v>2</v>
+      </c>
+      <c r="D240" s="40">
+        <v>1</v>
+      </c>
+      <c r="E240" s="40" t="s">
+        <v>272</v>
+      </c>
+      <c r="F240" s="40" t="s">
+        <v>271</v>
+      </c>
+      <c r="G240" s="40"/>
+      <c r="H240" s="40"/>
+      <c r="I240" s="40"/>
+      <c r="J240" s="40"/>
+      <c r="K240" s="40"/>
+      <c r="L240" s="40"/>
+      <c r="M240" s="40"/>
+      <c r="N240" s="40"/>
+      <c r="O240" s="40"/>
+      <c r="P240" s="40"/>
+      <c r="Q240" s="40"/>
+      <c r="R240" s="40"/>
+    </row>
+    <row r="241" spans="1:18">
+      <c r="A241" s="22" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Data View Section Items-3</v>
+      </c>
+      <c r="B241" s="40" t="s">
+        <v>619</v>
+      </c>
+      <c r="C241" s="22">
+        <f>COUNTIF($B$1:$B240,[Table Name])</f>
+        <v>3</v>
+      </c>
+      <c r="D241" s="40">
+        <v>1</v>
+      </c>
+      <c r="E241" s="40" t="s">
+        <v>180</v>
+      </c>
+      <c r="F241" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="G241" s="40">
+        <v>1</v>
+      </c>
+      <c r="H241" s="40"/>
+      <c r="I241" s="40"/>
+      <c r="J241" s="40"/>
+      <c r="K241" s="40"/>
+      <c r="L241" s="40"/>
+      <c r="M241" s="40"/>
+      <c r="N241" s="40"/>
+      <c r="O241" s="40"/>
+      <c r="P241" s="40"/>
+      <c r="Q241" s="40"/>
+      <c r="R241" s="40"/>
+    </row>
+    <row r="242" spans="1:18">
+      <c r="A242" s="22" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Data View Section Items-4</v>
+      </c>
+      <c r="B242" s="40" t="s">
+        <v>619</v>
+      </c>
+      <c r="C242" s="22">
+        <f>COUNTIF($B$1:$B241,[Table Name])</f>
+        <v>4</v>
+      </c>
+      <c r="D242" s="40">
+        <v>2</v>
+      </c>
+      <c r="E242" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="F242" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="G242" s="40"/>
+      <c r="H242" s="40"/>
+      <c r="I242" s="40"/>
+      <c r="J242" s="40"/>
+      <c r="K242" s="40"/>
+      <c r="L242" s="40"/>
+      <c r="M242" s="40"/>
+      <c r="N242" s="40"/>
+      <c r="O242" s="40"/>
+      <c r="P242" s="40"/>
+      <c r="Q242" s="40"/>
+      <c r="R242" s="40"/>
+    </row>
+    <row r="243" spans="1:18">
+      <c r="A243" s="42" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Data View Section Items-5</v>
+      </c>
+      <c r="B243" s="40" t="s">
+        <v>619</v>
+      </c>
+      <c r="C243" s="42">
+        <f>COUNTIF($B$1:$B242,[Table Name])</f>
+        <v>5</v>
+      </c>
+      <c r="D243" s="43">
+        <v>2</v>
+      </c>
+      <c r="E243" s="43" t="s">
+        <v>272</v>
+      </c>
+      <c r="F243" s="43" t="s">
+        <v>271</v>
+      </c>
+      <c r="G243" s="43"/>
+      <c r="H243" s="43"/>
+      <c r="I243" s="43"/>
+      <c r="J243" s="43"/>
+      <c r="K243" s="43"/>
+      <c r="L243" s="43"/>
+      <c r="M243" s="43"/>
+      <c r="N243" s="43"/>
+      <c r="O243" s="43"/>
+      <c r="P243" s="43"/>
+      <c r="Q243" s="43"/>
+      <c r="R243" s="43"/>
+    </row>
+    <row r="244" spans="1:18">
+      <c r="A244" s="22" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Data View Section Items-6</v>
+      </c>
+      <c r="B244" s="40" t="s">
+        <v>619</v>
+      </c>
+      <c r="C244" s="22">
+        <f>COUNTIF($B$1:$B243,[Table Name])</f>
+        <v>6</v>
+      </c>
+      <c r="D244" s="40">
+        <v>3</v>
+      </c>
+      <c r="E244" s="40" t="s">
+        <v>274</v>
+      </c>
+      <c r="F244" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="G244" s="40"/>
+      <c r="H244" s="40"/>
+      <c r="I244" s="40"/>
+      <c r="J244" s="40"/>
+      <c r="K244" s="40"/>
+      <c r="L244" s="40"/>
+      <c r="M244" s="40"/>
+      <c r="N244" s="40"/>
+      <c r="O244" s="40"/>
+      <c r="P244" s="40"/>
+      <c r="Q244" s="40"/>
+      <c r="R244" s="40"/>
+    </row>
+    <row r="245" spans="1:18">
+      <c r="A245" s="22" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Data View Section Items-7</v>
+      </c>
+      <c r="B245" s="40" t="s">
+        <v>619</v>
+      </c>
+      <c r="C245" s="22">
+        <f>COUNTIF($B$1:$B244,[Table Name])</f>
+        <v>7</v>
+      </c>
+      <c r="D245" s="40">
+        <v>3</v>
+      </c>
+      <c r="E245" s="40" t="s">
+        <v>298</v>
+      </c>
+      <c r="F245" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="G245" s="40"/>
+      <c r="H245" s="40"/>
+      <c r="I245" s="40"/>
+      <c r="J245" s="40"/>
+      <c r="K245" s="40"/>
+      <c r="L245" s="40"/>
+      <c r="M245" s="40"/>
+      <c r="N245" s="40"/>
+      <c r="O245" s="40"/>
+      <c r="P245" s="40"/>
+      <c r="Q245" s="40"/>
+      <c r="R245" s="40"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
@@ -32086,10 +32502,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -32540,12 +32956,52 @@
         <v>truncate</v>
       </c>
     </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="4" t="s">
+        <v>612</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>604</v>
+      </c>
+      <c r="C23" s="4" t="str">
+        <f>VLOOKUP([FW Table Name],Tables[],4,0)</f>
+        <v>Milestone\Appframe\Model</v>
+      </c>
+      <c r="D23" s="4" t="str">
+        <f>VLOOKUP([FW Table Name],Tables[],5,0)</f>
+        <v>ResourceDataViewSection</v>
+      </c>
+      <c r="E23" s="7" t="str">
+        <f>"truncate"</f>
+        <v>truncate</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="4" t="s">
+        <v>619</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>605</v>
+      </c>
+      <c r="C24" s="4" t="str">
+        <f>VLOOKUP([FW Table Name],Tables[],4,0)</f>
+        <v>Milestone\Appframe\Model</v>
+      </c>
+      <c r="D24" s="4" t="str">
+        <f>VLOOKUP([FW Table Name],Tables[],5,0)</f>
+        <v>ResourceDataViewSectionItem</v>
+      </c>
+      <c r="E24" s="7" t="str">
+        <f>"truncate"</f>
+        <v>truncate</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E24">
       <formula1>"truncate,query"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B24">
       <formula1>TableNames</formula1>
     </dataValidation>
   </dataValidations>
@@ -34684,8 +35140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:R47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -34695,14 +35151,14 @@
   <sheetData>
     <row r="1" spans="1:20" s="38" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="47" t="s">
-        <v>443</v>
+        <v>619</v>
       </c>
       <c r="B1" s="47"/>
       <c r="C1" s="47"/>
       <c r="D1" s="47"/>
       <c r="E1" s="48" t="str">
         <f>"\"&amp;VLOOKUP($A$1,SeedMap[],3,0)&amp;"\"&amp;VLOOKUP($A$1,SeedMap[],4,0)&amp;"::"&amp;VLOOKUP($A$1,SeedMap[],5,0)&amp;"()"</f>
-        <v>\Milestone\Appframe\Model\ResourceRelation::truncate()</v>
+        <v>\Milestone\Appframe\Model\ResourceDataViewSectionItem::truncate()</v>
       </c>
       <c r="F1" s="48"/>
       <c r="G1" s="48"/>
@@ -34846,27 +35302,27 @@
       <c r="B5" s="28"/>
       <c r="C5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],C$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],C$4+$B$4,0))</f>
-        <v>resource</v>
+        <v>section</v>
       </c>
       <c r="D5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],D$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],D$4+$B$4,0))</f>
-        <v>name</v>
+        <v>label</v>
       </c>
       <c r="E5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0))</f>
-        <v>description</v>
+        <v>attribute</v>
       </c>
       <c r="F5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0))</f>
-        <v>method</v>
+        <v>relation</v>
       </c>
       <c r="G5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0))</f>
-        <v>type</v>
+        <v/>
       </c>
       <c r="H5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],H$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],H$4+$B$4,0))</f>
-        <v>relate_resource</v>
+        <v/>
       </c>
       <c r="I5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],I$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],I$4+$B$4,0))</f>
@@ -34960,7 +35416,7 @@
       <c r="A8" s="32"/>
       <c r="B8" s="46" t="str">
         <f>$E$1</f>
-        <v>\Milestone\Appframe\Model\ResourceRelation::truncate()</v>
+        <v>\Milestone\Appframe\Model\ResourceDataViewSectionItem::truncate()</v>
       </c>
       <c r="C8" s="46"/>
       <c r="D8" s="46"/>
@@ -34989,27 +35445,27 @@
       </c>
       <c r="C9" s="33" t="str">
         <f ca="1">IF(AND($B9=$S$4,C$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),C$4+$B$4,0)="","","'"&amp;C$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),C$4+$B$4,0)&amp;"', "),"")</f>
-        <v xml:space="preserve">'resource' =&gt; '1', </v>
+        <v xml:space="preserve">'section' =&gt; '1', </v>
       </c>
       <c r="D9" s="33" t="str">
         <f t="shared" ref="D9:Q24" ca="1" si="0">IF(AND($B9=$S$4,D$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),D$4+$B$4,0)="","","'"&amp;D$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),D$4+$B$4,0)&amp;"', "),"")</f>
-        <v xml:space="preserve">'name' =&gt; 'User Groups', </v>
+        <v xml:space="preserve">'label' =&gt; 'Name', </v>
       </c>
       <c r="E9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Which groups this user belongs to', </v>
+        <v xml:space="preserve">'attribute' =&gt; 'name', </v>
       </c>
       <c r="F9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Groups', </v>
+        <v/>
       </c>
       <c r="G9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
+        <v/>
       </c>
       <c r="H9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '2', </v>
+        <v/>
       </c>
       <c r="I9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -35062,27 +35518,27 @@
       </c>
       <c r="C10" s="33" t="str">
         <f ca="1">IF(AND($B10=$S$4,C$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A10,INDIRECT($E$2),C$4+$B$4,0)="","","'"&amp;C$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A10,INDIRECT($E$2),C$4+$B$4,0)&amp;"', "),"")</f>
-        <v xml:space="preserve">'resource' =&gt; '2', </v>
+        <v xml:space="preserve">'section' =&gt; '1', </v>
       </c>
       <c r="D10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Group Users', </v>
+        <v xml:space="preserve">'label' =&gt; 'Email', </v>
       </c>
       <c r="E10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'List of users belongs to this group', </v>
+        <v xml:space="preserve">'attribute' =&gt; 'email', </v>
       </c>
       <c r="F10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Users', </v>
+        <v/>
       </c>
       <c r="G10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
+        <v/>
       </c>
       <c r="H10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '1', </v>
+        <v/>
       </c>
       <c r="I10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -35135,27 +35591,27 @@
       </c>
       <c r="C11" s="33" t="str">
         <f t="shared" ref="C11:G74" ca="1" si="3">IF(AND($B11=$S$4,C$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A11,INDIRECT($E$2),C$4+$B$4,0)="","","'"&amp;C$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A11,INDIRECT($E$2),C$4+$B$4,0)&amp;"', "),"")</f>
-        <v xml:space="preserve">'resource' =&gt; '2', </v>
+        <v xml:space="preserve">'section' =&gt; '1', </v>
       </c>
       <c r="D11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Group Roles', </v>
+        <v xml:space="preserve">'label' =&gt; 'Groups', </v>
       </c>
       <c r="E11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Roles assigneed to this group', </v>
+        <v xml:space="preserve">'attribute' =&gt; 'title', </v>
       </c>
       <c r="F11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Roles', </v>
+        <v xml:space="preserve">'relation' =&gt; '1', </v>
       </c>
       <c r="G11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
+        <v/>
       </c>
       <c r="H11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '3', </v>
+        <v/>
       </c>
       <c r="I11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -35208,27 +35664,27 @@
       </c>
       <c r="C12" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '3', </v>
+        <v xml:space="preserve">'section' =&gt; '2', </v>
       </c>
       <c r="D12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Role Groups', </v>
+        <v xml:space="preserve">'label' =&gt; 'Name', </v>
       </c>
       <c r="E12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Details of groups this role assigned to', </v>
+        <v xml:space="preserve">'attribute' =&gt; 'name', </v>
       </c>
       <c r="F12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Groups', </v>
+        <v/>
       </c>
       <c r="G12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
+        <v/>
       </c>
       <c r="H12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '2', </v>
+        <v/>
       </c>
       <c r="I12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -35281,27 +35737,27 @@
       </c>
       <c r="C13" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '3', </v>
+        <v xml:space="preserve">'section' =&gt; '2', </v>
       </c>
       <c r="D13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Role Resource', </v>
+        <v xml:space="preserve">'label' =&gt; 'Email', </v>
       </c>
       <c r="E13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Resources assigned to a role', </v>
+        <v xml:space="preserve">'attribute' =&gt; 'email', </v>
       </c>
       <c r="F13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Resources', </v>
+        <v/>
       </c>
       <c r="G13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '11', </v>
+        <v/>
       </c>
       <c r="I13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -35354,27 +35810,27 @@
       </c>
       <c r="C14" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '4', </v>
+        <v xml:space="preserve">'section' =&gt; '3', </v>
       </c>
       <c r="D14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Resource Roles', </v>
+        <v xml:space="preserve">'label' =&gt; 'Group', </v>
       </c>
       <c r="E14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'The details of roles who have access to this resource', </v>
+        <v xml:space="preserve">'attribute' =&gt; 'title', </v>
       </c>
       <c r="F14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Roles', </v>
+        <v/>
       </c>
       <c r="G14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
+        <v/>
       </c>
       <c r="H14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '3', </v>
+        <v/>
       </c>
       <c r="I14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -35427,27 +35883,27 @@
       </c>
       <c r="C15" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '4', </v>
+        <v xml:space="preserve">'section' =&gt; '3', </v>
       </c>
       <c r="D15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Resource Actions', </v>
+        <v xml:space="preserve">'label' =&gt; 'Description', </v>
       </c>
       <c r="E15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Get actions available for the resource', </v>
+        <v xml:space="preserve">'attribute' =&gt; 'description', </v>
       </c>
       <c r="F15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Actions', </v>
+        <v/>
       </c>
       <c r="G15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '7', </v>
+        <v/>
       </c>
       <c r="I15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -35496,31 +35952,31 @@
       </c>
       <c r="B16" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v>;</v>
       </c>
       <c r="C16" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '7', </v>
+        <v/>
       </c>
       <c r="D16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Resource Action Methods', </v>
+        <v/>
       </c>
       <c r="E16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Handler details of an action', </v>
+        <v/>
       </c>
       <c r="F16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Method', </v>
+        <v/>
       </c>
       <c r="G16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'hasOne', </v>
+        <v/>
       </c>
       <c r="H16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '8', </v>
+        <v/>
       </c>
       <c r="I16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -35560,7 +36016,7 @@
       </c>
       <c r="R16" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="17" spans="1:18">
@@ -35569,31 +36025,31 @@
       </c>
       <c r="B17" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
       </c>
       <c r="C17" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '7', </v>
+        <v/>
       </c>
       <c r="D17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Resource Action Lists', </v>
+        <v/>
       </c>
       <c r="E17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Lists where action available', </v>
+        <v/>
       </c>
       <c r="F17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Lists', </v>
+        <v/>
       </c>
       <c r="G17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '9', </v>
+        <v/>
       </c>
       <c r="I17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -35633,7 +36089,7 @@
       </c>
       <c r="R17" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="18" spans="1:18">
@@ -35642,31 +36098,31 @@
       </c>
       <c r="B18" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C18" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '7', </v>
+        <v/>
       </c>
       <c r="D18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Resource Action Data', </v>
+        <v/>
       </c>
       <c r="E18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Resource data where action available', </v>
+        <v/>
       </c>
       <c r="F18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Data', </v>
+        <v/>
       </c>
       <c r="G18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '10', </v>
+        <v/>
       </c>
       <c r="I18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -35706,7 +36162,7 @@
       </c>
       <c r="R18" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="19" spans="1:18">
@@ -35715,31 +36171,31 @@
       </c>
       <c r="B19" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C19" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '5', </v>
+        <v/>
       </c>
       <c r="D19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Organisation Contacts', </v>
+        <v/>
       </c>
       <c r="E19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Contact details of organisation', </v>
+        <v/>
       </c>
       <c r="F19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Contacts', </v>
+        <v/>
       </c>
       <c r="G19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '6', </v>
+        <v/>
       </c>
       <c r="I19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -35779,7 +36235,7 @@
       </c>
       <c r="R19" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="20" spans="1:18">
@@ -35788,31 +36244,31 @@
       </c>
       <c r="B20" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C20" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '11', </v>
+        <v/>
       </c>
       <c r="D20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Resource Details', </v>
+        <v/>
       </c>
       <c r="E20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Resource details', </v>
+        <v/>
       </c>
       <c r="F20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Resource', </v>
+        <v/>
       </c>
       <c r="G20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
+        <v/>
       </c>
       <c r="H20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
+        <v/>
       </c>
       <c r="I20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -35852,7 +36308,7 @@
       </c>
       <c r="R20" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="21" spans="1:18">
@@ -35861,31 +36317,31 @@
       </c>
       <c r="B21" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C21" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '4', </v>
+        <v/>
       </c>
       <c r="D21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Resource Forms', </v>
+        <v/>
       </c>
       <c r="E21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Forms available for a resource', </v>
+        <v/>
       </c>
       <c r="F21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Forms', </v>
+        <v/>
       </c>
       <c r="G21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '12', </v>
+        <v/>
       </c>
       <c r="I21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -35925,7 +36381,7 @@
       </c>
       <c r="R21" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="22" spans="1:18">
@@ -35934,31 +36390,31 @@
       </c>
       <c r="B22" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C22" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '12', </v>
+        <v/>
       </c>
       <c r="D22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Form Fields', </v>
+        <v/>
       </c>
       <c r="E22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Fields associated with a form', </v>
+        <v/>
       </c>
       <c r="F22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Fields', </v>
+        <v/>
       </c>
       <c r="G22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '13', </v>
+        <v/>
       </c>
       <c r="I22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -35998,7 +36454,7 @@
       </c>
       <c r="R22" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="23" spans="1:18">
@@ -36007,31 +36463,31 @@
       </c>
       <c r="B23" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C23" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '13', </v>
+        <v/>
       </c>
       <c r="D23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Field Attributes', </v>
+        <v/>
       </c>
       <c r="E23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Attributes of Field', </v>
+        <v/>
       </c>
       <c r="F23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Attributes', </v>
+        <v/>
       </c>
       <c r="G23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '14', </v>
+        <v/>
       </c>
       <c r="I23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -36071,7 +36527,7 @@
       </c>
       <c r="R23" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="24" spans="1:18">
@@ -36080,31 +36536,31 @@
       </c>
       <c r="B24" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C24" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '13', </v>
+        <v/>
       </c>
       <c r="D24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Field Options', </v>
+        <v/>
       </c>
       <c r="E24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Options of Field', </v>
+        <v/>
       </c>
       <c r="F24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Options', </v>
+        <v/>
       </c>
       <c r="G24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'hasOne', </v>
+        <v/>
       </c>
       <c r="H24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '15', </v>
+        <v/>
       </c>
       <c r="I24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -36144,7 +36600,7 @@
       </c>
       <c r="R24" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="25" spans="1:18">
@@ -36153,31 +36609,31 @@
       </c>
       <c r="B25" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '13', </v>
+        <v/>
       </c>
       <c r="D25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Field Validations', </v>
+        <v/>
       </c>
       <c r="E25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Validation details of field', </v>
+        <v/>
       </c>
       <c r="F25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Validations', </v>
+        <v/>
       </c>
       <c r="G25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H25" s="33" t="str">
         <f t="shared" ref="H25:K88" ca="1" si="4">IF(AND($B25=$S$4,H$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A25,INDIRECT($E$2),H$4+$B$4,0)="","","'"&amp;H$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A25,INDIRECT($E$2),H$4+$B$4,0)&amp;"', "),"")</f>
-        <v xml:space="preserve">'relate_resource' =&gt; '16', </v>
+        <v/>
       </c>
       <c r="I25" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -36217,7 +36673,7 @@
       </c>
       <c r="R25" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="26" spans="1:18">
@@ -36226,31 +36682,31 @@
       </c>
       <c r="B26" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '12', </v>
+        <v/>
       </c>
       <c r="D26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'From Resource', </v>
+        <v/>
       </c>
       <c r="E26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Resource this form belongs to', </v>
+        <v/>
       </c>
       <c r="F26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Resource', </v>
+        <v/>
       </c>
       <c r="G26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
+        <v/>
       </c>
       <c r="H26" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
+        <v/>
       </c>
       <c r="I26" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -36290,7 +36746,7 @@
       </c>
       <c r="R26" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="27" spans="1:18">
@@ -36299,31 +36755,31 @@
       </c>
       <c r="B27" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '12', </v>
+        <v/>
       </c>
       <c r="D27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Form Defaults', </v>
+        <v/>
       </c>
       <c r="E27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Predefined values for a form', </v>
+        <v/>
       </c>
       <c r="F27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Defaults', </v>
+        <v/>
       </c>
       <c r="G27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H27" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '17', </v>
+        <v/>
       </c>
       <c r="I27" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -36363,7 +36819,7 @@
       </c>
       <c r="R27" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="28" spans="1:18">
@@ -36372,31 +36828,31 @@
       </c>
       <c r="B28" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '13', </v>
+        <v/>
       </c>
       <c r="D28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Field Data', </v>
+        <v/>
       </c>
       <c r="E28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Fields Database binding details', </v>
+        <v/>
       </c>
       <c r="F28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Data', </v>
+        <v/>
       </c>
       <c r="G28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasOne', </v>
+        <v/>
       </c>
       <c r="H28" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '18', </v>
+        <v/>
       </c>
       <c r="I28" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -36436,7 +36892,7 @@
       </c>
       <c r="R28" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="29" spans="1:18">
@@ -36445,31 +36901,31 @@
       </c>
       <c r="B29" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '4', </v>
+        <v/>
       </c>
       <c r="D29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Resource Relations', </v>
+        <v/>
       </c>
       <c r="E29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Relation of  a resource to another resource', </v>
+        <v/>
       </c>
       <c r="F29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Relations', </v>
+        <v/>
       </c>
       <c r="G29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H29" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
+        <v/>
       </c>
       <c r="I29" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -36509,7 +36965,7 @@
       </c>
       <c r="R29" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="30" spans="1:18">
@@ -36518,31 +36974,31 @@
       </c>
       <c r="B30" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '18', </v>
+        <v/>
       </c>
       <c r="D30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Bind Data Resource', </v>
+        <v/>
       </c>
       <c r="E30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Resource to which the data to be bind', </v>
+        <v/>
       </c>
       <c r="F30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
+        <v/>
       </c>
       <c r="G30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
+        <v/>
       </c>
       <c r="H30" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
+        <v/>
       </c>
       <c r="I30" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -36582,7 +37038,7 @@
       </c>
       <c r="R30" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="31" spans="1:18">
@@ -36591,31 +37047,31 @@
       </c>
       <c r="B31" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '17', </v>
+        <v/>
       </c>
       <c r="D31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Default Data Resource', </v>
+        <v/>
       </c>
       <c r="E31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Resource to which the forms predefined data to be bind', </v>
+        <v/>
       </c>
       <c r="F31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
+        <v/>
       </c>
       <c r="G31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
+        <v/>
       </c>
       <c r="H31" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
+        <v/>
       </c>
       <c r="I31" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -36655,7 +37111,7 @@
       </c>
       <c r="R31" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="32" spans="1:18">
@@ -36664,31 +37120,31 @@
       </c>
       <c r="B32" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '19', </v>
+        <v/>
       </c>
       <c r="D32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Resource Details', </v>
+        <v/>
       </c>
       <c r="E32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Resource details of a list', </v>
+        <v/>
       </c>
       <c r="F32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Resource', </v>
+        <v/>
       </c>
       <c r="G32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
+        <v/>
       </c>
       <c r="H32" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
+        <v/>
       </c>
       <c r="I32" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -36728,7 +37184,7 @@
       </c>
       <c r="R32" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="33" spans="1:18">
@@ -36737,31 +37193,31 @@
       </c>
       <c r="B33" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '19', </v>
+        <v/>
       </c>
       <c r="D33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'List Relations', </v>
+        <v/>
       </c>
       <c r="E33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Relations to be loaded on accessing list', </v>
+        <v/>
       </c>
       <c r="F33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Relations', </v>
+        <v/>
       </c>
       <c r="G33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H33" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '20', </v>
+        <v/>
       </c>
       <c r="I33" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -36801,7 +37257,7 @@
       </c>
       <c r="R33" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="34" spans="1:18">
@@ -36810,31 +37266,31 @@
       </c>
       <c r="B34" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '4', </v>
+        <v/>
       </c>
       <c r="D34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Resource Scopes', </v>
+        <v/>
       </c>
       <c r="E34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Scopes available on a Resource', </v>
+        <v/>
       </c>
       <c r="F34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Scopes', </v>
+        <v/>
       </c>
       <c r="G34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H34" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '21', </v>
+        <v/>
       </c>
       <c r="I34" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -36874,7 +37330,7 @@
       </c>
       <c r="R34" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="35" spans="1:18">
@@ -36883,31 +37339,31 @@
       </c>
       <c r="B35" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '19', </v>
+        <v/>
       </c>
       <c r="D35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'List Scopes', </v>
+        <v/>
       </c>
       <c r="E35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Scopes by which a list to be filtered', </v>
+        <v/>
       </c>
       <c r="F35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Scopes', </v>
+        <v/>
       </c>
       <c r="G35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
+        <v/>
       </c>
       <c r="H35" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '21', </v>
+        <v/>
       </c>
       <c r="I35" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -36947,7 +37403,7 @@
       </c>
       <c r="R35" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="36" spans="1:18">
@@ -36956,31 +37412,31 @@
       </c>
       <c r="B36" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '23', </v>
+        <v/>
       </c>
       <c r="D36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Data Relation', </v>
+        <v/>
       </c>
       <c r="E36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Relations to be loaded on a data view', </v>
+        <v/>
       </c>
       <c r="F36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Relations', </v>
+        <v/>
       </c>
       <c r="G36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H36" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '24', </v>
+        <v/>
       </c>
       <c r="I36" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -37020,7 +37476,7 @@
       </c>
       <c r="R36" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="37" spans="1:18">
@@ -37029,31 +37485,31 @@
       </c>
       <c r="B37" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '23', </v>
+        <v/>
       </c>
       <c r="D37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Resource Details', </v>
+        <v/>
       </c>
       <c r="E37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Details of resource of a record', </v>
+        <v/>
       </c>
       <c r="F37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Resource', </v>
+        <v/>
       </c>
       <c r="G37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
+        <v/>
       </c>
       <c r="H37" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
+        <v/>
       </c>
       <c r="I37" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -37093,7 +37549,7 @@
       </c>
       <c r="R37" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="38" spans="1:18">
@@ -37102,31 +37558,31 @@
       </c>
       <c r="B38" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '19', </v>
+        <v/>
       </c>
       <c r="D38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'List Layout', </v>
+        <v/>
       </c>
       <c r="E38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Layout of a list', </v>
+        <v/>
       </c>
       <c r="F38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Layout', </v>
+        <v/>
       </c>
       <c r="G38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H38" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '25', </v>
+        <v/>
       </c>
       <c r="I38" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -37166,7 +37622,7 @@
       </c>
       <c r="R38" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="39" spans="1:18">
@@ -37175,31 +37631,31 @@
       </c>
       <c r="B39" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C39" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '26', </v>
+        <v/>
       </c>
       <c r="D39" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Nested Relation', </v>
+        <v/>
       </c>
       <c r="E39" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Nested Relation', </v>
+        <v/>
       </c>
       <c r="F39" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Nest', </v>
+        <v/>
       </c>
       <c r="G39" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H39" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
+        <v/>
       </c>
       <c r="I39" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -37239,7 +37695,7 @@
       </c>
       <c r="R39" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="40" spans="1:18">
@@ -37248,31 +37704,31 @@
       </c>
       <c r="B40" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C40" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '26', </v>
+        <v/>
       </c>
       <c r="D40" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Related Resource', </v>
+        <v/>
       </c>
       <c r="E40" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Related Resource Details', </v>
+        <v/>
       </c>
       <c r="F40" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
+        <v/>
       </c>
       <c r="G40" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
+        <v/>
       </c>
       <c r="H40" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
+        <v/>
       </c>
       <c r="I40" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -37312,7 +37768,7 @@
       </c>
       <c r="R40" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="41" spans="1:18">
@@ -37321,31 +37777,31 @@
       </c>
       <c r="B41" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C41" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '26', </v>
+        <v/>
       </c>
       <c r="D41" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Form Layout', </v>
+        <v/>
       </c>
       <c r="E41" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Layout details', </v>
+        <v/>
       </c>
       <c r="F41" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Layout', </v>
+        <v/>
       </c>
       <c r="G41" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H41" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '27', </v>
+        <v/>
       </c>
       <c r="I41" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -37385,7 +37841,7 @@
       </c>
       <c r="R41" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="42" spans="1:18">
@@ -37394,31 +37850,31 @@
       </c>
       <c r="B42" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C42" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '23', </v>
+        <v/>
       </c>
       <c r="D42" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Data View Section', </v>
+        <v/>
       </c>
       <c r="E42" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Section details of data view', </v>
+        <v/>
       </c>
       <c r="F42" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Sections', </v>
+        <v/>
       </c>
       <c r="G42" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H42" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '28', </v>
+        <v/>
       </c>
       <c r="I42" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -37458,7 +37914,7 @@
       </c>
       <c r="R42" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="43" spans="1:18">
@@ -37467,31 +37923,31 @@
       </c>
       <c r="B43" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C43" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '26', </v>
+        <v/>
       </c>
       <c r="D43" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Data View Section Items', </v>
+        <v/>
       </c>
       <c r="E43" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Items of a data view section', </v>
+        <v/>
       </c>
       <c r="F43" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Items', </v>
+        <v/>
       </c>
       <c r="G43" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H43" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '29', </v>
+        <v/>
       </c>
       <c r="I43" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -37531,7 +37987,7 @@
       </c>
       <c r="R43" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="44" spans="1:18">
@@ -37540,31 +37996,31 @@
       </c>
       <c r="B44" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C44" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '28', </v>
+        <v/>
       </c>
       <c r="D44" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Data Relation', </v>
+        <v/>
       </c>
       <c r="E44" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'View relation of a data', </v>
+        <v/>
       </c>
       <c r="F44" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
+        <v/>
       </c>
       <c r="G44" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
+        <v/>
       </c>
       <c r="H44" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
+        <v/>
       </c>
       <c r="I44" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -37604,7 +38060,7 @@
       </c>
       <c r="R44" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="45" spans="1:18">
@@ -37613,31 +38069,31 @@
       </c>
       <c r="B45" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C45" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '29', </v>
+        <v/>
       </c>
       <c r="D45" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Data item relation', </v>
+        <v/>
       </c>
       <c r="E45" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'View relation of a data item', </v>
+        <v/>
       </c>
       <c r="F45" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
+        <v/>
       </c>
       <c r="G45" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
+        <v/>
       </c>
       <c r="H45" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
+        <v/>
       </c>
       <c r="I45" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -37677,7 +38133,7 @@
       </c>
       <c r="R45" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="46" spans="1:18">
@@ -37686,7 +38142,7 @@
       </c>
       <c r="B46" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>;</v>
+        <v/>
       </c>
       <c r="C46" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -37759,7 +38215,7 @@
       </c>
       <c r="B47" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
+        <v/>
       </c>
       <c r="C47" s="33" t="str">
         <f t="shared" ca="1" si="3"/>

</xml_diff>

<commit_message>
Assets compiled for Production and Excel updated
</commit_message>
<xml_diff>
--- a/Helper.xlsx
+++ b/Helper.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Tables" sheetId="1" r:id="rId1"/>
@@ -4066,12 +4066,7 @@
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R270" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
   <autoFilter ref="A1:R270">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Resource Action Data"/>
-        <filter val="Resource Actions"/>
-      </filters>
-    </filterColumn>
+    <filterColumn colId="1"/>
   </autoFilter>
   <tableColumns count="18">
     <tableColumn id="19" name="TRCode" dataDxfId="81">
@@ -23515,8 +23510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R270"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B271" sqref="B271"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -23583,7 +23578,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="2" spans="1:18" hidden="1">
+    <row r="2" spans="1:18">
       <c r="A2" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Groups-0</v>
@@ -23617,7 +23612,7 @@
       <c r="Q2" s="15"/>
       <c r="R2" s="15"/>
     </row>
-    <row r="3" spans="1:18" hidden="1">
+    <row r="3" spans="1:18">
       <c r="A3" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Groups-1</v>
@@ -23651,7 +23646,7 @@
       <c r="Q3" s="16"/>
       <c r="R3" s="16"/>
     </row>
-    <row r="4" spans="1:18" hidden="1">
+    <row r="4" spans="1:18">
       <c r="A4" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Groups-2</v>
@@ -23685,7 +23680,7 @@
       <c r="Q4" s="16"/>
       <c r="R4" s="16"/>
     </row>
-    <row r="5" spans="1:18" hidden="1">
+    <row r="5" spans="1:18">
       <c r="A5" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Groups-3</v>
@@ -23719,7 +23714,7 @@
       <c r="Q5" s="16"/>
       <c r="R5" s="16"/>
     </row>
-    <row r="6" spans="1:18" hidden="1">
+    <row r="6" spans="1:18">
       <c r="A6" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Roles-0</v>
@@ -23753,7 +23748,7 @@
       <c r="Q6" s="16"/>
       <c r="R6" s="16"/>
     </row>
-    <row r="7" spans="1:18" hidden="1">
+    <row r="7" spans="1:18">
       <c r="A7" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Roles-1</v>
@@ -23787,7 +23782,7 @@
       <c r="Q7" s="16"/>
       <c r="R7" s="16"/>
     </row>
-    <row r="8" spans="1:18" hidden="1">
+    <row r="8" spans="1:18">
       <c r="A8" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Roles-2</v>
@@ -23821,7 +23816,7 @@
       <c r="Q8" s="16"/>
       <c r="R8" s="16"/>
     </row>
-    <row r="9" spans="1:18" hidden="1">
+    <row r="9" spans="1:18">
       <c r="A9" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Roles-3</v>
@@ -23855,7 +23850,7 @@
       <c r="Q9" s="16"/>
       <c r="R9" s="16"/>
     </row>
-    <row r="10" spans="1:18" hidden="1">
+    <row r="10" spans="1:18">
       <c r="A10" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Group Roles-0</v>
@@ -23887,7 +23882,7 @@
       <c r="Q10" s="16"/>
       <c r="R10" s="16"/>
     </row>
-    <row r="11" spans="1:18" hidden="1">
+    <row r="11" spans="1:18">
       <c r="A11" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Group Roles-1</v>
@@ -23919,7 +23914,7 @@
       <c r="Q11" s="16"/>
       <c r="R11" s="16"/>
     </row>
-    <row r="12" spans="1:18" hidden="1">
+    <row r="12" spans="1:18">
       <c r="A12" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Group Roles-2</v>
@@ -23951,7 +23946,7 @@
       <c r="Q12" s="16"/>
       <c r="R12" s="16"/>
     </row>
-    <row r="13" spans="1:18" hidden="1">
+    <row r="13" spans="1:18">
       <c r="A13" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Group Roles-3</v>
@@ -23983,7 +23978,7 @@
       <c r="Q13" s="16"/>
       <c r="R13" s="16"/>
     </row>
-    <row r="14" spans="1:18" hidden="1">
+    <row r="14" spans="1:18">
       <c r="A14" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-0</v>
@@ -24027,7 +24022,7 @@
       <c r="Q14" s="16"/>
       <c r="R14" s="16"/>
     </row>
-    <row r="15" spans="1:18" hidden="1">
+    <row r="15" spans="1:18">
       <c r="A15" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-1</v>
@@ -24067,7 +24062,7 @@
       <c r="Q15" s="15"/>
       <c r="R15" s="15"/>
     </row>
-    <row r="16" spans="1:18" hidden="1">
+    <row r="16" spans="1:18">
       <c r="A16" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-2</v>
@@ -24107,7 +24102,7 @@
       <c r="Q16" s="15"/>
       <c r="R16" s="15"/>
     </row>
-    <row r="17" spans="1:18" hidden="1">
+    <row r="17" spans="1:18">
       <c r="A17" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-3</v>
@@ -24147,7 +24142,7 @@
       <c r="Q17" s="15"/>
       <c r="R17" s="15"/>
     </row>
-    <row r="18" spans="1:18" hidden="1">
+    <row r="18" spans="1:18">
       <c r="A18" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-4</v>
@@ -24187,7 +24182,7 @@
       <c r="Q18" s="15"/>
       <c r="R18" s="15"/>
     </row>
-    <row r="19" spans="1:18" hidden="1">
+    <row r="19" spans="1:18">
       <c r="A19" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-5</v>
@@ -24227,7 +24222,7 @@
       <c r="Q19" s="15"/>
       <c r="R19" s="15"/>
     </row>
-    <row r="20" spans="1:18" hidden="1">
+    <row r="20" spans="1:18">
       <c r="A20" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-6</v>
@@ -24267,7 +24262,7 @@
       <c r="Q20" s="15"/>
       <c r="R20" s="15"/>
     </row>
-    <row r="21" spans="1:18" hidden="1">
+    <row r="21" spans="1:18">
       <c r="A21" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-7</v>
@@ -24307,7 +24302,7 @@
       <c r="Q21" s="15"/>
       <c r="R21" s="15"/>
     </row>
-    <row r="22" spans="1:18" hidden="1">
+    <row r="22" spans="1:18">
       <c r="A22" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-8</v>
@@ -24347,7 +24342,7 @@
       <c r="Q22" s="15"/>
       <c r="R22" s="15"/>
     </row>
-    <row r="23" spans="1:18" hidden="1">
+    <row r="23" spans="1:18">
       <c r="A23" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-9</v>
@@ -24387,7 +24382,7 @@
       <c r="Q23" s="15"/>
       <c r="R23" s="15"/>
     </row>
-    <row r="24" spans="1:18" hidden="1">
+    <row r="24" spans="1:18">
       <c r="A24" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-10</v>
@@ -24427,7 +24422,7 @@
       <c r="Q24" s="15"/>
       <c r="R24" s="15"/>
     </row>
-    <row r="25" spans="1:18" hidden="1">
+    <row r="25" spans="1:18">
       <c r="A25" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-11</v>
@@ -24467,7 +24462,7 @@
       <c r="Q25" s="15"/>
       <c r="R25" s="15"/>
     </row>
-    <row r="26" spans="1:18" hidden="1">
+    <row r="26" spans="1:18">
       <c r="A26" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-12</v>
@@ -24507,7 +24502,7 @@
       <c r="Q26" s="15"/>
       <c r="R26" s="15"/>
     </row>
-    <row r="27" spans="1:18" hidden="1">
+    <row r="27" spans="1:18">
       <c r="A27" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-13</v>
@@ -24547,7 +24542,7 @@
       <c r="Q27" s="16"/>
       <c r="R27" s="16"/>
     </row>
-    <row r="28" spans="1:18" hidden="1">
+    <row r="28" spans="1:18">
       <c r="A28" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Roles-0</v>
@@ -24583,7 +24578,7 @@
       <c r="Q28" s="16"/>
       <c r="R28" s="16"/>
     </row>
-    <row r="29" spans="1:18" hidden="1">
+    <row r="29" spans="1:18">
       <c r="A29" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Roles-1</v>
@@ -24619,7 +24614,7 @@
       <c r="Q29" s="16"/>
       <c r="R29" s="16"/>
     </row>
-    <row r="30" spans="1:18" hidden="1">
+    <row r="30" spans="1:18">
       <c r="A30" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Roles-2</v>
@@ -24651,7 +24646,7 @@
       <c r="Q30" s="16"/>
       <c r="R30" s="16"/>
     </row>
-    <row r="31" spans="1:18" hidden="1">
+    <row r="31" spans="1:18">
       <c r="A31" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Roles-3</v>
@@ -24683,7 +24678,7 @@
       <c r="Q31" s="16"/>
       <c r="R31" s="16"/>
     </row>
-    <row r="32" spans="1:18" hidden="1">
+    <row r="32" spans="1:18">
       <c r="A32" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Roles-4</v>
@@ -24715,7 +24710,7 @@
       <c r="Q32" s="16"/>
       <c r="R32" s="16"/>
     </row>
-    <row r="33" spans="1:18" hidden="1">
+    <row r="33" spans="1:18">
       <c r="A33" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Roles-5</v>
@@ -24747,7 +24742,7 @@
       <c r="Q33" s="16"/>
       <c r="R33" s="16"/>
     </row>
-    <row r="34" spans="1:18" hidden="1">
+    <row r="34" spans="1:18">
       <c r="A34" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Roles-6</v>
@@ -24779,7 +24774,7 @@
       <c r="Q34" s="16"/>
       <c r="R34" s="16"/>
     </row>
-    <row r="35" spans="1:18" hidden="1">
+    <row r="35" spans="1:18">
       <c r="A35" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Roles-7</v>
@@ -24811,7 +24806,7 @@
       <c r="Q35" s="16"/>
       <c r="R35" s="16"/>
     </row>
-    <row r="36" spans="1:18" hidden="1">
+    <row r="36" spans="1:18">
       <c r="A36" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-0</v>
@@ -24851,7 +24846,7 @@
       <c r="Q36" s="16"/>
       <c r="R36" s="16"/>
     </row>
-    <row r="37" spans="1:18" hidden="1">
+    <row r="37" spans="1:18">
       <c r="A37" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-1</v>
@@ -24891,7 +24886,7 @@
       <c r="Q37" s="15"/>
       <c r="R37" s="15"/>
     </row>
-    <row r="38" spans="1:18" hidden="1">
+    <row r="38" spans="1:18">
       <c r="A38" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-2</v>
@@ -24931,7 +24926,7 @@
       <c r="Q38" s="15"/>
       <c r="R38" s="15"/>
     </row>
-    <row r="39" spans="1:18" hidden="1">
+    <row r="39" spans="1:18">
       <c r="A39" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-3</v>
@@ -24971,7 +24966,7 @@
       <c r="Q39" s="15"/>
       <c r="R39" s="15"/>
     </row>
-    <row r="40" spans="1:18" hidden="1">
+    <row r="40" spans="1:18">
       <c r="A40" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-4</v>
@@ -25011,7 +25006,7 @@
       <c r="Q40" s="15"/>
       <c r="R40" s="15"/>
     </row>
-    <row r="41" spans="1:18" hidden="1">
+    <row r="41" spans="1:18">
       <c r="A41" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-5</v>
@@ -25051,7 +25046,7 @@
       <c r="Q41" s="15"/>
       <c r="R41" s="15"/>
     </row>
-    <row r="42" spans="1:18" hidden="1">
+    <row r="42" spans="1:18">
       <c r="A42" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-6</v>
@@ -25091,7 +25086,7 @@
       <c r="Q42" s="15"/>
       <c r="R42" s="15"/>
     </row>
-    <row r="43" spans="1:18" hidden="1">
+    <row r="43" spans="1:18">
       <c r="A43" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-7</v>
@@ -25131,7 +25126,7 @@
       <c r="Q43" s="15"/>
       <c r="R43" s="15"/>
     </row>
-    <row r="44" spans="1:18" hidden="1">
+    <row r="44" spans="1:18">
       <c r="A44" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-8</v>
@@ -25171,7 +25166,7 @@
       <c r="Q44" s="15"/>
       <c r="R44" s="15"/>
     </row>
-    <row r="45" spans="1:18" hidden="1">
+    <row r="45" spans="1:18">
       <c r="A45" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-9</v>
@@ -25211,7 +25206,7 @@
       <c r="Q45" s="15"/>
       <c r="R45" s="15"/>
     </row>
-    <row r="46" spans="1:18" hidden="1">
+    <row r="46" spans="1:18">
       <c r="A46" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-10</v>
@@ -25251,7 +25246,7 @@
       <c r="Q46" s="15"/>
       <c r="R46" s="15"/>
     </row>
-    <row r="47" spans="1:18" hidden="1">
+    <row r="47" spans="1:18">
       <c r="A47" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-11</v>
@@ -25291,7 +25286,7 @@
       <c r="Q47" s="15"/>
       <c r="R47" s="15"/>
     </row>
-    <row r="48" spans="1:18" hidden="1">
+    <row r="48" spans="1:18">
       <c r="A48" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-12</v>
@@ -25331,7 +25326,7 @@
       <c r="Q48" s="15"/>
       <c r="R48" s="15"/>
     </row>
-    <row r="49" spans="1:18" hidden="1">
+    <row r="49" spans="1:18">
       <c r="A49" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-13</v>
@@ -25371,7 +25366,7 @@
       <c r="Q49" s="15"/>
       <c r="R49" s="15"/>
     </row>
-    <row r="50" spans="1:18" hidden="1">
+    <row r="50" spans="1:18">
       <c r="A50" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-14</v>
@@ -25411,7 +25406,7 @@
       <c r="Q50" s="16"/>
       <c r="R50" s="16"/>
     </row>
-    <row r="51" spans="1:18" hidden="1">
+    <row r="51" spans="1:18">
       <c r="A51" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Scopes-0</v>
@@ -25447,7 +25442,7 @@
       <c r="Q51" s="16"/>
       <c r="R51" s="16"/>
     </row>
-    <row r="52" spans="1:18" hidden="1">
+    <row r="52" spans="1:18">
       <c r="A52" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Scopes-1</v>
@@ -25483,7 +25478,7 @@
       <c r="Q52" s="15"/>
       <c r="R52" s="15"/>
     </row>
-    <row r="53" spans="1:18" hidden="1">
+    <row r="53" spans="1:18">
       <c r="A53" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Scopes-2</v>
@@ -25519,7 +25514,7 @@
       <c r="Q53" s="16"/>
       <c r="R53" s="16"/>
     </row>
-    <row r="54" spans="1:18" hidden="1">
+    <row r="54" spans="1:18">
       <c r="A54" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Lists-0</v>
@@ -25555,7 +25550,7 @@
       <c r="Q54" s="16"/>
       <c r="R54" s="16"/>
     </row>
-    <row r="55" spans="1:18" hidden="1">
+    <row r="55" spans="1:18">
       <c r="A55" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Lists-1</v>
@@ -25591,7 +25586,7 @@
       <c r="Q55" s="15"/>
       <c r="R55" s="15"/>
     </row>
-    <row r="56" spans="1:18" hidden="1">
+    <row r="56" spans="1:18">
       <c r="A56" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Lists-2</v>
@@ -25627,7 +25622,7 @@
       <c r="Q56" s="15"/>
       <c r="R56" s="15"/>
     </row>
-    <row r="57" spans="1:18" hidden="1">
+    <row r="57" spans="1:18">
       <c r="A57" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Lists-3</v>
@@ -25663,7 +25658,7 @@
       <c r="Q57" s="15"/>
       <c r="R57" s="15"/>
     </row>
-    <row r="58" spans="1:18" hidden="1">
+    <row r="58" spans="1:18">
       <c r="A58" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Lists-4</v>
@@ -25699,7 +25694,7 @@
       <c r="Q58" s="15"/>
       <c r="R58" s="15"/>
     </row>
-    <row r="59" spans="1:18" hidden="1">
+    <row r="59" spans="1:18">
       <c r="A59" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Lists-5</v>
@@ -25735,7 +25730,7 @@
       <c r="Q59" s="15"/>
       <c r="R59" s="15"/>
     </row>
-    <row r="60" spans="1:18" hidden="1">
+    <row r="60" spans="1:18">
       <c r="A60" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Lists-6</v>
@@ -25771,7 +25766,7 @@
       <c r="Q60" s="16"/>
       <c r="R60" s="16"/>
     </row>
-    <row r="61" spans="1:18" hidden="1">
+    <row r="61" spans="1:18">
       <c r="A61" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource List Scopes-0</v>
@@ -25803,7 +25798,7 @@
       <c r="Q61" s="16"/>
       <c r="R61" s="16"/>
     </row>
-    <row r="62" spans="1:18" hidden="1">
+    <row r="62" spans="1:18">
       <c r="A62" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource List Scopes-1</v>
@@ -25835,7 +25830,7 @@
       <c r="Q62" s="15"/>
       <c r="R62" s="15"/>
     </row>
-    <row r="63" spans="1:18" hidden="1">
+    <row r="63" spans="1:18">
       <c r="A63" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource List Scopes-2</v>
@@ -25867,7 +25862,7 @@
       <c r="Q63" s="16"/>
       <c r="R63" s="16"/>
     </row>
-    <row r="64" spans="1:18" hidden="1">
+    <row r="64" spans="1:18">
       <c r="A64" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Forms-0</v>
@@ -25905,7 +25900,7 @@
       <c r="Q64" s="16"/>
       <c r="R64" s="16"/>
     </row>
-    <row r="65" spans="1:18" hidden="1">
+    <row r="65" spans="1:18">
       <c r="A65" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Forms-1</v>
@@ -25943,7 +25938,7 @@
       <c r="Q65" s="15"/>
       <c r="R65" s="15"/>
     </row>
-    <row r="66" spans="1:18" hidden="1">
+    <row r="66" spans="1:18">
       <c r="A66" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Forms-2</v>
@@ -25981,7 +25976,7 @@
       <c r="Q66" s="15"/>
       <c r="R66" s="15"/>
     </row>
-    <row r="67" spans="1:18" hidden="1">
+    <row r="67" spans="1:18">
       <c r="A67" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Forms-3</v>
@@ -26019,7 +26014,7 @@
       <c r="Q67" s="15"/>
       <c r="R67" s="15"/>
     </row>
-    <row r="68" spans="1:18" hidden="1">
+    <row r="68" spans="1:18">
       <c r="A68" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Forms-4</v>
@@ -26057,7 +26052,7 @@
       <c r="Q68" s="15"/>
       <c r="R68" s="15"/>
     </row>
-    <row r="69" spans="1:18" hidden="1">
+    <row r="69" spans="1:18">
       <c r="A69" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Forms-5</v>
@@ -26095,7 +26090,7 @@
       <c r="Q69" s="15"/>
       <c r="R69" s="15"/>
     </row>
-    <row r="70" spans="1:18" hidden="1">
+    <row r="70" spans="1:18">
       <c r="A70" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Forms-6</v>
@@ -26133,7 +26128,7 @@
       <c r="Q70" s="15"/>
       <c r="R70" s="15"/>
     </row>
-    <row r="71" spans="1:18" hidden="1">
+    <row r="71" spans="1:18">
       <c r="A71" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Forms-7</v>
@@ -26171,7 +26166,7 @@
       <c r="Q71" s="16"/>
       <c r="R71" s="16"/>
     </row>
-    <row r="72" spans="1:18" hidden="1">
+    <row r="72" spans="1:18">
       <c r="A72" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-0</v>
@@ -26209,7 +26204,7 @@
       <c r="Q72" s="16"/>
       <c r="R72" s="16"/>
     </row>
-    <row r="73" spans="1:18" hidden="1">
+    <row r="73" spans="1:18">
       <c r="A73" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-1</v>
@@ -26247,7 +26242,7 @@
       <c r="Q73" s="15"/>
       <c r="R73" s="15"/>
     </row>
-    <row r="74" spans="1:18" hidden="1">
+    <row r="74" spans="1:18">
       <c r="A74" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-2</v>
@@ -26285,7 +26280,7 @@
       <c r="Q74" s="15"/>
       <c r="R74" s="15"/>
     </row>
-    <row r="75" spans="1:18" hidden="1">
+    <row r="75" spans="1:18">
       <c r="A75" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-3</v>
@@ -26323,7 +26318,7 @@
       <c r="Q75" s="15"/>
       <c r="R75" s="15"/>
     </row>
-    <row r="76" spans="1:18" hidden="1">
+    <row r="76" spans="1:18">
       <c r="A76" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-4</v>
@@ -26361,7 +26356,7 @@
       <c r="Q76" s="15"/>
       <c r="R76" s="15"/>
     </row>
-    <row r="77" spans="1:18" hidden="1">
+    <row r="77" spans="1:18">
       <c r="A77" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-5</v>
@@ -26399,7 +26394,7 @@
       <c r="Q77" s="15"/>
       <c r="R77" s="15"/>
     </row>
-    <row r="78" spans="1:18" hidden="1">
+    <row r="78" spans="1:18">
       <c r="A78" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-6</v>
@@ -26437,7 +26432,7 @@
       <c r="Q78" s="15"/>
       <c r="R78" s="15"/>
     </row>
-    <row r="79" spans="1:18" hidden="1">
+    <row r="79" spans="1:18">
       <c r="A79" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-7</v>
@@ -26475,7 +26470,7 @@
       <c r="Q79" s="15"/>
       <c r="R79" s="15"/>
     </row>
-    <row r="80" spans="1:18" hidden="1">
+    <row r="80" spans="1:18">
       <c r="A80" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-8</v>
@@ -26513,7 +26508,7 @@
       <c r="Q80" s="15"/>
       <c r="R80" s="15"/>
     </row>
-    <row r="81" spans="1:18" hidden="1">
+    <row r="81" spans="1:18">
       <c r="A81" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-9</v>
@@ -26551,7 +26546,7 @@
       <c r="Q81" s="15"/>
       <c r="R81" s="15"/>
     </row>
-    <row r="82" spans="1:18" hidden="1">
+    <row r="82" spans="1:18">
       <c r="A82" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-10</v>
@@ -26589,7 +26584,7 @@
       <c r="Q82" s="15"/>
       <c r="R82" s="15"/>
     </row>
-    <row r="83" spans="1:18" hidden="1">
+    <row r="83" spans="1:18">
       <c r="A83" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-11</v>
@@ -26627,7 +26622,7 @@
       <c r="Q83" s="15"/>
       <c r="R83" s="15"/>
     </row>
-    <row r="84" spans="1:18" hidden="1">
+    <row r="84" spans="1:18">
       <c r="A84" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-12</v>
@@ -26665,7 +26660,7 @@
       <c r="Q84" s="15"/>
       <c r="R84" s="15"/>
     </row>
-    <row r="85" spans="1:18" hidden="1">
+    <row r="85" spans="1:18">
       <c r="A85" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-13</v>
@@ -26703,7 +26698,7 @@
       <c r="Q85" s="15"/>
       <c r="R85" s="15"/>
     </row>
-    <row r="86" spans="1:18" hidden="1">
+    <row r="86" spans="1:18">
       <c r="A86" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-14</v>
@@ -26741,7 +26736,7 @@
       <c r="Q86" s="15"/>
       <c r="R86" s="15"/>
     </row>
-    <row r="87" spans="1:18" hidden="1">
+    <row r="87" spans="1:18">
       <c r="A87" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-15</v>
@@ -26779,7 +26774,7 @@
       <c r="Q87" s="15"/>
       <c r="R87" s="15"/>
     </row>
-    <row r="88" spans="1:18" hidden="1">
+    <row r="88" spans="1:18">
       <c r="A88" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-16</v>
@@ -26817,7 +26812,7 @@
       <c r="Q88" s="15"/>
       <c r="R88" s="15"/>
     </row>
-    <row r="89" spans="1:18" hidden="1">
+    <row r="89" spans="1:18">
       <c r="A89" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-17</v>
@@ -26855,7 +26850,7 @@
       <c r="Q89" s="15"/>
       <c r="R89" s="15"/>
     </row>
-    <row r="90" spans="1:18" hidden="1">
+    <row r="90" spans="1:18">
       <c r="A90" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-18</v>
@@ -26893,7 +26888,7 @@
       <c r="Q90" s="15"/>
       <c r="R90" s="15"/>
     </row>
-    <row r="91" spans="1:18" hidden="1">
+    <row r="91" spans="1:18">
       <c r="A91" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-19</v>
@@ -26931,7 +26926,7 @@
       <c r="Q91" s="15"/>
       <c r="R91" s="15"/>
     </row>
-    <row r="92" spans="1:18" hidden="1">
+    <row r="92" spans="1:18">
       <c r="A92" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-20</v>
@@ -26969,7 +26964,7 @@
       <c r="Q92" s="15"/>
       <c r="R92" s="15"/>
     </row>
-    <row r="93" spans="1:18" hidden="1">
+    <row r="93" spans="1:18">
       <c r="A93" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-21</v>
@@ -27007,7 +27002,7 @@
       <c r="Q93" s="15"/>
       <c r="R93" s="15"/>
     </row>
-    <row r="94" spans="1:18" hidden="1">
+    <row r="94" spans="1:18">
       <c r="A94" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-22</v>
@@ -27045,7 +27040,7 @@
       <c r="Q94" s="15"/>
       <c r="R94" s="15"/>
     </row>
-    <row r="95" spans="1:18" hidden="1">
+    <row r="95" spans="1:18">
       <c r="A95" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-23</v>
@@ -27083,7 +27078,7 @@
       <c r="Q95" s="15"/>
       <c r="R95" s="15"/>
     </row>
-    <row r="96" spans="1:18" hidden="1">
+    <row r="96" spans="1:18">
       <c r="A96" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-24</v>
@@ -27121,7 +27116,7 @@
       <c r="Q96" s="15"/>
       <c r="R96" s="15"/>
     </row>
-    <row r="97" spans="1:18" hidden="1">
+    <row r="97" spans="1:18">
       <c r="A97" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-25</v>
@@ -27159,7 +27154,7 @@
       <c r="Q97" s="15"/>
       <c r="R97" s="15"/>
     </row>
-    <row r="98" spans="1:18" hidden="1">
+    <row r="98" spans="1:18">
       <c r="A98" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-26</v>
@@ -27197,7 +27192,7 @@
       <c r="Q98" s="15"/>
       <c r="R98" s="15"/>
     </row>
-    <row r="99" spans="1:18" hidden="1">
+    <row r="99" spans="1:18">
       <c r="A99" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-27</v>
@@ -27235,7 +27230,7 @@
       <c r="Q99" s="15"/>
       <c r="R99" s="15"/>
     </row>
-    <row r="100" spans="1:18" hidden="1">
+    <row r="100" spans="1:18">
       <c r="A100" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-28</v>
@@ -27273,7 +27268,7 @@
       <c r="Q100" s="15"/>
       <c r="R100" s="15"/>
     </row>
-    <row r="101" spans="1:18" hidden="1">
+    <row r="101" spans="1:18">
       <c r="A101" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-29</v>
@@ -27311,7 +27306,7 @@
       <c r="Q101" s="15"/>
       <c r="R101" s="15"/>
     </row>
-    <row r="102" spans="1:18" hidden="1">
+    <row r="102" spans="1:18">
       <c r="A102" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-30</v>
@@ -27349,7 +27344,7 @@
       <c r="Q102" s="15"/>
       <c r="R102" s="15"/>
     </row>
-    <row r="103" spans="1:18" hidden="1">
+    <row r="103" spans="1:18">
       <c r="A103" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-31</v>
@@ -27387,7 +27382,7 @@
       <c r="Q103" s="16"/>
       <c r="R103" s="16"/>
     </row>
-    <row r="104" spans="1:18" hidden="1">
+    <row r="104" spans="1:18">
       <c r="A104" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-0</v>
@@ -27427,7 +27422,7 @@
       <c r="Q104" s="16"/>
       <c r="R104" s="16"/>
     </row>
-    <row r="105" spans="1:18" hidden="1">
+    <row r="105" spans="1:18">
       <c r="A105" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-1</v>
@@ -27459,7 +27454,7 @@
       <c r="Q105" s="16"/>
       <c r="R105" s="16"/>
     </row>
-    <row r="106" spans="1:18" hidden="1">
+    <row r="106" spans="1:18">
       <c r="A106" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-2</v>
@@ -27491,7 +27486,7 @@
       <c r="Q106" s="16"/>
       <c r="R106" s="16"/>
     </row>
-    <row r="107" spans="1:18" hidden="1">
+    <row r="107" spans="1:18">
       <c r="A107" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-3</v>
@@ -27523,7 +27518,7 @@
       <c r="Q107" s="16"/>
       <c r="R107" s="16"/>
     </row>
-    <row r="108" spans="1:18" hidden="1">
+    <row r="108" spans="1:18">
       <c r="A108" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-4</v>
@@ -27555,7 +27550,7 @@
       <c r="Q108" s="16"/>
       <c r="R108" s="16"/>
     </row>
-    <row r="109" spans="1:18" hidden="1">
+    <row r="109" spans="1:18">
       <c r="A109" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-5</v>
@@ -27587,7 +27582,7 @@
       <c r="Q109" s="16"/>
       <c r="R109" s="16"/>
     </row>
-    <row r="110" spans="1:18" hidden="1">
+    <row r="110" spans="1:18">
       <c r="A110" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-6</v>
@@ -27619,7 +27614,7 @@
       <c r="Q110" s="16"/>
       <c r="R110" s="16"/>
     </row>
-    <row r="111" spans="1:18" hidden="1">
+    <row r="111" spans="1:18">
       <c r="A111" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-7</v>
@@ -27651,7 +27646,7 @@
       <c r="Q111" s="16"/>
       <c r="R111" s="16"/>
     </row>
-    <row r="112" spans="1:18" hidden="1">
+    <row r="112" spans="1:18">
       <c r="A112" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-8</v>
@@ -27683,7 +27678,7 @@
       <c r="Q112" s="16"/>
       <c r="R112" s="16"/>
     </row>
-    <row r="113" spans="1:18" hidden="1">
+    <row r="113" spans="1:18">
       <c r="A113" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-9</v>
@@ -27715,7 +27710,7 @@
       <c r="Q113" s="16"/>
       <c r="R113" s="16"/>
     </row>
-    <row r="114" spans="1:18" hidden="1">
+    <row r="114" spans="1:18">
       <c r="A114" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-10</v>
@@ -27747,7 +27742,7 @@
       <c r="Q114" s="16"/>
       <c r="R114" s="16"/>
     </row>
-    <row r="115" spans="1:18" hidden="1">
+    <row r="115" spans="1:18">
       <c r="A115" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-11</v>
@@ -27779,7 +27774,7 @@
       <c r="Q115" s="16"/>
       <c r="R115" s="16"/>
     </row>
-    <row r="116" spans="1:18" hidden="1">
+    <row r="116" spans="1:18">
       <c r="A116" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-12</v>
@@ -27811,7 +27806,7 @@
       <c r="Q116" s="16"/>
       <c r="R116" s="16"/>
     </row>
-    <row r="117" spans="1:18" hidden="1">
+    <row r="117" spans="1:18">
       <c r="A117" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-13</v>
@@ -27843,7 +27838,7 @@
       <c r="Q117" s="16"/>
       <c r="R117" s="16"/>
     </row>
-    <row r="118" spans="1:18" hidden="1">
+    <row r="118" spans="1:18">
       <c r="A118" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-14</v>
@@ -27875,7 +27870,7 @@
       <c r="Q118" s="16"/>
       <c r="R118" s="16"/>
     </row>
-    <row r="119" spans="1:18" hidden="1">
+    <row r="119" spans="1:18">
       <c r="A119" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-15</v>
@@ -27907,7 +27902,7 @@
       <c r="Q119" s="16"/>
       <c r="R119" s="16"/>
     </row>
-    <row r="120" spans="1:18" hidden="1">
+    <row r="120" spans="1:18">
       <c r="A120" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-16</v>
@@ -27939,7 +27934,7 @@
       <c r="Q120" s="16"/>
       <c r="R120" s="16"/>
     </row>
-    <row r="121" spans="1:18" hidden="1">
+    <row r="121" spans="1:18">
       <c r="A121" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-17</v>
@@ -27971,7 +27966,7 @@
       <c r="Q121" s="16"/>
       <c r="R121" s="16"/>
     </row>
-    <row r="122" spans="1:18" hidden="1">
+    <row r="122" spans="1:18">
       <c r="A122" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-18</v>
@@ -28003,7 +27998,7 @@
       <c r="Q122" s="16"/>
       <c r="R122" s="16"/>
     </row>
-    <row r="123" spans="1:18" hidden="1">
+    <row r="123" spans="1:18">
       <c r="A123" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-19</v>
@@ -28035,7 +28030,7 @@
       <c r="Q123" s="16"/>
       <c r="R123" s="16"/>
     </row>
-    <row r="124" spans="1:18" hidden="1">
+    <row r="124" spans="1:18">
       <c r="A124" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-20</v>
@@ -28067,7 +28062,7 @@
       <c r="Q124" s="16"/>
       <c r="R124" s="16"/>
     </row>
-    <row r="125" spans="1:18" hidden="1">
+    <row r="125" spans="1:18">
       <c r="A125" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-21</v>
@@ -28099,7 +28094,7 @@
       <c r="Q125" s="16"/>
       <c r="R125" s="16"/>
     </row>
-    <row r="126" spans="1:18" hidden="1">
+    <row r="126" spans="1:18">
       <c r="A126" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-22</v>
@@ -28131,7 +28126,7 @@
       <c r="Q126" s="16"/>
       <c r="R126" s="16"/>
     </row>
-    <row r="127" spans="1:18" hidden="1">
+    <row r="127" spans="1:18">
       <c r="A127" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-23</v>
@@ -28163,7 +28158,7 @@
       <c r="Q127" s="16"/>
       <c r="R127" s="16"/>
     </row>
-    <row r="128" spans="1:18" hidden="1">
+    <row r="128" spans="1:18">
       <c r="A128" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-24</v>
@@ -28195,7 +28190,7 @@
       <c r="Q128" s="16"/>
       <c r="R128" s="16"/>
     </row>
-    <row r="129" spans="1:18" hidden="1">
+    <row r="129" spans="1:18">
       <c r="A129" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-25</v>
@@ -28227,7 +28222,7 @@
       <c r="Q129" s="16"/>
       <c r="R129" s="16"/>
     </row>
-    <row r="130" spans="1:18" hidden="1">
+    <row r="130" spans="1:18">
       <c r="A130" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-26</v>
@@ -28259,7 +28254,7 @@
       <c r="Q130" s="16"/>
       <c r="R130" s="16"/>
     </row>
-    <row r="131" spans="1:18" hidden="1">
+    <row r="131" spans="1:18">
       <c r="A131" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-27</v>
@@ -28291,7 +28286,7 @@
       <c r="Q131" s="16"/>
       <c r="R131" s="16"/>
     </row>
-    <row r="132" spans="1:18" hidden="1">
+    <row r="132" spans="1:18">
       <c r="A132" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-28</v>
@@ -28323,7 +28318,7 @@
       <c r="Q132" s="16"/>
       <c r="R132" s="16"/>
     </row>
-    <row r="133" spans="1:18" hidden="1">
+    <row r="133" spans="1:18">
       <c r="A133" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-29</v>
@@ -28357,7 +28352,7 @@
       <c r="Q133" s="16"/>
       <c r="R133" s="16"/>
     </row>
-    <row r="134" spans="1:18" hidden="1">
+    <row r="134" spans="1:18">
       <c r="A134" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-30</v>
@@ -28391,7 +28386,7 @@
       <c r="Q134" s="16"/>
       <c r="R134" s="16"/>
     </row>
-    <row r="135" spans="1:18" hidden="1">
+    <row r="135" spans="1:18">
       <c r="A135" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-31</v>
@@ -28733,7 +28728,7 @@
       <c r="Q142" s="16"/>
       <c r="R142" s="16"/>
     </row>
-    <row r="143" spans="1:18" hidden="1">
+    <row r="143" spans="1:18">
       <c r="A143" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Method-0</v>
@@ -28777,7 +28772,7 @@
       <c r="Q143" s="16"/>
       <c r="R143" s="16"/>
     </row>
-    <row r="144" spans="1:18" hidden="1">
+    <row r="144" spans="1:18">
       <c r="A144" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Method-1</v>
@@ -28811,7 +28806,7 @@
       <c r="Q144" s="15"/>
       <c r="R144" s="15"/>
     </row>
-    <row r="145" spans="1:18" hidden="1">
+    <row r="145" spans="1:18">
       <c r="A145" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Method-2</v>
@@ -28845,7 +28840,7 @@
       <c r="Q145" s="15"/>
       <c r="R145" s="15"/>
     </row>
-    <row r="146" spans="1:18" hidden="1">
+    <row r="146" spans="1:18">
       <c r="A146" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Method-3</v>
@@ -28879,7 +28874,7 @@
       <c r="Q146" s="15"/>
       <c r="R146" s="15"/>
     </row>
-    <row r="147" spans="1:18" hidden="1">
+    <row r="147" spans="1:18">
       <c r="A147" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Method-4</v>
@@ -28913,7 +28908,7 @@
       <c r="Q147" s="15"/>
       <c r="R147" s="15"/>
     </row>
-    <row r="148" spans="1:18" hidden="1">
+    <row r="148" spans="1:18">
       <c r="A148" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Method-5</v>
@@ -28947,7 +28942,7 @@
       <c r="Q148" s="15"/>
       <c r="R148" s="15"/>
     </row>
-    <row r="149" spans="1:18" hidden="1">
+    <row r="149" spans="1:18">
       <c r="A149" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Method-6</v>
@@ -28981,7 +28976,7 @@
       <c r="Q149" s="16"/>
       <c r="R149" s="16"/>
     </row>
-    <row r="150" spans="1:18" hidden="1">
+    <row r="150" spans="1:18">
       <c r="A150" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Attrs-0</v>
@@ -29015,7 +29010,7 @@
       <c r="Q150" s="40"/>
       <c r="R150" s="40"/>
     </row>
-    <row r="151" spans="1:18" hidden="1">
+    <row r="151" spans="1:18">
       <c r="A151" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-14</v>
@@ -29055,7 +29050,7 @@
       <c r="Q151" s="40"/>
       <c r="R151" s="40"/>
     </row>
-    <row r="152" spans="1:18" hidden="1">
+    <row r="152" spans="1:18">
       <c r="A152" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-15</v>
@@ -29095,7 +29090,7 @@
       <c r="Q152" s="40"/>
       <c r="R152" s="40"/>
     </row>
-    <row r="153" spans="1:18" hidden="1">
+    <row r="153" spans="1:18">
       <c r="A153" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-15</v>
@@ -29135,7 +29130,7 @@
       <c r="Q153" s="40"/>
       <c r="R153" s="40"/>
     </row>
-    <row r="154" spans="1:18" hidden="1">
+    <row r="154" spans="1:18">
       <c r="A154" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-16</v>
@@ -29175,7 +29170,7 @@
       <c r="Q154" s="40"/>
       <c r="R154" s="40"/>
     </row>
-    <row r="155" spans="1:18" hidden="1">
+    <row r="155" spans="1:18">
       <c r="A155" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-16</v>
@@ -29215,7 +29210,7 @@
       <c r="Q155" s="40"/>
       <c r="R155" s="40"/>
     </row>
-    <row r="156" spans="1:18" hidden="1">
+    <row r="156" spans="1:18">
       <c r="A156" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-17</v>
@@ -29255,7 +29250,7 @@
       <c r="Q156" s="40"/>
       <c r="R156" s="40"/>
     </row>
-    <row r="157" spans="1:18" hidden="1">
+    <row r="157" spans="1:18">
       <c r="A157" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-0</v>
@@ -29299,7 +29294,7 @@
       <c r="Q157" s="40"/>
       <c r="R157" s="40"/>
     </row>
-    <row r="158" spans="1:18" hidden="1">
+    <row r="158" spans="1:18">
       <c r="A158" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-1</v>
@@ -29333,7 +29328,7 @@
       <c r="Q158" s="40"/>
       <c r="R158" s="40"/>
     </row>
-    <row r="159" spans="1:18" hidden="1">
+    <row r="159" spans="1:18">
       <c r="A159" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-2</v>
@@ -29367,7 +29362,7 @@
       <c r="Q159" s="40"/>
       <c r="R159" s="40"/>
     </row>
-    <row r="160" spans="1:18" hidden="1">
+    <row r="160" spans="1:18">
       <c r="A160" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-3</v>
@@ -29401,7 +29396,7 @@
       <c r="Q160" s="40"/>
       <c r="R160" s="40"/>
     </row>
-    <row r="161" spans="1:18" hidden="1">
+    <row r="161" spans="1:18">
       <c r="A161" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-4</v>
@@ -29439,7 +29434,7 @@
       <c r="Q161" s="40"/>
       <c r="R161" s="40"/>
     </row>
-    <row r="162" spans="1:18" hidden="1">
+    <row r="162" spans="1:18">
       <c r="A162" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-5</v>
@@ -29473,7 +29468,7 @@
       <c r="Q162" s="40"/>
       <c r="R162" s="40"/>
     </row>
-    <row r="163" spans="1:18" hidden="1">
+    <row r="163" spans="1:18">
       <c r="A163" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-6</v>
@@ -29507,7 +29502,7 @@
       <c r="Q163" s="40"/>
       <c r="R163" s="40"/>
     </row>
-    <row r="164" spans="1:18" hidden="1">
+    <row r="164" spans="1:18">
       <c r="A164" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-7</v>
@@ -29541,7 +29536,7 @@
       <c r="Q164" s="40"/>
       <c r="R164" s="40"/>
     </row>
-    <row r="165" spans="1:18" hidden="1">
+    <row r="165" spans="1:18">
       <c r="A165" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-8</v>
@@ -29579,7 +29574,7 @@
       <c r="Q165" s="40"/>
       <c r="R165" s="40"/>
     </row>
-    <row r="166" spans="1:18" hidden="1">
+    <row r="166" spans="1:18">
       <c r="A166" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-18</v>
@@ -29619,7 +29614,7 @@
       <c r="Q166" s="40"/>
       <c r="R166" s="40"/>
     </row>
-    <row r="167" spans="1:18" hidden="1">
+    <row r="167" spans="1:18">
       <c r="A167" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-17</v>
@@ -29659,7 +29654,7 @@
       <c r="Q167" s="40"/>
       <c r="R167" s="40"/>
     </row>
-    <row r="168" spans="1:18" hidden="1">
+    <row r="168" spans="1:18">
       <c r="A168" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-19</v>
@@ -29699,7 +29694,7 @@
       <c r="Q168" s="40"/>
       <c r="R168" s="40"/>
     </row>
-    <row r="169" spans="1:18" hidden="1">
+    <row r="169" spans="1:18">
       <c r="A169" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Defaults-0</v>
@@ -29745,7 +29740,7 @@
       <c r="Q169" s="40"/>
       <c r="R169" s="40"/>
     </row>
-    <row r="170" spans="1:18" hidden="1">
+    <row r="170" spans="1:18">
       <c r="A170" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Defaults-1</v>
@@ -29781,7 +29776,7 @@
       <c r="Q170" s="40"/>
       <c r="R170" s="40"/>
     </row>
-    <row r="171" spans="1:18" hidden="1">
+    <row r="171" spans="1:18">
       <c r="A171" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Defaults-2</v>
@@ -29817,7 +29812,7 @@
       <c r="Q171" s="40"/>
       <c r="R171" s="40"/>
     </row>
-    <row r="172" spans="1:18" hidden="1">
+    <row r="172" spans="1:18">
       <c r="A172" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-18</v>
@@ -29857,7 +29852,7 @@
       <c r="Q172" s="40"/>
       <c r="R172" s="40"/>
     </row>
-    <row r="173" spans="1:18" hidden="1">
+    <row r="173" spans="1:18">
       <c r="A173" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-20</v>
@@ -29897,7 +29892,7 @@
       <c r="Q173" s="40"/>
       <c r="R173" s="40"/>
     </row>
-    <row r="174" spans="1:18" hidden="1">
+    <row r="174" spans="1:18">
       <c r="A174" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-21</v>
@@ -29937,7 +29932,7 @@
       <c r="Q174" s="40"/>
       <c r="R174" s="40"/>
     </row>
-    <row r="175" spans="1:18" hidden="1">
+    <row r="175" spans="1:18">
       <c r="A175" s="42" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-22</v>
@@ -29977,7 +29972,7 @@
       <c r="Q175" s="43"/>
       <c r="R175" s="43"/>
     </row>
-    <row r="176" spans="1:18" hidden="1">
+    <row r="176" spans="1:18">
       <c r="A176" s="42" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-23</v>
@@ -30017,7 +30012,7 @@
       <c r="Q176" s="43"/>
       <c r="R176" s="43"/>
     </row>
-    <row r="177" spans="1:18" hidden="1">
+    <row r="177" spans="1:18">
       <c r="A177" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-32</v>
@@ -30053,7 +30048,7 @@
       <c r="Q177" s="40"/>
       <c r="R177" s="40"/>
     </row>
-    <row r="178" spans="1:18" hidden="1">
+    <row r="178" spans="1:18">
       <c r="A178" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-33</v>
@@ -30089,7 +30084,7 @@
       <c r="Q178" s="40"/>
       <c r="R178" s="40"/>
     </row>
-    <row r="179" spans="1:18" hidden="1">
+    <row r="179" spans="1:18">
       <c r="A179" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-32</v>
@@ -30121,7 +30116,7 @@
       <c r="Q179" s="40"/>
       <c r="R179" s="40"/>
     </row>
-    <row r="180" spans="1:18" hidden="1">
+    <row r="180" spans="1:18">
       <c r="A180" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-33</v>
@@ -30153,7 +30148,7 @@
       <c r="Q180" s="40"/>
       <c r="R180" s="40"/>
     </row>
-    <row r="181" spans="1:18" hidden="1">
+    <row r="181" spans="1:18">
       <c r="A181" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-9</v>
@@ -30187,7 +30182,7 @@
       <c r="Q181" s="40"/>
       <c r="R181" s="40"/>
     </row>
-    <row r="182" spans="1:18" hidden="1">
+    <row r="182" spans="1:18">
       <c r="A182" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-10</v>
@@ -30223,7 +30218,7 @@
       <c r="Q182" s="40"/>
       <c r="R182" s="40"/>
     </row>
-    <row r="183" spans="1:18" hidden="1">
+    <row r="183" spans="1:18">
       <c r="A183" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-11</v>
@@ -30257,7 +30252,7 @@
       <c r="Q183" s="40"/>
       <c r="R183" s="40"/>
     </row>
-    <row r="184" spans="1:18" hidden="1">
+    <row r="184" spans="1:18">
       <c r="A184" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-12</v>
@@ -30293,7 +30288,7 @@
       <c r="Q184" s="40"/>
       <c r="R184" s="40"/>
     </row>
-    <row r="185" spans="1:18" hidden="1">
+    <row r="185" spans="1:18">
       <c r="A185" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-19</v>
@@ -30333,7 +30328,7 @@
       <c r="Q185" s="40"/>
       <c r="R185" s="40"/>
     </row>
-    <row r="186" spans="1:18" hidden="1">
+    <row r="186" spans="1:18">
       <c r="A186" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-24</v>
@@ -30373,7 +30368,7 @@
       <c r="Q186" s="40"/>
       <c r="R186" s="40"/>
     </row>
-    <row r="187" spans="1:18" hidden="1">
+    <row r="187" spans="1:18">
       <c r="A187" s="42" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-20</v>
@@ -30413,7 +30408,7 @@
       <c r="Q187" s="43"/>
       <c r="R187" s="43"/>
     </row>
-    <row r="188" spans="1:18" hidden="1">
+    <row r="188" spans="1:18">
       <c r="A188" s="42" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-21</v>
@@ -30453,7 +30448,7 @@
       <c r="Q188" s="43"/>
       <c r="R188" s="43"/>
     </row>
-    <row r="189" spans="1:18" hidden="1">
+    <row r="189" spans="1:18">
       <c r="A189" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-22</v>
@@ -30493,7 +30488,7 @@
       <c r="Q189" s="40"/>
       <c r="R189" s="40"/>
     </row>
-    <row r="190" spans="1:18" hidden="1">
+    <row r="190" spans="1:18">
       <c r="A190" s="42" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-25</v>
@@ -30533,7 +30528,7 @@
       <c r="Q190" s="43"/>
       <c r="R190" s="43"/>
     </row>
-    <row r="191" spans="1:18" hidden="1">
+    <row r="191" spans="1:18">
       <c r="A191" s="42" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-26</v>
@@ -30573,7 +30568,7 @@
       <c r="Q191" s="43"/>
       <c r="R191" s="43"/>
     </row>
-    <row r="192" spans="1:18" hidden="1">
+    <row r="192" spans="1:18">
       <c r="A192" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-27</v>
@@ -30613,7 +30608,7 @@
       <c r="Q192" s="40"/>
       <c r="R192" s="40"/>
     </row>
-    <row r="193" spans="1:18" hidden="1">
+    <row r="193" spans="1:18">
       <c r="A193" s="42" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-23</v>
@@ -30653,7 +30648,7 @@
       <c r="Q193" s="43"/>
       <c r="R193" s="43"/>
     </row>
-    <row r="194" spans="1:18" hidden="1">
+    <row r="194" spans="1:18">
       <c r="A194" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-24</v>
@@ -30693,7 +30688,7 @@
       <c r="Q194" s="40"/>
       <c r="R194" s="40"/>
     </row>
-    <row r="195" spans="1:18" hidden="1">
+    <row r="195" spans="1:18">
       <c r="A195" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-28</v>
@@ -30733,7 +30728,7 @@
       <c r="Q195" s="40"/>
       <c r="R195" s="40"/>
     </row>
-    <row r="196" spans="1:18" hidden="1">
+    <row r="196" spans="1:18">
       <c r="A196" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-29</v>
@@ -30815,7 +30810,7 @@
       <c r="Q197" s="40"/>
       <c r="R197" s="40"/>
     </row>
-    <row r="198" spans="1:18" hidden="1">
+    <row r="198" spans="1:18">
       <c r="A198" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Method-7</v>
@@ -30849,7 +30844,7 @@
       <c r="Q198" s="40"/>
       <c r="R198" s="40"/>
     </row>
-    <row r="199" spans="1:18" hidden="1">
+    <row r="199" spans="1:18">
       <c r="A199" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action List-0</v>
@@ -30881,7 +30876,7 @@
       <c r="Q199" s="40"/>
       <c r="R199" s="40"/>
     </row>
-    <row r="200" spans="1:18" hidden="1">
+    <row r="200" spans="1:18">
       <c r="A200" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action List-1</v>
@@ -30913,7 +30908,7 @@
       <c r="Q200" s="40"/>
       <c r="R200" s="40"/>
     </row>
-    <row r="201" spans="1:18" hidden="1">
+    <row r="201" spans="1:18">
       <c r="A201" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Data-0</v>
@@ -30951,7 +30946,7 @@
       <c r="Q201" s="40"/>
       <c r="R201" s="40"/>
     </row>
-    <row r="202" spans="1:18" hidden="1">
+    <row r="202" spans="1:18">
       <c r="A202" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Data-1</v>
@@ -30987,7 +30982,7 @@
       <c r="Q202" s="40"/>
       <c r="R202" s="40"/>
     </row>
-    <row r="203" spans="1:18" hidden="1">
+    <row r="203" spans="1:18">
       <c r="A203" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Data-2</v>
@@ -31065,7 +31060,7 @@
       <c r="Q204" s="40"/>
       <c r="R204" s="40"/>
     </row>
-    <row r="205" spans="1:18" hidden="1">
+    <row r="205" spans="1:18">
       <c r="A205" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Method-8</v>
@@ -31099,7 +31094,7 @@
       <c r="Q205" s="40"/>
       <c r="R205" s="40"/>
     </row>
-    <row r="206" spans="1:18" hidden="1">
+    <row r="206" spans="1:18">
       <c r="A206" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action List-2</v>
@@ -31131,7 +31126,7 @@
       <c r="Q206" s="40"/>
       <c r="R206" s="40"/>
     </row>
-    <row r="207" spans="1:18" hidden="1">
+    <row r="207" spans="1:18">
       <c r="A207" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource List Layout-0</v>
@@ -31171,7 +31166,7 @@
       <c r="Q207" s="40"/>
       <c r="R207" s="40"/>
     </row>
-    <row r="208" spans="1:18" hidden="1">
+    <row r="208" spans="1:18">
       <c r="A208" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource List Layout-1</v>
@@ -31205,7 +31200,7 @@
       <c r="Q208" s="40"/>
       <c r="R208" s="40"/>
     </row>
-    <row r="209" spans="1:18" hidden="1">
+    <row r="209" spans="1:18">
       <c r="A209" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource List Layout-2</v>
@@ -31239,7 +31234,7 @@
       <c r="Q209" s="40"/>
       <c r="R209" s="40"/>
     </row>
-    <row r="210" spans="1:18" hidden="1">
+    <row r="210" spans="1:18">
       <c r="A210" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource List Layout-3</v>
@@ -31273,7 +31268,7 @@
       <c r="Q210" s="40"/>
       <c r="R210" s="40"/>
     </row>
-    <row r="211" spans="1:18" hidden="1">
+    <row r="211" spans="1:18">
       <c r="A211" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource List Layout-4</v>
@@ -31307,7 +31302,7 @@
       <c r="Q211" s="40"/>
       <c r="R211" s="40"/>
     </row>
-    <row r="212" spans="1:18" hidden="1">
+    <row r="212" spans="1:18">
       <c r="A212" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-25</v>
@@ -31347,7 +31342,7 @@
       <c r="Q212" s="16"/>
       <c r="R212" s="16"/>
     </row>
-    <row r="213" spans="1:18" hidden="1">
+    <row r="213" spans="1:18">
       <c r="A213" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-30</v>
@@ -31387,7 +31382,7 @@
       <c r="Q213" s="16"/>
       <c r="R213" s="16"/>
     </row>
-    <row r="214" spans="1:18" hidden="1">
+    <row r="214" spans="1:18">
       <c r="A214" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-26</v>
@@ -31427,7 +31422,7 @@
       <c r="Q214" s="40"/>
       <c r="R214" s="40"/>
     </row>
-    <row r="215" spans="1:18" hidden="1">
+    <row r="215" spans="1:18">
       <c r="A215" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-31</v>
@@ -31467,7 +31462,7 @@
       <c r="Q215" s="40"/>
       <c r="R215" s="40"/>
     </row>
-    <row r="216" spans="1:18" hidden="1">
+    <row r="216" spans="1:18">
       <c r="A216" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-32</v>
@@ -31507,7 +31502,7 @@
       <c r="Q216" s="40"/>
       <c r="R216" s="40"/>
     </row>
-    <row r="217" spans="1:18" hidden="1">
+    <row r="217" spans="1:18">
       <c r="A217" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-27</v>
@@ -31547,7 +31542,7 @@
       <c r="Q217" s="40"/>
       <c r="R217" s="40"/>
     </row>
-    <row r="218" spans="1:18" hidden="1">
+    <row r="218" spans="1:18">
       <c r="A218" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-33</v>
@@ -31587,7 +31582,7 @@
       <c r="Q218" s="40"/>
       <c r="R218" s="40"/>
     </row>
-    <row r="219" spans="1:18" hidden="1">
+    <row r="219" spans="1:18">
       <c r="A219" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Layout-0</v>
@@ -31621,7 +31616,7 @@
       <c r="Q219" s="40"/>
       <c r="R219" s="40"/>
     </row>
-    <row r="220" spans="1:18" hidden="1">
+    <row r="220" spans="1:18">
       <c r="A220" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Layout-1</v>
@@ -31655,7 +31650,7 @@
       <c r="Q220" s="40"/>
       <c r="R220" s="40"/>
     </row>
-    <row r="221" spans="1:18" hidden="1">
+    <row r="221" spans="1:18">
       <c r="A221" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Layout-2</v>
@@ -31689,7 +31684,7 @@
       <c r="Q221" s="40"/>
       <c r="R221" s="40"/>
     </row>
-    <row r="222" spans="1:18" hidden="1">
+    <row r="222" spans="1:18">
       <c r="A222" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Layout-3</v>
@@ -31723,7 +31718,7 @@
       <c r="Q222" s="40"/>
       <c r="R222" s="40"/>
     </row>
-    <row r="223" spans="1:18" hidden="1">
+    <row r="223" spans="1:18">
       <c r="A223" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Layout-4</v>
@@ -31757,7 +31752,7 @@
       <c r="Q223" s="40"/>
       <c r="R223" s="40"/>
     </row>
-    <row r="224" spans="1:18" hidden="1">
+    <row r="224" spans="1:18">
       <c r="A224" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Layout-5</v>
@@ -31791,7 +31786,7 @@
       <c r="Q224" s="40"/>
       <c r="R224" s="40"/>
     </row>
-    <row r="225" spans="1:18" hidden="1">
+    <row r="225" spans="1:18">
       <c r="A225" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Layout-6</v>
@@ -31825,7 +31820,7 @@
       <c r="Q225" s="40"/>
       <c r="R225" s="40"/>
     </row>
-    <row r="226" spans="1:18" hidden="1">
+    <row r="226" spans="1:18">
       <c r="A226" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-28</v>
@@ -31865,7 +31860,7 @@
       <c r="Q226" s="40"/>
       <c r="R226" s="40"/>
     </row>
-    <row r="227" spans="1:18" hidden="1">
+    <row r="227" spans="1:18">
       <c r="A227" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-34</v>
@@ -31905,7 +31900,7 @@
       <c r="Q227" s="40"/>
       <c r="R227" s="40"/>
     </row>
-    <row r="228" spans="1:18" hidden="1">
+    <row r="228" spans="1:18">
       <c r="A228" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-29</v>
@@ -31945,7 +31940,7 @@
       <c r="Q228" s="40"/>
       <c r="R228" s="40"/>
     </row>
-    <row r="229" spans="1:18" hidden="1">
+    <row r="229" spans="1:18">
       <c r="A229" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-35</v>
@@ -31985,7 +31980,7 @@
       <c r="Q229" s="40"/>
       <c r="R229" s="40"/>
     </row>
-    <row r="230" spans="1:18" hidden="1">
+    <row r="230" spans="1:18">
       <c r="A230" s="42" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-36</v>
@@ -32025,7 +32020,7 @@
       <c r="Q230" s="43"/>
       <c r="R230" s="43"/>
     </row>
-    <row r="231" spans="1:18" hidden="1">
+    <row r="231" spans="1:18">
       <c r="A231" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-37</v>
@@ -32065,7 +32060,7 @@
       <c r="Q231" s="40"/>
       <c r="R231" s="40"/>
     </row>
-    <row r="232" spans="1:18" hidden="1">
+    <row r="232" spans="1:18">
       <c r="A232" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Data View Section-0</v>
@@ -32103,7 +32098,7 @@
       <c r="Q232" s="40"/>
       <c r="R232" s="40"/>
     </row>
-    <row r="233" spans="1:18" hidden="1">
+    <row r="233" spans="1:18">
       <c r="A233" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Data View Section-1</v>
@@ -32135,7 +32130,7 @@
       <c r="Q233" s="40"/>
       <c r="R233" s="40"/>
     </row>
-    <row r="234" spans="1:18" hidden="1">
+    <row r="234" spans="1:18">
       <c r="A234" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Data View Section-2</v>
@@ -32167,7 +32162,7 @@
       <c r="Q234" s="40"/>
       <c r="R234" s="40"/>
     </row>
-    <row r="235" spans="1:18" hidden="1">
+    <row r="235" spans="1:18">
       <c r="A235" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Data View Section Items-0</v>
@@ -32203,7 +32198,7 @@
       <c r="Q235" s="40"/>
       <c r="R235" s="40"/>
     </row>
-    <row r="236" spans="1:18" hidden="1">
+    <row r="236" spans="1:18">
       <c r="A236" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Data View Section Items-1</v>
@@ -32237,7 +32232,7 @@
       <c r="Q236" s="40"/>
       <c r="R236" s="40"/>
     </row>
-    <row r="237" spans="1:18" hidden="1">
+    <row r="237" spans="1:18">
       <c r="A237" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Data View Section Items-2</v>
@@ -32271,7 +32266,7 @@
       <c r="Q237" s="40"/>
       <c r="R237" s="40"/>
     </row>
-    <row r="238" spans="1:18" hidden="1">
+    <row r="238" spans="1:18">
       <c r="A238" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Data View Section Items-3</v>
@@ -32305,7 +32300,7 @@
       <c r="Q238" s="40"/>
       <c r="R238" s="40"/>
     </row>
-    <row r="239" spans="1:18" hidden="1">
+    <row r="239" spans="1:18">
       <c r="A239" s="42" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Data View Section Items-4</v>
@@ -32339,7 +32334,7 @@
       <c r="Q239" s="43"/>
       <c r="R239" s="43"/>
     </row>
-    <row r="240" spans="1:18" hidden="1">
+    <row r="240" spans="1:18">
       <c r="A240" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Forms-8</v>
@@ -32377,7 +32372,7 @@
       <c r="Q240" s="40"/>
       <c r="R240" s="40"/>
     </row>
-    <row r="241" spans="1:18" hidden="1">
+    <row r="241" spans="1:18">
       <c r="A241" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Forms-9</v>
@@ -32415,7 +32410,7 @@
       <c r="Q241" s="40"/>
       <c r="R241" s="40"/>
     </row>
-    <row r="242" spans="1:18" hidden="1">
+    <row r="242" spans="1:18">
       <c r="A242" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-34</v>
@@ -32451,7 +32446,7 @@
       <c r="Q242" s="40"/>
       <c r="R242" s="40"/>
     </row>
-    <row r="243" spans="1:18" hidden="1">
+    <row r="243" spans="1:18">
       <c r="A243" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-35</v>
@@ -32487,7 +32482,7 @@
       <c r="Q243" s="40"/>
       <c r="R243" s="40"/>
     </row>
-    <row r="244" spans="1:18" hidden="1">
+    <row r="244" spans="1:18">
       <c r="A244" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-36</v>
@@ -32523,7 +32518,7 @@
       <c r="Q244" s="40"/>
       <c r="R244" s="40"/>
     </row>
-    <row r="245" spans="1:18" hidden="1">
+    <row r="245" spans="1:18">
       <c r="A245" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-37</v>
@@ -32559,7 +32554,7 @@
       <c r="Q245" s="40"/>
       <c r="R245" s="40"/>
     </row>
-    <row r="246" spans="1:18" hidden="1">
+    <row r="246" spans="1:18">
       <c r="A246" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Attrs-1</v>
@@ -32593,7 +32588,7 @@
       <c r="Q246" s="40"/>
       <c r="R246" s="40"/>
     </row>
-    <row r="247" spans="1:18" hidden="1">
+    <row r="247" spans="1:18">
       <c r="A247" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Attrs-2</v>
@@ -32627,7 +32622,7 @@
       <c r="Q247" s="40"/>
       <c r="R247" s="40"/>
     </row>
-    <row r="248" spans="1:18" hidden="1">
+    <row r="248" spans="1:18">
       <c r="A248" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Attrs-3</v>
@@ -32661,7 +32656,7 @@
       <c r="Q248" s="40"/>
       <c r="R248" s="40"/>
     </row>
-    <row r="249" spans="1:18" hidden="1">
+    <row r="249" spans="1:18">
       <c r="A249" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Attrs-4</v>
@@ -32695,7 +32690,7 @@
       <c r="Q249" s="40"/>
       <c r="R249" s="40"/>
     </row>
-    <row r="250" spans="1:18" hidden="1">
+    <row r="250" spans="1:18">
       <c r="A250" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-34</v>
@@ -32727,7 +32722,7 @@
       <c r="Q250" s="40"/>
       <c r="R250" s="40"/>
     </row>
-    <row r="251" spans="1:18" hidden="1">
+    <row r="251" spans="1:18">
       <c r="A251" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-35</v>
@@ -32759,7 +32754,7 @@
       <c r="Q251" s="40"/>
       <c r="R251" s="40"/>
     </row>
-    <row r="252" spans="1:18" hidden="1">
+    <row r="252" spans="1:18">
       <c r="A252" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-36</v>
@@ -32791,7 +32786,7 @@
       <c r="Q252" s="40"/>
       <c r="R252" s="40"/>
     </row>
-    <row r="253" spans="1:18" hidden="1">
+    <row r="253" spans="1:18">
       <c r="A253" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-37</v>
@@ -32823,7 +32818,7 @@
       <c r="Q253" s="40"/>
       <c r="R253" s="40"/>
     </row>
-    <row r="254" spans="1:18" hidden="1">
+    <row r="254" spans="1:18">
       <c r="A254" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-13</v>
@@ -32857,7 +32852,7 @@
       <c r="Q254" s="40"/>
       <c r="R254" s="40"/>
     </row>
-    <row r="255" spans="1:18" hidden="1">
+    <row r="255" spans="1:18">
       <c r="A255" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-14</v>
@@ -32891,7 +32886,7 @@
       <c r="Q255" s="40"/>
       <c r="R255" s="40"/>
     </row>
-    <row r="256" spans="1:18" hidden="1">
+    <row r="256" spans="1:18">
       <c r="A256" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-15</v>
@@ -32925,7 +32920,7 @@
       <c r="Q256" s="40"/>
       <c r="R256" s="40"/>
     </row>
-    <row r="257" spans="1:18" hidden="1">
+    <row r="257" spans="1:18">
       <c r="A257" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-16</v>
@@ -32965,7 +32960,7 @@
       <c r="Q257" s="40"/>
       <c r="R257" s="40"/>
     </row>
-    <row r="258" spans="1:18" hidden="1">
+    <row r="258" spans="1:18">
       <c r="A258" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-17</v>
@@ -32999,7 +32994,7 @@
       <c r="Q258" s="40"/>
       <c r="R258" s="40"/>
     </row>
-    <row r="259" spans="1:18" hidden="1">
+    <row r="259" spans="1:18">
       <c r="A259" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-18</v>
@@ -33033,7 +33028,7 @@
       <c r="Q259" s="40"/>
       <c r="R259" s="40"/>
     </row>
-    <row r="260" spans="1:18" hidden="1">
+    <row r="260" spans="1:18">
       <c r="A260" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-19</v>
@@ -33067,7 +33062,7 @@
       <c r="Q260" s="40"/>
       <c r="R260" s="40"/>
     </row>
-    <row r="261" spans="1:18" hidden="1">
+    <row r="261" spans="1:18">
       <c r="A261" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-20</v>
@@ -33191,7 +33186,7 @@
       <c r="Q263" s="40"/>
       <c r="R263" s="40"/>
     </row>
-    <row r="264" spans="1:18" hidden="1">
+    <row r="264" spans="1:18">
       <c r="A264" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action List-3</v>
@@ -33223,7 +33218,7 @@
       <c r="Q264" s="40"/>
       <c r="R264" s="40"/>
     </row>
-    <row r="265" spans="1:18" hidden="1">
+    <row r="265" spans="1:18">
       <c r="A265" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action List-4</v>
@@ -33351,7 +33346,7 @@
       <c r="Q268" s="40"/>
       <c r="R268" s="40"/>
     </row>
-    <row r="269" spans="1:18" hidden="1">
+    <row r="269" spans="1:18">
       <c r="A269" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Method-9</v>
@@ -33387,7 +33382,7 @@
       <c r="Q269" s="40"/>
       <c r="R269" s="40"/>
     </row>
-    <row r="270" spans="1:18" hidden="1">
+    <row r="270" spans="1:18">
       <c r="A270" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Method-10</v>
@@ -36112,7 +36107,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
New relation from ResourceRelation to Resource as Owner created
</commit_message>
<xml_diff>
--- a/Helper.xlsx
+++ b/Helper.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Tables" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3088" uniqueCount="643">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3099" uniqueCount="646">
   <si>
     <t>resource_scopes</t>
   </si>
@@ -1967,6 +1967,15 @@
   </si>
   <si>
     <t>Resource List Relation</t>
+  </si>
+  <si>
+    <t>Owner Relation</t>
+  </si>
+  <si>
+    <t>View the owner resource</t>
+  </si>
+  <si>
+    <t>Owner</t>
   </si>
 </sst>
 </file>
@@ -4064,9 +4073,13 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R270" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
-  <autoFilter ref="A1:R270">
-    <filterColumn colId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R271" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
+  <autoFilter ref="A1:R271">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Resource Relations"/>
+      </filters>
+    </filterColumn>
   </autoFilter>
   <tableColumns count="18">
     <tableColumn id="19" name="TRCode" dataDxfId="81">
@@ -4141,8 +4154,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RelationTable" displayName="RelationTable" ref="A1:I38" totalsRowShown="0" dataDxfId="47">
-  <autoFilter ref="A1:I38"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RelationTable" displayName="RelationTable" ref="A1:I39" totalsRowShown="0" dataDxfId="47">
+  <autoFilter ref="A1:I39"/>
   <tableColumns count="9">
     <tableColumn id="1" name="No" dataDxfId="46">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
@@ -23508,10 +23521,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R270"/>
+  <dimension ref="A1:R271"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="B156" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -23578,7 +23591,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" hidden="1">
       <c r="A2" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Groups-0</v>
@@ -23612,7 +23625,7 @@
       <c r="Q2" s="15"/>
       <c r="R2" s="15"/>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" hidden="1">
       <c r="A3" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Groups-1</v>
@@ -23646,7 +23659,7 @@
       <c r="Q3" s="16"/>
       <c r="R3" s="16"/>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" hidden="1">
       <c r="A4" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Groups-2</v>
@@ -23680,7 +23693,7 @@
       <c r="Q4" s="16"/>
       <c r="R4" s="16"/>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" hidden="1">
       <c r="A5" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Groups-3</v>
@@ -23714,7 +23727,7 @@
       <c r="Q5" s="16"/>
       <c r="R5" s="16"/>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" hidden="1">
       <c r="A6" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Roles-0</v>
@@ -23748,7 +23761,7 @@
       <c r="Q6" s="16"/>
       <c r="R6" s="16"/>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" hidden="1">
       <c r="A7" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Roles-1</v>
@@ -23782,7 +23795,7 @@
       <c r="Q7" s="16"/>
       <c r="R7" s="16"/>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" hidden="1">
       <c r="A8" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Roles-2</v>
@@ -23816,7 +23829,7 @@
       <c r="Q8" s="16"/>
       <c r="R8" s="16"/>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" hidden="1">
       <c r="A9" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Roles-3</v>
@@ -23850,7 +23863,7 @@
       <c r="Q9" s="16"/>
       <c r="R9" s="16"/>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" hidden="1">
       <c r="A10" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Group Roles-0</v>
@@ -23882,7 +23895,7 @@
       <c r="Q10" s="16"/>
       <c r="R10" s="16"/>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" hidden="1">
       <c r="A11" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Group Roles-1</v>
@@ -23914,7 +23927,7 @@
       <c r="Q11" s="16"/>
       <c r="R11" s="16"/>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" hidden="1">
       <c r="A12" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Group Roles-2</v>
@@ -23946,7 +23959,7 @@
       <c r="Q12" s="16"/>
       <c r="R12" s="16"/>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" hidden="1">
       <c r="A13" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Group Roles-3</v>
@@ -23978,7 +23991,7 @@
       <c r="Q13" s="16"/>
       <c r="R13" s="16"/>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" hidden="1">
       <c r="A14" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-0</v>
@@ -24022,7 +24035,7 @@
       <c r="Q14" s="16"/>
       <c r="R14" s="16"/>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" hidden="1">
       <c r="A15" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-1</v>
@@ -24062,7 +24075,7 @@
       <c r="Q15" s="15"/>
       <c r="R15" s="15"/>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" hidden="1">
       <c r="A16" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-2</v>
@@ -24102,7 +24115,7 @@
       <c r="Q16" s="15"/>
       <c r="R16" s="15"/>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" hidden="1">
       <c r="A17" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-3</v>
@@ -24142,7 +24155,7 @@
       <c r="Q17" s="15"/>
       <c r="R17" s="15"/>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" hidden="1">
       <c r="A18" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-4</v>
@@ -24182,7 +24195,7 @@
       <c r="Q18" s="15"/>
       <c r="R18" s="15"/>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" hidden="1">
       <c r="A19" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-5</v>
@@ -24222,7 +24235,7 @@
       <c r="Q19" s="15"/>
       <c r="R19" s="15"/>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" hidden="1">
       <c r="A20" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-6</v>
@@ -24262,7 +24275,7 @@
       <c r="Q20" s="15"/>
       <c r="R20" s="15"/>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" hidden="1">
       <c r="A21" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-7</v>
@@ -24302,7 +24315,7 @@
       <c r="Q21" s="15"/>
       <c r="R21" s="15"/>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" hidden="1">
       <c r="A22" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-8</v>
@@ -24342,7 +24355,7 @@
       <c r="Q22" s="15"/>
       <c r="R22" s="15"/>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" hidden="1">
       <c r="A23" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-9</v>
@@ -24382,7 +24395,7 @@
       <c r="Q23" s="15"/>
       <c r="R23" s="15"/>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" hidden="1">
       <c r="A24" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-10</v>
@@ -24422,7 +24435,7 @@
       <c r="Q24" s="15"/>
       <c r="R24" s="15"/>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" hidden="1">
       <c r="A25" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-11</v>
@@ -24462,7 +24475,7 @@
       <c r="Q25" s="15"/>
       <c r="R25" s="15"/>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:18" hidden="1">
       <c r="A26" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-12</v>
@@ -24502,7 +24515,7 @@
       <c r="Q26" s="15"/>
       <c r="R26" s="15"/>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:18" hidden="1">
       <c r="A27" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-13</v>
@@ -24542,7 +24555,7 @@
       <c r="Q27" s="16"/>
       <c r="R27" s="16"/>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:18" hidden="1">
       <c r="A28" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Roles-0</v>
@@ -24578,7 +24591,7 @@
       <c r="Q28" s="16"/>
       <c r="R28" s="16"/>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:18" hidden="1">
       <c r="A29" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Roles-1</v>
@@ -24614,7 +24627,7 @@
       <c r="Q29" s="16"/>
       <c r="R29" s="16"/>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:18" hidden="1">
       <c r="A30" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Roles-2</v>
@@ -24646,7 +24659,7 @@
       <c r="Q30" s="16"/>
       <c r="R30" s="16"/>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:18" hidden="1">
       <c r="A31" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Roles-3</v>
@@ -24678,7 +24691,7 @@
       <c r="Q31" s="16"/>
       <c r="R31" s="16"/>
     </row>
-    <row r="32" spans="1:18">
+    <row r="32" spans="1:18" hidden="1">
       <c r="A32" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Roles-4</v>
@@ -24710,7 +24723,7 @@
       <c r="Q32" s="16"/>
       <c r="R32" s="16"/>
     </row>
-    <row r="33" spans="1:18">
+    <row r="33" spans="1:18" hidden="1">
       <c r="A33" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Roles-5</v>
@@ -24742,7 +24755,7 @@
       <c r="Q33" s="16"/>
       <c r="R33" s="16"/>
     </row>
-    <row r="34" spans="1:18">
+    <row r="34" spans="1:18" hidden="1">
       <c r="A34" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Roles-6</v>
@@ -24774,7 +24787,7 @@
       <c r="Q34" s="16"/>
       <c r="R34" s="16"/>
     </row>
-    <row r="35" spans="1:18">
+    <row r="35" spans="1:18" hidden="1">
       <c r="A35" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Roles-7</v>
@@ -25406,7 +25419,7 @@
       <c r="Q50" s="16"/>
       <c r="R50" s="16"/>
     </row>
-    <row r="51" spans="1:18">
+    <row r="51" spans="1:18" hidden="1">
       <c r="A51" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Scopes-0</v>
@@ -25442,7 +25455,7 @@
       <c r="Q51" s="16"/>
       <c r="R51" s="16"/>
     </row>
-    <row r="52" spans="1:18">
+    <row r="52" spans="1:18" hidden="1">
       <c r="A52" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Scopes-1</v>
@@ -25478,7 +25491,7 @@
       <c r="Q52" s="15"/>
       <c r="R52" s="15"/>
     </row>
-    <row r="53" spans="1:18">
+    <row r="53" spans="1:18" hidden="1">
       <c r="A53" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Scopes-2</v>
@@ -25514,7 +25527,7 @@
       <c r="Q53" s="16"/>
       <c r="R53" s="16"/>
     </row>
-    <row r="54" spans="1:18">
+    <row r="54" spans="1:18" hidden="1">
       <c r="A54" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Lists-0</v>
@@ -25550,7 +25563,7 @@
       <c r="Q54" s="16"/>
       <c r="R54" s="16"/>
     </row>
-    <row r="55" spans="1:18">
+    <row r="55" spans="1:18" hidden="1">
       <c r="A55" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Lists-1</v>
@@ -25586,7 +25599,7 @@
       <c r="Q55" s="15"/>
       <c r="R55" s="15"/>
     </row>
-    <row r="56" spans="1:18">
+    <row r="56" spans="1:18" hidden="1">
       <c r="A56" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Lists-2</v>
@@ -25622,7 +25635,7 @@
       <c r="Q56" s="15"/>
       <c r="R56" s="15"/>
     </row>
-    <row r="57" spans="1:18">
+    <row r="57" spans="1:18" hidden="1">
       <c r="A57" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Lists-3</v>
@@ -25658,7 +25671,7 @@
       <c r="Q57" s="15"/>
       <c r="R57" s="15"/>
     </row>
-    <row r="58" spans="1:18">
+    <row r="58" spans="1:18" hidden="1">
       <c r="A58" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Lists-4</v>
@@ -25694,7 +25707,7 @@
       <c r="Q58" s="15"/>
       <c r="R58" s="15"/>
     </row>
-    <row r="59" spans="1:18">
+    <row r="59" spans="1:18" hidden="1">
       <c r="A59" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Lists-5</v>
@@ -25730,7 +25743,7 @@
       <c r="Q59" s="15"/>
       <c r="R59" s="15"/>
     </row>
-    <row r="60" spans="1:18">
+    <row r="60" spans="1:18" hidden="1">
       <c r="A60" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Lists-6</v>
@@ -25766,7 +25779,7 @@
       <c r="Q60" s="16"/>
       <c r="R60" s="16"/>
     </row>
-    <row r="61" spans="1:18">
+    <row r="61" spans="1:18" hidden="1">
       <c r="A61" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource List Scopes-0</v>
@@ -25798,7 +25811,7 @@
       <c r="Q61" s="16"/>
       <c r="R61" s="16"/>
     </row>
-    <row r="62" spans="1:18">
+    <row r="62" spans="1:18" hidden="1">
       <c r="A62" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource List Scopes-1</v>
@@ -25830,7 +25843,7 @@
       <c r="Q62" s="15"/>
       <c r="R62" s="15"/>
     </row>
-    <row r="63" spans="1:18">
+    <row r="63" spans="1:18" hidden="1">
       <c r="A63" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource List Scopes-2</v>
@@ -25862,7 +25875,7 @@
       <c r="Q63" s="16"/>
       <c r="R63" s="16"/>
     </row>
-    <row r="64" spans="1:18">
+    <row r="64" spans="1:18" hidden="1">
       <c r="A64" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Forms-0</v>
@@ -25900,7 +25913,7 @@
       <c r="Q64" s="16"/>
       <c r="R64" s="16"/>
     </row>
-    <row r="65" spans="1:18">
+    <row r="65" spans="1:18" hidden="1">
       <c r="A65" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Forms-1</v>
@@ -25938,7 +25951,7 @@
       <c r="Q65" s="15"/>
       <c r="R65" s="15"/>
     </row>
-    <row r="66" spans="1:18">
+    <row r="66" spans="1:18" hidden="1">
       <c r="A66" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Forms-2</v>
@@ -25976,7 +25989,7 @@
       <c r="Q66" s="15"/>
       <c r="R66" s="15"/>
     </row>
-    <row r="67" spans="1:18">
+    <row r="67" spans="1:18" hidden="1">
       <c r="A67" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Forms-3</v>
@@ -26014,7 +26027,7 @@
       <c r="Q67" s="15"/>
       <c r="R67" s="15"/>
     </row>
-    <row r="68" spans="1:18">
+    <row r="68" spans="1:18" hidden="1">
       <c r="A68" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Forms-4</v>
@@ -26052,7 +26065,7 @@
       <c r="Q68" s="15"/>
       <c r="R68" s="15"/>
     </row>
-    <row r="69" spans="1:18">
+    <row r="69" spans="1:18" hidden="1">
       <c r="A69" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Forms-5</v>
@@ -26090,7 +26103,7 @@
       <c r="Q69" s="15"/>
       <c r="R69" s="15"/>
     </row>
-    <row r="70" spans="1:18">
+    <row r="70" spans="1:18" hidden="1">
       <c r="A70" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Forms-6</v>
@@ -26128,7 +26141,7 @@
       <c r="Q70" s="15"/>
       <c r="R70" s="15"/>
     </row>
-    <row r="71" spans="1:18">
+    <row r="71" spans="1:18" hidden="1">
       <c r="A71" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Forms-7</v>
@@ -26166,7 +26179,7 @@
       <c r="Q71" s="16"/>
       <c r="R71" s="16"/>
     </row>
-    <row r="72" spans="1:18">
+    <row r="72" spans="1:18" hidden="1">
       <c r="A72" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-0</v>
@@ -26204,7 +26217,7 @@
       <c r="Q72" s="16"/>
       <c r="R72" s="16"/>
     </row>
-    <row r="73" spans="1:18">
+    <row r="73" spans="1:18" hidden="1">
       <c r="A73" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-1</v>
@@ -26242,7 +26255,7 @@
       <c r="Q73" s="15"/>
       <c r="R73" s="15"/>
     </row>
-    <row r="74" spans="1:18">
+    <row r="74" spans="1:18" hidden="1">
       <c r="A74" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-2</v>
@@ -26280,7 +26293,7 @@
       <c r="Q74" s="15"/>
       <c r="R74" s="15"/>
     </row>
-    <row r="75" spans="1:18">
+    <row r="75" spans="1:18" hidden="1">
       <c r="A75" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-3</v>
@@ -26318,7 +26331,7 @@
       <c r="Q75" s="15"/>
       <c r="R75" s="15"/>
     </row>
-    <row r="76" spans="1:18">
+    <row r="76" spans="1:18" hidden="1">
       <c r="A76" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-4</v>
@@ -26356,7 +26369,7 @@
       <c r="Q76" s="15"/>
       <c r="R76" s="15"/>
     </row>
-    <row r="77" spans="1:18">
+    <row r="77" spans="1:18" hidden="1">
       <c r="A77" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-5</v>
@@ -26394,7 +26407,7 @@
       <c r="Q77" s="15"/>
       <c r="R77" s="15"/>
     </row>
-    <row r="78" spans="1:18">
+    <row r="78" spans="1:18" hidden="1">
       <c r="A78" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-6</v>
@@ -26432,7 +26445,7 @@
       <c r="Q78" s="15"/>
       <c r="R78" s="15"/>
     </row>
-    <row r="79" spans="1:18">
+    <row r="79" spans="1:18" hidden="1">
       <c r="A79" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-7</v>
@@ -26470,7 +26483,7 @@
       <c r="Q79" s="15"/>
       <c r="R79" s="15"/>
     </row>
-    <row r="80" spans="1:18">
+    <row r="80" spans="1:18" hidden="1">
       <c r="A80" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-8</v>
@@ -26508,7 +26521,7 @@
       <c r="Q80" s="15"/>
       <c r="R80" s="15"/>
     </row>
-    <row r="81" spans="1:18">
+    <row r="81" spans="1:18" hidden="1">
       <c r="A81" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-9</v>
@@ -26546,7 +26559,7 @@
       <c r="Q81" s="15"/>
       <c r="R81" s="15"/>
     </row>
-    <row r="82" spans="1:18">
+    <row r="82" spans="1:18" hidden="1">
       <c r="A82" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-10</v>
@@ -26584,7 +26597,7 @@
       <c r="Q82" s="15"/>
       <c r="R82" s="15"/>
     </row>
-    <row r="83" spans="1:18">
+    <row r="83" spans="1:18" hidden="1">
       <c r="A83" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-11</v>
@@ -26622,7 +26635,7 @@
       <c r="Q83" s="15"/>
       <c r="R83" s="15"/>
     </row>
-    <row r="84" spans="1:18">
+    <row r="84" spans="1:18" hidden="1">
       <c r="A84" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-12</v>
@@ -26660,7 +26673,7 @@
       <c r="Q84" s="15"/>
       <c r="R84" s="15"/>
     </row>
-    <row r="85" spans="1:18">
+    <row r="85" spans="1:18" hidden="1">
       <c r="A85" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-13</v>
@@ -26698,7 +26711,7 @@
       <c r="Q85" s="15"/>
       <c r="R85" s="15"/>
     </row>
-    <row r="86" spans="1:18">
+    <row r="86" spans="1:18" hidden="1">
       <c r="A86" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-14</v>
@@ -26736,7 +26749,7 @@
       <c r="Q86" s="15"/>
       <c r="R86" s="15"/>
     </row>
-    <row r="87" spans="1:18">
+    <row r="87" spans="1:18" hidden="1">
       <c r="A87" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-15</v>
@@ -26774,7 +26787,7 @@
       <c r="Q87" s="15"/>
       <c r="R87" s="15"/>
     </row>
-    <row r="88" spans="1:18">
+    <row r="88" spans="1:18" hidden="1">
       <c r="A88" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-16</v>
@@ -26812,7 +26825,7 @@
       <c r="Q88" s="15"/>
       <c r="R88" s="15"/>
     </row>
-    <row r="89" spans="1:18">
+    <row r="89" spans="1:18" hidden="1">
       <c r="A89" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-17</v>
@@ -26850,7 +26863,7 @@
       <c r="Q89" s="15"/>
       <c r="R89" s="15"/>
     </row>
-    <row r="90" spans="1:18">
+    <row r="90" spans="1:18" hidden="1">
       <c r="A90" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-18</v>
@@ -26888,7 +26901,7 @@
       <c r="Q90" s="15"/>
       <c r="R90" s="15"/>
     </row>
-    <row r="91" spans="1:18">
+    <row r="91" spans="1:18" hidden="1">
       <c r="A91" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-19</v>
@@ -26926,7 +26939,7 @@
       <c r="Q91" s="15"/>
       <c r="R91" s="15"/>
     </row>
-    <row r="92" spans="1:18">
+    <row r="92" spans="1:18" hidden="1">
       <c r="A92" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-20</v>
@@ -26964,7 +26977,7 @@
       <c r="Q92" s="15"/>
       <c r="R92" s="15"/>
     </row>
-    <row r="93" spans="1:18">
+    <row r="93" spans="1:18" hidden="1">
       <c r="A93" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-21</v>
@@ -27002,7 +27015,7 @@
       <c r="Q93" s="15"/>
       <c r="R93" s="15"/>
     </row>
-    <row r="94" spans="1:18">
+    <row r="94" spans="1:18" hidden="1">
       <c r="A94" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-22</v>
@@ -27040,7 +27053,7 @@
       <c r="Q94" s="15"/>
       <c r="R94" s="15"/>
     </row>
-    <row r="95" spans="1:18">
+    <row r="95" spans="1:18" hidden="1">
       <c r="A95" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-23</v>
@@ -27078,7 +27091,7 @@
       <c r="Q95" s="15"/>
       <c r="R95" s="15"/>
     </row>
-    <row r="96" spans="1:18">
+    <row r="96" spans="1:18" hidden="1">
       <c r="A96" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-24</v>
@@ -27116,7 +27129,7 @@
       <c r="Q96" s="15"/>
       <c r="R96" s="15"/>
     </row>
-    <row r="97" spans="1:18">
+    <row r="97" spans="1:18" hidden="1">
       <c r="A97" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-25</v>
@@ -27154,7 +27167,7 @@
       <c r="Q97" s="15"/>
       <c r="R97" s="15"/>
     </row>
-    <row r="98" spans="1:18">
+    <row r="98" spans="1:18" hidden="1">
       <c r="A98" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-26</v>
@@ -27192,7 +27205,7 @@
       <c r="Q98" s="15"/>
       <c r="R98" s="15"/>
     </row>
-    <row r="99" spans="1:18">
+    <row r="99" spans="1:18" hidden="1">
       <c r="A99" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-27</v>
@@ -27230,7 +27243,7 @@
       <c r="Q99" s="15"/>
       <c r="R99" s="15"/>
     </row>
-    <row r="100" spans="1:18">
+    <row r="100" spans="1:18" hidden="1">
       <c r="A100" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-28</v>
@@ -27268,7 +27281,7 @@
       <c r="Q100" s="15"/>
       <c r="R100" s="15"/>
     </row>
-    <row r="101" spans="1:18">
+    <row r="101" spans="1:18" hidden="1">
       <c r="A101" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-29</v>
@@ -27306,7 +27319,7 @@
       <c r="Q101" s="15"/>
       <c r="R101" s="15"/>
     </row>
-    <row r="102" spans="1:18">
+    <row r="102" spans="1:18" hidden="1">
       <c r="A102" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-30</v>
@@ -27344,7 +27357,7 @@
       <c r="Q102" s="15"/>
       <c r="R102" s="15"/>
     </row>
-    <row r="103" spans="1:18">
+    <row r="103" spans="1:18" hidden="1">
       <c r="A103" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-31</v>
@@ -27382,7 +27395,7 @@
       <c r="Q103" s="16"/>
       <c r="R103" s="16"/>
     </row>
-    <row r="104" spans="1:18">
+    <row r="104" spans="1:18" hidden="1">
       <c r="A104" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-0</v>
@@ -27422,7 +27435,7 @@
       <c r="Q104" s="16"/>
       <c r="R104" s="16"/>
     </row>
-    <row r="105" spans="1:18">
+    <row r="105" spans="1:18" hidden="1">
       <c r="A105" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-1</v>
@@ -27454,7 +27467,7 @@
       <c r="Q105" s="16"/>
       <c r="R105" s="16"/>
     </row>
-    <row r="106" spans="1:18">
+    <row r="106" spans="1:18" hidden="1">
       <c r="A106" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-2</v>
@@ -27486,7 +27499,7 @@
       <c r="Q106" s="16"/>
       <c r="R106" s="16"/>
     </row>
-    <row r="107" spans="1:18">
+    <row r="107" spans="1:18" hidden="1">
       <c r="A107" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-3</v>
@@ -27518,7 +27531,7 @@
       <c r="Q107" s="16"/>
       <c r="R107" s="16"/>
     </row>
-    <row r="108" spans="1:18">
+    <row r="108" spans="1:18" hidden="1">
       <c r="A108" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-4</v>
@@ -27550,7 +27563,7 @@
       <c r="Q108" s="16"/>
       <c r="R108" s="16"/>
     </row>
-    <row r="109" spans="1:18">
+    <row r="109" spans="1:18" hidden="1">
       <c r="A109" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-5</v>
@@ -27582,7 +27595,7 @@
       <c r="Q109" s="16"/>
       <c r="R109" s="16"/>
     </row>
-    <row r="110" spans="1:18">
+    <row r="110" spans="1:18" hidden="1">
       <c r="A110" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-6</v>
@@ -27614,7 +27627,7 @@
       <c r="Q110" s="16"/>
       <c r="R110" s="16"/>
     </row>
-    <row r="111" spans="1:18">
+    <row r="111" spans="1:18" hidden="1">
       <c r="A111" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-7</v>
@@ -27646,7 +27659,7 @@
       <c r="Q111" s="16"/>
       <c r="R111" s="16"/>
     </row>
-    <row r="112" spans="1:18">
+    <row r="112" spans="1:18" hidden="1">
       <c r="A112" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-8</v>
@@ -27678,7 +27691,7 @@
       <c r="Q112" s="16"/>
       <c r="R112" s="16"/>
     </row>
-    <row r="113" spans="1:18">
+    <row r="113" spans="1:18" hidden="1">
       <c r="A113" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-9</v>
@@ -27710,7 +27723,7 @@
       <c r="Q113" s="16"/>
       <c r="R113" s="16"/>
     </row>
-    <row r="114" spans="1:18">
+    <row r="114" spans="1:18" hidden="1">
       <c r="A114" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-10</v>
@@ -27742,7 +27755,7 @@
       <c r="Q114" s="16"/>
       <c r="R114" s="16"/>
     </row>
-    <row r="115" spans="1:18">
+    <row r="115" spans="1:18" hidden="1">
       <c r="A115" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-11</v>
@@ -27774,7 +27787,7 @@
       <c r="Q115" s="16"/>
       <c r="R115" s="16"/>
     </row>
-    <row r="116" spans="1:18">
+    <row r="116" spans="1:18" hidden="1">
       <c r="A116" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-12</v>
@@ -27806,7 +27819,7 @@
       <c r="Q116" s="16"/>
       <c r="R116" s="16"/>
     </row>
-    <row r="117" spans="1:18">
+    <row r="117" spans="1:18" hidden="1">
       <c r="A117" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-13</v>
@@ -27838,7 +27851,7 @@
       <c r="Q117" s="16"/>
       <c r="R117" s="16"/>
     </row>
-    <row r="118" spans="1:18">
+    <row r="118" spans="1:18" hidden="1">
       <c r="A118" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-14</v>
@@ -27870,7 +27883,7 @@
       <c r="Q118" s="16"/>
       <c r="R118" s="16"/>
     </row>
-    <row r="119" spans="1:18">
+    <row r="119" spans="1:18" hidden="1">
       <c r="A119" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-15</v>
@@ -27902,7 +27915,7 @@
       <c r="Q119" s="16"/>
       <c r="R119" s="16"/>
     </row>
-    <row r="120" spans="1:18">
+    <row r="120" spans="1:18" hidden="1">
       <c r="A120" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-16</v>
@@ -27934,7 +27947,7 @@
       <c r="Q120" s="16"/>
       <c r="R120" s="16"/>
     </row>
-    <row r="121" spans="1:18">
+    <row r="121" spans="1:18" hidden="1">
       <c r="A121" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-17</v>
@@ -27966,7 +27979,7 @@
       <c r="Q121" s="16"/>
       <c r="R121" s="16"/>
     </row>
-    <row r="122" spans="1:18">
+    <row r="122" spans="1:18" hidden="1">
       <c r="A122" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-18</v>
@@ -27998,7 +28011,7 @@
       <c r="Q122" s="16"/>
       <c r="R122" s="16"/>
     </row>
-    <row r="123" spans="1:18">
+    <row r="123" spans="1:18" hidden="1">
       <c r="A123" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-19</v>
@@ -28030,7 +28043,7 @@
       <c r="Q123" s="16"/>
       <c r="R123" s="16"/>
     </row>
-    <row r="124" spans="1:18">
+    <row r="124" spans="1:18" hidden="1">
       <c r="A124" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-20</v>
@@ -28062,7 +28075,7 @@
       <c r="Q124" s="16"/>
       <c r="R124" s="16"/>
     </row>
-    <row r="125" spans="1:18">
+    <row r="125" spans="1:18" hidden="1">
       <c r="A125" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-21</v>
@@ -28094,7 +28107,7 @@
       <c r="Q125" s="16"/>
       <c r="R125" s="16"/>
     </row>
-    <row r="126" spans="1:18">
+    <row r="126" spans="1:18" hidden="1">
       <c r="A126" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-22</v>
@@ -28126,7 +28139,7 @@
       <c r="Q126" s="16"/>
       <c r="R126" s="16"/>
     </row>
-    <row r="127" spans="1:18">
+    <row r="127" spans="1:18" hidden="1">
       <c r="A127" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-23</v>
@@ -28158,7 +28171,7 @@
       <c r="Q127" s="16"/>
       <c r="R127" s="16"/>
     </row>
-    <row r="128" spans="1:18">
+    <row r="128" spans="1:18" hidden="1">
       <c r="A128" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-24</v>
@@ -28190,7 +28203,7 @@
       <c r="Q128" s="16"/>
       <c r="R128" s="16"/>
     </row>
-    <row r="129" spans="1:18">
+    <row r="129" spans="1:18" hidden="1">
       <c r="A129" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-25</v>
@@ -28222,7 +28235,7 @@
       <c r="Q129" s="16"/>
       <c r="R129" s="16"/>
     </row>
-    <row r="130" spans="1:18">
+    <row r="130" spans="1:18" hidden="1">
       <c r="A130" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-26</v>
@@ -28254,7 +28267,7 @@
       <c r="Q130" s="16"/>
       <c r="R130" s="16"/>
     </row>
-    <row r="131" spans="1:18">
+    <row r="131" spans="1:18" hidden="1">
       <c r="A131" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-27</v>
@@ -28286,7 +28299,7 @@
       <c r="Q131" s="16"/>
       <c r="R131" s="16"/>
     </row>
-    <row r="132" spans="1:18">
+    <row r="132" spans="1:18" hidden="1">
       <c r="A132" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-28</v>
@@ -28318,7 +28331,7 @@
       <c r="Q132" s="16"/>
       <c r="R132" s="16"/>
     </row>
-    <row r="133" spans="1:18">
+    <row r="133" spans="1:18" hidden="1">
       <c r="A133" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-29</v>
@@ -28352,7 +28365,7 @@
       <c r="Q133" s="16"/>
       <c r="R133" s="16"/>
     </row>
-    <row r="134" spans="1:18">
+    <row r="134" spans="1:18" hidden="1">
       <c r="A134" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-30</v>
@@ -28386,7 +28399,7 @@
       <c r="Q134" s="16"/>
       <c r="R134" s="16"/>
     </row>
-    <row r="135" spans="1:18">
+    <row r="135" spans="1:18" hidden="1">
       <c r="A135" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-31</v>
@@ -28420,7 +28433,7 @@
       <c r="Q135" s="16"/>
       <c r="R135" s="16"/>
     </row>
-    <row r="136" spans="1:18">
+    <row r="136" spans="1:18" hidden="1">
       <c r="A136" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Actions-0</v>
@@ -28464,7 +28477,7 @@
       <c r="Q136" s="16"/>
       <c r="R136" s="16"/>
     </row>
-    <row r="137" spans="1:18">
+    <row r="137" spans="1:18" hidden="1">
       <c r="A137" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Actions-1</v>
@@ -28508,7 +28521,7 @@
       <c r="Q137" s="15"/>
       <c r="R137" s="15"/>
     </row>
-    <row r="138" spans="1:18">
+    <row r="138" spans="1:18" hidden="1">
       <c r="A138" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Actions-2</v>
@@ -28552,7 +28565,7 @@
       <c r="Q138" s="15"/>
       <c r="R138" s="15"/>
     </row>
-    <row r="139" spans="1:18">
+    <row r="139" spans="1:18" hidden="1">
       <c r="A139" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Actions-3</v>
@@ -28596,7 +28609,7 @@
       <c r="Q139" s="15"/>
       <c r="R139" s="15"/>
     </row>
-    <row r="140" spans="1:18">
+    <row r="140" spans="1:18" hidden="1">
       <c r="A140" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Actions-4</v>
@@ -28640,7 +28653,7 @@
       <c r="Q140" s="15"/>
       <c r="R140" s="15"/>
     </row>
-    <row r="141" spans="1:18">
+    <row r="141" spans="1:18" hidden="1">
       <c r="A141" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Actions-5</v>
@@ -28684,7 +28697,7 @@
       <c r="Q141" s="15"/>
       <c r="R141" s="15"/>
     </row>
-    <row r="142" spans="1:18">
+    <row r="142" spans="1:18" hidden="1">
       <c r="A142" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Actions-6</v>
@@ -28728,7 +28741,7 @@
       <c r="Q142" s="16"/>
       <c r="R142" s="16"/>
     </row>
-    <row r="143" spans="1:18">
+    <row r="143" spans="1:18" hidden="1">
       <c r="A143" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Method-0</v>
@@ -28772,7 +28785,7 @@
       <c r="Q143" s="16"/>
       <c r="R143" s="16"/>
     </row>
-    <row r="144" spans="1:18">
+    <row r="144" spans="1:18" hidden="1">
       <c r="A144" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Method-1</v>
@@ -28806,7 +28819,7 @@
       <c r="Q144" s="15"/>
       <c r="R144" s="15"/>
     </row>
-    <row r="145" spans="1:18">
+    <row r="145" spans="1:18" hidden="1">
       <c r="A145" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Method-2</v>
@@ -28840,7 +28853,7 @@
       <c r="Q145" s="15"/>
       <c r="R145" s="15"/>
     </row>
-    <row r="146" spans="1:18">
+    <row r="146" spans="1:18" hidden="1">
       <c r="A146" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Method-3</v>
@@ -28874,7 +28887,7 @@
       <c r="Q146" s="15"/>
       <c r="R146" s="15"/>
     </row>
-    <row r="147" spans="1:18">
+    <row r="147" spans="1:18" hidden="1">
       <c r="A147" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Method-4</v>
@@ -28908,7 +28921,7 @@
       <c r="Q147" s="15"/>
       <c r="R147" s="15"/>
     </row>
-    <row r="148" spans="1:18">
+    <row r="148" spans="1:18" hidden="1">
       <c r="A148" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Method-5</v>
@@ -28942,7 +28955,7 @@
       <c r="Q148" s="15"/>
       <c r="R148" s="15"/>
     </row>
-    <row r="149" spans="1:18">
+    <row r="149" spans="1:18" hidden="1">
       <c r="A149" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Method-6</v>
@@ -28976,7 +28989,7 @@
       <c r="Q149" s="16"/>
       <c r="R149" s="16"/>
     </row>
-    <row r="150" spans="1:18">
+    <row r="150" spans="1:18" hidden="1">
       <c r="A150" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Attrs-0</v>
@@ -29010,7 +29023,7 @@
       <c r="Q150" s="40"/>
       <c r="R150" s="40"/>
     </row>
-    <row r="151" spans="1:18">
+    <row r="151" spans="1:18" hidden="1">
       <c r="A151" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-14</v>
@@ -29090,7 +29103,7 @@
       <c r="Q152" s="40"/>
       <c r="R152" s="40"/>
     </row>
-    <row r="153" spans="1:18">
+    <row r="153" spans="1:18" hidden="1">
       <c r="A153" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-15</v>
@@ -29170,7 +29183,7 @@
       <c r="Q154" s="40"/>
       <c r="R154" s="40"/>
     </row>
-    <row r="155" spans="1:18">
+    <row r="155" spans="1:18" hidden="1">
       <c r="A155" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-16</v>
@@ -29250,7 +29263,7 @@
       <c r="Q156" s="40"/>
       <c r="R156" s="40"/>
     </row>
-    <row r="157" spans="1:18">
+    <row r="157" spans="1:18" hidden="1">
       <c r="A157" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-0</v>
@@ -29294,7 +29307,7 @@
       <c r="Q157" s="40"/>
       <c r="R157" s="40"/>
     </row>
-    <row r="158" spans="1:18">
+    <row r="158" spans="1:18" hidden="1">
       <c r="A158" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-1</v>
@@ -29328,7 +29341,7 @@
       <c r="Q158" s="40"/>
       <c r="R158" s="40"/>
     </row>
-    <row r="159" spans="1:18">
+    <row r="159" spans="1:18" hidden="1">
       <c r="A159" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-2</v>
@@ -29362,7 +29375,7 @@
       <c r="Q159" s="40"/>
       <c r="R159" s="40"/>
     </row>
-    <row r="160" spans="1:18">
+    <row r="160" spans="1:18" hidden="1">
       <c r="A160" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-3</v>
@@ -29396,7 +29409,7 @@
       <c r="Q160" s="40"/>
       <c r="R160" s="40"/>
     </row>
-    <row r="161" spans="1:18">
+    <row r="161" spans="1:18" hidden="1">
       <c r="A161" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-4</v>
@@ -29434,7 +29447,7 @@
       <c r="Q161" s="40"/>
       <c r="R161" s="40"/>
     </row>
-    <row r="162" spans="1:18">
+    <row r="162" spans="1:18" hidden="1">
       <c r="A162" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-5</v>
@@ -29468,7 +29481,7 @@
       <c r="Q162" s="40"/>
       <c r="R162" s="40"/>
     </row>
-    <row r="163" spans="1:18">
+    <row r="163" spans="1:18" hidden="1">
       <c r="A163" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-6</v>
@@ -29502,7 +29515,7 @@
       <c r="Q163" s="40"/>
       <c r="R163" s="40"/>
     </row>
-    <row r="164" spans="1:18">
+    <row r="164" spans="1:18" hidden="1">
       <c r="A164" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-7</v>
@@ -29536,7 +29549,7 @@
       <c r="Q164" s="40"/>
       <c r="R164" s="40"/>
     </row>
-    <row r="165" spans="1:18">
+    <row r="165" spans="1:18" hidden="1">
       <c r="A165" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-8</v>
@@ -29614,7 +29627,7 @@
       <c r="Q166" s="40"/>
       <c r="R166" s="40"/>
     </row>
-    <row r="167" spans="1:18">
+    <row r="167" spans="1:18" hidden="1">
       <c r="A167" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-17</v>
@@ -29694,7 +29707,7 @@
       <c r="Q168" s="40"/>
       <c r="R168" s="40"/>
     </row>
-    <row r="169" spans="1:18">
+    <row r="169" spans="1:18" hidden="1">
       <c r="A169" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Defaults-0</v>
@@ -29740,7 +29753,7 @@
       <c r="Q169" s="40"/>
       <c r="R169" s="40"/>
     </row>
-    <row r="170" spans="1:18">
+    <row r="170" spans="1:18" hidden="1">
       <c r="A170" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Defaults-1</v>
@@ -29776,7 +29789,7 @@
       <c r="Q170" s="40"/>
       <c r="R170" s="40"/>
     </row>
-    <row r="171" spans="1:18">
+    <row r="171" spans="1:18" hidden="1">
       <c r="A171" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Defaults-2</v>
@@ -29812,7 +29825,7 @@
       <c r="Q171" s="40"/>
       <c r="R171" s="40"/>
     </row>
-    <row r="172" spans="1:18">
+    <row r="172" spans="1:18" hidden="1">
       <c r="A172" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-18</v>
@@ -30012,7 +30025,7 @@
       <c r="Q176" s="43"/>
       <c r="R176" s="43"/>
     </row>
-    <row r="177" spans="1:18">
+    <row r="177" spans="1:18" hidden="1">
       <c r="A177" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-32</v>
@@ -30048,7 +30061,7 @@
       <c r="Q177" s="40"/>
       <c r="R177" s="40"/>
     </row>
-    <row r="178" spans="1:18">
+    <row r="178" spans="1:18" hidden="1">
       <c r="A178" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-33</v>
@@ -30084,7 +30097,7 @@
       <c r="Q178" s="40"/>
       <c r="R178" s="40"/>
     </row>
-    <row r="179" spans="1:18">
+    <row r="179" spans="1:18" hidden="1">
       <c r="A179" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-32</v>
@@ -30116,7 +30129,7 @@
       <c r="Q179" s="40"/>
       <c r="R179" s="40"/>
     </row>
-    <row r="180" spans="1:18">
+    <row r="180" spans="1:18" hidden="1">
       <c r="A180" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-33</v>
@@ -30148,7 +30161,7 @@
       <c r="Q180" s="40"/>
       <c r="R180" s="40"/>
     </row>
-    <row r="181" spans="1:18">
+    <row r="181" spans="1:18" hidden="1">
       <c r="A181" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-9</v>
@@ -30182,7 +30195,7 @@
       <c r="Q181" s="40"/>
       <c r="R181" s="40"/>
     </row>
-    <row r="182" spans="1:18">
+    <row r="182" spans="1:18" hidden="1">
       <c r="A182" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-10</v>
@@ -30218,7 +30231,7 @@
       <c r="Q182" s="40"/>
       <c r="R182" s="40"/>
     </row>
-    <row r="183" spans="1:18">
+    <row r="183" spans="1:18" hidden="1">
       <c r="A183" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-11</v>
@@ -30252,7 +30265,7 @@
       <c r="Q183" s="40"/>
       <c r="R183" s="40"/>
     </row>
-    <row r="184" spans="1:18">
+    <row r="184" spans="1:18" hidden="1">
       <c r="A184" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-12</v>
@@ -30288,7 +30301,7 @@
       <c r="Q184" s="40"/>
       <c r="R184" s="40"/>
     </row>
-    <row r="185" spans="1:18">
+    <row r="185" spans="1:18" hidden="1">
       <c r="A185" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-19</v>
@@ -30368,7 +30381,7 @@
       <c r="Q186" s="40"/>
       <c r="R186" s="40"/>
     </row>
-    <row r="187" spans="1:18">
+    <row r="187" spans="1:18" hidden="1">
       <c r="A187" s="42" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-20</v>
@@ -30408,7 +30421,7 @@
       <c r="Q187" s="43"/>
       <c r="R187" s="43"/>
     </row>
-    <row r="188" spans="1:18">
+    <row r="188" spans="1:18" hidden="1">
       <c r="A188" s="42" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-21</v>
@@ -30448,7 +30461,7 @@
       <c r="Q188" s="43"/>
       <c r="R188" s="43"/>
     </row>
-    <row r="189" spans="1:18">
+    <row r="189" spans="1:18" hidden="1">
       <c r="A189" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-22</v>
@@ -30608,7 +30621,7 @@
       <c r="Q192" s="40"/>
       <c r="R192" s="40"/>
     </row>
-    <row r="193" spans="1:18">
+    <row r="193" spans="1:18" hidden="1">
       <c r="A193" s="42" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-23</v>
@@ -30648,7 +30661,7 @@
       <c r="Q193" s="43"/>
       <c r="R193" s="43"/>
     </row>
-    <row r="194" spans="1:18">
+    <row r="194" spans="1:18" hidden="1">
       <c r="A194" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-24</v>
@@ -30768,7 +30781,7 @@
       <c r="Q196" s="40"/>
       <c r="R196" s="40"/>
     </row>
-    <row r="197" spans="1:18">
+    <row r="197" spans="1:18" hidden="1">
       <c r="A197" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Actions-7</v>
@@ -30810,7 +30823,7 @@
       <c r="Q197" s="40"/>
       <c r="R197" s="40"/>
     </row>
-    <row r="198" spans="1:18">
+    <row r="198" spans="1:18" hidden="1">
       <c r="A198" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Method-7</v>
@@ -30844,7 +30857,7 @@
       <c r="Q198" s="40"/>
       <c r="R198" s="40"/>
     </row>
-    <row r="199" spans="1:18">
+    <row r="199" spans="1:18" hidden="1">
       <c r="A199" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action List-0</v>
@@ -30876,7 +30889,7 @@
       <c r="Q199" s="40"/>
       <c r="R199" s="40"/>
     </row>
-    <row r="200" spans="1:18">
+    <row r="200" spans="1:18" hidden="1">
       <c r="A200" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action List-1</v>
@@ -30908,7 +30921,7 @@
       <c r="Q200" s="40"/>
       <c r="R200" s="40"/>
     </row>
-    <row r="201" spans="1:18">
+    <row r="201" spans="1:18" hidden="1">
       <c r="A201" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Data-0</v>
@@ -30946,7 +30959,7 @@
       <c r="Q201" s="40"/>
       <c r="R201" s="40"/>
     </row>
-    <row r="202" spans="1:18">
+    <row r="202" spans="1:18" hidden="1">
       <c r="A202" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Data-1</v>
@@ -30982,7 +30995,7 @@
       <c r="Q202" s="40"/>
       <c r="R202" s="40"/>
     </row>
-    <row r="203" spans="1:18">
+    <row r="203" spans="1:18" hidden="1">
       <c r="A203" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Data-2</v>
@@ -31018,7 +31031,7 @@
       <c r="Q203" s="40"/>
       <c r="R203" s="40"/>
     </row>
-    <row r="204" spans="1:18">
+    <row r="204" spans="1:18" hidden="1">
       <c r="A204" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Actions-8</v>
@@ -31060,7 +31073,7 @@
       <c r="Q204" s="40"/>
       <c r="R204" s="40"/>
     </row>
-    <row r="205" spans="1:18">
+    <row r="205" spans="1:18" hidden="1">
       <c r="A205" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Method-8</v>
@@ -31094,7 +31107,7 @@
       <c r="Q205" s="40"/>
       <c r="R205" s="40"/>
     </row>
-    <row r="206" spans="1:18">
+    <row r="206" spans="1:18" hidden="1">
       <c r="A206" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action List-2</v>
@@ -31126,7 +31139,7 @@
       <c r="Q206" s="40"/>
       <c r="R206" s="40"/>
     </row>
-    <row r="207" spans="1:18">
+    <row r="207" spans="1:18" hidden="1">
       <c r="A207" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource List Layout-0</v>
@@ -31166,7 +31179,7 @@
       <c r="Q207" s="40"/>
       <c r="R207" s="40"/>
     </row>
-    <row r="208" spans="1:18">
+    <row r="208" spans="1:18" hidden="1">
       <c r="A208" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource List Layout-1</v>
@@ -31200,7 +31213,7 @@
       <c r="Q208" s="40"/>
       <c r="R208" s="40"/>
     </row>
-    <row r="209" spans="1:18">
+    <row r="209" spans="1:18" hidden="1">
       <c r="A209" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource List Layout-2</v>
@@ -31234,7 +31247,7 @@
       <c r="Q209" s="40"/>
       <c r="R209" s="40"/>
     </row>
-    <row r="210" spans="1:18">
+    <row r="210" spans="1:18" hidden="1">
       <c r="A210" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource List Layout-3</v>
@@ -31268,7 +31281,7 @@
       <c r="Q210" s="40"/>
       <c r="R210" s="40"/>
     </row>
-    <row r="211" spans="1:18">
+    <row r="211" spans="1:18" hidden="1">
       <c r="A211" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource List Layout-4</v>
@@ -31302,7 +31315,7 @@
       <c r="Q211" s="40"/>
       <c r="R211" s="40"/>
     </row>
-    <row r="212" spans="1:18">
+    <row r="212" spans="1:18" hidden="1">
       <c r="A212" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-25</v>
@@ -31382,7 +31395,7 @@
       <c r="Q213" s="16"/>
       <c r="R213" s="16"/>
     </row>
-    <row r="214" spans="1:18">
+    <row r="214" spans="1:18" hidden="1">
       <c r="A214" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-26</v>
@@ -31502,7 +31515,7 @@
       <c r="Q216" s="40"/>
       <c r="R216" s="40"/>
     </row>
-    <row r="217" spans="1:18">
+    <row r="217" spans="1:18" hidden="1">
       <c r="A217" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-27</v>
@@ -31582,7 +31595,7 @@
       <c r="Q218" s="40"/>
       <c r="R218" s="40"/>
     </row>
-    <row r="219" spans="1:18">
+    <row r="219" spans="1:18" hidden="1">
       <c r="A219" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Layout-0</v>
@@ -31616,7 +31629,7 @@
       <c r="Q219" s="40"/>
       <c r="R219" s="40"/>
     </row>
-    <row r="220" spans="1:18">
+    <row r="220" spans="1:18" hidden="1">
       <c r="A220" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Layout-1</v>
@@ -31650,7 +31663,7 @@
       <c r="Q220" s="40"/>
       <c r="R220" s="40"/>
     </row>
-    <row r="221" spans="1:18">
+    <row r="221" spans="1:18" hidden="1">
       <c r="A221" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Layout-2</v>
@@ -31684,7 +31697,7 @@
       <c r="Q221" s="40"/>
       <c r="R221" s="40"/>
     </row>
-    <row r="222" spans="1:18">
+    <row r="222" spans="1:18" hidden="1">
       <c r="A222" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Layout-3</v>
@@ -31718,7 +31731,7 @@
       <c r="Q222" s="40"/>
       <c r="R222" s="40"/>
     </row>
-    <row r="223" spans="1:18">
+    <row r="223" spans="1:18" hidden="1">
       <c r="A223" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Layout-4</v>
@@ -31752,7 +31765,7 @@
       <c r="Q223" s="40"/>
       <c r="R223" s="40"/>
     </row>
-    <row r="224" spans="1:18">
+    <row r="224" spans="1:18" hidden="1">
       <c r="A224" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Layout-5</v>
@@ -31786,7 +31799,7 @@
       <c r="Q224" s="40"/>
       <c r="R224" s="40"/>
     </row>
-    <row r="225" spans="1:18">
+    <row r="225" spans="1:18" hidden="1">
       <c r="A225" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Layout-6</v>
@@ -31820,7 +31833,7 @@
       <c r="Q225" s="40"/>
       <c r="R225" s="40"/>
     </row>
-    <row r="226" spans="1:18">
+    <row r="226" spans="1:18" hidden="1">
       <c r="A226" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-28</v>
@@ -31900,7 +31913,7 @@
       <c r="Q227" s="40"/>
       <c r="R227" s="40"/>
     </row>
-    <row r="228" spans="1:18">
+    <row r="228" spans="1:18" hidden="1">
       <c r="A228" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-29</v>
@@ -32060,7 +32073,7 @@
       <c r="Q231" s="40"/>
       <c r="R231" s="40"/>
     </row>
-    <row r="232" spans="1:18">
+    <row r="232" spans="1:18" hidden="1">
       <c r="A232" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Data View Section-0</v>
@@ -32098,7 +32111,7 @@
       <c r="Q232" s="40"/>
       <c r="R232" s="40"/>
     </row>
-    <row r="233" spans="1:18">
+    <row r="233" spans="1:18" hidden="1">
       <c r="A233" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Data View Section-1</v>
@@ -32130,7 +32143,7 @@
       <c r="Q233" s="40"/>
       <c r="R233" s="40"/>
     </row>
-    <row r="234" spans="1:18">
+    <row r="234" spans="1:18" hidden="1">
       <c r="A234" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Data View Section-2</v>
@@ -32162,7 +32175,7 @@
       <c r="Q234" s="40"/>
       <c r="R234" s="40"/>
     </row>
-    <row r="235" spans="1:18">
+    <row r="235" spans="1:18" hidden="1">
       <c r="A235" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Data View Section Items-0</v>
@@ -32198,7 +32211,7 @@
       <c r="Q235" s="40"/>
       <c r="R235" s="40"/>
     </row>
-    <row r="236" spans="1:18">
+    <row r="236" spans="1:18" hidden="1">
       <c r="A236" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Data View Section Items-1</v>
@@ -32232,7 +32245,7 @@
       <c r="Q236" s="40"/>
       <c r="R236" s="40"/>
     </row>
-    <row r="237" spans="1:18">
+    <row r="237" spans="1:18" hidden="1">
       <c r="A237" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Data View Section Items-2</v>
@@ -32266,7 +32279,7 @@
       <c r="Q237" s="40"/>
       <c r="R237" s="40"/>
     </row>
-    <row r="238" spans="1:18">
+    <row r="238" spans="1:18" hidden="1">
       <c r="A238" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Data View Section Items-3</v>
@@ -32300,7 +32313,7 @@
       <c r="Q238" s="40"/>
       <c r="R238" s="40"/>
     </row>
-    <row r="239" spans="1:18">
+    <row r="239" spans="1:18" hidden="1">
       <c r="A239" s="42" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Data View Section Items-4</v>
@@ -32334,7 +32347,7 @@
       <c r="Q239" s="43"/>
       <c r="R239" s="43"/>
     </row>
-    <row r="240" spans="1:18">
+    <row r="240" spans="1:18" hidden="1">
       <c r="A240" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Forms-8</v>
@@ -32372,7 +32385,7 @@
       <c r="Q240" s="40"/>
       <c r="R240" s="40"/>
     </row>
-    <row r="241" spans="1:18">
+    <row r="241" spans="1:18" hidden="1">
       <c r="A241" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Forms-9</v>
@@ -32410,7 +32423,7 @@
       <c r="Q241" s="40"/>
       <c r="R241" s="40"/>
     </row>
-    <row r="242" spans="1:18">
+    <row r="242" spans="1:18" hidden="1">
       <c r="A242" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-34</v>
@@ -32446,7 +32459,7 @@
       <c r="Q242" s="40"/>
       <c r="R242" s="40"/>
     </row>
-    <row r="243" spans="1:18">
+    <row r="243" spans="1:18" hidden="1">
       <c r="A243" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-35</v>
@@ -32482,7 +32495,7 @@
       <c r="Q243" s="40"/>
       <c r="R243" s="40"/>
     </row>
-    <row r="244" spans="1:18">
+    <row r="244" spans="1:18" hidden="1">
       <c r="A244" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-36</v>
@@ -32518,7 +32531,7 @@
       <c r="Q244" s="40"/>
       <c r="R244" s="40"/>
     </row>
-    <row r="245" spans="1:18">
+    <row r="245" spans="1:18" hidden="1">
       <c r="A245" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-37</v>
@@ -32554,7 +32567,7 @@
       <c r="Q245" s="40"/>
       <c r="R245" s="40"/>
     </row>
-    <row r="246" spans="1:18">
+    <row r="246" spans="1:18" hidden="1">
       <c r="A246" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Attrs-1</v>
@@ -32588,7 +32601,7 @@
       <c r="Q246" s="40"/>
       <c r="R246" s="40"/>
     </row>
-    <row r="247" spans="1:18">
+    <row r="247" spans="1:18" hidden="1">
       <c r="A247" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Attrs-2</v>
@@ -32622,7 +32635,7 @@
       <c r="Q247" s="40"/>
       <c r="R247" s="40"/>
     </row>
-    <row r="248" spans="1:18">
+    <row r="248" spans="1:18" hidden="1">
       <c r="A248" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Attrs-3</v>
@@ -32656,7 +32669,7 @@
       <c r="Q248" s="40"/>
       <c r="R248" s="40"/>
     </row>
-    <row r="249" spans="1:18">
+    <row r="249" spans="1:18" hidden="1">
       <c r="A249" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Attrs-4</v>
@@ -32690,7 +32703,7 @@
       <c r="Q249" s="40"/>
       <c r="R249" s="40"/>
     </row>
-    <row r="250" spans="1:18">
+    <row r="250" spans="1:18" hidden="1">
       <c r="A250" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-34</v>
@@ -32722,7 +32735,7 @@
       <c r="Q250" s="40"/>
       <c r="R250" s="40"/>
     </row>
-    <row r="251" spans="1:18">
+    <row r="251" spans="1:18" hidden="1">
       <c r="A251" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-35</v>
@@ -32754,7 +32767,7 @@
       <c r="Q251" s="40"/>
       <c r="R251" s="40"/>
     </row>
-    <row r="252" spans="1:18">
+    <row r="252" spans="1:18" hidden="1">
       <c r="A252" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-36</v>
@@ -32786,7 +32799,7 @@
       <c r="Q252" s="40"/>
       <c r="R252" s="40"/>
     </row>
-    <row r="253" spans="1:18">
+    <row r="253" spans="1:18" hidden="1">
       <c r="A253" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-37</v>
@@ -32818,7 +32831,7 @@
       <c r="Q253" s="40"/>
       <c r="R253" s="40"/>
     </row>
-    <row r="254" spans="1:18">
+    <row r="254" spans="1:18" hidden="1">
       <c r="A254" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-13</v>
@@ -32852,7 +32865,7 @@
       <c r="Q254" s="40"/>
       <c r="R254" s="40"/>
     </row>
-    <row r="255" spans="1:18">
+    <row r="255" spans="1:18" hidden="1">
       <c r="A255" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-14</v>
@@ -32886,7 +32899,7 @@
       <c r="Q255" s="40"/>
       <c r="R255" s="40"/>
     </row>
-    <row r="256" spans="1:18">
+    <row r="256" spans="1:18" hidden="1">
       <c r="A256" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-15</v>
@@ -32920,7 +32933,7 @@
       <c r="Q256" s="40"/>
       <c r="R256" s="40"/>
     </row>
-    <row r="257" spans="1:18">
+    <row r="257" spans="1:18" hidden="1">
       <c r="A257" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-16</v>
@@ -32960,7 +32973,7 @@
       <c r="Q257" s="40"/>
       <c r="R257" s="40"/>
     </row>
-    <row r="258" spans="1:18">
+    <row r="258" spans="1:18" hidden="1">
       <c r="A258" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-17</v>
@@ -32994,7 +33007,7 @@
       <c r="Q258" s="40"/>
       <c r="R258" s="40"/>
     </row>
-    <row r="259" spans="1:18">
+    <row r="259" spans="1:18" hidden="1">
       <c r="A259" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-18</v>
@@ -33028,7 +33041,7 @@
       <c r="Q259" s="40"/>
       <c r="R259" s="40"/>
     </row>
-    <row r="260" spans="1:18">
+    <row r="260" spans="1:18" hidden="1">
       <c r="A260" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-19</v>
@@ -33062,7 +33075,7 @@
       <c r="Q260" s="40"/>
       <c r="R260" s="40"/>
     </row>
-    <row r="261" spans="1:18">
+    <row r="261" spans="1:18" hidden="1">
       <c r="A261" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-20</v>
@@ -33102,7 +33115,7 @@
       <c r="Q261" s="40"/>
       <c r="R261" s="40"/>
     </row>
-    <row r="262" spans="1:18">
+    <row r="262" spans="1:18" hidden="1">
       <c r="A262" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Actions-9</v>
@@ -33144,7 +33157,7 @@
       <c r="Q262" s="40"/>
       <c r="R262" s="40"/>
     </row>
-    <row r="263" spans="1:18">
+    <row r="263" spans="1:18" hidden="1">
       <c r="A263" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Actions-10</v>
@@ -33186,7 +33199,7 @@
       <c r="Q263" s="40"/>
       <c r="R263" s="40"/>
     </row>
-    <row r="264" spans="1:18">
+    <row r="264" spans="1:18" hidden="1">
       <c r="A264" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action List-3</v>
@@ -33218,7 +33231,7 @@
       <c r="Q264" s="40"/>
       <c r="R264" s="40"/>
     </row>
-    <row r="265" spans="1:18">
+    <row r="265" spans="1:18" hidden="1">
       <c r="A265" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action List-4</v>
@@ -33250,7 +33263,7 @@
       <c r="Q265" s="40"/>
       <c r="R265" s="40"/>
     </row>
-    <row r="266" spans="1:18">
+    <row r="266" spans="1:18" hidden="1">
       <c r="A266" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Data-0</v>
@@ -33282,7 +33295,7 @@
       <c r="Q266" s="40"/>
       <c r="R266" s="40"/>
     </row>
-    <row r="267" spans="1:18">
+    <row r="267" spans="1:18" hidden="1">
       <c r="A267" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Data-1</v>
@@ -33314,7 +33327,7 @@
       <c r="Q267" s="40"/>
       <c r="R267" s="40"/>
     </row>
-    <row r="268" spans="1:18">
+    <row r="268" spans="1:18" hidden="1">
       <c r="A268" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Data-2</v>
@@ -33346,7 +33359,7 @@
       <c r="Q268" s="40"/>
       <c r="R268" s="40"/>
     </row>
-    <row r="269" spans="1:18">
+    <row r="269" spans="1:18" hidden="1">
       <c r="A269" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Method-9</v>
@@ -33382,7 +33395,7 @@
       <c r="Q269" s="40"/>
       <c r="R269" s="40"/>
     </row>
-    <row r="270" spans="1:18">
+    <row r="270" spans="1:18" hidden="1">
       <c r="A270" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Method-10</v>
@@ -33417,6 +33430,46 @@
       <c r="P270" s="40"/>
       <c r="Q270" s="40"/>
       <c r="R270" s="40"/>
+    </row>
+    <row r="271" spans="1:18">
+      <c r="A271" s="22" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resource Relations-38</v>
+      </c>
+      <c r="B271" s="40" t="s">
+        <v>443</v>
+      </c>
+      <c r="C271" s="22">
+        <f>COUNTIF($B$1:$B270,[Table Name])</f>
+        <v>38</v>
+      </c>
+      <c r="D271" s="40">
+        <v>26</v>
+      </c>
+      <c r="E271" s="40" t="s">
+        <v>643</v>
+      </c>
+      <c r="F271" s="40" t="s">
+        <v>644</v>
+      </c>
+      <c r="G271" s="40" t="s">
+        <v>645</v>
+      </c>
+      <c r="H271" s="40" t="s">
+        <v>403</v>
+      </c>
+      <c r="I271" s="40">
+        <v>4</v>
+      </c>
+      <c r="J271" s="40"/>
+      <c r="K271" s="40"/>
+      <c r="L271" s="40"/>
+      <c r="M271" s="40"/>
+      <c r="N271" s="40"/>
+      <c r="O271" s="40"/>
+      <c r="P271" s="40"/>
+      <c r="Q271" s="40"/>
+      <c r="R271" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -34855,10 +34908,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37:I38"/>
+      <selection activeCell="I39" sqref="D39:I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -36090,9 +36143,41 @@
         <v>26</v>
       </c>
     </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="20">
+        <f>IFERROR($A38+1,1)</f>
+        <v>38</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>572</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="D39" s="7">
+        <f>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</f>
+        <v>26</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>643</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>644</v>
+      </c>
+      <c r="G39" s="22" t="s">
+        <v>645</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="I39" s="41">
+        <f>VLOOKUP([Relate Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</f>
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C38">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C39">
       <formula1>Resources</formula1>
     </dataValidation>
   </dataValidations>
@@ -36107,8 +36192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T109"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -36118,14 +36203,14 @@
   <sheetData>
     <row r="1" spans="1:20" s="38" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="48" t="s">
-        <v>389</v>
+        <v>443</v>
       </c>
       <c r="B1" s="48"/>
       <c r="C1" s="48"/>
       <c r="D1" s="48"/>
       <c r="E1" s="49" t="str">
         <f>"\"&amp;VLOOKUP($A$1,SeedMap[],3,0)&amp;"\"&amp;VLOOKUP($A$1,SeedMap[],4,0)&amp;"::"&amp;VLOOKUP($A$1,SeedMap[],5,0)&amp;"()"</f>
-        <v>\Milestone\Appframe\Model\ResourceActionData::truncate()</v>
+        <v>\Milestone\Appframe\Model\ResourceRelation::truncate()</v>
       </c>
       <c r="F1" s="49"/>
       <c r="G1" s="49"/>
@@ -36269,27 +36354,27 @@
       <c r="B5" s="28"/>
       <c r="C5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],C$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],C$4+$B$4,0))</f>
-        <v>resource_action</v>
+        <v>resource</v>
       </c>
       <c r="D5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],D$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],D$4+$B$4,0))</f>
-        <v>resource_data</v>
+        <v>name</v>
       </c>
       <c r="E5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0))</f>
-        <v/>
+        <v>description</v>
       </c>
       <c r="F5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0))</f>
-        <v/>
+        <v>method</v>
       </c>
       <c r="G5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0))</f>
-        <v/>
+        <v>type</v>
       </c>
       <c r="H5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],H$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],H$4+$B$4,0))</f>
-        <v/>
+        <v>relate_resource</v>
       </c>
       <c r="I5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],I$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],I$4+$B$4,0))</f>
@@ -36383,7 +36468,7 @@
       <c r="A8" s="32"/>
       <c r="B8" s="47" t="str">
         <f>$E$1</f>
-        <v>\Milestone\Appframe\Model\ResourceActionData::truncate()</v>
+        <v>\Milestone\Appframe\Model\ResourceRelation::truncate()</v>
       </c>
       <c r="C8" s="47"/>
       <c r="D8" s="47"/>
@@ -36412,27 +36497,27 @@
       </c>
       <c r="C9" s="33" t="str">
         <f ca="1">IF(AND($B9=$S$4,C$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),C$4+$B$4,0)="","","'"&amp;C$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),C$4+$B$4,0)&amp;"', "),"")</f>
-        <v xml:space="preserve">'resource_action' =&gt; '9', </v>
+        <v xml:space="preserve">'resource' =&gt; '1', </v>
       </c>
       <c r="D9" s="33" t="str">
         <f t="shared" ref="D9:Q24" ca="1" si="0">IF(AND($B9=$S$4,D$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),D$4+$B$4,0)="","","'"&amp;D$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),D$4+$B$4,0)&amp;"', "),"")</f>
-        <v xml:space="preserve">'resource_data' =&gt; '1', </v>
+        <v xml:space="preserve">'name' =&gt; 'User Groups', </v>
       </c>
       <c r="E9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Which groups this user belongs to', </v>
       </c>
       <c r="F9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Groups', </v>
       </c>
       <c r="G9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
       </c>
       <c r="H9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '2', </v>
       </c>
       <c r="I9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -36485,27 +36570,27 @@
       </c>
       <c r="C10" s="33" t="str">
         <f ca="1">IF(AND($B10=$S$4,C$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A10,INDIRECT($E$2),C$4+$B$4,0)="","","'"&amp;C$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A10,INDIRECT($E$2),C$4+$B$4,0)&amp;"', "),"")</f>
-        <v xml:space="preserve">'resource_action' =&gt; '10', </v>
+        <v xml:space="preserve">'resource' =&gt; '2', </v>
       </c>
       <c r="D10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'resource_data' =&gt; '2', </v>
+        <v xml:space="preserve">'name' =&gt; 'Group Users', </v>
       </c>
       <c r="E10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'List of users belongs to this group', </v>
       </c>
       <c r="F10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Users', </v>
       </c>
       <c r="G10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
       </c>
       <c r="H10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '1', </v>
       </c>
       <c r="I10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -36554,31 +36639,31 @@
       </c>
       <c r="B11" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>;</v>
+        <v>-&gt;create([</v>
       </c>
       <c r="C11" s="33" t="str">
         <f t="shared" ref="C11:G74" ca="1" si="3">IF(AND($B11=$S$4,C$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A11,INDIRECT($E$2),C$4+$B$4,0)="","","'"&amp;C$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A11,INDIRECT($E$2),C$4+$B$4,0)&amp;"', "),"")</f>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '2', </v>
       </c>
       <c r="D11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Group Roles', </v>
       </c>
       <c r="E11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Roles assigneed to this group', </v>
       </c>
       <c r="F11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Roles', </v>
       </c>
       <c r="G11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
       </c>
       <c r="H11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '3', </v>
       </c>
       <c r="I11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -36618,7 +36703,7 @@
       </c>
       <c r="R11" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -36627,31 +36712,31 @@
       </c>
       <c r="B12" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
+        <v>-&gt;create([</v>
       </c>
       <c r="C12" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '3', </v>
       </c>
       <c r="D12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Role Groups', </v>
       </c>
       <c r="E12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Details of groups this role assigned to', </v>
       </c>
       <c r="F12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Groups', </v>
       </c>
       <c r="G12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
       </c>
       <c r="H12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '2', </v>
       </c>
       <c r="I12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -36691,7 +36776,7 @@
       </c>
       <c r="R12" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -36700,31 +36785,31 @@
       </c>
       <c r="B13" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C13" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '3', </v>
       </c>
       <c r="D13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Role Resource', </v>
       </c>
       <c r="E13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Resources assigned to a role', </v>
       </c>
       <c r="F13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Resources', </v>
       </c>
       <c r="G13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '11', </v>
       </c>
       <c r="I13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -36764,7 +36849,7 @@
       </c>
       <c r="R13" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -36773,31 +36858,31 @@
       </c>
       <c r="B14" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C14" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '4', </v>
       </c>
       <c r="D14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Resource Roles', </v>
       </c>
       <c r="E14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'The details of roles who have access to this resource', </v>
       </c>
       <c r="F14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Roles', </v>
       </c>
       <c r="G14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
       </c>
       <c r="H14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '3', </v>
       </c>
       <c r="I14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -36837,7 +36922,7 @@
       </c>
       <c r="R14" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -36846,31 +36931,31 @@
       </c>
       <c r="B15" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C15" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '4', </v>
       </c>
       <c r="D15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Resource Actions', </v>
       </c>
       <c r="E15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Get actions available for the resource', </v>
       </c>
       <c r="F15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Actions', </v>
       </c>
       <c r="G15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '7', </v>
       </c>
       <c r="I15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -36910,7 +36995,7 @@
       </c>
       <c r="R15" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="16" spans="1:20">
@@ -36919,31 +37004,31 @@
       </c>
       <c r="B16" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C16" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '7', </v>
       </c>
       <c r="D16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Resource Action Methods', </v>
       </c>
       <c r="E16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Handler details of an action', </v>
       </c>
       <c r="F16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Method', </v>
       </c>
       <c r="G16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasOne', </v>
       </c>
       <c r="H16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '8', </v>
       </c>
       <c r="I16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -36983,7 +37068,7 @@
       </c>
       <c r="R16" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="17" spans="1:18">
@@ -36992,31 +37077,31 @@
       </c>
       <c r="B17" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C17" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '7', </v>
       </c>
       <c r="D17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Resource Action Lists', </v>
       </c>
       <c r="E17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Lists where action available', </v>
       </c>
       <c r="F17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Lists', </v>
       </c>
       <c r="G17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '9', </v>
       </c>
       <c r="I17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -37056,7 +37141,7 @@
       </c>
       <c r="R17" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="18" spans="1:18">
@@ -37065,31 +37150,31 @@
       </c>
       <c r="B18" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C18" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '7', </v>
       </c>
       <c r="D18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Resource Action Data', </v>
       </c>
       <c r="E18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Resource data where action available', </v>
       </c>
       <c r="F18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Data', </v>
       </c>
       <c r="G18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '10', </v>
       </c>
       <c r="I18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -37129,7 +37214,7 @@
       </c>
       <c r="R18" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="19" spans="1:18">
@@ -37138,31 +37223,31 @@
       </c>
       <c r="B19" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C19" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '5', </v>
       </c>
       <c r="D19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Organisation Contacts', </v>
       </c>
       <c r="E19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Contact details of organisation', </v>
       </c>
       <c r="F19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Contacts', </v>
       </c>
       <c r="G19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '6', </v>
       </c>
       <c r="I19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -37202,7 +37287,7 @@
       </c>
       <c r="R19" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="20" spans="1:18">
@@ -37211,31 +37296,31 @@
       </c>
       <c r="B20" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C20" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '11', </v>
       </c>
       <c r="D20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Resource Details', </v>
       </c>
       <c r="E20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Resource details', </v>
       </c>
       <c r="F20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Resource', </v>
       </c>
       <c r="G20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
       </c>
       <c r="I20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -37275,7 +37360,7 @@
       </c>
       <c r="R20" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="21" spans="1:18">
@@ -37284,31 +37369,31 @@
       </c>
       <c r="B21" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C21" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '4', </v>
       </c>
       <c r="D21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Resource Forms', </v>
       </c>
       <c r="E21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Forms available for a resource', </v>
       </c>
       <c r="F21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Forms', </v>
       </c>
       <c r="G21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '12', </v>
       </c>
       <c r="I21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -37348,7 +37433,7 @@
       </c>
       <c r="R21" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="22" spans="1:18">
@@ -37357,31 +37442,31 @@
       </c>
       <c r="B22" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C22" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '12', </v>
       </c>
       <c r="D22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Form Fields', </v>
       </c>
       <c r="E22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Fields associated with a form', </v>
       </c>
       <c r="F22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Fields', </v>
       </c>
       <c r="G22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '13', </v>
       </c>
       <c r="I22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -37421,7 +37506,7 @@
       </c>
       <c r="R22" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="23" spans="1:18">
@@ -37430,31 +37515,31 @@
       </c>
       <c r="B23" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C23" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '13', </v>
       </c>
       <c r="D23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Field Attributes', </v>
       </c>
       <c r="E23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Attributes of Field', </v>
       </c>
       <c r="F23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Attributes', </v>
       </c>
       <c r="G23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '14', </v>
       </c>
       <c r="I23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -37494,7 +37579,7 @@
       </c>
       <c r="R23" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="24" spans="1:18">
@@ -37503,31 +37588,31 @@
       </c>
       <c r="B24" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C24" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '13', </v>
       </c>
       <c r="D24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Field Options', </v>
       </c>
       <c r="E24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Options of Field', </v>
       </c>
       <c r="F24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Options', </v>
       </c>
       <c r="G24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasOne', </v>
       </c>
       <c r="H24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '15', </v>
       </c>
       <c r="I24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -37567,7 +37652,7 @@
       </c>
       <c r="R24" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="25" spans="1:18">
@@ -37576,31 +37661,31 @@
       </c>
       <c r="B25" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '13', </v>
       </c>
       <c r="D25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Field Validations', </v>
       </c>
       <c r="E25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Validation details of field', </v>
       </c>
       <c r="F25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Validations', </v>
       </c>
       <c r="G25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H25" s="33" t="str">
         <f t="shared" ref="H25:K88" ca="1" si="4">IF(AND($B25=$S$4,H$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A25,INDIRECT($E$2),H$4+$B$4,0)="","","'"&amp;H$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A25,INDIRECT($E$2),H$4+$B$4,0)&amp;"', "),"")</f>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '16', </v>
       </c>
       <c r="I25" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -37640,7 +37725,7 @@
       </c>
       <c r="R25" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="26" spans="1:18">
@@ -37649,31 +37734,31 @@
       </c>
       <c r="B26" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '12', </v>
       </c>
       <c r="D26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'From Resource', </v>
       </c>
       <c r="E26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Resource this form belongs to', </v>
       </c>
       <c r="F26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Resource', </v>
       </c>
       <c r="G26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H26" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
       </c>
       <c r="I26" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -37713,7 +37798,7 @@
       </c>
       <c r="R26" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="27" spans="1:18">
@@ -37722,31 +37807,31 @@
       </c>
       <c r="B27" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '12', </v>
       </c>
       <c r="D27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Form Defaults', </v>
       </c>
       <c r="E27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Predefined values for a form', </v>
       </c>
       <c r="F27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Defaults', </v>
       </c>
       <c r="G27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H27" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '17', </v>
       </c>
       <c r="I27" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -37786,7 +37871,7 @@
       </c>
       <c r="R27" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="28" spans="1:18">
@@ -37795,31 +37880,31 @@
       </c>
       <c r="B28" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '13', </v>
       </c>
       <c r="D28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Field Data', </v>
       </c>
       <c r="E28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Fields Database binding details', </v>
       </c>
       <c r="F28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Data', </v>
       </c>
       <c r="G28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasOne', </v>
       </c>
       <c r="H28" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '18', </v>
       </c>
       <c r="I28" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -37859,7 +37944,7 @@
       </c>
       <c r="R28" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="29" spans="1:18">
@@ -37868,31 +37953,31 @@
       </c>
       <c r="B29" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '4', </v>
       </c>
       <c r="D29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Resource Relations', </v>
       </c>
       <c r="E29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Relation of  a resource to another resource', </v>
       </c>
       <c r="F29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Relations', </v>
       </c>
       <c r="G29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H29" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
       </c>
       <c r="I29" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -37932,7 +38017,7 @@
       </c>
       <c r="R29" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="30" spans="1:18">
@@ -37941,31 +38026,31 @@
       </c>
       <c r="B30" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '18', </v>
       </c>
       <c r="D30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Bind Data Resource', </v>
       </c>
       <c r="E30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Resource to which the data to be bind', </v>
       </c>
       <c r="F30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
       </c>
       <c r="G30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H30" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
       </c>
       <c r="I30" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -38005,7 +38090,7 @@
       </c>
       <c r="R30" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="31" spans="1:18">
@@ -38014,31 +38099,31 @@
       </c>
       <c r="B31" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '17', </v>
       </c>
       <c r="D31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Default Data Resource', </v>
       </c>
       <c r="E31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Resource to which the forms predefined data to be bind', </v>
       </c>
       <c r="F31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
       </c>
       <c r="G31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H31" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
       </c>
       <c r="I31" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -38078,7 +38163,7 @@
       </c>
       <c r="R31" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="32" spans="1:18">
@@ -38087,31 +38172,31 @@
       </c>
       <c r="B32" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '19', </v>
       </c>
       <c r="D32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Resource Details', </v>
       </c>
       <c r="E32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Resource details of a list', </v>
       </c>
       <c r="F32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Resource', </v>
       </c>
       <c r="G32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H32" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
       </c>
       <c r="I32" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -38151,7 +38236,7 @@
       </c>
       <c r="R32" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="33" spans="1:18">
@@ -38160,31 +38245,31 @@
       </c>
       <c r="B33" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '19', </v>
       </c>
       <c r="D33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'List Relations', </v>
       </c>
       <c r="E33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Relations to be loaded on accessing list', </v>
       </c>
       <c r="F33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Relations', </v>
       </c>
       <c r="G33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H33" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '20', </v>
       </c>
       <c r="I33" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -38224,7 +38309,7 @@
       </c>
       <c r="R33" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="34" spans="1:18">
@@ -38233,31 +38318,31 @@
       </c>
       <c r="B34" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '4', </v>
       </c>
       <c r="D34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Resource Scopes', </v>
       </c>
       <c r="E34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Scopes available on a Resource', </v>
       </c>
       <c r="F34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Scopes', </v>
       </c>
       <c r="G34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H34" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '21', </v>
       </c>
       <c r="I34" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -38297,7 +38382,7 @@
       </c>
       <c r="R34" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="35" spans="1:18">
@@ -38306,31 +38391,31 @@
       </c>
       <c r="B35" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '19', </v>
       </c>
       <c r="D35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'List Scopes', </v>
       </c>
       <c r="E35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Scopes by which a list to be filtered', </v>
       </c>
       <c r="F35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Scopes', </v>
       </c>
       <c r="G35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
       </c>
       <c r="H35" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '21', </v>
       </c>
       <c r="I35" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -38370,7 +38455,7 @@
       </c>
       <c r="R35" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="36" spans="1:18">
@@ -38379,31 +38464,31 @@
       </c>
       <c r="B36" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '23', </v>
       </c>
       <c r="D36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Data Relation', </v>
       </c>
       <c r="E36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Relations to be loaded on a data view', </v>
       </c>
       <c r="F36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Relations', </v>
       </c>
       <c r="G36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H36" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '24', </v>
       </c>
       <c r="I36" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -38443,7 +38528,7 @@
       </c>
       <c r="R36" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="37" spans="1:18">
@@ -38452,31 +38537,31 @@
       </c>
       <c r="B37" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '23', </v>
       </c>
       <c r="D37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Resource Details', </v>
       </c>
       <c r="E37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Details of resource of a record', </v>
       </c>
       <c r="F37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Resource', </v>
       </c>
       <c r="G37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H37" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
       </c>
       <c r="I37" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -38516,7 +38601,7 @@
       </c>
       <c r="R37" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="38" spans="1:18">
@@ -38525,31 +38610,31 @@
       </c>
       <c r="B38" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '19', </v>
       </c>
       <c r="D38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'List Layout', </v>
       </c>
       <c r="E38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Layout of a list', </v>
       </c>
       <c r="F38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Layout', </v>
       </c>
       <c r="G38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H38" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '25', </v>
       </c>
       <c r="I38" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -38589,7 +38674,7 @@
       </c>
       <c r="R38" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="39" spans="1:18">
@@ -38598,31 +38683,31 @@
       </c>
       <c r="B39" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C39" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '26', </v>
       </c>
       <c r="D39" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Nested Relation', </v>
       </c>
       <c r="E39" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Nested Relation', </v>
       </c>
       <c r="F39" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Nest', </v>
       </c>
       <c r="G39" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H39" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
       </c>
       <c r="I39" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -38662,7 +38747,7 @@
       </c>
       <c r="R39" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="40" spans="1:18">
@@ -38671,31 +38756,31 @@
       </c>
       <c r="B40" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C40" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '26', </v>
       </c>
       <c r="D40" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Related Resource', </v>
       </c>
       <c r="E40" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Related Resource Details', </v>
       </c>
       <c r="F40" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
       </c>
       <c r="G40" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H40" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
       </c>
       <c r="I40" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -38735,7 +38820,7 @@
       </c>
       <c r="R40" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="41" spans="1:18">
@@ -38744,31 +38829,31 @@
       </c>
       <c r="B41" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C41" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '26', </v>
       </c>
       <c r="D41" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Form Layout', </v>
       </c>
       <c r="E41" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Layout details', </v>
       </c>
       <c r="F41" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Layout', </v>
       </c>
       <c r="G41" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H41" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '27', </v>
       </c>
       <c r="I41" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -38808,7 +38893,7 @@
       </c>
       <c r="R41" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="42" spans="1:18">
@@ -38817,31 +38902,31 @@
       </c>
       <c r="B42" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C42" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '23', </v>
       </c>
       <c r="D42" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Data View Section', </v>
       </c>
       <c r="E42" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Section details of data view', </v>
       </c>
       <c r="F42" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Sections', </v>
       </c>
       <c r="G42" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H42" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '28', </v>
       </c>
       <c r="I42" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -38881,7 +38966,7 @@
       </c>
       <c r="R42" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="43" spans="1:18">
@@ -38890,31 +38975,31 @@
       </c>
       <c r="B43" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C43" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '26', </v>
       </c>
       <c r="D43" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Data View Section Items', </v>
       </c>
       <c r="E43" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Items of a data view section', </v>
       </c>
       <c r="F43" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Items', </v>
       </c>
       <c r="G43" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H43" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '29', </v>
       </c>
       <c r="I43" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -38954,7 +39039,7 @@
       </c>
       <c r="R43" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="44" spans="1:18">
@@ -38963,31 +39048,31 @@
       </c>
       <c r="B44" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C44" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '28', </v>
       </c>
       <c r="D44" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Data Relation', </v>
       </c>
       <c r="E44" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'View relation of a data', </v>
       </c>
       <c r="F44" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
       </c>
       <c r="G44" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H44" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
       </c>
       <c r="I44" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -39027,7 +39112,7 @@
       </c>
       <c r="R44" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="45" spans="1:18">
@@ -39036,31 +39121,31 @@
       </c>
       <c r="B45" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C45" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '29', </v>
       </c>
       <c r="D45" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Data item relation', </v>
       </c>
       <c r="E45" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'View relation of a data item', </v>
       </c>
       <c r="F45" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
       </c>
       <c r="G45" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H45" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
       </c>
       <c r="I45" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -39100,7 +39185,7 @@
       </c>
       <c r="R45" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="46" spans="1:18">
@@ -39109,31 +39194,31 @@
       </c>
       <c r="B46" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C46" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '26', </v>
       </c>
       <c r="D46" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Owner Relation', </v>
       </c>
       <c r="E46" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'View the owner resource', </v>
       </c>
       <c r="F46" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Owner', </v>
       </c>
       <c r="G46" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H46" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
       </c>
       <c r="I46" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -39173,7 +39258,7 @@
       </c>
       <c r="R46" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="47" spans="1:18">
@@ -39182,7 +39267,7 @@
       </c>
       <c r="B47" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>;</v>
       </c>
       <c r="C47" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -39255,7 +39340,7 @@
       </c>
       <c r="B48" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
       </c>
       <c r="C48" s="33" t="str">
         <f t="shared" ca="1" si="3"/>

</xml_diff>

<commit_message>
New Table, Resource Form Collection added
</commit_message>
<xml_diff>
--- a/Helper.xlsx
+++ b/Helper.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Tables" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3120" uniqueCount="650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3148" uniqueCount="653">
   <si>
     <t>resource_scopes</t>
   </si>
@@ -1988,6 +1988,15 @@
   </si>
   <si>
     <t>resource_list_nullable_foreign</t>
+  </si>
+  <si>
+    <t>resource_form_collection</t>
+  </si>
+  <si>
+    <t>resource_form_collection_foreign</t>
+  </si>
+  <si>
+    <t>collection_form</t>
   </si>
 </sst>
 </file>
@@ -2217,127 +2226,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="130">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="125">
     <dxf>
       <font>
         <condense val="0"/>
@@ -3891,6 +3780,66 @@
     </dxf>
     <dxf>
       <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -4075,35 +4024,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tables" displayName="Tables" ref="A1:J35" totalsRowShown="0" dataDxfId="129">
-  <autoFilter ref="A1:J35"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tables" displayName="Tables" ref="A1:J36" totalsRowShown="0" dataDxfId="124">
+  <autoFilter ref="A1:J36"/>
   <tableColumns count="10">
-    <tableColumn id="2" name="Name" dataDxfId="128"/>
-    <tableColumn id="10" name="Table" dataDxfId="127">
+    <tableColumn id="2" name="Name" dataDxfId="123"/>
+    <tableColumn id="10" name="Table" dataDxfId="122">
       <calculatedColumnFormula>"__"&amp;[Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Singular Name" dataDxfId="126">
+    <tableColumn id="5" name="Singular Name" dataDxfId="121">
       <calculatedColumnFormula>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Model NS" dataDxfId="125">
+    <tableColumn id="8" name="Model NS" dataDxfId="120">
       <calculatedColumnFormula>"Milestone\Appframe\Model"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Class Name" dataDxfId="124">
+    <tableColumn id="4" name="Class Name" dataDxfId="119">
       <calculatedColumnFormula>SUBSTITUTE(PROPER([Singular Name]),"_","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Migration Artisan" dataDxfId="123">
+    <tableColumn id="1" name="Migration Artisan" dataDxfId="118">
       <calculatedColumnFormula>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Model Artisan" dataDxfId="122">
+    <tableColumn id="6" name="Model Artisan" dataDxfId="117">
       <calculatedColumnFormula>"php artisan make:model "&amp;[Class Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Model Statement" dataDxfId="121">
+    <tableColumn id="3" name="Model Statement" dataDxfId="116">
       <calculatedColumnFormula>"protected $table = '"&amp;[Table]&amp;"';"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Seeder Artisan" dataDxfId="120">
+    <tableColumn id="7" name="Seeder Artisan" dataDxfId="115">
       <calculatedColumnFormula>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Seeder Class" dataDxfId="119">
+    <tableColumn id="9" name="Seeder Class" dataDxfId="114">
       <calculatedColumnFormula>[Class Name]&amp;"TableSeeder"&amp;"::class,"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4112,87 +4061,87 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="ResourceActions" displayName="ResourceActions" ref="A1:P9" totalsRowShown="0" dataDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="ResourceActions" displayName="ResourceActions" ref="A1:P9" totalsRowShown="0" dataDxfId="19">
   <autoFilter ref="A1:P9"/>
   <tableColumns count="16">
-    <tableColumn id="1" name="No" dataDxfId="28">
+    <tableColumn id="1" name="No" dataDxfId="18">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Resource" dataDxfId="27"/>
-    <tableColumn id="13" name="Resource Id" dataDxfId="26">
+    <tableColumn id="2" name="Resource" dataDxfId="17"/>
+    <tableColumn id="13" name="Resource Id" dataDxfId="16">
       <calculatedColumnFormula>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Action Name" dataDxfId="25"/>
-    <tableColumn id="4" name="Description" dataDxfId="24"/>
-    <tableColumn id="5" name="Action Title" dataDxfId="23"/>
-    <tableColumn id="6" name="Button Type" dataDxfId="22"/>
-    <tableColumn id="7" name="Menu" dataDxfId="21"/>
-    <tableColumn id="8" name="Icon" dataDxfId="20"/>
-    <tableColumn id="9" name="Set" dataDxfId="19"/>
-    <tableColumn id="14" name="Action Type" dataDxfId="18"/>
-    <tableColumn id="15" name="ID1" dataDxfId="17"/>
-    <tableColumn id="16" name="ID2" dataDxfId="16"/>
-    <tableColumn id="10" name="On" dataDxfId="15"/>
-    <tableColumn id="11" name="Confirm" dataDxfId="14"/>
-    <tableColumn id="12" name="handler" dataDxfId="13"/>
+    <tableColumn id="3" name="Action Name" dataDxfId="15"/>
+    <tableColumn id="4" name="Description" dataDxfId="14"/>
+    <tableColumn id="5" name="Action Title" dataDxfId="13"/>
+    <tableColumn id="6" name="Button Type" dataDxfId="12"/>
+    <tableColumn id="7" name="Menu" dataDxfId="11"/>
+    <tableColumn id="8" name="Icon" dataDxfId="10"/>
+    <tableColumn id="9" name="Set" dataDxfId="9"/>
+    <tableColumn id="14" name="Action Type" dataDxfId="8"/>
+    <tableColumn id="15" name="ID1" dataDxfId="7"/>
+    <tableColumn id="16" name="ID2" dataDxfId="6"/>
+    <tableColumn id="10" name="On" dataDxfId="5"/>
+    <tableColumn id="11" name="Confirm" dataDxfId="4"/>
+    <tableColumn id="12" name="handler" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Columns" displayName="Columns" ref="A1:I129" totalsRowShown="0" dataDxfId="118">
-  <autoFilter ref="A1:I129">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Columns" displayName="Columns" ref="A1:I131" totalsRowShown="0" dataDxfId="108">
+  <autoFilter ref="A1:I131">
     <filterColumn colId="0"/>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" name="Column" dataDxfId="117"/>
-    <tableColumn id="2" name="Type" dataDxfId="116"/>
-    <tableColumn id="3" name="Name" dataDxfId="115"/>
-    <tableColumn id="4" name="Length" dataDxfId="114"/>
-    <tableColumn id="5" name="Method1" dataDxfId="113"/>
-    <tableColumn id="6" name="Method2" dataDxfId="112"/>
-    <tableColumn id="7" name="Method3" dataDxfId="111"/>
-    <tableColumn id="8" name="Method4" dataDxfId="110"/>
-    <tableColumn id="9" name="Method5" dataDxfId="109"/>
+    <tableColumn id="1" name="Column" dataDxfId="107"/>
+    <tableColumn id="2" name="Type" dataDxfId="106"/>
+    <tableColumn id="3" name="Name" dataDxfId="105"/>
+    <tableColumn id="4" name="Length" dataDxfId="104"/>
+    <tableColumn id="5" name="Method1" dataDxfId="103"/>
+    <tableColumn id="6" name="Method2" dataDxfId="102"/>
+    <tableColumn id="7" name="Method3" dataDxfId="101"/>
+    <tableColumn id="8" name="Method4" dataDxfId="100"/>
+    <tableColumn id="9" name="Method5" dataDxfId="99"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TableFields" displayName="TableFields" ref="A1:K302" totalsRowShown="0" dataDxfId="108">
-  <autoFilter ref="A1:K302">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TableFields" displayName="TableFields" ref="A1:K310" totalsRowShown="0" dataDxfId="98">
+  <autoFilter ref="A1:K310">
     <filterColumn colId="0"/>
   </autoFilter>
   <tableColumns count="11">
-    <tableColumn id="2" name="Table" dataDxfId="107"/>
-    <tableColumn id="3" name="Field" dataDxfId="106"/>
-    <tableColumn id="5" name="Type" dataDxfId="105">
+    <tableColumn id="2" name="Table" dataDxfId="97"/>
+    <tableColumn id="3" name="Field" dataDxfId="96"/>
+    <tableColumn id="5" name="Type" dataDxfId="95">
       <calculatedColumnFormula>VLOOKUP([Field],Columns[],2,0)&amp;"("</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Name" dataDxfId="104">
+    <tableColumn id="4" name="Name" dataDxfId="94">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Arg2" dataDxfId="103">
+    <tableColumn id="6" name="Arg2" dataDxfId="93">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Method1" dataDxfId="102">
+    <tableColumn id="7" name="Method1" dataDxfId="92">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Method2" dataDxfId="101">
+    <tableColumn id="8" name="Method2" dataDxfId="91">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Method3" dataDxfId="100">
+    <tableColumn id="9" name="Method3" dataDxfId="90">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Method4" dataDxfId="99">
+    <tableColumn id="10" name="Method4" dataDxfId="89">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Method5" dataDxfId="98">
+    <tableColumn id="11" name="Method5" dataDxfId="88">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Statement" dataDxfId="97">
+    <tableColumn id="12" name="Statement" dataDxfId="87">
       <calculatedColumnFormula>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4201,7 +4150,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R271" totalsRowShown="0" headerRowDxfId="96" dataDxfId="95">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R271" totalsRowShown="0" headerRowDxfId="86" dataDxfId="85">
   <autoFilter ref="A1:R271">
     <filterColumn colId="1">
       <filters>
@@ -4210,46 +4159,46 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="18">
-    <tableColumn id="19" name="TRCode" dataDxfId="94">
+    <tableColumn id="19" name="TRCode" dataDxfId="84">
       <calculatedColumnFormula>[Table Name]&amp;"-"&amp;[Record No]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Table Name" dataDxfId="93"/>
-    <tableColumn id="2" name="Record No" dataDxfId="92">
+    <tableColumn id="1" name="Table Name" dataDxfId="83"/>
+    <tableColumn id="2" name="Record No" dataDxfId="82">
       <calculatedColumnFormula>COUNTIF($B$1:$B1,[Table Name])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="1" dataDxfId="91"/>
-    <tableColumn id="4" name="2" dataDxfId="90"/>
-    <tableColumn id="5" name="3" dataDxfId="89"/>
-    <tableColumn id="6" name="4" dataDxfId="88"/>
-    <tableColumn id="7" name="5" dataDxfId="87"/>
-    <tableColumn id="8" name="6" dataDxfId="86"/>
-    <tableColumn id="9" name="7" dataDxfId="85"/>
-    <tableColumn id="10" name="8" dataDxfId="84"/>
-    <tableColumn id="11" name="9" dataDxfId="83"/>
-    <tableColumn id="12" name="10" dataDxfId="82"/>
-    <tableColumn id="13" name="11" dataDxfId="81"/>
-    <tableColumn id="14" name="12" dataDxfId="80"/>
-    <tableColumn id="15" name="13" dataDxfId="79"/>
-    <tableColumn id="16" name="14" dataDxfId="78"/>
-    <tableColumn id="17" name="15" dataDxfId="77"/>
+    <tableColumn id="3" name="1" dataDxfId="81"/>
+    <tableColumn id="4" name="2" dataDxfId="80"/>
+    <tableColumn id="5" name="3" dataDxfId="79"/>
+    <tableColumn id="6" name="4" dataDxfId="78"/>
+    <tableColumn id="7" name="5" dataDxfId="77"/>
+    <tableColumn id="8" name="6" dataDxfId="76"/>
+    <tableColumn id="9" name="7" dataDxfId="75"/>
+    <tableColumn id="10" name="8" dataDxfId="74"/>
+    <tableColumn id="11" name="9" dataDxfId="73"/>
+    <tableColumn id="12" name="10" dataDxfId="72"/>
+    <tableColumn id="13" name="11" dataDxfId="71"/>
+    <tableColumn id="14" name="12" dataDxfId="70"/>
+    <tableColumn id="15" name="13" dataDxfId="69"/>
+    <tableColumn id="16" name="14" dataDxfId="68"/>
+    <tableColumn id="17" name="15" dataDxfId="67"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SeedMap" displayName="SeedMap" ref="A1:E26" totalsRowShown="0" dataDxfId="76">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SeedMap" displayName="SeedMap" ref="A1:E26" totalsRowShown="0" dataDxfId="66">
   <autoFilter ref="A1:E26"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Name" dataDxfId="75"/>
-    <tableColumn id="3" name="FW Table Name" dataDxfId="74"/>
-    <tableColumn id="20" name="NS" dataDxfId="73">
+    <tableColumn id="1" name="Name" dataDxfId="65"/>
+    <tableColumn id="3" name="FW Table Name" dataDxfId="64"/>
+    <tableColumn id="20" name="NS" dataDxfId="63">
       <calculatedColumnFormula>VLOOKUP([FW Table Name],Tables[],4,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="Model" dataDxfId="72">
+    <tableColumn id="21" name="Model" dataDxfId="62">
       <calculatedColumnFormula>VLOOKUP([FW Table Name],Tables[],5,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Query Method" dataDxfId="71">
+    <tableColumn id="4" name="Query Method" dataDxfId="61">
       <calculatedColumnFormula>"truncate"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4258,46 +4207,46 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="ResourceTable" displayName="ResourceTable" ref="A1:I30" totalsRowShown="0" dataDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="ResourceTable" displayName="ResourceTable" ref="A1:I30" totalsRowShown="0" dataDxfId="60">
   <autoFilter ref="A1:I30"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="No" dataDxfId="69">
+    <tableColumn id="1" name="No" dataDxfId="59">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Name" dataDxfId="68"/>
-    <tableColumn id="3" name="Description" dataDxfId="67"/>
-    <tableColumn id="4" name="Title" dataDxfId="66"/>
-    <tableColumn id="5" name="NS" dataDxfId="65">
+    <tableColumn id="2" name="Name" dataDxfId="58"/>
+    <tableColumn id="3" name="Description" dataDxfId="57"/>
+    <tableColumn id="4" name="Title" dataDxfId="56"/>
+    <tableColumn id="5" name="NS" dataDxfId="55">
       <calculatedColumnFormula>"Milestone\Appframe\Model"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Table" dataDxfId="64"/>
-    <tableColumn id="7" name="Key" dataDxfId="63">
+    <tableColumn id="6" name="Table" dataDxfId="54"/>
+    <tableColumn id="7" name="Key" dataDxfId="53">
       <calculatedColumnFormula>"id"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Controller" dataDxfId="62"/>
-    <tableColumn id="9" name="Controller NS" dataDxfId="61"/>
+    <tableColumn id="8" name="Controller" dataDxfId="52"/>
+    <tableColumn id="9" name="Controller NS" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RelationTable" displayName="RelationTable" ref="A1:I39" totalsRowShown="0" dataDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RelationTable" displayName="RelationTable" ref="A1:I39" totalsRowShown="0" dataDxfId="50">
   <autoFilter ref="A1:I39"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="No" dataDxfId="59">
+    <tableColumn id="1" name="No" dataDxfId="49">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Resource" dataDxfId="58"/>
-    <tableColumn id="4" name="Relate Resource" dataDxfId="57"/>
-    <tableColumn id="2" name="Resource Id" dataDxfId="56">
+    <tableColumn id="3" name="Resource" dataDxfId="48"/>
+    <tableColumn id="4" name="Relate Resource" dataDxfId="47"/>
+    <tableColumn id="2" name="Resource Id" dataDxfId="46">
       <calculatedColumnFormula>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Name" dataDxfId="55"/>
-    <tableColumn id="6" name="Description" dataDxfId="54"/>
-    <tableColumn id="7" name="Method" dataDxfId="53"/>
-    <tableColumn id="8" name="Type" dataDxfId="52"/>
-    <tableColumn id="10" name="Relate Id" dataDxfId="51">
+    <tableColumn id="5" name="Name" dataDxfId="45"/>
+    <tableColumn id="6" name="Description" dataDxfId="44"/>
+    <tableColumn id="7" name="Method" dataDxfId="43"/>
+    <tableColumn id="8" name="Type" dataDxfId="42"/>
+    <tableColumn id="10" name="Relate Id" dataDxfId="41">
       <calculatedColumnFormula>VLOOKUP([Relate Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4306,47 +4255,47 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="ResourceForms" displayName="ResourceForms" ref="A1:G9" totalsRowShown="0" dataDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="ResourceForms" displayName="ResourceForms" ref="A1:G9" totalsRowShown="0" dataDxfId="40">
   <autoFilter ref="A1:G9"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="No" dataDxfId="49">
+    <tableColumn id="1" name="No" dataDxfId="39">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Resource ID" dataDxfId="48"/>
-    <tableColumn id="3" name="Resource Name" dataDxfId="47">
+    <tableColumn id="2" name="Resource ID" dataDxfId="38"/>
+    <tableColumn id="3" name="Resource Name" dataDxfId="37">
       <calculatedColumnFormula>VLOOKUP([Resource ID],ResourceTable[],2,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Form Name" dataDxfId="46"/>
-    <tableColumn id="6" name="Title" dataDxfId="45"/>
-    <tableColumn id="7" name="Action Text" dataDxfId="44"/>
-    <tableColumn id="8" name="Description" dataDxfId="43"/>
+    <tableColumn id="4" name="Form Name" dataDxfId="36"/>
+    <tableColumn id="6" name="Title" dataDxfId="35"/>
+    <tableColumn id="7" name="Action Text" dataDxfId="34"/>
+    <tableColumn id="8" name="Description" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="FormFields" displayName="FormFields" ref="A1:L33" totalsRowShown="0" dataDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="FormFields" displayName="FormFields" ref="A1:L33" totalsRowShown="0" dataDxfId="32">
   <autoFilter ref="A1:L33"/>
   <tableColumns count="12">
-    <tableColumn id="9" name="No" dataDxfId="41">
+    <tableColumn id="9" name="No" dataDxfId="31">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Form Id" dataDxfId="40"/>
-    <tableColumn id="7" name="Form Name" dataDxfId="39">
+    <tableColumn id="1" name="Form Id" dataDxfId="30"/>
+    <tableColumn id="7" name="Form Name" dataDxfId="29">
       <calculatedColumnFormula>VLOOKUP([Form Id],ResourceForms[],4,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Name" dataDxfId="38"/>
-    <tableColumn id="2" name="Type" dataDxfId="37"/>
-    <tableColumn id="5" name="Label" dataDxfId="36"/>
-    <tableColumn id="6" name="Collection" dataDxfId="35"/>
-    <tableColumn id="14" name="Attribute" dataDxfId="34">
+    <tableColumn id="4" name="Name" dataDxfId="28"/>
+    <tableColumn id="2" name="Type" dataDxfId="27"/>
+    <tableColumn id="5" name="Label" dataDxfId="26"/>
+    <tableColumn id="6" name="Collection" dataDxfId="25"/>
+    <tableColumn id="14" name="Attribute" dataDxfId="24">
       <calculatedColumnFormula>[Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Relation" dataDxfId="33"/>
-    <tableColumn id="11" name="Deep 1" dataDxfId="32"/>
-    <tableColumn id="12" name="Deep 2" dataDxfId="31"/>
-    <tableColumn id="13" name="Deep 3" dataDxfId="30"/>
+    <tableColumn id="10" name="Relation" dataDxfId="23"/>
+    <tableColumn id="11" name="Deep 1" dataDxfId="22"/>
+    <tableColumn id="12" name="Deep 2" dataDxfId="21"/>
+    <tableColumn id="13" name="Deep 3" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4637,10 +4586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView topLeftCell="E8" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4700,7 +4649,7 @@
         <v>user</v>
       </c>
       <c r="D2" s="8" t="str">
-        <f t="shared" ref="D2:D35" si="0">"Milestone\Appframe\Model"</f>
+        <f t="shared" ref="D2:D36" si="0">"Milestone\Appframe\Model"</f>
         <v>Milestone\Appframe\Model</v>
       </c>
       <c r="E2" s="8" t="str">
@@ -6001,56 +5950,56 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="B34" s="7" t="str">
+        <f>"__"&amp;[Name]</f>
+        <v>__resource_form_collection</v>
+      </c>
+      <c r="C34" s="7" t="str">
+        <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
+        <v>resource_form_collection</v>
+      </c>
+      <c r="D34" s="7" t="str">
+        <f>"Milestone\Appframe\Model"</f>
+        <v>Milestone\Appframe\Model</v>
+      </c>
+      <c r="E34" s="8" t="str">
+        <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
+        <v>ResourceFormCollection</v>
+      </c>
+      <c r="F34" s="8" t="str">
+        <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
+        <v>php artisan make:migration create___resource_form_collection_table --create=__resource_form_collection</v>
+      </c>
+      <c r="G34" s="8" t="str">
+        <f>"php artisan make:model "&amp;[Class Name]</f>
+        <v>php artisan make:model ResourceFormCollection</v>
+      </c>
+      <c r="H34" s="8" t="str">
+        <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
+        <v>protected $table = '__resource_form_collection';</v>
+      </c>
+      <c r="I34" s="8" t="str">
+        <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
+        <v>php artisan make:seed ResourceFormCollectionTableSeeder</v>
+      </c>
+      <c r="J34" s="8" t="str">
+        <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
+        <v>ResourceFormCollectionTableSeeder::class,</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B34" s="9" t="str">
+      <c r="B35" s="9" t="str">
         <f>"__"&amp;[Name]</f>
         <v>__organisation</v>
       </c>
-      <c r="C34" s="9" t="str">
+      <c r="C35" s="9" t="str">
         <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
         <v>organisation</v>
-      </c>
-      <c r="D34" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Milestone\Appframe\Model</v>
-      </c>
-      <c r="E34" s="9" t="str">
-        <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
-        <v>Organisation</v>
-      </c>
-      <c r="F34" s="9" t="str">
-        <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
-        <v>php artisan make:migration create___organisation_table --create=__organisation</v>
-      </c>
-      <c r="G34" s="9" t="str">
-        <f>"php artisan make:model "&amp;[Class Name]</f>
-        <v>php artisan make:model Organisation</v>
-      </c>
-      <c r="H34" s="9" t="str">
-        <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
-        <v>protected $table = '__organisation';</v>
-      </c>
-      <c r="I34" s="9" t="str">
-        <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
-        <v>php artisan make:seed OrganisationTableSeeder</v>
-      </c>
-      <c r="J34" s="9" t="str">
-        <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
-        <v>OrganisationTableSeeder::class,</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10">
-      <c r="A35" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="B35" s="9" t="str">
-        <f>"__"&amp;[Name]</f>
-        <v>__organisation_contacts</v>
-      </c>
-      <c r="C35" s="9" t="str">
-        <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
-        <v>organisation_contact</v>
       </c>
       <c r="D35" s="9" t="str">
         <f t="shared" si="0"/>
@@ -6058,25 +6007,66 @@
       </c>
       <c r="E35" s="9" t="str">
         <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
-        <v>OrganisationContact</v>
+        <v>Organisation</v>
       </c>
       <c r="F35" s="9" t="str">
         <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
-        <v>php artisan make:migration create___organisation_contacts_table --create=__organisation_contacts</v>
+        <v>php artisan make:migration create___organisation_table --create=__organisation</v>
       </c>
       <c r="G35" s="9" t="str">
         <f>"php artisan make:model "&amp;[Class Name]</f>
-        <v>php artisan make:model OrganisationContact</v>
+        <v>php artisan make:model Organisation</v>
       </c>
       <c r="H35" s="9" t="str">
         <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
-        <v>protected $table = '__organisation_contacts';</v>
+        <v>protected $table = '__organisation';</v>
       </c>
       <c r="I35" s="9" t="str">
         <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
+        <v>php artisan make:seed OrganisationTableSeeder</v>
+      </c>
+      <c r="J35" s="9" t="str">
+        <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
+        <v>OrganisationTableSeeder::class,</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B36" s="9" t="str">
+        <f>"__"&amp;[Name]</f>
+        <v>__organisation_contacts</v>
+      </c>
+      <c r="C36" s="9" t="str">
+        <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
+        <v>organisation_contact</v>
+      </c>
+      <c r="D36" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>Milestone\Appframe\Model</v>
+      </c>
+      <c r="E36" s="9" t="str">
+        <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
+        <v>OrganisationContact</v>
+      </c>
+      <c r="F36" s="9" t="str">
+        <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
+        <v>php artisan make:migration create___organisation_contacts_table --create=__organisation_contacts</v>
+      </c>
+      <c r="G36" s="9" t="str">
+        <f>"php artisan make:model "&amp;[Class Name]</f>
+        <v>php artisan make:model OrganisationContact</v>
+      </c>
+      <c r="H36" s="9" t="str">
+        <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
+        <v>protected $table = '__organisation_contacts';</v>
+      </c>
+      <c r="I36" s="9" t="str">
+        <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
         <v>php artisan make:seed OrganisationContactTableSeeder</v>
       </c>
-      <c r="J35" s="9" t="str">
+      <c r="J36" s="9" t="str">
         <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
         <v>OrganisationContactTableSeeder::class,</v>
       </c>
@@ -7662,10 +7652,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I129"/>
+  <dimension ref="A1:I131"/>
   <sheetViews>
-    <sheetView topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="E105" sqref="E105"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A130" sqref="A130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="15"/>
@@ -10471,21 +10461,68 @@
       </c>
       <c r="I129" s="4"/>
     </row>
+    <row r="130" spans="1:9">
+      <c r="A130" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="B130" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C130" s="5" t="s">
+        <v>652</v>
+      </c>
+      <c r="D130" s="5"/>
+      <c r="E130" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F130" s="5"/>
+      <c r="G130" s="5"/>
+      <c r="H130" s="5"/>
+      <c r="I130" s="5"/>
+    </row>
+    <row r="131" spans="1:9">
+      <c r="A131" s="4" t="s">
+        <v>651</v>
+      </c>
+      <c r="B131" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C131" s="4" t="s">
+        <v>652</v>
+      </c>
+      <c r="D131" s="4"/>
+      <c r="E131" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F131" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G131" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H131" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I131" s="4"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A43:A46">
-    <cfRule type="duplicateValues" dxfId="12" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="113" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56:A59">
-    <cfRule type="duplicateValues" dxfId="11" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="112" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A129">
-    <cfRule type="duplicateValues" dxfId="10" priority="23"/>
+  <conditionalFormatting sqref="A2:A131">
+    <cfRule type="duplicateValues" dxfId="111" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A128:A129">
-    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="110" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A128:A129">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="109" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A130:A131">
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -10497,10 +10534,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K302"/>
+  <dimension ref="A1:K310"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A288" workbookViewId="0">
+      <selection activeCell="K304" sqref="K304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="15"/>
@@ -23790,13 +23827,365 @@
         <v>$table-&gt;foreign('relation')-&gt;references('id')-&gt;on('__resource_relations')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
       </c>
     </row>
+    <row r="303" spans="1:11">
+      <c r="A303" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="B303" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C303" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>increments(</v>
+      </c>
+      <c r="D303" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'id'</v>
+      </c>
+      <c r="E303" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>)</v>
+      </c>
+      <c r="F303" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v/>
+      </c>
+      <c r="G303" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v/>
+      </c>
+      <c r="H303" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v/>
+      </c>
+      <c r="I303" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v/>
+      </c>
+      <c r="J303" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K303" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;increments('id');</v>
+      </c>
+    </row>
+    <row r="304" spans="1:11">
+      <c r="A304" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="B304" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C304" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>unsignedInteger(</v>
+      </c>
+      <c r="D304" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'resource_form'</v>
+      </c>
+      <c r="E304" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>)</v>
+      </c>
+      <c r="F304" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>-&gt;index()</v>
+      </c>
+      <c r="G304" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v/>
+      </c>
+      <c r="H304" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v/>
+      </c>
+      <c r="I304" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v/>
+      </c>
+      <c r="J304" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K304" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;unsignedInteger('resource_form')-&gt;index();</v>
+      </c>
+    </row>
+    <row r="305" spans="1:11">
+      <c r="A305" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="B305" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="C305" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>unsignedInteger(</v>
+      </c>
+      <c r="D305" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'collection_form'</v>
+      </c>
+      <c r="E305" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>)</v>
+      </c>
+      <c r="F305" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>-&gt;index()</v>
+      </c>
+      <c r="G305" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v/>
+      </c>
+      <c r="H305" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v/>
+      </c>
+      <c r="I305" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v/>
+      </c>
+      <c r="J305" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K305" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;unsignedInteger('collection_form')-&gt;index();</v>
+      </c>
+    </row>
+    <row r="306" spans="1:11">
+      <c r="A306" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="B306" s="4" t="s">
+        <v>575</v>
+      </c>
+      <c r="C306" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>unsignedInteger(</v>
+      </c>
+      <c r="D306" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'relation'</v>
+      </c>
+      <c r="E306" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>)</v>
+      </c>
+      <c r="F306" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>-&gt;index()</v>
+      </c>
+      <c r="G306" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v>-&gt;nullable()</v>
+      </c>
+      <c r="H306" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v/>
+      </c>
+      <c r="I306" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v/>
+      </c>
+      <c r="J306" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K306" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;unsignedInteger('relation')-&gt;index()-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="307" spans="1:11">
+      <c r="A307" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="B307" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C307" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>timestamps(</v>
+      </c>
+      <c r="D307" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v/>
+      </c>
+      <c r="E307" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>)</v>
+      </c>
+      <c r="F307" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v/>
+      </c>
+      <c r="G307" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v/>
+      </c>
+      <c r="H307" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v/>
+      </c>
+      <c r="I307" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v/>
+      </c>
+      <c r="J307" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K307" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;timestamps();</v>
+      </c>
+    </row>
+    <row r="308" spans="1:11">
+      <c r="A308" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="B308" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C308" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>foreign(</v>
+      </c>
+      <c r="D308" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'resource_form'</v>
+      </c>
+      <c r="E308" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>)</v>
+      </c>
+      <c r="F308" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>-&gt;references('id')</v>
+      </c>
+      <c r="G308" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v>-&gt;on('__resource_forms')</v>
+      </c>
+      <c r="H308" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v>-&gt;onUpdate('cascade')</v>
+      </c>
+      <c r="I308" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v>-&gt;onDelete('cascade')</v>
+      </c>
+      <c r="J308" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K308" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;foreign('resource_form')-&gt;references('id')-&gt;on('__resource_forms')-&gt;onUpdate('cascade')-&gt;onDelete('cascade');</v>
+      </c>
+    </row>
+    <row r="309" spans="1:11">
+      <c r="A309" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="B309" s="4" t="s">
+        <v>651</v>
+      </c>
+      <c r="C309" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>foreign(</v>
+      </c>
+      <c r="D309" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'collection_form'</v>
+      </c>
+      <c r="E309" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>)</v>
+      </c>
+      <c r="F309" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>-&gt;references('id')</v>
+      </c>
+      <c r="G309" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v>-&gt;on('__resource_forms')</v>
+      </c>
+      <c r="H309" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v>-&gt;onUpdate('cascade')</v>
+      </c>
+      <c r="I309" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v>-&gt;onDelete('cascade')</v>
+      </c>
+      <c r="J309" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K309" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;foreign('collection_form')-&gt;references('id')-&gt;on('__resource_forms')-&gt;onUpdate('cascade')-&gt;onDelete('cascade');</v>
+      </c>
+    </row>
+    <row r="310" spans="1:11">
+      <c r="A310" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="B310" s="4" t="s">
+        <v>576</v>
+      </c>
+      <c r="C310" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>foreign(</v>
+      </c>
+      <c r="D310" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'relation'</v>
+      </c>
+      <c r="E310" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>)</v>
+      </c>
+      <c r="F310" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>-&gt;references('id')</v>
+      </c>
+      <c r="G310" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v>-&gt;on('__resource_relations')</v>
+      </c>
+      <c r="H310" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v>-&gt;onUpdate('cascade')</v>
+      </c>
+      <c r="I310" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v>-&gt;onDelete('set null')</v>
+      </c>
+      <c r="J310" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K310" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;foreign('relation')-&gt;references('id')-&gt;on('__resource_relations')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B302">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B310">
       <formula1>AvailableFields</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A302">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A310">
       <formula1>TableNames</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Collection to Form relation added
</commit_message>
<xml_diff>
--- a/Helper.xlsx
+++ b/Helper.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3170" uniqueCount="659">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3183" uniqueCount="660">
   <si>
     <t>resource_scopes</t>
   </si>
@@ -2015,6 +2015,9 @@
   </si>
   <si>
     <t>Collection/Detail form</t>
+  </si>
+  <si>
+    <t>Form Collection</t>
   </si>
 </sst>
 </file>
@@ -4144,11 +4147,11 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R273" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
-  <autoFilter ref="A1:R273">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R274" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
+  <autoFilter ref="A1:R274">
     <filterColumn colId="1">
       <filters>
-        <filter val="Resources"/>
+        <filter val="Resource Relations"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -4181,8 +4184,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SeedMap" displayName="SeedMap" ref="A1:E26" totalsRowShown="0" dataDxfId="63">
-  <autoFilter ref="A1:E26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SeedMap" displayName="SeedMap" ref="A1:E27" totalsRowShown="0" dataDxfId="63">
+  <autoFilter ref="A1:E27"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Name" dataDxfId="62"/>
     <tableColumn id="3" name="FW Table Name" dataDxfId="61"/>
@@ -4225,8 +4228,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RelationTable" displayName="RelationTable" ref="A1:I40" totalsRowShown="0" dataDxfId="47">
-  <autoFilter ref="A1:I40"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RelationTable" displayName="RelationTable" ref="A1:I41" totalsRowShown="0" dataDxfId="47">
+  <autoFilter ref="A1:I41"/>
   <tableColumns count="9">
     <tableColumn id="1" name="No" dataDxfId="46">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
@@ -24193,10 +24196,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R273"/>
+  <dimension ref="A1:R274"/>
   <sheetViews>
-    <sheetView topLeftCell="B167" workbookViewId="0">
-      <selection activeCell="G272" sqref="G272"/>
+    <sheetView topLeftCell="B213" workbookViewId="0">
+      <selection activeCell="B274" sqref="B274"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -24663,7 +24666,7 @@
       <c r="Q13" s="16"/>
       <c r="R13" s="16"/>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" hidden="1">
       <c r="A14" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-0</v>
@@ -24707,7 +24710,7 @@
       <c r="Q14" s="16"/>
       <c r="R14" s="16"/>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" hidden="1">
       <c r="A15" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-1</v>
@@ -24747,7 +24750,7 @@
       <c r="Q15" s="15"/>
       <c r="R15" s="15"/>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" hidden="1">
       <c r="A16" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-2</v>
@@ -24787,7 +24790,7 @@
       <c r="Q16" s="15"/>
       <c r="R16" s="15"/>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" hidden="1">
       <c r="A17" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-3</v>
@@ -24827,7 +24830,7 @@
       <c r="Q17" s="15"/>
       <c r="R17" s="15"/>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" hidden="1">
       <c r="A18" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-4</v>
@@ -24867,7 +24870,7 @@
       <c r="Q18" s="15"/>
       <c r="R18" s="15"/>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" hidden="1">
       <c r="A19" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-5</v>
@@ -24907,7 +24910,7 @@
       <c r="Q19" s="15"/>
       <c r="R19" s="15"/>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" hidden="1">
       <c r="A20" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-6</v>
@@ -24947,7 +24950,7 @@
       <c r="Q20" s="15"/>
       <c r="R20" s="15"/>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" hidden="1">
       <c r="A21" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-7</v>
@@ -24987,7 +24990,7 @@
       <c r="Q21" s="15"/>
       <c r="R21" s="15"/>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" hidden="1">
       <c r="A22" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-8</v>
@@ -25027,7 +25030,7 @@
       <c r="Q22" s="15"/>
       <c r="R22" s="15"/>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" hidden="1">
       <c r="A23" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-9</v>
@@ -25067,7 +25070,7 @@
       <c r="Q23" s="15"/>
       <c r="R23" s="15"/>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" hidden="1">
       <c r="A24" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-10</v>
@@ -25107,7 +25110,7 @@
       <c r="Q24" s="15"/>
       <c r="R24" s="15"/>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" hidden="1">
       <c r="A25" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-11</v>
@@ -25147,7 +25150,7 @@
       <c r="Q25" s="15"/>
       <c r="R25" s="15"/>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:18" hidden="1">
       <c r="A26" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-12</v>
@@ -25187,7 +25190,7 @@
       <c r="Q26" s="15"/>
       <c r="R26" s="15"/>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:18" hidden="1">
       <c r="A27" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-13</v>
@@ -25491,7 +25494,7 @@
       <c r="Q35" s="16"/>
       <c r="R35" s="16"/>
     </row>
-    <row r="36" spans="1:18" hidden="1">
+    <row r="36" spans="1:18">
       <c r="A36" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-0</v>
@@ -25531,7 +25534,7 @@
       <c r="Q36" s="16"/>
       <c r="R36" s="16"/>
     </row>
-    <row r="37" spans="1:18" hidden="1">
+    <row r="37" spans="1:18">
       <c r="A37" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-1</v>
@@ -25571,7 +25574,7 @@
       <c r="Q37" s="15"/>
       <c r="R37" s="15"/>
     </row>
-    <row r="38" spans="1:18" hidden="1">
+    <row r="38" spans="1:18">
       <c r="A38" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-2</v>
@@ -25611,7 +25614,7 @@
       <c r="Q38" s="15"/>
       <c r="R38" s="15"/>
     </row>
-    <row r="39" spans="1:18" hidden="1">
+    <row r="39" spans="1:18">
       <c r="A39" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-3</v>
@@ -25651,7 +25654,7 @@
       <c r="Q39" s="15"/>
       <c r="R39" s="15"/>
     </row>
-    <row r="40" spans="1:18" hidden="1">
+    <row r="40" spans="1:18">
       <c r="A40" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-4</v>
@@ -25691,7 +25694,7 @@
       <c r="Q40" s="15"/>
       <c r="R40" s="15"/>
     </row>
-    <row r="41" spans="1:18" hidden="1">
+    <row r="41" spans="1:18">
       <c r="A41" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-5</v>
@@ -25731,7 +25734,7 @@
       <c r="Q41" s="15"/>
       <c r="R41" s="15"/>
     </row>
-    <row r="42" spans="1:18" hidden="1">
+    <row r="42" spans="1:18">
       <c r="A42" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-6</v>
@@ -25771,7 +25774,7 @@
       <c r="Q42" s="15"/>
       <c r="R42" s="15"/>
     </row>
-    <row r="43" spans="1:18" hidden="1">
+    <row r="43" spans="1:18">
       <c r="A43" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-7</v>
@@ -25811,7 +25814,7 @@
       <c r="Q43" s="15"/>
       <c r="R43" s="15"/>
     </row>
-    <row r="44" spans="1:18" hidden="1">
+    <row r="44" spans="1:18">
       <c r="A44" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-8</v>
@@ -25851,7 +25854,7 @@
       <c r="Q44" s="15"/>
       <c r="R44" s="15"/>
     </row>
-    <row r="45" spans="1:18" hidden="1">
+    <row r="45" spans="1:18">
       <c r="A45" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-9</v>
@@ -25891,7 +25894,7 @@
       <c r="Q45" s="15"/>
       <c r="R45" s="15"/>
     </row>
-    <row r="46" spans="1:18" hidden="1">
+    <row r="46" spans="1:18">
       <c r="A46" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-10</v>
@@ -25931,7 +25934,7 @@
       <c r="Q46" s="15"/>
       <c r="R46" s="15"/>
     </row>
-    <row r="47" spans="1:18" hidden="1">
+    <row r="47" spans="1:18">
       <c r="A47" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-11</v>
@@ -25971,7 +25974,7 @@
       <c r="Q47" s="15"/>
       <c r="R47" s="15"/>
     </row>
-    <row r="48" spans="1:18" hidden="1">
+    <row r="48" spans="1:18">
       <c r="A48" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-12</v>
@@ -26011,7 +26014,7 @@
       <c r="Q48" s="15"/>
       <c r="R48" s="15"/>
     </row>
-    <row r="49" spans="1:18" hidden="1">
+    <row r="49" spans="1:18">
       <c r="A49" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-13</v>
@@ -26051,7 +26054,7 @@
       <c r="Q49" s="15"/>
       <c r="R49" s="15"/>
     </row>
-    <row r="50" spans="1:18" hidden="1">
+    <row r="50" spans="1:18">
       <c r="A50" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-14</v>
@@ -29695,7 +29698,7 @@
       <c r="Q150" s="40"/>
       <c r="R150" s="40"/>
     </row>
-    <row r="151" spans="1:18">
+    <row r="151" spans="1:18" hidden="1">
       <c r="A151" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-14</v>
@@ -29735,7 +29738,7 @@
       <c r="Q151" s="40"/>
       <c r="R151" s="40"/>
     </row>
-    <row r="152" spans="1:18" hidden="1">
+    <row r="152" spans="1:18">
       <c r="A152" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-15</v>
@@ -29775,7 +29778,7 @@
       <c r="Q152" s="40"/>
       <c r="R152" s="40"/>
     </row>
-    <row r="153" spans="1:18">
+    <row r="153" spans="1:18" hidden="1">
       <c r="A153" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-15</v>
@@ -29815,7 +29818,7 @@
       <c r="Q153" s="40"/>
       <c r="R153" s="40"/>
     </row>
-    <row r="154" spans="1:18" hidden="1">
+    <row r="154" spans="1:18">
       <c r="A154" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-16</v>
@@ -29855,7 +29858,7 @@
       <c r="Q154" s="40"/>
       <c r="R154" s="40"/>
     </row>
-    <row r="155" spans="1:18">
+    <row r="155" spans="1:18" hidden="1">
       <c r="A155" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-16</v>
@@ -29895,7 +29898,7 @@
       <c r="Q155" s="40"/>
       <c r="R155" s="40"/>
     </row>
-    <row r="156" spans="1:18" hidden="1">
+    <row r="156" spans="1:18">
       <c r="A156" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-17</v>
@@ -30259,7 +30262,7 @@
       <c r="Q165" s="40"/>
       <c r="R165" s="40"/>
     </row>
-    <row r="166" spans="1:18" hidden="1">
+    <row r="166" spans="1:18">
       <c r="A166" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-18</v>
@@ -30299,7 +30302,7 @@
       <c r="Q166" s="40"/>
       <c r="R166" s="40"/>
     </row>
-    <row r="167" spans="1:18">
+    <row r="167" spans="1:18" hidden="1">
       <c r="A167" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-17</v>
@@ -30339,7 +30342,7 @@
       <c r="Q167" s="40"/>
       <c r="R167" s="40"/>
     </row>
-    <row r="168" spans="1:18" hidden="1">
+    <row r="168" spans="1:18">
       <c r="A168" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-19</v>
@@ -30497,7 +30500,7 @@
       <c r="Q171" s="40"/>
       <c r="R171" s="40"/>
     </row>
-    <row r="172" spans="1:18">
+    <row r="172" spans="1:18" hidden="1">
       <c r="A172" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-18</v>
@@ -30537,7 +30540,7 @@
       <c r="Q172" s="40"/>
       <c r="R172" s="40"/>
     </row>
-    <row r="173" spans="1:18" hidden="1">
+    <row r="173" spans="1:18">
       <c r="A173" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-20</v>
@@ -30577,7 +30580,7 @@
       <c r="Q173" s="40"/>
       <c r="R173" s="40"/>
     </row>
-    <row r="174" spans="1:18" hidden="1">
+    <row r="174" spans="1:18">
       <c r="A174" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-21</v>
@@ -30617,7 +30620,7 @@
       <c r="Q174" s="40"/>
       <c r="R174" s="40"/>
     </row>
-    <row r="175" spans="1:18" hidden="1">
+    <row r="175" spans="1:18">
       <c r="A175" s="42" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-22</v>
@@ -30657,7 +30660,7 @@
       <c r="Q175" s="43"/>
       <c r="R175" s="43"/>
     </row>
-    <row r="176" spans="1:18" hidden="1">
+    <row r="176" spans="1:18">
       <c r="A176" s="42" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-23</v>
@@ -30973,7 +30976,7 @@
       <c r="Q184" s="40"/>
       <c r="R184" s="40"/>
     </row>
-    <row r="185" spans="1:18">
+    <row r="185" spans="1:18" hidden="1">
       <c r="A185" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-19</v>
@@ -31013,7 +31016,7 @@
       <c r="Q185" s="40"/>
       <c r="R185" s="40"/>
     </row>
-    <row r="186" spans="1:18" hidden="1">
+    <row r="186" spans="1:18">
       <c r="A186" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-24</v>
@@ -31053,7 +31056,7 @@
       <c r="Q186" s="40"/>
       <c r="R186" s="40"/>
     </row>
-    <row r="187" spans="1:18">
+    <row r="187" spans="1:18" hidden="1">
       <c r="A187" s="42" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-20</v>
@@ -31093,7 +31096,7 @@
       <c r="Q187" s="43"/>
       <c r="R187" s="43"/>
     </row>
-    <row r="188" spans="1:18">
+    <row r="188" spans="1:18" hidden="1">
       <c r="A188" s="42" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-21</v>
@@ -31133,7 +31136,7 @@
       <c r="Q188" s="43"/>
       <c r="R188" s="43"/>
     </row>
-    <row r="189" spans="1:18">
+    <row r="189" spans="1:18" hidden="1">
       <c r="A189" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-22</v>
@@ -31173,7 +31176,7 @@
       <c r="Q189" s="40"/>
       <c r="R189" s="40"/>
     </row>
-    <row r="190" spans="1:18" hidden="1">
+    <row r="190" spans="1:18">
       <c r="A190" s="42" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-25</v>
@@ -31213,7 +31216,7 @@
       <c r="Q190" s="43"/>
       <c r="R190" s="43"/>
     </row>
-    <row r="191" spans="1:18" hidden="1">
+    <row r="191" spans="1:18">
       <c r="A191" s="42" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-26</v>
@@ -31253,7 +31256,7 @@
       <c r="Q191" s="43"/>
       <c r="R191" s="43"/>
     </row>
-    <row r="192" spans="1:18" hidden="1">
+    <row r="192" spans="1:18">
       <c r="A192" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-27</v>
@@ -31293,7 +31296,7 @@
       <c r="Q192" s="40"/>
       <c r="R192" s="40"/>
     </row>
-    <row r="193" spans="1:18">
+    <row r="193" spans="1:18" hidden="1">
       <c r="A193" s="42" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-23</v>
@@ -31333,7 +31336,7 @@
       <c r="Q193" s="43"/>
       <c r="R193" s="43"/>
     </row>
-    <row r="194" spans="1:18">
+    <row r="194" spans="1:18" hidden="1">
       <c r="A194" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-24</v>
@@ -31373,7 +31376,7 @@
       <c r="Q194" s="40"/>
       <c r="R194" s="40"/>
     </row>
-    <row r="195" spans="1:18" hidden="1">
+    <row r="195" spans="1:18">
       <c r="A195" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-28</v>
@@ -31413,7 +31416,7 @@
       <c r="Q195" s="40"/>
       <c r="R195" s="40"/>
     </row>
-    <row r="196" spans="1:18" hidden="1">
+    <row r="196" spans="1:18">
       <c r="A196" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-29</v>
@@ -31987,7 +31990,7 @@
       <c r="Q211" s="40"/>
       <c r="R211" s="40"/>
     </row>
-    <row r="212" spans="1:18">
+    <row r="212" spans="1:18" hidden="1">
       <c r="A212" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-25</v>
@@ -32027,7 +32030,7 @@
       <c r="Q212" s="16"/>
       <c r="R212" s="16"/>
     </row>
-    <row r="213" spans="1:18" hidden="1">
+    <row r="213" spans="1:18">
       <c r="A213" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-30</v>
@@ -32067,7 +32070,7 @@
       <c r="Q213" s="16"/>
       <c r="R213" s="16"/>
     </row>
-    <row r="214" spans="1:18">
+    <row r="214" spans="1:18" hidden="1">
       <c r="A214" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-26</v>
@@ -32107,7 +32110,7 @@
       <c r="Q214" s="40"/>
       <c r="R214" s="40"/>
     </row>
-    <row r="215" spans="1:18" hidden="1">
+    <row r="215" spans="1:18">
       <c r="A215" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-31</v>
@@ -32147,7 +32150,7 @@
       <c r="Q215" s="40"/>
       <c r="R215" s="40"/>
     </row>
-    <row r="216" spans="1:18" hidden="1">
+    <row r="216" spans="1:18">
       <c r="A216" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-32</v>
@@ -32187,7 +32190,7 @@
       <c r="Q216" s="40"/>
       <c r="R216" s="40"/>
     </row>
-    <row r="217" spans="1:18">
+    <row r="217" spans="1:18" hidden="1">
       <c r="A217" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-27</v>
@@ -32227,7 +32230,7 @@
       <c r="Q217" s="40"/>
       <c r="R217" s="40"/>
     </row>
-    <row r="218" spans="1:18" hidden="1">
+    <row r="218" spans="1:18">
       <c r="A218" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-33</v>
@@ -32505,7 +32508,7 @@
       <c r="Q225" s="40"/>
       <c r="R225" s="40"/>
     </row>
-    <row r="226" spans="1:18">
+    <row r="226" spans="1:18" hidden="1">
       <c r="A226" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-28</v>
@@ -32545,7 +32548,7 @@
       <c r="Q226" s="40"/>
       <c r="R226" s="40"/>
     </row>
-    <row r="227" spans="1:18" hidden="1">
+    <row r="227" spans="1:18">
       <c r="A227" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-34</v>
@@ -32585,7 +32588,7 @@
       <c r="Q227" s="40"/>
       <c r="R227" s="40"/>
     </row>
-    <row r="228" spans="1:18">
+    <row r="228" spans="1:18" hidden="1">
       <c r="A228" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-29</v>
@@ -32625,7 +32628,7 @@
       <c r="Q228" s="40"/>
       <c r="R228" s="40"/>
     </row>
-    <row r="229" spans="1:18" hidden="1">
+    <row r="229" spans="1:18">
       <c r="A229" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-35</v>
@@ -32665,7 +32668,7 @@
       <c r="Q229" s="40"/>
       <c r="R229" s="40"/>
     </row>
-    <row r="230" spans="1:18" hidden="1">
+    <row r="230" spans="1:18">
       <c r="A230" s="42" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-36</v>
@@ -32705,7 +32708,7 @@
       <c r="Q230" s="43"/>
       <c r="R230" s="43"/>
     </row>
-    <row r="231" spans="1:18" hidden="1">
+    <row r="231" spans="1:18">
       <c r="A231" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-37</v>
@@ -34103,7 +34106,7 @@
       <c r="Q270" s="40"/>
       <c r="R270" s="40"/>
     </row>
-    <row r="271" spans="1:18" hidden="1">
+    <row r="271" spans="1:18">
       <c r="A271" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-38</v>
@@ -34143,7 +34146,7 @@
       <c r="Q271" s="40"/>
       <c r="R271" s="40"/>
     </row>
-    <row r="272" spans="1:18">
+    <row r="272" spans="1:18" hidden="1">
       <c r="A272" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-30</v>
@@ -34183,7 +34186,7 @@
       <c r="Q272" s="40"/>
       <c r="R272" s="40"/>
     </row>
-    <row r="273" spans="1:18" hidden="1">
+    <row r="273" spans="1:18">
       <c r="A273" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-39</v>
@@ -34222,6 +34225,46 @@
       <c r="P273" s="40"/>
       <c r="Q273" s="40"/>
       <c r="R273" s="40"/>
+    </row>
+    <row r="274" spans="1:18">
+      <c r="A274" s="22" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resource Relations-40</v>
+      </c>
+      <c r="B274" s="40" t="s">
+        <v>442</v>
+      </c>
+      <c r="C274" s="22">
+        <f>COUNTIF($B$1:$B273,[Table Name])</f>
+        <v>40</v>
+      </c>
+      <c r="D274" s="40">
+        <v>30</v>
+      </c>
+      <c r="E274" s="40" t="s">
+        <v>655</v>
+      </c>
+      <c r="F274" s="40" t="s">
+        <v>655</v>
+      </c>
+      <c r="G274" s="40" t="s">
+        <v>350</v>
+      </c>
+      <c r="H274" s="40" t="s">
+        <v>402</v>
+      </c>
+      <c r="I274" s="40">
+        <v>12</v>
+      </c>
+      <c r="J274" s="40"/>
+      <c r="K274" s="40"/>
+      <c r="L274" s="40"/>
+      <c r="M274" s="40"/>
+      <c r="N274" s="40"/>
+      <c r="O274" s="40"/>
+      <c r="P274" s="40"/>
+      <c r="Q274" s="40"/>
+      <c r="R274" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -34234,10 +34277,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -34768,12 +34811,32 @@
         <v>truncate</v>
       </c>
     </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="4" t="s">
+        <v>659</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="C27" s="4" t="str">
+        <f>VLOOKUP([FW Table Name],Tables[],4,0)</f>
+        <v>Milestone\Appframe\Model</v>
+      </c>
+      <c r="D27" s="4" t="str">
+        <f>VLOOKUP([FW Table Name],Tables[],5,0)</f>
+        <v>ResourceFormCollection</v>
+      </c>
+      <c r="E27" s="7" t="str">
+        <f>"truncate"</f>
+        <v>truncate</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E26">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E27">
       <formula1>"truncate,query"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B26">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B27">
       <formula1>TableNames</formula1>
     </dataValidation>
   </dataValidations>
@@ -35688,10 +35751,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40:I40"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41:I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -36987,9 +37050,41 @@
         <v>30</v>
       </c>
     </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="20">
+        <f>IFERROR($A40+1,1)</f>
+        <v>40</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>653</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="D41" s="7">
+        <f>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</f>
+        <v>30</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>655</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>655</v>
+      </c>
+      <c r="G41" s="22" t="s">
+        <v>350</v>
+      </c>
+      <c r="H41" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="I41" s="41">
+        <f>VLOOKUP([Relate Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</f>
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C40">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C41">
       <formula1>Resources</formula1>
     </dataValidation>
   </dataValidations>
@@ -37004,8 +37099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -40152,31 +40247,31 @@
       </c>
       <c r="B48" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>;</v>
+        <v>-&gt;create([</v>
       </c>
       <c r="C48" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '30', </v>
       </c>
       <c r="D48" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Collection Form', </v>
       </c>
       <c r="E48" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Collection Form', </v>
       </c>
       <c r="F48" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Form', </v>
       </c>
       <c r="G48" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H48" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '12', </v>
       </c>
       <c r="I48" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -40216,7 +40311,7 @@
       </c>
       <c r="R48" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="49" spans="1:18">
@@ -40225,7 +40320,7 @@
       </c>
       <c r="B49" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
+        <v>;</v>
       </c>
       <c r="C49" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -40298,7 +40393,7 @@
       </c>
       <c r="B50" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
       </c>
       <c r="C50" s="33" t="str">
         <f t="shared" ca="1" si="3"/>

</xml_diff>

<commit_message>
New Relation named "Relation" added for Form Collection
</commit_message>
<xml_diff>
--- a/Helper.xlsx
+++ b/Helper.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3183" uniqueCount="660">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3194" uniqueCount="661">
   <si>
     <t>resource_scopes</t>
   </si>
@@ -2018,6 +2018,9 @@
   </si>
   <si>
     <t>Form Collection</t>
+  </si>
+  <si>
+    <t>Details of Relation</t>
   </si>
 </sst>
 </file>
@@ -4147,8 +4150,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R274" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
-  <autoFilter ref="A1:R274">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R275" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
+  <autoFilter ref="A1:R275">
     <filterColumn colId="1">
       <filters>
         <filter val="Resource Relations"/>
@@ -4228,8 +4231,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RelationTable" displayName="RelationTable" ref="A1:I41" totalsRowShown="0" dataDxfId="47">
-  <autoFilter ref="A1:I41"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RelationTable" displayName="RelationTable" ref="A1:I42" totalsRowShown="0" dataDxfId="47">
+  <autoFilter ref="A1:I42"/>
   <tableColumns count="9">
     <tableColumn id="1" name="No" dataDxfId="46">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
@@ -24196,10 +24199,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R274"/>
+  <dimension ref="A1:R275"/>
   <sheetViews>
     <sheetView topLeftCell="B213" workbookViewId="0">
-      <selection activeCell="B274" sqref="B274"/>
+      <selection activeCell="B275" sqref="B275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -34265,6 +34268,46 @@
       <c r="P274" s="40"/>
       <c r="Q274" s="40"/>
       <c r="R274" s="40"/>
+    </row>
+    <row r="275" spans="1:18">
+      <c r="A275" s="22" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resource Relations-41</v>
+      </c>
+      <c r="B275" s="40" t="s">
+        <v>442</v>
+      </c>
+      <c r="C275" s="22">
+        <f>COUNTIF($B$1:$B274,[Table Name])</f>
+        <v>41</v>
+      </c>
+      <c r="D275" s="40">
+        <v>30</v>
+      </c>
+      <c r="E275" s="40" t="s">
+        <v>304</v>
+      </c>
+      <c r="F275" s="40" t="s">
+        <v>660</v>
+      </c>
+      <c r="G275" s="40" t="s">
+        <v>304</v>
+      </c>
+      <c r="H275" s="40" t="s">
+        <v>402</v>
+      </c>
+      <c r="I275" s="40">
+        <v>26</v>
+      </c>
+      <c r="J275" s="40"/>
+      <c r="K275" s="40"/>
+      <c r="L275" s="40"/>
+      <c r="M275" s="40"/>
+      <c r="N275" s="40"/>
+      <c r="O275" s="40"/>
+      <c r="P275" s="40"/>
+      <c r="Q275" s="40"/>
+      <c r="R275" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -35751,10 +35794,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41:I41"/>
+      <selection activeCell="D42" sqref="D42:I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -37082,9 +37125,41 @@
         <v>12</v>
       </c>
     </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="20">
+        <f>IFERROR($A41+1,1)</f>
+        <v>41</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>653</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>571</v>
+      </c>
+      <c r="D42" s="7">
+        <f>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</f>
+        <v>30</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>660</v>
+      </c>
+      <c r="G42" s="22" t="s">
+        <v>304</v>
+      </c>
+      <c r="H42" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="I42" s="41">
+        <f>VLOOKUP([Relate Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</f>
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C41">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C42">
       <formula1>Resources</formula1>
     </dataValidation>
   </dataValidations>
@@ -37099,8 +37174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -40320,31 +40395,31 @@
       </c>
       <c r="B49" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>;</v>
+        <v>-&gt;create([</v>
       </c>
       <c r="C49" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '30', </v>
       </c>
       <c r="D49" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Relation', </v>
       </c>
       <c r="E49" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Details of Relation', </v>
       </c>
       <c r="F49" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
       </c>
       <c r="G49" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H49" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
       </c>
       <c r="I49" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -40384,7 +40459,7 @@
       </c>
       <c r="R49" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="50" spans="1:18">
@@ -40393,7 +40468,7 @@
       </c>
       <c r="B50" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
+        <v>;</v>
       </c>
       <c r="C50" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -40466,7 +40541,7 @@
       </c>
       <c r="B51" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
       </c>
       <c r="C51" s="33" t="str">
         <f t="shared" ca="1" si="3"/>

</xml_diff>

<commit_message>
Relations from Option to Field to Form added
</commit_message>
<xml_diff>
--- a/Helper.xlsx
+++ b/Helper.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3194" uniqueCount="661">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3216" uniqueCount="663">
   <si>
     <t>resource_scopes</t>
   </si>
@@ -2021,6 +2021,12 @@
   </si>
   <si>
     <t>Details of Relation</t>
+  </si>
+  <si>
+    <t>Field details</t>
+  </si>
+  <si>
+    <t>Form details</t>
   </si>
 </sst>
 </file>
@@ -4150,8 +4156,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R275" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
-  <autoFilter ref="A1:R275">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R277" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
+  <autoFilter ref="A1:R277">
     <filterColumn colId="1">
       <filters>
         <filter val="Resource Relations"/>
@@ -4231,8 +4237,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RelationTable" displayName="RelationTable" ref="A1:I42" totalsRowShown="0" dataDxfId="47">
-  <autoFilter ref="A1:I42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RelationTable" displayName="RelationTable" ref="A1:I44" totalsRowShown="0" dataDxfId="47">
+  <autoFilter ref="A1:I44"/>
   <tableColumns count="9">
     <tableColumn id="1" name="No" dataDxfId="46">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
@@ -24199,10 +24205,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R275"/>
+  <dimension ref="A1:R277"/>
   <sheetViews>
     <sheetView topLeftCell="B213" workbookViewId="0">
-      <selection activeCell="B275" sqref="B275"/>
+      <selection activeCell="C277" sqref="C277"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -34308,6 +34314,86 @@
       <c r="P275" s="40"/>
       <c r="Q275" s="40"/>
       <c r="R275" s="40"/>
+    </row>
+    <row r="276" spans="1:18">
+      <c r="A276" s="42" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resource Relations-42</v>
+      </c>
+      <c r="B276" s="40" t="s">
+        <v>442</v>
+      </c>
+      <c r="C276" s="42">
+        <f>COUNTIF($B$1:$B275,[Table Name])</f>
+        <v>42</v>
+      </c>
+      <c r="D276" s="43">
+        <v>15</v>
+      </c>
+      <c r="E276" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="F276" s="43" t="s">
+        <v>661</v>
+      </c>
+      <c r="G276" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="H276" s="43" t="s">
+        <v>402</v>
+      </c>
+      <c r="I276" s="43">
+        <v>13</v>
+      </c>
+      <c r="J276" s="43"/>
+      <c r="K276" s="43"/>
+      <c r="L276" s="43"/>
+      <c r="M276" s="43"/>
+      <c r="N276" s="43"/>
+      <c r="O276" s="43"/>
+      <c r="P276" s="43"/>
+      <c r="Q276" s="43"/>
+      <c r="R276" s="43"/>
+    </row>
+    <row r="277" spans="1:18">
+      <c r="A277" s="22" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resource Relations-43</v>
+      </c>
+      <c r="B277" s="40" t="s">
+        <v>442</v>
+      </c>
+      <c r="C277" s="22">
+        <f>COUNTIF($B$1:$B276,[Table Name])</f>
+        <v>43</v>
+      </c>
+      <c r="D277" s="40">
+        <v>13</v>
+      </c>
+      <c r="E277" s="40" t="s">
+        <v>350</v>
+      </c>
+      <c r="F277" s="40" t="s">
+        <v>662</v>
+      </c>
+      <c r="G277" s="40" t="s">
+        <v>350</v>
+      </c>
+      <c r="H277" s="40" t="s">
+        <v>402</v>
+      </c>
+      <c r="I277" s="40">
+        <v>12</v>
+      </c>
+      <c r="J277" s="40"/>
+      <c r="K277" s="40"/>
+      <c r="L277" s="40"/>
+      <c r="M277" s="40"/>
+      <c r="N277" s="40"/>
+      <c r="O277" s="40"/>
+      <c r="P277" s="40"/>
+      <c r="Q277" s="40"/>
+      <c r="R277" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -35794,10 +35880,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42:I42"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43:I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -36967,7 +37053,7 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="20">
-        <f>IFERROR($A36+1,1)</f>
+        <f t="shared" ref="A37:A42" si="6">IFERROR($A36+1,1)</f>
         <v>36</v>
       </c>
       <c r="B37" s="7" t="s">
@@ -36999,7 +37085,7 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="20">
-        <f>IFERROR($A37+1,1)</f>
+        <f t="shared" si="6"/>
         <v>37</v>
       </c>
       <c r="B38" s="7" t="s">
@@ -37031,7 +37117,7 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="20">
-        <f>IFERROR($A38+1,1)</f>
+        <f t="shared" si="6"/>
         <v>38</v>
       </c>
       <c r="B39" s="7" t="s">
@@ -37063,7 +37149,7 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="20">
-        <f>IFERROR($A39+1,1)</f>
+        <f t="shared" si="6"/>
         <v>39</v>
       </c>
       <c r="B40" s="7" t="s">
@@ -37095,7 +37181,7 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="20">
-        <f>IFERROR($A40+1,1)</f>
+        <f t="shared" si="6"/>
         <v>40</v>
       </c>
       <c r="B41" s="7" t="s">
@@ -37127,7 +37213,7 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="20">
-        <f>IFERROR($A41+1,1)</f>
+        <f t="shared" si="6"/>
         <v>41</v>
       </c>
       <c r="B42" s="7" t="s">
@@ -37157,9 +37243,73 @@
         <v>26</v>
       </c>
     </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="20">
+        <f>IFERROR($A42+1,1)</f>
+        <v>42</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>463</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="D43" s="7">
+        <f>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</f>
+        <v>15</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>661</v>
+      </c>
+      <c r="G43" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="H43" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="I43" s="41">
+        <f>VLOOKUP([Relate Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="20">
+        <f>IFERROR($A43+1,1)</f>
+        <v>43</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="D44" s="7">
+        <f>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</f>
+        <v>13</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>662</v>
+      </c>
+      <c r="G44" s="22" t="s">
+        <v>350</v>
+      </c>
+      <c r="H44" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="I44" s="41">
+        <f>VLOOKUP([Relate Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</f>
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C42">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C44">
       <formula1>Resources</formula1>
     </dataValidation>
   </dataValidations>
@@ -37174,8 +37324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -40468,31 +40618,31 @@
       </c>
       <c r="B50" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>;</v>
+        <v>-&gt;create([</v>
       </c>
       <c r="C50" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '15', </v>
       </c>
       <c r="D50" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Field', </v>
       </c>
       <c r="E50" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Field details', </v>
       </c>
       <c r="F50" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Field', </v>
       </c>
       <c r="G50" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H50" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '13', </v>
       </c>
       <c r="I50" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -40532,7 +40682,7 @@
       </c>
       <c r="R50" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="51" spans="1:18">
@@ -40541,31 +40691,31 @@
       </c>
       <c r="B51" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
+        <v>-&gt;create([</v>
       </c>
       <c r="C51" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '13', </v>
       </c>
       <c r="D51" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Form', </v>
       </c>
       <c r="E51" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Form details', </v>
       </c>
       <c r="F51" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Form', </v>
       </c>
       <c r="G51" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H51" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '12', </v>
       </c>
       <c r="I51" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -40605,7 +40755,7 @@
       </c>
       <c r="R51" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="52" spans="1:18">
@@ -40614,7 +40764,7 @@
       </c>
       <c r="B52" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>;</v>
       </c>
       <c r="C52" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -40687,7 +40837,7 @@
       </c>
       <c r="B53" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
       </c>
       <c r="C53" s="33" t="str">
         <f t="shared" ca="1" si="3"/>

</xml_diff>

<commit_message>
User table seeder added
</commit_message>
<xml_diff>
--- a/Helper.xlsx
+++ b/Helper.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3216" uniqueCount="663">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3222" uniqueCount="663">
   <si>
     <t>resource_scopes</t>
   </si>
@@ -4156,8 +4156,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R277" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
-  <autoFilter ref="A1:R277">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R278" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
+  <autoFilter ref="A1:R278">
     <filterColumn colId="1">
       <filters>
         <filter val="Resource Relations"/>
@@ -4193,8 +4193,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SeedMap" displayName="SeedMap" ref="A1:E27" totalsRowShown="0" dataDxfId="63">
-  <autoFilter ref="A1:E27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SeedMap" displayName="SeedMap" ref="A1:E28" totalsRowShown="0" dataDxfId="63">
+  <autoFilter ref="A1:E28"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Name" dataDxfId="62"/>
     <tableColumn id="3" name="FW Table Name" dataDxfId="61"/>
@@ -4595,7 +4595,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -24205,10 +24205,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R277"/>
+  <dimension ref="A1:R278"/>
   <sheetViews>
-    <sheetView topLeftCell="B152" workbookViewId="0">
-      <selection activeCell="D175" sqref="D175:I175"/>
+    <sheetView topLeftCell="B213" workbookViewId="0">
+      <selection activeCell="B278" sqref="B278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -34395,6 +34395,40 @@
       <c r="Q277" s="40"/>
       <c r="R277" s="40"/>
     </row>
+    <row r="278" spans="1:18">
+      <c r="A278" s="22" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Users-0</v>
+      </c>
+      <c r="B278" s="40" t="s">
+        <v>184</v>
+      </c>
+      <c r="C278" s="22">
+        <f>COUNTIF($B$1:$B277,[Table Name])</f>
+        <v>0</v>
+      </c>
+      <c r="D278" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="E278" s="40" t="s">
+        <v>271</v>
+      </c>
+      <c r="F278" s="40" t="s">
+        <v>511</v>
+      </c>
+      <c r="G278" s="40"/>
+      <c r="H278" s="40"/>
+      <c r="I278" s="40"/>
+      <c r="J278" s="40"/>
+      <c r="K278" s="40"/>
+      <c r="L278" s="40"/>
+      <c r="M278" s="40"/>
+      <c r="N278" s="40"/>
+      <c r="O278" s="40"/>
+      <c r="P278" s="40"/>
+      <c r="Q278" s="40"/>
+      <c r="R278" s="40"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
@@ -34406,10 +34440,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -34960,12 +34994,32 @@
         <v>truncate</v>
       </c>
     </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C28" s="4" t="str">
+        <f>VLOOKUP([FW Table Name],Tables[],4,0)</f>
+        <v>Milestone\Appframe\Model</v>
+      </c>
+      <c r="D28" s="4" t="str">
+        <f>VLOOKUP([FW Table Name],Tables[],5,0)</f>
+        <v>User</v>
+      </c>
+      <c r="E28" s="7" t="str">
+        <f>"truncate"</f>
+        <v>truncate</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E27">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E28">
       <formula1>"truncate,query"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B27">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B28">
       <formula1>TableNames</formula1>
     </dataValidation>
   </dataValidations>
@@ -37324,8 +37378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -37335,14 +37389,14 @@
   <sheetData>
     <row r="1" spans="1:20" s="38" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="48" t="s">
-        <v>442</v>
+        <v>184</v>
       </c>
       <c r="B1" s="48"/>
       <c r="C1" s="48"/>
       <c r="D1" s="48"/>
       <c r="E1" s="49" t="str">
         <f>"\"&amp;VLOOKUP($A$1,SeedMap[],3,0)&amp;"\"&amp;VLOOKUP($A$1,SeedMap[],4,0)&amp;"::"&amp;VLOOKUP($A$1,SeedMap[],5,0)&amp;"()"</f>
-        <v>\Milestone\Appframe\Model\ResourceRelation::truncate()</v>
+        <v>\Milestone\Appframe\Model\User::truncate()</v>
       </c>
       <c r="F1" s="49"/>
       <c r="G1" s="49"/>
@@ -37486,27 +37540,27 @@
       <c r="B5" s="28"/>
       <c r="C5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],C$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],C$4+$B$4,0))</f>
-        <v>resource</v>
+        <v>name</v>
       </c>
       <c r="D5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],D$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],D$4+$B$4,0))</f>
-        <v>name</v>
+        <v>email</v>
       </c>
       <c r="E5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0))</f>
-        <v>description</v>
+        <v>password</v>
       </c>
       <c r="F5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0))</f>
-        <v>method</v>
+        <v/>
       </c>
       <c r="G5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0))</f>
-        <v>type</v>
+        <v/>
       </c>
       <c r="H5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],H$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],H$4+$B$4,0))</f>
-        <v>relate_resource</v>
+        <v/>
       </c>
       <c r="I5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],I$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],I$4+$B$4,0))</f>
@@ -37600,7 +37654,7 @@
       <c r="A8" s="32"/>
       <c r="B8" s="47" t="str">
         <f>$E$1</f>
-        <v>\Milestone\Appframe\Model\ResourceRelation::truncate()</v>
+        <v>\Milestone\Appframe\Model\User::truncate()</v>
       </c>
       <c r="C8" s="47"/>
       <c r="D8" s="47"/>
@@ -37625,31 +37679,31 @@
       </c>
       <c r="B9" s="30" t="str">
         <f ca="1">IF($B8="","",IF($B8=";",$I$3,IF($B8=$I$3,"",IF(ISNA(VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),1,0)),";",$S$4))))</f>
-        <v>-&gt;create([</v>
+        <v>;</v>
       </c>
       <c r="C9" s="33" t="str">
         <f ca="1">IF(AND($B9=$S$4,C$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),C$4+$B$4,0)="","","'"&amp;C$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),C$4+$B$4,0)&amp;"', "),"")</f>
-        <v xml:space="preserve">'resource' =&gt; '1', </v>
+        <v/>
       </c>
       <c r="D9" s="33" t="str">
         <f t="shared" ref="D9:Q24" ca="1" si="0">IF(AND($B9=$S$4,D$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),D$4+$B$4,0)="","","'"&amp;D$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),D$4+$B$4,0)&amp;"', "),"")</f>
-        <v xml:space="preserve">'name' =&gt; 'User Groups', </v>
+        <v/>
       </c>
       <c r="E9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Which groups this user belongs to', </v>
+        <v/>
       </c>
       <c r="F9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Groups', </v>
+        <v/>
       </c>
       <c r="G9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
+        <v/>
       </c>
       <c r="H9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '2', </v>
+        <v/>
       </c>
       <c r="I9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -37689,7 +37743,7 @@
       </c>
       <c r="R9" s="33" t="str">
         <f ca="1">IF(B9=$S$4,$T$4,"")</f>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="10" spans="1:20">
@@ -37698,31 +37752,31 @@
       </c>
       <c r="B10" s="30" t="str">
         <f t="shared" ref="B10:B73" ca="1" si="1">IF($B9="","",IF($B9=";",$I$3,IF($B9=$I$3,"",IF(ISNA(VLOOKUP($A$1&amp;"-"&amp;$A10,INDIRECT($E$2),1,0)),";",$S$4))))</f>
-        <v>-&gt;create([</v>
+        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
       </c>
       <c r="C10" s="33" t="str">
         <f ca="1">IF(AND($B10=$S$4,C$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A10,INDIRECT($E$2),C$4+$B$4,0)="","","'"&amp;C$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A10,INDIRECT($E$2),C$4+$B$4,0)&amp;"', "),"")</f>
-        <v xml:space="preserve">'resource' =&gt; '2', </v>
+        <v/>
       </c>
       <c r="D10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Group Users', </v>
+        <v/>
       </c>
       <c r="E10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'List of users belongs to this group', </v>
+        <v/>
       </c>
       <c r="F10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Users', </v>
+        <v/>
       </c>
       <c r="G10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
+        <v/>
       </c>
       <c r="H10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '1', </v>
+        <v/>
       </c>
       <c r="I10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -37762,7 +37816,7 @@
       </c>
       <c r="R10" s="33" t="str">
         <f t="shared" ref="R10:R73" ca="1" si="2">IF(B10=$S$4,$T$4,"")</f>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -37771,31 +37825,31 @@
       </c>
       <c r="B11" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C11" s="33" t="str">
         <f t="shared" ref="C11:G74" ca="1" si="3">IF(AND($B11=$S$4,C$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A11,INDIRECT($E$2),C$4+$B$4,0)="","","'"&amp;C$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A11,INDIRECT($E$2),C$4+$B$4,0)&amp;"', "),"")</f>
-        <v xml:space="preserve">'resource' =&gt; '2', </v>
+        <v/>
       </c>
       <c r="D11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Group Roles', </v>
+        <v/>
       </c>
       <c r="E11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Roles assigneed to this group', </v>
+        <v/>
       </c>
       <c r="F11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Roles', </v>
+        <v/>
       </c>
       <c r="G11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
+        <v/>
       </c>
       <c r="H11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '3', </v>
+        <v/>
       </c>
       <c r="I11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -37835,7 +37889,7 @@
       </c>
       <c r="R11" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -37844,31 +37898,31 @@
       </c>
       <c r="B12" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C12" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '3', </v>
+        <v/>
       </c>
       <c r="D12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Role Groups', </v>
+        <v/>
       </c>
       <c r="E12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Details of groups this role assigned to', </v>
+        <v/>
       </c>
       <c r="F12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Groups', </v>
+        <v/>
       </c>
       <c r="G12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
+        <v/>
       </c>
       <c r="H12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '2', </v>
+        <v/>
       </c>
       <c r="I12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -37908,7 +37962,7 @@
       </c>
       <c r="R12" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -37917,31 +37971,31 @@
       </c>
       <c r="B13" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C13" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '3', </v>
+        <v/>
       </c>
       <c r="D13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Role Resource', </v>
+        <v/>
       </c>
       <c r="E13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Resources assigned to a role', </v>
+        <v/>
       </c>
       <c r="F13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Resources', </v>
+        <v/>
       </c>
       <c r="G13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '11', </v>
+        <v/>
       </c>
       <c r="I13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -37981,7 +38035,7 @@
       </c>
       <c r="R13" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -37990,31 +38044,31 @@
       </c>
       <c r="B14" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C14" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '4', </v>
+        <v/>
       </c>
       <c r="D14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Resource Roles', </v>
+        <v/>
       </c>
       <c r="E14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'The details of roles who have access to this resource', </v>
+        <v/>
       </c>
       <c r="F14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Roles', </v>
+        <v/>
       </c>
       <c r="G14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
+        <v/>
       </c>
       <c r="H14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '3', </v>
+        <v/>
       </c>
       <c r="I14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -38054,7 +38108,7 @@
       </c>
       <c r="R14" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -38063,31 +38117,31 @@
       </c>
       <c r="B15" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C15" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '4', </v>
+        <v/>
       </c>
       <c r="D15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Resource Actions', </v>
+        <v/>
       </c>
       <c r="E15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Get actions available for the resource', </v>
+        <v/>
       </c>
       <c r="F15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Actions', </v>
+        <v/>
       </c>
       <c r="G15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '7', </v>
+        <v/>
       </c>
       <c r="I15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -38127,7 +38181,7 @@
       </c>
       <c r="R15" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="16" spans="1:20">
@@ -38136,31 +38190,31 @@
       </c>
       <c r="B16" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C16" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '7', </v>
+        <v/>
       </c>
       <c r="D16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Resource Action Methods', </v>
+        <v/>
       </c>
       <c r="E16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Handler details of an action', </v>
+        <v/>
       </c>
       <c r="F16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Method', </v>
+        <v/>
       </c>
       <c r="G16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'hasOne', </v>
+        <v/>
       </c>
       <c r="H16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '8', </v>
+        <v/>
       </c>
       <c r="I16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -38200,7 +38254,7 @@
       </c>
       <c r="R16" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="17" spans="1:18">
@@ -38209,31 +38263,31 @@
       </c>
       <c r="B17" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C17" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '7', </v>
+        <v/>
       </c>
       <c r="D17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Resource Action Lists', </v>
+        <v/>
       </c>
       <c r="E17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Lists where action available', </v>
+        <v/>
       </c>
       <c r="F17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Lists', </v>
+        <v/>
       </c>
       <c r="G17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '9', </v>
+        <v/>
       </c>
       <c r="I17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -38273,7 +38327,7 @@
       </c>
       <c r="R17" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="18" spans="1:18">
@@ -38282,31 +38336,31 @@
       </c>
       <c r="B18" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C18" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '7', </v>
+        <v/>
       </c>
       <c r="D18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Resource Action Data', </v>
+        <v/>
       </c>
       <c r="E18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Resource data where action available', </v>
+        <v/>
       </c>
       <c r="F18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Data', </v>
+        <v/>
       </c>
       <c r="G18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '10', </v>
+        <v/>
       </c>
       <c r="I18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -38346,7 +38400,7 @@
       </c>
       <c r="R18" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="19" spans="1:18">
@@ -38355,31 +38409,31 @@
       </c>
       <c r="B19" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C19" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '5', </v>
+        <v/>
       </c>
       <c r="D19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Organisation Contacts', </v>
+        <v/>
       </c>
       <c r="E19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Contact details of organisation', </v>
+        <v/>
       </c>
       <c r="F19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Contacts', </v>
+        <v/>
       </c>
       <c r="G19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '6', </v>
+        <v/>
       </c>
       <c r="I19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -38419,7 +38473,7 @@
       </c>
       <c r="R19" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="20" spans="1:18">
@@ -38428,31 +38482,31 @@
       </c>
       <c r="B20" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C20" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '11', </v>
+        <v/>
       </c>
       <c r="D20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Resource Details', </v>
+        <v/>
       </c>
       <c r="E20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Resource details', </v>
+        <v/>
       </c>
       <c r="F20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Resource', </v>
+        <v/>
       </c>
       <c r="G20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
+        <v/>
       </c>
       <c r="H20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
+        <v/>
       </c>
       <c r="I20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -38492,7 +38546,7 @@
       </c>
       <c r="R20" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="21" spans="1:18">
@@ -38501,31 +38555,31 @@
       </c>
       <c r="B21" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C21" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '4', </v>
+        <v/>
       </c>
       <c r="D21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Resource Forms', </v>
+        <v/>
       </c>
       <c r="E21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Forms available for a resource', </v>
+        <v/>
       </c>
       <c r="F21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Forms', </v>
+        <v/>
       </c>
       <c r="G21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '12', </v>
+        <v/>
       </c>
       <c r="I21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -38565,7 +38619,7 @@
       </c>
       <c r="R21" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="22" spans="1:18">
@@ -38574,31 +38628,31 @@
       </c>
       <c r="B22" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C22" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '12', </v>
+        <v/>
       </c>
       <c r="D22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Form Fields', </v>
+        <v/>
       </c>
       <c r="E22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Fields associated with a form', </v>
+        <v/>
       </c>
       <c r="F22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Fields', </v>
+        <v/>
       </c>
       <c r="G22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '13', </v>
+        <v/>
       </c>
       <c r="I22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -38638,7 +38692,7 @@
       </c>
       <c r="R22" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="23" spans="1:18">
@@ -38647,31 +38701,31 @@
       </c>
       <c r="B23" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C23" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '13', </v>
+        <v/>
       </c>
       <c r="D23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Field Attributes', </v>
+        <v/>
       </c>
       <c r="E23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Attributes of Field', </v>
+        <v/>
       </c>
       <c r="F23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Attributes', </v>
+        <v/>
       </c>
       <c r="G23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '14', </v>
+        <v/>
       </c>
       <c r="I23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -38711,7 +38765,7 @@
       </c>
       <c r="R23" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="24" spans="1:18">
@@ -38720,31 +38774,31 @@
       </c>
       <c r="B24" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C24" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '13', </v>
+        <v/>
       </c>
       <c r="D24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Field Options', </v>
+        <v/>
       </c>
       <c r="E24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Options of Field', </v>
+        <v/>
       </c>
       <c r="F24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Options', </v>
+        <v/>
       </c>
       <c r="G24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'hasOne', </v>
+        <v/>
       </c>
       <c r="H24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '15', </v>
+        <v/>
       </c>
       <c r="I24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -38784,7 +38838,7 @@
       </c>
       <c r="R24" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="25" spans="1:18">
@@ -38793,31 +38847,31 @@
       </c>
       <c r="B25" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '13', </v>
+        <v/>
       </c>
       <c r="D25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Field Validations', </v>
+        <v/>
       </c>
       <c r="E25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Validation details of field', </v>
+        <v/>
       </c>
       <c r="F25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Validations', </v>
+        <v/>
       </c>
       <c r="G25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H25" s="33" t="str">
         <f t="shared" ref="H25:K88" ca="1" si="4">IF(AND($B25=$S$4,H$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A25,INDIRECT($E$2),H$4+$B$4,0)="","","'"&amp;H$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A25,INDIRECT($E$2),H$4+$B$4,0)&amp;"', "),"")</f>
-        <v xml:space="preserve">'relate_resource' =&gt; '16', </v>
+        <v/>
       </c>
       <c r="I25" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -38857,7 +38911,7 @@
       </c>
       <c r="R25" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="26" spans="1:18">
@@ -38866,31 +38920,31 @@
       </c>
       <c r="B26" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '12', </v>
+        <v/>
       </c>
       <c r="D26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'From Resource', </v>
+        <v/>
       </c>
       <c r="E26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Resource this form belongs to', </v>
+        <v/>
       </c>
       <c r="F26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Resource', </v>
+        <v/>
       </c>
       <c r="G26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
+        <v/>
       </c>
       <c r="H26" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
+        <v/>
       </c>
       <c r="I26" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -38930,7 +38984,7 @@
       </c>
       <c r="R26" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="27" spans="1:18">
@@ -38939,31 +38993,31 @@
       </c>
       <c r="B27" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '12', </v>
+        <v/>
       </c>
       <c r="D27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Form Defaults', </v>
+        <v/>
       </c>
       <c r="E27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Predefined values for a form', </v>
+        <v/>
       </c>
       <c r="F27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Defaults', </v>
+        <v/>
       </c>
       <c r="G27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H27" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '17', </v>
+        <v/>
       </c>
       <c r="I27" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -39003,7 +39057,7 @@
       </c>
       <c r="R27" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="28" spans="1:18">
@@ -39012,31 +39066,31 @@
       </c>
       <c r="B28" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '13', </v>
+        <v/>
       </c>
       <c r="D28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Field Data', </v>
+        <v/>
       </c>
       <c r="E28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Fields Database binding details', </v>
+        <v/>
       </c>
       <c r="F28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Data', </v>
+        <v/>
       </c>
       <c r="G28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasOne', </v>
+        <v/>
       </c>
       <c r="H28" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '18', </v>
+        <v/>
       </c>
       <c r="I28" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -39076,7 +39130,7 @@
       </c>
       <c r="R28" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="29" spans="1:18">
@@ -39085,31 +39139,31 @@
       </c>
       <c r="B29" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '4', </v>
+        <v/>
       </c>
       <c r="D29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Resource Relations', </v>
+        <v/>
       </c>
       <c r="E29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Relation of  a resource to another resource', </v>
+        <v/>
       </c>
       <c r="F29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Relations', </v>
+        <v/>
       </c>
       <c r="G29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H29" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
+        <v/>
       </c>
       <c r="I29" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -39149,7 +39203,7 @@
       </c>
       <c r="R29" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="30" spans="1:18">
@@ -39158,31 +39212,31 @@
       </c>
       <c r="B30" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '18', </v>
+        <v/>
       </c>
       <c r="D30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Bind Data Relation', </v>
+        <v/>
       </c>
       <c r="E30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Relation to which the data to be bind', </v>
+        <v/>
       </c>
       <c r="F30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
+        <v/>
       </c>
       <c r="G30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
+        <v/>
       </c>
       <c r="H30" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
+        <v/>
       </c>
       <c r="I30" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -39222,7 +39276,7 @@
       </c>
       <c r="R30" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="31" spans="1:18">
@@ -39231,31 +39285,31 @@
       </c>
       <c r="B31" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '17', </v>
+        <v/>
       </c>
       <c r="D31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Default Data Resource', </v>
+        <v/>
       </c>
       <c r="E31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Resource to which the forms predefined data to be bind', </v>
+        <v/>
       </c>
       <c r="F31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
+        <v/>
       </c>
       <c r="G31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
+        <v/>
       </c>
       <c r="H31" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
+        <v/>
       </c>
       <c r="I31" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -39295,7 +39349,7 @@
       </c>
       <c r="R31" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="32" spans="1:18">
@@ -39304,31 +39358,31 @@
       </c>
       <c r="B32" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '19', </v>
+        <v/>
       </c>
       <c r="D32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Resource Details', </v>
+        <v/>
       </c>
       <c r="E32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Resource details of a list', </v>
+        <v/>
       </c>
       <c r="F32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Resource', </v>
+        <v/>
       </c>
       <c r="G32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
+        <v/>
       </c>
       <c r="H32" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
+        <v/>
       </c>
       <c r="I32" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -39368,7 +39422,7 @@
       </c>
       <c r="R32" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="33" spans="1:18">
@@ -39377,31 +39431,31 @@
       </c>
       <c r="B33" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '19', </v>
+        <v/>
       </c>
       <c r="D33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'List Relations', </v>
+        <v/>
       </c>
       <c r="E33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Relations to be loaded on accessing list', </v>
+        <v/>
       </c>
       <c r="F33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Relations', </v>
+        <v/>
       </c>
       <c r="G33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H33" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '20', </v>
+        <v/>
       </c>
       <c r="I33" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -39441,7 +39495,7 @@
       </c>
       <c r="R33" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="34" spans="1:18">
@@ -39450,31 +39504,31 @@
       </c>
       <c r="B34" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '4', </v>
+        <v/>
       </c>
       <c r="D34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Resource Scopes', </v>
+        <v/>
       </c>
       <c r="E34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Scopes available on a Resource', </v>
+        <v/>
       </c>
       <c r="F34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Scopes', </v>
+        <v/>
       </c>
       <c r="G34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H34" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '21', </v>
+        <v/>
       </c>
       <c r="I34" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -39514,7 +39568,7 @@
       </c>
       <c r="R34" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="35" spans="1:18">
@@ -39523,31 +39577,31 @@
       </c>
       <c r="B35" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '19', </v>
+        <v/>
       </c>
       <c r="D35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'List Scopes', </v>
+        <v/>
       </c>
       <c r="E35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Scopes by which a list to be filtered', </v>
+        <v/>
       </c>
       <c r="F35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Scopes', </v>
+        <v/>
       </c>
       <c r="G35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
+        <v/>
       </c>
       <c r="H35" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '21', </v>
+        <v/>
       </c>
       <c r="I35" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -39587,7 +39641,7 @@
       </c>
       <c r="R35" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="36" spans="1:18">
@@ -39596,31 +39650,31 @@
       </c>
       <c r="B36" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '23', </v>
+        <v/>
       </c>
       <c r="D36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Data Relation', </v>
+        <v/>
       </c>
       <c r="E36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Relations to be loaded on a data view', </v>
+        <v/>
       </c>
       <c r="F36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Relations', </v>
+        <v/>
       </c>
       <c r="G36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H36" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '24', </v>
+        <v/>
       </c>
       <c r="I36" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -39660,7 +39714,7 @@
       </c>
       <c r="R36" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="37" spans="1:18">
@@ -39669,31 +39723,31 @@
       </c>
       <c r="B37" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '23', </v>
+        <v/>
       </c>
       <c r="D37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Resource Details', </v>
+        <v/>
       </c>
       <c r="E37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Details of resource of a record', </v>
+        <v/>
       </c>
       <c r="F37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Resource', </v>
+        <v/>
       </c>
       <c r="G37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
+        <v/>
       </c>
       <c r="H37" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
+        <v/>
       </c>
       <c r="I37" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -39733,7 +39787,7 @@
       </c>
       <c r="R37" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="38" spans="1:18">
@@ -39742,31 +39796,31 @@
       </c>
       <c r="B38" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '19', </v>
+        <v/>
       </c>
       <c r="D38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'List Layout', </v>
+        <v/>
       </c>
       <c r="E38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Layout of a list', </v>
+        <v/>
       </c>
       <c r="F38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Layout', </v>
+        <v/>
       </c>
       <c r="G38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H38" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '25', </v>
+        <v/>
       </c>
       <c r="I38" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -39806,7 +39860,7 @@
       </c>
       <c r="R38" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="39" spans="1:18">
@@ -39815,31 +39869,31 @@
       </c>
       <c r="B39" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C39" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '26', </v>
+        <v/>
       </c>
       <c r="D39" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Nested Relation', </v>
+        <v/>
       </c>
       <c r="E39" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Nested Relation', </v>
+        <v/>
       </c>
       <c r="F39" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Nest', </v>
+        <v/>
       </c>
       <c r="G39" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H39" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
+        <v/>
       </c>
       <c r="I39" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -39879,7 +39933,7 @@
       </c>
       <c r="R39" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="40" spans="1:18">
@@ -39888,31 +39942,31 @@
       </c>
       <c r="B40" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C40" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '26', </v>
+        <v/>
       </c>
       <c r="D40" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Related Resource', </v>
+        <v/>
       </c>
       <c r="E40" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Related Resource Details', </v>
+        <v/>
       </c>
       <c r="F40" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
+        <v/>
       </c>
       <c r="G40" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
+        <v/>
       </c>
       <c r="H40" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
+        <v/>
       </c>
       <c r="I40" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -39952,7 +40006,7 @@
       </c>
       <c r="R40" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="41" spans="1:18">
@@ -39961,31 +40015,31 @@
       </c>
       <c r="B41" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C41" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '26', </v>
+        <v/>
       </c>
       <c r="D41" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Form Layout', </v>
+        <v/>
       </c>
       <c r="E41" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Layout details', </v>
+        <v/>
       </c>
       <c r="F41" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Layout', </v>
+        <v/>
       </c>
       <c r="G41" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H41" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '27', </v>
+        <v/>
       </c>
       <c r="I41" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -40025,7 +40079,7 @@
       </c>
       <c r="R41" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="42" spans="1:18">
@@ -40034,31 +40088,31 @@
       </c>
       <c r="B42" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C42" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '23', </v>
+        <v/>
       </c>
       <c r="D42" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Data View Section', </v>
+        <v/>
       </c>
       <c r="E42" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Section details of data view', </v>
+        <v/>
       </c>
       <c r="F42" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Sections', </v>
+        <v/>
       </c>
       <c r="G42" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H42" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '28', </v>
+        <v/>
       </c>
       <c r="I42" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -40098,7 +40152,7 @@
       </c>
       <c r="R42" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="43" spans="1:18">
@@ -40107,31 +40161,31 @@
       </c>
       <c r="B43" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C43" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '26', </v>
+        <v/>
       </c>
       <c r="D43" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Data View Section Items', </v>
+        <v/>
       </c>
       <c r="E43" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Items of a data view section', </v>
+        <v/>
       </c>
       <c r="F43" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Items', </v>
+        <v/>
       </c>
       <c r="G43" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H43" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '29', </v>
+        <v/>
       </c>
       <c r="I43" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -40171,7 +40225,7 @@
       </c>
       <c r="R43" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="44" spans="1:18">
@@ -40180,31 +40234,31 @@
       </c>
       <c r="B44" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C44" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '28', </v>
+        <v/>
       </c>
       <c r="D44" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Data Relation', </v>
+        <v/>
       </c>
       <c r="E44" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'View relation of a data', </v>
+        <v/>
       </c>
       <c r="F44" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
+        <v/>
       </c>
       <c r="G44" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
+        <v/>
       </c>
       <c r="H44" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
+        <v/>
       </c>
       <c r="I44" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -40244,7 +40298,7 @@
       </c>
       <c r="R44" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="45" spans="1:18">
@@ -40253,31 +40307,31 @@
       </c>
       <c r="B45" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C45" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '29', </v>
+        <v/>
       </c>
       <c r="D45" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Data item relation', </v>
+        <v/>
       </c>
       <c r="E45" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'View relation of a data item', </v>
+        <v/>
       </c>
       <c r="F45" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
+        <v/>
       </c>
       <c r="G45" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
+        <v/>
       </c>
       <c r="H45" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
+        <v/>
       </c>
       <c r="I45" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -40317,7 +40371,7 @@
       </c>
       <c r="R45" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="46" spans="1:18">
@@ -40326,31 +40380,31 @@
       </c>
       <c r="B46" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C46" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '26', </v>
+        <v/>
       </c>
       <c r="D46" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Owner Relation', </v>
+        <v/>
       </c>
       <c r="E46" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'View the owner resource', </v>
+        <v/>
       </c>
       <c r="F46" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Owner', </v>
+        <v/>
       </c>
       <c r="G46" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
+        <v/>
       </c>
       <c r="H46" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
+        <v/>
       </c>
       <c r="I46" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -40390,7 +40444,7 @@
       </c>
       <c r="R46" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="47" spans="1:18">
@@ -40399,31 +40453,31 @@
       </c>
       <c r="B47" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C47" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '12', </v>
+        <v/>
       </c>
       <c r="D47" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Collections', </v>
+        <v/>
       </c>
       <c r="E47" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Collection/Detail form', </v>
+        <v/>
       </c>
       <c r="F47" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Collections', </v>
+        <v/>
       </c>
       <c r="G47" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H47" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '30', </v>
+        <v/>
       </c>
       <c r="I47" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -40463,7 +40517,7 @@
       </c>
       <c r="R47" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="48" spans="1:18">
@@ -40472,31 +40526,31 @@
       </c>
       <c r="B48" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C48" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '30', </v>
+        <v/>
       </c>
       <c r="D48" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Collection Form', </v>
+        <v/>
       </c>
       <c r="E48" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Collection Form', </v>
+        <v/>
       </c>
       <c r="F48" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Form', </v>
+        <v/>
       </c>
       <c r="G48" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
+        <v/>
       </c>
       <c r="H48" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '12', </v>
+        <v/>
       </c>
       <c r="I48" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -40536,7 +40590,7 @@
       </c>
       <c r="R48" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="49" spans="1:18">
@@ -40545,31 +40599,31 @@
       </c>
       <c r="B49" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C49" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '30', </v>
+        <v/>
       </c>
       <c r="D49" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Relation', </v>
+        <v/>
       </c>
       <c r="E49" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Details of Relation', </v>
+        <v/>
       </c>
       <c r="F49" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
+        <v/>
       </c>
       <c r="G49" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
+        <v/>
       </c>
       <c r="H49" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
+        <v/>
       </c>
       <c r="I49" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -40609,7 +40663,7 @@
       </c>
       <c r="R49" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="50" spans="1:18">
@@ -40618,31 +40672,31 @@
       </c>
       <c r="B50" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C50" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '15', </v>
+        <v/>
       </c>
       <c r="D50" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Field', </v>
+        <v/>
       </c>
       <c r="E50" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Field details', </v>
+        <v/>
       </c>
       <c r="F50" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Field', </v>
+        <v/>
       </c>
       <c r="G50" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
+        <v/>
       </c>
       <c r="H50" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '13', </v>
+        <v/>
       </c>
       <c r="I50" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -40682,7 +40736,7 @@
       </c>
       <c r="R50" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="51" spans="1:18">
@@ -40691,31 +40745,31 @@
       </c>
       <c r="B51" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C51" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '13', </v>
+        <v/>
       </c>
       <c r="D51" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Form', </v>
+        <v/>
       </c>
       <c r="E51" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Form details', </v>
+        <v/>
       </c>
       <c r="F51" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Form', </v>
+        <v/>
       </c>
       <c r="G51" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
+        <v/>
       </c>
       <c r="H51" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '12', </v>
+        <v/>
       </c>
       <c r="I51" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -40755,7 +40809,7 @@
       </c>
       <c r="R51" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="52" spans="1:18">
@@ -40764,7 +40818,7 @@
       </c>
       <c r="B52" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>;</v>
+        <v/>
       </c>
       <c r="C52" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -40837,7 +40891,7 @@
       </c>
       <c r="B53" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
+        <v/>
       </c>
       <c r="C53" s="33" t="str">
         <f t="shared" ca="1" si="3"/>

</xml_diff>

<commit_message>
Field Option table modified
</commit_message>
<xml_diff>
--- a/Helper.xlsx
+++ b/Helper.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3230" uniqueCount="667">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3232" uniqueCount="667">
   <si>
     <t>resource_scopes</t>
   </si>
@@ -4634,8 +4634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7700,8 +7700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I133"/>
   <sheetViews>
-    <sheetView topLeftCell="A110" workbookViewId="0">
-      <selection activeCell="A134" sqref="A134"/>
+    <sheetView topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="C133" sqref="C133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="15"/>
@@ -10577,10 +10577,10 @@
         <v>666</v>
       </c>
       <c r="B133" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="C133" s="4" t="s">
         <v>204</v>
-      </c>
-      <c r="C133" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="D133" s="4">
         <v>128</v>
@@ -10625,7 +10625,7 @@
   <dimension ref="A1:K308"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B258" sqref="B258"/>
+      <selection activeCell="B257" sqref="B257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="15"/>
@@ -21724,11 +21724,11 @@
       </c>
       <c r="C253" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>detail(</v>
+        <v>text(</v>
       </c>
       <c r="D253" s="4" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'method'</v>
+        <v>'detail'</v>
       </c>
       <c r="E253" s="7" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -21756,7 +21756,7 @@
       </c>
       <c r="K253" s="4" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;detail('method', 128)-&gt;nullable();</v>
+        <v>$table-&gt;text('detail', 128)-&gt;nullable();</v>
       </c>
     </row>
     <row r="254" spans="1:11">
@@ -24202,7 +24202,7 @@
   <dimension ref="A1:R279"/>
   <sheetViews>
     <sheetView topLeftCell="B213" workbookViewId="0">
-      <selection activeCell="D279" sqref="D279"/>
+      <selection activeCell="F279" sqref="F279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -34435,8 +34435,12 @@
         <f>COUNTIF($B$1:$B278,[Table Name])</f>
         <v>0</v>
       </c>
-      <c r="D279" s="40"/>
-      <c r="E279" s="40"/>
+      <c r="D279" s="40" t="s">
+        <v>122</v>
+      </c>
+      <c r="E279" s="40" t="s">
+        <v>49</v>
+      </c>
       <c r="F279" s="40"/>
       <c r="G279" s="40"/>
       <c r="H279" s="40"/>

</xml_diff>

<commit_message>
Seeder which does not exists are created
</commit_message>
<xml_diff>
--- a/Helper.xlsx
+++ b/Helper.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3253" uniqueCount="670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3258" uniqueCount="671">
   <si>
     <t>resource_scopes</t>
   </si>
@@ -2048,6 +2048,9 @@
   </si>
   <si>
     <t>Length/Enum</t>
+  </si>
+  <si>
+    <t>Data Scopes</t>
   </si>
 </sst>
 </file>
@@ -2277,31 +2280,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="125">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="123">
     <dxf>
       <font>
         <strike val="0"/>
@@ -4075,35 +4054,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tables" displayName="Tables" ref="A1:J36" totalsRowShown="0" dataDxfId="124">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tables" displayName="Tables" ref="A1:J36" totalsRowShown="0" dataDxfId="122">
   <autoFilter ref="A1:J36"/>
   <tableColumns count="10">
-    <tableColumn id="2" name="Name" dataDxfId="123"/>
-    <tableColumn id="10" name="Table" dataDxfId="122">
+    <tableColumn id="2" name="Name" dataDxfId="121"/>
+    <tableColumn id="10" name="Table" dataDxfId="120">
       <calculatedColumnFormula>"__"&amp;[Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Singular Name" dataDxfId="121">
+    <tableColumn id="5" name="Singular Name" dataDxfId="119">
       <calculatedColumnFormula>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Model NS" dataDxfId="120">
+    <tableColumn id="8" name="Model NS" dataDxfId="118">
       <calculatedColumnFormula>"Milestone\Appframe\Model"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Class Name" dataDxfId="119">
+    <tableColumn id="4" name="Class Name" dataDxfId="117">
       <calculatedColumnFormula>SUBSTITUTE(PROPER([Singular Name]),"_","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Migration Artisan" dataDxfId="118">
+    <tableColumn id="1" name="Migration Artisan" dataDxfId="116">
       <calculatedColumnFormula>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Model Artisan" dataDxfId="117">
+    <tableColumn id="6" name="Model Artisan" dataDxfId="115">
       <calculatedColumnFormula>"php artisan make:model "&amp;[Class Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Model Statement" dataDxfId="116">
+    <tableColumn id="3" name="Model Statement" dataDxfId="114">
       <calculatedColumnFormula>"protected $table = '"&amp;[Table]&amp;"';"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Seeder Artisan" dataDxfId="115">
+    <tableColumn id="7" name="Seeder Artisan" dataDxfId="113">
       <calculatedColumnFormula>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Seeder Class" dataDxfId="114">
+    <tableColumn id="9" name="Seeder Class" dataDxfId="112">
       <calculatedColumnFormula>[Class Name]&amp;"TableSeeder"&amp;"::class,"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4112,56 +4091,56 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="ResourceActions" displayName="ResourceActions" ref="A1:P9" totalsRowShown="0" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="ResourceActions" displayName="ResourceActions" ref="A1:P9" totalsRowShown="0" dataDxfId="16">
   <autoFilter ref="A1:P9"/>
   <tableColumns count="16">
-    <tableColumn id="1" name="No" dataDxfId="17">
+    <tableColumn id="1" name="No" dataDxfId="15">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Resource" dataDxfId="16"/>
-    <tableColumn id="13" name="Resource Id" dataDxfId="15">
+    <tableColumn id="2" name="Resource" dataDxfId="14"/>
+    <tableColumn id="13" name="Resource Id" dataDxfId="13">
       <calculatedColumnFormula>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Action Name" dataDxfId="14"/>
-    <tableColumn id="4" name="Description" dataDxfId="13"/>
-    <tableColumn id="5" name="Action Title" dataDxfId="12"/>
-    <tableColumn id="6" name="Button Type" dataDxfId="11"/>
-    <tableColumn id="7" name="Menu" dataDxfId="10"/>
-    <tableColumn id="8" name="Icon" dataDxfId="9"/>
-    <tableColumn id="9" name="Set" dataDxfId="8"/>
-    <tableColumn id="14" name="Action Type" dataDxfId="7"/>
-    <tableColumn id="15" name="ID1" dataDxfId="6"/>
-    <tableColumn id="16" name="ID2" dataDxfId="5"/>
-    <tableColumn id="10" name="On" dataDxfId="4"/>
-    <tableColumn id="11" name="Confirm" dataDxfId="3"/>
-    <tableColumn id="12" name="handler" dataDxfId="2"/>
+    <tableColumn id="3" name="Action Name" dataDxfId="12"/>
+    <tableColumn id="4" name="Description" dataDxfId="11"/>
+    <tableColumn id="5" name="Action Title" dataDxfId="10"/>
+    <tableColumn id="6" name="Button Type" dataDxfId="9"/>
+    <tableColumn id="7" name="Menu" dataDxfId="8"/>
+    <tableColumn id="8" name="Icon" dataDxfId="7"/>
+    <tableColumn id="9" name="Set" dataDxfId="6"/>
+    <tableColumn id="14" name="Action Type" dataDxfId="5"/>
+    <tableColumn id="15" name="ID1" dataDxfId="4"/>
+    <tableColumn id="16" name="ID2" dataDxfId="3"/>
+    <tableColumn id="10" name="On" dataDxfId="2"/>
+    <tableColumn id="11" name="Confirm" dataDxfId="1"/>
+    <tableColumn id="12" name="handler" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Columns" displayName="Columns" ref="A1:I135" totalsRowShown="0" dataDxfId="107">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Columns" displayName="Columns" ref="A1:I135" totalsRowShown="0" dataDxfId="105">
   <autoFilter ref="A1:I135">
     <filterColumn colId="0"/>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" name="Column" dataDxfId="106"/>
-    <tableColumn id="2" name="Type" dataDxfId="105"/>
-    <tableColumn id="3" name="Name" dataDxfId="104"/>
-    <tableColumn id="4" name="Length/Enum" dataDxfId="103"/>
-    <tableColumn id="5" name="Method1" dataDxfId="102"/>
-    <tableColumn id="6" name="Method2" dataDxfId="101"/>
-    <tableColumn id="7" name="Method3" dataDxfId="100"/>
-    <tableColumn id="8" name="Method4" dataDxfId="99"/>
-    <tableColumn id="9" name="Method5" dataDxfId="98"/>
+    <tableColumn id="1" name="Column" dataDxfId="104"/>
+    <tableColumn id="2" name="Type" dataDxfId="103"/>
+    <tableColumn id="3" name="Name" dataDxfId="102"/>
+    <tableColumn id="4" name="Length/Enum" dataDxfId="101"/>
+    <tableColumn id="5" name="Method1" dataDxfId="100"/>
+    <tableColumn id="6" name="Method2" dataDxfId="99"/>
+    <tableColumn id="7" name="Method3" dataDxfId="98"/>
+    <tableColumn id="8" name="Method4" dataDxfId="97"/>
+    <tableColumn id="9" name="Method5" dataDxfId="96"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TableFields" displayName="TableFields" ref="A1:K310" totalsRowShown="0" dataDxfId="97">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TableFields" displayName="TableFields" ref="A1:K310" totalsRowShown="0" dataDxfId="95">
   <autoFilter ref="A1:K310">
     <filterColumn colId="0">
       <filters>
@@ -4170,33 +4149,33 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="11">
-    <tableColumn id="2" name="Table" dataDxfId="96"/>
-    <tableColumn id="3" name="Field" dataDxfId="95"/>
-    <tableColumn id="5" name="Type" dataDxfId="94">
+    <tableColumn id="2" name="Table" dataDxfId="94"/>
+    <tableColumn id="3" name="Field" dataDxfId="93"/>
+    <tableColumn id="5" name="Type" dataDxfId="92">
       <calculatedColumnFormula>VLOOKUP([Field],Columns[],2,0)&amp;"("</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Name" dataDxfId="93">
+    <tableColumn id="4" name="Name" dataDxfId="91">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Arg2" dataDxfId="92">
+    <tableColumn id="6" name="Arg2" dataDxfId="90">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Method1" dataDxfId="91">
+    <tableColumn id="7" name="Method1" dataDxfId="89">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Method2" dataDxfId="90">
+    <tableColumn id="8" name="Method2" dataDxfId="88">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Method3" dataDxfId="89">
+    <tableColumn id="9" name="Method3" dataDxfId="87">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Method4" dataDxfId="88">
+    <tableColumn id="10" name="Method4" dataDxfId="86">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Method5" dataDxfId="87">
+    <tableColumn id="11" name="Method5" dataDxfId="85">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Statement" dataDxfId="86">
+    <tableColumn id="12" name="Statement" dataDxfId="84">
       <calculatedColumnFormula>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4205,51 +4184,51 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R280" totalsRowShown="0" headerRowDxfId="85" dataDxfId="84">
-  <autoFilter ref="A1:R280">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R281" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
+  <autoFilter ref="A1:R281">
     <filterColumn colId="1"/>
   </autoFilter>
   <tableColumns count="18">
-    <tableColumn id="19" name="TRCode" dataDxfId="83">
+    <tableColumn id="19" name="TRCode" dataDxfId="81">
       <calculatedColumnFormula>[Table Name]&amp;"-"&amp;[Record No]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Table Name" dataDxfId="82"/>
-    <tableColumn id="2" name="Record No" dataDxfId="81">
+    <tableColumn id="1" name="Table Name" dataDxfId="80"/>
+    <tableColumn id="2" name="Record No" dataDxfId="79">
       <calculatedColumnFormula>COUNTIF($B$1:$B1,[Table Name])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="1" dataDxfId="80"/>
-    <tableColumn id="4" name="2" dataDxfId="79"/>
-    <tableColumn id="5" name="3" dataDxfId="78"/>
-    <tableColumn id="6" name="4" dataDxfId="77"/>
-    <tableColumn id="7" name="5" dataDxfId="76"/>
-    <tableColumn id="8" name="6" dataDxfId="75"/>
-    <tableColumn id="9" name="7" dataDxfId="74"/>
-    <tableColumn id="10" name="8" dataDxfId="73"/>
-    <tableColumn id="11" name="9" dataDxfId="72"/>
-    <tableColumn id="12" name="10" dataDxfId="71"/>
-    <tableColumn id="13" name="11" dataDxfId="70"/>
-    <tableColumn id="14" name="12" dataDxfId="69"/>
-    <tableColumn id="15" name="13" dataDxfId="68"/>
-    <tableColumn id="16" name="14" dataDxfId="67"/>
-    <tableColumn id="17" name="15" dataDxfId="66"/>
+    <tableColumn id="3" name="1" dataDxfId="78"/>
+    <tableColumn id="4" name="2" dataDxfId="77"/>
+    <tableColumn id="5" name="3" dataDxfId="76"/>
+    <tableColumn id="6" name="4" dataDxfId="75"/>
+    <tableColumn id="7" name="5" dataDxfId="74"/>
+    <tableColumn id="8" name="6" dataDxfId="73"/>
+    <tableColumn id="9" name="7" dataDxfId="72"/>
+    <tableColumn id="10" name="8" dataDxfId="71"/>
+    <tableColumn id="11" name="9" dataDxfId="70"/>
+    <tableColumn id="12" name="10" dataDxfId="69"/>
+    <tableColumn id="13" name="11" dataDxfId="68"/>
+    <tableColumn id="14" name="12" dataDxfId="67"/>
+    <tableColumn id="15" name="13" dataDxfId="66"/>
+    <tableColumn id="16" name="14" dataDxfId="65"/>
+    <tableColumn id="17" name="15" dataDxfId="64"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SeedMap" displayName="SeedMap" ref="A1:E29" totalsRowShown="0" dataDxfId="65">
-  <autoFilter ref="A1:E29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SeedMap" displayName="SeedMap" ref="A1:E30" totalsRowShown="0" dataDxfId="63">
+  <autoFilter ref="A1:E30"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Name" dataDxfId="64"/>
-    <tableColumn id="3" name="FW Table Name" dataDxfId="63"/>
-    <tableColumn id="20" name="NS" dataDxfId="62">
+    <tableColumn id="1" name="Name" dataDxfId="62"/>
+    <tableColumn id="3" name="FW Table Name" dataDxfId="61"/>
+    <tableColumn id="20" name="NS" dataDxfId="60">
       <calculatedColumnFormula>VLOOKUP([FW Table Name],Tables[],4,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="Model" dataDxfId="61">
+    <tableColumn id="21" name="Model" dataDxfId="59">
       <calculatedColumnFormula>VLOOKUP([FW Table Name],Tables[],5,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Query Method" dataDxfId="60">
+    <tableColumn id="4" name="Query Method" dataDxfId="58">
       <calculatedColumnFormula>"truncate"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4258,46 +4237,46 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="ResourceTable" displayName="ResourceTable" ref="A1:I31" totalsRowShown="0" dataDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="ResourceTable" displayName="ResourceTable" ref="A1:I31" totalsRowShown="0" dataDxfId="57">
   <autoFilter ref="A1:I31"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="No" dataDxfId="58">
+    <tableColumn id="1" name="No" dataDxfId="56">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Name" dataDxfId="57"/>
-    <tableColumn id="3" name="Description" dataDxfId="56"/>
-    <tableColumn id="4" name="Title" dataDxfId="55"/>
-    <tableColumn id="5" name="NS" dataDxfId="54">
+    <tableColumn id="2" name="Name" dataDxfId="55"/>
+    <tableColumn id="3" name="Description" dataDxfId="54"/>
+    <tableColumn id="4" name="Title" dataDxfId="53"/>
+    <tableColumn id="5" name="NS" dataDxfId="52">
       <calculatedColumnFormula>"Milestone\Appframe\Model"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Table" dataDxfId="53"/>
-    <tableColumn id="7" name="Key" dataDxfId="52">
+    <tableColumn id="6" name="Table" dataDxfId="51"/>
+    <tableColumn id="7" name="Key" dataDxfId="50">
       <calculatedColumnFormula>"id"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Controller" dataDxfId="51"/>
-    <tableColumn id="9" name="Controller NS" dataDxfId="50"/>
+    <tableColumn id="8" name="Controller" dataDxfId="49"/>
+    <tableColumn id="9" name="Controller NS" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RelationTable" displayName="RelationTable" ref="A1:I44" totalsRowShown="0" dataDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RelationTable" displayName="RelationTable" ref="A1:I44" totalsRowShown="0" dataDxfId="47">
   <autoFilter ref="A1:I44"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="No" dataDxfId="48">
+    <tableColumn id="1" name="No" dataDxfId="46">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Resource" dataDxfId="47"/>
-    <tableColumn id="4" name="Relate Resource" dataDxfId="46"/>
-    <tableColumn id="2" name="Resource Id" dataDxfId="45">
+    <tableColumn id="3" name="Resource" dataDxfId="45"/>
+    <tableColumn id="4" name="Relate Resource" dataDxfId="44"/>
+    <tableColumn id="2" name="Resource Id" dataDxfId="43">
       <calculatedColumnFormula>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Name" dataDxfId="44"/>
-    <tableColumn id="6" name="Description" dataDxfId="43"/>
-    <tableColumn id="7" name="Method" dataDxfId="42"/>
-    <tableColumn id="8" name="Type" dataDxfId="41"/>
-    <tableColumn id="10" name="Relate Id" dataDxfId="40">
+    <tableColumn id="5" name="Name" dataDxfId="42"/>
+    <tableColumn id="6" name="Description" dataDxfId="41"/>
+    <tableColumn id="7" name="Method" dataDxfId="40"/>
+    <tableColumn id="8" name="Type" dataDxfId="39"/>
+    <tableColumn id="10" name="Relate Id" dataDxfId="38">
       <calculatedColumnFormula>VLOOKUP([Relate Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4306,47 +4285,47 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="ResourceForms" displayName="ResourceForms" ref="A1:G9" totalsRowShown="0" dataDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="ResourceForms" displayName="ResourceForms" ref="A1:G9" totalsRowShown="0" dataDxfId="37">
   <autoFilter ref="A1:G9"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="No" dataDxfId="38">
+    <tableColumn id="1" name="No" dataDxfId="36">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Resource ID" dataDxfId="37"/>
-    <tableColumn id="3" name="Resource Name" dataDxfId="36">
+    <tableColumn id="2" name="Resource ID" dataDxfId="35"/>
+    <tableColumn id="3" name="Resource Name" dataDxfId="34">
       <calculatedColumnFormula>VLOOKUP([Resource ID],ResourceTable[],2,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Form Name" dataDxfId="35"/>
-    <tableColumn id="6" name="Title" dataDxfId="34"/>
-    <tableColumn id="7" name="Action Text" dataDxfId="33"/>
-    <tableColumn id="8" name="Description" dataDxfId="32"/>
+    <tableColumn id="4" name="Form Name" dataDxfId="33"/>
+    <tableColumn id="6" name="Title" dataDxfId="32"/>
+    <tableColumn id="7" name="Action Text" dataDxfId="31"/>
+    <tableColumn id="8" name="Description" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="FormFields" displayName="FormFields" ref="A1:L33" totalsRowShown="0" dataDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="FormFields" displayName="FormFields" ref="A1:L33" totalsRowShown="0" dataDxfId="29">
   <autoFilter ref="A1:L33"/>
   <tableColumns count="12">
-    <tableColumn id="9" name="No" dataDxfId="30">
+    <tableColumn id="9" name="No" dataDxfId="28">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Form Id" dataDxfId="29"/>
-    <tableColumn id="7" name="Form Name" dataDxfId="28">
+    <tableColumn id="1" name="Form Id" dataDxfId="27"/>
+    <tableColumn id="7" name="Form Name" dataDxfId="26">
       <calculatedColumnFormula>VLOOKUP([Form Id],ResourceForms[],4,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Name" dataDxfId="27"/>
-    <tableColumn id="2" name="Type" dataDxfId="26"/>
-    <tableColumn id="5" name="Label" dataDxfId="25"/>
-    <tableColumn id="6" name="Collection" dataDxfId="24"/>
-    <tableColumn id="14" name="Attribute" dataDxfId="23">
+    <tableColumn id="4" name="Name" dataDxfId="25"/>
+    <tableColumn id="2" name="Type" dataDxfId="24"/>
+    <tableColumn id="5" name="Label" dataDxfId="23"/>
+    <tableColumn id="6" name="Collection" dataDxfId="22"/>
+    <tableColumn id="14" name="Attribute" dataDxfId="21">
       <calculatedColumnFormula>[Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Relation" dataDxfId="22"/>
-    <tableColumn id="11" name="Deep 1" dataDxfId="21"/>
-    <tableColumn id="12" name="Deep 2" dataDxfId="20"/>
-    <tableColumn id="13" name="Deep 3" dataDxfId="19"/>
+    <tableColumn id="10" name="Relation" dataDxfId="20"/>
+    <tableColumn id="11" name="Deep 1" dataDxfId="19"/>
+    <tableColumn id="12" name="Deep 2" dataDxfId="18"/>
+    <tableColumn id="13" name="Deep 3" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -10648,22 +10627,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A43:A46">
-    <cfRule type="duplicateValues" dxfId="113" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="111" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56:A59">
-    <cfRule type="duplicateValues" dxfId="112" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="110" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A135">
-    <cfRule type="duplicateValues" dxfId="111" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="109" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A128:A129">
-    <cfRule type="duplicateValues" dxfId="110" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="108" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A128:A129">
-    <cfRule type="duplicateValues" dxfId="109" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="107" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A130:A131">
-    <cfRule type="duplicateValues" dxfId="108" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="106" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -24340,10 +24319,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R280"/>
+  <dimension ref="A1:R281"/>
   <sheetViews>
     <sheetView topLeftCell="B268" workbookViewId="0">
-      <selection activeCell="D281" sqref="D281"/>
+      <selection activeCell="B282" sqref="B282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -34632,6 +34611,38 @@
       <c r="Q280" s="40"/>
       <c r="R280" s="40"/>
     </row>
+    <row r="281" spans="1:18">
+      <c r="A281" s="22" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Data Scopes-0</v>
+      </c>
+      <c r="B281" s="40" t="s">
+        <v>670</v>
+      </c>
+      <c r="C281" s="22">
+        <f>COUNTIF($B$1:$B280,[Table Name])</f>
+        <v>0</v>
+      </c>
+      <c r="D281" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="E281" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="F281" s="40"/>
+      <c r="G281" s="40"/>
+      <c r="H281" s="40"/>
+      <c r="I281" s="40"/>
+      <c r="J281" s="40"/>
+      <c r="K281" s="40"/>
+      <c r="L281" s="40"/>
+      <c r="M281" s="40"/>
+      <c r="N281" s="40"/>
+      <c r="O281" s="40"/>
+      <c r="P281" s="40"/>
+      <c r="Q281" s="40"/>
+      <c r="R281" s="40"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
@@ -34643,10 +34654,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -35237,12 +35248,32 @@
         <v>truncate</v>
       </c>
     </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="4" t="s">
+        <v>670</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>567</v>
+      </c>
+      <c r="C30" s="4" t="str">
+        <f>VLOOKUP([FW Table Name],Tables[],4,0)</f>
+        <v>Milestone\Appframe\Model</v>
+      </c>
+      <c r="D30" s="4" t="str">
+        <f>VLOOKUP([FW Table Name],Tables[],5,0)</f>
+        <v>ResourceDataScope</v>
+      </c>
+      <c r="E30" s="7" t="str">
+        <f>"truncate"</f>
+        <v>truncate</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E29">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E30">
       <formula1>"truncate,query"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B29">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B30">
       <formula1>TableNames</formula1>
     </dataValidation>
   </dataValidations>
@@ -37602,7 +37633,7 @@
   <dimension ref="A1:T109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -37612,14 +37643,14 @@
   <sheetData>
     <row r="1" spans="1:20" s="38" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="48" t="s">
-        <v>656</v>
+        <v>464</v>
       </c>
       <c r="B1" s="48"/>
       <c r="C1" s="48"/>
       <c r="D1" s="48"/>
       <c r="E1" s="49" t="str">
         <f>"\"&amp;VLOOKUP($A$1,SeedMap[],3,0)&amp;"\"&amp;VLOOKUP($A$1,SeedMap[],4,0)&amp;"::"&amp;VLOOKUP($A$1,SeedMap[],5,0)&amp;"()"</f>
-        <v>\Milestone\Appframe\Model\ResourceFormCollection::truncate()</v>
+        <v>\Milestone\Appframe\Model\ResourceFormFieldOption::truncate()</v>
       </c>
       <c r="F1" s="49"/>
       <c r="G1" s="49"/>
@@ -37763,19 +37794,19 @@
       <c r="B5" s="28"/>
       <c r="C5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],C$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],C$4+$B$4,0))</f>
-        <v>resource_form</v>
+        <v>form_field</v>
       </c>
       <c r="D5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],D$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],D$4+$B$4,0))</f>
-        <v>collection_form</v>
+        <v>type</v>
       </c>
       <c r="E5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0))</f>
-        <v>relation</v>
+        <v/>
       </c>
       <c r="F5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0))</f>
-        <v>foreign_field</v>
+        <v/>
       </c>
       <c r="G5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0))</f>
@@ -37877,7 +37908,7 @@
       <c r="A8" s="32"/>
       <c r="B8" s="47" t="str">
         <f>$E$1</f>
-        <v>\Milestone\Appframe\Model\ResourceFormCollection::truncate()</v>
+        <v>\Milestone\Appframe\Model\ResourceFormFieldOption::truncate()</v>
       </c>
       <c r="C8" s="47"/>
       <c r="D8" s="47"/>

</xml_diff>

<commit_message>
Resources added to Developer role
</commit_message>
<xml_diff>
--- a/Helper.xlsx
+++ b/Helper.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3258" uniqueCount="671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3281" uniqueCount="671">
   <si>
     <t>resource_scopes</t>
   </si>
@@ -4184,9 +4184,13 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R281" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
-  <autoFilter ref="A1:R281">
-    <filterColumn colId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R304" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
+  <autoFilter ref="A1:R304">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Resource Roles"/>
+      </filters>
+    </filterColumn>
   </autoFilter>
   <tableColumns count="18">
     <tableColumn id="19" name="TRCode" dataDxfId="81">
@@ -4618,8 +4622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -24319,10 +24323,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R281"/>
+  <dimension ref="A1:R304"/>
   <sheetViews>
-    <sheetView topLeftCell="B268" workbookViewId="0">
-      <selection activeCell="B282" sqref="B282"/>
+    <sheetView topLeftCell="B29" workbookViewId="0">
+      <selection activeCell="D282" sqref="D282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -24389,7 +24393,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" hidden="1">
       <c r="A2" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Groups-0</v>
@@ -24423,7 +24427,7 @@
       <c r="Q2" s="15"/>
       <c r="R2" s="15"/>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" hidden="1">
       <c r="A3" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Groups-1</v>
@@ -24457,7 +24461,7 @@
       <c r="Q3" s="16"/>
       <c r="R3" s="16"/>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" hidden="1">
       <c r="A4" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Groups-2</v>
@@ -24491,7 +24495,7 @@
       <c r="Q4" s="16"/>
       <c r="R4" s="16"/>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" hidden="1">
       <c r="A5" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Groups-3</v>
@@ -24525,7 +24529,7 @@
       <c r="Q5" s="16"/>
       <c r="R5" s="16"/>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" hidden="1">
       <c r="A6" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Roles-0</v>
@@ -24559,7 +24563,7 @@
       <c r="Q6" s="16"/>
       <c r="R6" s="16"/>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" hidden="1">
       <c r="A7" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Roles-1</v>
@@ -24593,7 +24597,7 @@
       <c r="Q7" s="16"/>
       <c r="R7" s="16"/>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" hidden="1">
       <c r="A8" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Roles-2</v>
@@ -24627,7 +24631,7 @@
       <c r="Q8" s="16"/>
       <c r="R8" s="16"/>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" hidden="1">
       <c r="A9" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Roles-3</v>
@@ -24661,7 +24665,7 @@
       <c r="Q9" s="16"/>
       <c r="R9" s="16"/>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" hidden="1">
       <c r="A10" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Group Roles-0</v>
@@ -24693,7 +24697,7 @@
       <c r="Q10" s="16"/>
       <c r="R10" s="16"/>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" hidden="1">
       <c r="A11" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Group Roles-1</v>
@@ -24725,7 +24729,7 @@
       <c r="Q11" s="16"/>
       <c r="R11" s="16"/>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" hidden="1">
       <c r="A12" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Group Roles-2</v>
@@ -24757,7 +24761,7 @@
       <c r="Q12" s="16"/>
       <c r="R12" s="16"/>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" hidden="1">
       <c r="A13" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Group Roles-3</v>
@@ -24789,7 +24793,7 @@
       <c r="Q13" s="16"/>
       <c r="R13" s="16"/>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" hidden="1">
       <c r="A14" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-0</v>
@@ -24833,7 +24837,7 @@
       <c r="Q14" s="16"/>
       <c r="R14" s="16"/>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" hidden="1">
       <c r="A15" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-1</v>
@@ -24873,7 +24877,7 @@
       <c r="Q15" s="15"/>
       <c r="R15" s="15"/>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" hidden="1">
       <c r="A16" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-2</v>
@@ -24913,7 +24917,7 @@
       <c r="Q16" s="15"/>
       <c r="R16" s="15"/>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" hidden="1">
       <c r="A17" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-3</v>
@@ -24953,7 +24957,7 @@
       <c r="Q17" s="15"/>
       <c r="R17" s="15"/>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" hidden="1">
       <c r="A18" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-4</v>
@@ -24993,7 +24997,7 @@
       <c r="Q18" s="15"/>
       <c r="R18" s="15"/>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" hidden="1">
       <c r="A19" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-5</v>
@@ -25033,7 +25037,7 @@
       <c r="Q19" s="15"/>
       <c r="R19" s="15"/>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" hidden="1">
       <c r="A20" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-6</v>
@@ -25073,7 +25077,7 @@
       <c r="Q20" s="15"/>
       <c r="R20" s="15"/>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" hidden="1">
       <c r="A21" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-7</v>
@@ -25113,7 +25117,7 @@
       <c r="Q21" s="15"/>
       <c r="R21" s="15"/>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" hidden="1">
       <c r="A22" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-8</v>
@@ -25153,7 +25157,7 @@
       <c r="Q22" s="15"/>
       <c r="R22" s="15"/>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" hidden="1">
       <c r="A23" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-9</v>
@@ -25193,7 +25197,7 @@
       <c r="Q23" s="15"/>
       <c r="R23" s="15"/>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" hidden="1">
       <c r="A24" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-10</v>
@@ -25233,7 +25237,7 @@
       <c r="Q24" s="15"/>
       <c r="R24" s="15"/>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" hidden="1">
       <c r="A25" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-11</v>
@@ -25273,7 +25277,7 @@
       <c r="Q25" s="15"/>
       <c r="R25" s="15"/>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:18" hidden="1">
       <c r="A26" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-12</v>
@@ -25313,7 +25317,7 @@
       <c r="Q26" s="15"/>
       <c r="R26" s="15"/>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:18" hidden="1">
       <c r="A27" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-13</v>
@@ -25617,7 +25621,7 @@
       <c r="Q35" s="16"/>
       <c r="R35" s="16"/>
     </row>
-    <row r="36" spans="1:18">
+    <row r="36" spans="1:18" hidden="1">
       <c r="A36" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-0</v>
@@ -25657,7 +25661,7 @@
       <c r="Q36" s="16"/>
       <c r="R36" s="16"/>
     </row>
-    <row r="37" spans="1:18">
+    <row r="37" spans="1:18" hidden="1">
       <c r="A37" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-1</v>
@@ -25697,7 +25701,7 @@
       <c r="Q37" s="15"/>
       <c r="R37" s="15"/>
     </row>
-    <row r="38" spans="1:18">
+    <row r="38" spans="1:18" hidden="1">
       <c r="A38" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-2</v>
@@ -25737,7 +25741,7 @@
       <c r="Q38" s="15"/>
       <c r="R38" s="15"/>
     </row>
-    <row r="39" spans="1:18">
+    <row r="39" spans="1:18" hidden="1">
       <c r="A39" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-3</v>
@@ -25777,7 +25781,7 @@
       <c r="Q39" s="15"/>
       <c r="R39" s="15"/>
     </row>
-    <row r="40" spans="1:18">
+    <row r="40" spans="1:18" hidden="1">
       <c r="A40" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-4</v>
@@ -25817,7 +25821,7 @@
       <c r="Q40" s="15"/>
       <c r="R40" s="15"/>
     </row>
-    <row r="41" spans="1:18">
+    <row r="41" spans="1:18" hidden="1">
       <c r="A41" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-5</v>
@@ -25857,7 +25861,7 @@
       <c r="Q41" s="15"/>
       <c r="R41" s="15"/>
     </row>
-    <row r="42" spans="1:18">
+    <row r="42" spans="1:18" hidden="1">
       <c r="A42" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-6</v>
@@ -25897,7 +25901,7 @@
       <c r="Q42" s="15"/>
       <c r="R42" s="15"/>
     </row>
-    <row r="43" spans="1:18">
+    <row r="43" spans="1:18" hidden="1">
       <c r="A43" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-7</v>
@@ -25937,7 +25941,7 @@
       <c r="Q43" s="15"/>
       <c r="R43" s="15"/>
     </row>
-    <row r="44" spans="1:18">
+    <row r="44" spans="1:18" hidden="1">
       <c r="A44" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-8</v>
@@ -25977,7 +25981,7 @@
       <c r="Q44" s="15"/>
       <c r="R44" s="15"/>
     </row>
-    <row r="45" spans="1:18">
+    <row r="45" spans="1:18" hidden="1">
       <c r="A45" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-9</v>
@@ -26017,7 +26021,7 @@
       <c r="Q45" s="15"/>
       <c r="R45" s="15"/>
     </row>
-    <row r="46" spans="1:18">
+    <row r="46" spans="1:18" hidden="1">
       <c r="A46" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-10</v>
@@ -26057,7 +26061,7 @@
       <c r="Q46" s="15"/>
       <c r="R46" s="15"/>
     </row>
-    <row r="47" spans="1:18">
+    <row r="47" spans="1:18" hidden="1">
       <c r="A47" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-11</v>
@@ -26097,7 +26101,7 @@
       <c r="Q47" s="15"/>
       <c r="R47" s="15"/>
     </row>
-    <row r="48" spans="1:18">
+    <row r="48" spans="1:18" hidden="1">
       <c r="A48" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-12</v>
@@ -26137,7 +26141,7 @@
       <c r="Q48" s="15"/>
       <c r="R48" s="15"/>
     </row>
-    <row r="49" spans="1:18">
+    <row r="49" spans="1:18" hidden="1">
       <c r="A49" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-13</v>
@@ -26177,7 +26181,7 @@
       <c r="Q49" s="15"/>
       <c r="R49" s="15"/>
     </row>
-    <row r="50" spans="1:18">
+    <row r="50" spans="1:18" hidden="1">
       <c r="A50" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-14</v>
@@ -26217,7 +26221,7 @@
       <c r="Q50" s="16"/>
       <c r="R50" s="16"/>
     </row>
-    <row r="51" spans="1:18">
+    <row r="51" spans="1:18" hidden="1">
       <c r="A51" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Scopes-0</v>
@@ -26253,7 +26257,7 @@
       <c r="Q51" s="16"/>
       <c r="R51" s="16"/>
     </row>
-    <row r="52" spans="1:18">
+    <row r="52" spans="1:18" hidden="1">
       <c r="A52" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Scopes-1</v>
@@ -26289,7 +26293,7 @@
       <c r="Q52" s="15"/>
       <c r="R52" s="15"/>
     </row>
-    <row r="53" spans="1:18">
+    <row r="53" spans="1:18" hidden="1">
       <c r="A53" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Scopes-2</v>
@@ -26325,7 +26329,7 @@
       <c r="Q53" s="16"/>
       <c r="R53" s="16"/>
     </row>
-    <row r="54" spans="1:18">
+    <row r="54" spans="1:18" hidden="1">
       <c r="A54" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Lists-0</v>
@@ -26361,7 +26365,7 @@
       <c r="Q54" s="16"/>
       <c r="R54" s="16"/>
     </row>
-    <row r="55" spans="1:18">
+    <row r="55" spans="1:18" hidden="1">
       <c r="A55" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Lists-1</v>
@@ -26397,7 +26401,7 @@
       <c r="Q55" s="15"/>
       <c r="R55" s="15"/>
     </row>
-    <row r="56" spans="1:18">
+    <row r="56" spans="1:18" hidden="1">
       <c r="A56" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Lists-2</v>
@@ -26433,7 +26437,7 @@
       <c r="Q56" s="15"/>
       <c r="R56" s="15"/>
     </row>
-    <row r="57" spans="1:18">
+    <row r="57" spans="1:18" hidden="1">
       <c r="A57" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Lists-3</v>
@@ -26469,7 +26473,7 @@
       <c r="Q57" s="15"/>
       <c r="R57" s="15"/>
     </row>
-    <row r="58" spans="1:18">
+    <row r="58" spans="1:18" hidden="1">
       <c r="A58" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Lists-4</v>
@@ -26505,7 +26509,7 @@
       <c r="Q58" s="15"/>
       <c r="R58" s="15"/>
     </row>
-    <row r="59" spans="1:18">
+    <row r="59" spans="1:18" hidden="1">
       <c r="A59" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Lists-5</v>
@@ -26541,7 +26545,7 @@
       <c r="Q59" s="15"/>
       <c r="R59" s="15"/>
     </row>
-    <row r="60" spans="1:18">
+    <row r="60" spans="1:18" hidden="1">
       <c r="A60" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Lists-6</v>
@@ -26577,7 +26581,7 @@
       <c r="Q60" s="16"/>
       <c r="R60" s="16"/>
     </row>
-    <row r="61" spans="1:18">
+    <row r="61" spans="1:18" hidden="1">
       <c r="A61" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource List Scopes-0</v>
@@ -26609,7 +26613,7 @@
       <c r="Q61" s="16"/>
       <c r="R61" s="16"/>
     </row>
-    <row r="62" spans="1:18">
+    <row r="62" spans="1:18" hidden="1">
       <c r="A62" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource List Scopes-1</v>
@@ -26641,7 +26645,7 @@
       <c r="Q62" s="15"/>
       <c r="R62" s="15"/>
     </row>
-    <row r="63" spans="1:18">
+    <row r="63" spans="1:18" hidden="1">
       <c r="A63" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource List Scopes-2</v>
@@ -26673,7 +26677,7 @@
       <c r="Q63" s="16"/>
       <c r="R63" s="16"/>
     </row>
-    <row r="64" spans="1:18">
+    <row r="64" spans="1:18" hidden="1">
       <c r="A64" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Forms-0</v>
@@ -26711,7 +26715,7 @@
       <c r="Q64" s="16"/>
       <c r="R64" s="16"/>
     </row>
-    <row r="65" spans="1:18">
+    <row r="65" spans="1:18" hidden="1">
       <c r="A65" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Forms-1</v>
@@ -26749,7 +26753,7 @@
       <c r="Q65" s="15"/>
       <c r="R65" s="15"/>
     </row>
-    <row r="66" spans="1:18">
+    <row r="66" spans="1:18" hidden="1">
       <c r="A66" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Forms-2</v>
@@ -26787,7 +26791,7 @@
       <c r="Q66" s="15"/>
       <c r="R66" s="15"/>
     </row>
-    <row r="67" spans="1:18">
+    <row r="67" spans="1:18" hidden="1">
       <c r="A67" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Forms-3</v>
@@ -26825,7 +26829,7 @@
       <c r="Q67" s="15"/>
       <c r="R67" s="15"/>
     </row>
-    <row r="68" spans="1:18">
+    <row r="68" spans="1:18" hidden="1">
       <c r="A68" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Forms-4</v>
@@ -26863,7 +26867,7 @@
       <c r="Q68" s="15"/>
       <c r="R68" s="15"/>
     </row>
-    <row r="69" spans="1:18">
+    <row r="69" spans="1:18" hidden="1">
       <c r="A69" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Forms-5</v>
@@ -26901,7 +26905,7 @@
       <c r="Q69" s="15"/>
       <c r="R69" s="15"/>
     </row>
-    <row r="70" spans="1:18">
+    <row r="70" spans="1:18" hidden="1">
       <c r="A70" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Forms-6</v>
@@ -26939,7 +26943,7 @@
       <c r="Q70" s="15"/>
       <c r="R70" s="15"/>
     </row>
-    <row r="71" spans="1:18">
+    <row r="71" spans="1:18" hidden="1">
       <c r="A71" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Forms-7</v>
@@ -26977,7 +26981,7 @@
       <c r="Q71" s="16"/>
       <c r="R71" s="16"/>
     </row>
-    <row r="72" spans="1:18">
+    <row r="72" spans="1:18" hidden="1">
       <c r="A72" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-0</v>
@@ -27015,7 +27019,7 @@
       <c r="Q72" s="16"/>
       <c r="R72" s="16"/>
     </row>
-    <row r="73" spans="1:18">
+    <row r="73" spans="1:18" hidden="1">
       <c r="A73" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-1</v>
@@ -27053,7 +27057,7 @@
       <c r="Q73" s="15"/>
       <c r="R73" s="15"/>
     </row>
-    <row r="74" spans="1:18">
+    <row r="74" spans="1:18" hidden="1">
       <c r="A74" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-2</v>
@@ -27091,7 +27095,7 @@
       <c r="Q74" s="15"/>
       <c r="R74" s="15"/>
     </row>
-    <row r="75" spans="1:18">
+    <row r="75" spans="1:18" hidden="1">
       <c r="A75" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-3</v>
@@ -27129,7 +27133,7 @@
       <c r="Q75" s="15"/>
       <c r="R75" s="15"/>
     </row>
-    <row r="76" spans="1:18">
+    <row r="76" spans="1:18" hidden="1">
       <c r="A76" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-4</v>
@@ -27167,7 +27171,7 @@
       <c r="Q76" s="15"/>
       <c r="R76" s="15"/>
     </row>
-    <row r="77" spans="1:18">
+    <row r="77" spans="1:18" hidden="1">
       <c r="A77" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-5</v>
@@ -27205,7 +27209,7 @@
       <c r="Q77" s="15"/>
       <c r="R77" s="15"/>
     </row>
-    <row r="78" spans="1:18">
+    <row r="78" spans="1:18" hidden="1">
       <c r="A78" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-6</v>
@@ -27243,7 +27247,7 @@
       <c r="Q78" s="15"/>
       <c r="R78" s="15"/>
     </row>
-    <row r="79" spans="1:18">
+    <row r="79" spans="1:18" hidden="1">
       <c r="A79" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-7</v>
@@ -27281,7 +27285,7 @@
       <c r="Q79" s="15"/>
       <c r="R79" s="15"/>
     </row>
-    <row r="80" spans="1:18">
+    <row r="80" spans="1:18" hidden="1">
       <c r="A80" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-8</v>
@@ -27319,7 +27323,7 @@
       <c r="Q80" s="15"/>
       <c r="R80" s="15"/>
     </row>
-    <row r="81" spans="1:18">
+    <row r="81" spans="1:18" hidden="1">
       <c r="A81" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-9</v>
@@ -27357,7 +27361,7 @@
       <c r="Q81" s="15"/>
       <c r="R81" s="15"/>
     </row>
-    <row r="82" spans="1:18">
+    <row r="82" spans="1:18" hidden="1">
       <c r="A82" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-10</v>
@@ -27395,7 +27399,7 @@
       <c r="Q82" s="15"/>
       <c r="R82" s="15"/>
     </row>
-    <row r="83" spans="1:18">
+    <row r="83" spans="1:18" hidden="1">
       <c r="A83" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-11</v>
@@ -27433,7 +27437,7 @@
       <c r="Q83" s="15"/>
       <c r="R83" s="15"/>
     </row>
-    <row r="84" spans="1:18">
+    <row r="84" spans="1:18" hidden="1">
       <c r="A84" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-12</v>
@@ -27471,7 +27475,7 @@
       <c r="Q84" s="15"/>
       <c r="R84" s="15"/>
     </row>
-    <row r="85" spans="1:18">
+    <row r="85" spans="1:18" hidden="1">
       <c r="A85" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-13</v>
@@ -27509,7 +27513,7 @@
       <c r="Q85" s="15"/>
       <c r="R85" s="15"/>
     </row>
-    <row r="86" spans="1:18">
+    <row r="86" spans="1:18" hidden="1">
       <c r="A86" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-14</v>
@@ -27547,7 +27551,7 @@
       <c r="Q86" s="15"/>
       <c r="R86" s="15"/>
     </row>
-    <row r="87" spans="1:18">
+    <row r="87" spans="1:18" hidden="1">
       <c r="A87" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-15</v>
@@ -27585,7 +27589,7 @@
       <c r="Q87" s="15"/>
       <c r="R87" s="15"/>
     </row>
-    <row r="88" spans="1:18">
+    <row r="88" spans="1:18" hidden="1">
       <c r="A88" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-16</v>
@@ -27623,7 +27627,7 @@
       <c r="Q88" s="15"/>
       <c r="R88" s="15"/>
     </row>
-    <row r="89" spans="1:18">
+    <row r="89" spans="1:18" hidden="1">
       <c r="A89" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-17</v>
@@ -27661,7 +27665,7 @@
       <c r="Q89" s="15"/>
       <c r="R89" s="15"/>
     </row>
-    <row r="90" spans="1:18">
+    <row r="90" spans="1:18" hidden="1">
       <c r="A90" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-18</v>
@@ -27699,7 +27703,7 @@
       <c r="Q90" s="15"/>
       <c r="R90" s="15"/>
     </row>
-    <row r="91" spans="1:18">
+    <row r="91" spans="1:18" hidden="1">
       <c r="A91" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-19</v>
@@ -27737,7 +27741,7 @@
       <c r="Q91" s="15"/>
       <c r="R91" s="15"/>
     </row>
-    <row r="92" spans="1:18">
+    <row r="92" spans="1:18" hidden="1">
       <c r="A92" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-20</v>
@@ -27775,7 +27779,7 @@
       <c r="Q92" s="15"/>
       <c r="R92" s="15"/>
     </row>
-    <row r="93" spans="1:18">
+    <row r="93" spans="1:18" hidden="1">
       <c r="A93" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-21</v>
@@ -27813,7 +27817,7 @@
       <c r="Q93" s="15"/>
       <c r="R93" s="15"/>
     </row>
-    <row r="94" spans="1:18">
+    <row r="94" spans="1:18" hidden="1">
       <c r="A94" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-22</v>
@@ -27851,7 +27855,7 @@
       <c r="Q94" s="15"/>
       <c r="R94" s="15"/>
     </row>
-    <row r="95" spans="1:18">
+    <row r="95" spans="1:18" hidden="1">
       <c r="A95" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-23</v>
@@ -27889,7 +27893,7 @@
       <c r="Q95" s="15"/>
       <c r="R95" s="15"/>
     </row>
-    <row r="96" spans="1:18">
+    <row r="96" spans="1:18" hidden="1">
       <c r="A96" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-24</v>
@@ -27927,7 +27931,7 @@
       <c r="Q96" s="15"/>
       <c r="R96" s="15"/>
     </row>
-    <row r="97" spans="1:18">
+    <row r="97" spans="1:18" hidden="1">
       <c r="A97" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-25</v>
@@ -27965,7 +27969,7 @@
       <c r="Q97" s="15"/>
       <c r="R97" s="15"/>
     </row>
-    <row r="98" spans="1:18">
+    <row r="98" spans="1:18" hidden="1">
       <c r="A98" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-26</v>
@@ -28003,7 +28007,7 @@
       <c r="Q98" s="15"/>
       <c r="R98" s="15"/>
     </row>
-    <row r="99" spans="1:18">
+    <row r="99" spans="1:18" hidden="1">
       <c r="A99" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-27</v>
@@ -28041,7 +28045,7 @@
       <c r="Q99" s="15"/>
       <c r="R99" s="15"/>
     </row>
-    <row r="100" spans="1:18">
+    <row r="100" spans="1:18" hidden="1">
       <c r="A100" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-28</v>
@@ -28079,7 +28083,7 @@
       <c r="Q100" s="15"/>
       <c r="R100" s="15"/>
     </row>
-    <row r="101" spans="1:18">
+    <row r="101" spans="1:18" hidden="1">
       <c r="A101" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-29</v>
@@ -28117,7 +28121,7 @@
       <c r="Q101" s="15"/>
       <c r="R101" s="15"/>
     </row>
-    <row r="102" spans="1:18">
+    <row r="102" spans="1:18" hidden="1">
       <c r="A102" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-30</v>
@@ -28155,7 +28159,7 @@
       <c r="Q102" s="15"/>
       <c r="R102" s="15"/>
     </row>
-    <row r="103" spans="1:18">
+    <row r="103" spans="1:18" hidden="1">
       <c r="A103" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-31</v>
@@ -28193,7 +28197,7 @@
       <c r="Q103" s="16"/>
       <c r="R103" s="16"/>
     </row>
-    <row r="104" spans="1:18">
+    <row r="104" spans="1:18" hidden="1">
       <c r="A104" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-0</v>
@@ -28233,7 +28237,7 @@
       <c r="Q104" s="16"/>
       <c r="R104" s="16"/>
     </row>
-    <row r="105" spans="1:18">
+    <row r="105" spans="1:18" hidden="1">
       <c r="A105" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-1</v>
@@ -28265,7 +28269,7 @@
       <c r="Q105" s="16"/>
       <c r="R105" s="16"/>
     </row>
-    <row r="106" spans="1:18">
+    <row r="106" spans="1:18" hidden="1">
       <c r="A106" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-2</v>
@@ -28297,7 +28301,7 @@
       <c r="Q106" s="16"/>
       <c r="R106" s="16"/>
     </row>
-    <row r="107" spans="1:18">
+    <row r="107" spans="1:18" hidden="1">
       <c r="A107" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-3</v>
@@ -28329,7 +28333,7 @@
       <c r="Q107" s="16"/>
       <c r="R107" s="16"/>
     </row>
-    <row r="108" spans="1:18">
+    <row r="108" spans="1:18" hidden="1">
       <c r="A108" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-4</v>
@@ -28361,7 +28365,7 @@
       <c r="Q108" s="16"/>
       <c r="R108" s="16"/>
     </row>
-    <row r="109" spans="1:18">
+    <row r="109" spans="1:18" hidden="1">
       <c r="A109" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-5</v>
@@ -28393,7 +28397,7 @@
       <c r="Q109" s="16"/>
       <c r="R109" s="16"/>
     </row>
-    <row r="110" spans="1:18">
+    <row r="110" spans="1:18" hidden="1">
       <c r="A110" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-6</v>
@@ -28425,7 +28429,7 @@
       <c r="Q110" s="16"/>
       <c r="R110" s="16"/>
     </row>
-    <row r="111" spans="1:18">
+    <row r="111" spans="1:18" hidden="1">
       <c r="A111" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-7</v>
@@ -28457,7 +28461,7 @@
       <c r="Q111" s="16"/>
       <c r="R111" s="16"/>
     </row>
-    <row r="112" spans="1:18">
+    <row r="112" spans="1:18" hidden="1">
       <c r="A112" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-8</v>
@@ -28489,7 +28493,7 @@
       <c r="Q112" s="16"/>
       <c r="R112" s="16"/>
     </row>
-    <row r="113" spans="1:18">
+    <row r="113" spans="1:18" hidden="1">
       <c r="A113" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-9</v>
@@ -28521,7 +28525,7 @@
       <c r="Q113" s="16"/>
       <c r="R113" s="16"/>
     </row>
-    <row r="114" spans="1:18">
+    <row r="114" spans="1:18" hidden="1">
       <c r="A114" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-10</v>
@@ -28553,7 +28557,7 @@
       <c r="Q114" s="16"/>
       <c r="R114" s="16"/>
     </row>
-    <row r="115" spans="1:18">
+    <row r="115" spans="1:18" hidden="1">
       <c r="A115" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-11</v>
@@ -28585,7 +28589,7 @@
       <c r="Q115" s="16"/>
       <c r="R115" s="16"/>
     </row>
-    <row r="116" spans="1:18">
+    <row r="116" spans="1:18" hidden="1">
       <c r="A116" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-12</v>
@@ -28617,7 +28621,7 @@
       <c r="Q116" s="16"/>
       <c r="R116" s="16"/>
     </row>
-    <row r="117" spans="1:18">
+    <row r="117" spans="1:18" hidden="1">
       <c r="A117" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-13</v>
@@ -28649,7 +28653,7 @@
       <c r="Q117" s="16"/>
       <c r="R117" s="16"/>
     </row>
-    <row r="118" spans="1:18">
+    <row r="118" spans="1:18" hidden="1">
       <c r="A118" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-14</v>
@@ -28681,7 +28685,7 @@
       <c r="Q118" s="16"/>
       <c r="R118" s="16"/>
     </row>
-    <row r="119" spans="1:18">
+    <row r="119" spans="1:18" hidden="1">
       <c r="A119" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-15</v>
@@ -28713,7 +28717,7 @@
       <c r="Q119" s="16"/>
       <c r="R119" s="16"/>
     </row>
-    <row r="120" spans="1:18">
+    <row r="120" spans="1:18" hidden="1">
       <c r="A120" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-16</v>
@@ -28745,7 +28749,7 @@
       <c r="Q120" s="16"/>
       <c r="R120" s="16"/>
     </row>
-    <row r="121" spans="1:18">
+    <row r="121" spans="1:18" hidden="1">
       <c r="A121" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-17</v>
@@ -28777,7 +28781,7 @@
       <c r="Q121" s="16"/>
       <c r="R121" s="16"/>
     </row>
-    <row r="122" spans="1:18">
+    <row r="122" spans="1:18" hidden="1">
       <c r="A122" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-18</v>
@@ -28809,7 +28813,7 @@
       <c r="Q122" s="16"/>
       <c r="R122" s="16"/>
     </row>
-    <row r="123" spans="1:18">
+    <row r="123" spans="1:18" hidden="1">
       <c r="A123" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-19</v>
@@ -28841,7 +28845,7 @@
       <c r="Q123" s="16"/>
       <c r="R123" s="16"/>
     </row>
-    <row r="124" spans="1:18">
+    <row r="124" spans="1:18" hidden="1">
       <c r="A124" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-20</v>
@@ -28873,7 +28877,7 @@
       <c r="Q124" s="16"/>
       <c r="R124" s="16"/>
     </row>
-    <row r="125" spans="1:18">
+    <row r="125" spans="1:18" hidden="1">
       <c r="A125" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-21</v>
@@ -28905,7 +28909,7 @@
       <c r="Q125" s="16"/>
       <c r="R125" s="16"/>
     </row>
-    <row r="126" spans="1:18">
+    <row r="126" spans="1:18" hidden="1">
       <c r="A126" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-22</v>
@@ -28937,7 +28941,7 @@
       <c r="Q126" s="16"/>
       <c r="R126" s="16"/>
     </row>
-    <row r="127" spans="1:18">
+    <row r="127" spans="1:18" hidden="1">
       <c r="A127" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-23</v>
@@ -28969,7 +28973,7 @@
       <c r="Q127" s="16"/>
       <c r="R127" s="16"/>
     </row>
-    <row r="128" spans="1:18">
+    <row r="128" spans="1:18" hidden="1">
       <c r="A128" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-24</v>
@@ -29001,7 +29005,7 @@
       <c r="Q128" s="16"/>
       <c r="R128" s="16"/>
     </row>
-    <row r="129" spans="1:18">
+    <row r="129" spans="1:18" hidden="1">
       <c r="A129" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-25</v>
@@ -29033,7 +29037,7 @@
       <c r="Q129" s="16"/>
       <c r="R129" s="16"/>
     </row>
-    <row r="130" spans="1:18">
+    <row r="130" spans="1:18" hidden="1">
       <c r="A130" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-26</v>
@@ -29065,7 +29069,7 @@
       <c r="Q130" s="16"/>
       <c r="R130" s="16"/>
     </row>
-    <row r="131" spans="1:18">
+    <row r="131" spans="1:18" hidden="1">
       <c r="A131" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-27</v>
@@ -29097,7 +29101,7 @@
       <c r="Q131" s="16"/>
       <c r="R131" s="16"/>
     </row>
-    <row r="132" spans="1:18">
+    <row r="132" spans="1:18" hidden="1">
       <c r="A132" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-28</v>
@@ -29129,7 +29133,7 @@
       <c r="Q132" s="16"/>
       <c r="R132" s="16"/>
     </row>
-    <row r="133" spans="1:18">
+    <row r="133" spans="1:18" hidden="1">
       <c r="A133" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-29</v>
@@ -29163,7 +29167,7 @@
       <c r="Q133" s="16"/>
       <c r="R133" s="16"/>
     </row>
-    <row r="134" spans="1:18">
+    <row r="134" spans="1:18" hidden="1">
       <c r="A134" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-30</v>
@@ -29197,7 +29201,7 @@
       <c r="Q134" s="16"/>
       <c r="R134" s="16"/>
     </row>
-    <row r="135" spans="1:18">
+    <row r="135" spans="1:18" hidden="1">
       <c r="A135" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-31</v>
@@ -29231,7 +29235,7 @@
       <c r="Q135" s="16"/>
       <c r="R135" s="16"/>
     </row>
-    <row r="136" spans="1:18">
+    <row r="136" spans="1:18" hidden="1">
       <c r="A136" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Actions-0</v>
@@ -29275,7 +29279,7 @@
       <c r="Q136" s="16"/>
       <c r="R136" s="16"/>
     </row>
-    <row r="137" spans="1:18">
+    <row r="137" spans="1:18" hidden="1">
       <c r="A137" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Actions-1</v>
@@ -29319,7 +29323,7 @@
       <c r="Q137" s="15"/>
       <c r="R137" s="15"/>
     </row>
-    <row r="138" spans="1:18">
+    <row r="138" spans="1:18" hidden="1">
       <c r="A138" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Actions-2</v>
@@ -29363,7 +29367,7 @@
       <c r="Q138" s="15"/>
       <c r="R138" s="15"/>
     </row>
-    <row r="139" spans="1:18">
+    <row r="139" spans="1:18" hidden="1">
       <c r="A139" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Actions-3</v>
@@ -29407,7 +29411,7 @@
       <c r="Q139" s="15"/>
       <c r="R139" s="15"/>
     </row>
-    <row r="140" spans="1:18">
+    <row r="140" spans="1:18" hidden="1">
       <c r="A140" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Actions-4</v>
@@ -29451,7 +29455,7 @@
       <c r="Q140" s="15"/>
       <c r="R140" s="15"/>
     </row>
-    <row r="141" spans="1:18">
+    <row r="141" spans="1:18" hidden="1">
       <c r="A141" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Actions-5</v>
@@ -29495,7 +29499,7 @@
       <c r="Q141" s="15"/>
       <c r="R141" s="15"/>
     </row>
-    <row r="142" spans="1:18">
+    <row r="142" spans="1:18" hidden="1">
       <c r="A142" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Actions-6</v>
@@ -29539,7 +29543,7 @@
       <c r="Q142" s="16"/>
       <c r="R142" s="16"/>
     </row>
-    <row r="143" spans="1:18">
+    <row r="143" spans="1:18" hidden="1">
       <c r="A143" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Method-0</v>
@@ -29583,7 +29587,7 @@
       <c r="Q143" s="16"/>
       <c r="R143" s="16"/>
     </row>
-    <row r="144" spans="1:18">
+    <row r="144" spans="1:18" hidden="1">
       <c r="A144" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Method-1</v>
@@ -29617,7 +29621,7 @@
       <c r="Q144" s="15"/>
       <c r="R144" s="15"/>
     </row>
-    <row r="145" spans="1:18">
+    <row r="145" spans="1:18" hidden="1">
       <c r="A145" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Method-2</v>
@@ -29651,7 +29655,7 @@
       <c r="Q145" s="15"/>
       <c r="R145" s="15"/>
     </row>
-    <row r="146" spans="1:18">
+    <row r="146" spans="1:18" hidden="1">
       <c r="A146" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Method-3</v>
@@ -29685,7 +29689,7 @@
       <c r="Q146" s="15"/>
       <c r="R146" s="15"/>
     </row>
-    <row r="147" spans="1:18">
+    <row r="147" spans="1:18" hidden="1">
       <c r="A147" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Method-4</v>
@@ -29719,7 +29723,7 @@
       <c r="Q147" s="15"/>
       <c r="R147" s="15"/>
     </row>
-    <row r="148" spans="1:18">
+    <row r="148" spans="1:18" hidden="1">
       <c r="A148" s="18" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Method-5</v>
@@ -29753,7 +29757,7 @@
       <c r="Q148" s="15"/>
       <c r="R148" s="15"/>
     </row>
-    <row r="149" spans="1:18">
+    <row r="149" spans="1:18" hidden="1">
       <c r="A149" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Method-6</v>
@@ -29787,7 +29791,7 @@
       <c r="Q149" s="16"/>
       <c r="R149" s="16"/>
     </row>
-    <row r="150" spans="1:18">
+    <row r="150" spans="1:18" hidden="1">
       <c r="A150" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Attrs-0</v>
@@ -29821,7 +29825,7 @@
       <c r="Q150" s="40"/>
       <c r="R150" s="40"/>
     </row>
-    <row r="151" spans="1:18">
+    <row r="151" spans="1:18" hidden="1">
       <c r="A151" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-14</v>
@@ -29861,7 +29865,7 @@
       <c r="Q151" s="40"/>
       <c r="R151" s="40"/>
     </row>
-    <row r="152" spans="1:18">
+    <row r="152" spans="1:18" hidden="1">
       <c r="A152" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-15</v>
@@ -29901,7 +29905,7 @@
       <c r="Q152" s="40"/>
       <c r="R152" s="40"/>
     </row>
-    <row r="153" spans="1:18">
+    <row r="153" spans="1:18" hidden="1">
       <c r="A153" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-15</v>
@@ -29941,7 +29945,7 @@
       <c r="Q153" s="40"/>
       <c r="R153" s="40"/>
     </row>
-    <row r="154" spans="1:18">
+    <row r="154" spans="1:18" hidden="1">
       <c r="A154" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-16</v>
@@ -29981,7 +29985,7 @@
       <c r="Q154" s="40"/>
       <c r="R154" s="40"/>
     </row>
-    <row r="155" spans="1:18">
+    <row r="155" spans="1:18" hidden="1">
       <c r="A155" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-16</v>
@@ -30021,7 +30025,7 @@
       <c r="Q155" s="40"/>
       <c r="R155" s="40"/>
     </row>
-    <row r="156" spans="1:18">
+    <row r="156" spans="1:18" hidden="1">
       <c r="A156" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-17</v>
@@ -30061,7 +30065,7 @@
       <c r="Q156" s="40"/>
       <c r="R156" s="40"/>
     </row>
-    <row r="157" spans="1:18">
+    <row r="157" spans="1:18" hidden="1">
       <c r="A157" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-0</v>
@@ -30105,7 +30109,7 @@
       <c r="Q157" s="40"/>
       <c r="R157" s="40"/>
     </row>
-    <row r="158" spans="1:18">
+    <row r="158" spans="1:18" hidden="1">
       <c r="A158" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-1</v>
@@ -30139,7 +30143,7 @@
       <c r="Q158" s="40"/>
       <c r="R158" s="40"/>
     </row>
-    <row r="159" spans="1:18">
+    <row r="159" spans="1:18" hidden="1">
       <c r="A159" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-2</v>
@@ -30173,7 +30177,7 @@
       <c r="Q159" s="40"/>
       <c r="R159" s="40"/>
     </row>
-    <row r="160" spans="1:18">
+    <row r="160" spans="1:18" hidden="1">
       <c r="A160" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-3</v>
@@ -30207,7 +30211,7 @@
       <c r="Q160" s="40"/>
       <c r="R160" s="40"/>
     </row>
-    <row r="161" spans="1:18">
+    <row r="161" spans="1:18" hidden="1">
       <c r="A161" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-4</v>
@@ -30245,7 +30249,7 @@
       <c r="Q161" s="40"/>
       <c r="R161" s="40"/>
     </row>
-    <row r="162" spans="1:18">
+    <row r="162" spans="1:18" hidden="1">
       <c r="A162" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-5</v>
@@ -30279,7 +30283,7 @@
       <c r="Q162" s="40"/>
       <c r="R162" s="40"/>
     </row>
-    <row r="163" spans="1:18">
+    <row r="163" spans="1:18" hidden="1">
       <c r="A163" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-6</v>
@@ -30313,7 +30317,7 @@
       <c r="Q163" s="40"/>
       <c r="R163" s="40"/>
     </row>
-    <row r="164" spans="1:18">
+    <row r="164" spans="1:18" hidden="1">
       <c r="A164" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-7</v>
@@ -30347,7 +30351,7 @@
       <c r="Q164" s="40"/>
       <c r="R164" s="40"/>
     </row>
-    <row r="165" spans="1:18">
+    <row r="165" spans="1:18" hidden="1">
       <c r="A165" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-8</v>
@@ -30385,7 +30389,7 @@
       <c r="Q165" s="40"/>
       <c r="R165" s="40"/>
     </row>
-    <row r="166" spans="1:18">
+    <row r="166" spans="1:18" hidden="1">
       <c r="A166" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-18</v>
@@ -30425,7 +30429,7 @@
       <c r="Q166" s="40"/>
       <c r="R166" s="40"/>
     </row>
-    <row r="167" spans="1:18">
+    <row r="167" spans="1:18" hidden="1">
       <c r="A167" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-17</v>
@@ -30465,7 +30469,7 @@
       <c r="Q167" s="40"/>
       <c r="R167" s="40"/>
     </row>
-    <row r="168" spans="1:18">
+    <row r="168" spans="1:18" hidden="1">
       <c r="A168" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-19</v>
@@ -30505,7 +30509,7 @@
       <c r="Q168" s="40"/>
       <c r="R168" s="40"/>
     </row>
-    <row r="169" spans="1:18">
+    <row r="169" spans="1:18" hidden="1">
       <c r="A169" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Defaults-0</v>
@@ -30551,7 +30555,7 @@
       <c r="Q169" s="40"/>
       <c r="R169" s="40"/>
     </row>
-    <row r="170" spans="1:18">
+    <row r="170" spans="1:18" hidden="1">
       <c r="A170" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Defaults-1</v>
@@ -30587,7 +30591,7 @@
       <c r="Q170" s="40"/>
       <c r="R170" s="40"/>
     </row>
-    <row r="171" spans="1:18">
+    <row r="171" spans="1:18" hidden="1">
       <c r="A171" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Defaults-2</v>
@@ -30623,7 +30627,7 @@
       <c r="Q171" s="40"/>
       <c r="R171" s="40"/>
     </row>
-    <row r="172" spans="1:18">
+    <row r="172" spans="1:18" hidden="1">
       <c r="A172" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-18</v>
@@ -30663,7 +30667,7 @@
       <c r="Q172" s="40"/>
       <c r="R172" s="40"/>
     </row>
-    <row r="173" spans="1:18">
+    <row r="173" spans="1:18" hidden="1">
       <c r="A173" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-20</v>
@@ -30703,7 +30707,7 @@
       <c r="Q173" s="40"/>
       <c r="R173" s="40"/>
     </row>
-    <row r="174" spans="1:18">
+    <row r="174" spans="1:18" hidden="1">
       <c r="A174" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-21</v>
@@ -30743,7 +30747,7 @@
       <c r="Q174" s="40"/>
       <c r="R174" s="40"/>
     </row>
-    <row r="175" spans="1:18">
+    <row r="175" spans="1:18" hidden="1">
       <c r="A175" s="42" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-22</v>
@@ -30783,7 +30787,7 @@
       <c r="Q175" s="43"/>
       <c r="R175" s="43"/>
     </row>
-    <row r="176" spans="1:18">
+    <row r="176" spans="1:18" hidden="1">
       <c r="A176" s="42" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-23</v>
@@ -30823,7 +30827,7 @@
       <c r="Q176" s="43"/>
       <c r="R176" s="43"/>
     </row>
-    <row r="177" spans="1:18">
+    <row r="177" spans="1:18" hidden="1">
       <c r="A177" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-32</v>
@@ -30859,7 +30863,7 @@
       <c r="Q177" s="40"/>
       <c r="R177" s="40"/>
     </row>
-    <row r="178" spans="1:18">
+    <row r="178" spans="1:18" hidden="1">
       <c r="A178" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-33</v>
@@ -30895,7 +30899,7 @@
       <c r="Q178" s="40"/>
       <c r="R178" s="40"/>
     </row>
-    <row r="179" spans="1:18">
+    <row r="179" spans="1:18" hidden="1">
       <c r="A179" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-32</v>
@@ -30927,7 +30931,7 @@
       <c r="Q179" s="40"/>
       <c r="R179" s="40"/>
     </row>
-    <row r="180" spans="1:18">
+    <row r="180" spans="1:18" hidden="1">
       <c r="A180" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-33</v>
@@ -30959,7 +30963,7 @@
       <c r="Q180" s="40"/>
       <c r="R180" s="40"/>
     </row>
-    <row r="181" spans="1:18">
+    <row r="181" spans="1:18" hidden="1">
       <c r="A181" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-9</v>
@@ -30993,7 +30997,7 @@
       <c r="Q181" s="40"/>
       <c r="R181" s="40"/>
     </row>
-    <row r="182" spans="1:18">
+    <row r="182" spans="1:18" hidden="1">
       <c r="A182" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-10</v>
@@ -31029,7 +31033,7 @@
       <c r="Q182" s="40"/>
       <c r="R182" s="40"/>
     </row>
-    <row r="183" spans="1:18">
+    <row r="183" spans="1:18" hidden="1">
       <c r="A183" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-11</v>
@@ -31063,7 +31067,7 @@
       <c r="Q183" s="40"/>
       <c r="R183" s="40"/>
     </row>
-    <row r="184" spans="1:18">
+    <row r="184" spans="1:18" hidden="1">
       <c r="A184" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-12</v>
@@ -31099,7 +31103,7 @@
       <c r="Q184" s="40"/>
       <c r="R184" s="40"/>
     </row>
-    <row r="185" spans="1:18">
+    <row r="185" spans="1:18" hidden="1">
       <c r="A185" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-19</v>
@@ -31139,7 +31143,7 @@
       <c r="Q185" s="40"/>
       <c r="R185" s="40"/>
     </row>
-    <row r="186" spans="1:18">
+    <row r="186" spans="1:18" hidden="1">
       <c r="A186" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-24</v>
@@ -31179,7 +31183,7 @@
       <c r="Q186" s="40"/>
       <c r="R186" s="40"/>
     </row>
-    <row r="187" spans="1:18">
+    <row r="187" spans="1:18" hidden="1">
       <c r="A187" s="42" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-20</v>
@@ -31219,7 +31223,7 @@
       <c r="Q187" s="43"/>
       <c r="R187" s="43"/>
     </row>
-    <row r="188" spans="1:18">
+    <row r="188" spans="1:18" hidden="1">
       <c r="A188" s="42" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-21</v>
@@ -31259,7 +31263,7 @@
       <c r="Q188" s="43"/>
       <c r="R188" s="43"/>
     </row>
-    <row r="189" spans="1:18">
+    <row r="189" spans="1:18" hidden="1">
       <c r="A189" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-22</v>
@@ -31299,7 +31303,7 @@
       <c r="Q189" s="40"/>
       <c r="R189" s="40"/>
     </row>
-    <row r="190" spans="1:18">
+    <row r="190" spans="1:18" hidden="1">
       <c r="A190" s="42" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-25</v>
@@ -31339,7 +31343,7 @@
       <c r="Q190" s="43"/>
       <c r="R190" s="43"/>
     </row>
-    <row r="191" spans="1:18">
+    <row r="191" spans="1:18" hidden="1">
       <c r="A191" s="42" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-26</v>
@@ -31379,7 +31383,7 @@
       <c r="Q191" s="43"/>
       <c r="R191" s="43"/>
     </row>
-    <row r="192" spans="1:18">
+    <row r="192" spans="1:18" hidden="1">
       <c r="A192" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-27</v>
@@ -31419,7 +31423,7 @@
       <c r="Q192" s="40"/>
       <c r="R192" s="40"/>
     </row>
-    <row r="193" spans="1:18">
+    <row r="193" spans="1:18" hidden="1">
       <c r="A193" s="42" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-23</v>
@@ -31459,7 +31463,7 @@
       <c r="Q193" s="43"/>
       <c r="R193" s="43"/>
     </row>
-    <row r="194" spans="1:18">
+    <row r="194" spans="1:18" hidden="1">
       <c r="A194" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-24</v>
@@ -31499,7 +31503,7 @@
       <c r="Q194" s="40"/>
       <c r="R194" s="40"/>
     </row>
-    <row r="195" spans="1:18">
+    <row r="195" spans="1:18" hidden="1">
       <c r="A195" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-28</v>
@@ -31539,7 +31543,7 @@
       <c r="Q195" s="40"/>
       <c r="R195" s="40"/>
     </row>
-    <row r="196" spans="1:18">
+    <row r="196" spans="1:18" hidden="1">
       <c r="A196" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-29</v>
@@ -31579,7 +31583,7 @@
       <c r="Q196" s="40"/>
       <c r="R196" s="40"/>
     </row>
-    <row r="197" spans="1:18">
+    <row r="197" spans="1:18" hidden="1">
       <c r="A197" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Actions-7</v>
@@ -31621,7 +31625,7 @@
       <c r="Q197" s="40"/>
       <c r="R197" s="40"/>
     </row>
-    <row r="198" spans="1:18">
+    <row r="198" spans="1:18" hidden="1">
       <c r="A198" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Method-7</v>
@@ -31655,7 +31659,7 @@
       <c r="Q198" s="40"/>
       <c r="R198" s="40"/>
     </row>
-    <row r="199" spans="1:18">
+    <row r="199" spans="1:18" hidden="1">
       <c r="A199" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action List-0</v>
@@ -31687,7 +31691,7 @@
       <c r="Q199" s="40"/>
       <c r="R199" s="40"/>
     </row>
-    <row r="200" spans="1:18">
+    <row r="200" spans="1:18" hidden="1">
       <c r="A200" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action List-1</v>
@@ -31719,7 +31723,7 @@
       <c r="Q200" s="40"/>
       <c r="R200" s="40"/>
     </row>
-    <row r="201" spans="1:18">
+    <row r="201" spans="1:18" hidden="1">
       <c r="A201" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Data-0</v>
@@ -31757,7 +31761,7 @@
       <c r="Q201" s="40"/>
       <c r="R201" s="40"/>
     </row>
-    <row r="202" spans="1:18">
+    <row r="202" spans="1:18" hidden="1">
       <c r="A202" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Data-1</v>
@@ -31793,7 +31797,7 @@
       <c r="Q202" s="40"/>
       <c r="R202" s="40"/>
     </row>
-    <row r="203" spans="1:18">
+    <row r="203" spans="1:18" hidden="1">
       <c r="A203" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Data-2</v>
@@ -31829,7 +31833,7 @@
       <c r="Q203" s="40"/>
       <c r="R203" s="40"/>
     </row>
-    <row r="204" spans="1:18">
+    <row r="204" spans="1:18" hidden="1">
       <c r="A204" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Actions-8</v>
@@ -31871,7 +31875,7 @@
       <c r="Q204" s="40"/>
       <c r="R204" s="40"/>
     </row>
-    <row r="205" spans="1:18">
+    <row r="205" spans="1:18" hidden="1">
       <c r="A205" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Method-8</v>
@@ -31905,7 +31909,7 @@
       <c r="Q205" s="40"/>
       <c r="R205" s="40"/>
     </row>
-    <row r="206" spans="1:18">
+    <row r="206" spans="1:18" hidden="1">
       <c r="A206" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action List-2</v>
@@ -31937,7 +31941,7 @@
       <c r="Q206" s="40"/>
       <c r="R206" s="40"/>
     </row>
-    <row r="207" spans="1:18">
+    <row r="207" spans="1:18" hidden="1">
       <c r="A207" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource List Layout-0</v>
@@ -31977,7 +31981,7 @@
       <c r="Q207" s="40"/>
       <c r="R207" s="40"/>
     </row>
-    <row r="208" spans="1:18">
+    <row r="208" spans="1:18" hidden="1">
       <c r="A208" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource List Layout-1</v>
@@ -32011,7 +32015,7 @@
       <c r="Q208" s="40"/>
       <c r="R208" s="40"/>
     </row>
-    <row r="209" spans="1:18">
+    <row r="209" spans="1:18" hidden="1">
       <c r="A209" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource List Layout-2</v>
@@ -32045,7 +32049,7 @@
       <c r="Q209" s="40"/>
       <c r="R209" s="40"/>
     </row>
-    <row r="210" spans="1:18">
+    <row r="210" spans="1:18" hidden="1">
       <c r="A210" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource List Layout-3</v>
@@ -32079,7 +32083,7 @@
       <c r="Q210" s="40"/>
       <c r="R210" s="40"/>
     </row>
-    <row r="211" spans="1:18">
+    <row r="211" spans="1:18" hidden="1">
       <c r="A211" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource List Layout-4</v>
@@ -32113,7 +32117,7 @@
       <c r="Q211" s="40"/>
       <c r="R211" s="40"/>
     </row>
-    <row r="212" spans="1:18">
+    <row r="212" spans="1:18" hidden="1">
       <c r="A212" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-25</v>
@@ -32153,7 +32157,7 @@
       <c r="Q212" s="16"/>
       <c r="R212" s="16"/>
     </row>
-    <row r="213" spans="1:18">
+    <row r="213" spans="1:18" hidden="1">
       <c r="A213" s="19" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-30</v>
@@ -32193,7 +32197,7 @@
       <c r="Q213" s="16"/>
       <c r="R213" s="16"/>
     </row>
-    <row r="214" spans="1:18">
+    <row r="214" spans="1:18" hidden="1">
       <c r="A214" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-26</v>
@@ -32233,7 +32237,7 @@
       <c r="Q214" s="40"/>
       <c r="R214" s="40"/>
     </row>
-    <row r="215" spans="1:18">
+    <row r="215" spans="1:18" hidden="1">
       <c r="A215" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-31</v>
@@ -32273,7 +32277,7 @@
       <c r="Q215" s="40"/>
       <c r="R215" s="40"/>
     </row>
-    <row r="216" spans="1:18">
+    <row r="216" spans="1:18" hidden="1">
       <c r="A216" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-32</v>
@@ -32313,7 +32317,7 @@
       <c r="Q216" s="40"/>
       <c r="R216" s="40"/>
     </row>
-    <row r="217" spans="1:18">
+    <row r="217" spans="1:18" hidden="1">
       <c r="A217" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-27</v>
@@ -32353,7 +32357,7 @@
       <c r="Q217" s="40"/>
       <c r="R217" s="40"/>
     </row>
-    <row r="218" spans="1:18">
+    <row r="218" spans="1:18" hidden="1">
       <c r="A218" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-33</v>
@@ -32393,7 +32397,7 @@
       <c r="Q218" s="40"/>
       <c r="R218" s="40"/>
     </row>
-    <row r="219" spans="1:18">
+    <row r="219" spans="1:18" hidden="1">
       <c r="A219" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Layout-0</v>
@@ -32427,7 +32431,7 @@
       <c r="Q219" s="40"/>
       <c r="R219" s="40"/>
     </row>
-    <row r="220" spans="1:18">
+    <row r="220" spans="1:18" hidden="1">
       <c r="A220" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Layout-1</v>
@@ -32461,7 +32465,7 @@
       <c r="Q220" s="40"/>
       <c r="R220" s="40"/>
     </row>
-    <row r="221" spans="1:18">
+    <row r="221" spans="1:18" hidden="1">
       <c r="A221" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Layout-2</v>
@@ -32495,7 +32499,7 @@
       <c r="Q221" s="40"/>
       <c r="R221" s="40"/>
     </row>
-    <row r="222" spans="1:18">
+    <row r="222" spans="1:18" hidden="1">
       <c r="A222" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Layout-3</v>
@@ -32529,7 +32533,7 @@
       <c r="Q222" s="40"/>
       <c r="R222" s="40"/>
     </row>
-    <row r="223" spans="1:18">
+    <row r="223" spans="1:18" hidden="1">
       <c r="A223" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Layout-4</v>
@@ -32563,7 +32567,7 @@
       <c r="Q223" s="40"/>
       <c r="R223" s="40"/>
     </row>
-    <row r="224" spans="1:18">
+    <row r="224" spans="1:18" hidden="1">
       <c r="A224" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Layout-5</v>
@@ -32597,7 +32601,7 @@
       <c r="Q224" s="40"/>
       <c r="R224" s="40"/>
     </row>
-    <row r="225" spans="1:18">
+    <row r="225" spans="1:18" hidden="1">
       <c r="A225" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Layout-6</v>
@@ -32631,7 +32635,7 @@
       <c r="Q225" s="40"/>
       <c r="R225" s="40"/>
     </row>
-    <row r="226" spans="1:18">
+    <row r="226" spans="1:18" hidden="1">
       <c r="A226" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-28</v>
@@ -32671,7 +32675,7 @@
       <c r="Q226" s="40"/>
       <c r="R226" s="40"/>
     </row>
-    <row r="227" spans="1:18">
+    <row r="227" spans="1:18" hidden="1">
       <c r="A227" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-34</v>
@@ -32711,7 +32715,7 @@
       <c r="Q227" s="40"/>
       <c r="R227" s="40"/>
     </row>
-    <row r="228" spans="1:18">
+    <row r="228" spans="1:18" hidden="1">
       <c r="A228" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-29</v>
@@ -32751,7 +32755,7 @@
       <c r="Q228" s="40"/>
       <c r="R228" s="40"/>
     </row>
-    <row r="229" spans="1:18">
+    <row r="229" spans="1:18" hidden="1">
       <c r="A229" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-35</v>
@@ -32791,7 +32795,7 @@
       <c r="Q229" s="40"/>
       <c r="R229" s="40"/>
     </row>
-    <row r="230" spans="1:18">
+    <row r="230" spans="1:18" hidden="1">
       <c r="A230" s="42" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-36</v>
@@ -32831,7 +32835,7 @@
       <c r="Q230" s="43"/>
       <c r="R230" s="43"/>
     </row>
-    <row r="231" spans="1:18">
+    <row r="231" spans="1:18" hidden="1">
       <c r="A231" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-37</v>
@@ -32871,7 +32875,7 @@
       <c r="Q231" s="40"/>
       <c r="R231" s="40"/>
     </row>
-    <row r="232" spans="1:18">
+    <row r="232" spans="1:18" hidden="1">
       <c r="A232" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Data View Section-0</v>
@@ -32909,7 +32913,7 @@
       <c r="Q232" s="40"/>
       <c r="R232" s="40"/>
     </row>
-    <row r="233" spans="1:18">
+    <row r="233" spans="1:18" hidden="1">
       <c r="A233" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Data View Section-1</v>
@@ -32941,7 +32945,7 @@
       <c r="Q233" s="40"/>
       <c r="R233" s="40"/>
     </row>
-    <row r="234" spans="1:18">
+    <row r="234" spans="1:18" hidden="1">
       <c r="A234" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Data View Section-2</v>
@@ -32973,7 +32977,7 @@
       <c r="Q234" s="40"/>
       <c r="R234" s="40"/>
     </row>
-    <row r="235" spans="1:18">
+    <row r="235" spans="1:18" hidden="1">
       <c r="A235" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Data View Section Items-0</v>
@@ -33009,7 +33013,7 @@
       <c r="Q235" s="40"/>
       <c r="R235" s="40"/>
     </row>
-    <row r="236" spans="1:18">
+    <row r="236" spans="1:18" hidden="1">
       <c r="A236" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Data View Section Items-1</v>
@@ -33043,7 +33047,7 @@
       <c r="Q236" s="40"/>
       <c r="R236" s="40"/>
     </row>
-    <row r="237" spans="1:18">
+    <row r="237" spans="1:18" hidden="1">
       <c r="A237" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Data View Section Items-2</v>
@@ -33077,7 +33081,7 @@
       <c r="Q237" s="40"/>
       <c r="R237" s="40"/>
     </row>
-    <row r="238" spans="1:18">
+    <row r="238" spans="1:18" hidden="1">
       <c r="A238" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Data View Section Items-3</v>
@@ -33111,7 +33115,7 @@
       <c r="Q238" s="40"/>
       <c r="R238" s="40"/>
     </row>
-    <row r="239" spans="1:18">
+    <row r="239" spans="1:18" hidden="1">
       <c r="A239" s="42" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Data View Section Items-4</v>
@@ -33145,7 +33149,7 @@
       <c r="Q239" s="43"/>
       <c r="R239" s="43"/>
     </row>
-    <row r="240" spans="1:18">
+    <row r="240" spans="1:18" hidden="1">
       <c r="A240" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Forms-8</v>
@@ -33183,7 +33187,7 @@
       <c r="Q240" s="40"/>
       <c r="R240" s="40"/>
     </row>
-    <row r="241" spans="1:18">
+    <row r="241" spans="1:18" hidden="1">
       <c r="A241" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Forms-9</v>
@@ -33221,7 +33225,7 @@
       <c r="Q241" s="40"/>
       <c r="R241" s="40"/>
     </row>
-    <row r="242" spans="1:18">
+    <row r="242" spans="1:18" hidden="1">
       <c r="A242" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-34</v>
@@ -33257,7 +33261,7 @@
       <c r="Q242" s="40"/>
       <c r="R242" s="40"/>
     </row>
-    <row r="243" spans="1:18">
+    <row r="243" spans="1:18" hidden="1">
       <c r="A243" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-35</v>
@@ -33293,7 +33297,7 @@
       <c r="Q243" s="40"/>
       <c r="R243" s="40"/>
     </row>
-    <row r="244" spans="1:18">
+    <row r="244" spans="1:18" hidden="1">
       <c r="A244" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-36</v>
@@ -33329,7 +33333,7 @@
       <c r="Q244" s="40"/>
       <c r="R244" s="40"/>
     </row>
-    <row r="245" spans="1:18">
+    <row r="245" spans="1:18" hidden="1">
       <c r="A245" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Fields-37</v>
@@ -33365,7 +33369,7 @@
       <c r="Q245" s="40"/>
       <c r="R245" s="40"/>
     </row>
-    <row r="246" spans="1:18">
+    <row r="246" spans="1:18" hidden="1">
       <c r="A246" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Attrs-1</v>
@@ -33399,7 +33403,7 @@
       <c r="Q246" s="40"/>
       <c r="R246" s="40"/>
     </row>
-    <row r="247" spans="1:18">
+    <row r="247" spans="1:18" hidden="1">
       <c r="A247" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Attrs-2</v>
@@ -33433,7 +33437,7 @@
       <c r="Q247" s="40"/>
       <c r="R247" s="40"/>
     </row>
-    <row r="248" spans="1:18">
+    <row r="248" spans="1:18" hidden="1">
       <c r="A248" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Attrs-3</v>
@@ -33467,7 +33471,7 @@
       <c r="Q248" s="40"/>
       <c r="R248" s="40"/>
     </row>
-    <row r="249" spans="1:18">
+    <row r="249" spans="1:18" hidden="1">
       <c r="A249" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Attrs-4</v>
@@ -33501,7 +33505,7 @@
       <c r="Q249" s="40"/>
       <c r="R249" s="40"/>
     </row>
-    <row r="250" spans="1:18">
+    <row r="250" spans="1:18" hidden="1">
       <c r="A250" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-34</v>
@@ -33533,7 +33537,7 @@
       <c r="Q250" s="40"/>
       <c r="R250" s="40"/>
     </row>
-    <row r="251" spans="1:18">
+    <row r="251" spans="1:18" hidden="1">
       <c r="A251" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-35</v>
@@ -33565,7 +33569,7 @@
       <c r="Q251" s="40"/>
       <c r="R251" s="40"/>
     </row>
-    <row r="252" spans="1:18">
+    <row r="252" spans="1:18" hidden="1">
       <c r="A252" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-36</v>
@@ -33597,7 +33601,7 @@
       <c r="Q252" s="40"/>
       <c r="R252" s="40"/>
     </row>
-    <row r="253" spans="1:18">
+    <row r="253" spans="1:18" hidden="1">
       <c r="A253" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Form Field Data-37</v>
@@ -33629,7 +33633,7 @@
       <c r="Q253" s="40"/>
       <c r="R253" s="40"/>
     </row>
-    <row r="254" spans="1:18">
+    <row r="254" spans="1:18" hidden="1">
       <c r="A254" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-13</v>
@@ -33663,7 +33667,7 @@
       <c r="Q254" s="40"/>
       <c r="R254" s="40"/>
     </row>
-    <row r="255" spans="1:18">
+    <row r="255" spans="1:18" hidden="1">
       <c r="A255" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-14</v>
@@ -33697,7 +33701,7 @@
       <c r="Q255" s="40"/>
       <c r="R255" s="40"/>
     </row>
-    <row r="256" spans="1:18">
+    <row r="256" spans="1:18" hidden="1">
       <c r="A256" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-15</v>
@@ -33731,7 +33735,7 @@
       <c r="Q256" s="40"/>
       <c r="R256" s="40"/>
     </row>
-    <row r="257" spans="1:18">
+    <row r="257" spans="1:18" hidden="1">
       <c r="A257" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-16</v>
@@ -33771,7 +33775,7 @@
       <c r="Q257" s="40"/>
       <c r="R257" s="40"/>
     </row>
-    <row r="258" spans="1:18">
+    <row r="258" spans="1:18" hidden="1">
       <c r="A258" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-17</v>
@@ -33805,7 +33809,7 @@
       <c r="Q258" s="40"/>
       <c r="R258" s="40"/>
     </row>
-    <row r="259" spans="1:18">
+    <row r="259" spans="1:18" hidden="1">
       <c r="A259" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-18</v>
@@ -33839,7 +33843,7 @@
       <c r="Q259" s="40"/>
       <c r="R259" s="40"/>
     </row>
-    <row r="260" spans="1:18">
+    <row r="260" spans="1:18" hidden="1">
       <c r="A260" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-19</v>
@@ -33873,7 +33877,7 @@
       <c r="Q260" s="40"/>
       <c r="R260" s="40"/>
     </row>
-    <row r="261" spans="1:18">
+    <row r="261" spans="1:18" hidden="1">
       <c r="A261" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Field Validations-20</v>
@@ -33913,7 +33917,7 @@
       <c r="Q261" s="40"/>
       <c r="R261" s="40"/>
     </row>
-    <row r="262" spans="1:18">
+    <row r="262" spans="1:18" hidden="1">
       <c r="A262" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Actions-9</v>
@@ -33955,7 +33959,7 @@
       <c r="Q262" s="40"/>
       <c r="R262" s="40"/>
     </row>
-    <row r="263" spans="1:18">
+    <row r="263" spans="1:18" hidden="1">
       <c r="A263" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Actions-10</v>
@@ -33997,7 +34001,7 @@
       <c r="Q263" s="40"/>
       <c r="R263" s="40"/>
     </row>
-    <row r="264" spans="1:18">
+    <row r="264" spans="1:18" hidden="1">
       <c r="A264" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action List-3</v>
@@ -34029,7 +34033,7 @@
       <c r="Q264" s="40"/>
       <c r="R264" s="40"/>
     </row>
-    <row r="265" spans="1:18">
+    <row r="265" spans="1:18" hidden="1">
       <c r="A265" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action List-4</v>
@@ -34061,7 +34065,7 @@
       <c r="Q265" s="40"/>
       <c r="R265" s="40"/>
     </row>
-    <row r="266" spans="1:18">
+    <row r="266" spans="1:18" hidden="1">
       <c r="A266" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Data-0</v>
@@ -34093,7 +34097,7 @@
       <c r="Q266" s="40"/>
       <c r="R266" s="40"/>
     </row>
-    <row r="267" spans="1:18">
+    <row r="267" spans="1:18" hidden="1">
       <c r="A267" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Data-1</v>
@@ -34125,7 +34129,7 @@
       <c r="Q267" s="40"/>
       <c r="R267" s="40"/>
     </row>
-    <row r="268" spans="1:18">
+    <row r="268" spans="1:18" hidden="1">
       <c r="A268" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Data-2</v>
@@ -34157,7 +34161,7 @@
       <c r="Q268" s="40"/>
       <c r="R268" s="40"/>
     </row>
-    <row r="269" spans="1:18">
+    <row r="269" spans="1:18" hidden="1">
       <c r="A269" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Method-9</v>
@@ -34193,7 +34197,7 @@
       <c r="Q269" s="40"/>
       <c r="R269" s="40"/>
     </row>
-    <row r="270" spans="1:18">
+    <row r="270" spans="1:18" hidden="1">
       <c r="A270" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Action Method-10</v>
@@ -34229,7 +34233,7 @@
       <c r="Q270" s="40"/>
       <c r="R270" s="40"/>
     </row>
-    <row r="271" spans="1:18">
+    <row r="271" spans="1:18" hidden="1">
       <c r="A271" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-38</v>
@@ -34269,7 +34273,7 @@
       <c r="Q271" s="40"/>
       <c r="R271" s="40"/>
     </row>
-    <row r="272" spans="1:18">
+    <row r="272" spans="1:18" hidden="1">
       <c r="A272" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resources-30</v>
@@ -34309,7 +34313,7 @@
       <c r="Q272" s="40"/>
       <c r="R272" s="40"/>
     </row>
-    <row r="273" spans="1:18">
+    <row r="273" spans="1:18" hidden="1">
       <c r="A273" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-39</v>
@@ -34349,7 +34353,7 @@
       <c r="Q273" s="40"/>
       <c r="R273" s="40"/>
     </row>
-    <row r="274" spans="1:18">
+    <row r="274" spans="1:18" hidden="1">
       <c r="A274" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-40</v>
@@ -34389,7 +34393,7 @@
       <c r="Q274" s="40"/>
       <c r="R274" s="40"/>
     </row>
-    <row r="275" spans="1:18">
+    <row r="275" spans="1:18" hidden="1">
       <c r="A275" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-41</v>
@@ -34429,7 +34433,7 @@
       <c r="Q275" s="40"/>
       <c r="R275" s="40"/>
     </row>
-    <row r="276" spans="1:18">
+    <row r="276" spans="1:18" hidden="1">
       <c r="A276" s="42" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-42</v>
@@ -34469,7 +34473,7 @@
       <c r="Q276" s="43"/>
       <c r="R276" s="43"/>
     </row>
-    <row r="277" spans="1:18">
+    <row r="277" spans="1:18" hidden="1">
       <c r="A277" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Resource Relations-43</v>
@@ -34509,7 +34513,7 @@
       <c r="Q277" s="40"/>
       <c r="R277" s="40"/>
     </row>
-    <row r="278" spans="1:18">
+    <row r="278" spans="1:18" hidden="1">
       <c r="A278" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Users-0</v>
@@ -34543,7 +34547,7 @@
       <c r="Q278" s="40"/>
       <c r="R278" s="40"/>
     </row>
-    <row r="279" spans="1:18">
+    <row r="279" spans="1:18" hidden="1">
       <c r="A279" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Field Options-0</v>
@@ -34575,7 +34579,7 @@
       <c r="Q279" s="40"/>
       <c r="R279" s="40"/>
     </row>
-    <row r="280" spans="1:18">
+    <row r="280" spans="1:18" hidden="1">
       <c r="A280" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Form Collection-0</v>
@@ -34611,7 +34615,7 @@
       <c r="Q280" s="40"/>
       <c r="R280" s="40"/>
     </row>
-    <row r="281" spans="1:18">
+    <row r="281" spans="1:18" hidden="1">
       <c r="A281" s="22" t="str">
         <f>[Table Name]&amp;"-"&amp;[Record No]</f>
         <v>Data Scopes-0</v>
@@ -34643,6 +34647,742 @@
       <c r="Q281" s="40"/>
       <c r="R281" s="40"/>
     </row>
+    <row r="282" spans="1:18">
+      <c r="A282" s="22" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resource Roles-8</v>
+      </c>
+      <c r="B282" s="40" t="s">
+        <v>227</v>
+      </c>
+      <c r="C282" s="22">
+        <f>COUNTIF($B$1:$B281,[Table Name])</f>
+        <v>8</v>
+      </c>
+      <c r="D282" s="40">
+        <v>7</v>
+      </c>
+      <c r="E282" s="40">
+        <v>2</v>
+      </c>
+      <c r="F282" s="40"/>
+      <c r="G282" s="40"/>
+      <c r="H282" s="40"/>
+      <c r="I282" s="40"/>
+      <c r="J282" s="40"/>
+      <c r="K282" s="40"/>
+      <c r="L282" s="40"/>
+      <c r="M282" s="40"/>
+      <c r="N282" s="40"/>
+      <c r="O282" s="40"/>
+      <c r="P282" s="40"/>
+      <c r="Q282" s="40"/>
+      <c r="R282" s="40"/>
+    </row>
+    <row r="283" spans="1:18">
+      <c r="A283" s="42" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resource Roles-9</v>
+      </c>
+      <c r="B283" s="40" t="s">
+        <v>227</v>
+      </c>
+      <c r="C283" s="42">
+        <f>COUNTIF($B$1:$B282,[Table Name])</f>
+        <v>9</v>
+      </c>
+      <c r="D283" s="43">
+        <v>8</v>
+      </c>
+      <c r="E283" s="43">
+        <v>2</v>
+      </c>
+      <c r="F283" s="43"/>
+      <c r="G283" s="43"/>
+      <c r="H283" s="43"/>
+      <c r="I283" s="43"/>
+      <c r="J283" s="43"/>
+      <c r="K283" s="43"/>
+      <c r="L283" s="43"/>
+      <c r="M283" s="43"/>
+      <c r="N283" s="43"/>
+      <c r="O283" s="43"/>
+      <c r="P283" s="43"/>
+      <c r="Q283" s="43"/>
+      <c r="R283" s="43"/>
+    </row>
+    <row r="284" spans="1:18">
+      <c r="A284" s="42" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resource Roles-10</v>
+      </c>
+      <c r="B284" s="40" t="s">
+        <v>227</v>
+      </c>
+      <c r="C284" s="42">
+        <f>COUNTIF($B$1:$B283,[Table Name])</f>
+        <v>10</v>
+      </c>
+      <c r="D284" s="43">
+        <v>9</v>
+      </c>
+      <c r="E284" s="43">
+        <v>2</v>
+      </c>
+      <c r="F284" s="43"/>
+      <c r="G284" s="43"/>
+      <c r="H284" s="43"/>
+      <c r="I284" s="43"/>
+      <c r="J284" s="43"/>
+      <c r="K284" s="43"/>
+      <c r="L284" s="43"/>
+      <c r="M284" s="43"/>
+      <c r="N284" s="43"/>
+      <c r="O284" s="43"/>
+      <c r="P284" s="43"/>
+      <c r="Q284" s="43"/>
+      <c r="R284" s="43"/>
+    </row>
+    <row r="285" spans="1:18">
+      <c r="A285" s="42" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resource Roles-11</v>
+      </c>
+      <c r="B285" s="40" t="s">
+        <v>227</v>
+      </c>
+      <c r="C285" s="42">
+        <f>COUNTIF($B$1:$B284,[Table Name])</f>
+        <v>11</v>
+      </c>
+      <c r="D285" s="43">
+        <v>10</v>
+      </c>
+      <c r="E285" s="43">
+        <v>2</v>
+      </c>
+      <c r="F285" s="43"/>
+      <c r="G285" s="43"/>
+      <c r="H285" s="43"/>
+      <c r="I285" s="43"/>
+      <c r="J285" s="43"/>
+      <c r="K285" s="43"/>
+      <c r="L285" s="43"/>
+      <c r="M285" s="43"/>
+      <c r="N285" s="43"/>
+      <c r="O285" s="43"/>
+      <c r="P285" s="43"/>
+      <c r="Q285" s="43"/>
+      <c r="R285" s="43"/>
+    </row>
+    <row r="286" spans="1:18">
+      <c r="A286" s="42" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resource Roles-12</v>
+      </c>
+      <c r="B286" s="40" t="s">
+        <v>227</v>
+      </c>
+      <c r="C286" s="42">
+        <f>COUNTIF($B$1:$B285,[Table Name])</f>
+        <v>12</v>
+      </c>
+      <c r="D286" s="43">
+        <v>12</v>
+      </c>
+      <c r="E286" s="43">
+        <v>2</v>
+      </c>
+      <c r="F286" s="43"/>
+      <c r="G286" s="43"/>
+      <c r="H286" s="43"/>
+      <c r="I286" s="43"/>
+      <c r="J286" s="43"/>
+      <c r="K286" s="43"/>
+      <c r="L286" s="43"/>
+      <c r="M286" s="43"/>
+      <c r="N286" s="43"/>
+      <c r="O286" s="43"/>
+      <c r="P286" s="43"/>
+      <c r="Q286" s="43"/>
+      <c r="R286" s="43"/>
+    </row>
+    <row r="287" spans="1:18">
+      <c r="A287" s="42" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resource Roles-13</v>
+      </c>
+      <c r="B287" s="40" t="s">
+        <v>227</v>
+      </c>
+      <c r="C287" s="42">
+        <f>COUNTIF($B$1:$B286,[Table Name])</f>
+        <v>13</v>
+      </c>
+      <c r="D287" s="43">
+        <v>13</v>
+      </c>
+      <c r="E287" s="43">
+        <v>2</v>
+      </c>
+      <c r="F287" s="43"/>
+      <c r="G287" s="43"/>
+      <c r="H287" s="43"/>
+      <c r="I287" s="43"/>
+      <c r="J287" s="43"/>
+      <c r="K287" s="43"/>
+      <c r="L287" s="43"/>
+      <c r="M287" s="43"/>
+      <c r="N287" s="43"/>
+      <c r="O287" s="43"/>
+      <c r="P287" s="43"/>
+      <c r="Q287" s="43"/>
+      <c r="R287" s="43"/>
+    </row>
+    <row r="288" spans="1:18">
+      <c r="A288" s="42" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resource Roles-14</v>
+      </c>
+      <c r="B288" s="40" t="s">
+        <v>227</v>
+      </c>
+      <c r="C288" s="42">
+        <f>COUNTIF($B$1:$B287,[Table Name])</f>
+        <v>14</v>
+      </c>
+      <c r="D288" s="43">
+        <v>14</v>
+      </c>
+      <c r="E288" s="43">
+        <v>2</v>
+      </c>
+      <c r="F288" s="43"/>
+      <c r="G288" s="43"/>
+      <c r="H288" s="43"/>
+      <c r="I288" s="43"/>
+      <c r="J288" s="43"/>
+      <c r="K288" s="43"/>
+      <c r="L288" s="43"/>
+      <c r="M288" s="43"/>
+      <c r="N288" s="43"/>
+      <c r="O288" s="43"/>
+      <c r="P288" s="43"/>
+      <c r="Q288" s="43"/>
+      <c r="R288" s="43"/>
+    </row>
+    <row r="289" spans="1:18">
+      <c r="A289" s="42" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resource Roles-15</v>
+      </c>
+      <c r="B289" s="40" t="s">
+        <v>227</v>
+      </c>
+      <c r="C289" s="42">
+        <f>COUNTIF($B$1:$B288,[Table Name])</f>
+        <v>15</v>
+      </c>
+      <c r="D289" s="43">
+        <v>15</v>
+      </c>
+      <c r="E289" s="43">
+        <v>2</v>
+      </c>
+      <c r="F289" s="43"/>
+      <c r="G289" s="43"/>
+      <c r="H289" s="43"/>
+      <c r="I289" s="43"/>
+      <c r="J289" s="43"/>
+      <c r="K289" s="43"/>
+      <c r="L289" s="43"/>
+      <c r="M289" s="43"/>
+      <c r="N289" s="43"/>
+      <c r="O289" s="43"/>
+      <c r="P289" s="43"/>
+      <c r="Q289" s="43"/>
+      <c r="R289" s="43"/>
+    </row>
+    <row r="290" spans="1:18">
+      <c r="A290" s="42" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resource Roles-16</v>
+      </c>
+      <c r="B290" s="40" t="s">
+        <v>227</v>
+      </c>
+      <c r="C290" s="42">
+        <f>COUNTIF($B$1:$B289,[Table Name])</f>
+        <v>16</v>
+      </c>
+      <c r="D290" s="43">
+        <v>16</v>
+      </c>
+      <c r="E290" s="43">
+        <v>2</v>
+      </c>
+      <c r="F290" s="43"/>
+      <c r="G290" s="43"/>
+      <c r="H290" s="43"/>
+      <c r="I290" s="43"/>
+      <c r="J290" s="43"/>
+      <c r="K290" s="43"/>
+      <c r="L290" s="43"/>
+      <c r="M290" s="43"/>
+      <c r="N290" s="43"/>
+      <c r="O290" s="43"/>
+      <c r="P290" s="43"/>
+      <c r="Q290" s="43"/>
+      <c r="R290" s="43"/>
+    </row>
+    <row r="291" spans="1:18">
+      <c r="A291" s="42" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resource Roles-17</v>
+      </c>
+      <c r="B291" s="40" t="s">
+        <v>227</v>
+      </c>
+      <c r="C291" s="42">
+        <f>COUNTIF($B$1:$B290,[Table Name])</f>
+        <v>17</v>
+      </c>
+      <c r="D291" s="43">
+        <v>17</v>
+      </c>
+      <c r="E291" s="43">
+        <v>2</v>
+      </c>
+      <c r="F291" s="43"/>
+      <c r="G291" s="43"/>
+      <c r="H291" s="43"/>
+      <c r="I291" s="43"/>
+      <c r="J291" s="43"/>
+      <c r="K291" s="43"/>
+      <c r="L291" s="43"/>
+      <c r="M291" s="43"/>
+      <c r="N291" s="43"/>
+      <c r="O291" s="43"/>
+      <c r="P291" s="43"/>
+      <c r="Q291" s="43"/>
+      <c r="R291" s="43"/>
+    </row>
+    <row r="292" spans="1:18">
+      <c r="A292" s="42" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resource Roles-18</v>
+      </c>
+      <c r="B292" s="40" t="s">
+        <v>227</v>
+      </c>
+      <c r="C292" s="42">
+        <f>COUNTIF($B$1:$B291,[Table Name])</f>
+        <v>18</v>
+      </c>
+      <c r="D292" s="43">
+        <v>18</v>
+      </c>
+      <c r="E292" s="43">
+        <v>2</v>
+      </c>
+      <c r="F292" s="43"/>
+      <c r="G292" s="43"/>
+      <c r="H292" s="43"/>
+      <c r="I292" s="43"/>
+      <c r="J292" s="43"/>
+      <c r="K292" s="43"/>
+      <c r="L292" s="43"/>
+      <c r="M292" s="43"/>
+      <c r="N292" s="43"/>
+      <c r="O292" s="43"/>
+      <c r="P292" s="43"/>
+      <c r="Q292" s="43"/>
+      <c r="R292" s="43"/>
+    </row>
+    <row r="293" spans="1:18">
+      <c r="A293" s="42" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resource Roles-19</v>
+      </c>
+      <c r="B293" s="40" t="s">
+        <v>227</v>
+      </c>
+      <c r="C293" s="42">
+        <f>COUNTIF($B$1:$B292,[Table Name])</f>
+        <v>19</v>
+      </c>
+      <c r="D293" s="43">
+        <v>19</v>
+      </c>
+      <c r="E293" s="43">
+        <v>2</v>
+      </c>
+      <c r="F293" s="43"/>
+      <c r="G293" s="43"/>
+      <c r="H293" s="43"/>
+      <c r="I293" s="43"/>
+      <c r="J293" s="43"/>
+      <c r="K293" s="43"/>
+      <c r="L293" s="43"/>
+      <c r="M293" s="43"/>
+      <c r="N293" s="43"/>
+      <c r="O293" s="43"/>
+      <c r="P293" s="43"/>
+      <c r="Q293" s="43"/>
+      <c r="R293" s="43"/>
+    </row>
+    <row r="294" spans="1:18">
+      <c r="A294" s="42" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resource Roles-20</v>
+      </c>
+      <c r="B294" s="40" t="s">
+        <v>227</v>
+      </c>
+      <c r="C294" s="42">
+        <f>COUNTIF($B$1:$B293,[Table Name])</f>
+        <v>20</v>
+      </c>
+      <c r="D294" s="43">
+        <v>20</v>
+      </c>
+      <c r="E294" s="43">
+        <v>2</v>
+      </c>
+      <c r="F294" s="43"/>
+      <c r="G294" s="43"/>
+      <c r="H294" s="43"/>
+      <c r="I294" s="43"/>
+      <c r="J294" s="43"/>
+      <c r="K294" s="43"/>
+      <c r="L294" s="43"/>
+      <c r="M294" s="43"/>
+      <c r="N294" s="43"/>
+      <c r="O294" s="43"/>
+      <c r="P294" s="43"/>
+      <c r="Q294" s="43"/>
+      <c r="R294" s="43"/>
+    </row>
+    <row r="295" spans="1:18">
+      <c r="A295" s="42" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resource Roles-21</v>
+      </c>
+      <c r="B295" s="40" t="s">
+        <v>227</v>
+      </c>
+      <c r="C295" s="42">
+        <f>COUNTIF($B$1:$B294,[Table Name])</f>
+        <v>21</v>
+      </c>
+      <c r="D295" s="43">
+        <v>21</v>
+      </c>
+      <c r="E295" s="43">
+        <v>2</v>
+      </c>
+      <c r="F295" s="43"/>
+      <c r="G295" s="43"/>
+      <c r="H295" s="43"/>
+      <c r="I295" s="43"/>
+      <c r="J295" s="43"/>
+      <c r="K295" s="43"/>
+      <c r="L295" s="43"/>
+      <c r="M295" s="43"/>
+      <c r="N295" s="43"/>
+      <c r="O295" s="43"/>
+      <c r="P295" s="43"/>
+      <c r="Q295" s="43"/>
+      <c r="R295" s="43"/>
+    </row>
+    <row r="296" spans="1:18">
+      <c r="A296" s="42" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resource Roles-22</v>
+      </c>
+      <c r="B296" s="40" t="s">
+        <v>227</v>
+      </c>
+      <c r="C296" s="42">
+        <f>COUNTIF($B$1:$B295,[Table Name])</f>
+        <v>22</v>
+      </c>
+      <c r="D296" s="43">
+        <v>22</v>
+      </c>
+      <c r="E296" s="43">
+        <v>2</v>
+      </c>
+      <c r="F296" s="43"/>
+      <c r="G296" s="43"/>
+      <c r="H296" s="43"/>
+      <c r="I296" s="43"/>
+      <c r="J296" s="43"/>
+      <c r="K296" s="43"/>
+      <c r="L296" s="43"/>
+      <c r="M296" s="43"/>
+      <c r="N296" s="43"/>
+      <c r="O296" s="43"/>
+      <c r="P296" s="43"/>
+      <c r="Q296" s="43"/>
+      <c r="R296" s="43"/>
+    </row>
+    <row r="297" spans="1:18">
+      <c r="A297" s="42" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resource Roles-23</v>
+      </c>
+      <c r="B297" s="40" t="s">
+        <v>227</v>
+      </c>
+      <c r="C297" s="42">
+        <f>COUNTIF($B$1:$B296,[Table Name])</f>
+        <v>23</v>
+      </c>
+      <c r="D297" s="43">
+        <v>23</v>
+      </c>
+      <c r="E297" s="43">
+        <v>2</v>
+      </c>
+      <c r="F297" s="43"/>
+      <c r="G297" s="43"/>
+      <c r="H297" s="43"/>
+      <c r="I297" s="43"/>
+      <c r="J297" s="43"/>
+      <c r="K297" s="43"/>
+      <c r="L297" s="43"/>
+      <c r="M297" s="43"/>
+      <c r="N297" s="43"/>
+      <c r="O297" s="43"/>
+      <c r="P297" s="43"/>
+      <c r="Q297" s="43"/>
+      <c r="R297" s="43"/>
+    </row>
+    <row r="298" spans="1:18">
+      <c r="A298" s="42" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resource Roles-24</v>
+      </c>
+      <c r="B298" s="40" t="s">
+        <v>227</v>
+      </c>
+      <c r="C298" s="42">
+        <f>COUNTIF($B$1:$B297,[Table Name])</f>
+        <v>24</v>
+      </c>
+      <c r="D298" s="43">
+        <v>24</v>
+      </c>
+      <c r="E298" s="43">
+        <v>2</v>
+      </c>
+      <c r="F298" s="43"/>
+      <c r="G298" s="43"/>
+      <c r="H298" s="43"/>
+      <c r="I298" s="43"/>
+      <c r="J298" s="43"/>
+      <c r="K298" s="43"/>
+      <c r="L298" s="43"/>
+      <c r="M298" s="43"/>
+      <c r="N298" s="43"/>
+      <c r="O298" s="43"/>
+      <c r="P298" s="43"/>
+      <c r="Q298" s="43"/>
+      <c r="R298" s="43"/>
+    </row>
+    <row r="299" spans="1:18">
+      <c r="A299" s="42" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resource Roles-25</v>
+      </c>
+      <c r="B299" s="40" t="s">
+        <v>227</v>
+      </c>
+      <c r="C299" s="42">
+        <f>COUNTIF($B$1:$B298,[Table Name])</f>
+        <v>25</v>
+      </c>
+      <c r="D299" s="43">
+        <v>25</v>
+      </c>
+      <c r="E299" s="43">
+        <v>2</v>
+      </c>
+      <c r="F299" s="43"/>
+      <c r="G299" s="43"/>
+      <c r="H299" s="43"/>
+      <c r="I299" s="43"/>
+      <c r="J299" s="43"/>
+      <c r="K299" s="43"/>
+      <c r="L299" s="43"/>
+      <c r="M299" s="43"/>
+      <c r="N299" s="43"/>
+      <c r="O299" s="43"/>
+      <c r="P299" s="43"/>
+      <c r="Q299" s="43"/>
+      <c r="R299" s="43"/>
+    </row>
+    <row r="300" spans="1:18">
+      <c r="A300" s="42" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resource Roles-26</v>
+      </c>
+      <c r="B300" s="40" t="s">
+        <v>227</v>
+      </c>
+      <c r="C300" s="42">
+        <f>COUNTIF($B$1:$B299,[Table Name])</f>
+        <v>26</v>
+      </c>
+      <c r="D300" s="43">
+        <v>26</v>
+      </c>
+      <c r="E300" s="43">
+        <v>2</v>
+      </c>
+      <c r="F300" s="43"/>
+      <c r="G300" s="43"/>
+      <c r="H300" s="43"/>
+      <c r="I300" s="43"/>
+      <c r="J300" s="43"/>
+      <c r="K300" s="43"/>
+      <c r="L300" s="43"/>
+      <c r="M300" s="43"/>
+      <c r="N300" s="43"/>
+      <c r="O300" s="43"/>
+      <c r="P300" s="43"/>
+      <c r="Q300" s="43"/>
+      <c r="R300" s="43"/>
+    </row>
+    <row r="301" spans="1:18">
+      <c r="A301" s="42" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resource Roles-27</v>
+      </c>
+      <c r="B301" s="40" t="s">
+        <v>227</v>
+      </c>
+      <c r="C301" s="42">
+        <f>COUNTIF($B$1:$B300,[Table Name])</f>
+        <v>27</v>
+      </c>
+      <c r="D301" s="43">
+        <v>27</v>
+      </c>
+      <c r="E301" s="43">
+        <v>2</v>
+      </c>
+      <c r="F301" s="43"/>
+      <c r="G301" s="43"/>
+      <c r="H301" s="43"/>
+      <c r="I301" s="43"/>
+      <c r="J301" s="43"/>
+      <c r="K301" s="43"/>
+      <c r="L301" s="43"/>
+      <c r="M301" s="43"/>
+      <c r="N301" s="43"/>
+      <c r="O301" s="43"/>
+      <c r="P301" s="43"/>
+      <c r="Q301" s="43"/>
+      <c r="R301" s="43"/>
+    </row>
+    <row r="302" spans="1:18">
+      <c r="A302" s="42" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resource Roles-28</v>
+      </c>
+      <c r="B302" s="40" t="s">
+        <v>227</v>
+      </c>
+      <c r="C302" s="42">
+        <f>COUNTIF($B$1:$B301,[Table Name])</f>
+        <v>28</v>
+      </c>
+      <c r="D302" s="43">
+        <v>28</v>
+      </c>
+      <c r="E302" s="43">
+        <v>2</v>
+      </c>
+      <c r="F302" s="43"/>
+      <c r="G302" s="43"/>
+      <c r="H302" s="43"/>
+      <c r="I302" s="43"/>
+      <c r="J302" s="43"/>
+      <c r="K302" s="43"/>
+      <c r="L302" s="43"/>
+      <c r="M302" s="43"/>
+      <c r="N302" s="43"/>
+      <c r="O302" s="43"/>
+      <c r="P302" s="43"/>
+      <c r="Q302" s="43"/>
+      <c r="R302" s="43"/>
+    </row>
+    <row r="303" spans="1:18">
+      <c r="A303" s="42" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resource Roles-29</v>
+      </c>
+      <c r="B303" s="40" t="s">
+        <v>227</v>
+      </c>
+      <c r="C303" s="42">
+        <f>COUNTIF($B$1:$B302,[Table Name])</f>
+        <v>29</v>
+      </c>
+      <c r="D303" s="43">
+        <v>29</v>
+      </c>
+      <c r="E303" s="43">
+        <v>2</v>
+      </c>
+      <c r="F303" s="43"/>
+      <c r="G303" s="43"/>
+      <c r="H303" s="43"/>
+      <c r="I303" s="43"/>
+      <c r="J303" s="43"/>
+      <c r="K303" s="43"/>
+      <c r="L303" s="43"/>
+      <c r="M303" s="43"/>
+      <c r="N303" s="43"/>
+      <c r="O303" s="43"/>
+      <c r="P303" s="43"/>
+      <c r="Q303" s="43"/>
+      <c r="R303" s="43"/>
+    </row>
+    <row r="304" spans="1:18">
+      <c r="A304" s="42" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resource Roles-30</v>
+      </c>
+      <c r="B304" s="40" t="s">
+        <v>227</v>
+      </c>
+      <c r="C304" s="42">
+        <f>COUNTIF($B$1:$B303,[Table Name])</f>
+        <v>30</v>
+      </c>
+      <c r="D304" s="43">
+        <v>30</v>
+      </c>
+      <c r="E304" s="43">
+        <v>2</v>
+      </c>
+      <c r="F304" s="43"/>
+      <c r="G304" s="43"/>
+      <c r="H304" s="43"/>
+      <c r="I304" s="43"/>
+      <c r="J304" s="43"/>
+      <c r="K304" s="43"/>
+      <c r="L304" s="43"/>
+      <c r="M304" s="43"/>
+      <c r="N304" s="43"/>
+      <c r="O304" s="43"/>
+      <c r="P304" s="43"/>
+      <c r="Q304" s="43"/>
+      <c r="R304" s="43"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
@@ -34656,8 +35396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -35164,7 +35904,7 @@
         <v>ResourceActionData</v>
       </c>
       <c r="E25" s="7" t="str">
-        <f>"truncate"</f>
+        <f t="shared" ref="E25:E30" si="2">"truncate"</f>
         <v>truncate</v>
       </c>
     </row>
@@ -35184,7 +35924,7 @@
         <v>ResourceListRelation</v>
       </c>
       <c r="E26" s="7" t="str">
-        <f>"truncate"</f>
+        <f t="shared" si="2"/>
         <v>truncate</v>
       </c>
     </row>
@@ -35204,7 +35944,7 @@
         <v>ResourceFormCollection</v>
       </c>
       <c r="E27" s="7" t="str">
-        <f>"truncate"</f>
+        <f t="shared" si="2"/>
         <v>truncate</v>
       </c>
     </row>
@@ -35224,7 +35964,7 @@
         <v>User</v>
       </c>
       <c r="E28" s="7" t="str">
-        <f>"truncate"</f>
+        <f t="shared" si="2"/>
         <v>truncate</v>
       </c>
     </row>
@@ -35244,7 +35984,7 @@
         <v>ResourceFormFieldOption</v>
       </c>
       <c r="E29" s="7" t="str">
-        <f>"truncate"</f>
+        <f t="shared" si="2"/>
         <v>truncate</v>
       </c>
     </row>
@@ -35264,7 +36004,7 @@
         <v>ResourceDataScope</v>
       </c>
       <c r="E30" s="7" t="str">
-        <f>"truncate"</f>
+        <f t="shared" si="2"/>
         <v>truncate</v>
       </c>
     </row>
@@ -37632,8 +38372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:R40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -37643,14 +38383,14 @@
   <sheetData>
     <row r="1" spans="1:20" s="38" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="48" t="s">
-        <v>464</v>
+        <v>227</v>
       </c>
       <c r="B1" s="48"/>
       <c r="C1" s="48"/>
       <c r="D1" s="48"/>
       <c r="E1" s="49" t="str">
         <f>"\"&amp;VLOOKUP($A$1,SeedMap[],3,0)&amp;"\"&amp;VLOOKUP($A$1,SeedMap[],4,0)&amp;"::"&amp;VLOOKUP($A$1,SeedMap[],5,0)&amp;"()"</f>
-        <v>\Milestone\Appframe\Model\ResourceFormFieldOption::truncate()</v>
+        <v>\Milestone\Appframe\Model\ResourceRole::truncate()</v>
       </c>
       <c r="F1" s="49"/>
       <c r="G1" s="49"/>
@@ -37794,19 +38534,19 @@
       <c r="B5" s="28"/>
       <c r="C5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],C$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],C$4+$B$4,0))</f>
-        <v>form_field</v>
+        <v>resource</v>
       </c>
       <c r="D5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],D$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],D$4+$B$4,0))</f>
-        <v>type</v>
+        <v>role</v>
       </c>
       <c r="E5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0))</f>
-        <v/>
+        <v>actions_availability</v>
       </c>
       <c r="F5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0))</f>
-        <v/>
+        <v>actions</v>
       </c>
       <c r="G5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0))</f>
@@ -37908,7 +38648,7 @@
       <c r="A8" s="32"/>
       <c r="B8" s="47" t="str">
         <f>$E$1</f>
-        <v>\Milestone\Appframe\Model\ResourceFormFieldOption::truncate()</v>
+        <v>\Milestone\Appframe\Model\ResourceRole::truncate()</v>
       </c>
       <c r="C8" s="47"/>
       <c r="D8" s="47"/>
@@ -37933,23 +38673,23 @@
       </c>
       <c r="B9" s="30" t="str">
         <f ca="1">IF($B8="","",IF($B8=";",$I$3,IF($B8=$I$3,"",IF(ISNA(VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),1,0)),";",$S$4))))</f>
-        <v>;</v>
+        <v>-&gt;create([</v>
       </c>
       <c r="C9" s="33" t="str">
         <f ca="1">IF(AND($B9=$S$4,C$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),C$4+$B$4,0)="","","'"&amp;C$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),C$4+$B$4,0)&amp;"', "),"")</f>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '1', </v>
       </c>
       <c r="D9" s="33" t="str">
         <f t="shared" ref="D9:Q24" ca="1" si="0">IF(AND($B9=$S$4,D$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),D$4+$B$4,0)="","","'"&amp;D$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),D$4+$B$4,0)&amp;"', "),"")</f>
-        <v/>
+        <v xml:space="preserve">'role' =&gt; '1', </v>
       </c>
       <c r="E9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'actions_availability' =&gt; 'Only', </v>
       </c>
       <c r="F9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'actions' =&gt; '2,3,5,6,7,8,9,10', </v>
       </c>
       <c r="G9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -37997,7 +38737,7 @@
       </c>
       <c r="R9" s="33" t="str">
         <f ca="1">IF(B9=$S$4,$T$4,"")</f>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="10" spans="1:20">
@@ -38006,15 +38746,15 @@
       </c>
       <c r="B10" s="30" t="str">
         <f t="shared" ref="B10:B73" ca="1" si="1">IF($B9="","",IF($B9=";",$I$3,IF($B9=$I$3,"",IF(ISNA(VLOOKUP($A$1&amp;"-"&amp;$A10,INDIRECT($E$2),1,0)),";",$S$4))))</f>
-        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
+        <v>-&gt;create([</v>
       </c>
       <c r="C10" s="33" t="str">
         <f ca="1">IF(AND($B10=$S$4,C$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A10,INDIRECT($E$2),C$4+$B$4,0)="","","'"&amp;C$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A10,INDIRECT($E$2),C$4+$B$4,0)&amp;"', "),"")</f>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '1', </v>
       </c>
       <c r="D10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'role' =&gt; '3', </v>
       </c>
       <c r="E10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -38070,7 +38810,7 @@
       </c>
       <c r="R10" s="33" t="str">
         <f t="shared" ref="R10:R73" ca="1" si="2">IF(B10=$S$4,$T$4,"")</f>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -38079,15 +38819,15 @@
       </c>
       <c r="B11" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C11" s="33" t="str">
         <f t="shared" ref="C11:G74" ca="1" si="3">IF(AND($B11=$S$4,C$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A11,INDIRECT($E$2),C$4+$B$4,0)="","","'"&amp;C$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A11,INDIRECT($E$2),C$4+$B$4,0)&amp;"', "),"")</f>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '2', </v>
       </c>
       <c r="D11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'role' =&gt; '3', </v>
       </c>
       <c r="E11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -38143,7 +38883,7 @@
       </c>
       <c r="R11" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -38152,15 +38892,15 @@
       </c>
       <c r="B12" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C12" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '3', </v>
       </c>
       <c r="D12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'role' =&gt; '3', </v>
       </c>
       <c r="E12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -38216,7 +38956,7 @@
       </c>
       <c r="R12" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -38225,15 +38965,15 @@
       </c>
       <c r="B13" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C13" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '4', </v>
       </c>
       <c r="D13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'role' =&gt; '2', </v>
       </c>
       <c r="E13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -38289,7 +39029,7 @@
       </c>
       <c r="R13" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -38298,15 +39038,15 @@
       </c>
       <c r="B14" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C14" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '5', </v>
       </c>
       <c r="D14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'role' =&gt; '1', </v>
       </c>
       <c r="E14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -38362,7 +39102,7 @@
       </c>
       <c r="R14" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -38371,15 +39111,15 @@
       </c>
       <c r="B15" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C15" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '5', </v>
       </c>
       <c r="D15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'role' =&gt; '3', </v>
       </c>
       <c r="E15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -38435,7 +39175,7 @@
       </c>
       <c r="R15" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="16" spans="1:20">
@@ -38444,15 +39184,15 @@
       </c>
       <c r="B16" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C16" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '7', </v>
       </c>
       <c r="D16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'role' =&gt; '2', </v>
       </c>
       <c r="E16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -38508,7 +39248,7 @@
       </c>
       <c r="R16" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="17" spans="1:18">
@@ -38517,15 +39257,15 @@
       </c>
       <c r="B17" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C17" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '8', </v>
       </c>
       <c r="D17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'role' =&gt; '2', </v>
       </c>
       <c r="E17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -38581,7 +39321,7 @@
       </c>
       <c r="R17" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="18" spans="1:18">
@@ -38590,15 +39330,15 @@
       </c>
       <c r="B18" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C18" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '9', </v>
       </c>
       <c r="D18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'role' =&gt; '2', </v>
       </c>
       <c r="E18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -38654,7 +39394,7 @@
       </c>
       <c r="R18" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="19" spans="1:18">
@@ -38663,15 +39403,15 @@
       </c>
       <c r="B19" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C19" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '10', </v>
       </c>
       <c r="D19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'role' =&gt; '2', </v>
       </c>
       <c r="E19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -38727,7 +39467,7 @@
       </c>
       <c r="R19" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="20" spans="1:18">
@@ -38736,15 +39476,15 @@
       </c>
       <c r="B20" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C20" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '12', </v>
       </c>
       <c r="D20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'role' =&gt; '2', </v>
       </c>
       <c r="E20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -38800,7 +39540,7 @@
       </c>
       <c r="R20" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="21" spans="1:18">
@@ -38809,15 +39549,15 @@
       </c>
       <c r="B21" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C21" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '13', </v>
       </c>
       <c r="D21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'role' =&gt; '2', </v>
       </c>
       <c r="E21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -38873,7 +39613,7 @@
       </c>
       <c r="R21" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="22" spans="1:18">
@@ -38882,15 +39622,15 @@
       </c>
       <c r="B22" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C22" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '14', </v>
       </c>
       <c r="D22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'role' =&gt; '2', </v>
       </c>
       <c r="E22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -38946,7 +39686,7 @@
       </c>
       <c r="R22" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="23" spans="1:18">
@@ -38955,15 +39695,15 @@
       </c>
       <c r="B23" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C23" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '15', </v>
       </c>
       <c r="D23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'role' =&gt; '2', </v>
       </c>
       <c r="E23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -39019,7 +39759,7 @@
       </c>
       <c r="R23" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="24" spans="1:18">
@@ -39028,15 +39768,15 @@
       </c>
       <c r="B24" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C24" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '16', </v>
       </c>
       <c r="D24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'role' =&gt; '2', </v>
       </c>
       <c r="E24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -39092,7 +39832,7 @@
       </c>
       <c r="R24" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="25" spans="1:18">
@@ -39101,15 +39841,15 @@
       </c>
       <c r="B25" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '17', </v>
       </c>
       <c r="D25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'role' =&gt; '2', </v>
       </c>
       <c r="E25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -39165,7 +39905,7 @@
       </c>
       <c r="R25" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="26" spans="1:18">
@@ -39174,15 +39914,15 @@
       </c>
       <c r="B26" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '18', </v>
       </c>
       <c r="D26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'role' =&gt; '2', </v>
       </c>
       <c r="E26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -39238,7 +39978,7 @@
       </c>
       <c r="R26" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="27" spans="1:18">
@@ -39247,15 +39987,15 @@
       </c>
       <c r="B27" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '19', </v>
       </c>
       <c r="D27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'role' =&gt; '2', </v>
       </c>
       <c r="E27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -39311,7 +40051,7 @@
       </c>
       <c r="R27" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="28" spans="1:18">
@@ -39320,15 +40060,15 @@
       </c>
       <c r="B28" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '20', </v>
       </c>
       <c r="D28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'role' =&gt; '2', </v>
       </c>
       <c r="E28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -39384,7 +40124,7 @@
       </c>
       <c r="R28" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="29" spans="1:18">
@@ -39393,15 +40133,15 @@
       </c>
       <c r="B29" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '21', </v>
       </c>
       <c r="D29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'role' =&gt; '2', </v>
       </c>
       <c r="E29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -39457,7 +40197,7 @@
       </c>
       <c r="R29" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="30" spans="1:18">
@@ -39466,15 +40206,15 @@
       </c>
       <c r="B30" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '22', </v>
       </c>
       <c r="D30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'role' =&gt; '2', </v>
       </c>
       <c r="E30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -39530,7 +40270,7 @@
       </c>
       <c r="R30" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="31" spans="1:18">
@@ -39539,15 +40279,15 @@
       </c>
       <c r="B31" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '23', </v>
       </c>
       <c r="D31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'role' =&gt; '2', </v>
       </c>
       <c r="E31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -39603,7 +40343,7 @@
       </c>
       <c r="R31" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="32" spans="1:18">
@@ -39612,15 +40352,15 @@
       </c>
       <c r="B32" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '24', </v>
       </c>
       <c r="D32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'role' =&gt; '2', </v>
       </c>
       <c r="E32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -39676,7 +40416,7 @@
       </c>
       <c r="R32" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="33" spans="1:18">
@@ -39685,15 +40425,15 @@
       </c>
       <c r="B33" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '25', </v>
       </c>
       <c r="D33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'role' =&gt; '2', </v>
       </c>
       <c r="E33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -39749,7 +40489,7 @@
       </c>
       <c r="R33" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="34" spans="1:18">
@@ -39758,15 +40498,15 @@
       </c>
       <c r="B34" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '26', </v>
       </c>
       <c r="D34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'role' =&gt; '2', </v>
       </c>
       <c r="E34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -39822,7 +40562,7 @@
       </c>
       <c r="R34" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="35" spans="1:18">
@@ -39831,15 +40571,15 @@
       </c>
       <c r="B35" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '27', </v>
       </c>
       <c r="D35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'role' =&gt; '2', </v>
       </c>
       <c r="E35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -39895,7 +40635,7 @@
       </c>
       <c r="R35" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="36" spans="1:18">
@@ -39904,15 +40644,15 @@
       </c>
       <c r="B36" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '28', </v>
       </c>
       <c r="D36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'role' =&gt; '2', </v>
       </c>
       <c r="E36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -39968,7 +40708,7 @@
       </c>
       <c r="R36" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="37" spans="1:18">
@@ -39977,15 +40717,15 @@
       </c>
       <c r="B37" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '29', </v>
       </c>
       <c r="D37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'role' =&gt; '2', </v>
       </c>
       <c r="E37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -40041,7 +40781,7 @@
       </c>
       <c r="R37" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="38" spans="1:18">
@@ -40050,15 +40790,15 @@
       </c>
       <c r="B38" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '30', </v>
       </c>
       <c r="D38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'role' =&gt; '2', </v>
       </c>
       <c r="E38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -40114,7 +40854,7 @@
       </c>
       <c r="R38" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="39" spans="1:18">
@@ -40123,7 +40863,7 @@
       </c>
       <c r="B39" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>;</v>
       </c>
       <c r="C39" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -40196,7 +40936,7 @@
       </c>
       <c r="B40" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
       </c>
       <c r="C40" s="33" t="str">
         <f t="shared" ca="1" si="3"/>

</xml_diff>

<commit_message>
New Resource, List Search added
</commit_message>
<xml_diff>
--- a/Helper.xlsx
+++ b/Helper.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3281" uniqueCount="671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3339" uniqueCount="679">
   <si>
     <t>resource_scopes</t>
   </si>
@@ -2051,6 +2051,30 @@
   </si>
   <si>
     <t>Data Scopes</t>
+  </si>
+  <si>
+    <t>resource_list_search</t>
+  </si>
+  <si>
+    <t>Resource List Search</t>
+  </si>
+  <si>
+    <t>ResourceListSearch</t>
+  </si>
+  <si>
+    <t>Searchable fields in a list</t>
+  </si>
+  <si>
+    <t>List Search</t>
+  </si>
+  <si>
+    <t>__resource_list_search</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>Search fields for a list</t>
   </si>
 </sst>
 </file>
@@ -4054,8 +4078,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tables" displayName="Tables" ref="A1:J36" totalsRowShown="0" dataDxfId="122">
-  <autoFilter ref="A1:J36"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tables" displayName="Tables" ref="A1:J37" totalsRowShown="0" dataDxfId="122">
+  <autoFilter ref="A1:J37"/>
   <tableColumns count="10">
     <tableColumn id="2" name="Name" dataDxfId="121"/>
     <tableColumn id="10" name="Table" dataDxfId="120">
@@ -4140,11 +4164,12 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TableFields" displayName="TableFields" ref="A1:K310" totalsRowShown="0" dataDxfId="95">
-  <autoFilter ref="A1:K310">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TableFields" displayName="TableFields" ref="A1:K323" totalsRowShown="0" dataDxfId="95">
+  <autoFilter ref="A1:K323">
     <filterColumn colId="0">
       <filters>
-        <filter val="resource_form_collection"/>
+        <filter val="resource_form_field_data"/>
+        <filter val="resource_list_search"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -4184,8 +4209,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R304" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
-  <autoFilter ref="A1:R304">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R307" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
+  <autoFilter ref="A1:R307">
     <filterColumn colId="1">
       <filters>
         <filter val="Resource Roles"/>
@@ -4221,8 +4246,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SeedMap" displayName="SeedMap" ref="A1:E30" totalsRowShown="0" dataDxfId="63">
-  <autoFilter ref="A1:E30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SeedMap" displayName="SeedMap" ref="A1:E31" totalsRowShown="0" dataDxfId="63">
+  <autoFilter ref="A1:E31"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Name" dataDxfId="62"/>
     <tableColumn id="3" name="FW Table Name" dataDxfId="61"/>
@@ -4241,8 +4266,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="ResourceTable" displayName="ResourceTable" ref="A1:I31" totalsRowShown="0" dataDxfId="57">
-  <autoFilter ref="A1:I31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="ResourceTable" displayName="ResourceTable" ref="A1:I32" totalsRowShown="0" dataDxfId="57">
+  <autoFilter ref="A1:I32"/>
   <tableColumns count="9">
     <tableColumn id="1" name="No" dataDxfId="56">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
@@ -4265,8 +4290,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RelationTable" displayName="RelationTable" ref="A1:I44" totalsRowShown="0" dataDxfId="47">
-  <autoFilter ref="A1:I44"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RelationTable" displayName="RelationTable" ref="A1:I45" totalsRowShown="0" dataDxfId="47">
+  <autoFilter ref="A1:I45"/>
   <tableColumns count="9">
     <tableColumn id="1" name="No" dataDxfId="46">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
@@ -4620,10 +4645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J36"/>
+    <sheetView topLeftCell="G31" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4683,7 +4708,7 @@
         <v>user</v>
       </c>
       <c r="D2" s="8" t="str">
-        <f t="shared" ref="D2:D36" si="0">"Milestone\Appframe\Model"</f>
+        <f t="shared" ref="D2:D37" si="0">"Milestone\Appframe\Model"</f>
         <v>Milestone\Appframe\Model</v>
       </c>
       <c r="E2" s="8" t="str">
@@ -5368,139 +5393,139 @@
       </c>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="4" t="s">
+        <v>671</v>
+      </c>
+      <c r="B19" s="7" t="str">
+        <f>"__"&amp;[Name]</f>
+        <v>__resource_list_search</v>
+      </c>
+      <c r="C19" s="7" t="str">
+        <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
+        <v>resource_list_search</v>
+      </c>
+      <c r="D19" s="7" t="str">
+        <f>"Milestone\Appframe\Model"</f>
+        <v>Milestone\Appframe\Model</v>
+      </c>
+      <c r="E19" s="8" t="str">
+        <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
+        <v>ResourceListSearch</v>
+      </c>
+      <c r="F19" s="8" t="str">
+        <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
+        <v>php artisan make:migration create___resource_list_search_table --create=__resource_list_search</v>
+      </c>
+      <c r="G19" s="8" t="str">
+        <f>"php artisan make:model "&amp;[Class Name]</f>
+        <v>php artisan make:model ResourceListSearch</v>
+      </c>
+      <c r="H19" s="8" t="str">
+        <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
+        <v>protected $table = '__resource_list_search';</v>
+      </c>
+      <c r="I19" s="8" t="str">
+        <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
+        <v>php artisan make:seed ResourceListSearchTableSeeder</v>
+      </c>
+      <c r="J19" s="8" t="str">
+        <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
+        <v>ResourceListSearchTableSeeder::class,</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="9" t="str">
+      <c r="B20" s="9" t="str">
         <f>"__"&amp;[Name]</f>
         <v>__resource_forms</v>
       </c>
-      <c r="C19" s="9" t="str">
+      <c r="C20" s="9" t="str">
         <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
         <v>resource_form</v>
       </c>
-      <c r="D19" s="9" t="str">
+      <c r="D20" s="9" t="str">
         <f t="shared" si="0"/>
         <v>Milestone\Appframe\Model</v>
       </c>
-      <c r="E19" s="8" t="str">
+      <c r="E20" s="8" t="str">
         <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
         <v>ResourceForm</v>
       </c>
-      <c r="F19" s="8" t="str">
+      <c r="F20" s="8" t="str">
         <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
         <v>php artisan make:migration create___resource_forms_table --create=__resource_forms</v>
       </c>
-      <c r="G19" s="8" t="str">
+      <c r="G20" s="8" t="str">
         <f>"php artisan make:model "&amp;[Class Name]</f>
         <v>php artisan make:model ResourceForm</v>
       </c>
-      <c r="H19" s="8" t="str">
+      <c r="H20" s="8" t="str">
         <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
         <v>protected $table = '__resource_forms';</v>
       </c>
-      <c r="I19" s="8" t="str">
+      <c r="I20" s="8" t="str">
         <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
         <v>php artisan make:seed ResourceFormTableSeeder</v>
       </c>
-      <c r="J19" s="8" t="str">
+      <c r="J20" s="8" t="str">
         <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
         <v>ResourceFormTableSeeder::class,</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="2" t="s">
+    <row r="21" spans="1:10">
+      <c r="A21" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B20" s="9" t="str">
+      <c r="B21" s="9" t="str">
         <f>"__"&amp;[Name]</f>
         <v>__resource_form_defaults</v>
       </c>
-      <c r="C20" s="7" t="str">
+      <c r="C21" s="7" t="str">
         <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
         <v>resource_form_default</v>
       </c>
-      <c r="D20" s="7" t="str">
+      <c r="D21" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Milestone\Appframe\Model</v>
       </c>
-      <c r="E20" s="8" t="str">
+      <c r="E21" s="8" t="str">
         <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
         <v>ResourceFormDefault</v>
       </c>
-      <c r="F20" s="8" t="str">
+      <c r="F21" s="8" t="str">
         <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
         <v>php artisan make:migration create___resource_form_defaults_table --create=__resource_form_defaults</v>
       </c>
-      <c r="G20" s="8" t="str">
+      <c r="G21" s="8" t="str">
         <f>"php artisan make:model "&amp;[Class Name]</f>
         <v>php artisan make:model ResourceFormDefault</v>
       </c>
-      <c r="H20" s="8" t="str">
+      <c r="H21" s="8" t="str">
         <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
         <v>protected $table = '__resource_form_defaults';</v>
       </c>
-      <c r="I20" s="8" t="str">
+      <c r="I21" s="8" t="str">
         <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
         <v>php artisan make:seed ResourceFormDefaultTableSeeder</v>
       </c>
-      <c r="J20" s="8" t="str">
+      <c r="J21" s="8" t="str">
         <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
         <v>ResourceFormDefaultTableSeeder::class,</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="2" t="s">
+    <row r="22" spans="1:10">
+      <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="9" t="str">
+      <c r="B22" s="9" t="str">
         <f>"__"&amp;[Name]</f>
         <v>__resource_defaults</v>
       </c>
-      <c r="C21" s="9" t="str">
+      <c r="C22" s="9" t="str">
         <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
         <v>resource_default</v>
-      </c>
-      <c r="D21" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Milestone\Appframe\Model</v>
-      </c>
-      <c r="E21" s="8" t="str">
-        <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
-        <v>ResourceDefault</v>
-      </c>
-      <c r="F21" s="8" t="str">
-        <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
-        <v>php artisan make:migration create___resource_defaults_table --create=__resource_defaults</v>
-      </c>
-      <c r="G21" s="8" t="str">
-        <f>"php artisan make:model "&amp;[Class Name]</f>
-        <v>php artisan make:model ResourceDefault</v>
-      </c>
-      <c r="H21" s="8" t="str">
-        <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
-        <v>protected $table = '__resource_defaults';</v>
-      </c>
-      <c r="I21" s="8" t="str">
-        <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
-        <v>php artisan make:seed ResourceDefaultTableSeeder</v>
-      </c>
-      <c r="J21" s="8" t="str">
-        <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
-        <v>ResourceDefaultTableSeeder::class,</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="9" t="str">
-        <f>"__"&amp;[Name]</f>
-        <v>__resource_actions</v>
-      </c>
-      <c r="C22" s="9" t="str">
-        <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
-        <v>resource_action</v>
       </c>
       <c r="D22" s="9" t="str">
         <f t="shared" si="0"/>
@@ -5508,40 +5533,40 @@
       </c>
       <c r="E22" s="8" t="str">
         <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
-        <v>ResourceAction</v>
+        <v>ResourceDefault</v>
       </c>
       <c r="F22" s="8" t="str">
         <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
-        <v>php artisan make:migration create___resource_actions_table --create=__resource_actions</v>
+        <v>php artisan make:migration create___resource_defaults_table --create=__resource_defaults</v>
       </c>
       <c r="G22" s="8" t="str">
         <f>"php artisan make:model "&amp;[Class Name]</f>
-        <v>php artisan make:model ResourceAction</v>
+        <v>php artisan make:model ResourceDefault</v>
       </c>
       <c r="H22" s="8" t="str">
         <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
-        <v>protected $table = '__resource_actions';</v>
+        <v>protected $table = '__resource_defaults';</v>
       </c>
       <c r="I22" s="8" t="str">
         <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
-        <v>php artisan make:seed ResourceActionTableSeeder</v>
+        <v>php artisan make:seed ResourceDefaultTableSeeder</v>
       </c>
       <c r="J22" s="8" t="str">
         <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
-        <v>ResourceActionTableSeeder::class,</v>
+        <v>ResourceDefaultTableSeeder::class,</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="2" t="s">
-        <v>100</v>
+        <v>8</v>
       </c>
       <c r="B23" s="9" t="str">
         <f>"__"&amp;[Name]</f>
-        <v>__resource_action_attrs</v>
+        <v>__resource_actions</v>
       </c>
       <c r="C23" s="9" t="str">
         <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
-        <v>resource_action_attr</v>
+        <v>resource_action</v>
       </c>
       <c r="D23" s="9" t="str">
         <f t="shared" si="0"/>
@@ -5549,40 +5574,40 @@
       </c>
       <c r="E23" s="8" t="str">
         <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
-        <v>ResourceActionAttr</v>
+        <v>ResourceAction</v>
       </c>
       <c r="F23" s="8" t="str">
         <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
-        <v>php artisan make:migration create___resource_action_attrs_table --create=__resource_action_attrs</v>
+        <v>php artisan make:migration create___resource_actions_table --create=__resource_actions</v>
       </c>
       <c r="G23" s="8" t="str">
         <f>"php artisan make:model "&amp;[Class Name]</f>
-        <v>php artisan make:model ResourceActionAttr</v>
+        <v>php artisan make:model ResourceAction</v>
       </c>
       <c r="H23" s="8" t="str">
         <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
-        <v>protected $table = '__resource_action_attrs';</v>
+        <v>protected $table = '__resource_actions';</v>
       </c>
       <c r="I23" s="8" t="str">
         <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
-        <v>php artisan make:seed ResourceActionAttrTableSeeder</v>
+        <v>php artisan make:seed ResourceActionTableSeeder</v>
       </c>
       <c r="J23" s="8" t="str">
         <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
-        <v>ResourceActionAttrTableSeeder::class,</v>
+        <v>ResourceActionTableSeeder::class,</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B24" s="9" t="str">
         <f>"__"&amp;[Name]</f>
-        <v>__resource_action_methods</v>
+        <v>__resource_action_attrs</v>
       </c>
       <c r="C24" s="9" t="str">
         <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
-        <v>resource_action_method</v>
+        <v>resource_action_attr</v>
       </c>
       <c r="D24" s="9" t="str">
         <f t="shared" si="0"/>
@@ -5590,81 +5615,81 @@
       </c>
       <c r="E24" s="8" t="str">
         <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
-        <v>ResourceActionMethod</v>
+        <v>ResourceActionAttr</v>
       </c>
       <c r="F24" s="8" t="str">
         <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
-        <v>php artisan make:migration create___resource_action_methods_table --create=__resource_action_methods</v>
+        <v>php artisan make:migration create___resource_action_attrs_table --create=__resource_action_attrs</v>
       </c>
       <c r="G24" s="8" t="str">
         <f>"php artisan make:model "&amp;[Class Name]</f>
-        <v>php artisan make:model ResourceActionMethod</v>
+        <v>php artisan make:model ResourceActionAttr</v>
       </c>
       <c r="H24" s="8" t="str">
         <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
-        <v>protected $table = '__resource_action_methods';</v>
+        <v>protected $table = '__resource_action_attrs';</v>
       </c>
       <c r="I24" s="8" t="str">
         <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
-        <v>php artisan make:seed ResourceActionMethodTableSeeder</v>
+        <v>php artisan make:seed ResourceActionAttrTableSeeder</v>
       </c>
       <c r="J24" s="8" t="str">
         <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
+        <v>ResourceActionAttrTableSeeder::class,</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B25" s="9" t="str">
+        <f>"__"&amp;[Name]</f>
+        <v>__resource_action_methods</v>
+      </c>
+      <c r="C25" s="9" t="str">
+        <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
+        <v>resource_action_method</v>
+      </c>
+      <c r="D25" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>Milestone\Appframe\Model</v>
+      </c>
+      <c r="E25" s="8" t="str">
+        <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
+        <v>ResourceActionMethod</v>
+      </c>
+      <c r="F25" s="8" t="str">
+        <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
+        <v>php artisan make:migration create___resource_action_methods_table --create=__resource_action_methods</v>
+      </c>
+      <c r="G25" s="8" t="str">
+        <f>"php artisan make:model "&amp;[Class Name]</f>
+        <v>php artisan make:model ResourceActionMethod</v>
+      </c>
+      <c r="H25" s="8" t="str">
+        <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
+        <v>protected $table = '__resource_action_methods';</v>
+      </c>
+      <c r="I25" s="8" t="str">
+        <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
+        <v>php artisan make:seed ResourceActionMethodTableSeeder</v>
+      </c>
+      <c r="J25" s="8" t="str">
+        <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
         <v>ResourceActionMethodTableSeeder::class,</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="4" t="s">
+    <row r="26" spans="1:10">
+      <c r="A26" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B25" s="7" t="str">
+      <c r="B26" s="7" t="str">
         <f>"__"&amp;[Name]</f>
         <v>__resource_action_lists</v>
       </c>
-      <c r="C25" s="7" t="str">
+      <c r="C26" s="7" t="str">
         <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
         <v>resource_action_list</v>
-      </c>
-      <c r="D25" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>Milestone\Appframe\Model</v>
-      </c>
-      <c r="E25" s="8" t="str">
-        <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
-        <v>ResourceActionList</v>
-      </c>
-      <c r="F25" s="8" t="str">
-        <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
-        <v>php artisan make:migration create___resource_action_lists_table --create=__resource_action_lists</v>
-      </c>
-      <c r="G25" s="8" t="str">
-        <f>"php artisan make:model "&amp;[Class Name]</f>
-        <v>php artisan make:model ResourceActionList</v>
-      </c>
-      <c r="H25" s="8" t="str">
-        <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
-        <v>protected $table = '__resource_action_lists';</v>
-      </c>
-      <c r="I25" s="8" t="str">
-        <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
-        <v>php artisan make:seed ResourceActionListTableSeeder</v>
-      </c>
-      <c r="J25" s="8" t="str">
-        <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
-        <v>ResourceActionListTableSeeder::class,</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="B26" s="7" t="str">
-        <f>"__"&amp;[Name]</f>
-        <v>__resource_action_data</v>
-      </c>
-      <c r="C26" s="7" t="str">
-        <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
-        <v>resource_action_data</v>
       </c>
       <c r="D26" s="7" t="str">
         <f t="shared" si="0"/>
@@ -5672,122 +5697,122 @@
       </c>
       <c r="E26" s="8" t="str">
         <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
-        <v>ResourceActionData</v>
+        <v>ResourceActionList</v>
       </c>
       <c r="F26" s="8" t="str">
         <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
-        <v>php artisan make:migration create___resource_action_data_table --create=__resource_action_data</v>
+        <v>php artisan make:migration create___resource_action_lists_table --create=__resource_action_lists</v>
       </c>
       <c r="G26" s="8" t="str">
         <f>"php artisan make:model "&amp;[Class Name]</f>
-        <v>php artisan make:model ResourceActionData</v>
+        <v>php artisan make:model ResourceActionList</v>
       </c>
       <c r="H26" s="8" t="str">
         <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
-        <v>protected $table = '__resource_action_data';</v>
+        <v>protected $table = '__resource_action_lists';</v>
       </c>
       <c r="I26" s="8" t="str">
         <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
-        <v>php artisan make:seed ResourceActionDataTableSeeder</v>
+        <v>php artisan make:seed ResourceActionListTableSeeder</v>
       </c>
       <c r="J26" s="8" t="str">
         <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
+        <v>ResourceActionListTableSeeder::class,</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B27" s="7" t="str">
+        <f>"__"&amp;[Name]</f>
+        <v>__resource_action_data</v>
+      </c>
+      <c r="C27" s="7" t="str">
+        <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
+        <v>resource_action_data</v>
+      </c>
+      <c r="D27" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>Milestone\Appframe\Model</v>
+      </c>
+      <c r="E27" s="8" t="str">
+        <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
+        <v>ResourceActionData</v>
+      </c>
+      <c r="F27" s="8" t="str">
+        <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
+        <v>php artisan make:migration create___resource_action_data_table --create=__resource_action_data</v>
+      </c>
+      <c r="G27" s="8" t="str">
+        <f>"php artisan make:model "&amp;[Class Name]</f>
+        <v>php artisan make:model ResourceActionData</v>
+      </c>
+      <c r="H27" s="8" t="str">
+        <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
+        <v>protected $table = '__resource_action_data';</v>
+      </c>
+      <c r="I27" s="8" t="str">
+        <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
+        <v>php artisan make:seed ResourceActionDataTableSeeder</v>
+      </c>
+      <c r="J27" s="8" t="str">
+        <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
         <v>ResourceActionDataTableSeeder::class,</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
-      <c r="A27" s="5" t="s">
+    <row r="28" spans="1:10">
+      <c r="A28" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="B27" s="8" t="str">
+      <c r="B28" s="8" t="str">
         <f>"__"&amp;[Name]</f>
         <v>__resource_roles</v>
       </c>
-      <c r="C27" s="8" t="str">
+      <c r="C28" s="8" t="str">
         <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
         <v>resource_role</v>
       </c>
-      <c r="D27" s="8" t="str">
+      <c r="D28" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Milestone\Appframe\Model</v>
       </c>
-      <c r="E27" s="8" t="str">
+      <c r="E28" s="8" t="str">
         <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
         <v>ResourceRole</v>
       </c>
-      <c r="F27" s="8" t="str">
+      <c r="F28" s="8" t="str">
         <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
         <v>php artisan make:migration create___resource_roles_table --create=__resource_roles</v>
       </c>
-      <c r="G27" s="8" t="str">
+      <c r="G28" s="8" t="str">
         <f>"php artisan make:model "&amp;[Class Name]</f>
         <v>php artisan make:model ResourceRole</v>
       </c>
-      <c r="H27" s="8" t="str">
+      <c r="H28" s="8" t="str">
         <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
         <v>protected $table = '__resource_roles';</v>
       </c>
-      <c r="I27" s="8" t="str">
+      <c r="I28" s="8" t="str">
         <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
         <v>php artisan make:seed ResourceRoleTableSeeder</v>
       </c>
-      <c r="J27" s="8" t="str">
+      <c r="J28" s="8" t="str">
         <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
         <v>ResourceRoleTableSeeder::class,</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
-      <c r="A28" s="2" t="s">
+    <row r="29" spans="1:10">
+      <c r="A29" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B28" s="9" t="str">
+      <c r="B29" s="9" t="str">
         <f>"__"&amp;[Name]</f>
         <v>__resource_form_fields</v>
       </c>
-      <c r="C28" s="9" t="str">
+      <c r="C29" s="9" t="str">
         <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
         <v>resource_form_field</v>
-      </c>
-      <c r="D28" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Milestone\Appframe\Model</v>
-      </c>
-      <c r="E28" s="8" t="str">
-        <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
-        <v>ResourceFormField</v>
-      </c>
-      <c r="F28" s="8" t="str">
-        <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
-        <v>php artisan make:migration create___resource_form_fields_table --create=__resource_form_fields</v>
-      </c>
-      <c r="G28" s="8" t="str">
-        <f>"php artisan make:model "&amp;[Class Name]</f>
-        <v>php artisan make:model ResourceFormField</v>
-      </c>
-      <c r="H28" s="8" t="str">
-        <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
-        <v>protected $table = '__resource_form_fields';</v>
-      </c>
-      <c r="I28" s="8" t="str">
-        <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
-        <v>php artisan make:seed ResourceFormFieldTableSeeder</v>
-      </c>
-      <c r="J28" s="8" t="str">
-        <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
-        <v>ResourceFormFieldTableSeeder::class,</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B29" s="9" t="str">
-        <f>"__"&amp;[Name]</f>
-        <v>__resource_form_field_attrs</v>
-      </c>
-      <c r="C29" s="9" t="str">
-        <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
-        <v>resource_form_field_attr</v>
       </c>
       <c r="D29" s="9" t="str">
         <f t="shared" si="0"/>
@@ -5795,40 +5820,40 @@
       </c>
       <c r="E29" s="8" t="str">
         <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
-        <v>ResourceFormFieldAttr</v>
+        <v>ResourceFormField</v>
       </c>
       <c r="F29" s="8" t="str">
         <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
-        <v>php artisan make:migration create___resource_form_field_attrs_table --create=__resource_form_field_attrs</v>
+        <v>php artisan make:migration create___resource_form_fields_table --create=__resource_form_fields</v>
       </c>
       <c r="G29" s="8" t="str">
         <f>"php artisan make:model "&amp;[Class Name]</f>
-        <v>php artisan make:model ResourceFormFieldAttr</v>
+        <v>php artisan make:model ResourceFormField</v>
       </c>
       <c r="H29" s="8" t="str">
         <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
-        <v>protected $table = '__resource_form_field_attrs';</v>
+        <v>protected $table = '__resource_form_fields';</v>
       </c>
       <c r="I29" s="8" t="str">
         <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
-        <v>php artisan make:seed ResourceFormFieldAttrTableSeeder</v>
+        <v>php artisan make:seed ResourceFormFieldTableSeeder</v>
       </c>
       <c r="J29" s="8" t="str">
         <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
-        <v>ResourceFormFieldAttrTableSeeder::class,</v>
+        <v>ResourceFormFieldTableSeeder::class,</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B30" s="9" t="str">
         <f>"__"&amp;[Name]</f>
-        <v>__resource_form_field_data</v>
+        <v>__resource_form_field_attrs</v>
       </c>
       <c r="C30" s="9" t="str">
         <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
-        <v>resource_form_field_data</v>
+        <v>resource_form_field_attr</v>
       </c>
       <c r="D30" s="9" t="str">
         <f t="shared" si="0"/>
@@ -5836,40 +5861,40 @@
       </c>
       <c r="E30" s="8" t="str">
         <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
-        <v>ResourceFormFieldData</v>
+        <v>ResourceFormFieldAttr</v>
       </c>
       <c r="F30" s="8" t="str">
         <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
-        <v>php artisan make:migration create___resource_form_field_data_table --create=__resource_form_field_data</v>
+        <v>php artisan make:migration create___resource_form_field_attrs_table --create=__resource_form_field_attrs</v>
       </c>
       <c r="G30" s="8" t="str">
         <f>"php artisan make:model "&amp;[Class Name]</f>
-        <v>php artisan make:model ResourceFormFieldData</v>
+        <v>php artisan make:model ResourceFormFieldAttr</v>
       </c>
       <c r="H30" s="8" t="str">
         <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
-        <v>protected $table = '__resource_form_field_data';</v>
+        <v>protected $table = '__resource_form_field_attrs';</v>
       </c>
       <c r="I30" s="8" t="str">
         <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
-        <v>php artisan make:seed ResourceFormFieldDataTableSeeder</v>
+        <v>php artisan make:seed ResourceFormFieldAttrTableSeeder</v>
       </c>
       <c r="J30" s="8" t="str">
         <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
-        <v>ResourceFormFieldDataTableSeeder::class,</v>
+        <v>ResourceFormFieldAttrTableSeeder::class,</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B31" s="9" t="str">
         <f>"__"&amp;[Name]</f>
-        <v>__resource_form_field_validations</v>
+        <v>__resource_form_field_data</v>
       </c>
       <c r="C31" s="9" t="str">
         <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
-        <v>resource_form_field_validation</v>
+        <v>resource_form_field_data</v>
       </c>
       <c r="D31" s="9" t="str">
         <f t="shared" si="0"/>
@@ -5877,122 +5902,122 @@
       </c>
       <c r="E31" s="8" t="str">
         <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
-        <v>ResourceFormFieldValidation</v>
+        <v>ResourceFormFieldData</v>
       </c>
       <c r="F31" s="8" t="str">
         <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
-        <v>php artisan make:migration create___resource_form_field_validations_table --create=__resource_form_field_validations</v>
+        <v>php artisan make:migration create___resource_form_field_data_table --create=__resource_form_field_data</v>
       </c>
       <c r="G31" s="8" t="str">
         <f>"php artisan make:model "&amp;[Class Name]</f>
-        <v>php artisan make:model ResourceFormFieldValidation</v>
+        <v>php artisan make:model ResourceFormFieldData</v>
       </c>
       <c r="H31" s="8" t="str">
         <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
-        <v>protected $table = '__resource_form_field_validations';</v>
+        <v>protected $table = '__resource_form_field_data';</v>
       </c>
       <c r="I31" s="8" t="str">
         <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
-        <v>php artisan make:seed ResourceFormFieldValidationTableSeeder</v>
+        <v>php artisan make:seed ResourceFormFieldDataTableSeeder</v>
       </c>
       <c r="J31" s="8" t="str">
         <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
-        <v>ResourceFormFieldValidationTableSeeder::class,</v>
+        <v>ResourceFormFieldDataTableSeeder::class,</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B32" s="9" t="str">
+        <f>"__"&amp;[Name]</f>
+        <v>__resource_form_field_validations</v>
+      </c>
+      <c r="C32" s="9" t="str">
+        <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
+        <v>resource_form_field_validation</v>
+      </c>
+      <c r="D32" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>Milestone\Appframe\Model</v>
+      </c>
+      <c r="E32" s="8" t="str">
+        <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
+        <v>ResourceFormFieldValidation</v>
+      </c>
+      <c r="F32" s="8" t="str">
+        <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
+        <v>php artisan make:migration create___resource_form_field_validations_table --create=__resource_form_field_validations</v>
+      </c>
+      <c r="G32" s="8" t="str">
+        <f>"php artisan make:model "&amp;[Class Name]</f>
+        <v>php artisan make:model ResourceFormFieldValidation</v>
+      </c>
+      <c r="H32" s="8" t="str">
+        <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
+        <v>protected $table = '__resource_form_field_validations';</v>
+      </c>
+      <c r="I32" s="8" t="str">
+        <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
+        <v>php artisan make:seed ResourceFormFieldValidationTableSeeder</v>
+      </c>
+      <c r="J32" s="8" t="str">
+        <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
+        <v>ResourceFormFieldValidationTableSeeder::class,</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="2" t="s">
         <v>453</v>
       </c>
-      <c r="B32" s="7" t="str">
+      <c r="B33" s="7" t="str">
         <f>"__"&amp;[Name]</f>
         <v>__resource_form_field_options</v>
       </c>
-      <c r="C32" s="7" t="str">
+      <c r="C33" s="7" t="str">
         <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
         <v>resource_form_field_option</v>
       </c>
-      <c r="D32" s="7" t="str">
+      <c r="D33" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Milestone\Appframe\Model</v>
       </c>
-      <c r="E32" s="8" t="str">
+      <c r="E33" s="8" t="str">
         <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
         <v>ResourceFormFieldOption</v>
       </c>
-      <c r="F32" s="8" t="str">
+      <c r="F33" s="8" t="str">
         <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
         <v>php artisan make:migration create___resource_form_field_options_table --create=__resource_form_field_options</v>
       </c>
-      <c r="G32" s="8" t="str">
+      <c r="G33" s="8" t="str">
         <f>"php artisan make:model "&amp;[Class Name]</f>
         <v>php artisan make:model ResourceFormFieldOption</v>
       </c>
-      <c r="H32" s="8" t="str">
+      <c r="H33" s="8" t="str">
         <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
         <v>protected $table = '__resource_form_field_options';</v>
       </c>
-      <c r="I32" s="8" t="str">
+      <c r="I33" s="8" t="str">
         <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
         <v>php artisan make:seed ResourceFormFieldOptionTableSeeder</v>
       </c>
-      <c r="J32" s="8" t="str">
+      <c r="J33" s="8" t="str">
         <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
         <v>ResourceFormFieldOptionTableSeeder::class,</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
-      <c r="A33" s="2" t="s">
+    <row r="34" spans="1:10">
+      <c r="A34" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="B33" s="7" t="str">
+      <c r="B34" s="7" t="str">
         <f>"__"&amp;[Name]</f>
         <v>__resource_form_layout</v>
       </c>
-      <c r="C33" s="7" t="str">
+      <c r="C34" s="7" t="str">
         <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
         <v>resource_form_layout</v>
-      </c>
-      <c r="D33" s="7" t="str">
-        <f>"Milestone\Appframe\Model"</f>
-        <v>Milestone\Appframe\Model</v>
-      </c>
-      <c r="E33" s="8" t="str">
-        <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
-        <v>ResourceFormLayout</v>
-      </c>
-      <c r="F33" s="8" t="str">
-        <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
-        <v>php artisan make:migration create___resource_form_layout_table --create=__resource_form_layout</v>
-      </c>
-      <c r="G33" s="8" t="str">
-        <f>"php artisan make:model "&amp;[Class Name]</f>
-        <v>php artisan make:model ResourceFormLayout</v>
-      </c>
-      <c r="H33" s="8" t="str">
-        <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
-        <v>protected $table = '__resource_form_layout';</v>
-      </c>
-      <c r="I33" s="8" t="str">
-        <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
-        <v>php artisan make:seed ResourceFormLayoutTableSeeder</v>
-      </c>
-      <c r="J33" s="8" t="str">
-        <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
-        <v>ResourceFormLayoutTableSeeder::class,</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10">
-      <c r="A34" s="2" t="s">
-        <v>647</v>
-      </c>
-      <c r="B34" s="7" t="str">
-        <f>"__"&amp;[Name]</f>
-        <v>__resource_form_collection</v>
-      </c>
-      <c r="C34" s="7" t="str">
-        <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
-        <v>resource_form_collection</v>
       </c>
       <c r="D34" s="7" t="str">
         <f>"Milestone\Appframe\Model"</f>
@@ -6000,81 +6025,81 @@
       </c>
       <c r="E34" s="8" t="str">
         <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
-        <v>ResourceFormCollection</v>
+        <v>ResourceFormLayout</v>
       </c>
       <c r="F34" s="8" t="str">
         <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
-        <v>php artisan make:migration create___resource_form_collection_table --create=__resource_form_collection</v>
+        <v>php artisan make:migration create___resource_form_layout_table --create=__resource_form_layout</v>
       </c>
       <c r="G34" s="8" t="str">
         <f>"php artisan make:model "&amp;[Class Name]</f>
-        <v>php artisan make:model ResourceFormCollection</v>
+        <v>php artisan make:model ResourceFormLayout</v>
       </c>
       <c r="H34" s="8" t="str">
         <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
-        <v>protected $table = '__resource_form_collection';</v>
+        <v>protected $table = '__resource_form_layout';</v>
       </c>
       <c r="I34" s="8" t="str">
         <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
-        <v>php artisan make:seed ResourceFormCollectionTableSeeder</v>
+        <v>php artisan make:seed ResourceFormLayoutTableSeeder</v>
       </c>
       <c r="J34" s="8" t="str">
         <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
-        <v>ResourceFormCollectionTableSeeder::class,</v>
+        <v>ResourceFormLayoutTableSeeder::class,</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="B35" s="7" t="str">
+        <f>"__"&amp;[Name]</f>
+        <v>__resource_form_collection</v>
+      </c>
+      <c r="C35" s="7" t="str">
+        <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
+        <v>resource_form_collection</v>
+      </c>
+      <c r="D35" s="7" t="str">
+        <f>"Milestone\Appframe\Model"</f>
+        <v>Milestone\Appframe\Model</v>
+      </c>
+      <c r="E35" s="8" t="str">
+        <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
+        <v>ResourceFormCollection</v>
+      </c>
+      <c r="F35" s="8" t="str">
+        <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
+        <v>php artisan make:migration create___resource_form_collection_table --create=__resource_form_collection</v>
+      </c>
+      <c r="G35" s="8" t="str">
+        <f>"php artisan make:model "&amp;[Class Name]</f>
+        <v>php artisan make:model ResourceFormCollection</v>
+      </c>
+      <c r="H35" s="8" t="str">
+        <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
+        <v>protected $table = '__resource_form_collection';</v>
+      </c>
+      <c r="I35" s="8" t="str">
+        <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
+        <v>php artisan make:seed ResourceFormCollectionTableSeeder</v>
+      </c>
+      <c r="J35" s="8" t="str">
+        <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
+        <v>ResourceFormCollectionTableSeeder::class,</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B35" s="9" t="str">
+      <c r="B36" s="9" t="str">
         <f>"__"&amp;[Name]</f>
         <v>__organisation</v>
       </c>
-      <c r="C35" s="9" t="str">
+      <c r="C36" s="9" t="str">
         <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
         <v>organisation</v>
-      </c>
-      <c r="D35" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Milestone\Appframe\Model</v>
-      </c>
-      <c r="E35" s="9" t="str">
-        <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
-        <v>Organisation</v>
-      </c>
-      <c r="F35" s="9" t="str">
-        <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
-        <v>php artisan make:migration create___organisation_table --create=__organisation</v>
-      </c>
-      <c r="G35" s="9" t="str">
-        <f>"php artisan make:model "&amp;[Class Name]</f>
-        <v>php artisan make:model Organisation</v>
-      </c>
-      <c r="H35" s="9" t="str">
-        <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
-        <v>protected $table = '__organisation';</v>
-      </c>
-      <c r="I35" s="9" t="str">
-        <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
-        <v>php artisan make:seed OrganisationTableSeeder</v>
-      </c>
-      <c r="J35" s="9" t="str">
-        <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
-        <v>OrganisationTableSeeder::class,</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10">
-      <c r="A36" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="B36" s="9" t="str">
-        <f>"__"&amp;[Name]</f>
-        <v>__organisation_contacts</v>
-      </c>
-      <c r="C36" s="9" t="str">
-        <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
-        <v>organisation_contact</v>
       </c>
       <c r="D36" s="9" t="str">
         <f t="shared" si="0"/>
@@ -6082,25 +6107,66 @@
       </c>
       <c r="E36" s="9" t="str">
         <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
-        <v>OrganisationContact</v>
+        <v>Organisation</v>
       </c>
       <c r="F36" s="9" t="str">
         <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
-        <v>php artisan make:migration create___organisation_contacts_table --create=__organisation_contacts</v>
+        <v>php artisan make:migration create___organisation_table --create=__organisation</v>
       </c>
       <c r="G36" s="9" t="str">
         <f>"php artisan make:model "&amp;[Class Name]</f>
-        <v>php artisan make:model OrganisationContact</v>
+        <v>php artisan make:model Organisation</v>
       </c>
       <c r="H36" s="9" t="str">
         <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
-        <v>protected $table = '__organisation_contacts';</v>
+        <v>protected $table = '__organisation';</v>
       </c>
       <c r="I36" s="9" t="str">
         <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
+        <v>php artisan make:seed OrganisationTableSeeder</v>
+      </c>
+      <c r="J36" s="9" t="str">
+        <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
+        <v>OrganisationTableSeeder::class,</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B37" s="9" t="str">
+        <f>"__"&amp;[Name]</f>
+        <v>__organisation_contacts</v>
+      </c>
+      <c r="C37" s="9" t="str">
+        <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
+        <v>organisation_contact</v>
+      </c>
+      <c r="D37" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>Milestone\Appframe\Model</v>
+      </c>
+      <c r="E37" s="9" t="str">
+        <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
+        <v>OrganisationContact</v>
+      </c>
+      <c r="F37" s="9" t="str">
+        <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
+        <v>php artisan make:migration create___organisation_contacts_table --create=__organisation_contacts</v>
+      </c>
+      <c r="G37" s="9" t="str">
+        <f>"php artisan make:model "&amp;[Class Name]</f>
+        <v>php artisan make:model OrganisationContact</v>
+      </c>
+      <c r="H37" s="9" t="str">
+        <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
+        <v>protected $table = '__organisation_contacts';</v>
+      </c>
+      <c r="I37" s="9" t="str">
+        <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
         <v>php artisan make:seed OrganisationContactTableSeeder</v>
       </c>
-      <c r="J36" s="9" t="str">
+      <c r="J37" s="9" t="str">
         <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
         <v>OrganisationContactTableSeeder::class,</v>
       </c>
@@ -7688,8 +7754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I135"/>
   <sheetViews>
-    <sheetView topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="A135" sqref="A135"/>
+    <sheetView topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="A136" sqref="A136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="15"/>
@@ -10658,10 +10724,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K310"/>
+  <dimension ref="A1:K323"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K301" sqref="K301:K310"/>
+    <sheetView topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="A324" sqref="A324"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="15"/>
@@ -17307,7 +17373,7 @@
         <v>$table-&gt;foreign('form_field')-&gt;references('id')-&gt;on('__resource_form_fields')-&gt;onUpdate('cascade')-&gt;onDelete('cascade');</v>
       </c>
     </row>
-    <row r="152" spans="1:11" hidden="1">
+    <row r="152" spans="1:11">
       <c r="A152" s="4" t="s">
         <v>104</v>
       </c>
@@ -17351,7 +17417,7 @@
         <v>$table-&gt;increments('id');</v>
       </c>
     </row>
-    <row r="153" spans="1:11" hidden="1">
+    <row r="153" spans="1:11">
       <c r="A153" s="4" t="s">
         <v>104</v>
       </c>
@@ -17395,7 +17461,7 @@
         <v>$table-&gt;unsignedInteger('form_field')-&gt;index();</v>
       </c>
     </row>
-    <row r="154" spans="1:11" hidden="1">
+    <row r="154" spans="1:11">
       <c r="A154" s="4" t="s">
         <v>104</v>
       </c>
@@ -17439,7 +17505,7 @@
         <v>$table-&gt;unsignedInteger('relation')-&gt;index()-&gt;nullable();</v>
       </c>
     </row>
-    <row r="155" spans="1:11" hidden="1">
+    <row r="155" spans="1:11">
       <c r="A155" s="4" t="s">
         <v>104</v>
       </c>
@@ -17483,7 +17549,7 @@
         <v>$table-&gt;unsignedInteger('nest_relation1')-&gt;index()-&gt;nullable();</v>
       </c>
     </row>
-    <row r="156" spans="1:11" hidden="1">
+    <row r="156" spans="1:11">
       <c r="A156" s="4" t="s">
         <v>104</v>
       </c>
@@ -17527,7 +17593,7 @@
         <v>$table-&gt;unsignedInteger('nest_relation2')-&gt;index()-&gt;nullable();</v>
       </c>
     </row>
-    <row r="157" spans="1:11" hidden="1">
+    <row r="157" spans="1:11">
       <c r="A157" s="4" t="s">
         <v>104</v>
       </c>
@@ -17571,7 +17637,7 @@
         <v>$table-&gt;unsignedInteger('nest_relation3')-&gt;index()-&gt;nullable();</v>
       </c>
     </row>
-    <row r="158" spans="1:11" hidden="1">
+    <row r="158" spans="1:11">
       <c r="A158" s="4" t="s">
         <v>104</v>
       </c>
@@ -17615,7 +17681,7 @@
         <v>$table-&gt;string('attribute', 64)-&gt;nullable();</v>
       </c>
     </row>
-    <row r="159" spans="1:11" hidden="1">
+    <row r="159" spans="1:11">
       <c r="A159" s="4" t="s">
         <v>104</v>
       </c>
@@ -17659,7 +17725,7 @@
         <v>$table-&gt;timestamps();</v>
       </c>
     </row>
-    <row r="160" spans="1:11" hidden="1">
+    <row r="160" spans="1:11">
       <c r="A160" s="4" t="s">
         <v>104</v>
       </c>
@@ -17703,7 +17769,7 @@
         <v>$table-&gt;foreign('form_field')-&gt;references('id')-&gt;on('__resource_form_fields')-&gt;onUpdate('cascade')-&gt;onDelete('cascade');</v>
       </c>
     </row>
-    <row r="161" spans="1:11" hidden="1">
+    <row r="161" spans="1:11">
       <c r="A161" s="4" t="s">
         <v>104</v>
       </c>
@@ -17747,7 +17813,7 @@
         <v>$table-&gt;foreign('relation')-&gt;references('id')-&gt;on('__resource_relations')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
       </c>
     </row>
-    <row r="162" spans="1:11" hidden="1">
+    <row r="162" spans="1:11">
       <c r="A162" s="4" t="s">
         <v>104</v>
       </c>
@@ -17791,7 +17857,7 @@
         <v>$table-&gt;foreign('nest_relation1')-&gt;references('id')-&gt;on('__resource_relations')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
       </c>
     </row>
-    <row r="163" spans="1:11" hidden="1">
+    <row r="163" spans="1:11">
       <c r="A163" s="4" t="s">
         <v>104</v>
       </c>
@@ -17835,7 +17901,7 @@
         <v>$table-&gt;foreign('nest_relation2')-&gt;references('id')-&gt;on('__resource_relations')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
       </c>
     </row>
-    <row r="164" spans="1:11" hidden="1">
+    <row r="164" spans="1:11">
       <c r="A164" s="4" t="s">
         <v>104</v>
       </c>
@@ -23863,7 +23929,7 @@
         <v>$table-&gt;foreign('relation')-&gt;references('id')-&gt;on('__resource_relations')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
       </c>
     </row>
-    <row r="301" spans="1:11">
+    <row r="301" spans="1:11" hidden="1">
       <c r="A301" s="4" t="s">
         <v>647</v>
       </c>
@@ -23907,7 +23973,7 @@
         <v>$table-&gt;increments('id');</v>
       </c>
     </row>
-    <row r="302" spans="1:11">
+    <row r="302" spans="1:11" hidden="1">
       <c r="A302" s="4" t="s">
         <v>647</v>
       </c>
@@ -23951,7 +24017,7 @@
         <v>$table-&gt;unsignedInteger('resource_form')-&gt;index();</v>
       </c>
     </row>
-    <row r="303" spans="1:11">
+    <row r="303" spans="1:11" hidden="1">
       <c r="A303" s="4" t="s">
         <v>647</v>
       </c>
@@ -23995,7 +24061,7 @@
         <v>$table-&gt;unsignedInteger('collection_form')-&gt;index();</v>
       </c>
     </row>
-    <row r="304" spans="1:11">
+    <row r="304" spans="1:11" hidden="1">
       <c r="A304" s="4" t="s">
         <v>647</v>
       </c>
@@ -24039,7 +24105,7 @@
         <v>$table-&gt;unsignedInteger('relation')-&gt;index()-&gt;nullable();</v>
       </c>
     </row>
-    <row r="305" spans="1:11" s="26" customFormat="1">
+    <row r="305" spans="1:11" s="26" customFormat="1" hidden="1">
       <c r="A305" s="4" t="s">
         <v>647</v>
       </c>
@@ -24083,7 +24149,7 @@
         <v>$table-&gt;unsignedInteger('foreign_field')-&gt;index()-&gt;nullable();</v>
       </c>
     </row>
-    <row r="306" spans="1:11">
+    <row r="306" spans="1:11" hidden="1">
       <c r="A306" s="4" t="s">
         <v>647</v>
       </c>
@@ -24127,7 +24193,7 @@
         <v>$table-&gt;timestamps();</v>
       </c>
     </row>
-    <row r="307" spans="1:11">
+    <row r="307" spans="1:11" hidden="1">
       <c r="A307" s="4" t="s">
         <v>647</v>
       </c>
@@ -24171,7 +24237,7 @@
         <v>$table-&gt;foreign('resource_form')-&gt;references('id')-&gt;on('__resource_forms')-&gt;onUpdate('cascade')-&gt;onDelete('cascade');</v>
       </c>
     </row>
-    <row r="308" spans="1:11">
+    <row r="308" spans="1:11" hidden="1">
       <c r="A308" s="4" t="s">
         <v>647</v>
       </c>
@@ -24215,7 +24281,7 @@
         <v>$table-&gt;foreign('collection_form')-&gt;references('id')-&gt;on('__resource_forms')-&gt;onUpdate('cascade')-&gt;onDelete('cascade');</v>
       </c>
     </row>
-    <row r="309" spans="1:11">
+    <row r="309" spans="1:11" hidden="1">
       <c r="A309" s="4" t="s">
         <v>647</v>
       </c>
@@ -24259,7 +24325,7 @@
         <v>$table-&gt;foreign('relation')-&gt;references('id')-&gt;on('__resource_relations')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
       </c>
     </row>
-    <row r="310" spans="1:11">
+    <row r="310" spans="1:11" hidden="1">
       <c r="A310" s="4" t="s">
         <v>647</v>
       </c>
@@ -24303,13 +24369,585 @@
         <v>$table-&gt;foreign('foreign_field')-&gt;references('id')-&gt;on('__resource_form_fields')-&gt;onUpdate('cascade')-&gt;onDelete('cascade');</v>
       </c>
     </row>
+    <row r="311" spans="1:11">
+      <c r="A311" s="4" t="s">
+        <v>671</v>
+      </c>
+      <c r="B311" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C311" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>increments(</v>
+      </c>
+      <c r="D311" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'id'</v>
+      </c>
+      <c r="E311" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>)</v>
+      </c>
+      <c r="F311" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v/>
+      </c>
+      <c r="G311" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v/>
+      </c>
+      <c r="H311" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v/>
+      </c>
+      <c r="I311" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v/>
+      </c>
+      <c r="J311" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K311" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;increments('id');</v>
+      </c>
+    </row>
+    <row r="312" spans="1:11">
+      <c r="A312" s="4" t="s">
+        <v>671</v>
+      </c>
+      <c r="B312" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C312" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>unsignedInteger(</v>
+      </c>
+      <c r="D312" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'resource_list'</v>
+      </c>
+      <c r="E312" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>)</v>
+      </c>
+      <c r="F312" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>-&gt;index()</v>
+      </c>
+      <c r="G312" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v/>
+      </c>
+      <c r="H312" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v/>
+      </c>
+      <c r="I312" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v/>
+      </c>
+      <c r="J312" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K312" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;unsignedInteger('resource_list')-&gt;index();</v>
+      </c>
+    </row>
+    <row r="313" spans="1:11">
+      <c r="A313" s="4" t="s">
+        <v>671</v>
+      </c>
+      <c r="B313" s="4" t="s">
+        <v>560</v>
+      </c>
+      <c r="C313" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>string(</v>
+      </c>
+      <c r="D313" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'field'</v>
+      </c>
+      <c r="E313" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>, 64)</v>
+      </c>
+      <c r="F313" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>-&gt;nullable()</v>
+      </c>
+      <c r="G313" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v/>
+      </c>
+      <c r="H313" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v/>
+      </c>
+      <c r="I313" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v/>
+      </c>
+      <c r="J313" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K313" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;string('field', 64)-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="314" spans="1:11">
+      <c r="A314" s="4" t="s">
+        <v>671</v>
+      </c>
+      <c r="B314" s="4" t="s">
+        <v>572</v>
+      </c>
+      <c r="C314" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>unsignedInteger(</v>
+      </c>
+      <c r="D314" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'relation'</v>
+      </c>
+      <c r="E314" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>)</v>
+      </c>
+      <c r="F314" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>-&gt;index()</v>
+      </c>
+      <c r="G314" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v>-&gt;nullable()</v>
+      </c>
+      <c r="H314" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v/>
+      </c>
+      <c r="I314" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v/>
+      </c>
+      <c r="J314" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K314" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;unsignedInteger('relation')-&gt;index()-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="315" spans="1:11">
+      <c r="A315" s="4" t="s">
+        <v>671</v>
+      </c>
+      <c r="B315" s="4" t="s">
+        <v>574</v>
+      </c>
+      <c r="C315" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>unsignedInteger(</v>
+      </c>
+      <c r="D315" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'nest_relation1'</v>
+      </c>
+      <c r="E315" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>)</v>
+      </c>
+      <c r="F315" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>-&gt;index()</v>
+      </c>
+      <c r="G315" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v>-&gt;nullable()</v>
+      </c>
+      <c r="H315" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v/>
+      </c>
+      <c r="I315" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v/>
+      </c>
+      <c r="J315" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K315" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;unsignedInteger('nest_relation1')-&gt;index()-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="316" spans="1:11">
+      <c r="A316" s="4" t="s">
+        <v>671</v>
+      </c>
+      <c r="B316" s="4" t="s">
+        <v>575</v>
+      </c>
+      <c r="C316" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>unsignedInteger(</v>
+      </c>
+      <c r="D316" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'nest_relation2'</v>
+      </c>
+      <c r="E316" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>)</v>
+      </c>
+      <c r="F316" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>-&gt;index()</v>
+      </c>
+      <c r="G316" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v>-&gt;nullable()</v>
+      </c>
+      <c r="H316" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v/>
+      </c>
+      <c r="I316" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v/>
+      </c>
+      <c r="J316" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K316" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;unsignedInteger('nest_relation2')-&gt;index()-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="317" spans="1:11">
+      <c r="A317" s="4" t="s">
+        <v>671</v>
+      </c>
+      <c r="B317" s="4" t="s">
+        <v>576</v>
+      </c>
+      <c r="C317" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>unsignedInteger(</v>
+      </c>
+      <c r="D317" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'nest_relation3'</v>
+      </c>
+      <c r="E317" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>)</v>
+      </c>
+      <c r="F317" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>-&gt;index()</v>
+      </c>
+      <c r="G317" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v>-&gt;nullable()</v>
+      </c>
+      <c r="H317" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v/>
+      </c>
+      <c r="I317" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v/>
+      </c>
+      <c r="J317" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K317" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;unsignedInteger('nest_relation3')-&gt;index()-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="318" spans="1:11">
+      <c r="A318" s="4" t="s">
+        <v>671</v>
+      </c>
+      <c r="B318" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C318" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>timestamps(</v>
+      </c>
+      <c r="D318" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v/>
+      </c>
+      <c r="E318" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>)</v>
+      </c>
+      <c r="F318" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v/>
+      </c>
+      <c r="G318" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v/>
+      </c>
+      <c r="H318" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v/>
+      </c>
+      <c r="I318" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v/>
+      </c>
+      <c r="J318" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K318" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;timestamps();</v>
+      </c>
+    </row>
+    <row r="319" spans="1:11">
+      <c r="A319" s="4" t="s">
+        <v>671</v>
+      </c>
+      <c r="B319" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C319" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>foreign(</v>
+      </c>
+      <c r="D319" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'resource_list'</v>
+      </c>
+      <c r="E319" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>)</v>
+      </c>
+      <c r="F319" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>-&gt;references('id')</v>
+      </c>
+      <c r="G319" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v>-&gt;on('__resource_lists')</v>
+      </c>
+      <c r="H319" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v>-&gt;onUpdate('cascade')</v>
+      </c>
+      <c r="I319" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v>-&gt;onDelete('cascade')</v>
+      </c>
+      <c r="J319" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K319" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;foreign('resource_list')-&gt;references('id')-&gt;on('__resource_lists')-&gt;onUpdate('cascade')-&gt;onDelete('cascade');</v>
+      </c>
+    </row>
+    <row r="320" spans="1:11">
+      <c r="A320" s="4" t="s">
+        <v>671</v>
+      </c>
+      <c r="B320" s="4" t="s">
+        <v>573</v>
+      </c>
+      <c r="C320" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>foreign(</v>
+      </c>
+      <c r="D320" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'relation'</v>
+      </c>
+      <c r="E320" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>)</v>
+      </c>
+      <c r="F320" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>-&gt;references('id')</v>
+      </c>
+      <c r="G320" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v>-&gt;on('__resource_relations')</v>
+      </c>
+      <c r="H320" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v>-&gt;onUpdate('cascade')</v>
+      </c>
+      <c r="I320" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v>-&gt;onDelete('set null')</v>
+      </c>
+      <c r="J320" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K320" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;foreign('relation')-&gt;references('id')-&gt;on('__resource_relations')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
+      </c>
+    </row>
+    <row r="321" spans="1:11">
+      <c r="A321" s="4" t="s">
+        <v>671</v>
+      </c>
+      <c r="B321" s="4" t="s">
+        <v>579</v>
+      </c>
+      <c r="C321" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>foreign(</v>
+      </c>
+      <c r="D321" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'nest_relation1'</v>
+      </c>
+      <c r="E321" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>)</v>
+      </c>
+      <c r="F321" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>-&gt;references('id')</v>
+      </c>
+      <c r="G321" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v>-&gt;on('__resource_relations')</v>
+      </c>
+      <c r="H321" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v>-&gt;onUpdate('cascade')</v>
+      </c>
+      <c r="I321" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v>-&gt;onDelete('set null')</v>
+      </c>
+      <c r="J321" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K321" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;foreign('nest_relation1')-&gt;references('id')-&gt;on('__resource_relations')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
+      </c>
+    </row>
+    <row r="322" spans="1:11">
+      <c r="A322" s="4" t="s">
+        <v>671</v>
+      </c>
+      <c r="B322" s="4" t="s">
+        <v>580</v>
+      </c>
+      <c r="C322" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>foreign(</v>
+      </c>
+      <c r="D322" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'nest_relation2'</v>
+      </c>
+      <c r="E322" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>)</v>
+      </c>
+      <c r="F322" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>-&gt;references('id')</v>
+      </c>
+      <c r="G322" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v>-&gt;on('__resource_relations')</v>
+      </c>
+      <c r="H322" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v>-&gt;onUpdate('cascade')</v>
+      </c>
+      <c r="I322" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v>-&gt;onDelete('set null')</v>
+      </c>
+      <c r="J322" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K322" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;foreign('nest_relation2')-&gt;references('id')-&gt;on('__resource_relations')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
+      </c>
+    </row>
+    <row r="323" spans="1:11">
+      <c r="A323" s="4" t="s">
+        <v>671</v>
+      </c>
+      <c r="B323" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="C323" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>foreign(</v>
+      </c>
+      <c r="D323" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'nest_relation3'</v>
+      </c>
+      <c r="E323" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>)</v>
+      </c>
+      <c r="F323" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>-&gt;references('id')</v>
+      </c>
+      <c r="G323" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v>-&gt;on('__resource_relations')</v>
+      </c>
+      <c r="H323" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v>-&gt;onUpdate('cascade')</v>
+      </c>
+      <c r="I323" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v>-&gt;onDelete('set null')</v>
+      </c>
+      <c r="J323" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K323" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;foreign('nest_relation3')-&gt;references('id')-&gt;on('__resource_relations')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B310">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B323">
       <formula1>AvailableFields</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A310">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A323">
       <formula1>TableNames</formula1>
     </dataValidation>
   </dataValidations>
@@ -24323,10 +24961,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R304"/>
+  <dimension ref="A1:R307"/>
   <sheetViews>
-    <sheetView topLeftCell="B29" workbookViewId="0">
-      <selection activeCell="D282" sqref="D282"/>
+    <sheetView topLeftCell="B291" workbookViewId="0">
+      <selection activeCell="C307" sqref="C307"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -35383,6 +36021,126 @@
       <c r="Q304" s="43"/>
       <c r="R304" s="43"/>
     </row>
+    <row r="305" spans="1:18">
+      <c r="A305" s="22" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resource List Search-0</v>
+      </c>
+      <c r="B305" s="40" t="s">
+        <v>672</v>
+      </c>
+      <c r="C305" s="22">
+        <f>COUNTIF($B$1:$B304,[Table Name])</f>
+        <v>0</v>
+      </c>
+      <c r="D305" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="E305" s="40" t="s">
+        <v>560</v>
+      </c>
+      <c r="F305" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="G305" s="40" t="s">
+        <v>574</v>
+      </c>
+      <c r="H305" s="40" t="s">
+        <v>575</v>
+      </c>
+      <c r="I305" s="40" t="s">
+        <v>576</v>
+      </c>
+      <c r="J305" s="40"/>
+      <c r="K305" s="40"/>
+      <c r="L305" s="40"/>
+      <c r="M305" s="40"/>
+      <c r="N305" s="40"/>
+      <c r="O305" s="40"/>
+      <c r="P305" s="40"/>
+      <c r="Q305" s="40"/>
+      <c r="R305" s="40"/>
+    </row>
+    <row r="306" spans="1:18">
+      <c r="A306" s="22" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resources-31</v>
+      </c>
+      <c r="B306" s="40" t="s">
+        <v>220</v>
+      </c>
+      <c r="C306" s="22">
+        <f>COUNTIF($B$1:$B305,[Table Name])</f>
+        <v>31</v>
+      </c>
+      <c r="D306" s="40" t="s">
+        <v>673</v>
+      </c>
+      <c r="E306" s="40" t="s">
+        <v>674</v>
+      </c>
+      <c r="F306" s="40" t="s">
+        <v>675</v>
+      </c>
+      <c r="G306" s="40" t="s">
+        <v>558</v>
+      </c>
+      <c r="H306" s="40" t="s">
+        <v>676</v>
+      </c>
+      <c r="I306" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="J306" s="40"/>
+      <c r="K306" s="40"/>
+      <c r="L306" s="40"/>
+      <c r="M306" s="40"/>
+      <c r="N306" s="40"/>
+      <c r="O306" s="40"/>
+      <c r="P306" s="40"/>
+      <c r="Q306" s="40"/>
+      <c r="R306" s="40"/>
+    </row>
+    <row r="307" spans="1:18">
+      <c r="A307" s="22" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resource Relations-44</v>
+      </c>
+      <c r="B307" s="40" t="s">
+        <v>441</v>
+      </c>
+      <c r="C307" s="22">
+        <f>COUNTIF($B$1:$B306,[Table Name])</f>
+        <v>44</v>
+      </c>
+      <c r="D307" s="40">
+        <v>19</v>
+      </c>
+      <c r="E307" s="40" t="s">
+        <v>675</v>
+      </c>
+      <c r="F307" s="40" t="s">
+        <v>678</v>
+      </c>
+      <c r="G307" s="40" t="s">
+        <v>677</v>
+      </c>
+      <c r="H307" s="40" t="s">
+        <v>310</v>
+      </c>
+      <c r="I307" s="40">
+        <v>31</v>
+      </c>
+      <c r="J307" s="40"/>
+      <c r="K307" s="40"/>
+      <c r="L307" s="40"/>
+      <c r="M307" s="40"/>
+      <c r="N307" s="40"/>
+      <c r="O307" s="40"/>
+      <c r="P307" s="40"/>
+      <c r="Q307" s="40"/>
+      <c r="R307" s="40"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
@@ -35394,10 +36152,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -36008,12 +36766,32 @@
         <v>truncate</v>
       </c>
     </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="4" t="s">
+        <v>672</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>671</v>
+      </c>
+      <c r="C31" s="4" t="str">
+        <f>VLOOKUP([FW Table Name],Tables[],4,0)</f>
+        <v>Milestone\Appframe\Model</v>
+      </c>
+      <c r="D31" s="4" t="str">
+        <f>VLOOKUP([FW Table Name],Tables[],5,0)</f>
+        <v>ResourceListSearch</v>
+      </c>
+      <c r="E31" s="7" t="str">
+        <f>"truncate"</f>
+        <v>truncate</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E30">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E31">
       <formula1>"truncate,query"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B30">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B31">
       <formula1>TableNames</formula1>
     </dataValidation>
   </dataValidations>
@@ -36027,10 +36805,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31:G31"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32:G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -36913,9 +37691,37 @@
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
     </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="20">
+        <f>IFERROR($A31+1,1)</f>
+        <v>31</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>673</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>674</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>675</v>
+      </c>
+      <c r="E32" s="7" t="str">
+        <f>"Milestone\Appframe\Model"</f>
+        <v>Milestone\Appframe\Model</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>676</v>
+      </c>
+      <c r="G32" s="21" t="str">
+        <f>"id"</f>
+        <v>id</v>
+      </c>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F32">
       <formula1>ActualTableNames</formula1>
     </dataValidation>
   </dataValidations>
@@ -36928,10 +37734,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23:I23"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45:I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -38355,15 +39161,48 @@
         <v>12</v>
       </c>
     </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="20">
+        <f>IFERROR($A44+1,1)</f>
+        <v>44</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>673</v>
+      </c>
+      <c r="D45" s="7">
+        <f>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</f>
+        <v>19</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>675</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>678</v>
+      </c>
+      <c r="G45" s="22" t="s">
+        <v>677</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="I45" s="41">
+        <f>VLOOKUP([Relate Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</f>
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C44">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C45">
       <formula1>Resources</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -38372,8 +39211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:R40"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -38383,14 +39222,14 @@
   <sheetData>
     <row r="1" spans="1:20" s="38" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="48" t="s">
-        <v>227</v>
+        <v>441</v>
       </c>
       <c r="B1" s="48"/>
       <c r="C1" s="48"/>
       <c r="D1" s="48"/>
       <c r="E1" s="49" t="str">
         <f>"\"&amp;VLOOKUP($A$1,SeedMap[],3,0)&amp;"\"&amp;VLOOKUP($A$1,SeedMap[],4,0)&amp;"::"&amp;VLOOKUP($A$1,SeedMap[],5,0)&amp;"()"</f>
-        <v>\Milestone\Appframe\Model\ResourceRole::truncate()</v>
+        <v>\Milestone\Appframe\Model\ResourceRelation::truncate()</v>
       </c>
       <c r="F1" s="49"/>
       <c r="G1" s="49"/>
@@ -38538,23 +39377,23 @@
       </c>
       <c r="D5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],D$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],D$4+$B$4,0))</f>
-        <v>role</v>
+        <v>name</v>
       </c>
       <c r="E5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0))</f>
-        <v>actions_availability</v>
+        <v>description</v>
       </c>
       <c r="F5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0))</f>
-        <v>actions</v>
+        <v>method</v>
       </c>
       <c r="G5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0))</f>
-        <v/>
+        <v>type</v>
       </c>
       <c r="H5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],H$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],H$4+$B$4,0))</f>
-        <v/>
+        <v>relate_resource</v>
       </c>
       <c r="I5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],I$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],I$4+$B$4,0))</f>
@@ -38648,7 +39487,7 @@
       <c r="A8" s="32"/>
       <c r="B8" s="47" t="str">
         <f>$E$1</f>
-        <v>\Milestone\Appframe\Model\ResourceRole::truncate()</v>
+        <v>\Milestone\Appframe\Model\ResourceRelation::truncate()</v>
       </c>
       <c r="C8" s="47"/>
       <c r="D8" s="47"/>
@@ -38681,23 +39520,23 @@
       </c>
       <c r="D9" s="33" t="str">
         <f t="shared" ref="D9:Q24" ca="1" si="0">IF(AND($B9=$S$4,D$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),D$4+$B$4,0)="","","'"&amp;D$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),D$4+$B$4,0)&amp;"', "),"")</f>
-        <v xml:space="preserve">'role' =&gt; '1', </v>
+        <v xml:space="preserve">'name' =&gt; 'User Groups', </v>
       </c>
       <c r="E9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'actions_availability' =&gt; 'Only', </v>
+        <v xml:space="preserve">'description' =&gt; 'Which groups this user belongs to', </v>
       </c>
       <c r="F9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'actions' =&gt; '2,3,5,6,7,8,9,10', </v>
+        <v xml:space="preserve">'method' =&gt; 'Groups', </v>
       </c>
       <c r="G9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
       </c>
       <c r="H9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '2', </v>
       </c>
       <c r="I9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -38750,27 +39589,27 @@
       </c>
       <c r="C10" s="33" t="str">
         <f ca="1">IF(AND($B10=$S$4,C$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A10,INDIRECT($E$2),C$4+$B$4,0)="","","'"&amp;C$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A10,INDIRECT($E$2),C$4+$B$4,0)&amp;"', "),"")</f>
-        <v xml:space="preserve">'resource' =&gt; '1', </v>
+        <v xml:space="preserve">'resource' =&gt; '2', </v>
       </c>
       <c r="D10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'role' =&gt; '3', </v>
+        <v xml:space="preserve">'name' =&gt; 'Group Users', </v>
       </c>
       <c r="E10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'List of users belongs to this group', </v>
       </c>
       <c r="F10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Users', </v>
       </c>
       <c r="G10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
       </c>
       <c r="H10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '1', </v>
       </c>
       <c r="I10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -38827,23 +39666,23 @@
       </c>
       <c r="D11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'role' =&gt; '3', </v>
+        <v xml:space="preserve">'name' =&gt; 'Group Roles', </v>
       </c>
       <c r="E11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Roles assigneed to this group', </v>
       </c>
       <c r="F11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Roles', </v>
       </c>
       <c r="G11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
       </c>
       <c r="H11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '3', </v>
       </c>
       <c r="I11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -38900,23 +39739,23 @@
       </c>
       <c r="D12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'role' =&gt; '3', </v>
+        <v xml:space="preserve">'name' =&gt; 'Role Groups', </v>
       </c>
       <c r="E12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Details of groups this role assigned to', </v>
       </c>
       <c r="F12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Groups', </v>
       </c>
       <c r="G12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
       </c>
       <c r="H12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '2', </v>
       </c>
       <c r="I12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -38969,27 +39808,27 @@
       </c>
       <c r="C13" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '4', </v>
+        <v xml:space="preserve">'resource' =&gt; '3', </v>
       </c>
       <c r="D13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'role' =&gt; '2', </v>
+        <v xml:space="preserve">'name' =&gt; 'Role Resource', </v>
       </c>
       <c r="E13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Resources assigned to a role', </v>
       </c>
       <c r="F13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Resources', </v>
       </c>
       <c r="G13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '11', </v>
       </c>
       <c r="I13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -39042,27 +39881,27 @@
       </c>
       <c r="C14" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '5', </v>
+        <v xml:space="preserve">'resource' =&gt; '4', </v>
       </c>
       <c r="D14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'role' =&gt; '1', </v>
+        <v xml:space="preserve">'name' =&gt; 'Resource Roles', </v>
       </c>
       <c r="E14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'The details of roles who have access to this resource', </v>
       </c>
       <c r="F14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Roles', </v>
       </c>
       <c r="G14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
       </c>
       <c r="H14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '3', </v>
       </c>
       <c r="I14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -39115,27 +39954,27 @@
       </c>
       <c r="C15" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '5', </v>
+        <v xml:space="preserve">'resource' =&gt; '4', </v>
       </c>
       <c r="D15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'role' =&gt; '3', </v>
+        <v xml:space="preserve">'name' =&gt; 'Resource Actions', </v>
       </c>
       <c r="E15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Get actions available for the resource', </v>
       </c>
       <c r="F15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Actions', </v>
       </c>
       <c r="G15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '7', </v>
       </c>
       <c r="I15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -39192,23 +40031,23 @@
       </c>
       <c r="D16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'role' =&gt; '2', </v>
+        <v xml:space="preserve">'name' =&gt; 'Resource Action Methods', </v>
       </c>
       <c r="E16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Handler details of an action', </v>
       </c>
       <c r="F16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Method', </v>
       </c>
       <c r="G16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasOne', </v>
       </c>
       <c r="H16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '8', </v>
       </c>
       <c r="I16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -39261,27 +40100,27 @@
       </c>
       <c r="C17" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '8', </v>
+        <v xml:space="preserve">'resource' =&gt; '7', </v>
       </c>
       <c r="D17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'role' =&gt; '2', </v>
+        <v xml:space="preserve">'name' =&gt; 'Resource Action Lists', </v>
       </c>
       <c r="E17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Lists where action available', </v>
       </c>
       <c r="F17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Lists', </v>
       </c>
       <c r="G17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '9', </v>
       </c>
       <c r="I17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -39334,27 +40173,27 @@
       </c>
       <c r="C18" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '9', </v>
+        <v xml:space="preserve">'resource' =&gt; '7', </v>
       </c>
       <c r="D18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'role' =&gt; '2', </v>
+        <v xml:space="preserve">'name' =&gt; 'Resource Action Data', </v>
       </c>
       <c r="E18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Resource data where action available', </v>
       </c>
       <c r="F18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Data', </v>
       </c>
       <c r="G18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '10', </v>
       </c>
       <c r="I18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -39407,27 +40246,27 @@
       </c>
       <c r="C19" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '10', </v>
+        <v xml:space="preserve">'resource' =&gt; '5', </v>
       </c>
       <c r="D19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'role' =&gt; '2', </v>
+        <v xml:space="preserve">'name' =&gt; 'Organisation Contacts', </v>
       </c>
       <c r="E19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Contact details of organisation', </v>
       </c>
       <c r="F19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Contacts', </v>
       </c>
       <c r="G19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '6', </v>
       </c>
       <c r="I19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -39480,27 +40319,27 @@
       </c>
       <c r="C20" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '12', </v>
+        <v xml:space="preserve">'resource' =&gt; '11', </v>
       </c>
       <c r="D20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'role' =&gt; '2', </v>
+        <v xml:space="preserve">'name' =&gt; 'Resource Details', </v>
       </c>
       <c r="E20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Resource details', </v>
       </c>
       <c r="F20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Resource', </v>
       </c>
       <c r="G20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
       </c>
       <c r="I20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -39553,27 +40392,27 @@
       </c>
       <c r="C21" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '13', </v>
+        <v xml:space="preserve">'resource' =&gt; '4', </v>
       </c>
       <c r="D21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'role' =&gt; '2', </v>
+        <v xml:space="preserve">'name' =&gt; 'Resource Forms', </v>
       </c>
       <c r="E21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Forms available for a resource', </v>
       </c>
       <c r="F21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Forms', </v>
       </c>
       <c r="G21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '12', </v>
       </c>
       <c r="I21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -39626,27 +40465,27 @@
       </c>
       <c r="C22" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '14', </v>
+        <v xml:space="preserve">'resource' =&gt; '12', </v>
       </c>
       <c r="D22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'role' =&gt; '2', </v>
+        <v xml:space="preserve">'name' =&gt; 'Form Fields', </v>
       </c>
       <c r="E22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Fields associated with a form', </v>
       </c>
       <c r="F22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Fields', </v>
       </c>
       <c r="G22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '13', </v>
       </c>
       <c r="I22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -39699,27 +40538,27 @@
       </c>
       <c r="C23" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '15', </v>
+        <v xml:space="preserve">'resource' =&gt; '13', </v>
       </c>
       <c r="D23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'role' =&gt; '2', </v>
+        <v xml:space="preserve">'name' =&gt; 'Field Attributes', </v>
       </c>
       <c r="E23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Attributes of Field', </v>
       </c>
       <c r="F23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Attributes', </v>
       </c>
       <c r="G23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '14', </v>
       </c>
       <c r="I23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -39772,27 +40611,27 @@
       </c>
       <c r="C24" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '16', </v>
+        <v xml:space="preserve">'resource' =&gt; '13', </v>
       </c>
       <c r="D24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'role' =&gt; '2', </v>
+        <v xml:space="preserve">'name' =&gt; 'Field Options', </v>
       </c>
       <c r="E24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Options of Field', </v>
       </c>
       <c r="F24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Options', </v>
       </c>
       <c r="G24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasOne', </v>
       </c>
       <c r="H24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '15', </v>
       </c>
       <c r="I24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -39845,27 +40684,27 @@
       </c>
       <c r="C25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '17', </v>
+        <v xml:space="preserve">'resource' =&gt; '13', </v>
       </c>
       <c r="D25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'role' =&gt; '2', </v>
+        <v xml:space="preserve">'name' =&gt; 'Field Validations', </v>
       </c>
       <c r="E25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Validation details of field', </v>
       </c>
       <c r="F25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Validations', </v>
       </c>
       <c r="G25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H25" s="33" t="str">
         <f t="shared" ref="H25:K88" ca="1" si="4">IF(AND($B25=$S$4,H$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A25,INDIRECT($E$2),H$4+$B$4,0)="","","'"&amp;H$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A25,INDIRECT($E$2),H$4+$B$4,0)&amp;"', "),"")</f>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '16', </v>
       </c>
       <c r="I25" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -39918,27 +40757,27 @@
       </c>
       <c r="C26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '18', </v>
+        <v xml:space="preserve">'resource' =&gt; '12', </v>
       </c>
       <c r="D26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'role' =&gt; '2', </v>
+        <v xml:space="preserve">'name' =&gt; 'From Resource', </v>
       </c>
       <c r="E26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Resource this form belongs to', </v>
       </c>
       <c r="F26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Resource', </v>
       </c>
       <c r="G26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H26" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
       </c>
       <c r="I26" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -39991,27 +40830,27 @@
       </c>
       <c r="C27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '19', </v>
+        <v xml:space="preserve">'resource' =&gt; '12', </v>
       </c>
       <c r="D27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'role' =&gt; '2', </v>
+        <v xml:space="preserve">'name' =&gt; 'Form Defaults', </v>
       </c>
       <c r="E27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Predefined values for a form', </v>
       </c>
       <c r="F27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Defaults', </v>
       </c>
       <c r="G27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H27" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '17', </v>
       </c>
       <c r="I27" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -40064,27 +40903,27 @@
       </c>
       <c r="C28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '20', </v>
+        <v xml:space="preserve">'resource' =&gt; '13', </v>
       </c>
       <c r="D28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'role' =&gt; '2', </v>
+        <v xml:space="preserve">'name' =&gt; 'Field Data', </v>
       </c>
       <c r="E28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Fields Database binding details', </v>
       </c>
       <c r="F28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Data', </v>
       </c>
       <c r="G28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasOne', </v>
       </c>
       <c r="H28" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '18', </v>
       </c>
       <c r="I28" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -40137,27 +40976,27 @@
       </c>
       <c r="C29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '21', </v>
+        <v xml:space="preserve">'resource' =&gt; '4', </v>
       </c>
       <c r="D29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'role' =&gt; '2', </v>
+        <v xml:space="preserve">'name' =&gt; 'Resource Relations', </v>
       </c>
       <c r="E29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Relation of  a resource to another resource', </v>
       </c>
       <c r="F29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Relations', </v>
       </c>
       <c r="G29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H29" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
       </c>
       <c r="I29" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -40210,27 +41049,27 @@
       </c>
       <c r="C30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '22', </v>
+        <v xml:space="preserve">'resource' =&gt; '18', </v>
       </c>
       <c r="D30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'role' =&gt; '2', </v>
+        <v xml:space="preserve">'name' =&gt; 'Bind Data Relation', </v>
       </c>
       <c r="E30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Relation to which the data to be bind', </v>
       </c>
       <c r="F30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
       </c>
       <c r="G30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H30" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
       </c>
       <c r="I30" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -40283,27 +41122,27 @@
       </c>
       <c r="C31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '23', </v>
+        <v xml:space="preserve">'resource' =&gt; '17', </v>
       </c>
       <c r="D31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'role' =&gt; '2', </v>
+        <v xml:space="preserve">'name' =&gt; 'Default Data Resource', </v>
       </c>
       <c r="E31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Resource to which the forms predefined data to be bind', </v>
       </c>
       <c r="F31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
       </c>
       <c r="G31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H31" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
       </c>
       <c r="I31" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -40356,27 +41195,27 @@
       </c>
       <c r="C32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '24', </v>
+        <v xml:space="preserve">'resource' =&gt; '19', </v>
       </c>
       <c r="D32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'role' =&gt; '2', </v>
+        <v xml:space="preserve">'name' =&gt; 'Resource Details', </v>
       </c>
       <c r="E32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Resource details of a list', </v>
       </c>
       <c r="F32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Resource', </v>
       </c>
       <c r="G32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H32" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
       </c>
       <c r="I32" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -40429,27 +41268,27 @@
       </c>
       <c r="C33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '25', </v>
+        <v xml:space="preserve">'resource' =&gt; '19', </v>
       </c>
       <c r="D33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'role' =&gt; '2', </v>
+        <v xml:space="preserve">'name' =&gt; 'List Relations', </v>
       </c>
       <c r="E33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Relations to be loaded on accessing list', </v>
       </c>
       <c r="F33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Relations', </v>
       </c>
       <c r="G33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H33" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '20', </v>
       </c>
       <c r="I33" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -40502,27 +41341,27 @@
       </c>
       <c r="C34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '26', </v>
+        <v xml:space="preserve">'resource' =&gt; '4', </v>
       </c>
       <c r="D34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'role' =&gt; '2', </v>
+        <v xml:space="preserve">'name' =&gt; 'Resource Scopes', </v>
       </c>
       <c r="E34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Scopes available on a Resource', </v>
       </c>
       <c r="F34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Scopes', </v>
       </c>
       <c r="G34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H34" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '21', </v>
       </c>
       <c r="I34" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -40575,27 +41414,27 @@
       </c>
       <c r="C35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '27', </v>
+        <v xml:space="preserve">'resource' =&gt; '19', </v>
       </c>
       <c r="D35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'role' =&gt; '2', </v>
+        <v xml:space="preserve">'name' =&gt; 'List Scopes', </v>
       </c>
       <c r="E35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Scopes by which a list to be filtered', </v>
       </c>
       <c r="F35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Scopes', </v>
       </c>
       <c r="G35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
       </c>
       <c r="H35" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '21', </v>
       </c>
       <c r="I35" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -40648,27 +41487,27 @@
       </c>
       <c r="C36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '28', </v>
+        <v xml:space="preserve">'resource' =&gt; '23', </v>
       </c>
       <c r="D36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'role' =&gt; '2', </v>
+        <v xml:space="preserve">'name' =&gt; 'Data Relation', </v>
       </c>
       <c r="E36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Relations to be loaded on a data view', </v>
       </c>
       <c r="F36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Relations', </v>
       </c>
       <c r="G36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H36" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '24', </v>
       </c>
       <c r="I36" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -40721,27 +41560,27 @@
       </c>
       <c r="C37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '29', </v>
+        <v xml:space="preserve">'resource' =&gt; '23', </v>
       </c>
       <c r="D37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'role' =&gt; '2', </v>
+        <v xml:space="preserve">'name' =&gt; 'Resource Details', </v>
       </c>
       <c r="E37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Details of resource of a record', </v>
       </c>
       <c r="F37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Resource', </v>
       </c>
       <c r="G37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H37" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
       </c>
       <c r="I37" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -40794,27 +41633,27 @@
       </c>
       <c r="C38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '30', </v>
+        <v xml:space="preserve">'resource' =&gt; '19', </v>
       </c>
       <c r="D38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'role' =&gt; '2', </v>
+        <v xml:space="preserve">'name' =&gt; 'List Layout', </v>
       </c>
       <c r="E38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Layout of a list', </v>
       </c>
       <c r="F38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Layout', </v>
       </c>
       <c r="G38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H38" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '25', </v>
       </c>
       <c r="I38" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -40863,31 +41702,31 @@
       </c>
       <c r="B39" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>;</v>
+        <v>-&gt;create([</v>
       </c>
       <c r="C39" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '26', </v>
       </c>
       <c r="D39" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Nested Relation', </v>
       </c>
       <c r="E39" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Nested Relation', </v>
       </c>
       <c r="F39" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Nest', </v>
       </c>
       <c r="G39" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H39" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
       </c>
       <c r="I39" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -40927,7 +41766,7 @@
       </c>
       <c r="R39" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="40" spans="1:18">
@@ -40936,31 +41775,31 @@
       </c>
       <c r="B40" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
+        <v>-&gt;create([</v>
       </c>
       <c r="C40" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '26', </v>
       </c>
       <c r="D40" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Related Resource', </v>
       </c>
       <c r="E40" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Related Resource Details', </v>
       </c>
       <c r="F40" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
       </c>
       <c r="G40" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H40" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
       </c>
       <c r="I40" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -41000,7 +41839,7 @@
       </c>
       <c r="R40" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="41" spans="1:18">
@@ -41009,31 +41848,31 @@
       </c>
       <c r="B41" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C41" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '26', </v>
       </c>
       <c r="D41" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Form Layout', </v>
       </c>
       <c r="E41" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Layout details', </v>
       </c>
       <c r="F41" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Layout', </v>
       </c>
       <c r="G41" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H41" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '27', </v>
       </c>
       <c r="I41" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -41073,7 +41912,7 @@
       </c>
       <c r="R41" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="42" spans="1:18">
@@ -41082,31 +41921,31 @@
       </c>
       <c r="B42" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C42" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '23', </v>
       </c>
       <c r="D42" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Data View Section', </v>
       </c>
       <c r="E42" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Section details of data view', </v>
       </c>
       <c r="F42" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Sections', </v>
       </c>
       <c r="G42" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H42" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '28', </v>
       </c>
       <c r="I42" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -41146,7 +41985,7 @@
       </c>
       <c r="R42" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="43" spans="1:18">
@@ -41155,31 +41994,31 @@
       </c>
       <c r="B43" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C43" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '26', </v>
       </c>
       <c r="D43" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Data View Section Items', </v>
       </c>
       <c r="E43" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Items of a data view section', </v>
       </c>
       <c r="F43" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Items', </v>
       </c>
       <c r="G43" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H43" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '29', </v>
       </c>
       <c r="I43" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -41219,7 +42058,7 @@
       </c>
       <c r="R43" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="44" spans="1:18">
@@ -41228,31 +42067,31 @@
       </c>
       <c r="B44" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C44" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '28', </v>
       </c>
       <c r="D44" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Data Relation', </v>
       </c>
       <c r="E44" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'View relation of a data', </v>
       </c>
       <c r="F44" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
       </c>
       <c r="G44" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H44" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
       </c>
       <c r="I44" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -41292,7 +42131,7 @@
       </c>
       <c r="R44" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="45" spans="1:18">
@@ -41301,31 +42140,31 @@
       </c>
       <c r="B45" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C45" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '29', </v>
       </c>
       <c r="D45" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Data item relation', </v>
       </c>
       <c r="E45" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'View relation of a data item', </v>
       </c>
       <c r="F45" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
       </c>
       <c r="G45" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H45" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
       </c>
       <c r="I45" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -41365,7 +42204,7 @@
       </c>
       <c r="R45" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="46" spans="1:18">
@@ -41374,31 +42213,31 @@
       </c>
       <c r="B46" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C46" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '26', </v>
       </c>
       <c r="D46" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Owner Relation', </v>
       </c>
       <c r="E46" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'View the owner resource', </v>
       </c>
       <c r="F46" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Owner', </v>
       </c>
       <c r="G46" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H46" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
       </c>
       <c r="I46" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -41438,7 +42277,7 @@
       </c>
       <c r="R46" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="47" spans="1:18">
@@ -41447,31 +42286,31 @@
       </c>
       <c r="B47" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C47" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '12', </v>
       </c>
       <c r="D47" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Collections', </v>
       </c>
       <c r="E47" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Collection/Detail form', </v>
       </c>
       <c r="F47" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Collections', </v>
       </c>
       <c r="G47" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H47" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '30', </v>
       </c>
       <c r="I47" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -41511,7 +42350,7 @@
       </c>
       <c r="R47" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="48" spans="1:18">
@@ -41520,31 +42359,31 @@
       </c>
       <c r="B48" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C48" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '30', </v>
       </c>
       <c r="D48" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Collection Form', </v>
       </c>
       <c r="E48" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Collection Form', </v>
       </c>
       <c r="F48" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Form', </v>
       </c>
       <c r="G48" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H48" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '12', </v>
       </c>
       <c r="I48" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -41584,7 +42423,7 @@
       </c>
       <c r="R48" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="49" spans="1:18">
@@ -41593,31 +42432,31 @@
       </c>
       <c r="B49" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C49" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '30', </v>
       </c>
       <c r="D49" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Relation', </v>
       </c>
       <c r="E49" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Details of Relation', </v>
       </c>
       <c r="F49" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
       </c>
       <c r="G49" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H49" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
       </c>
       <c r="I49" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -41657,7 +42496,7 @@
       </c>
       <c r="R49" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="50" spans="1:18">
@@ -41666,31 +42505,31 @@
       </c>
       <c r="B50" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C50" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '15', </v>
       </c>
       <c r="D50" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Field', </v>
       </c>
       <c r="E50" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Field details', </v>
       </c>
       <c r="F50" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Field', </v>
       </c>
       <c r="G50" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H50" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '13', </v>
       </c>
       <c r="I50" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -41730,7 +42569,7 @@
       </c>
       <c r="R50" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="51" spans="1:18">
@@ -41739,31 +42578,31 @@
       </c>
       <c r="B51" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C51" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '13', </v>
       </c>
       <c r="D51" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Form', </v>
       </c>
       <c r="E51" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Form details', </v>
       </c>
       <c r="F51" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Form', </v>
       </c>
       <c r="G51" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H51" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '12', </v>
       </c>
       <c r="I51" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -41803,7 +42642,7 @@
       </c>
       <c r="R51" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="52" spans="1:18">
@@ -41812,31 +42651,31 @@
       </c>
       <c r="B52" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C52" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '19', </v>
       </c>
       <c r="D52" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'List Search', </v>
       </c>
       <c r="E52" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Search fields for a list', </v>
       </c>
       <c r="F52" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Search', </v>
       </c>
       <c r="G52" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H52" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '31', </v>
       </c>
       <c r="I52" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -41876,7 +42715,7 @@
       </c>
       <c r="R52" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="53" spans="1:18">
@@ -41885,7 +42724,7 @@
       </c>
       <c r="B53" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>;</v>
       </c>
       <c r="C53" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -41958,7 +42797,7 @@
       </c>
       <c r="B54" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
       </c>
       <c r="C54" s="33" t="str">
         <f t="shared" ca="1" si="3"/>

</xml_diff>

<commit_message>
New Resource, ResourceFormFieldDepends, added and related
</commit_message>
<xml_diff>
--- a/Helper.xlsx
+++ b/Helper.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Tables" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3339" uniqueCount="679">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3407" uniqueCount="698">
   <si>
     <t>resource_scopes</t>
   </si>
@@ -2075,6 +2075,63 @@
   </si>
   <si>
     <t>Search fields for a list</t>
+  </si>
+  <si>
+    <t>resource_form_field_depends</t>
+  </si>
+  <si>
+    <t>form_field_depend_field</t>
+  </si>
+  <si>
+    <t>depend_field</t>
+  </si>
+  <si>
+    <t>form_field_depend_db_field</t>
+  </si>
+  <si>
+    <t>db_field</t>
+  </si>
+  <si>
+    <t>sql_query_comparison_operator</t>
+  </si>
+  <si>
+    <t>operator</t>
+  </si>
+  <si>
+    <t>['=','&lt;','&gt;','&lt;=','&gt;=','&lt;&gt;','In','NotIn','like']</t>
+  </si>
+  <si>
+    <t>default('=')</t>
+  </si>
+  <si>
+    <t>form_field_depend_compare_method</t>
+  </si>
+  <si>
+    <t>compare_method</t>
+  </si>
+  <si>
+    <t>Field Depends</t>
+  </si>
+  <si>
+    <t>ResourceFormFieldDepend</t>
+  </si>
+  <si>
+    <t>Dependent fields in a form</t>
+  </si>
+  <si>
+    <t>Dependent Fields</t>
+  </si>
+  <si>
+    <t>__resource_form_field_depends</t>
+  </si>
+  <si>
+    <t>Depending Fields</t>
+  </si>
+  <si>
+    <t>Dependent fields</t>
+  </si>
+  <si>
+    <t>Depends</t>
   </si>
 </sst>
 </file>
@@ -2304,7 +2361,212 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="123">
+  <dxfs count="127">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -3623,163 +3885,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -4078,35 +4183,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tables" displayName="Tables" ref="A1:J37" totalsRowShown="0" dataDxfId="122">
-  <autoFilter ref="A1:J37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tables" displayName="Tables" ref="A1:J38" totalsRowShown="0" dataDxfId="126">
+  <autoFilter ref="A1:J38"/>
   <tableColumns count="10">
-    <tableColumn id="2" name="Name" dataDxfId="121"/>
-    <tableColumn id="10" name="Table" dataDxfId="120">
+    <tableColumn id="2" name="Name" dataDxfId="125"/>
+    <tableColumn id="10" name="Table" dataDxfId="124">
       <calculatedColumnFormula>"__"&amp;[Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Singular Name" dataDxfId="119">
+    <tableColumn id="5" name="Singular Name" dataDxfId="123">
       <calculatedColumnFormula>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Model NS" dataDxfId="118">
+    <tableColumn id="8" name="Model NS" dataDxfId="122">
       <calculatedColumnFormula>"Milestone\Appframe\Model"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Class Name" dataDxfId="117">
+    <tableColumn id="4" name="Class Name" dataDxfId="121">
       <calculatedColumnFormula>SUBSTITUTE(PROPER([Singular Name]),"_","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Migration Artisan" dataDxfId="116">
+    <tableColumn id="1" name="Migration Artisan" dataDxfId="120">
       <calculatedColumnFormula>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Model Artisan" dataDxfId="115">
+    <tableColumn id="6" name="Model Artisan" dataDxfId="119">
       <calculatedColumnFormula>"php artisan make:model "&amp;[Class Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Model Statement" dataDxfId="114">
+    <tableColumn id="3" name="Model Statement" dataDxfId="118">
       <calculatedColumnFormula>"protected $table = '"&amp;[Table]&amp;"';"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Seeder Artisan" dataDxfId="113">
+    <tableColumn id="7" name="Seeder Artisan" dataDxfId="117">
       <calculatedColumnFormula>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Seeder Class" dataDxfId="112">
+    <tableColumn id="9" name="Seeder Class" dataDxfId="116">
       <calculatedColumnFormula>[Class Name]&amp;"TableSeeder"&amp;"::class,"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4115,92 +4220,92 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="ResourceActions" displayName="ResourceActions" ref="A1:P9" totalsRowShown="0" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="ResourceActions" displayName="ResourceActions" ref="A1:P9" totalsRowShown="0" dataDxfId="32">
   <autoFilter ref="A1:P9"/>
   <tableColumns count="16">
-    <tableColumn id="1" name="No" dataDxfId="15">
+    <tableColumn id="1" name="No" dataDxfId="31">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Resource" dataDxfId="14"/>
-    <tableColumn id="13" name="Resource Id" dataDxfId="13">
+    <tableColumn id="2" name="Resource" dataDxfId="30"/>
+    <tableColumn id="13" name="Resource Id" dataDxfId="29">
       <calculatedColumnFormula>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Action Name" dataDxfId="12"/>
-    <tableColumn id="4" name="Description" dataDxfId="11"/>
-    <tableColumn id="5" name="Action Title" dataDxfId="10"/>
-    <tableColumn id="6" name="Button Type" dataDxfId="9"/>
-    <tableColumn id="7" name="Menu" dataDxfId="8"/>
-    <tableColumn id="8" name="Icon" dataDxfId="7"/>
-    <tableColumn id="9" name="Set" dataDxfId="6"/>
-    <tableColumn id="14" name="Action Type" dataDxfId="5"/>
-    <tableColumn id="15" name="ID1" dataDxfId="4"/>
-    <tableColumn id="16" name="ID2" dataDxfId="3"/>
-    <tableColumn id="10" name="On" dataDxfId="2"/>
-    <tableColumn id="11" name="Confirm" dataDxfId="1"/>
-    <tableColumn id="12" name="handler" dataDxfId="0"/>
+    <tableColumn id="3" name="Action Name" dataDxfId="28"/>
+    <tableColumn id="4" name="Description" dataDxfId="27"/>
+    <tableColumn id="5" name="Action Title" dataDxfId="26"/>
+    <tableColumn id="6" name="Button Type" dataDxfId="25"/>
+    <tableColumn id="7" name="Menu" dataDxfId="24"/>
+    <tableColumn id="8" name="Icon" dataDxfId="23"/>
+    <tableColumn id="9" name="Set" dataDxfId="22"/>
+    <tableColumn id="14" name="Action Type" dataDxfId="21"/>
+    <tableColumn id="15" name="ID1" dataDxfId="20"/>
+    <tableColumn id="16" name="ID2" dataDxfId="19"/>
+    <tableColumn id="10" name="On" dataDxfId="18"/>
+    <tableColumn id="11" name="Confirm" dataDxfId="17"/>
+    <tableColumn id="12" name="handler" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Columns" displayName="Columns" ref="A1:I135" totalsRowShown="0" dataDxfId="105">
-  <autoFilter ref="A1:I135">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Columns" displayName="Columns" ref="A1:I139" totalsRowShown="0" dataDxfId="109">
+  <autoFilter ref="A1:I139">
     <filterColumn colId="0"/>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" name="Column" dataDxfId="104"/>
-    <tableColumn id="2" name="Type" dataDxfId="103"/>
-    <tableColumn id="3" name="Name" dataDxfId="102"/>
-    <tableColumn id="4" name="Length/Enum" dataDxfId="101"/>
-    <tableColumn id="5" name="Method1" dataDxfId="100"/>
-    <tableColumn id="6" name="Method2" dataDxfId="99"/>
-    <tableColumn id="7" name="Method3" dataDxfId="98"/>
-    <tableColumn id="8" name="Method4" dataDxfId="97"/>
-    <tableColumn id="9" name="Method5" dataDxfId="96"/>
+    <tableColumn id="1" name="Column" dataDxfId="108"/>
+    <tableColumn id="2" name="Type" dataDxfId="107"/>
+    <tableColumn id="3" name="Name" dataDxfId="106"/>
+    <tableColumn id="4" name="Length/Enum" dataDxfId="105"/>
+    <tableColumn id="5" name="Method1" dataDxfId="104"/>
+    <tableColumn id="6" name="Method2" dataDxfId="103"/>
+    <tableColumn id="7" name="Method3" dataDxfId="102"/>
+    <tableColumn id="8" name="Method4" dataDxfId="101"/>
+    <tableColumn id="9" name="Method5" dataDxfId="100"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TableFields" displayName="TableFields" ref="A1:K323" totalsRowShown="0" dataDxfId="95">
-  <autoFilter ref="A1:K323">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TableFields" displayName="TableFields" ref="A1:K332" totalsRowShown="0" dataDxfId="4">
+  <autoFilter ref="A1:K332">
     <filterColumn colId="0">
       <filters>
-        <filter val="resource_form_field_data"/>
-        <filter val="resource_list_search"/>
+        <filter val="resource_form_field_depends"/>
+        <filter val="resource_form_fields"/>
       </filters>
     </filterColumn>
   </autoFilter>
   <tableColumns count="11">
-    <tableColumn id="2" name="Table" dataDxfId="94"/>
-    <tableColumn id="3" name="Field" dataDxfId="93"/>
-    <tableColumn id="5" name="Type" dataDxfId="92">
+    <tableColumn id="2" name="Table" dataDxfId="15"/>
+    <tableColumn id="3" name="Field" dataDxfId="14"/>
+    <tableColumn id="5" name="Type" dataDxfId="13">
       <calculatedColumnFormula>VLOOKUP([Field],Columns[],2,0)&amp;"("</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Name" dataDxfId="91">
+    <tableColumn id="4" name="Name" dataDxfId="12">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Arg2" dataDxfId="90">
+    <tableColumn id="6" name="Arg2" dataDxfId="11">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Method1" dataDxfId="89">
+    <tableColumn id="7" name="Method1" dataDxfId="10">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Method2" dataDxfId="88">
+    <tableColumn id="8" name="Method2" dataDxfId="9">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Method3" dataDxfId="87">
+    <tableColumn id="9" name="Method3" dataDxfId="8">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Method4" dataDxfId="86">
+    <tableColumn id="10" name="Method4" dataDxfId="7">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Method5" dataDxfId="85">
+    <tableColumn id="11" name="Method5" dataDxfId="6">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Statement" dataDxfId="84">
+    <tableColumn id="12" name="Statement" dataDxfId="5">
       <calculatedColumnFormula>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4209,8 +4314,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R307" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
-  <autoFilter ref="A1:R307">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R310" totalsRowShown="0" headerRowDxfId="99" dataDxfId="98">
+  <autoFilter ref="A1:R310">
     <filterColumn colId="1">
       <filters>
         <filter val="Resource Roles"/>
@@ -4218,46 +4323,46 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="18">
-    <tableColumn id="19" name="TRCode" dataDxfId="81">
+    <tableColumn id="19" name="TRCode" dataDxfId="97">
       <calculatedColumnFormula>[Table Name]&amp;"-"&amp;[Record No]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Table Name" dataDxfId="80"/>
-    <tableColumn id="2" name="Record No" dataDxfId="79">
+    <tableColumn id="1" name="Table Name" dataDxfId="96"/>
+    <tableColumn id="2" name="Record No" dataDxfId="95">
       <calculatedColumnFormula>COUNTIF($B$1:$B1,[Table Name])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="1" dataDxfId="78"/>
-    <tableColumn id="4" name="2" dataDxfId="77"/>
-    <tableColumn id="5" name="3" dataDxfId="76"/>
-    <tableColumn id="6" name="4" dataDxfId="75"/>
-    <tableColumn id="7" name="5" dataDxfId="74"/>
-    <tableColumn id="8" name="6" dataDxfId="73"/>
-    <tableColumn id="9" name="7" dataDxfId="72"/>
-    <tableColumn id="10" name="8" dataDxfId="71"/>
-    <tableColumn id="11" name="9" dataDxfId="70"/>
-    <tableColumn id="12" name="10" dataDxfId="69"/>
-    <tableColumn id="13" name="11" dataDxfId="68"/>
-    <tableColumn id="14" name="12" dataDxfId="67"/>
-    <tableColumn id="15" name="13" dataDxfId="66"/>
-    <tableColumn id="16" name="14" dataDxfId="65"/>
-    <tableColumn id="17" name="15" dataDxfId="64"/>
+    <tableColumn id="3" name="1" dataDxfId="94"/>
+    <tableColumn id="4" name="2" dataDxfId="93"/>
+    <tableColumn id="5" name="3" dataDxfId="92"/>
+    <tableColumn id="6" name="4" dataDxfId="91"/>
+    <tableColumn id="7" name="5" dataDxfId="90"/>
+    <tableColumn id="8" name="6" dataDxfId="89"/>
+    <tableColumn id="9" name="7" dataDxfId="88"/>
+    <tableColumn id="10" name="8" dataDxfId="87"/>
+    <tableColumn id="11" name="9" dataDxfId="86"/>
+    <tableColumn id="12" name="10" dataDxfId="85"/>
+    <tableColumn id="13" name="11" dataDxfId="84"/>
+    <tableColumn id="14" name="12" dataDxfId="83"/>
+    <tableColumn id="15" name="13" dataDxfId="82"/>
+    <tableColumn id="16" name="14" dataDxfId="81"/>
+    <tableColumn id="17" name="15" dataDxfId="80"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SeedMap" displayName="SeedMap" ref="A1:E31" totalsRowShown="0" dataDxfId="63">
-  <autoFilter ref="A1:E31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SeedMap" displayName="SeedMap" ref="A1:E32" totalsRowShown="0" dataDxfId="79">
+  <autoFilter ref="A1:E32"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Name" dataDxfId="62"/>
-    <tableColumn id="3" name="FW Table Name" dataDxfId="61"/>
-    <tableColumn id="20" name="NS" dataDxfId="60">
+    <tableColumn id="1" name="Name" dataDxfId="78"/>
+    <tableColumn id="3" name="FW Table Name" dataDxfId="77"/>
+    <tableColumn id="20" name="NS" dataDxfId="76">
       <calculatedColumnFormula>VLOOKUP([FW Table Name],Tables[],4,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="Model" dataDxfId="59">
+    <tableColumn id="21" name="Model" dataDxfId="75">
       <calculatedColumnFormula>VLOOKUP([FW Table Name],Tables[],5,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Query Method" dataDxfId="58">
+    <tableColumn id="4" name="Query Method" dataDxfId="74">
       <calculatedColumnFormula>"truncate"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4266,46 +4371,46 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="ResourceTable" displayName="ResourceTable" ref="A1:I32" totalsRowShown="0" dataDxfId="57">
-  <autoFilter ref="A1:I32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="ResourceTable" displayName="ResourceTable" ref="A1:I33" totalsRowShown="0" dataDxfId="73">
+  <autoFilter ref="A1:I33"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="No" dataDxfId="56">
+    <tableColumn id="1" name="No" dataDxfId="72">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Name" dataDxfId="55"/>
-    <tableColumn id="3" name="Description" dataDxfId="54"/>
-    <tableColumn id="4" name="Title" dataDxfId="53"/>
-    <tableColumn id="5" name="NS" dataDxfId="52">
+    <tableColumn id="2" name="Name" dataDxfId="71"/>
+    <tableColumn id="3" name="Description" dataDxfId="70"/>
+    <tableColumn id="4" name="Title" dataDxfId="69"/>
+    <tableColumn id="5" name="NS" dataDxfId="68">
       <calculatedColumnFormula>"Milestone\Appframe\Model"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Table" dataDxfId="51"/>
-    <tableColumn id="7" name="Key" dataDxfId="50">
+    <tableColumn id="6" name="Table" dataDxfId="67"/>
+    <tableColumn id="7" name="Key" dataDxfId="66">
       <calculatedColumnFormula>"id"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Controller" dataDxfId="49"/>
-    <tableColumn id="9" name="Controller NS" dataDxfId="48"/>
+    <tableColumn id="8" name="Controller" dataDxfId="65"/>
+    <tableColumn id="9" name="Controller NS" dataDxfId="64"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RelationTable" displayName="RelationTable" ref="A1:I45" totalsRowShown="0" dataDxfId="47">
-  <autoFilter ref="A1:I45"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RelationTable" displayName="RelationTable" ref="A1:I46" totalsRowShown="0" dataDxfId="63">
+  <autoFilter ref="A1:I46"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="No" dataDxfId="46">
+    <tableColumn id="1" name="No" dataDxfId="62">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Resource" dataDxfId="45"/>
-    <tableColumn id="4" name="Relate Resource" dataDxfId="44"/>
-    <tableColumn id="2" name="Resource Id" dataDxfId="43">
+    <tableColumn id="3" name="Resource" dataDxfId="61"/>
+    <tableColumn id="4" name="Relate Resource" dataDxfId="60"/>
+    <tableColumn id="2" name="Resource Id" dataDxfId="59">
       <calculatedColumnFormula>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Name" dataDxfId="42"/>
-    <tableColumn id="6" name="Description" dataDxfId="41"/>
-    <tableColumn id="7" name="Method" dataDxfId="40"/>
-    <tableColumn id="8" name="Type" dataDxfId="39"/>
-    <tableColumn id="10" name="Relate Id" dataDxfId="38">
+    <tableColumn id="5" name="Name" dataDxfId="58"/>
+    <tableColumn id="6" name="Description" dataDxfId="57"/>
+    <tableColumn id="7" name="Method" dataDxfId="56"/>
+    <tableColumn id="8" name="Type" dataDxfId="55"/>
+    <tableColumn id="10" name="Relate Id" dataDxfId="54">
       <calculatedColumnFormula>VLOOKUP([Relate Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4314,47 +4419,47 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="ResourceForms" displayName="ResourceForms" ref="A1:G9" totalsRowShown="0" dataDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="ResourceForms" displayName="ResourceForms" ref="A1:G9" totalsRowShown="0" dataDxfId="53">
   <autoFilter ref="A1:G9"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="No" dataDxfId="36">
+    <tableColumn id="1" name="No" dataDxfId="52">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Resource ID" dataDxfId="35"/>
-    <tableColumn id="3" name="Resource Name" dataDxfId="34">
+    <tableColumn id="2" name="Resource ID" dataDxfId="51"/>
+    <tableColumn id="3" name="Resource Name" dataDxfId="50">
       <calculatedColumnFormula>VLOOKUP([Resource ID],ResourceTable[],2,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Form Name" dataDxfId="33"/>
-    <tableColumn id="6" name="Title" dataDxfId="32"/>
-    <tableColumn id="7" name="Action Text" dataDxfId="31"/>
-    <tableColumn id="8" name="Description" dataDxfId="30"/>
+    <tableColumn id="4" name="Form Name" dataDxfId="49"/>
+    <tableColumn id="6" name="Title" dataDxfId="48"/>
+    <tableColumn id="7" name="Action Text" dataDxfId="47"/>
+    <tableColumn id="8" name="Description" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="FormFields" displayName="FormFields" ref="A1:L33" totalsRowShown="0" dataDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="FormFields" displayName="FormFields" ref="A1:L33" totalsRowShown="0" dataDxfId="45">
   <autoFilter ref="A1:L33"/>
   <tableColumns count="12">
-    <tableColumn id="9" name="No" dataDxfId="28">
+    <tableColumn id="9" name="No" dataDxfId="44">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Form Id" dataDxfId="27"/>
-    <tableColumn id="7" name="Form Name" dataDxfId="26">
+    <tableColumn id="1" name="Form Id" dataDxfId="43"/>
+    <tableColumn id="7" name="Form Name" dataDxfId="42">
       <calculatedColumnFormula>VLOOKUP([Form Id],ResourceForms[],4,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Name" dataDxfId="25"/>
-    <tableColumn id="2" name="Type" dataDxfId="24"/>
-    <tableColumn id="5" name="Label" dataDxfId="23"/>
-    <tableColumn id="6" name="Collection" dataDxfId="22"/>
-    <tableColumn id="14" name="Attribute" dataDxfId="21">
+    <tableColumn id="4" name="Name" dataDxfId="41"/>
+    <tableColumn id="2" name="Type" dataDxfId="40"/>
+    <tableColumn id="5" name="Label" dataDxfId="39"/>
+    <tableColumn id="6" name="Collection" dataDxfId="38"/>
+    <tableColumn id="14" name="Attribute" dataDxfId="37">
       <calculatedColumnFormula>[Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Relation" dataDxfId="20"/>
-    <tableColumn id="11" name="Deep 1" dataDxfId="19"/>
-    <tableColumn id="12" name="Deep 2" dataDxfId="18"/>
-    <tableColumn id="13" name="Deep 3" dataDxfId="17"/>
+    <tableColumn id="10" name="Relation" dataDxfId="36"/>
+    <tableColumn id="11" name="Deep 1" dataDxfId="35"/>
+    <tableColumn id="12" name="Deep 2" dataDxfId="34"/>
+    <tableColumn id="13" name="Deep 3" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4645,10 +4750,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView topLeftCell="G31" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J37"/>
+    <sheetView tabSelected="1" topLeftCell="G31" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4708,7 +4813,7 @@
         <v>user</v>
       </c>
       <c r="D2" s="8" t="str">
-        <f t="shared" ref="D2:D37" si="0">"Milestone\Appframe\Model"</f>
+        <f t="shared" ref="D2:D38" si="0">"Milestone\Appframe\Model"</f>
         <v>Milestone\Appframe\Model</v>
       </c>
       <c r="E2" s="8" t="str">
@@ -6009,15 +6114,15 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="2" t="s">
-        <v>589</v>
+        <v>679</v>
       </c>
       <c r="B34" s="7" t="str">
         <f>"__"&amp;[Name]</f>
-        <v>__resource_form_layout</v>
+        <v>__resource_form_field_depends</v>
       </c>
       <c r="C34" s="7" t="str">
         <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
-        <v>resource_form_layout</v>
+        <v>resource_form_field_depend</v>
       </c>
       <c r="D34" s="7" t="str">
         <f>"Milestone\Appframe\Model"</f>
@@ -6025,40 +6130,40 @@
       </c>
       <c r="E34" s="8" t="str">
         <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
-        <v>ResourceFormLayout</v>
+        <v>ResourceFormFieldDepend</v>
       </c>
       <c r="F34" s="8" t="str">
         <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
-        <v>php artisan make:migration create___resource_form_layout_table --create=__resource_form_layout</v>
+        <v>php artisan make:migration create___resource_form_field_depends_table --create=__resource_form_field_depends</v>
       </c>
       <c r="G34" s="8" t="str">
         <f>"php artisan make:model "&amp;[Class Name]</f>
-        <v>php artisan make:model ResourceFormLayout</v>
+        <v>php artisan make:model ResourceFormFieldDepend</v>
       </c>
       <c r="H34" s="8" t="str">
         <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
-        <v>protected $table = '__resource_form_layout';</v>
+        <v>protected $table = '__resource_form_field_depends';</v>
       </c>
       <c r="I34" s="8" t="str">
         <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
-        <v>php artisan make:seed ResourceFormLayoutTableSeeder</v>
+        <v>php artisan make:seed ResourceFormFieldDependTableSeeder</v>
       </c>
       <c r="J34" s="8" t="str">
         <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
-        <v>ResourceFormLayoutTableSeeder::class,</v>
+        <v>ResourceFormFieldDependTableSeeder::class,</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="2" t="s">
-        <v>647</v>
+        <v>589</v>
       </c>
       <c r="B35" s="7" t="str">
         <f>"__"&amp;[Name]</f>
-        <v>__resource_form_collection</v>
+        <v>__resource_form_layout</v>
       </c>
       <c r="C35" s="7" t="str">
         <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
-        <v>resource_form_collection</v>
+        <v>resource_form_layout</v>
       </c>
       <c r="D35" s="7" t="str">
         <f>"Milestone\Appframe\Model"</f>
@@ -6066,81 +6171,81 @@
       </c>
       <c r="E35" s="8" t="str">
         <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
-        <v>ResourceFormCollection</v>
+        <v>ResourceFormLayout</v>
       </c>
       <c r="F35" s="8" t="str">
         <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
-        <v>php artisan make:migration create___resource_form_collection_table --create=__resource_form_collection</v>
+        <v>php artisan make:migration create___resource_form_layout_table --create=__resource_form_layout</v>
       </c>
       <c r="G35" s="8" t="str">
         <f>"php artisan make:model "&amp;[Class Name]</f>
-        <v>php artisan make:model ResourceFormCollection</v>
+        <v>php artisan make:model ResourceFormLayout</v>
       </c>
       <c r="H35" s="8" t="str">
         <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
-        <v>protected $table = '__resource_form_collection';</v>
+        <v>protected $table = '__resource_form_layout';</v>
       </c>
       <c r="I35" s="8" t="str">
         <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
-        <v>php artisan make:seed ResourceFormCollectionTableSeeder</v>
+        <v>php artisan make:seed ResourceFormLayoutTableSeeder</v>
       </c>
       <c r="J35" s="8" t="str">
         <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
-        <v>ResourceFormCollectionTableSeeder::class,</v>
+        <v>ResourceFormLayoutTableSeeder::class,</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="B36" s="7" t="str">
+        <f>"__"&amp;[Name]</f>
+        <v>__resource_form_collection</v>
+      </c>
+      <c r="C36" s="7" t="str">
+        <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
+        <v>resource_form_collection</v>
+      </c>
+      <c r="D36" s="7" t="str">
+        <f>"Milestone\Appframe\Model"</f>
+        <v>Milestone\Appframe\Model</v>
+      </c>
+      <c r="E36" s="8" t="str">
+        <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
+        <v>ResourceFormCollection</v>
+      </c>
+      <c r="F36" s="8" t="str">
+        <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
+        <v>php artisan make:migration create___resource_form_collection_table --create=__resource_form_collection</v>
+      </c>
+      <c r="G36" s="8" t="str">
+        <f>"php artisan make:model "&amp;[Class Name]</f>
+        <v>php artisan make:model ResourceFormCollection</v>
+      </c>
+      <c r="H36" s="8" t="str">
+        <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
+        <v>protected $table = '__resource_form_collection';</v>
+      </c>
+      <c r="I36" s="8" t="str">
+        <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
+        <v>php artisan make:seed ResourceFormCollectionTableSeeder</v>
+      </c>
+      <c r="J36" s="8" t="str">
+        <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
+        <v>ResourceFormCollectionTableSeeder::class,</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B36" s="9" t="str">
+      <c r="B37" s="9" t="str">
         <f>"__"&amp;[Name]</f>
         <v>__organisation</v>
       </c>
-      <c r="C36" s="9" t="str">
+      <c r="C37" s="9" t="str">
         <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
         <v>organisation</v>
-      </c>
-      <c r="D36" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Milestone\Appframe\Model</v>
-      </c>
-      <c r="E36" s="9" t="str">
-        <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
-        <v>Organisation</v>
-      </c>
-      <c r="F36" s="9" t="str">
-        <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
-        <v>php artisan make:migration create___organisation_table --create=__organisation</v>
-      </c>
-      <c r="G36" s="9" t="str">
-        <f>"php artisan make:model "&amp;[Class Name]</f>
-        <v>php artisan make:model Organisation</v>
-      </c>
-      <c r="H36" s="9" t="str">
-        <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
-        <v>protected $table = '__organisation';</v>
-      </c>
-      <c r="I36" s="9" t="str">
-        <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
-        <v>php artisan make:seed OrganisationTableSeeder</v>
-      </c>
-      <c r="J36" s="9" t="str">
-        <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
-        <v>OrganisationTableSeeder::class,</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10">
-      <c r="A37" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="B37" s="9" t="str">
-        <f>"__"&amp;[Name]</f>
-        <v>__organisation_contacts</v>
-      </c>
-      <c r="C37" s="9" t="str">
-        <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
-        <v>organisation_contact</v>
       </c>
       <c r="D37" s="9" t="str">
         <f t="shared" si="0"/>
@@ -6148,25 +6253,66 @@
       </c>
       <c r="E37" s="9" t="str">
         <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
-        <v>OrganisationContact</v>
+        <v>Organisation</v>
       </c>
       <c r="F37" s="9" t="str">
         <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
-        <v>php artisan make:migration create___organisation_contacts_table --create=__organisation_contacts</v>
+        <v>php artisan make:migration create___organisation_table --create=__organisation</v>
       </c>
       <c r="G37" s="9" t="str">
         <f>"php artisan make:model "&amp;[Class Name]</f>
-        <v>php artisan make:model OrganisationContact</v>
+        <v>php artisan make:model Organisation</v>
       </c>
       <c r="H37" s="9" t="str">
         <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
-        <v>protected $table = '__organisation_contacts';</v>
+        <v>protected $table = '__organisation';</v>
       </c>
       <c r="I37" s="9" t="str">
         <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
+        <v>php artisan make:seed OrganisationTableSeeder</v>
+      </c>
+      <c r="J37" s="9" t="str">
+        <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
+        <v>OrganisationTableSeeder::class,</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B38" s="9" t="str">
+        <f>"__"&amp;[Name]</f>
+        <v>__organisation_contacts</v>
+      </c>
+      <c r="C38" s="9" t="str">
+        <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
+        <v>organisation_contact</v>
+      </c>
+      <c r="D38" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>Milestone\Appframe\Model</v>
+      </c>
+      <c r="E38" s="9" t="str">
+        <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
+        <v>OrganisationContact</v>
+      </c>
+      <c r="F38" s="9" t="str">
+        <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
+        <v>php artisan make:migration create___organisation_contacts_table --create=__organisation_contacts</v>
+      </c>
+      <c r="G38" s="9" t="str">
+        <f>"php artisan make:model "&amp;[Class Name]</f>
+        <v>php artisan make:model OrganisationContact</v>
+      </c>
+      <c r="H38" s="9" t="str">
+        <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
+        <v>protected $table = '__organisation_contacts';</v>
+      </c>
+      <c r="I38" s="9" t="str">
+        <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
         <v>php artisan make:seed OrganisationContactTableSeeder</v>
       </c>
-      <c r="J37" s="9" t="str">
+      <c r="J38" s="9" t="str">
         <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
         <v>OrganisationContactTableSeeder::class,</v>
       </c>
@@ -7752,10 +7898,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I135"/>
+  <dimension ref="A1:I139"/>
   <sheetViews>
-    <sheetView topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="A136" sqref="A136"/>
+    <sheetView topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="B140" sqref="B140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="15"/>
@@ -10695,24 +10841,110 @@
       </c>
       <c r="I135" s="4"/>
     </row>
+    <row r="136" spans="1:9">
+      <c r="A136" s="4" t="s">
+        <v>680</v>
+      </c>
+      <c r="B136" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C136" s="4" t="s">
+        <v>681</v>
+      </c>
+      <c r="D136" s="4">
+        <v>64</v>
+      </c>
+      <c r="E136" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F136" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G136" s="4"/>
+      <c r="H136" s="4"/>
+      <c r="I136" s="4"/>
+    </row>
+    <row r="137" spans="1:9">
+      <c r="A137" s="4" t="s">
+        <v>682</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C137" s="4" t="s">
+        <v>683</v>
+      </c>
+      <c r="D137" s="4">
+        <v>64</v>
+      </c>
+      <c r="E137" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F137" s="4"/>
+      <c r="G137" s="4"/>
+      <c r="H137" s="4"/>
+      <c r="I137" s="4"/>
+    </row>
+    <row r="138" spans="1:9">
+      <c r="A138" s="4" t="s">
+        <v>684</v>
+      </c>
+      <c r="B138" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C138" s="4" t="s">
+        <v>685</v>
+      </c>
+      <c r="D138" s="4" t="s">
+        <v>686</v>
+      </c>
+      <c r="E138" s="4" t="s">
+        <v>687</v>
+      </c>
+      <c r="F138" s="4"/>
+      <c r="G138" s="4"/>
+      <c r="H138" s="4"/>
+      <c r="I138" s="4"/>
+    </row>
+    <row r="139" spans="1:9">
+      <c r="A139" s="4" t="s">
+        <v>688</v>
+      </c>
+      <c r="B139" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C139" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="D139" s="4">
+        <v>128</v>
+      </c>
+      <c r="E139" s="4"/>
+      <c r="F139" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G139" s="4"/>
+      <c r="H139" s="4"/>
+      <c r="I139" s="4"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A43:A46">
-    <cfRule type="duplicateValues" dxfId="111" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="115" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56:A59">
-    <cfRule type="duplicateValues" dxfId="110" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="114" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A135">
-    <cfRule type="duplicateValues" dxfId="109" priority="24"/>
+  <conditionalFormatting sqref="A2:A139">
+    <cfRule type="duplicateValues" dxfId="113" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A128:A129">
-    <cfRule type="duplicateValues" dxfId="108" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="112" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A128:A129">
-    <cfRule type="duplicateValues" dxfId="107" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="111" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A130:A131">
-    <cfRule type="duplicateValues" dxfId="106" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="110" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -10724,10 +10956,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K323"/>
+  <dimension ref="A1:K332"/>
   <sheetViews>
-    <sheetView topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="A324" sqref="A324"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K324" sqref="K324:K332"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="15"/>
@@ -16757,7 +16989,7 @@
         <v>$table-&gt;foreign('resource_action')-&gt;references('id')-&gt;on('__resource_actions')-&gt;onUpdate('cascade')-&gt;onDelete('cascade');</v>
       </c>
     </row>
-    <row r="138" spans="1:11" hidden="1">
+    <row r="138" spans="1:11">
       <c r="A138" s="4" t="s">
         <v>102</v>
       </c>
@@ -16801,7 +17033,7 @@
         <v>$table-&gt;increments('id');</v>
       </c>
     </row>
-    <row r="139" spans="1:11" hidden="1">
+    <row r="139" spans="1:11">
       <c r="A139" s="4" t="s">
         <v>102</v>
       </c>
@@ -16845,7 +17077,7 @@
         <v>$table-&gt;unsignedInteger('resource_form')-&gt;index();</v>
       </c>
     </row>
-    <row r="140" spans="1:11" hidden="1">
+    <row r="140" spans="1:11">
       <c r="A140" s="4" t="s">
         <v>102</v>
       </c>
@@ -16889,7 +17121,7 @@
         <v>$table-&gt;string('name', 64)-&gt;index();</v>
       </c>
     </row>
-    <row r="141" spans="1:11" hidden="1">
+    <row r="141" spans="1:11">
       <c r="A141" s="4" t="s">
         <v>102</v>
       </c>
@@ -16933,7 +17165,7 @@
         <v>$table-&gt;string('type', 128)-&gt;nullable();</v>
       </c>
     </row>
-    <row r="142" spans="1:11" hidden="1">
+    <row r="142" spans="1:11">
       <c r="A142" s="4" t="s">
         <v>102</v>
       </c>
@@ -16977,7 +17209,7 @@
         <v>$table-&gt;string('label', 256)-&gt;nullable();</v>
       </c>
     </row>
-    <row r="143" spans="1:11" hidden="1">
+    <row r="143" spans="1:11">
       <c r="A143" s="4" t="s">
         <v>102</v>
       </c>
@@ -17021,7 +17253,7 @@
         <v>$table-&gt;string('collection', 64)-&gt;nullable();</v>
       </c>
     </row>
-    <row r="144" spans="1:11" hidden="1">
+    <row r="144" spans="1:11">
       <c r="A144" s="4" t="s">
         <v>102</v>
       </c>
@@ -17065,7 +17297,7 @@
         <v>$table-&gt;timestamps();</v>
       </c>
     </row>
-    <row r="145" spans="1:11" hidden="1">
+    <row r="145" spans="1:11">
       <c r="A145" s="4" t="s">
         <v>102</v>
       </c>
@@ -17373,7 +17605,7 @@
         <v>$table-&gt;foreign('form_field')-&gt;references('id')-&gt;on('__resource_form_fields')-&gt;onUpdate('cascade')-&gt;onDelete('cascade');</v>
       </c>
     </row>
-    <row r="152" spans="1:11">
+    <row r="152" spans="1:11" hidden="1">
       <c r="A152" s="4" t="s">
         <v>104</v>
       </c>
@@ -17417,7 +17649,7 @@
         <v>$table-&gt;increments('id');</v>
       </c>
     </row>
-    <row r="153" spans="1:11">
+    <row r="153" spans="1:11" hidden="1">
       <c r="A153" s="4" t="s">
         <v>104</v>
       </c>
@@ -17461,7 +17693,7 @@
         <v>$table-&gt;unsignedInteger('form_field')-&gt;index();</v>
       </c>
     </row>
-    <row r="154" spans="1:11">
+    <row r="154" spans="1:11" hidden="1">
       <c r="A154" s="4" t="s">
         <v>104</v>
       </c>
@@ -17505,7 +17737,7 @@
         <v>$table-&gt;unsignedInteger('relation')-&gt;index()-&gt;nullable();</v>
       </c>
     </row>
-    <row r="155" spans="1:11">
+    <row r="155" spans="1:11" hidden="1">
       <c r="A155" s="4" t="s">
         <v>104</v>
       </c>
@@ -17549,7 +17781,7 @@
         <v>$table-&gt;unsignedInteger('nest_relation1')-&gt;index()-&gt;nullable();</v>
       </c>
     </row>
-    <row r="156" spans="1:11">
+    <row r="156" spans="1:11" hidden="1">
       <c r="A156" s="4" t="s">
         <v>104</v>
       </c>
@@ -17593,7 +17825,7 @@
         <v>$table-&gt;unsignedInteger('nest_relation2')-&gt;index()-&gt;nullable();</v>
       </c>
     </row>
-    <row r="157" spans="1:11">
+    <row r="157" spans="1:11" hidden="1">
       <c r="A157" s="4" t="s">
         <v>104</v>
       </c>
@@ -17637,7 +17869,7 @@
         <v>$table-&gt;unsignedInteger('nest_relation3')-&gt;index()-&gt;nullable();</v>
       </c>
     </row>
-    <row r="158" spans="1:11">
+    <row r="158" spans="1:11" hidden="1">
       <c r="A158" s="4" t="s">
         <v>104</v>
       </c>
@@ -17681,7 +17913,7 @@
         <v>$table-&gt;string('attribute', 64)-&gt;nullable();</v>
       </c>
     </row>
-    <row r="159" spans="1:11">
+    <row r="159" spans="1:11" hidden="1">
       <c r="A159" s="4" t="s">
         <v>104</v>
       </c>
@@ -17725,7 +17957,7 @@
         <v>$table-&gt;timestamps();</v>
       </c>
     </row>
-    <row r="160" spans="1:11">
+    <row r="160" spans="1:11" hidden="1">
       <c r="A160" s="4" t="s">
         <v>104</v>
       </c>
@@ -17769,7 +18001,7 @@
         <v>$table-&gt;foreign('form_field')-&gt;references('id')-&gt;on('__resource_form_fields')-&gt;onUpdate('cascade')-&gt;onDelete('cascade');</v>
       </c>
     </row>
-    <row r="161" spans="1:11">
+    <row r="161" spans="1:11" hidden="1">
       <c r="A161" s="4" t="s">
         <v>104</v>
       </c>
@@ -17813,7 +18045,7 @@
         <v>$table-&gt;foreign('relation')-&gt;references('id')-&gt;on('__resource_relations')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
       </c>
     </row>
-    <row r="162" spans="1:11">
+    <row r="162" spans="1:11" hidden="1">
       <c r="A162" s="4" t="s">
         <v>104</v>
       </c>
@@ -17857,7 +18089,7 @@
         <v>$table-&gt;foreign('nest_relation1')-&gt;references('id')-&gt;on('__resource_relations')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
       </c>
     </row>
-    <row r="163" spans="1:11">
+    <row r="163" spans="1:11" hidden="1">
       <c r="A163" s="4" t="s">
         <v>104</v>
       </c>
@@ -17901,7 +18133,7 @@
         <v>$table-&gt;foreign('nest_relation2')-&gt;references('id')-&gt;on('__resource_relations')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
       </c>
     </row>
-    <row r="164" spans="1:11">
+    <row r="164" spans="1:11" hidden="1">
       <c r="A164" s="4" t="s">
         <v>104</v>
       </c>
@@ -24369,7 +24601,7 @@
         <v>$table-&gt;foreign('foreign_field')-&gt;references('id')-&gt;on('__resource_form_fields')-&gt;onUpdate('cascade')-&gt;onDelete('cascade');</v>
       </c>
     </row>
-    <row r="311" spans="1:11">
+    <row r="311" spans="1:11" hidden="1">
       <c r="A311" s="4" t="s">
         <v>671</v>
       </c>
@@ -24413,7 +24645,7 @@
         <v>$table-&gt;increments('id');</v>
       </c>
     </row>
-    <row r="312" spans="1:11">
+    <row r="312" spans="1:11" hidden="1">
       <c r="A312" s="4" t="s">
         <v>671</v>
       </c>
@@ -24457,7 +24689,7 @@
         <v>$table-&gt;unsignedInteger('resource_list')-&gt;index();</v>
       </c>
     </row>
-    <row r="313" spans="1:11">
+    <row r="313" spans="1:11" hidden="1">
       <c r="A313" s="4" t="s">
         <v>671</v>
       </c>
@@ -24501,7 +24733,7 @@
         <v>$table-&gt;string('field', 64)-&gt;nullable();</v>
       </c>
     </row>
-    <row r="314" spans="1:11">
+    <row r="314" spans="1:11" hidden="1">
       <c r="A314" s="4" t="s">
         <v>671</v>
       </c>
@@ -24545,7 +24777,7 @@
         <v>$table-&gt;unsignedInteger('relation')-&gt;index()-&gt;nullable();</v>
       </c>
     </row>
-    <row r="315" spans="1:11">
+    <row r="315" spans="1:11" hidden="1">
       <c r="A315" s="4" t="s">
         <v>671</v>
       </c>
@@ -24589,7 +24821,7 @@
         <v>$table-&gt;unsignedInteger('nest_relation1')-&gt;index()-&gt;nullable();</v>
       </c>
     </row>
-    <row r="316" spans="1:11">
+    <row r="316" spans="1:11" hidden="1">
       <c r="A316" s="4" t="s">
         <v>671</v>
       </c>
@@ -24633,7 +24865,7 @@
         <v>$table-&gt;unsignedInteger('nest_relation2')-&gt;index()-&gt;nullable();</v>
       </c>
     </row>
-    <row r="317" spans="1:11">
+    <row r="317" spans="1:11" hidden="1">
       <c r="A317" s="4" t="s">
         <v>671</v>
       </c>
@@ -24677,7 +24909,7 @@
         <v>$table-&gt;unsignedInteger('nest_relation3')-&gt;index()-&gt;nullable();</v>
       </c>
     </row>
-    <row r="318" spans="1:11">
+    <row r="318" spans="1:11" hidden="1">
       <c r="A318" s="4" t="s">
         <v>671</v>
       </c>
@@ -24721,7 +24953,7 @@
         <v>$table-&gt;timestamps();</v>
       </c>
     </row>
-    <row r="319" spans="1:11">
+    <row r="319" spans="1:11" hidden="1">
       <c r="A319" s="4" t="s">
         <v>671</v>
       </c>
@@ -24765,7 +24997,7 @@
         <v>$table-&gt;foreign('resource_list')-&gt;references('id')-&gt;on('__resource_lists')-&gt;onUpdate('cascade')-&gt;onDelete('cascade');</v>
       </c>
     </row>
-    <row r="320" spans="1:11">
+    <row r="320" spans="1:11" hidden="1">
       <c r="A320" s="4" t="s">
         <v>671</v>
       </c>
@@ -24809,7 +25041,7 @@
         <v>$table-&gt;foreign('relation')-&gt;references('id')-&gt;on('__resource_relations')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
       </c>
     </row>
-    <row r="321" spans="1:11">
+    <row r="321" spans="1:11" hidden="1">
       <c r="A321" s="4" t="s">
         <v>671</v>
       </c>
@@ -24853,7 +25085,7 @@
         <v>$table-&gt;foreign('nest_relation1')-&gt;references('id')-&gt;on('__resource_relations')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
       </c>
     </row>
-    <row r="322" spans="1:11">
+    <row r="322" spans="1:11" hidden="1">
       <c r="A322" s="4" t="s">
         <v>671</v>
       </c>
@@ -24897,7 +25129,7 @@
         <v>$table-&gt;foreign('nest_relation2')-&gt;references('id')-&gt;on('__resource_relations')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
       </c>
     </row>
-    <row r="323" spans="1:11">
+    <row r="323" spans="1:11" hidden="1">
       <c r="A323" s="4" t="s">
         <v>671</v>
       </c>
@@ -24941,13 +25173,409 @@
         <v>$table-&gt;foreign('nest_relation3')-&gt;references('id')-&gt;on('__resource_relations')-&gt;onUpdate('cascade')-&gt;onDelete('set null');</v>
       </c>
     </row>
+    <row r="324" spans="1:11">
+      <c r="A324" s="4" t="s">
+        <v>679</v>
+      </c>
+      <c r="B324" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C324" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>increments(</v>
+      </c>
+      <c r="D324" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'id'</v>
+      </c>
+      <c r="E324" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>)</v>
+      </c>
+      <c r="F324" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v/>
+      </c>
+      <c r="G324" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v/>
+      </c>
+      <c r="H324" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v/>
+      </c>
+      <c r="I324" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v/>
+      </c>
+      <c r="J324" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K324" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;increments('id');</v>
+      </c>
+    </row>
+    <row r="325" spans="1:11">
+      <c r="A325" s="4" t="s">
+        <v>679</v>
+      </c>
+      <c r="B325" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C325" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>unsignedInteger(</v>
+      </c>
+      <c r="D325" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'form_field'</v>
+      </c>
+      <c r="E325" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>)</v>
+      </c>
+      <c r="F325" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>-&gt;index()</v>
+      </c>
+      <c r="G325" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v/>
+      </c>
+      <c r="H325" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v/>
+      </c>
+      <c r="I325" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v/>
+      </c>
+      <c r="J325" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K325" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;unsignedInteger('form_field')-&gt;index();</v>
+      </c>
+    </row>
+    <row r="326" spans="1:11">
+      <c r="A326" s="4" t="s">
+        <v>679</v>
+      </c>
+      <c r="B326" s="4" t="s">
+        <v>680</v>
+      </c>
+      <c r="C326" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>string(</v>
+      </c>
+      <c r="D326" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'depend_field'</v>
+      </c>
+      <c r="E326" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>, 64)</v>
+      </c>
+      <c r="F326" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>-&gt;index()</v>
+      </c>
+      <c r="G326" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v>-&gt;nullable()</v>
+      </c>
+      <c r="H326" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v/>
+      </c>
+      <c r="I326" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v/>
+      </c>
+      <c r="J326" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K326" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;string('depend_field', 64)-&gt;index()-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="327" spans="1:11">
+      <c r="A327" s="4" t="s">
+        <v>679</v>
+      </c>
+      <c r="B327" s="4" t="s">
+        <v>682</v>
+      </c>
+      <c r="C327" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>string(</v>
+      </c>
+      <c r="D327" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'db_field'</v>
+      </c>
+      <c r="E327" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>, 64)</v>
+      </c>
+      <c r="F327" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>-&gt;nullable()</v>
+      </c>
+      <c r="G327" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v/>
+      </c>
+      <c r="H327" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v/>
+      </c>
+      <c r="I327" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v/>
+      </c>
+      <c r="J327" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K327" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;string('db_field', 64)-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="328" spans="1:11">
+      <c r="A328" s="4" t="s">
+        <v>679</v>
+      </c>
+      <c r="B328" s="4" t="s">
+        <v>684</v>
+      </c>
+      <c r="C328" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>enum(</v>
+      </c>
+      <c r="D328" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'operator'</v>
+      </c>
+      <c r="E328" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>, ['=','&lt;','&gt;','&lt;=','&gt;=','&lt;&gt;','In','NotIn','like'])</v>
+      </c>
+      <c r="F328" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>-&gt;default('=')</v>
+      </c>
+      <c r="G328" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v/>
+      </c>
+      <c r="H328" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v/>
+      </c>
+      <c r="I328" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v/>
+      </c>
+      <c r="J328" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K328" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;enum('operator', ['=','&lt;','&gt;','&lt;=','&gt;=','&lt;&gt;','In','NotIn','like'])-&gt;default('=');</v>
+      </c>
+    </row>
+    <row r="329" spans="1:11">
+      <c r="A329" s="4" t="s">
+        <v>679</v>
+      </c>
+      <c r="B329" s="4" t="s">
+        <v>688</v>
+      </c>
+      <c r="C329" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>string(</v>
+      </c>
+      <c r="D329" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'compare_method'</v>
+      </c>
+      <c r="E329" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>, 128)</v>
+      </c>
+      <c r="F329" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v/>
+      </c>
+      <c r="G329" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v>-&gt;nullable()</v>
+      </c>
+      <c r="H329" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v/>
+      </c>
+      <c r="I329" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v/>
+      </c>
+      <c r="J329" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K329" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;string('compare_method', 128)-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="330" spans="1:11">
+      <c r="A330" s="4" t="s">
+        <v>679</v>
+      </c>
+      <c r="B330" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C330" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>string(</v>
+      </c>
+      <c r="D330" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'method'</v>
+      </c>
+      <c r="E330" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>, 128)</v>
+      </c>
+      <c r="F330" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>-&gt;nullable()</v>
+      </c>
+      <c r="G330" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v/>
+      </c>
+      <c r="H330" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v/>
+      </c>
+      <c r="I330" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v/>
+      </c>
+      <c r="J330" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K330" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;string('method', 128)-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="331" spans="1:11">
+      <c r="A331" s="4" t="s">
+        <v>679</v>
+      </c>
+      <c r="B331" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C331" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>timestamps(</v>
+      </c>
+      <c r="D331" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v/>
+      </c>
+      <c r="E331" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>)</v>
+      </c>
+      <c r="F331" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v/>
+      </c>
+      <c r="G331" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v/>
+      </c>
+      <c r="H331" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v/>
+      </c>
+      <c r="I331" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v/>
+      </c>
+      <c r="J331" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K331" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;timestamps();</v>
+      </c>
+    </row>
+    <row r="332" spans="1:11">
+      <c r="A332" s="4" t="s">
+        <v>679</v>
+      </c>
+      <c r="B332" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C332" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>foreign(</v>
+      </c>
+      <c r="D332" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'form_field'</v>
+      </c>
+      <c r="E332" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>)</v>
+      </c>
+      <c r="F332" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>-&gt;references('id')</v>
+      </c>
+      <c r="G332" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v>-&gt;on('__resource_form_fields')</v>
+      </c>
+      <c r="H332" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v>-&gt;onUpdate('cascade')</v>
+      </c>
+      <c r="I332" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v>-&gt;onDelete('cascade')</v>
+      </c>
+      <c r="J332" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K332" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;foreign('form_field')-&gt;references('id')-&gt;on('__resource_form_fields')-&gt;onUpdate('cascade')-&gt;onDelete('cascade');</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B323">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B332">
       <formula1>AvailableFields</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A323">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A332">
       <formula1>TableNames</formula1>
     </dataValidation>
   </dataValidations>
@@ -24961,10 +25589,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R307"/>
+  <dimension ref="A1:R310"/>
   <sheetViews>
     <sheetView topLeftCell="B291" workbookViewId="0">
-      <selection activeCell="C307" sqref="C307"/>
+      <selection activeCell="D310" sqref="D310:I310"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -36141,6 +36769,126 @@
       <c r="Q307" s="40"/>
       <c r="R307" s="40"/>
     </row>
+    <row r="308" spans="1:18">
+      <c r="A308" s="22" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Field Depends-0</v>
+      </c>
+      <c r="B308" s="40" t="s">
+        <v>690</v>
+      </c>
+      <c r="C308" s="22">
+        <f>COUNTIF($B$1:$B307,[Table Name])</f>
+        <v>0</v>
+      </c>
+      <c r="D308" s="40" t="s">
+        <v>122</v>
+      </c>
+      <c r="E308" s="40" t="s">
+        <v>681</v>
+      </c>
+      <c r="F308" s="40" t="s">
+        <v>683</v>
+      </c>
+      <c r="G308" s="40" t="s">
+        <v>685</v>
+      </c>
+      <c r="H308" s="40" t="s">
+        <v>689</v>
+      </c>
+      <c r="I308" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="J308" s="40"/>
+      <c r="K308" s="40"/>
+      <c r="L308" s="40"/>
+      <c r="M308" s="40"/>
+      <c r="N308" s="40"/>
+      <c r="O308" s="40"/>
+      <c r="P308" s="40"/>
+      <c r="Q308" s="40"/>
+      <c r="R308" s="40"/>
+    </row>
+    <row r="309" spans="1:18">
+      <c r="A309" s="22" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resources-32</v>
+      </c>
+      <c r="B309" s="40" t="s">
+        <v>220</v>
+      </c>
+      <c r="C309" s="22">
+        <f>COUNTIF($B$1:$B308,[Table Name])</f>
+        <v>32</v>
+      </c>
+      <c r="D309" s="40" t="s">
+        <v>691</v>
+      </c>
+      <c r="E309" s="40" t="s">
+        <v>692</v>
+      </c>
+      <c r="F309" s="40" t="s">
+        <v>693</v>
+      </c>
+      <c r="G309" s="40" t="s">
+        <v>558</v>
+      </c>
+      <c r="H309" s="40" t="s">
+        <v>694</v>
+      </c>
+      <c r="I309" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="J309" s="40"/>
+      <c r="K309" s="40"/>
+      <c r="L309" s="40"/>
+      <c r="M309" s="40"/>
+      <c r="N309" s="40"/>
+      <c r="O309" s="40"/>
+      <c r="P309" s="40"/>
+      <c r="Q309" s="40"/>
+      <c r="R309" s="40"/>
+    </row>
+    <row r="310" spans="1:18">
+      <c r="A310" s="22" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resource Relations-45</v>
+      </c>
+      <c r="B310" s="40" t="s">
+        <v>441</v>
+      </c>
+      <c r="C310" s="22">
+        <f>COUNTIF($B$1:$B309,[Table Name])</f>
+        <v>45</v>
+      </c>
+      <c r="D310" s="40">
+        <v>13</v>
+      </c>
+      <c r="E310" s="40" t="s">
+        <v>695</v>
+      </c>
+      <c r="F310" s="40" t="s">
+        <v>696</v>
+      </c>
+      <c r="G310" s="40" t="s">
+        <v>697</v>
+      </c>
+      <c r="H310" s="40" t="s">
+        <v>310</v>
+      </c>
+      <c r="I310" s="40">
+        <v>32</v>
+      </c>
+      <c r="J310" s="40"/>
+      <c r="K310" s="40"/>
+      <c r="L310" s="40"/>
+      <c r="M310" s="40"/>
+      <c r="N310" s="40"/>
+      <c r="O310" s="40"/>
+      <c r="P310" s="40"/>
+      <c r="Q310" s="40"/>
+      <c r="R310" s="40"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
@@ -36152,10 +36900,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -36786,12 +37534,32 @@
         <v>truncate</v>
       </c>
     </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="4" t="s">
+        <v>690</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>679</v>
+      </c>
+      <c r="C32" s="4" t="str">
+        <f>VLOOKUP([FW Table Name],Tables[],4,0)</f>
+        <v>Milestone\Appframe\Model</v>
+      </c>
+      <c r="D32" s="4" t="str">
+        <f>VLOOKUP([FW Table Name],Tables[],5,0)</f>
+        <v>ResourceFormFieldDepend</v>
+      </c>
+      <c r="E32" s="7" t="str">
+        <f>"truncate"</f>
+        <v>truncate</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E32">
       <formula1>"truncate,query"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B32">
       <formula1>TableNames</formula1>
     </dataValidation>
   </dataValidations>
@@ -36805,10 +37573,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32:G32"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -37566,14 +38334,14 @@
         <v>441</v>
       </c>
       <c r="E27" s="7" t="str">
-        <f>"Milestone\Appframe\Model"</f>
+        <f t="shared" ref="E27:E32" si="9">"Milestone\Appframe\Model"</f>
         <v>Milestone\Appframe\Model</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>570</v>
       </c>
       <c r="G27" s="21" t="str">
-        <f>"id"</f>
+        <f t="shared" ref="G27:G32" si="10">"id"</f>
         <v>id</v>
       </c>
       <c r="H27" s="4"/>
@@ -37594,14 +38362,14 @@
         <v>595</v>
       </c>
       <c r="E28" s="7" t="str">
-        <f>"Milestone\Appframe\Model"</f>
+        <f t="shared" si="9"/>
         <v>Milestone\Appframe\Model</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>596</v>
       </c>
       <c r="G28" s="21" t="str">
-        <f>"id"</f>
+        <f t="shared" si="10"/>
         <v>id</v>
       </c>
       <c r="H28" s="4"/>
@@ -37622,14 +38390,14 @@
         <v>607</v>
       </c>
       <c r="E29" s="7" t="str">
-        <f>"Milestone\Appframe\Model"</f>
+        <f t="shared" si="9"/>
         <v>Milestone\Appframe\Model</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>608</v>
       </c>
       <c r="G29" s="21" t="str">
-        <f>"id"</f>
+        <f t="shared" si="10"/>
         <v>id</v>
       </c>
       <c r="H29" s="4"/>
@@ -37650,14 +38418,14 @@
         <v>614</v>
       </c>
       <c r="E30" s="7" t="str">
-        <f>"Milestone\Appframe\Model"</f>
+        <f t="shared" si="9"/>
         <v>Milestone\Appframe\Model</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>615</v>
       </c>
       <c r="G30" s="21" t="str">
-        <f>"id"</f>
+        <f t="shared" si="10"/>
         <v>id</v>
       </c>
       <c r="H30" s="4"/>
@@ -37678,14 +38446,14 @@
         <v>652</v>
       </c>
       <c r="E31" s="7" t="str">
-        <f>"Milestone\Appframe\Model"</f>
+        <f t="shared" si="9"/>
         <v>Milestone\Appframe\Model</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>653</v>
       </c>
       <c r="G31" s="21" t="str">
-        <f>"id"</f>
+        <f t="shared" si="10"/>
         <v>id</v>
       </c>
       <c r="H31" s="4"/>
@@ -37706,22 +38474,50 @@
         <v>675</v>
       </c>
       <c r="E32" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>Milestone\Appframe\Model</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>676</v>
+      </c>
+      <c r="G32" s="21" t="str">
+        <f t="shared" si="10"/>
+        <v>id</v>
+      </c>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="20">
+        <f>IFERROR($A32+1,1)</f>
+        <v>32</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>691</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>692</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>693</v>
+      </c>
+      <c r="E33" s="7" t="str">
         <f>"Milestone\Appframe\Model"</f>
         <v>Milestone\Appframe\Model</v>
       </c>
-      <c r="F32" s="4" t="s">
-        <v>676</v>
-      </c>
-      <c r="G32" s="21" t="str">
+      <c r="F33" s="4" t="s">
+        <v>694</v>
+      </c>
+      <c r="G33" s="21" t="str">
         <f>"id"</f>
         <v>id</v>
       </c>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F33">
       <formula1>ActualTableNames</formula1>
     </dataValidation>
   </dataValidations>
@@ -37734,10 +38530,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45:I45"/>
+      <selection activeCell="D46" sqref="D46:I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -39193,9 +39989,41 @@
         <v>31</v>
       </c>
     </row>
+    <row r="46" spans="1:9">
+      <c r="A46" s="20">
+        <f>IFERROR($A45+1,1)</f>
+        <v>45</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>691</v>
+      </c>
+      <c r="D46" s="7">
+        <f>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</f>
+        <v>13</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>695</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>696</v>
+      </c>
+      <c r="G46" s="22" t="s">
+        <v>697</v>
+      </c>
+      <c r="H46" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="I46" s="41">
+        <f>VLOOKUP([Relate Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</f>
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C45">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C46">
       <formula1>Resources</formula1>
     </dataValidation>
   </dataValidations>
@@ -39211,8 +40039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:R55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -42724,31 +43552,31 @@
       </c>
       <c r="B53" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>;</v>
+        <v>-&gt;create([</v>
       </c>
       <c r="C53" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '13', </v>
       </c>
       <c r="D53" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Depending Fields', </v>
       </c>
       <c r="E53" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Dependent fields', </v>
       </c>
       <c r="F53" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Depends', </v>
       </c>
       <c r="G53" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H53" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '32', </v>
       </c>
       <c r="I53" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -42788,7 +43616,7 @@
       </c>
       <c r="R53" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="54" spans="1:18">
@@ -42797,7 +43625,7 @@
       </c>
       <c r="B54" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
+        <v>;</v>
       </c>
       <c r="C54" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -42870,7 +43698,7 @@
       </c>
       <c r="B55" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
       </c>
       <c r="C55" s="33" t="str">
         <f t="shared" ca="1" si="3"/>

</xml_diff>

<commit_message>
ignore_null field have added to resource_form_field_depends table
</commit_message>
<xml_diff>
--- a/Helper.xlsx
+++ b/Helper.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Tables" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3407" uniqueCount="698">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3415" uniqueCount="700">
   <si>
     <t>resource_scopes</t>
   </si>
@@ -2132,6 +2132,12 @@
   </si>
   <si>
     <t>Depends</t>
+  </si>
+  <si>
+    <t>form_field_depend_ignore_null</t>
+  </si>
+  <si>
+    <t>ignore_null</t>
   </si>
 </sst>
 </file>
@@ -2361,7 +2367,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="127">
+  <dxfs count="124">
     <dxf>
       <font>
         <condense val="0"/>
@@ -2373,199 +2379,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -3885,6 +3698,163 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -4183,35 +4153,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tables" displayName="Tables" ref="A1:J38" totalsRowShown="0" dataDxfId="126">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tables" displayName="Tables" ref="A1:J38" totalsRowShown="0" dataDxfId="123">
   <autoFilter ref="A1:J38"/>
   <tableColumns count="10">
-    <tableColumn id="2" name="Name" dataDxfId="125"/>
-    <tableColumn id="10" name="Table" dataDxfId="124">
+    <tableColumn id="2" name="Name" dataDxfId="122"/>
+    <tableColumn id="10" name="Table" dataDxfId="121">
       <calculatedColumnFormula>"__"&amp;[Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Singular Name" dataDxfId="123">
+    <tableColumn id="5" name="Singular Name" dataDxfId="120">
       <calculatedColumnFormula>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Model NS" dataDxfId="122">
+    <tableColumn id="8" name="Model NS" dataDxfId="119">
       <calculatedColumnFormula>"Milestone\Appframe\Model"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Class Name" dataDxfId="121">
+    <tableColumn id="4" name="Class Name" dataDxfId="118">
       <calculatedColumnFormula>SUBSTITUTE(PROPER([Singular Name]),"_","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Migration Artisan" dataDxfId="120">
+    <tableColumn id="1" name="Migration Artisan" dataDxfId="117">
       <calculatedColumnFormula>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Model Artisan" dataDxfId="119">
+    <tableColumn id="6" name="Model Artisan" dataDxfId="116">
       <calculatedColumnFormula>"php artisan make:model "&amp;[Class Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Model Statement" dataDxfId="118">
+    <tableColumn id="3" name="Model Statement" dataDxfId="115">
       <calculatedColumnFormula>"protected $table = '"&amp;[Table]&amp;"';"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Seeder Artisan" dataDxfId="117">
+    <tableColumn id="7" name="Seeder Artisan" dataDxfId="114">
       <calculatedColumnFormula>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Seeder Class" dataDxfId="116">
+    <tableColumn id="9" name="Seeder Class" dataDxfId="113">
       <calculatedColumnFormula>[Class Name]&amp;"TableSeeder"&amp;"::class,"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4220,57 +4190,57 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="ResourceActions" displayName="ResourceActions" ref="A1:P9" totalsRowShown="0" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="ResourceActions" displayName="ResourceActions" ref="A1:P9" totalsRowShown="0" dataDxfId="17">
   <autoFilter ref="A1:P9"/>
   <tableColumns count="16">
-    <tableColumn id="1" name="No" dataDxfId="31">
+    <tableColumn id="1" name="No" dataDxfId="16">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Resource" dataDxfId="30"/>
-    <tableColumn id="13" name="Resource Id" dataDxfId="29">
+    <tableColumn id="2" name="Resource" dataDxfId="15"/>
+    <tableColumn id="13" name="Resource Id" dataDxfId="14">
       <calculatedColumnFormula>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Action Name" dataDxfId="28"/>
-    <tableColumn id="4" name="Description" dataDxfId="27"/>
-    <tableColumn id="5" name="Action Title" dataDxfId="26"/>
-    <tableColumn id="6" name="Button Type" dataDxfId="25"/>
-    <tableColumn id="7" name="Menu" dataDxfId="24"/>
-    <tableColumn id="8" name="Icon" dataDxfId="23"/>
-    <tableColumn id="9" name="Set" dataDxfId="22"/>
-    <tableColumn id="14" name="Action Type" dataDxfId="21"/>
-    <tableColumn id="15" name="ID1" dataDxfId="20"/>
-    <tableColumn id="16" name="ID2" dataDxfId="19"/>
-    <tableColumn id="10" name="On" dataDxfId="18"/>
-    <tableColumn id="11" name="Confirm" dataDxfId="17"/>
-    <tableColumn id="12" name="handler" dataDxfId="16"/>
+    <tableColumn id="3" name="Action Name" dataDxfId="13"/>
+    <tableColumn id="4" name="Description" dataDxfId="12"/>
+    <tableColumn id="5" name="Action Title" dataDxfId="11"/>
+    <tableColumn id="6" name="Button Type" dataDxfId="10"/>
+    <tableColumn id="7" name="Menu" dataDxfId="9"/>
+    <tableColumn id="8" name="Icon" dataDxfId="8"/>
+    <tableColumn id="9" name="Set" dataDxfId="7"/>
+    <tableColumn id="14" name="Action Type" dataDxfId="6"/>
+    <tableColumn id="15" name="ID1" dataDxfId="5"/>
+    <tableColumn id="16" name="ID2" dataDxfId="4"/>
+    <tableColumn id="10" name="On" dataDxfId="3"/>
+    <tableColumn id="11" name="Confirm" dataDxfId="2"/>
+    <tableColumn id="12" name="handler" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Columns" displayName="Columns" ref="A1:I139" totalsRowShown="0" dataDxfId="109">
-  <autoFilter ref="A1:I139">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Columns" displayName="Columns" ref="A1:I140" totalsRowShown="0" dataDxfId="106">
+  <autoFilter ref="A1:I140">
     <filterColumn colId="0"/>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" name="Column" dataDxfId="108"/>
-    <tableColumn id="2" name="Type" dataDxfId="107"/>
-    <tableColumn id="3" name="Name" dataDxfId="106"/>
-    <tableColumn id="4" name="Length/Enum" dataDxfId="105"/>
-    <tableColumn id="5" name="Method1" dataDxfId="104"/>
-    <tableColumn id="6" name="Method2" dataDxfId="103"/>
-    <tableColumn id="7" name="Method3" dataDxfId="102"/>
-    <tableColumn id="8" name="Method4" dataDxfId="101"/>
-    <tableColumn id="9" name="Method5" dataDxfId="100"/>
+    <tableColumn id="1" name="Column" dataDxfId="105"/>
+    <tableColumn id="2" name="Type" dataDxfId="104"/>
+    <tableColumn id="3" name="Name" dataDxfId="103"/>
+    <tableColumn id="4" name="Length/Enum" dataDxfId="102"/>
+    <tableColumn id="5" name="Method1" dataDxfId="101"/>
+    <tableColumn id="6" name="Method2" dataDxfId="100"/>
+    <tableColumn id="7" name="Method3" dataDxfId="99"/>
+    <tableColumn id="8" name="Method4" dataDxfId="98"/>
+    <tableColumn id="9" name="Method5" dataDxfId="97"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TableFields" displayName="TableFields" ref="A1:K332" totalsRowShown="0" dataDxfId="4">
-  <autoFilter ref="A1:K332">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TableFields" displayName="TableFields" ref="A1:K333" totalsRowShown="0" dataDxfId="96">
+  <autoFilter ref="A1:K333">
     <filterColumn colId="0">
       <filters>
         <filter val="resource_form_field_depends"/>
@@ -4279,33 +4249,33 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="11">
-    <tableColumn id="2" name="Table" dataDxfId="15"/>
-    <tableColumn id="3" name="Field" dataDxfId="14"/>
-    <tableColumn id="5" name="Type" dataDxfId="13">
+    <tableColumn id="2" name="Table" dataDxfId="95"/>
+    <tableColumn id="3" name="Field" dataDxfId="94"/>
+    <tableColumn id="5" name="Type" dataDxfId="93">
       <calculatedColumnFormula>VLOOKUP([Field],Columns[],2,0)&amp;"("</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Name" dataDxfId="12">
+    <tableColumn id="4" name="Name" dataDxfId="92">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Arg2" dataDxfId="11">
+    <tableColumn id="6" name="Arg2" dataDxfId="91">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Method1" dataDxfId="10">
+    <tableColumn id="7" name="Method1" dataDxfId="90">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Method2" dataDxfId="9">
+    <tableColumn id="8" name="Method2" dataDxfId="89">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Method3" dataDxfId="8">
+    <tableColumn id="9" name="Method3" dataDxfId="88">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Method4" dataDxfId="7">
+    <tableColumn id="10" name="Method4" dataDxfId="87">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Method5" dataDxfId="6">
+    <tableColumn id="11" name="Method5" dataDxfId="86">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Statement" dataDxfId="5">
+    <tableColumn id="12" name="Statement" dataDxfId="85">
       <calculatedColumnFormula>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4314,7 +4284,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R310" totalsRowShown="0" headerRowDxfId="99" dataDxfId="98">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R310" totalsRowShown="0" headerRowDxfId="84" dataDxfId="83">
   <autoFilter ref="A1:R310">
     <filterColumn colId="1">
       <filters>
@@ -4323,46 +4293,46 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="18">
-    <tableColumn id="19" name="TRCode" dataDxfId="97">
+    <tableColumn id="19" name="TRCode" dataDxfId="82">
       <calculatedColumnFormula>[Table Name]&amp;"-"&amp;[Record No]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Table Name" dataDxfId="96"/>
-    <tableColumn id="2" name="Record No" dataDxfId="95">
+    <tableColumn id="1" name="Table Name" dataDxfId="81"/>
+    <tableColumn id="2" name="Record No" dataDxfId="80">
       <calculatedColumnFormula>COUNTIF($B$1:$B1,[Table Name])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="1" dataDxfId="94"/>
-    <tableColumn id="4" name="2" dataDxfId="93"/>
-    <tableColumn id="5" name="3" dataDxfId="92"/>
-    <tableColumn id="6" name="4" dataDxfId="91"/>
-    <tableColumn id="7" name="5" dataDxfId="90"/>
-    <tableColumn id="8" name="6" dataDxfId="89"/>
-    <tableColumn id="9" name="7" dataDxfId="88"/>
-    <tableColumn id="10" name="8" dataDxfId="87"/>
-    <tableColumn id="11" name="9" dataDxfId="86"/>
-    <tableColumn id="12" name="10" dataDxfId="85"/>
-    <tableColumn id="13" name="11" dataDxfId="84"/>
-    <tableColumn id="14" name="12" dataDxfId="83"/>
-    <tableColumn id="15" name="13" dataDxfId="82"/>
-    <tableColumn id="16" name="14" dataDxfId="81"/>
-    <tableColumn id="17" name="15" dataDxfId="80"/>
+    <tableColumn id="3" name="1" dataDxfId="79"/>
+    <tableColumn id="4" name="2" dataDxfId="78"/>
+    <tableColumn id="5" name="3" dataDxfId="77"/>
+    <tableColumn id="6" name="4" dataDxfId="76"/>
+    <tableColumn id="7" name="5" dataDxfId="75"/>
+    <tableColumn id="8" name="6" dataDxfId="74"/>
+    <tableColumn id="9" name="7" dataDxfId="73"/>
+    <tableColumn id="10" name="8" dataDxfId="72"/>
+    <tableColumn id="11" name="9" dataDxfId="71"/>
+    <tableColumn id="12" name="10" dataDxfId="70"/>
+    <tableColumn id="13" name="11" dataDxfId="69"/>
+    <tableColumn id="14" name="12" dataDxfId="68"/>
+    <tableColumn id="15" name="13" dataDxfId="67"/>
+    <tableColumn id="16" name="14" dataDxfId="66"/>
+    <tableColumn id="17" name="15" dataDxfId="65"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SeedMap" displayName="SeedMap" ref="A1:E32" totalsRowShown="0" dataDxfId="79">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SeedMap" displayName="SeedMap" ref="A1:E32" totalsRowShown="0" dataDxfId="64">
   <autoFilter ref="A1:E32"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Name" dataDxfId="78"/>
-    <tableColumn id="3" name="FW Table Name" dataDxfId="77"/>
-    <tableColumn id="20" name="NS" dataDxfId="76">
+    <tableColumn id="1" name="Name" dataDxfId="63"/>
+    <tableColumn id="3" name="FW Table Name" dataDxfId="62"/>
+    <tableColumn id="20" name="NS" dataDxfId="61">
       <calculatedColumnFormula>VLOOKUP([FW Table Name],Tables[],4,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="Model" dataDxfId="75">
+    <tableColumn id="21" name="Model" dataDxfId="60">
       <calculatedColumnFormula>VLOOKUP([FW Table Name],Tables[],5,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Query Method" dataDxfId="74">
+    <tableColumn id="4" name="Query Method" dataDxfId="59">
       <calculatedColumnFormula>"truncate"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4371,46 +4341,46 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="ResourceTable" displayName="ResourceTable" ref="A1:I33" totalsRowShown="0" dataDxfId="73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="ResourceTable" displayName="ResourceTable" ref="A1:I33" totalsRowShown="0" dataDxfId="58">
   <autoFilter ref="A1:I33"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="No" dataDxfId="72">
+    <tableColumn id="1" name="No" dataDxfId="57">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Name" dataDxfId="71"/>
-    <tableColumn id="3" name="Description" dataDxfId="70"/>
-    <tableColumn id="4" name="Title" dataDxfId="69"/>
-    <tableColumn id="5" name="NS" dataDxfId="68">
+    <tableColumn id="2" name="Name" dataDxfId="56"/>
+    <tableColumn id="3" name="Description" dataDxfId="55"/>
+    <tableColumn id="4" name="Title" dataDxfId="54"/>
+    <tableColumn id="5" name="NS" dataDxfId="53">
       <calculatedColumnFormula>"Milestone\Appframe\Model"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Table" dataDxfId="67"/>
-    <tableColumn id="7" name="Key" dataDxfId="66">
+    <tableColumn id="6" name="Table" dataDxfId="52"/>
+    <tableColumn id="7" name="Key" dataDxfId="51">
       <calculatedColumnFormula>"id"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Controller" dataDxfId="65"/>
-    <tableColumn id="9" name="Controller NS" dataDxfId="64"/>
+    <tableColumn id="8" name="Controller" dataDxfId="50"/>
+    <tableColumn id="9" name="Controller NS" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RelationTable" displayName="RelationTable" ref="A1:I46" totalsRowShown="0" dataDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RelationTable" displayName="RelationTable" ref="A1:I46" totalsRowShown="0" dataDxfId="48">
   <autoFilter ref="A1:I46"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="No" dataDxfId="62">
+    <tableColumn id="1" name="No" dataDxfId="47">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Resource" dataDxfId="61"/>
-    <tableColumn id="4" name="Relate Resource" dataDxfId="60"/>
-    <tableColumn id="2" name="Resource Id" dataDxfId="59">
+    <tableColumn id="3" name="Resource" dataDxfId="46"/>
+    <tableColumn id="4" name="Relate Resource" dataDxfId="45"/>
+    <tableColumn id="2" name="Resource Id" dataDxfId="44">
       <calculatedColumnFormula>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Name" dataDxfId="58"/>
-    <tableColumn id="6" name="Description" dataDxfId="57"/>
-    <tableColumn id="7" name="Method" dataDxfId="56"/>
-    <tableColumn id="8" name="Type" dataDxfId="55"/>
-    <tableColumn id="10" name="Relate Id" dataDxfId="54">
+    <tableColumn id="5" name="Name" dataDxfId="43"/>
+    <tableColumn id="6" name="Description" dataDxfId="42"/>
+    <tableColumn id="7" name="Method" dataDxfId="41"/>
+    <tableColumn id="8" name="Type" dataDxfId="40"/>
+    <tableColumn id="10" name="Relate Id" dataDxfId="39">
       <calculatedColumnFormula>VLOOKUP([Relate Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4419,47 +4389,47 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="ResourceForms" displayName="ResourceForms" ref="A1:G9" totalsRowShown="0" dataDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="ResourceForms" displayName="ResourceForms" ref="A1:G9" totalsRowShown="0" dataDxfId="38">
   <autoFilter ref="A1:G9"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="No" dataDxfId="52">
+    <tableColumn id="1" name="No" dataDxfId="37">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Resource ID" dataDxfId="51"/>
-    <tableColumn id="3" name="Resource Name" dataDxfId="50">
+    <tableColumn id="2" name="Resource ID" dataDxfId="36"/>
+    <tableColumn id="3" name="Resource Name" dataDxfId="35">
       <calculatedColumnFormula>VLOOKUP([Resource ID],ResourceTable[],2,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Form Name" dataDxfId="49"/>
-    <tableColumn id="6" name="Title" dataDxfId="48"/>
-    <tableColumn id="7" name="Action Text" dataDxfId="47"/>
-    <tableColumn id="8" name="Description" dataDxfId="46"/>
+    <tableColumn id="4" name="Form Name" dataDxfId="34"/>
+    <tableColumn id="6" name="Title" dataDxfId="33"/>
+    <tableColumn id="7" name="Action Text" dataDxfId="32"/>
+    <tableColumn id="8" name="Description" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="FormFields" displayName="FormFields" ref="A1:L33" totalsRowShown="0" dataDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="FormFields" displayName="FormFields" ref="A1:L33" totalsRowShown="0" dataDxfId="30">
   <autoFilter ref="A1:L33"/>
   <tableColumns count="12">
-    <tableColumn id="9" name="No" dataDxfId="44">
+    <tableColumn id="9" name="No" dataDxfId="29">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Form Id" dataDxfId="43"/>
-    <tableColumn id="7" name="Form Name" dataDxfId="42">
+    <tableColumn id="1" name="Form Id" dataDxfId="28"/>
+    <tableColumn id="7" name="Form Name" dataDxfId="27">
       <calculatedColumnFormula>VLOOKUP([Form Id],ResourceForms[],4,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Name" dataDxfId="41"/>
-    <tableColumn id="2" name="Type" dataDxfId="40"/>
-    <tableColumn id="5" name="Label" dataDxfId="39"/>
-    <tableColumn id="6" name="Collection" dataDxfId="38"/>
-    <tableColumn id="14" name="Attribute" dataDxfId="37">
+    <tableColumn id="4" name="Name" dataDxfId="26"/>
+    <tableColumn id="2" name="Type" dataDxfId="25"/>
+    <tableColumn id="5" name="Label" dataDxfId="24"/>
+    <tableColumn id="6" name="Collection" dataDxfId="23"/>
+    <tableColumn id="14" name="Attribute" dataDxfId="22">
       <calculatedColumnFormula>[Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Relation" dataDxfId="36"/>
-    <tableColumn id="11" name="Deep 1" dataDxfId="35"/>
-    <tableColumn id="12" name="Deep 2" dataDxfId="34"/>
-    <tableColumn id="13" name="Deep 3" dataDxfId="33"/>
+    <tableColumn id="10" name="Relation" dataDxfId="21"/>
+    <tableColumn id="11" name="Deep 1" dataDxfId="20"/>
+    <tableColumn id="12" name="Deep 2" dataDxfId="19"/>
+    <tableColumn id="13" name="Deep 3" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4752,8 +4722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G31" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7898,10 +7868,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I139"/>
+  <dimension ref="A1:I140"/>
   <sheetViews>
     <sheetView topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="B140" sqref="B140"/>
+      <selection activeCell="A140" sqref="A140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="15"/>
@@ -10927,24 +10897,45 @@
       <c r="H139" s="4"/>
       <c r="I139" s="4"/>
     </row>
+    <row r="140" spans="1:9">
+      <c r="A140" s="4" t="s">
+        <v>698</v>
+      </c>
+      <c r="B140" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C140" s="4" t="s">
+        <v>699</v>
+      </c>
+      <c r="D140" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="E140" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="F140" s="4"/>
+      <c r="G140" s="4"/>
+      <c r="H140" s="4"/>
+      <c r="I140" s="4"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A43:A46">
-    <cfRule type="duplicateValues" dxfId="115" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="112" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56:A59">
-    <cfRule type="duplicateValues" dxfId="114" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="111" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A139">
-    <cfRule type="duplicateValues" dxfId="113" priority="24"/>
+  <conditionalFormatting sqref="A2:A140">
+    <cfRule type="duplicateValues" dxfId="110" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A128:A129">
-    <cfRule type="duplicateValues" dxfId="112" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="109" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A128:A129">
-    <cfRule type="duplicateValues" dxfId="111" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="108" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A130:A131">
-    <cfRule type="duplicateValues" dxfId="110" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="107" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -10956,10 +10947,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K332"/>
+  <dimension ref="A1:K333"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K324" sqref="K324:K332"/>
+      <selection activeCell="K324" sqref="K324:K333"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="15"/>
@@ -25481,28 +25472,28 @@
         <v>$table-&gt;string('method', 128)-&gt;nullable();</v>
       </c>
     </row>
-    <row r="331" spans="1:11">
+    <row r="331" spans="1:11" s="26" customFormat="1">
       <c r="A331" s="4" t="s">
         <v>679</v>
       </c>
       <c r="B331" s="4" t="s">
-        <v>40</v>
+        <v>698</v>
       </c>
       <c r="C331" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>timestamps(</v>
+        <v>enum(</v>
       </c>
       <c r="D331" s="4" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v/>
+        <v>'ignore_null'</v>
       </c>
       <c r="E331" s="7" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>)</v>
+        <v>, ['Yes','No'])</v>
       </c>
       <c r="F331" s="4" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v/>
+        <v>-&gt;default('Yes')</v>
       </c>
       <c r="G331" s="4" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
@@ -25522,7 +25513,7 @@
       </c>
       <c r="K331" s="4" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;timestamps();</v>
+        <v>$table-&gt;enum('ignore_null', ['Yes','No'])-&gt;default('Yes');</v>
       </c>
     </row>
     <row r="332" spans="1:11">
@@ -25530,15 +25521,15 @@
         <v>679</v>
       </c>
       <c r="B332" s="4" t="s">
-        <v>123</v>
+        <v>40</v>
       </c>
       <c r="C332" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>foreign(</v>
+        <v>timestamps(</v>
       </c>
       <c r="D332" s="4" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'form_field'</v>
+        <v/>
       </c>
       <c r="E332" s="7" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -25546,25 +25537,69 @@
       </c>
       <c r="F332" s="4" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;references('id')</v>
+        <v/>
       </c>
       <c r="G332" s="4" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v>-&gt;on('__resource_form_fields')</v>
+        <v/>
       </c>
       <c r="H332" s="4" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
-        <v>-&gt;onUpdate('cascade')</v>
+        <v/>
       </c>
       <c r="I332" s="4" t="str">
         <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
-        <v>-&gt;onDelete('cascade')</v>
+        <v/>
       </c>
       <c r="J332" s="4" t="str">
         <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
         <v/>
       </c>
       <c r="K332" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;timestamps();</v>
+      </c>
+    </row>
+    <row r="333" spans="1:11">
+      <c r="A333" s="4" t="s">
+        <v>679</v>
+      </c>
+      <c r="B333" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C333" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>foreign(</v>
+      </c>
+      <c r="D333" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'form_field'</v>
+      </c>
+      <c r="E333" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>)</v>
+      </c>
+      <c r="F333" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>-&gt;references('id')</v>
+      </c>
+      <c r="G333" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v>-&gt;on('__resource_form_fields')</v>
+      </c>
+      <c r="H333" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v>-&gt;onUpdate('cascade')</v>
+      </c>
+      <c r="I333" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v>-&gt;onDelete('cascade')</v>
+      </c>
+      <c r="J333" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K333" s="4" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
         <v>$table-&gt;foreign('form_field')-&gt;references('id')-&gt;on('__resource_form_fields')-&gt;onUpdate('cascade')-&gt;onDelete('cascade');</v>
       </c>
@@ -25572,10 +25607,10 @@
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B332">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B333">
       <formula1>AvailableFields</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A332">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A333">
       <formula1>TableNames</formula1>
     </dataValidation>
   </dataValidations>
@@ -25591,8 +25626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R310"/>
   <sheetViews>
-    <sheetView topLeftCell="B291" workbookViewId="0">
-      <selection activeCell="D310" sqref="D310:I310"/>
+    <sheetView topLeftCell="F291" workbookViewId="0">
+      <selection activeCell="J309" sqref="J309"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -36799,7 +36834,9 @@
       <c r="I308" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="J308" s="40"/>
+      <c r="J308" s="40" t="s">
+        <v>699</v>
+      </c>
       <c r="K308" s="40"/>
       <c r="L308" s="40"/>
       <c r="M308" s="40"/>
@@ -40039,8 +40076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T109"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:R55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -40050,14 +40087,14 @@
   <sheetData>
     <row r="1" spans="1:20" s="38" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="48" t="s">
-        <v>441</v>
+        <v>690</v>
       </c>
       <c r="B1" s="48"/>
       <c r="C1" s="48"/>
       <c r="D1" s="48"/>
       <c r="E1" s="49" t="str">
         <f>"\"&amp;VLOOKUP($A$1,SeedMap[],3,0)&amp;"\"&amp;VLOOKUP($A$1,SeedMap[],4,0)&amp;"::"&amp;VLOOKUP($A$1,SeedMap[],5,0)&amp;"()"</f>
-        <v>\Milestone\Appframe\Model\ResourceRelation::truncate()</v>
+        <v>\Milestone\Appframe\Model\ResourceFormFieldDepend::truncate()</v>
       </c>
       <c r="F1" s="49"/>
       <c r="G1" s="49"/>
@@ -40201,31 +40238,31 @@
       <c r="B5" s="28"/>
       <c r="C5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],C$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],C$4+$B$4,0))</f>
-        <v>resource</v>
+        <v>form_field</v>
       </c>
       <c r="D5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],D$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],D$4+$B$4,0))</f>
-        <v>name</v>
+        <v>depend_field</v>
       </c>
       <c r="E5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0))</f>
-        <v>description</v>
+        <v>db_field</v>
       </c>
       <c r="F5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0))</f>
-        <v>method</v>
+        <v>operator</v>
       </c>
       <c r="G5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0))</f>
-        <v>type</v>
+        <v>compare_method</v>
       </c>
       <c r="H5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],H$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],H$4+$B$4,0))</f>
-        <v>relate_resource</v>
+        <v>method</v>
       </c>
       <c r="I5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],I$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],I$4+$B$4,0))</f>
-        <v/>
+        <v>ignore_null</v>
       </c>
       <c r="J5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],J$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],J$4+$B$4,0))</f>
@@ -40315,7 +40352,7 @@
       <c r="A8" s="32"/>
       <c r="B8" s="47" t="str">
         <f>$E$1</f>
-        <v>\Milestone\Appframe\Model\ResourceRelation::truncate()</v>
+        <v>\Milestone\Appframe\Model\ResourceFormFieldDepend::truncate()</v>
       </c>
       <c r="C8" s="47"/>
       <c r="D8" s="47"/>
@@ -40340,31 +40377,31 @@
       </c>
       <c r="B9" s="30" t="str">
         <f ca="1">IF($B8="","",IF($B8=";",$I$3,IF($B8=$I$3,"",IF(ISNA(VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),1,0)),";",$S$4))))</f>
-        <v>-&gt;create([</v>
+        <v>;</v>
       </c>
       <c r="C9" s="33" t="str">
         <f ca="1">IF(AND($B9=$S$4,C$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),C$4+$B$4,0)="","","'"&amp;C$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),C$4+$B$4,0)&amp;"', "),"")</f>
-        <v xml:space="preserve">'resource' =&gt; '1', </v>
+        <v/>
       </c>
       <c r="D9" s="33" t="str">
         <f t="shared" ref="D9:Q24" ca="1" si="0">IF(AND($B9=$S$4,D$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),D$4+$B$4,0)="","","'"&amp;D$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),D$4+$B$4,0)&amp;"', "),"")</f>
-        <v xml:space="preserve">'name' =&gt; 'User Groups', </v>
+        <v/>
       </c>
       <c r="E9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Which groups this user belongs to', </v>
+        <v/>
       </c>
       <c r="F9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Groups', </v>
+        <v/>
       </c>
       <c r="G9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
+        <v/>
       </c>
       <c r="H9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '2', </v>
+        <v/>
       </c>
       <c r="I9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -40404,7 +40441,7 @@
       </c>
       <c r="R9" s="33" t="str">
         <f ca="1">IF(B9=$S$4,$T$4,"")</f>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="10" spans="1:20">
@@ -40413,31 +40450,31 @@
       </c>
       <c r="B10" s="30" t="str">
         <f t="shared" ref="B10:B73" ca="1" si="1">IF($B9="","",IF($B9=";",$I$3,IF($B9=$I$3,"",IF(ISNA(VLOOKUP($A$1&amp;"-"&amp;$A10,INDIRECT($E$2),1,0)),";",$S$4))))</f>
-        <v>-&gt;create([</v>
+        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
       </c>
       <c r="C10" s="33" t="str">
         <f ca="1">IF(AND($B10=$S$4,C$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A10,INDIRECT($E$2),C$4+$B$4,0)="","","'"&amp;C$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A10,INDIRECT($E$2),C$4+$B$4,0)&amp;"', "),"")</f>
-        <v xml:space="preserve">'resource' =&gt; '2', </v>
+        <v/>
       </c>
       <c r="D10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Group Users', </v>
+        <v/>
       </c>
       <c r="E10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'List of users belongs to this group', </v>
+        <v/>
       </c>
       <c r="F10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Users', </v>
+        <v/>
       </c>
       <c r="G10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
+        <v/>
       </c>
       <c r="H10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '1', </v>
+        <v/>
       </c>
       <c r="I10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -40477,7 +40514,7 @@
       </c>
       <c r="R10" s="33" t="str">
         <f t="shared" ref="R10:R73" ca="1" si="2">IF(B10=$S$4,$T$4,"")</f>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -40486,31 +40523,31 @@
       </c>
       <c r="B11" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C11" s="33" t="str">
         <f t="shared" ref="C11:G74" ca="1" si="3">IF(AND($B11=$S$4,C$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A11,INDIRECT($E$2),C$4+$B$4,0)="","","'"&amp;C$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A11,INDIRECT($E$2),C$4+$B$4,0)&amp;"', "),"")</f>
-        <v xml:space="preserve">'resource' =&gt; '2', </v>
+        <v/>
       </c>
       <c r="D11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Group Roles', </v>
+        <v/>
       </c>
       <c r="E11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Roles assigneed to this group', </v>
+        <v/>
       </c>
       <c r="F11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Roles', </v>
+        <v/>
       </c>
       <c r="G11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
+        <v/>
       </c>
       <c r="H11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '3', </v>
+        <v/>
       </c>
       <c r="I11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -40550,7 +40587,7 @@
       </c>
       <c r="R11" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -40559,31 +40596,31 @@
       </c>
       <c r="B12" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C12" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '3', </v>
+        <v/>
       </c>
       <c r="D12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Role Groups', </v>
+        <v/>
       </c>
       <c r="E12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Details of groups this role assigned to', </v>
+        <v/>
       </c>
       <c r="F12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Groups', </v>
+        <v/>
       </c>
       <c r="G12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
+        <v/>
       </c>
       <c r="H12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '2', </v>
+        <v/>
       </c>
       <c r="I12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -40623,7 +40660,7 @@
       </c>
       <c r="R12" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -40632,31 +40669,31 @@
       </c>
       <c r="B13" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C13" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '3', </v>
+        <v/>
       </c>
       <c r="D13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Role Resource', </v>
+        <v/>
       </c>
       <c r="E13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Resources assigned to a role', </v>
+        <v/>
       </c>
       <c r="F13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Resources', </v>
+        <v/>
       </c>
       <c r="G13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '11', </v>
+        <v/>
       </c>
       <c r="I13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -40696,7 +40733,7 @@
       </c>
       <c r="R13" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -40705,31 +40742,31 @@
       </c>
       <c r="B14" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C14" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '4', </v>
+        <v/>
       </c>
       <c r="D14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Resource Roles', </v>
+        <v/>
       </c>
       <c r="E14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'The details of roles who have access to this resource', </v>
+        <v/>
       </c>
       <c r="F14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Roles', </v>
+        <v/>
       </c>
       <c r="G14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
+        <v/>
       </c>
       <c r="H14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '3', </v>
+        <v/>
       </c>
       <c r="I14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -40769,7 +40806,7 @@
       </c>
       <c r="R14" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -40778,31 +40815,31 @@
       </c>
       <c r="B15" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C15" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '4', </v>
+        <v/>
       </c>
       <c r="D15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Resource Actions', </v>
+        <v/>
       </c>
       <c r="E15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Get actions available for the resource', </v>
+        <v/>
       </c>
       <c r="F15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Actions', </v>
+        <v/>
       </c>
       <c r="G15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '7', </v>
+        <v/>
       </c>
       <c r="I15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -40842,7 +40879,7 @@
       </c>
       <c r="R15" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="16" spans="1:20">
@@ -40851,31 +40888,31 @@
       </c>
       <c r="B16" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C16" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '7', </v>
+        <v/>
       </c>
       <c r="D16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Resource Action Methods', </v>
+        <v/>
       </c>
       <c r="E16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Handler details of an action', </v>
+        <v/>
       </c>
       <c r="F16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Method', </v>
+        <v/>
       </c>
       <c r="G16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'hasOne', </v>
+        <v/>
       </c>
       <c r="H16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '8', </v>
+        <v/>
       </c>
       <c r="I16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -40915,7 +40952,7 @@
       </c>
       <c r="R16" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="17" spans="1:18">
@@ -40924,31 +40961,31 @@
       </c>
       <c r="B17" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C17" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '7', </v>
+        <v/>
       </c>
       <c r="D17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Resource Action Lists', </v>
+        <v/>
       </c>
       <c r="E17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Lists where action available', </v>
+        <v/>
       </c>
       <c r="F17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Lists', </v>
+        <v/>
       </c>
       <c r="G17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '9', </v>
+        <v/>
       </c>
       <c r="I17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -40988,7 +41025,7 @@
       </c>
       <c r="R17" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="18" spans="1:18">
@@ -40997,31 +41034,31 @@
       </c>
       <c r="B18" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C18" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '7', </v>
+        <v/>
       </c>
       <c r="D18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Resource Action Data', </v>
+        <v/>
       </c>
       <c r="E18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Resource data where action available', </v>
+        <v/>
       </c>
       <c r="F18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Data', </v>
+        <v/>
       </c>
       <c r="G18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '10', </v>
+        <v/>
       </c>
       <c r="I18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -41061,7 +41098,7 @@
       </c>
       <c r="R18" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="19" spans="1:18">
@@ -41070,31 +41107,31 @@
       </c>
       <c r="B19" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C19" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '5', </v>
+        <v/>
       </c>
       <c r="D19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Organisation Contacts', </v>
+        <v/>
       </c>
       <c r="E19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Contact details of organisation', </v>
+        <v/>
       </c>
       <c r="F19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Contacts', </v>
+        <v/>
       </c>
       <c r="G19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '6', </v>
+        <v/>
       </c>
       <c r="I19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -41134,7 +41171,7 @@
       </c>
       <c r="R19" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="20" spans="1:18">
@@ -41143,31 +41180,31 @@
       </c>
       <c r="B20" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C20" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '11', </v>
+        <v/>
       </c>
       <c r="D20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Resource Details', </v>
+        <v/>
       </c>
       <c r="E20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Resource details', </v>
+        <v/>
       </c>
       <c r="F20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Resource', </v>
+        <v/>
       </c>
       <c r="G20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
+        <v/>
       </c>
       <c r="H20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
+        <v/>
       </c>
       <c r="I20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -41207,7 +41244,7 @@
       </c>
       <c r="R20" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="21" spans="1:18">
@@ -41216,31 +41253,31 @@
       </c>
       <c r="B21" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C21" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '4', </v>
+        <v/>
       </c>
       <c r="D21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Resource Forms', </v>
+        <v/>
       </c>
       <c r="E21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Forms available for a resource', </v>
+        <v/>
       </c>
       <c r="F21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Forms', </v>
+        <v/>
       </c>
       <c r="G21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '12', </v>
+        <v/>
       </c>
       <c r="I21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -41280,7 +41317,7 @@
       </c>
       <c r="R21" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="22" spans="1:18">
@@ -41289,31 +41326,31 @@
       </c>
       <c r="B22" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C22" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '12', </v>
+        <v/>
       </c>
       <c r="D22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Form Fields', </v>
+        <v/>
       </c>
       <c r="E22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Fields associated with a form', </v>
+        <v/>
       </c>
       <c r="F22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Fields', </v>
+        <v/>
       </c>
       <c r="G22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '13', </v>
+        <v/>
       </c>
       <c r="I22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -41353,7 +41390,7 @@
       </c>
       <c r="R22" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="23" spans="1:18">
@@ -41362,31 +41399,31 @@
       </c>
       <c r="B23" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C23" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '13', </v>
+        <v/>
       </c>
       <c r="D23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Field Attributes', </v>
+        <v/>
       </c>
       <c r="E23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Attributes of Field', </v>
+        <v/>
       </c>
       <c r="F23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Attributes', </v>
+        <v/>
       </c>
       <c r="G23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '14', </v>
+        <v/>
       </c>
       <c r="I23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -41426,7 +41463,7 @@
       </c>
       <c r="R23" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="24" spans="1:18">
@@ -41435,31 +41472,31 @@
       </c>
       <c r="B24" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C24" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '13', </v>
+        <v/>
       </c>
       <c r="D24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'name' =&gt; 'Field Options', </v>
+        <v/>
       </c>
       <c r="E24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'description' =&gt; 'Options of Field', </v>
+        <v/>
       </c>
       <c r="F24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'method' =&gt; 'Options', </v>
+        <v/>
       </c>
       <c r="G24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'type' =&gt; 'hasOne', </v>
+        <v/>
       </c>
       <c r="H24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '15', </v>
+        <v/>
       </c>
       <c r="I24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -41499,7 +41536,7 @@
       </c>
       <c r="R24" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="25" spans="1:18">
@@ -41508,31 +41545,31 @@
       </c>
       <c r="B25" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '13', </v>
+        <v/>
       </c>
       <c r="D25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Field Validations', </v>
+        <v/>
       </c>
       <c r="E25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Validation details of field', </v>
+        <v/>
       </c>
       <c r="F25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Validations', </v>
+        <v/>
       </c>
       <c r="G25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H25" s="33" t="str">
         <f t="shared" ref="H25:K88" ca="1" si="4">IF(AND($B25=$S$4,H$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A25,INDIRECT($E$2),H$4+$B$4,0)="","","'"&amp;H$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A25,INDIRECT($E$2),H$4+$B$4,0)&amp;"', "),"")</f>
-        <v xml:space="preserve">'relate_resource' =&gt; '16', </v>
+        <v/>
       </c>
       <c r="I25" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -41572,7 +41609,7 @@
       </c>
       <c r="R25" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="26" spans="1:18">
@@ -41581,31 +41618,31 @@
       </c>
       <c r="B26" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '12', </v>
+        <v/>
       </c>
       <c r="D26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'From Resource', </v>
+        <v/>
       </c>
       <c r="E26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Resource this form belongs to', </v>
+        <v/>
       </c>
       <c r="F26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Resource', </v>
+        <v/>
       </c>
       <c r="G26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
+        <v/>
       </c>
       <c r="H26" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
+        <v/>
       </c>
       <c r="I26" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -41645,7 +41682,7 @@
       </c>
       <c r="R26" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="27" spans="1:18">
@@ -41654,31 +41691,31 @@
       </c>
       <c r="B27" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '12', </v>
+        <v/>
       </c>
       <c r="D27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Form Defaults', </v>
+        <v/>
       </c>
       <c r="E27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Predefined values for a form', </v>
+        <v/>
       </c>
       <c r="F27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Defaults', </v>
+        <v/>
       </c>
       <c r="G27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H27" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '17', </v>
+        <v/>
       </c>
       <c r="I27" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -41718,7 +41755,7 @@
       </c>
       <c r="R27" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="28" spans="1:18">
@@ -41727,31 +41764,31 @@
       </c>
       <c r="B28" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '13', </v>
+        <v/>
       </c>
       <c r="D28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Field Data', </v>
+        <v/>
       </c>
       <c r="E28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Fields Database binding details', </v>
+        <v/>
       </c>
       <c r="F28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Data', </v>
+        <v/>
       </c>
       <c r="G28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasOne', </v>
+        <v/>
       </c>
       <c r="H28" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '18', </v>
+        <v/>
       </c>
       <c r="I28" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -41791,7 +41828,7 @@
       </c>
       <c r="R28" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="29" spans="1:18">
@@ -41800,31 +41837,31 @@
       </c>
       <c r="B29" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '4', </v>
+        <v/>
       </c>
       <c r="D29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Resource Relations', </v>
+        <v/>
       </c>
       <c r="E29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Relation of  a resource to another resource', </v>
+        <v/>
       </c>
       <c r="F29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Relations', </v>
+        <v/>
       </c>
       <c r="G29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H29" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
+        <v/>
       </c>
       <c r="I29" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -41864,7 +41901,7 @@
       </c>
       <c r="R29" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="30" spans="1:18">
@@ -41873,31 +41910,31 @@
       </c>
       <c r="B30" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '18', </v>
+        <v/>
       </c>
       <c r="D30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Bind Data Relation', </v>
+        <v/>
       </c>
       <c r="E30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Relation to which the data to be bind', </v>
+        <v/>
       </c>
       <c r="F30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
+        <v/>
       </c>
       <c r="G30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
+        <v/>
       </c>
       <c r="H30" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
+        <v/>
       </c>
       <c r="I30" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -41937,7 +41974,7 @@
       </c>
       <c r="R30" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="31" spans="1:18">
@@ -41946,31 +41983,31 @@
       </c>
       <c r="B31" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '17', </v>
+        <v/>
       </c>
       <c r="D31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Default Data Resource', </v>
+        <v/>
       </c>
       <c r="E31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Resource to which the forms predefined data to be bind', </v>
+        <v/>
       </c>
       <c r="F31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
+        <v/>
       </c>
       <c r="G31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
+        <v/>
       </c>
       <c r="H31" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
+        <v/>
       </c>
       <c r="I31" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -42010,7 +42047,7 @@
       </c>
       <c r="R31" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="32" spans="1:18">
@@ -42019,31 +42056,31 @@
       </c>
       <c r="B32" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '19', </v>
+        <v/>
       </c>
       <c r="D32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Resource Details', </v>
+        <v/>
       </c>
       <c r="E32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Resource details of a list', </v>
+        <v/>
       </c>
       <c r="F32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Resource', </v>
+        <v/>
       </c>
       <c r="G32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
+        <v/>
       </c>
       <c r="H32" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
+        <v/>
       </c>
       <c r="I32" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -42083,7 +42120,7 @@
       </c>
       <c r="R32" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="33" spans="1:18">
@@ -42092,31 +42129,31 @@
       </c>
       <c r="B33" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '19', </v>
+        <v/>
       </c>
       <c r="D33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'List Relations', </v>
+        <v/>
       </c>
       <c r="E33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Relations to be loaded on accessing list', </v>
+        <v/>
       </c>
       <c r="F33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Relations', </v>
+        <v/>
       </c>
       <c r="G33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H33" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '20', </v>
+        <v/>
       </c>
       <c r="I33" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -42156,7 +42193,7 @@
       </c>
       <c r="R33" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="34" spans="1:18">
@@ -42165,31 +42202,31 @@
       </c>
       <c r="B34" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '4', </v>
+        <v/>
       </c>
       <c r="D34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Resource Scopes', </v>
+        <v/>
       </c>
       <c r="E34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Scopes available on a Resource', </v>
+        <v/>
       </c>
       <c r="F34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Scopes', </v>
+        <v/>
       </c>
       <c r="G34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H34" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '21', </v>
+        <v/>
       </c>
       <c r="I34" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -42229,7 +42266,7 @@
       </c>
       <c r="R34" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="35" spans="1:18">
@@ -42238,31 +42275,31 @@
       </c>
       <c r="B35" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '19', </v>
+        <v/>
       </c>
       <c r="D35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'List Scopes', </v>
+        <v/>
       </c>
       <c r="E35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Scopes by which a list to be filtered', </v>
+        <v/>
       </c>
       <c r="F35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Scopes', </v>
+        <v/>
       </c>
       <c r="G35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
+        <v/>
       </c>
       <c r="H35" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '21', </v>
+        <v/>
       </c>
       <c r="I35" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -42302,7 +42339,7 @@
       </c>
       <c r="R35" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="36" spans="1:18">
@@ -42311,31 +42348,31 @@
       </c>
       <c r="B36" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '23', </v>
+        <v/>
       </c>
       <c r="D36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Data Relation', </v>
+        <v/>
       </c>
       <c r="E36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Relations to be loaded on a data view', </v>
+        <v/>
       </c>
       <c r="F36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Relations', </v>
+        <v/>
       </c>
       <c r="G36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H36" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '24', </v>
+        <v/>
       </c>
       <c r="I36" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -42375,7 +42412,7 @@
       </c>
       <c r="R36" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="37" spans="1:18">
@@ -42384,31 +42421,31 @@
       </c>
       <c r="B37" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '23', </v>
+        <v/>
       </c>
       <c r="D37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Resource Details', </v>
+        <v/>
       </c>
       <c r="E37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Details of resource of a record', </v>
+        <v/>
       </c>
       <c r="F37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Resource', </v>
+        <v/>
       </c>
       <c r="G37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
+        <v/>
       </c>
       <c r="H37" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
+        <v/>
       </c>
       <c r="I37" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -42448,7 +42485,7 @@
       </c>
       <c r="R37" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="38" spans="1:18">
@@ -42457,31 +42494,31 @@
       </c>
       <c r="B38" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '19', </v>
+        <v/>
       </c>
       <c r="D38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'List Layout', </v>
+        <v/>
       </c>
       <c r="E38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Layout of a list', </v>
+        <v/>
       </c>
       <c r="F38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Layout', </v>
+        <v/>
       </c>
       <c r="G38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H38" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '25', </v>
+        <v/>
       </c>
       <c r="I38" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -42521,7 +42558,7 @@
       </c>
       <c r="R38" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="39" spans="1:18">
@@ -42530,31 +42567,31 @@
       </c>
       <c r="B39" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C39" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '26', </v>
+        <v/>
       </c>
       <c r="D39" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Nested Relation', </v>
+        <v/>
       </c>
       <c r="E39" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Nested Relation', </v>
+        <v/>
       </c>
       <c r="F39" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Nest', </v>
+        <v/>
       </c>
       <c r="G39" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H39" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
+        <v/>
       </c>
       <c r="I39" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -42594,7 +42631,7 @@
       </c>
       <c r="R39" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="40" spans="1:18">
@@ -42603,31 +42640,31 @@
       </c>
       <c r="B40" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C40" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '26', </v>
+        <v/>
       </c>
       <c r="D40" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Related Resource', </v>
+        <v/>
       </c>
       <c r="E40" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Related Resource Details', </v>
+        <v/>
       </c>
       <c r="F40" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
+        <v/>
       </c>
       <c r="G40" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
+        <v/>
       </c>
       <c r="H40" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
+        <v/>
       </c>
       <c r="I40" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -42667,7 +42704,7 @@
       </c>
       <c r="R40" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="41" spans="1:18">
@@ -42676,31 +42713,31 @@
       </c>
       <c r="B41" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C41" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '26', </v>
+        <v/>
       </c>
       <c r="D41" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Form Layout', </v>
+        <v/>
       </c>
       <c r="E41" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Layout details', </v>
+        <v/>
       </c>
       <c r="F41" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Layout', </v>
+        <v/>
       </c>
       <c r="G41" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H41" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '27', </v>
+        <v/>
       </c>
       <c r="I41" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -42740,7 +42777,7 @@
       </c>
       <c r="R41" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="42" spans="1:18">
@@ -42749,31 +42786,31 @@
       </c>
       <c r="B42" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C42" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '23', </v>
+        <v/>
       </c>
       <c r="D42" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Data View Section', </v>
+        <v/>
       </c>
       <c r="E42" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Section details of data view', </v>
+        <v/>
       </c>
       <c r="F42" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Sections', </v>
+        <v/>
       </c>
       <c r="G42" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H42" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '28', </v>
+        <v/>
       </c>
       <c r="I42" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -42813,7 +42850,7 @@
       </c>
       <c r="R42" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="43" spans="1:18">
@@ -42822,31 +42859,31 @@
       </c>
       <c r="B43" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C43" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '26', </v>
+        <v/>
       </c>
       <c r="D43" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Data View Section Items', </v>
+        <v/>
       </c>
       <c r="E43" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Items of a data view section', </v>
+        <v/>
       </c>
       <c r="F43" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Items', </v>
+        <v/>
       </c>
       <c r="G43" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H43" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '29', </v>
+        <v/>
       </c>
       <c r="I43" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -42886,7 +42923,7 @@
       </c>
       <c r="R43" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="44" spans="1:18">
@@ -42895,31 +42932,31 @@
       </c>
       <c r="B44" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C44" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '28', </v>
+        <v/>
       </c>
       <c r="D44" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Data Relation', </v>
+        <v/>
       </c>
       <c r="E44" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'View relation of a data', </v>
+        <v/>
       </c>
       <c r="F44" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
+        <v/>
       </c>
       <c r="G44" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
+        <v/>
       </c>
       <c r="H44" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
+        <v/>
       </c>
       <c r="I44" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -42959,7 +42996,7 @@
       </c>
       <c r="R44" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="45" spans="1:18">
@@ -42968,31 +43005,31 @@
       </c>
       <c r="B45" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C45" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '29', </v>
+        <v/>
       </c>
       <c r="D45" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Data item relation', </v>
+        <v/>
       </c>
       <c r="E45" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'View relation of a data item', </v>
+        <v/>
       </c>
       <c r="F45" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
+        <v/>
       </c>
       <c r="G45" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
+        <v/>
       </c>
       <c r="H45" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
+        <v/>
       </c>
       <c r="I45" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -43032,7 +43069,7 @@
       </c>
       <c r="R45" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="46" spans="1:18">
@@ -43041,31 +43078,31 @@
       </c>
       <c r="B46" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C46" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '26', </v>
+        <v/>
       </c>
       <c r="D46" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Owner Relation', </v>
+        <v/>
       </c>
       <c r="E46" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'View the owner resource', </v>
+        <v/>
       </c>
       <c r="F46" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Owner', </v>
+        <v/>
       </c>
       <c r="G46" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
+        <v/>
       </c>
       <c r="H46" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
+        <v/>
       </c>
       <c r="I46" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -43105,7 +43142,7 @@
       </c>
       <c r="R46" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="47" spans="1:18">
@@ -43114,31 +43151,31 @@
       </c>
       <c r="B47" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C47" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '12', </v>
+        <v/>
       </c>
       <c r="D47" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Collections', </v>
+        <v/>
       </c>
       <c r="E47" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Collection/Detail form', </v>
+        <v/>
       </c>
       <c r="F47" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Collections', </v>
+        <v/>
       </c>
       <c r="G47" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H47" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '30', </v>
+        <v/>
       </c>
       <c r="I47" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -43178,7 +43215,7 @@
       </c>
       <c r="R47" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="48" spans="1:18">
@@ -43187,31 +43224,31 @@
       </c>
       <c r="B48" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C48" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '30', </v>
+        <v/>
       </c>
       <c r="D48" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Collection Form', </v>
+        <v/>
       </c>
       <c r="E48" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Collection Form', </v>
+        <v/>
       </c>
       <c r="F48" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Form', </v>
+        <v/>
       </c>
       <c r="G48" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
+        <v/>
       </c>
       <c r="H48" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '12', </v>
+        <v/>
       </c>
       <c r="I48" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -43251,7 +43288,7 @@
       </c>
       <c r="R48" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="49" spans="1:18">
@@ -43260,31 +43297,31 @@
       </c>
       <c r="B49" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C49" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '30', </v>
+        <v/>
       </c>
       <c r="D49" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Relation', </v>
+        <v/>
       </c>
       <c r="E49" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Details of Relation', </v>
+        <v/>
       </c>
       <c r="F49" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
+        <v/>
       </c>
       <c r="G49" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
+        <v/>
       </c>
       <c r="H49" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
+        <v/>
       </c>
       <c r="I49" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -43324,7 +43361,7 @@
       </c>
       <c r="R49" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="50" spans="1:18">
@@ -43333,31 +43370,31 @@
       </c>
       <c r="B50" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C50" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '15', </v>
+        <v/>
       </c>
       <c r="D50" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Field', </v>
+        <v/>
       </c>
       <c r="E50" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Field details', </v>
+        <v/>
       </c>
       <c r="F50" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Field', </v>
+        <v/>
       </c>
       <c r="G50" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
+        <v/>
       </c>
       <c r="H50" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '13', </v>
+        <v/>
       </c>
       <c r="I50" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -43397,7 +43434,7 @@
       </c>
       <c r="R50" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="51" spans="1:18">
@@ -43406,31 +43443,31 @@
       </c>
       <c r="B51" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C51" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '13', </v>
+        <v/>
       </c>
       <c r="D51" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Form', </v>
+        <v/>
       </c>
       <c r="E51" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Form details', </v>
+        <v/>
       </c>
       <c r="F51" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Form', </v>
+        <v/>
       </c>
       <c r="G51" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
+        <v/>
       </c>
       <c r="H51" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '12', </v>
+        <v/>
       </c>
       <c r="I51" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -43470,7 +43507,7 @@
       </c>
       <c r="R51" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="52" spans="1:18">
@@ -43479,31 +43516,31 @@
       </c>
       <c r="B52" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C52" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '19', </v>
+        <v/>
       </c>
       <c r="D52" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'List Search', </v>
+        <v/>
       </c>
       <c r="E52" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Search fields for a list', </v>
+        <v/>
       </c>
       <c r="F52" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Search', </v>
+        <v/>
       </c>
       <c r="G52" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H52" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '31', </v>
+        <v/>
       </c>
       <c r="I52" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -43543,7 +43580,7 @@
       </c>
       <c r="R52" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="53" spans="1:18">
@@ -43552,31 +43589,31 @@
       </c>
       <c r="B53" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>-&gt;create([</v>
+        <v/>
       </c>
       <c r="C53" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'resource' =&gt; '13', </v>
+        <v/>
       </c>
       <c r="D53" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'name' =&gt; 'Depending Fields', </v>
+        <v/>
       </c>
       <c r="E53" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'description' =&gt; 'Dependent fields', </v>
+        <v/>
       </c>
       <c r="F53" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'method' =&gt; 'Depends', </v>
+        <v/>
       </c>
       <c r="G53" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
+        <v/>
       </c>
       <c r="H53" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">'relate_resource' =&gt; '32', </v>
+        <v/>
       </c>
       <c r="I53" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -43616,7 +43653,7 @@
       </c>
       <c r="R53" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>])</v>
+        <v/>
       </c>
     </row>
     <row r="54" spans="1:18">
@@ -43625,7 +43662,7 @@
       </c>
       <c r="B54" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>;</v>
+        <v/>
       </c>
       <c r="C54" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -43698,7 +43735,7 @@
       </c>
       <c r="B55" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
+        <v/>
       </c>
       <c r="C55" s="33" t="str">
         <f t="shared" ca="1" si="3"/>

</xml_diff>

<commit_message>
Column,Value DB Field, for non option depended field, added
</commit_message>
<xml_diff>
--- a/Helper.xlsx
+++ b/Helper.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Tables" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3415" uniqueCount="700">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3421" uniqueCount="702">
   <si>
     <t>resource_scopes</t>
   </si>
@@ -2138,6 +2138,12 @@
   </si>
   <si>
     <t>ignore_null</t>
+  </si>
+  <si>
+    <t>form_field_depend_value_db_field</t>
+  </si>
+  <si>
+    <t>value_db_field</t>
   </si>
 </sst>
 </file>
@@ -4219,8 +4225,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Columns" displayName="Columns" ref="A1:I140" totalsRowShown="0" dataDxfId="106">
-  <autoFilter ref="A1:I140">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Columns" displayName="Columns" ref="A1:I141" totalsRowShown="0" dataDxfId="106">
+  <autoFilter ref="A1:I141">
     <filterColumn colId="0"/>
   </autoFilter>
   <tableColumns count="9">
@@ -4239,8 +4245,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TableFields" displayName="TableFields" ref="A1:K333" totalsRowShown="0" dataDxfId="96">
-  <autoFilter ref="A1:K333">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TableFields" displayName="TableFields" ref="A1:K334" totalsRowShown="0" dataDxfId="96">
+  <autoFilter ref="A1:K334">
     <filterColumn colId="0">
       <filters>
         <filter val="resource_form_field_depends"/>
@@ -7868,10 +7874,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I140"/>
+  <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="A140" sqref="A140"/>
+    <sheetView topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="C140" sqref="C140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="15"/>
@@ -10918,6 +10924,27 @@
       <c r="H140" s="4"/>
       <c r="I140" s="4"/>
     </row>
+    <row r="141" spans="1:9">
+      <c r="A141" s="4" t="s">
+        <v>700</v>
+      </c>
+      <c r="B141" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C141" s="4" t="s">
+        <v>701</v>
+      </c>
+      <c r="D141" s="4">
+        <v>64</v>
+      </c>
+      <c r="E141" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F141" s="4"/>
+      <c r="G141" s="4"/>
+      <c r="H141" s="4"/>
+      <c r="I141" s="4"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A43:A46">
     <cfRule type="duplicateValues" dxfId="112" priority="5"/>
@@ -10925,7 +10952,7 @@
   <conditionalFormatting sqref="A56:A59">
     <cfRule type="duplicateValues" dxfId="111" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A140">
+  <conditionalFormatting sqref="A2:A141">
     <cfRule type="duplicateValues" dxfId="110" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A128:A129">
@@ -10947,10 +10974,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K333"/>
+  <dimension ref="A1:K334"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K324" sqref="K324:K333"/>
+      <selection activeCell="B331" sqref="B331"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="15"/>
@@ -25476,88 +25503,86 @@
       <c r="A331" s="4" t="s">
         <v>679</v>
       </c>
-      <c r="B331" s="4" t="s">
+      <c r="B331" s="4"/>
+      <c r="C331" s="4" t="e">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D331" s="4" t="e">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E331" s="7" t="e">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F331" s="4" t="e">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G331" s="4" t="e">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H331" s="4" t="e">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I331" s="4" t="e">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J331" s="4" t="e">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K331" s="4" t="e">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="332" spans="1:11" s="26" customFormat="1">
+      <c r="A332" s="4" t="s">
+        <v>679</v>
+      </c>
+      <c r="B332" s="4" t="s">
         <v>698</v>
       </c>
-      <c r="C331" s="4" t="str">
+      <c r="C332" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
         <v>enum(</v>
       </c>
-      <c r="D331" s="4" t="str">
+      <c r="D332" s="4" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
         <v>'ignore_null'</v>
       </c>
-      <c r="E331" s="7" t="str">
+      <c r="E332" s="7" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
         <v>, ['Yes','No'])</v>
       </c>
-      <c r="F331" s="4" t="str">
+      <c r="F332" s="4" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
         <v>-&gt;default('Yes')</v>
       </c>
-      <c r="G331" s="4" t="str">
+      <c r="G332" s="4" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
         <v/>
       </c>
-      <c r="H331" s="4" t="str">
+      <c r="H332" s="4" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
         <v/>
       </c>
-      <c r="I331" s="4" t="str">
+      <c r="I332" s="4" t="str">
         <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
         <v/>
       </c>
-      <c r="J331" s="4" t="str">
+      <c r="J332" s="4" t="str">
         <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
         <v/>
       </c>
-      <c r="K331" s="4" t="str">
+      <c r="K332" s="4" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
         <v>$table-&gt;enum('ignore_null', ['Yes','No'])-&gt;default('Yes');</v>
-      </c>
-    </row>
-    <row r="332" spans="1:11">
-      <c r="A332" s="4" t="s">
-        <v>679</v>
-      </c>
-      <c r="B332" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C332" s="4" t="str">
-        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>timestamps(</v>
-      </c>
-      <c r="D332" s="4" t="str">
-        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v/>
-      </c>
-      <c r="E332" s="7" t="str">
-        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>)</v>
-      </c>
-      <c r="F332" s="4" t="str">
-        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v/>
-      </c>
-      <c r="G332" s="4" t="str">
-        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v/>
-      </c>
-      <c r="H332" s="4" t="str">
-        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
-        <v/>
-      </c>
-      <c r="I332" s="4" t="str">
-        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
-        <v/>
-      </c>
-      <c r="J332" s="4" t="str">
-        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
-        <v/>
-      </c>
-      <c r="K332" s="4" t="str">
-        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;timestamps();</v>
       </c>
     </row>
     <row r="333" spans="1:11">
@@ -25565,15 +25590,15 @@
         <v>679</v>
       </c>
       <c r="B333" s="4" t="s">
-        <v>123</v>
+        <v>40</v>
       </c>
       <c r="C333" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
-        <v>foreign(</v>
+        <v>timestamps(</v>
       </c>
       <c r="D333" s="4" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'form_field'</v>
+        <v/>
       </c>
       <c r="E333" s="7" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -25581,25 +25606,69 @@
       </c>
       <c r="F333" s="4" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
-        <v>-&gt;references('id')</v>
+        <v/>
       </c>
       <c r="G333" s="4" t="str">
         <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
-        <v>-&gt;on('__resource_form_fields')</v>
+        <v/>
       </c>
       <c r="H333" s="4" t="str">
         <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
-        <v>-&gt;onUpdate('cascade')</v>
+        <v/>
       </c>
       <c r="I333" s="4" t="str">
         <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
-        <v>-&gt;onDelete('cascade')</v>
+        <v/>
       </c>
       <c r="J333" s="4" t="str">
         <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
         <v/>
       </c>
       <c r="K333" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;timestamps();</v>
+      </c>
+    </row>
+    <row r="334" spans="1:11">
+      <c r="A334" s="4" t="s">
+        <v>679</v>
+      </c>
+      <c r="B334" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C334" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>foreign(</v>
+      </c>
+      <c r="D334" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'form_field'</v>
+      </c>
+      <c r="E334" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>)</v>
+      </c>
+      <c r="F334" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>-&gt;references('id')</v>
+      </c>
+      <c r="G334" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v>-&gt;on('__resource_form_fields')</v>
+      </c>
+      <c r="H334" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v>-&gt;onUpdate('cascade')</v>
+      </c>
+      <c r="I334" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v>-&gt;onDelete('cascade')</v>
+      </c>
+      <c r="J334" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K334" s="4" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
         <v>$table-&gt;foreign('form_field')-&gt;references('id')-&gt;on('__resource_form_fields')-&gt;onUpdate('cascade')-&gt;onDelete('cascade');</v>
       </c>
@@ -25607,10 +25676,10 @@
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B333">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B334">
       <formula1>AvailableFields</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A333">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A334">
       <formula1>TableNames</formula1>
     </dataValidation>
   </dataValidations>
@@ -25626,8 +25695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R310"/>
   <sheetViews>
-    <sheetView topLeftCell="F291" workbookViewId="0">
-      <selection activeCell="J309" sqref="J309"/>
+    <sheetView topLeftCell="B291" workbookViewId="0">
+      <selection activeCell="B308" sqref="B308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -36835,9 +36904,11 @@
         <v>36</v>
       </c>
       <c r="J308" s="40" t="s">
+        <v>701</v>
+      </c>
+      <c r="K308" s="40" t="s">
         <v>699</v>
       </c>
-      <c r="K308" s="40"/>
       <c r="L308" s="40"/>
       <c r="M308" s="40"/>
       <c r="N308" s="40"/>
@@ -36939,8 +37010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -40076,7 +40147,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:R8"/>
     </sheetView>
   </sheetViews>
@@ -40262,11 +40333,11 @@
       </c>
       <c r="I5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],I$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],I$4+$B$4,0))</f>
-        <v>ignore_null</v>
+        <v>value_db_field</v>
       </c>
       <c r="J5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],J$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],J$4+$B$4,0))</f>
-        <v/>
+        <v>ignore_null</v>
       </c>
       <c r="K5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],K$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],K$4+$B$4,0))</f>

</xml_diff>

<commit_message>
Dashboard Models and Seeders added
</commit_message>
<xml_diff>
--- a/Helper.xlsx
+++ b/Helper.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Tables" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3579" uniqueCount="744">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3617" uniqueCount="748">
   <si>
     <t>resource_scopes</t>
   </si>
@@ -2270,6 +2270,18 @@
   </si>
   <si>
     <t>['Metric','List','ListRelation']</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>Dashboard Sections</t>
+  </si>
+  <si>
+    <t>Dashboard Section Items</t>
+  </si>
+  <si>
+    <t>Resource Metrics</t>
   </si>
 </sst>
 </file>
@@ -2499,7 +2511,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="133">
+  <dxfs count="130">
     <dxf>
       <font>
         <condense val="0"/>
@@ -2692,42 +2704,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -4393,35 +4369,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tables" displayName="Tables" ref="A1:J42" totalsRowShown="0" dataDxfId="132">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tables" displayName="Tables" ref="A1:J42" totalsRowShown="0" dataDxfId="129">
   <autoFilter ref="A1:J42"/>
   <tableColumns count="10">
-    <tableColumn id="2" name="Name" dataDxfId="131"/>
-    <tableColumn id="10" name="Table" dataDxfId="130">
+    <tableColumn id="2" name="Name" dataDxfId="128"/>
+    <tableColumn id="10" name="Table" dataDxfId="127">
       <calculatedColumnFormula>"__"&amp;[Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Singular Name" dataDxfId="129">
+    <tableColumn id="5" name="Singular Name" dataDxfId="126">
       <calculatedColumnFormula>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Model NS" dataDxfId="128">
+    <tableColumn id="8" name="Model NS" dataDxfId="125">
       <calculatedColumnFormula>"Milestone\Appframe\Model"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Class Name" dataDxfId="127">
+    <tableColumn id="4" name="Class Name" dataDxfId="124">
       <calculatedColumnFormula>SUBSTITUTE(PROPER([Singular Name]),"_","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Migration Artisan" dataDxfId="126">
+    <tableColumn id="1" name="Migration Artisan" dataDxfId="123">
       <calculatedColumnFormula>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Model Artisan" dataDxfId="125">
+    <tableColumn id="6" name="Model Artisan" dataDxfId="122">
       <calculatedColumnFormula>"php artisan make:model "&amp;[Class Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Model Statement" dataDxfId="124">
+    <tableColumn id="3" name="Model Statement" dataDxfId="121">
       <calculatedColumnFormula>"protected $table = '"&amp;[Table]&amp;"';"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Seeder Artisan" dataDxfId="123">
+    <tableColumn id="7" name="Seeder Artisan" dataDxfId="120">
       <calculatedColumnFormula>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Seeder Class" dataDxfId="122">
+    <tableColumn id="9" name="Seeder Class" dataDxfId="119">
       <calculatedColumnFormula>[Class Name]&amp;"TableSeeder"&amp;"::class,"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4430,49 +4406,49 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="ResourceActions" displayName="ResourceActions" ref="A1:P9" totalsRowShown="0" dataDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="ResourceActions" displayName="ResourceActions" ref="A1:P9" totalsRowShown="0" dataDxfId="35">
   <autoFilter ref="A1:P9"/>
   <tableColumns count="16">
-    <tableColumn id="1" name="No" dataDxfId="37">
+    <tableColumn id="1" name="No" dataDxfId="34">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Resource" dataDxfId="36"/>
-    <tableColumn id="13" name="Resource Id" dataDxfId="35">
+    <tableColumn id="2" name="Resource" dataDxfId="33"/>
+    <tableColumn id="13" name="Resource Id" dataDxfId="32">
       <calculatedColumnFormula>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Action Name" dataDxfId="34"/>
-    <tableColumn id="4" name="Description" dataDxfId="33"/>
-    <tableColumn id="5" name="Action Title" dataDxfId="32"/>
-    <tableColumn id="6" name="Button Type" dataDxfId="31"/>
-    <tableColumn id="7" name="Menu" dataDxfId="30"/>
-    <tableColumn id="8" name="Icon" dataDxfId="29"/>
-    <tableColumn id="9" name="Set" dataDxfId="28"/>
-    <tableColumn id="14" name="Action Type" dataDxfId="27"/>
-    <tableColumn id="15" name="ID1" dataDxfId="26"/>
-    <tableColumn id="16" name="ID2" dataDxfId="25"/>
-    <tableColumn id="10" name="On" dataDxfId="24"/>
-    <tableColumn id="11" name="Confirm" dataDxfId="23"/>
-    <tableColumn id="12" name="handler" dataDxfId="22"/>
+    <tableColumn id="3" name="Action Name" dataDxfId="31"/>
+    <tableColumn id="4" name="Description" dataDxfId="30"/>
+    <tableColumn id="5" name="Action Title" dataDxfId="29"/>
+    <tableColumn id="6" name="Button Type" dataDxfId="28"/>
+    <tableColumn id="7" name="Menu" dataDxfId="27"/>
+    <tableColumn id="8" name="Icon" dataDxfId="26"/>
+    <tableColumn id="9" name="Set" dataDxfId="25"/>
+    <tableColumn id="14" name="Action Type" dataDxfId="24"/>
+    <tableColumn id="15" name="ID1" dataDxfId="23"/>
+    <tableColumn id="16" name="ID2" dataDxfId="22"/>
+    <tableColumn id="10" name="On" dataDxfId="21"/>
+    <tableColumn id="11" name="Confirm" dataDxfId="20"/>
+    <tableColumn id="12" name="handler" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Columns" displayName="Columns" ref="A1:I157" totalsRowShown="0" dataDxfId="115">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Columns" displayName="Columns" ref="A1:I157" totalsRowShown="0" dataDxfId="112">
   <autoFilter ref="A1:I157">
     <filterColumn colId="0"/>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" name="Column" dataDxfId="114"/>
-    <tableColumn id="2" name="Type" dataDxfId="113"/>
-    <tableColumn id="3" name="Name" dataDxfId="112"/>
-    <tableColumn id="4" name="Length/Enum" dataDxfId="111"/>
-    <tableColumn id="5" name="Method1" dataDxfId="110"/>
-    <tableColumn id="6" name="Method2" dataDxfId="109"/>
-    <tableColumn id="7" name="Method3" dataDxfId="108"/>
-    <tableColumn id="8" name="Method4" dataDxfId="107"/>
-    <tableColumn id="9" name="Method5" dataDxfId="106"/>
+    <tableColumn id="1" name="Column" dataDxfId="111"/>
+    <tableColumn id="2" name="Type" dataDxfId="110"/>
+    <tableColumn id="3" name="Name" dataDxfId="109"/>
+    <tableColumn id="4" name="Length/Enum" dataDxfId="108"/>
+    <tableColumn id="5" name="Method1" dataDxfId="107"/>
+    <tableColumn id="6" name="Method2" dataDxfId="106"/>
+    <tableColumn id="7" name="Method3" dataDxfId="105"/>
+    <tableColumn id="8" name="Method4" dataDxfId="104"/>
+    <tableColumn id="9" name="Method5" dataDxfId="103"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4524,8 +4500,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R310" totalsRowShown="0" headerRowDxfId="105" dataDxfId="104">
-  <autoFilter ref="A1:R310">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R314" totalsRowShown="0" headerRowDxfId="102" dataDxfId="101">
+  <autoFilter ref="A1:R314">
     <filterColumn colId="1">
       <filters>
         <filter val="Resource Roles"/>
@@ -4533,46 +4509,46 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="18">
-    <tableColumn id="19" name="TRCode" dataDxfId="103">
+    <tableColumn id="19" name="TRCode" dataDxfId="100">
       <calculatedColumnFormula>[Table Name]&amp;"-"&amp;[Record No]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Table Name" dataDxfId="102"/>
-    <tableColumn id="2" name="Record No" dataDxfId="101">
+    <tableColumn id="1" name="Table Name" dataDxfId="99"/>
+    <tableColumn id="2" name="Record No" dataDxfId="98">
       <calculatedColumnFormula>COUNTIF($B$1:$B1,[Table Name])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="1" dataDxfId="100"/>
-    <tableColumn id="4" name="2" dataDxfId="99"/>
-    <tableColumn id="5" name="3" dataDxfId="98"/>
-    <tableColumn id="6" name="4" dataDxfId="97"/>
-    <tableColumn id="7" name="5" dataDxfId="96"/>
-    <tableColumn id="8" name="6" dataDxfId="95"/>
-    <tableColumn id="9" name="7" dataDxfId="94"/>
-    <tableColumn id="10" name="8" dataDxfId="93"/>
-    <tableColumn id="11" name="9" dataDxfId="92"/>
-    <tableColumn id="12" name="10" dataDxfId="91"/>
-    <tableColumn id="13" name="11" dataDxfId="90"/>
-    <tableColumn id="14" name="12" dataDxfId="89"/>
-    <tableColumn id="15" name="13" dataDxfId="88"/>
-    <tableColumn id="16" name="14" dataDxfId="87"/>
-    <tableColumn id="17" name="15" dataDxfId="86"/>
+    <tableColumn id="3" name="1" dataDxfId="97"/>
+    <tableColumn id="4" name="2" dataDxfId="96"/>
+    <tableColumn id="5" name="3" dataDxfId="95"/>
+    <tableColumn id="6" name="4" dataDxfId="94"/>
+    <tableColumn id="7" name="5" dataDxfId="93"/>
+    <tableColumn id="8" name="6" dataDxfId="92"/>
+    <tableColumn id="9" name="7" dataDxfId="91"/>
+    <tableColumn id="10" name="8" dataDxfId="90"/>
+    <tableColumn id="11" name="9" dataDxfId="89"/>
+    <tableColumn id="12" name="10" dataDxfId="88"/>
+    <tableColumn id="13" name="11" dataDxfId="87"/>
+    <tableColumn id="14" name="12" dataDxfId="86"/>
+    <tableColumn id="15" name="13" dataDxfId="85"/>
+    <tableColumn id="16" name="14" dataDxfId="84"/>
+    <tableColumn id="17" name="15" dataDxfId="83"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SeedMap" displayName="SeedMap" ref="A1:E32" totalsRowShown="0" dataDxfId="85">
-  <autoFilter ref="A1:E32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SeedMap" displayName="SeedMap" ref="A1:E36" totalsRowShown="0" dataDxfId="82">
+  <autoFilter ref="A1:E36"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Name" dataDxfId="84"/>
-    <tableColumn id="3" name="FW Table Name" dataDxfId="83"/>
-    <tableColumn id="20" name="NS" dataDxfId="82">
+    <tableColumn id="1" name="Name" dataDxfId="81"/>
+    <tableColumn id="3" name="FW Table Name" dataDxfId="80"/>
+    <tableColumn id="20" name="NS" dataDxfId="79">
       <calculatedColumnFormula>VLOOKUP([FW Table Name],Tables[],4,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="Model" dataDxfId="81">
+    <tableColumn id="21" name="Model" dataDxfId="78">
       <calculatedColumnFormula>VLOOKUP([FW Table Name],Tables[],5,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Query Method" dataDxfId="80">
+    <tableColumn id="4" name="Query Method" dataDxfId="77">
       <calculatedColumnFormula>"truncate"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4581,46 +4557,46 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="ResourceTable" displayName="ResourceTable" ref="A1:I33" totalsRowShown="0" dataDxfId="79">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="ResourceTable" displayName="ResourceTable" ref="A1:I33" totalsRowShown="0" dataDxfId="76">
   <autoFilter ref="A1:I33"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="No" dataDxfId="78">
+    <tableColumn id="1" name="No" dataDxfId="75">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Name" dataDxfId="77"/>
-    <tableColumn id="3" name="Description" dataDxfId="76"/>
-    <tableColumn id="4" name="Title" dataDxfId="75"/>
-    <tableColumn id="5" name="NS" dataDxfId="74">
+    <tableColumn id="2" name="Name" dataDxfId="74"/>
+    <tableColumn id="3" name="Description" dataDxfId="73"/>
+    <tableColumn id="4" name="Title" dataDxfId="72"/>
+    <tableColumn id="5" name="NS" dataDxfId="71">
       <calculatedColumnFormula>"Milestone\Appframe\Model"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Table" dataDxfId="73"/>
-    <tableColumn id="7" name="Key" dataDxfId="72">
+    <tableColumn id="6" name="Table" dataDxfId="70"/>
+    <tableColumn id="7" name="Key" dataDxfId="69">
       <calculatedColumnFormula>"id"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Controller" dataDxfId="71"/>
-    <tableColumn id="9" name="Controller NS" dataDxfId="70"/>
+    <tableColumn id="8" name="Controller" dataDxfId="68"/>
+    <tableColumn id="9" name="Controller NS" dataDxfId="67"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RelationTable" displayName="RelationTable" ref="A1:I46" totalsRowShown="0" dataDxfId="69">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RelationTable" displayName="RelationTable" ref="A1:I46" totalsRowShown="0" dataDxfId="66">
   <autoFilter ref="A1:I46"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="No" dataDxfId="68">
+    <tableColumn id="1" name="No" dataDxfId="65">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Resource" dataDxfId="67"/>
-    <tableColumn id="4" name="Relate Resource" dataDxfId="66"/>
-    <tableColumn id="2" name="Resource Id" dataDxfId="65">
+    <tableColumn id="3" name="Resource" dataDxfId="64"/>
+    <tableColumn id="4" name="Relate Resource" dataDxfId="63"/>
+    <tableColumn id="2" name="Resource Id" dataDxfId="62">
       <calculatedColumnFormula>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Name" dataDxfId="64"/>
-    <tableColumn id="6" name="Description" dataDxfId="63"/>
-    <tableColumn id="7" name="Method" dataDxfId="62"/>
-    <tableColumn id="8" name="Type" dataDxfId="61"/>
-    <tableColumn id="10" name="Relate Id" dataDxfId="60">
+    <tableColumn id="5" name="Name" dataDxfId="61"/>
+    <tableColumn id="6" name="Description" dataDxfId="60"/>
+    <tableColumn id="7" name="Method" dataDxfId="59"/>
+    <tableColumn id="8" name="Type" dataDxfId="58"/>
+    <tableColumn id="10" name="Relate Id" dataDxfId="57">
       <calculatedColumnFormula>VLOOKUP([Relate Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4629,47 +4605,47 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="ResourceForms" displayName="ResourceForms" ref="A1:G9" totalsRowShown="0" dataDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="ResourceForms" displayName="ResourceForms" ref="A1:G9" totalsRowShown="0" dataDxfId="56">
   <autoFilter ref="A1:G9"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="No" dataDxfId="58">
+    <tableColumn id="1" name="No" dataDxfId="55">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Resource ID" dataDxfId="57"/>
-    <tableColumn id="3" name="Resource Name" dataDxfId="56">
+    <tableColumn id="2" name="Resource ID" dataDxfId="54"/>
+    <tableColumn id="3" name="Resource Name" dataDxfId="53">
       <calculatedColumnFormula>VLOOKUP([Resource ID],ResourceTable[],2,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Form Name" dataDxfId="55"/>
-    <tableColumn id="6" name="Title" dataDxfId="54"/>
-    <tableColumn id="7" name="Action Text" dataDxfId="53"/>
-    <tableColumn id="8" name="Description" dataDxfId="52"/>
+    <tableColumn id="4" name="Form Name" dataDxfId="52"/>
+    <tableColumn id="6" name="Title" dataDxfId="51"/>
+    <tableColumn id="7" name="Action Text" dataDxfId="50"/>
+    <tableColumn id="8" name="Description" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="FormFields" displayName="FormFields" ref="A1:L33" totalsRowShown="0" dataDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="FormFields" displayName="FormFields" ref="A1:L33" totalsRowShown="0" dataDxfId="48">
   <autoFilter ref="A1:L33"/>
   <tableColumns count="12">
-    <tableColumn id="9" name="No" dataDxfId="50">
+    <tableColumn id="9" name="No" dataDxfId="47">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Form Id" dataDxfId="49"/>
-    <tableColumn id="7" name="Form Name" dataDxfId="48">
+    <tableColumn id="1" name="Form Id" dataDxfId="46"/>
+    <tableColumn id="7" name="Form Name" dataDxfId="45">
       <calculatedColumnFormula>VLOOKUP([Form Id],ResourceForms[],4,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Name" dataDxfId="47"/>
-    <tableColumn id="2" name="Type" dataDxfId="46"/>
-    <tableColumn id="5" name="Label" dataDxfId="45"/>
-    <tableColumn id="6" name="Collection" dataDxfId="44"/>
-    <tableColumn id="14" name="Attribute" dataDxfId="43">
+    <tableColumn id="4" name="Name" dataDxfId="44"/>
+    <tableColumn id="2" name="Type" dataDxfId="43"/>
+    <tableColumn id="5" name="Label" dataDxfId="42"/>
+    <tableColumn id="6" name="Collection" dataDxfId="41"/>
+    <tableColumn id="14" name="Attribute" dataDxfId="40">
       <calculatedColumnFormula>[Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Relation" dataDxfId="42"/>
-    <tableColumn id="11" name="Deep 1" dataDxfId="41"/>
-    <tableColumn id="12" name="Deep 2" dataDxfId="40"/>
-    <tableColumn id="13" name="Deep 3" dataDxfId="39"/>
+    <tableColumn id="10" name="Relation" dataDxfId="39"/>
+    <tableColumn id="11" name="Deep 1" dataDxfId="38"/>
+    <tableColumn id="12" name="Deep 2" dataDxfId="37"/>
+    <tableColumn id="13" name="Deep 3" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4962,8 +4938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8274,7 +8250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I157"/>
   <sheetViews>
-    <sheetView topLeftCell="A145" workbookViewId="0">
+    <sheetView topLeftCell="A130" workbookViewId="0">
       <selection activeCell="D156" sqref="D156"/>
     </sheetView>
   </sheetViews>
@@ -11679,22 +11655,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A43:A46">
-    <cfRule type="duplicateValues" dxfId="121" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="118" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56:A59">
-    <cfRule type="duplicateValues" dxfId="120" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="117" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A157">
-    <cfRule type="duplicateValues" dxfId="119" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="116" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A128:A129">
-    <cfRule type="duplicateValues" dxfId="118" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="115" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A128:A129">
-    <cfRule type="duplicateValues" dxfId="117" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="114" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A130:A131">
-    <cfRule type="duplicateValues" dxfId="116" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="113" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A152:A153">
     <cfRule type="duplicateValues" dxfId="18" priority="1"/>
@@ -11711,8 +11687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K373"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A353" workbookViewId="0">
-      <selection activeCell="B368" sqref="B368"/>
+    <sheetView topLeftCell="A327" workbookViewId="0">
+      <selection activeCell="B336" sqref="B336:B346"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="15"/>
@@ -28146,10 +28122,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R310"/>
+  <dimension ref="A1:R314"/>
   <sheetViews>
-    <sheetView topLeftCell="B291" workbookViewId="0">
-      <selection activeCell="B308" sqref="B308"/>
+    <sheetView topLeftCell="B297" workbookViewId="0">
+      <selection activeCell="B311" sqref="B311:B314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -39450,6 +39426,170 @@
       <c r="Q310" s="40"/>
       <c r="R310" s="40"/>
     </row>
+    <row r="311" spans="1:18">
+      <c r="A311" s="42" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Dashboard-0</v>
+      </c>
+      <c r="B311" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="C311" s="42">
+        <f>COUNTIF($B$1:$B310,[Table Name])</f>
+        <v>0</v>
+      </c>
+      <c r="D311" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="E311" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="F311" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="G311" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="H311" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="I311" s="43"/>
+      <c r="J311" s="43"/>
+      <c r="K311" s="43"/>
+      <c r="L311" s="43"/>
+      <c r="M311" s="43"/>
+      <c r="N311" s="43"/>
+      <c r="O311" s="43"/>
+      <c r="P311" s="43"/>
+      <c r="Q311" s="43"/>
+      <c r="R311" s="43"/>
+    </row>
+    <row r="312" spans="1:18">
+      <c r="A312" s="42" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Dashboard Sections-0</v>
+      </c>
+      <c r="B312" s="43" t="s">
+        <v>745</v>
+      </c>
+      <c r="C312" s="42">
+        <f>COUNTIF($B$1:$B311,[Table Name])</f>
+        <v>0</v>
+      </c>
+      <c r="D312" s="43" t="s">
+        <v>725</v>
+      </c>
+      <c r="E312" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="F312" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="G312" s="43" t="s">
+        <v>728</v>
+      </c>
+      <c r="H312" s="43"/>
+      <c r="I312" s="43"/>
+      <c r="J312" s="43"/>
+      <c r="K312" s="43"/>
+      <c r="L312" s="43"/>
+      <c r="M312" s="43"/>
+      <c r="N312" s="43"/>
+      <c r="O312" s="43"/>
+      <c r="P312" s="43"/>
+      <c r="Q312" s="43"/>
+      <c r="R312" s="43"/>
+    </row>
+    <row r="313" spans="1:18">
+      <c r="A313" s="42" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Dashboard Section Items-0</v>
+      </c>
+      <c r="B313" s="43" t="s">
+        <v>746</v>
+      </c>
+      <c r="C313" s="42">
+        <f>COUNTIF($B$1:$B312,[Table Name])</f>
+        <v>0</v>
+      </c>
+      <c r="D313" s="43" t="s">
+        <v>602</v>
+      </c>
+      <c r="E313" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="F313" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="G313" s="43" t="s">
+        <v>736</v>
+      </c>
+      <c r="H313" s="43" t="s">
+        <v>740</v>
+      </c>
+      <c r="I313" s="43" t="s">
+        <v>741</v>
+      </c>
+      <c r="J313" s="43"/>
+      <c r="K313" s="43"/>
+      <c r="L313" s="43"/>
+      <c r="M313" s="43"/>
+      <c r="N313" s="43"/>
+      <c r="O313" s="43"/>
+      <c r="P313" s="43"/>
+      <c r="Q313" s="43"/>
+      <c r="R313" s="43"/>
+    </row>
+    <row r="314" spans="1:18">
+      <c r="A314" s="22" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resource Metrics-0</v>
+      </c>
+      <c r="B314" s="40" t="s">
+        <v>747</v>
+      </c>
+      <c r="C314" s="22">
+        <f>COUNTIF($B$1:$B313,[Table Name])</f>
+        <v>0</v>
+      </c>
+      <c r="D314" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="E314" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="F314" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="G314" s="40" t="s">
+        <v>704</v>
+      </c>
+      <c r="H314" s="40" t="s">
+        <v>707</v>
+      </c>
+      <c r="I314" s="40" t="s">
+        <v>710</v>
+      </c>
+      <c r="J314" s="40" t="s">
+        <v>713</v>
+      </c>
+      <c r="K314" s="40" t="s">
+        <v>717</v>
+      </c>
+      <c r="L314" s="40" t="s">
+        <v>721</v>
+      </c>
+      <c r="M314" s="40" t="s">
+        <v>724</v>
+      </c>
+      <c r="N314" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="O314" s="40"/>
+      <c r="P314" s="40"/>
+      <c r="Q314" s="40"/>
+      <c r="R314" s="40"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
@@ -39461,10 +39601,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -40115,12 +40255,92 @@
         <v>truncate</v>
       </c>
     </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="5" t="s">
+        <v>744</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>725</v>
+      </c>
+      <c r="C33" s="5" t="str">
+        <f>VLOOKUP([FW Table Name],Tables[],4,0)</f>
+        <v>Milestone\Appframe\Model</v>
+      </c>
+      <c r="D33" s="5" t="str">
+        <f>VLOOKUP([FW Table Name],Tables[],5,0)</f>
+        <v>ResourceDashboard</v>
+      </c>
+      <c r="E33" s="8" t="str">
+        <f>"truncate"</f>
+        <v>truncate</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="5" t="s">
+        <v>745</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>726</v>
+      </c>
+      <c r="C34" s="5" t="str">
+        <f>VLOOKUP([FW Table Name],Tables[],4,0)</f>
+        <v>Milestone\Appframe\Model</v>
+      </c>
+      <c r="D34" s="5" t="str">
+        <f>VLOOKUP([FW Table Name],Tables[],5,0)</f>
+        <v>ResourceDashboardSection</v>
+      </c>
+      <c r="E34" s="8" t="str">
+        <f>"truncate"</f>
+        <v>truncate</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="5" t="s">
+        <v>746</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>732</v>
+      </c>
+      <c r="C35" s="5" t="str">
+        <f>VLOOKUP([FW Table Name],Tables[],4,0)</f>
+        <v>Milestone\Appframe\Model</v>
+      </c>
+      <c r="D35" s="5" t="str">
+        <f>VLOOKUP([FW Table Name],Tables[],5,0)</f>
+        <v>ResourceDashboardSectionItem</v>
+      </c>
+      <c r="E35" s="8" t="str">
+        <f>"truncate"</f>
+        <v>truncate</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="4" t="s">
+        <v>747</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>702</v>
+      </c>
+      <c r="C36" s="4" t="str">
+        <f>VLOOKUP([FW Table Name],Tables[],4,0)</f>
+        <v>Milestone\Appframe\Model</v>
+      </c>
+      <c r="D36" s="4" t="str">
+        <f>VLOOKUP([FW Table Name],Tables[],5,0)</f>
+        <v>ResourceMetric</v>
+      </c>
+      <c r="E36" s="7" t="str">
+        <f>"truncate"</f>
+        <v>truncate</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E36">
       <formula1>"truncate,query"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B36">
       <formula1>TableNames</formula1>
     </dataValidation>
   </dataValidations>
@@ -42601,7 +42821,7 @@
   <dimension ref="A1:T109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:R8"/>
+      <selection activeCell="B6" sqref="B6:R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -42611,14 +42831,14 @@
   <sheetData>
     <row r="1" spans="1:20" s="38" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="48" t="s">
-        <v>690</v>
+        <v>747</v>
       </c>
       <c r="B1" s="48"/>
       <c r="C1" s="48"/>
       <c r="D1" s="48"/>
       <c r="E1" s="49" t="str">
         <f>"\"&amp;VLOOKUP($A$1,SeedMap[],3,0)&amp;"\"&amp;VLOOKUP($A$1,SeedMap[],4,0)&amp;"::"&amp;VLOOKUP($A$1,SeedMap[],5,0)&amp;"()"</f>
-        <v>\Milestone\Appframe\Model\ResourceFormFieldDepend::truncate()</v>
+        <v>\Milestone\Appframe\Model\ResourceMetric::truncate()</v>
       </c>
       <c r="F1" s="49"/>
       <c r="G1" s="49"/>
@@ -42762,47 +42982,47 @@
       <c r="B5" s="28"/>
       <c r="C5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],C$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],C$4+$B$4,0))</f>
-        <v>form_field</v>
+        <v>resource</v>
       </c>
       <c r="D5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],D$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],D$4+$B$4,0))</f>
-        <v>depend_field</v>
+        <v>name</v>
       </c>
       <c r="E5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0))</f>
-        <v>db_field</v>
+        <v>resource_list</v>
       </c>
       <c r="F5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0))</f>
-        <v>operator</v>
+        <v>aggregates</v>
       </c>
       <c r="G5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0))</f>
-        <v>compare_method</v>
+        <v>aggregate_field</v>
       </c>
       <c r="H5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],H$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],H$4+$B$4,0))</f>
-        <v>method</v>
+        <v>aggregate_distinct</v>
       </c>
       <c r="I5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],I$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],I$4+$B$4,0))</f>
-        <v>value_db_field</v>
+        <v>date_field</v>
       </c>
       <c r="J5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],J$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],J$4+$B$4,0))</f>
-        <v>ignore_null</v>
+        <v>range_unit</v>
       </c>
       <c r="K5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],K$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],K$4+$B$4,0))</f>
-        <v/>
+        <v>range</v>
       </c>
       <c r="L5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],L$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],L$4+$B$4,0))</f>
-        <v/>
+        <v>groupby</v>
       </c>
       <c r="M5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],M$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],M$4+$B$4,0))</f>
-        <v/>
+        <v>method</v>
       </c>
       <c r="N5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],N$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],N$4+$B$4,0))</f>
@@ -42876,7 +43096,7 @@
       <c r="A8" s="32"/>
       <c r="B8" s="47" t="str">
         <f>$E$1</f>
-        <v>\Milestone\Appframe\Model\ResourceFormFieldDepend::truncate()</v>
+        <v>\Milestone\Appframe\Model\ResourceMetric::truncate()</v>
       </c>
       <c r="C8" s="47"/>
       <c r="D8" s="47"/>

</xml_diff>

<commit_message>
Dashboard related Relations added
</commit_message>
<xml_diff>
--- a/Helper.xlsx
+++ b/Helper.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Tables" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3617" uniqueCount="748">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3705" uniqueCount="769">
   <si>
     <t>resource_scopes</t>
   </si>
@@ -2282,6 +2282,69 @@
   </si>
   <si>
     <t>Resource Metrics</t>
+  </si>
+  <si>
+    <t>ResourceDashboard</t>
+  </si>
+  <si>
+    <t>ResourceDashboardSection</t>
+  </si>
+  <si>
+    <t>ResourceDashboardSectionItem</t>
+  </si>
+  <si>
+    <t>ResourceMetric</t>
+  </si>
+  <si>
+    <t>Dashboard details for a Resource</t>
+  </si>
+  <si>
+    <t>Sections of a Dashboard</t>
+  </si>
+  <si>
+    <t>Items of a Dashboard Section</t>
+  </si>
+  <si>
+    <t>Resource Dashboard</t>
+  </si>
+  <si>
+    <t>__resource_dashboard</t>
+  </si>
+  <si>
+    <t>__resource_dashboard_sections</t>
+  </si>
+  <si>
+    <t>__resource_dashboard_section_items</t>
+  </si>
+  <si>
+    <t>__resource_metrics</t>
+  </si>
+  <si>
+    <t>Dashboard Section</t>
+  </si>
+  <si>
+    <t>Metrics defined for a resource</t>
+  </si>
+  <si>
+    <t>Dashboards</t>
+  </si>
+  <si>
+    <t>Dashboards of a Resource</t>
+  </si>
+  <si>
+    <t>Resource Dashboards</t>
+  </si>
+  <si>
+    <t>Sections of a dashboard</t>
+  </si>
+  <si>
+    <t>Items of a dashboard section</t>
+  </si>
+  <si>
+    <t>Dashboard Resource</t>
+  </si>
+  <si>
+    <t>Resource details of a dashboard</t>
   </si>
 </sst>
 </file>
@@ -2401,7 +2464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2507,46 +2570,161 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="130">
+  <dxfs count="124">
     <dxf>
       <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
-        <color rgb="FF9C0006"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2704,42 +2882,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -3324,151 +3466,6 @@
         <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
       </font>
     </dxf>
     <dxf>
@@ -4369,35 +4366,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tables" displayName="Tables" ref="A1:J42" totalsRowShown="0" dataDxfId="129">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tables" displayName="Tables" ref="A1:J42" totalsRowShown="0" dataDxfId="123">
   <autoFilter ref="A1:J42"/>
   <tableColumns count="10">
-    <tableColumn id="2" name="Name" dataDxfId="128"/>
-    <tableColumn id="10" name="Table" dataDxfId="127">
+    <tableColumn id="2" name="Name" dataDxfId="122"/>
+    <tableColumn id="10" name="Table" dataDxfId="121">
       <calculatedColumnFormula>"__"&amp;[Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Singular Name" dataDxfId="126">
+    <tableColumn id="5" name="Singular Name" dataDxfId="120">
       <calculatedColumnFormula>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Model NS" dataDxfId="125">
+    <tableColumn id="8" name="Model NS" dataDxfId="119">
       <calculatedColumnFormula>"Milestone\Appframe\Model"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Class Name" dataDxfId="124">
+    <tableColumn id="4" name="Class Name" dataDxfId="118">
       <calculatedColumnFormula>SUBSTITUTE(PROPER([Singular Name]),"_","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Migration Artisan" dataDxfId="123">
+    <tableColumn id="1" name="Migration Artisan" dataDxfId="117">
       <calculatedColumnFormula>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Model Artisan" dataDxfId="122">
+    <tableColumn id="6" name="Model Artisan" dataDxfId="116">
       <calculatedColumnFormula>"php artisan make:model "&amp;[Class Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Model Statement" dataDxfId="121">
+    <tableColumn id="3" name="Model Statement" dataDxfId="115">
       <calculatedColumnFormula>"protected $table = '"&amp;[Table]&amp;"';"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Seeder Artisan" dataDxfId="120">
+    <tableColumn id="7" name="Seeder Artisan" dataDxfId="114">
       <calculatedColumnFormula>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Seeder Class" dataDxfId="119">
+    <tableColumn id="9" name="Seeder Class" dataDxfId="113">
       <calculatedColumnFormula>[Class Name]&amp;"TableSeeder"&amp;"::class,"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4406,56 +4403,56 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="ResourceActions" displayName="ResourceActions" ref="A1:P9" totalsRowShown="0" dataDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="ResourceActions" displayName="ResourceActions" ref="A1:P9" totalsRowShown="0" dataDxfId="39">
   <autoFilter ref="A1:P9"/>
   <tableColumns count="16">
-    <tableColumn id="1" name="No" dataDxfId="34">
+    <tableColumn id="1" name="No" dataDxfId="38">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Resource" dataDxfId="33"/>
-    <tableColumn id="13" name="Resource Id" dataDxfId="32">
+    <tableColumn id="2" name="Resource" dataDxfId="37"/>
+    <tableColumn id="13" name="Resource Id" dataDxfId="36">
       <calculatedColumnFormula>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Action Name" dataDxfId="31"/>
-    <tableColumn id="4" name="Description" dataDxfId="30"/>
-    <tableColumn id="5" name="Action Title" dataDxfId="29"/>
-    <tableColumn id="6" name="Button Type" dataDxfId="28"/>
-    <tableColumn id="7" name="Menu" dataDxfId="27"/>
-    <tableColumn id="8" name="Icon" dataDxfId="26"/>
-    <tableColumn id="9" name="Set" dataDxfId="25"/>
-    <tableColumn id="14" name="Action Type" dataDxfId="24"/>
-    <tableColumn id="15" name="ID1" dataDxfId="23"/>
-    <tableColumn id="16" name="ID2" dataDxfId="22"/>
-    <tableColumn id="10" name="On" dataDxfId="21"/>
-    <tableColumn id="11" name="Confirm" dataDxfId="20"/>
-    <tableColumn id="12" name="handler" dataDxfId="19"/>
+    <tableColumn id="3" name="Action Name" dataDxfId="35"/>
+    <tableColumn id="4" name="Description" dataDxfId="34"/>
+    <tableColumn id="5" name="Action Title" dataDxfId="33"/>
+    <tableColumn id="6" name="Button Type" dataDxfId="32"/>
+    <tableColumn id="7" name="Menu" dataDxfId="31"/>
+    <tableColumn id="8" name="Icon" dataDxfId="30"/>
+    <tableColumn id="9" name="Set" dataDxfId="29"/>
+    <tableColumn id="14" name="Action Type" dataDxfId="28"/>
+    <tableColumn id="15" name="ID1" dataDxfId="27"/>
+    <tableColumn id="16" name="ID2" dataDxfId="26"/>
+    <tableColumn id="10" name="On" dataDxfId="25"/>
+    <tableColumn id="11" name="Confirm" dataDxfId="24"/>
+    <tableColumn id="12" name="handler" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Columns" displayName="Columns" ref="A1:I157" totalsRowShown="0" dataDxfId="112">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Columns" displayName="Columns" ref="A1:I157" totalsRowShown="0" dataDxfId="106">
   <autoFilter ref="A1:I157">
     <filterColumn colId="0"/>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" name="Column" dataDxfId="111"/>
-    <tableColumn id="2" name="Type" dataDxfId="110"/>
-    <tableColumn id="3" name="Name" dataDxfId="109"/>
-    <tableColumn id="4" name="Length/Enum" dataDxfId="108"/>
-    <tableColumn id="5" name="Method1" dataDxfId="107"/>
-    <tableColumn id="6" name="Method2" dataDxfId="106"/>
-    <tableColumn id="7" name="Method3" dataDxfId="105"/>
-    <tableColumn id="8" name="Method4" dataDxfId="104"/>
-    <tableColumn id="9" name="Method5" dataDxfId="103"/>
+    <tableColumn id="1" name="Column" dataDxfId="105"/>
+    <tableColumn id="2" name="Type" dataDxfId="104"/>
+    <tableColumn id="3" name="Name" dataDxfId="103"/>
+    <tableColumn id="4" name="Length/Enum" dataDxfId="102"/>
+    <tableColumn id="5" name="Method1" dataDxfId="101"/>
+    <tableColumn id="6" name="Method2" dataDxfId="100"/>
+    <tableColumn id="7" name="Method3" dataDxfId="99"/>
+    <tableColumn id="8" name="Method4" dataDxfId="98"/>
+    <tableColumn id="9" name="Method5" dataDxfId="97"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TableFields" displayName="TableFields" ref="A1:K373" totalsRowShown="0" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TableFields" displayName="TableFields" ref="A1:K373" totalsRowShown="0" dataDxfId="10">
   <autoFilter ref="A1:K373">
     <filterColumn colId="0">
       <filters>
@@ -4465,33 +4462,33 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="11">
-    <tableColumn id="2" name="Table" dataDxfId="14"/>
-    <tableColumn id="3" name="Field" dataDxfId="13"/>
-    <tableColumn id="5" name="Type" dataDxfId="12">
+    <tableColumn id="2" name="Table" dataDxfId="21"/>
+    <tableColumn id="3" name="Field" dataDxfId="20"/>
+    <tableColumn id="5" name="Type" dataDxfId="19">
       <calculatedColumnFormula>VLOOKUP([Field],Columns[],2,0)&amp;"("</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Name" dataDxfId="11">
+    <tableColumn id="4" name="Name" dataDxfId="18">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Arg2" dataDxfId="10">
+    <tableColumn id="6" name="Arg2" dataDxfId="17">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Method1" dataDxfId="9">
+    <tableColumn id="7" name="Method1" dataDxfId="16">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Method2" dataDxfId="8">
+    <tableColumn id="8" name="Method2" dataDxfId="15">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Method3" dataDxfId="7">
+    <tableColumn id="9" name="Method3" dataDxfId="14">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Method4" dataDxfId="6">
+    <tableColumn id="10" name="Method4" dataDxfId="13">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Method5" dataDxfId="5">
+    <tableColumn id="11" name="Method5" dataDxfId="12">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Statement" dataDxfId="4">
+    <tableColumn id="12" name="Statement" dataDxfId="11">
       <calculatedColumnFormula>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4500,8 +4497,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R314" totalsRowShown="0" headerRowDxfId="102" dataDxfId="101">
-  <autoFilter ref="A1:R314">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R322" totalsRowShown="0" headerRowDxfId="96" dataDxfId="95">
+  <autoFilter ref="A1:R322">
     <filterColumn colId="1">
       <filters>
         <filter val="Resource Roles"/>
@@ -4509,46 +4506,46 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="18">
-    <tableColumn id="19" name="TRCode" dataDxfId="100">
+    <tableColumn id="19" name="TRCode" dataDxfId="94">
       <calculatedColumnFormula>[Table Name]&amp;"-"&amp;[Record No]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Table Name" dataDxfId="99"/>
-    <tableColumn id="2" name="Record No" dataDxfId="98">
+    <tableColumn id="1" name="Table Name" dataDxfId="93"/>
+    <tableColumn id="2" name="Record No" dataDxfId="92">
       <calculatedColumnFormula>COUNTIF($B$1:$B1,[Table Name])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="1" dataDxfId="97"/>
-    <tableColumn id="4" name="2" dataDxfId="96"/>
-    <tableColumn id="5" name="3" dataDxfId="95"/>
-    <tableColumn id="6" name="4" dataDxfId="94"/>
-    <tableColumn id="7" name="5" dataDxfId="93"/>
-    <tableColumn id="8" name="6" dataDxfId="92"/>
-    <tableColumn id="9" name="7" dataDxfId="91"/>
-    <tableColumn id="10" name="8" dataDxfId="90"/>
-    <tableColumn id="11" name="9" dataDxfId="89"/>
-    <tableColumn id="12" name="10" dataDxfId="88"/>
-    <tableColumn id="13" name="11" dataDxfId="87"/>
-    <tableColumn id="14" name="12" dataDxfId="86"/>
-    <tableColumn id="15" name="13" dataDxfId="85"/>
-    <tableColumn id="16" name="14" dataDxfId="84"/>
-    <tableColumn id="17" name="15" dataDxfId="83"/>
+    <tableColumn id="3" name="1" dataDxfId="91"/>
+    <tableColumn id="4" name="2" dataDxfId="90"/>
+    <tableColumn id="5" name="3" dataDxfId="89"/>
+    <tableColumn id="6" name="4" dataDxfId="88"/>
+    <tableColumn id="7" name="5" dataDxfId="87"/>
+    <tableColumn id="8" name="6" dataDxfId="86"/>
+    <tableColumn id="9" name="7" dataDxfId="85"/>
+    <tableColumn id="10" name="8" dataDxfId="84"/>
+    <tableColumn id="11" name="9" dataDxfId="83"/>
+    <tableColumn id="12" name="10" dataDxfId="82"/>
+    <tableColumn id="13" name="11" dataDxfId="81"/>
+    <tableColumn id="14" name="12" dataDxfId="80"/>
+    <tableColumn id="15" name="13" dataDxfId="79"/>
+    <tableColumn id="16" name="14" dataDxfId="78"/>
+    <tableColumn id="17" name="15" dataDxfId="77"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SeedMap" displayName="SeedMap" ref="A1:E36" totalsRowShown="0" dataDxfId="82">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SeedMap" displayName="SeedMap" ref="A1:E36" totalsRowShown="0" dataDxfId="76">
   <autoFilter ref="A1:E36"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Name" dataDxfId="81"/>
-    <tableColumn id="3" name="FW Table Name" dataDxfId="80"/>
-    <tableColumn id="20" name="NS" dataDxfId="79">
+    <tableColumn id="1" name="Name" dataDxfId="75"/>
+    <tableColumn id="3" name="FW Table Name" dataDxfId="74"/>
+    <tableColumn id="20" name="NS" dataDxfId="73">
       <calculatedColumnFormula>VLOOKUP([FW Table Name],Tables[],4,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="Model" dataDxfId="78">
+    <tableColumn id="21" name="Model" dataDxfId="72">
       <calculatedColumnFormula>VLOOKUP([FW Table Name],Tables[],5,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Query Method" dataDxfId="77">
+    <tableColumn id="4" name="Query Method" dataDxfId="71">
       <calculatedColumnFormula>"truncate"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4557,46 +4554,46 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="ResourceTable" displayName="ResourceTable" ref="A1:I33" totalsRowShown="0" dataDxfId="76">
-  <autoFilter ref="A1:I33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="ResourceTable" displayName="ResourceTable" ref="A1:I37" totalsRowShown="0" dataDxfId="70">
+  <autoFilter ref="A1:I37"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="No" dataDxfId="75">
+    <tableColumn id="1" name="No" dataDxfId="69">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Name" dataDxfId="74"/>
-    <tableColumn id="3" name="Description" dataDxfId="73"/>
-    <tableColumn id="4" name="Title" dataDxfId="72"/>
-    <tableColumn id="5" name="NS" dataDxfId="71">
+    <tableColumn id="2" name="Name" dataDxfId="68"/>
+    <tableColumn id="3" name="Description" dataDxfId="67"/>
+    <tableColumn id="4" name="Title" dataDxfId="66"/>
+    <tableColumn id="5" name="NS" dataDxfId="65">
       <calculatedColumnFormula>"Milestone\Appframe\Model"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Table" dataDxfId="70"/>
-    <tableColumn id="7" name="Key" dataDxfId="69">
+    <tableColumn id="6" name="Table" dataDxfId="64"/>
+    <tableColumn id="7" name="Key" dataDxfId="63">
       <calculatedColumnFormula>"id"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Controller" dataDxfId="68"/>
-    <tableColumn id="9" name="Controller NS" dataDxfId="67"/>
+    <tableColumn id="8" name="Controller" dataDxfId="62"/>
+    <tableColumn id="9" name="Controller NS" dataDxfId="61"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RelationTable" displayName="RelationTable" ref="A1:I46" totalsRowShown="0" dataDxfId="66">
-  <autoFilter ref="A1:I46"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RelationTable" displayName="RelationTable" ref="A1:I50" totalsRowShown="0" dataDxfId="0">
+  <autoFilter ref="A1:I50"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="No" dataDxfId="65">
+    <tableColumn id="1" name="No" dataDxfId="9">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Resource" dataDxfId="64"/>
-    <tableColumn id="4" name="Relate Resource" dataDxfId="63"/>
-    <tableColumn id="2" name="Resource Id" dataDxfId="62">
+    <tableColumn id="3" name="Resource" dataDxfId="8"/>
+    <tableColumn id="4" name="Relate Resource" dataDxfId="7"/>
+    <tableColumn id="2" name="Resource Id" dataDxfId="6">
       <calculatedColumnFormula>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Name" dataDxfId="61"/>
-    <tableColumn id="6" name="Description" dataDxfId="60"/>
-    <tableColumn id="7" name="Method" dataDxfId="59"/>
-    <tableColumn id="8" name="Type" dataDxfId="58"/>
-    <tableColumn id="10" name="Relate Id" dataDxfId="57">
+    <tableColumn id="5" name="Name" dataDxfId="5"/>
+    <tableColumn id="6" name="Description" dataDxfId="4"/>
+    <tableColumn id="7" name="Method" dataDxfId="3"/>
+    <tableColumn id="8" name="Type" dataDxfId="2"/>
+    <tableColumn id="10" name="Relate Id" dataDxfId="1">
       <calculatedColumnFormula>VLOOKUP([Relate Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4605,47 +4602,47 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="ResourceForms" displayName="ResourceForms" ref="A1:G9" totalsRowShown="0" dataDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="ResourceForms" displayName="ResourceForms" ref="A1:G9" totalsRowShown="0" dataDxfId="60">
   <autoFilter ref="A1:G9"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="No" dataDxfId="55">
+    <tableColumn id="1" name="No" dataDxfId="59">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Resource ID" dataDxfId="54"/>
-    <tableColumn id="3" name="Resource Name" dataDxfId="53">
+    <tableColumn id="2" name="Resource ID" dataDxfId="58"/>
+    <tableColumn id="3" name="Resource Name" dataDxfId="57">
       <calculatedColumnFormula>VLOOKUP([Resource ID],ResourceTable[],2,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Form Name" dataDxfId="52"/>
-    <tableColumn id="6" name="Title" dataDxfId="51"/>
-    <tableColumn id="7" name="Action Text" dataDxfId="50"/>
-    <tableColumn id="8" name="Description" dataDxfId="49"/>
+    <tableColumn id="4" name="Form Name" dataDxfId="56"/>
+    <tableColumn id="6" name="Title" dataDxfId="55"/>
+    <tableColumn id="7" name="Action Text" dataDxfId="54"/>
+    <tableColumn id="8" name="Description" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="FormFields" displayName="FormFields" ref="A1:L33" totalsRowShown="0" dataDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="FormFields" displayName="FormFields" ref="A1:L33" totalsRowShown="0" dataDxfId="52">
   <autoFilter ref="A1:L33"/>
   <tableColumns count="12">
-    <tableColumn id="9" name="No" dataDxfId="47">
+    <tableColumn id="9" name="No" dataDxfId="51">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Form Id" dataDxfId="46"/>
-    <tableColumn id="7" name="Form Name" dataDxfId="45">
+    <tableColumn id="1" name="Form Id" dataDxfId="50"/>
+    <tableColumn id="7" name="Form Name" dataDxfId="49">
       <calculatedColumnFormula>VLOOKUP([Form Id],ResourceForms[],4,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Name" dataDxfId="44"/>
-    <tableColumn id="2" name="Type" dataDxfId="43"/>
-    <tableColumn id="5" name="Label" dataDxfId="42"/>
-    <tableColumn id="6" name="Collection" dataDxfId="41"/>
-    <tableColumn id="14" name="Attribute" dataDxfId="40">
+    <tableColumn id="4" name="Name" dataDxfId="48"/>
+    <tableColumn id="2" name="Type" dataDxfId="47"/>
+    <tableColumn id="5" name="Label" dataDxfId="46"/>
+    <tableColumn id="6" name="Collection" dataDxfId="45"/>
+    <tableColumn id="14" name="Attribute" dataDxfId="44">
       <calculatedColumnFormula>[Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Relation" dataDxfId="39"/>
-    <tableColumn id="11" name="Deep 1" dataDxfId="38"/>
-    <tableColumn id="12" name="Deep 2" dataDxfId="37"/>
-    <tableColumn id="13" name="Deep 3" dataDxfId="36"/>
+    <tableColumn id="10" name="Relation" dataDxfId="43"/>
+    <tableColumn id="11" name="Deep 1" dataDxfId="42"/>
+    <tableColumn id="12" name="Deep 2" dataDxfId="41"/>
+    <tableColumn id="13" name="Deep 3" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4938,8 +4935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11655,25 +11652,25 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A43:A46">
-    <cfRule type="duplicateValues" dxfId="118" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="112" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56:A59">
-    <cfRule type="duplicateValues" dxfId="117" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="111" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A157">
-    <cfRule type="duplicateValues" dxfId="116" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="110" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A128:A129">
-    <cfRule type="duplicateValues" dxfId="115" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="109" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A128:A129">
-    <cfRule type="duplicateValues" dxfId="114" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="108" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A130:A131">
-    <cfRule type="duplicateValues" dxfId="113" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="107" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A152:A153">
-    <cfRule type="duplicateValues" dxfId="18" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -11687,8 +11684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K373"/>
   <sheetViews>
-    <sheetView topLeftCell="A327" workbookViewId="0">
-      <selection activeCell="B336" sqref="B336:B346"/>
+    <sheetView topLeftCell="A354" workbookViewId="0">
+      <selection activeCell="K359" sqref="K359"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="15"/>
@@ -28122,10 +28119,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R314"/>
+  <dimension ref="A1:R322"/>
   <sheetViews>
-    <sheetView topLeftCell="B297" workbookViewId="0">
-      <selection activeCell="B311" sqref="B311:B314"/>
+    <sheetView topLeftCell="B300" workbookViewId="0">
+      <selection activeCell="B319" sqref="B319:B322"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -39589,6 +39586,326 @@
       <c r="P314" s="40"/>
       <c r="Q314" s="40"/>
       <c r="R314" s="40"/>
+    </row>
+    <row r="315" spans="1:18">
+      <c r="A315" s="42" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resources-33</v>
+      </c>
+      <c r="B315" s="40" t="s">
+        <v>220</v>
+      </c>
+      <c r="C315" s="42">
+        <f>COUNTIF($B$1:$B314,[Table Name])</f>
+        <v>33</v>
+      </c>
+      <c r="D315" s="43" t="s">
+        <v>748</v>
+      </c>
+      <c r="E315" s="43" t="s">
+        <v>752</v>
+      </c>
+      <c r="F315" s="43" t="s">
+        <v>755</v>
+      </c>
+      <c r="G315" s="43" t="s">
+        <v>558</v>
+      </c>
+      <c r="H315" s="43" t="s">
+        <v>756</v>
+      </c>
+      <c r="I315" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="J315" s="43"/>
+      <c r="K315" s="43"/>
+      <c r="L315" s="43"/>
+      <c r="M315" s="43"/>
+      <c r="N315" s="43"/>
+      <c r="O315" s="43"/>
+      <c r="P315" s="43"/>
+      <c r="Q315" s="43"/>
+      <c r="R315" s="43"/>
+    </row>
+    <row r="316" spans="1:18">
+      <c r="A316" s="42" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resources-34</v>
+      </c>
+      <c r="B316" s="40" t="s">
+        <v>220</v>
+      </c>
+      <c r="C316" s="42">
+        <f>COUNTIF($B$1:$B315,[Table Name])</f>
+        <v>34</v>
+      </c>
+      <c r="D316" s="43" t="s">
+        <v>749</v>
+      </c>
+      <c r="E316" s="43" t="s">
+        <v>753</v>
+      </c>
+      <c r="F316" s="43" t="s">
+        <v>760</v>
+      </c>
+      <c r="G316" s="43" t="s">
+        <v>558</v>
+      </c>
+      <c r="H316" s="43" t="s">
+        <v>757</v>
+      </c>
+      <c r="I316" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="J316" s="43"/>
+      <c r="K316" s="43"/>
+      <c r="L316" s="43"/>
+      <c r="M316" s="43"/>
+      <c r="N316" s="43"/>
+      <c r="O316" s="43"/>
+      <c r="P316" s="43"/>
+      <c r="Q316" s="43"/>
+      <c r="R316" s="43"/>
+    </row>
+    <row r="317" spans="1:18">
+      <c r="A317" s="42" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resources-35</v>
+      </c>
+      <c r="B317" s="40" t="s">
+        <v>220</v>
+      </c>
+      <c r="C317" s="42">
+        <f>COUNTIF($B$1:$B316,[Table Name])</f>
+        <v>35</v>
+      </c>
+      <c r="D317" s="43" t="s">
+        <v>750</v>
+      </c>
+      <c r="E317" s="43" t="s">
+        <v>754</v>
+      </c>
+      <c r="F317" s="43" t="s">
+        <v>746</v>
+      </c>
+      <c r="G317" s="43" t="s">
+        <v>558</v>
+      </c>
+      <c r="H317" s="43" t="s">
+        <v>758</v>
+      </c>
+      <c r="I317" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="J317" s="43"/>
+      <c r="K317" s="43"/>
+      <c r="L317" s="43"/>
+      <c r="M317" s="43"/>
+      <c r="N317" s="43"/>
+      <c r="O317" s="43"/>
+      <c r="P317" s="43"/>
+      <c r="Q317" s="43"/>
+      <c r="R317" s="43"/>
+    </row>
+    <row r="318" spans="1:18">
+      <c r="A318" s="22" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resources-36</v>
+      </c>
+      <c r="B318" s="40" t="s">
+        <v>220</v>
+      </c>
+      <c r="C318" s="22">
+        <f>COUNTIF($B$1:$B317,[Table Name])</f>
+        <v>36</v>
+      </c>
+      <c r="D318" s="40" t="s">
+        <v>751</v>
+      </c>
+      <c r="E318" s="40" t="s">
+        <v>761</v>
+      </c>
+      <c r="F318" s="40" t="s">
+        <v>747</v>
+      </c>
+      <c r="G318" s="40" t="s">
+        <v>558</v>
+      </c>
+      <c r="H318" s="40" t="s">
+        <v>759</v>
+      </c>
+      <c r="I318" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="J318" s="40"/>
+      <c r="K318" s="40"/>
+      <c r="L318" s="40"/>
+      <c r="M318" s="40"/>
+      <c r="N318" s="40"/>
+      <c r="O318" s="40"/>
+      <c r="P318" s="40"/>
+      <c r="Q318" s="40"/>
+      <c r="R318" s="40"/>
+    </row>
+    <row r="319" spans="1:18">
+      <c r="A319" s="42" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resource Relations-46</v>
+      </c>
+      <c r="B319" s="40" t="s">
+        <v>441</v>
+      </c>
+      <c r="C319" s="42">
+        <f>COUNTIF($B$1:$B318,[Table Name])</f>
+        <v>46</v>
+      </c>
+      <c r="D319" s="43">
+        <v>4</v>
+      </c>
+      <c r="E319" s="43" t="s">
+        <v>764</v>
+      </c>
+      <c r="F319" s="43" t="s">
+        <v>763</v>
+      </c>
+      <c r="G319" s="43" t="s">
+        <v>762</v>
+      </c>
+      <c r="H319" s="43" t="s">
+        <v>310</v>
+      </c>
+      <c r="I319" s="43">
+        <v>33</v>
+      </c>
+      <c r="J319" s="43"/>
+      <c r="K319" s="43"/>
+      <c r="L319" s="43"/>
+      <c r="M319" s="43"/>
+      <c r="N319" s="43"/>
+      <c r="O319" s="43"/>
+      <c r="P319" s="43"/>
+      <c r="Q319" s="43"/>
+      <c r="R319" s="43"/>
+    </row>
+    <row r="320" spans="1:18">
+      <c r="A320" s="42" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resource Relations-47</v>
+      </c>
+      <c r="B320" s="40" t="s">
+        <v>441</v>
+      </c>
+      <c r="C320" s="42">
+        <f>COUNTIF($B$1:$B319,[Table Name])</f>
+        <v>47</v>
+      </c>
+      <c r="D320" s="43">
+        <v>33</v>
+      </c>
+      <c r="E320" s="43" t="s">
+        <v>745</v>
+      </c>
+      <c r="F320" s="43" t="s">
+        <v>765</v>
+      </c>
+      <c r="G320" s="43" t="s">
+        <v>609</v>
+      </c>
+      <c r="H320" s="43" t="s">
+        <v>310</v>
+      </c>
+      <c r="I320" s="43">
+        <v>34</v>
+      </c>
+      <c r="J320" s="43"/>
+      <c r="K320" s="43"/>
+      <c r="L320" s="43"/>
+      <c r="M320" s="43"/>
+      <c r="N320" s="43"/>
+      <c r="O320" s="43"/>
+      <c r="P320" s="43"/>
+      <c r="Q320" s="43"/>
+      <c r="R320" s="43"/>
+    </row>
+    <row r="321" spans="1:18">
+      <c r="A321" s="42" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resource Relations-48</v>
+      </c>
+      <c r="B321" s="40" t="s">
+        <v>441</v>
+      </c>
+      <c r="C321" s="42">
+        <f>COUNTIF($B$1:$B320,[Table Name])</f>
+        <v>48</v>
+      </c>
+      <c r="D321" s="43">
+        <v>34</v>
+      </c>
+      <c r="E321" s="43" t="s">
+        <v>746</v>
+      </c>
+      <c r="F321" s="43" t="s">
+        <v>766</v>
+      </c>
+      <c r="G321" s="43" t="s">
+        <v>616</v>
+      </c>
+      <c r="H321" s="43" t="s">
+        <v>310</v>
+      </c>
+      <c r="I321" s="43">
+        <v>35</v>
+      </c>
+      <c r="J321" s="43"/>
+      <c r="K321" s="43"/>
+      <c r="L321" s="43"/>
+      <c r="M321" s="43"/>
+      <c r="N321" s="43"/>
+      <c r="O321" s="43"/>
+      <c r="P321" s="43"/>
+      <c r="Q321" s="43"/>
+      <c r="R321" s="43"/>
+    </row>
+    <row r="322" spans="1:18">
+      <c r="A322" s="22" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resource Relations-49</v>
+      </c>
+      <c r="B322" s="40" t="s">
+        <v>441</v>
+      </c>
+      <c r="C322" s="22">
+        <f>COUNTIF($B$1:$B321,[Table Name])</f>
+        <v>49</v>
+      </c>
+      <c r="D322" s="40">
+        <v>33</v>
+      </c>
+      <c r="E322" s="40" t="s">
+        <v>767</v>
+      </c>
+      <c r="F322" s="40" t="s">
+        <v>768</v>
+      </c>
+      <c r="G322" s="40" t="s">
+        <v>208</v>
+      </c>
+      <c r="H322" s="40" t="s">
+        <v>401</v>
+      </c>
+      <c r="I322" s="40">
+        <v>4</v>
+      </c>
+      <c r="J322" s="40"/>
+      <c r="K322" s="40"/>
+      <c r="L322" s="40"/>
+      <c r="M322" s="40"/>
+      <c r="N322" s="40"/>
+      <c r="O322" s="40"/>
+      <c r="P322" s="40"/>
+      <c r="Q322" s="40"/>
+      <c r="R322" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -40354,10 +40671,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34:G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -41296,9 +41613,121 @@
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
     </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="51">
+        <f>IFERROR($A33+1,1)</f>
+        <v>33</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>748</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>752</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>755</v>
+      </c>
+      <c r="E34" s="8" t="str">
+        <f>"Milestone\Appframe\Model"</f>
+        <v>Milestone\Appframe\Model</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>756</v>
+      </c>
+      <c r="G34" s="52" t="str">
+        <f>"id"</f>
+        <v>id</v>
+      </c>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="51">
+        <f>IFERROR($A34+1,1)</f>
+        <v>34</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>749</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>753</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>760</v>
+      </c>
+      <c r="E35" s="8" t="str">
+        <f>"Milestone\Appframe\Model"</f>
+        <v>Milestone\Appframe\Model</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>757</v>
+      </c>
+      <c r="G35" s="52" t="str">
+        <f>"id"</f>
+        <v>id</v>
+      </c>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="51">
+        <f>IFERROR($A35+1,1)</f>
+        <v>35</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>750</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>754</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>746</v>
+      </c>
+      <c r="E36" s="8" t="str">
+        <f>"Milestone\Appframe\Model"</f>
+        <v>Milestone\Appframe\Model</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>758</v>
+      </c>
+      <c r="G36" s="52" t="str">
+        <f>"id"</f>
+        <v>id</v>
+      </c>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="20">
+        <f>IFERROR($A36+1,1)</f>
+        <v>36</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>751</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>761</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>747</v>
+      </c>
+      <c r="E37" s="7" t="str">
+        <f>"Milestone\Appframe\Model"</f>
+        <v>Milestone\Appframe\Model</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>759</v>
+      </c>
+      <c r="G37" s="21" t="str">
+        <f>"id"</f>
+        <v>id</v>
+      </c>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F33">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F37">
       <formula1>ActualTableNames</formula1>
     </dataValidation>
   </dataValidations>
@@ -41311,10 +41740,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46:I46"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47:I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -42802,9 +43231,137 @@
         <v>32</v>
       </c>
     </row>
+    <row r="47" spans="1:9">
+      <c r="A47" s="20">
+        <f>IFERROR($A46+1,1)</f>
+        <v>46</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>748</v>
+      </c>
+      <c r="D47" s="7">
+        <f>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</f>
+        <v>4</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>764</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>763</v>
+      </c>
+      <c r="G47" s="22" t="s">
+        <v>762</v>
+      </c>
+      <c r="H47" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="I47" s="41">
+        <f>VLOOKUP([Relate Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" s="20">
+        <f>IFERROR($A47+1,1)</f>
+        <v>47</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>748</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>749</v>
+      </c>
+      <c r="D48" s="7">
+        <f>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</f>
+        <v>33</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>745</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>765</v>
+      </c>
+      <c r="G48" s="22" t="s">
+        <v>609</v>
+      </c>
+      <c r="H48" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="I48" s="41">
+        <f>VLOOKUP([Relate Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" s="20">
+        <f>IFERROR($A48+1,1)</f>
+        <v>48</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>749</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>750</v>
+      </c>
+      <c r="D49" s="7">
+        <f>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</f>
+        <v>34</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>746</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>766</v>
+      </c>
+      <c r="G49" s="22" t="s">
+        <v>616</v>
+      </c>
+      <c r="H49" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="I49" s="41">
+        <f>VLOOKUP([Relate Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="20">
+        <f>IFERROR($A49+1,1)</f>
+        <v>49</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>748</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="D50" s="7">
+        <f>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</f>
+        <v>33</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>767</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>768</v>
+      </c>
+      <c r="G50" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="H50" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="I50" s="41">
+        <f>VLOOKUP([Relate Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</f>
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C46">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C50">
       <formula1>Resources</formula1>
     </dataValidation>
   </dataValidations>
@@ -42820,8 +43377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T109"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:R10"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -42831,14 +43388,14 @@
   <sheetData>
     <row r="1" spans="1:20" s="38" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="48" t="s">
-        <v>747</v>
+        <v>441</v>
       </c>
       <c r="B1" s="48"/>
       <c r="C1" s="48"/>
       <c r="D1" s="48"/>
       <c r="E1" s="49" t="str">
         <f>"\"&amp;VLOOKUP($A$1,SeedMap[],3,0)&amp;"\"&amp;VLOOKUP($A$1,SeedMap[],4,0)&amp;"::"&amp;VLOOKUP($A$1,SeedMap[],5,0)&amp;"()"</f>
-        <v>\Milestone\Appframe\Model\ResourceMetric::truncate()</v>
+        <v>\Milestone\Appframe\Model\ResourceRelation::truncate()</v>
       </c>
       <c r="F1" s="49"/>
       <c r="G1" s="49"/>
@@ -42990,39 +43547,39 @@
       </c>
       <c r="E5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0))</f>
-        <v>resource_list</v>
+        <v>description</v>
       </c>
       <c r="F5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0))</f>
-        <v>aggregates</v>
+        <v>method</v>
       </c>
       <c r="G5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0))</f>
-        <v>aggregate_field</v>
+        <v>type</v>
       </c>
       <c r="H5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],H$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],H$4+$B$4,0))</f>
-        <v>aggregate_distinct</v>
+        <v>relate_resource</v>
       </c>
       <c r="I5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],I$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],I$4+$B$4,0))</f>
-        <v>date_field</v>
+        <v/>
       </c>
       <c r="J5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],J$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],J$4+$B$4,0))</f>
-        <v>range_unit</v>
+        <v/>
       </c>
       <c r="K5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],K$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],K$4+$B$4,0))</f>
-        <v>range</v>
+        <v/>
       </c>
       <c r="L5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],L$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],L$4+$B$4,0))</f>
-        <v>groupby</v>
+        <v/>
       </c>
       <c r="M5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],M$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],M$4+$B$4,0))</f>
-        <v>method</v>
+        <v/>
       </c>
       <c r="N5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],N$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],N$4+$B$4,0))</f>
@@ -43096,7 +43653,7 @@
       <c r="A8" s="32"/>
       <c r="B8" s="47" t="str">
         <f>$E$1</f>
-        <v>\Milestone\Appframe\Model\ResourceMetric::truncate()</v>
+        <v>\Milestone\Appframe\Model\ResourceRelation::truncate()</v>
       </c>
       <c r="C8" s="47"/>
       <c r="D8" s="47"/>
@@ -43121,31 +43678,31 @@
       </c>
       <c r="B9" s="30" t="str">
         <f ca="1">IF($B8="","",IF($B8=";",$I$3,IF($B8=$I$3,"",IF(ISNA(VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),1,0)),";",$S$4))))</f>
-        <v>;</v>
+        <v>-&gt;create([</v>
       </c>
       <c r="C9" s="33" t="str">
         <f ca="1">IF(AND($B9=$S$4,C$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),C$4+$B$4,0)="","","'"&amp;C$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),C$4+$B$4,0)&amp;"', "),"")</f>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '1', </v>
       </c>
       <c r="D9" s="33" t="str">
         <f t="shared" ref="D9:Q24" ca="1" si="0">IF(AND($B9=$S$4,D$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),D$4+$B$4,0)="","","'"&amp;D$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),D$4+$B$4,0)&amp;"', "),"")</f>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'User Groups', </v>
       </c>
       <c r="E9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Which groups this user belongs to', </v>
       </c>
       <c r="F9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Groups', </v>
       </c>
       <c r="G9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
       </c>
       <c r="H9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '2', </v>
       </c>
       <c r="I9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -43185,7 +43742,7 @@
       </c>
       <c r="R9" s="33" t="str">
         <f ca="1">IF(B9=$S$4,$T$4,"")</f>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="10" spans="1:20">
@@ -43194,31 +43751,31 @@
       </c>
       <c r="B10" s="30" t="str">
         <f t="shared" ref="B10:B73" ca="1" si="1">IF($B9="","",IF($B9=";",$I$3,IF($B9=$I$3,"",IF(ISNA(VLOOKUP($A$1&amp;"-"&amp;$A10,INDIRECT($E$2),1,0)),";",$S$4))))</f>
-        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
+        <v>-&gt;create([</v>
       </c>
       <c r="C10" s="33" t="str">
         <f ca="1">IF(AND($B10=$S$4,C$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A10,INDIRECT($E$2),C$4+$B$4,0)="","","'"&amp;C$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A10,INDIRECT($E$2),C$4+$B$4,0)&amp;"', "),"")</f>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '2', </v>
       </c>
       <c r="D10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Group Users', </v>
       </c>
       <c r="E10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'List of users belongs to this group', </v>
       </c>
       <c r="F10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Users', </v>
       </c>
       <c r="G10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
       </c>
       <c r="H10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '1', </v>
       </c>
       <c r="I10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -43258,7 +43815,7 @@
       </c>
       <c r="R10" s="33" t="str">
         <f t="shared" ref="R10:R73" ca="1" si="2">IF(B10=$S$4,$T$4,"")</f>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -43267,31 +43824,31 @@
       </c>
       <c r="B11" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C11" s="33" t="str">
         <f t="shared" ref="C11:G74" ca="1" si="3">IF(AND($B11=$S$4,C$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A11,INDIRECT($E$2),C$4+$B$4,0)="","","'"&amp;C$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A11,INDIRECT($E$2),C$4+$B$4,0)&amp;"', "),"")</f>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '2', </v>
       </c>
       <c r="D11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Group Roles', </v>
       </c>
       <c r="E11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Roles assigneed to this group', </v>
       </c>
       <c r="F11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Roles', </v>
       </c>
       <c r="G11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
       </c>
       <c r="H11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '3', </v>
       </c>
       <c r="I11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -43331,7 +43888,7 @@
       </c>
       <c r="R11" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -43340,31 +43897,31 @@
       </c>
       <c r="B12" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C12" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '3', </v>
       </c>
       <c r="D12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Role Groups', </v>
       </c>
       <c r="E12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Details of groups this role assigned to', </v>
       </c>
       <c r="F12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Groups', </v>
       </c>
       <c r="G12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
       </c>
       <c r="H12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '2', </v>
       </c>
       <c r="I12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -43404,7 +43961,7 @@
       </c>
       <c r="R12" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -43413,31 +43970,31 @@
       </c>
       <c r="B13" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C13" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '3', </v>
       </c>
       <c r="D13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Role Resource', </v>
       </c>
       <c r="E13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Resources assigned to a role', </v>
       </c>
       <c r="F13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Resources', </v>
       </c>
       <c r="G13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '11', </v>
       </c>
       <c r="I13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -43477,7 +44034,7 @@
       </c>
       <c r="R13" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -43486,31 +44043,31 @@
       </c>
       <c r="B14" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C14" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '4', </v>
       </c>
       <c r="D14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Resource Roles', </v>
       </c>
       <c r="E14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'The details of roles who have access to this resource', </v>
       </c>
       <c r="F14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Roles', </v>
       </c>
       <c r="G14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
       </c>
       <c r="H14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '3', </v>
       </c>
       <c r="I14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -43550,7 +44107,7 @@
       </c>
       <c r="R14" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -43559,31 +44116,31 @@
       </c>
       <c r="B15" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C15" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '4', </v>
       </c>
       <c r="D15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Resource Actions', </v>
       </c>
       <c r="E15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Get actions available for the resource', </v>
       </c>
       <c r="F15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Actions', </v>
       </c>
       <c r="G15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '7', </v>
       </c>
       <c r="I15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -43623,7 +44180,7 @@
       </c>
       <c r="R15" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="16" spans="1:20">
@@ -43632,31 +44189,31 @@
       </c>
       <c r="B16" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C16" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '7', </v>
       </c>
       <c r="D16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Resource Action Methods', </v>
       </c>
       <c r="E16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Handler details of an action', </v>
       </c>
       <c r="F16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Method', </v>
       </c>
       <c r="G16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasOne', </v>
       </c>
       <c r="H16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '8', </v>
       </c>
       <c r="I16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -43696,7 +44253,7 @@
       </c>
       <c r="R16" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="17" spans="1:18">
@@ -43705,31 +44262,31 @@
       </c>
       <c r="B17" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C17" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '7', </v>
       </c>
       <c r="D17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Resource Action Lists', </v>
       </c>
       <c r="E17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Lists where action available', </v>
       </c>
       <c r="F17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Lists', </v>
       </c>
       <c r="G17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '9', </v>
       </c>
       <c r="I17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -43769,7 +44326,7 @@
       </c>
       <c r="R17" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="18" spans="1:18">
@@ -43778,31 +44335,31 @@
       </c>
       <c r="B18" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C18" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '7', </v>
       </c>
       <c r="D18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Resource Action Data', </v>
       </c>
       <c r="E18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Resource data where action available', </v>
       </c>
       <c r="F18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Data', </v>
       </c>
       <c r="G18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '10', </v>
       </c>
       <c r="I18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -43842,7 +44399,7 @@
       </c>
       <c r="R18" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="19" spans="1:18">
@@ -43851,31 +44408,31 @@
       </c>
       <c r="B19" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C19" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '5', </v>
       </c>
       <c r="D19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Organisation Contacts', </v>
       </c>
       <c r="E19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Contact details of organisation', </v>
       </c>
       <c r="F19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Contacts', </v>
       </c>
       <c r="G19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '6', </v>
       </c>
       <c r="I19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -43915,7 +44472,7 @@
       </c>
       <c r="R19" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="20" spans="1:18">
@@ -43924,31 +44481,31 @@
       </c>
       <c r="B20" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C20" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '11', </v>
       </c>
       <c r="D20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Resource Details', </v>
       </c>
       <c r="E20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Resource details', </v>
       </c>
       <c r="F20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Resource', </v>
       </c>
       <c r="G20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
       </c>
       <c r="I20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -43988,7 +44545,7 @@
       </c>
       <c r="R20" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="21" spans="1:18">
@@ -43997,31 +44554,31 @@
       </c>
       <c r="B21" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C21" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '4', </v>
       </c>
       <c r="D21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Resource Forms', </v>
       </c>
       <c r="E21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Forms available for a resource', </v>
       </c>
       <c r="F21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Forms', </v>
       </c>
       <c r="G21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '12', </v>
       </c>
       <c r="I21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44061,7 +44618,7 @@
       </c>
       <c r="R21" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="22" spans="1:18">
@@ -44070,31 +44627,31 @@
       </c>
       <c r="B22" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C22" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '12', </v>
       </c>
       <c r="D22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Form Fields', </v>
       </c>
       <c r="E22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Fields associated with a form', </v>
       </c>
       <c r="F22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Fields', </v>
       </c>
       <c r="G22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '13', </v>
       </c>
       <c r="I22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44134,7 +44691,7 @@
       </c>
       <c r="R22" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="23" spans="1:18">
@@ -44143,31 +44700,31 @@
       </c>
       <c r="B23" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C23" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '13', </v>
       </c>
       <c r="D23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Field Attributes', </v>
       </c>
       <c r="E23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Attributes of Field', </v>
       </c>
       <c r="F23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Attributes', </v>
       </c>
       <c r="G23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '14', </v>
       </c>
       <c r="I23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44207,7 +44764,7 @@
       </c>
       <c r="R23" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="24" spans="1:18">
@@ -44216,31 +44773,31 @@
       </c>
       <c r="B24" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C24" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '13', </v>
       </c>
       <c r="D24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Field Options', </v>
       </c>
       <c r="E24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Options of Field', </v>
       </c>
       <c r="F24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Options', </v>
       </c>
       <c r="G24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasOne', </v>
       </c>
       <c r="H24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '15', </v>
       </c>
       <c r="I24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44280,7 +44837,7 @@
       </c>
       <c r="R24" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="25" spans="1:18">
@@ -44289,31 +44846,31 @@
       </c>
       <c r="B25" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '13', </v>
       </c>
       <c r="D25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Field Validations', </v>
       </c>
       <c r="E25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Validation details of field', </v>
       </c>
       <c r="F25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Validations', </v>
       </c>
       <c r="G25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H25" s="33" t="str">
         <f t="shared" ref="H25:K88" ca="1" si="4">IF(AND($B25=$S$4,H$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A25,INDIRECT($E$2),H$4+$B$4,0)="","","'"&amp;H$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A25,INDIRECT($E$2),H$4+$B$4,0)&amp;"', "),"")</f>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '16', </v>
       </c>
       <c r="I25" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -44353,7 +44910,7 @@
       </c>
       <c r="R25" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="26" spans="1:18">
@@ -44362,31 +44919,31 @@
       </c>
       <c r="B26" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '12', </v>
       </c>
       <c r="D26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'From Resource', </v>
       </c>
       <c r="E26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Resource this form belongs to', </v>
       </c>
       <c r="F26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Resource', </v>
       </c>
       <c r="G26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H26" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
       </c>
       <c r="I26" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -44426,7 +44983,7 @@
       </c>
       <c r="R26" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="27" spans="1:18">
@@ -44435,31 +44992,31 @@
       </c>
       <c r="B27" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '12', </v>
       </c>
       <c r="D27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Form Defaults', </v>
       </c>
       <c r="E27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Predefined values for a form', </v>
       </c>
       <c r="F27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Defaults', </v>
       </c>
       <c r="G27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H27" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '17', </v>
       </c>
       <c r="I27" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -44499,7 +45056,7 @@
       </c>
       <c r="R27" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="28" spans="1:18">
@@ -44508,31 +45065,31 @@
       </c>
       <c r="B28" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '13', </v>
       </c>
       <c r="D28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Field Data', </v>
       </c>
       <c r="E28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Fields Database binding details', </v>
       </c>
       <c r="F28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Data', </v>
       </c>
       <c r="G28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasOne', </v>
       </c>
       <c r="H28" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '18', </v>
       </c>
       <c r="I28" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -44572,7 +45129,7 @@
       </c>
       <c r="R28" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="29" spans="1:18">
@@ -44581,31 +45138,31 @@
       </c>
       <c r="B29" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '4', </v>
       </c>
       <c r="D29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Resource Relations', </v>
       </c>
       <c r="E29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Relation of  a resource to another resource', </v>
       </c>
       <c r="F29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Relations', </v>
       </c>
       <c r="G29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H29" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
       </c>
       <c r="I29" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -44645,7 +45202,7 @@
       </c>
       <c r="R29" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="30" spans="1:18">
@@ -44654,31 +45211,31 @@
       </c>
       <c r="B30" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '18', </v>
       </c>
       <c r="D30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Bind Data Relation', </v>
       </c>
       <c r="E30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Relation to which the data to be bind', </v>
       </c>
       <c r="F30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
       </c>
       <c r="G30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H30" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
       </c>
       <c r="I30" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -44718,7 +45275,7 @@
       </c>
       <c r="R30" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="31" spans="1:18">
@@ -44727,31 +45284,31 @@
       </c>
       <c r="B31" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '17', </v>
       </c>
       <c r="D31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Default Data Resource', </v>
       </c>
       <c r="E31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Resource to which the forms predefined data to be bind', </v>
       </c>
       <c r="F31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
       </c>
       <c r="G31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H31" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
       </c>
       <c r="I31" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -44791,7 +45348,7 @@
       </c>
       <c r="R31" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="32" spans="1:18">
@@ -44800,31 +45357,31 @@
       </c>
       <c r="B32" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '19', </v>
       </c>
       <c r="D32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Resource Details', </v>
       </c>
       <c r="E32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Resource details of a list', </v>
       </c>
       <c r="F32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Resource', </v>
       </c>
       <c r="G32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H32" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
       </c>
       <c r="I32" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -44864,7 +45421,7 @@
       </c>
       <c r="R32" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="33" spans="1:18">
@@ -44873,31 +45430,31 @@
       </c>
       <c r="B33" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '19', </v>
       </c>
       <c r="D33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'List Relations', </v>
       </c>
       <c r="E33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Relations to be loaded on accessing list', </v>
       </c>
       <c r="F33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Relations', </v>
       </c>
       <c r="G33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H33" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '20', </v>
       </c>
       <c r="I33" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -44937,7 +45494,7 @@
       </c>
       <c r="R33" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="34" spans="1:18">
@@ -44946,31 +45503,31 @@
       </c>
       <c r="B34" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '4', </v>
       </c>
       <c r="D34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Resource Scopes', </v>
       </c>
       <c r="E34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Scopes available on a Resource', </v>
       </c>
       <c r="F34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Scopes', </v>
       </c>
       <c r="G34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H34" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '21', </v>
       </c>
       <c r="I34" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -45010,7 +45567,7 @@
       </c>
       <c r="R34" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="35" spans="1:18">
@@ -45019,31 +45576,31 @@
       </c>
       <c r="B35" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '19', </v>
       </c>
       <c r="D35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'List Scopes', </v>
       </c>
       <c r="E35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Scopes by which a list to be filtered', </v>
       </c>
       <c r="F35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Scopes', </v>
       </c>
       <c r="G35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
       </c>
       <c r="H35" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '21', </v>
       </c>
       <c r="I35" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -45083,7 +45640,7 @@
       </c>
       <c r="R35" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="36" spans="1:18">
@@ -45092,31 +45649,31 @@
       </c>
       <c r="B36" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '23', </v>
       </c>
       <c r="D36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Data Relation', </v>
       </c>
       <c r="E36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Relations to be loaded on a data view', </v>
       </c>
       <c r="F36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Relations', </v>
       </c>
       <c r="G36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H36" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '24', </v>
       </c>
       <c r="I36" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -45156,7 +45713,7 @@
       </c>
       <c r="R36" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="37" spans="1:18">
@@ -45165,31 +45722,31 @@
       </c>
       <c r="B37" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '23', </v>
       </c>
       <c r="D37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Resource Details', </v>
       </c>
       <c r="E37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Details of resource of a record', </v>
       </c>
       <c r="F37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Resource', </v>
       </c>
       <c r="G37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H37" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
       </c>
       <c r="I37" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -45229,7 +45786,7 @@
       </c>
       <c r="R37" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="38" spans="1:18">
@@ -45238,31 +45795,31 @@
       </c>
       <c r="B38" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '19', </v>
       </c>
       <c r="D38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'List Layout', </v>
       </c>
       <c r="E38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Layout of a list', </v>
       </c>
       <c r="F38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Layout', </v>
       </c>
       <c r="G38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H38" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '25', </v>
       </c>
       <c r="I38" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -45302,7 +45859,7 @@
       </c>
       <c r="R38" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="39" spans="1:18">
@@ -45311,31 +45868,31 @@
       </c>
       <c r="B39" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C39" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '26', </v>
       </c>
       <c r="D39" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Nested Relation', </v>
       </c>
       <c r="E39" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Nested Relation', </v>
       </c>
       <c r="F39" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Nest', </v>
       </c>
       <c r="G39" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H39" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
       </c>
       <c r="I39" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -45375,7 +45932,7 @@
       </c>
       <c r="R39" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="40" spans="1:18">
@@ -45384,31 +45941,31 @@
       </c>
       <c r="B40" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C40" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '26', </v>
       </c>
       <c r="D40" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Related Resource', </v>
       </c>
       <c r="E40" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Related Resource Details', </v>
       </c>
       <c r="F40" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
       </c>
       <c r="G40" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H40" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
       </c>
       <c r="I40" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -45448,7 +46005,7 @@
       </c>
       <c r="R40" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="41" spans="1:18">
@@ -45457,31 +46014,31 @@
       </c>
       <c r="B41" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C41" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '26', </v>
       </c>
       <c r="D41" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Form Layout', </v>
       </c>
       <c r="E41" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Layout details', </v>
       </c>
       <c r="F41" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Layout', </v>
       </c>
       <c r="G41" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H41" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '27', </v>
       </c>
       <c r="I41" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -45521,7 +46078,7 @@
       </c>
       <c r="R41" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="42" spans="1:18">
@@ -45530,31 +46087,31 @@
       </c>
       <c r="B42" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C42" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '23', </v>
       </c>
       <c r="D42" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Data View Section', </v>
       </c>
       <c r="E42" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Section details of data view', </v>
       </c>
       <c r="F42" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Sections', </v>
       </c>
       <c r="G42" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H42" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '28', </v>
       </c>
       <c r="I42" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -45594,7 +46151,7 @@
       </c>
       <c r="R42" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="43" spans="1:18">
@@ -45603,31 +46160,31 @@
       </c>
       <c r="B43" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C43" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '26', </v>
       </c>
       <c r="D43" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Data View Section Items', </v>
       </c>
       <c r="E43" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Items of a data view section', </v>
       </c>
       <c r="F43" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Items', </v>
       </c>
       <c r="G43" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H43" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '29', </v>
       </c>
       <c r="I43" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -45667,7 +46224,7 @@
       </c>
       <c r="R43" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="44" spans="1:18">
@@ -45676,31 +46233,31 @@
       </c>
       <c r="B44" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C44" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '28', </v>
       </c>
       <c r="D44" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Data Relation', </v>
       </c>
       <c r="E44" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'View relation of a data', </v>
       </c>
       <c r="F44" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
       </c>
       <c r="G44" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H44" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
       </c>
       <c r="I44" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -45740,7 +46297,7 @@
       </c>
       <c r="R44" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="45" spans="1:18">
@@ -45749,31 +46306,31 @@
       </c>
       <c r="B45" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C45" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '29', </v>
       </c>
       <c r="D45" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Data item relation', </v>
       </c>
       <c r="E45" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'View relation of a data item', </v>
       </c>
       <c r="F45" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
       </c>
       <c r="G45" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H45" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
       </c>
       <c r="I45" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -45813,7 +46370,7 @@
       </c>
       <c r="R45" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="46" spans="1:18">
@@ -45822,31 +46379,31 @@
       </c>
       <c r="B46" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C46" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '26', </v>
       </c>
       <c r="D46" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Owner Relation', </v>
       </c>
       <c r="E46" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'View the owner resource', </v>
       </c>
       <c r="F46" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Owner', </v>
       </c>
       <c r="G46" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H46" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
       </c>
       <c r="I46" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -45886,7 +46443,7 @@
       </c>
       <c r="R46" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="47" spans="1:18">
@@ -45895,31 +46452,31 @@
       </c>
       <c r="B47" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C47" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '12', </v>
       </c>
       <c r="D47" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Collections', </v>
       </c>
       <c r="E47" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Collection/Detail form', </v>
       </c>
       <c r="F47" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Collections', </v>
       </c>
       <c r="G47" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H47" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '30', </v>
       </c>
       <c r="I47" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -45959,7 +46516,7 @@
       </c>
       <c r="R47" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="48" spans="1:18">
@@ -45968,31 +46525,31 @@
       </c>
       <c r="B48" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C48" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '30', </v>
       </c>
       <c r="D48" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Collection Form', </v>
       </c>
       <c r="E48" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Collection Form', </v>
       </c>
       <c r="F48" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Form', </v>
       </c>
       <c r="G48" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H48" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '12', </v>
       </c>
       <c r="I48" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -46032,7 +46589,7 @@
       </c>
       <c r="R48" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="49" spans="1:18">
@@ -46041,31 +46598,31 @@
       </c>
       <c r="B49" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C49" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '30', </v>
       </c>
       <c r="D49" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Relation', </v>
       </c>
       <c r="E49" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Details of Relation', </v>
       </c>
       <c r="F49" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
       </c>
       <c r="G49" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H49" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
       </c>
       <c r="I49" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -46105,7 +46662,7 @@
       </c>
       <c r="R49" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="50" spans="1:18">
@@ -46114,31 +46671,31 @@
       </c>
       <c r="B50" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C50" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '15', </v>
       </c>
       <c r="D50" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Field', </v>
       </c>
       <c r="E50" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Field details', </v>
       </c>
       <c r="F50" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Field', </v>
       </c>
       <c r="G50" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H50" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '13', </v>
       </c>
       <c r="I50" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -46178,7 +46735,7 @@
       </c>
       <c r="R50" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="51" spans="1:18">
@@ -46187,31 +46744,31 @@
       </c>
       <c r="B51" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C51" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '13', </v>
       </c>
       <c r="D51" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Form', </v>
       </c>
       <c r="E51" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Form details', </v>
       </c>
       <c r="F51" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Form', </v>
       </c>
       <c r="G51" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H51" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '12', </v>
       </c>
       <c r="I51" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -46251,7 +46808,7 @@
       </c>
       <c r="R51" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="52" spans="1:18">
@@ -46260,31 +46817,31 @@
       </c>
       <c r="B52" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C52" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '19', </v>
       </c>
       <c r="D52" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'List Search', </v>
       </c>
       <c r="E52" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Search fields for a list', </v>
       </c>
       <c r="F52" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Search', </v>
       </c>
       <c r="G52" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H52" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '31', </v>
       </c>
       <c r="I52" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -46324,7 +46881,7 @@
       </c>
       <c r="R52" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="53" spans="1:18">
@@ -46333,31 +46890,31 @@
       </c>
       <c r="B53" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C53" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '13', </v>
       </c>
       <c r="D53" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Depending Fields', </v>
       </c>
       <c r="E53" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Dependent fields', </v>
       </c>
       <c r="F53" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Depends', </v>
       </c>
       <c r="G53" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H53" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '32', </v>
       </c>
       <c r="I53" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -46397,7 +46954,7 @@
       </c>
       <c r="R53" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="54" spans="1:18">
@@ -46406,31 +46963,31 @@
       </c>
       <c r="B54" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C54" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '4', </v>
       </c>
       <c r="D54" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Resource Dashboards', </v>
       </c>
       <c r="E54" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Dashboards of a Resource', </v>
       </c>
       <c r="F54" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Dashboards', </v>
       </c>
       <c r="G54" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H54" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '33', </v>
       </c>
       <c r="I54" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -46470,7 +47027,7 @@
       </c>
       <c r="R54" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="55" spans="1:18">
@@ -46479,31 +47036,31 @@
       </c>
       <c r="B55" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C55" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '33', </v>
       </c>
       <c r="D55" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Dashboard Sections', </v>
       </c>
       <c r="E55" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Sections of a dashboard', </v>
       </c>
       <c r="F55" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Sections', </v>
       </c>
       <c r="G55" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H55" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '34', </v>
       </c>
       <c r="I55" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -46543,7 +47100,7 @@
       </c>
       <c r="R55" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="56" spans="1:18">
@@ -46552,31 +47109,31 @@
       </c>
       <c r="B56" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C56" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '34', </v>
       </c>
       <c r="D56" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Dashboard Section Items', </v>
       </c>
       <c r="E56" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Items of a dashboard section', </v>
       </c>
       <c r="F56" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Items', </v>
       </c>
       <c r="G56" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H56" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '35', </v>
       </c>
       <c r="I56" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -46616,7 +47173,7 @@
       </c>
       <c r="R56" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="57" spans="1:18">
@@ -46625,31 +47182,31 @@
       </c>
       <c r="B57" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C57" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '33', </v>
       </c>
       <c r="D57" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Dashboard Resource', </v>
       </c>
       <c r="E57" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Resource details of a dashboard', </v>
       </c>
       <c r="F57" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Resource', </v>
       </c>
       <c r="G57" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H57" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
       </c>
       <c r="I57" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -46689,7 +47246,7 @@
       </c>
       <c r="R57" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="58" spans="1:18">
@@ -46698,7 +47255,7 @@
       </c>
       <c r="B58" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>;</v>
       </c>
       <c r="C58" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -46771,7 +47328,7 @@
       </c>
       <c r="B59" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
       </c>
       <c r="C59" s="33" t="str">
         <f t="shared" ca="1" si="3"/>

</xml_diff>

<commit_message>
Dashboard also added to Action Method
</commit_message>
<xml_diff>
--- a/Helper.xlsx
+++ b/Helper.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Tables" sheetId="1" r:id="rId1"/>
@@ -1966,9 +1966,6 @@
     <t>Owner</t>
   </si>
   <si>
-    <t>['Method','Form','List','Data','FormWithData','ListRelation','AddRelation','ManageRelation']</t>
-  </si>
-  <si>
     <t>field_option_enum</t>
   </si>
   <si>
@@ -2345,6 +2342,9 @@
   </si>
   <si>
     <t>Resource details of a dashboard</t>
+  </si>
+  <si>
+    <t>['Method','Dashboard','Form','List','Data','FormWithData','ListRelation','AddRelation','ManageRelation']</t>
   </si>
 </sst>
 </file>
@@ -2554,6 +2554,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -2570,331 +2576,11 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="124">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -3466,6 +3152,151 @@
         <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
       </font>
     </dxf>
     <dxf>
@@ -4068,6 +3899,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -4107,6 +3939,174 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -4403,56 +4403,56 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="ResourceActions" displayName="ResourceActions" ref="A1:P9" totalsRowShown="0" dataDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="ResourceActions" displayName="ResourceActions" ref="A1:P9" totalsRowShown="0" dataDxfId="16">
   <autoFilter ref="A1:P9"/>
   <tableColumns count="16">
-    <tableColumn id="1" name="No" dataDxfId="38">
+    <tableColumn id="1" name="No" dataDxfId="15">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Resource" dataDxfId="37"/>
-    <tableColumn id="13" name="Resource Id" dataDxfId="36">
+    <tableColumn id="2" name="Resource" dataDxfId="14"/>
+    <tableColumn id="13" name="Resource Id" dataDxfId="13">
       <calculatedColumnFormula>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Action Name" dataDxfId="35"/>
-    <tableColumn id="4" name="Description" dataDxfId="34"/>
-    <tableColumn id="5" name="Action Title" dataDxfId="33"/>
-    <tableColumn id="6" name="Button Type" dataDxfId="32"/>
-    <tableColumn id="7" name="Menu" dataDxfId="31"/>
-    <tableColumn id="8" name="Icon" dataDxfId="30"/>
-    <tableColumn id="9" name="Set" dataDxfId="29"/>
-    <tableColumn id="14" name="Action Type" dataDxfId="28"/>
-    <tableColumn id="15" name="ID1" dataDxfId="27"/>
-    <tableColumn id="16" name="ID2" dataDxfId="26"/>
-    <tableColumn id="10" name="On" dataDxfId="25"/>
-    <tableColumn id="11" name="Confirm" dataDxfId="24"/>
-    <tableColumn id="12" name="handler" dataDxfId="23"/>
+    <tableColumn id="3" name="Action Name" dataDxfId="12"/>
+    <tableColumn id="4" name="Description" dataDxfId="11"/>
+    <tableColumn id="5" name="Action Title" dataDxfId="10"/>
+    <tableColumn id="6" name="Button Type" dataDxfId="9"/>
+    <tableColumn id="7" name="Menu" dataDxfId="8"/>
+    <tableColumn id="8" name="Icon" dataDxfId="7"/>
+    <tableColumn id="9" name="Set" dataDxfId="6"/>
+    <tableColumn id="14" name="Action Type" dataDxfId="5"/>
+    <tableColumn id="15" name="ID1" dataDxfId="4"/>
+    <tableColumn id="16" name="ID2" dataDxfId="3"/>
+    <tableColumn id="10" name="On" dataDxfId="2"/>
+    <tableColumn id="11" name="Confirm" dataDxfId="1"/>
+    <tableColumn id="12" name="handler" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Columns" displayName="Columns" ref="A1:I157" totalsRowShown="0" dataDxfId="106">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Columns" displayName="Columns" ref="A1:I157" totalsRowShown="0" dataDxfId="105">
   <autoFilter ref="A1:I157">
     <filterColumn colId="0"/>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" name="Column" dataDxfId="105"/>
-    <tableColumn id="2" name="Type" dataDxfId="104"/>
-    <tableColumn id="3" name="Name" dataDxfId="103"/>
-    <tableColumn id="4" name="Length/Enum" dataDxfId="102"/>
-    <tableColumn id="5" name="Method1" dataDxfId="101"/>
-    <tableColumn id="6" name="Method2" dataDxfId="100"/>
-    <tableColumn id="7" name="Method3" dataDxfId="99"/>
-    <tableColumn id="8" name="Method4" dataDxfId="98"/>
-    <tableColumn id="9" name="Method5" dataDxfId="97"/>
+    <tableColumn id="1" name="Column" dataDxfId="104"/>
+    <tableColumn id="2" name="Type" dataDxfId="103"/>
+    <tableColumn id="3" name="Name" dataDxfId="102"/>
+    <tableColumn id="4" name="Length/Enum" dataDxfId="101"/>
+    <tableColumn id="5" name="Method1" dataDxfId="100"/>
+    <tableColumn id="6" name="Method2" dataDxfId="99"/>
+    <tableColumn id="7" name="Method3" dataDxfId="98"/>
+    <tableColumn id="8" name="Method4" dataDxfId="97"/>
+    <tableColumn id="9" name="Method5" dataDxfId="96"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TableFields" displayName="TableFields" ref="A1:K373" totalsRowShown="0" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TableFields" displayName="TableFields" ref="A1:K373" totalsRowShown="0" dataDxfId="95">
   <autoFilter ref="A1:K373">
     <filterColumn colId="0">
       <filters>
@@ -4462,33 +4462,33 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="11">
-    <tableColumn id="2" name="Table" dataDxfId="21"/>
-    <tableColumn id="3" name="Field" dataDxfId="20"/>
-    <tableColumn id="5" name="Type" dataDxfId="19">
+    <tableColumn id="2" name="Table" dataDxfId="94"/>
+    <tableColumn id="3" name="Field" dataDxfId="93"/>
+    <tableColumn id="5" name="Type" dataDxfId="92">
       <calculatedColumnFormula>VLOOKUP([Field],Columns[],2,0)&amp;"("</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Name" dataDxfId="18">
+    <tableColumn id="4" name="Name" dataDxfId="91">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Arg2" dataDxfId="17">
+    <tableColumn id="6" name="Arg2" dataDxfId="90">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Method1" dataDxfId="16">
+    <tableColumn id="7" name="Method1" dataDxfId="89">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Method2" dataDxfId="15">
+    <tableColumn id="8" name="Method2" dataDxfId="88">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Method3" dataDxfId="14">
+    <tableColumn id="9" name="Method3" dataDxfId="87">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Method4" dataDxfId="13">
+    <tableColumn id="10" name="Method4" dataDxfId="86">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Method5" dataDxfId="12">
+    <tableColumn id="11" name="Method5" dataDxfId="85">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Statement" dataDxfId="11">
+    <tableColumn id="12" name="Statement" dataDxfId="84">
       <calculatedColumnFormula>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4497,51 +4497,51 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R322" totalsRowShown="0" headerRowDxfId="96" dataDxfId="95">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R322" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
   <autoFilter ref="A1:R322">
     <filterColumn colId="1"/>
   </autoFilter>
   <tableColumns count="18">
-    <tableColumn id="19" name="TRCode" dataDxfId="94">
+    <tableColumn id="19" name="TRCode" dataDxfId="81">
       <calculatedColumnFormula>[Table Name]&amp;"-"&amp;[Record No]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Table Name" dataDxfId="93"/>
-    <tableColumn id="2" name="Record No" dataDxfId="92">
+    <tableColumn id="1" name="Table Name" dataDxfId="80"/>
+    <tableColumn id="2" name="Record No" dataDxfId="79">
       <calculatedColumnFormula>COUNTIF($B$1:$B1,[Table Name])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="1" dataDxfId="91"/>
-    <tableColumn id="4" name="2" dataDxfId="90"/>
-    <tableColumn id="5" name="3" dataDxfId="89"/>
-    <tableColumn id="6" name="4" dataDxfId="88"/>
-    <tableColumn id="7" name="5" dataDxfId="87"/>
-    <tableColumn id="8" name="6" dataDxfId="86"/>
-    <tableColumn id="9" name="7" dataDxfId="85"/>
-    <tableColumn id="10" name="8" dataDxfId="84"/>
-    <tableColumn id="11" name="9" dataDxfId="83"/>
-    <tableColumn id="12" name="10" dataDxfId="82"/>
-    <tableColumn id="13" name="11" dataDxfId="81"/>
-    <tableColumn id="14" name="12" dataDxfId="80"/>
-    <tableColumn id="15" name="13" dataDxfId="79"/>
-    <tableColumn id="16" name="14" dataDxfId="78"/>
-    <tableColumn id="17" name="15" dataDxfId="77"/>
+    <tableColumn id="3" name="1" dataDxfId="78"/>
+    <tableColumn id="4" name="2" dataDxfId="77"/>
+    <tableColumn id="5" name="3" dataDxfId="76"/>
+    <tableColumn id="6" name="4" dataDxfId="75"/>
+    <tableColumn id="7" name="5" dataDxfId="74"/>
+    <tableColumn id="8" name="6" dataDxfId="73"/>
+    <tableColumn id="9" name="7" dataDxfId="72"/>
+    <tableColumn id="10" name="8" dataDxfId="71"/>
+    <tableColumn id="11" name="9" dataDxfId="70"/>
+    <tableColumn id="12" name="10" dataDxfId="69"/>
+    <tableColumn id="13" name="11" dataDxfId="68"/>
+    <tableColumn id="14" name="12" dataDxfId="67"/>
+    <tableColumn id="15" name="13" dataDxfId="66"/>
+    <tableColumn id="16" name="14" dataDxfId="65"/>
+    <tableColumn id="17" name="15" dataDxfId="64"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SeedMap" displayName="SeedMap" ref="A1:E36" totalsRowShown="0" dataDxfId="76">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SeedMap" displayName="SeedMap" ref="A1:E36" totalsRowShown="0" dataDxfId="63">
   <autoFilter ref="A1:E36"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Name" dataDxfId="75"/>
-    <tableColumn id="3" name="FW Table Name" dataDxfId="74"/>
-    <tableColumn id="20" name="NS" dataDxfId="73">
+    <tableColumn id="1" name="Name" dataDxfId="62"/>
+    <tableColumn id="3" name="FW Table Name" dataDxfId="61"/>
+    <tableColumn id="20" name="NS" dataDxfId="60">
       <calculatedColumnFormula>VLOOKUP([FW Table Name],Tables[],4,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="Model" dataDxfId="72">
+    <tableColumn id="21" name="Model" dataDxfId="59">
       <calculatedColumnFormula>VLOOKUP([FW Table Name],Tables[],5,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Query Method" dataDxfId="71">
+    <tableColumn id="4" name="Query Method" dataDxfId="58">
       <calculatedColumnFormula>"truncate"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4550,46 +4550,46 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="ResourceTable" displayName="ResourceTable" ref="A1:I37" totalsRowShown="0" dataDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="ResourceTable" displayName="ResourceTable" ref="A1:I37" totalsRowShown="0" dataDxfId="57">
   <autoFilter ref="A1:I37"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="No" dataDxfId="69">
+    <tableColumn id="1" name="No" dataDxfId="56">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Name" dataDxfId="68"/>
-    <tableColumn id="3" name="Description" dataDxfId="67"/>
-    <tableColumn id="4" name="Title" dataDxfId="66"/>
-    <tableColumn id="5" name="NS" dataDxfId="65">
+    <tableColumn id="2" name="Name" dataDxfId="55"/>
+    <tableColumn id="3" name="Description" dataDxfId="54"/>
+    <tableColumn id="4" name="Title" dataDxfId="53"/>
+    <tableColumn id="5" name="NS" dataDxfId="52">
       <calculatedColumnFormula>"Milestone\Appframe\Model"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Table" dataDxfId="64"/>
-    <tableColumn id="7" name="Key" dataDxfId="63">
+    <tableColumn id="6" name="Table" dataDxfId="51"/>
+    <tableColumn id="7" name="Key" dataDxfId="50">
       <calculatedColumnFormula>"id"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Controller" dataDxfId="62"/>
-    <tableColumn id="9" name="Controller NS" dataDxfId="61"/>
+    <tableColumn id="8" name="Controller" dataDxfId="49"/>
+    <tableColumn id="9" name="Controller NS" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RelationTable" displayName="RelationTable" ref="A1:I50" totalsRowShown="0" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RelationTable" displayName="RelationTable" ref="A1:I50" totalsRowShown="0" dataDxfId="47">
   <autoFilter ref="A1:I50"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="No" dataDxfId="9">
+    <tableColumn id="1" name="No" dataDxfId="46">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Resource" dataDxfId="8"/>
-    <tableColumn id="4" name="Relate Resource" dataDxfId="7"/>
-    <tableColumn id="2" name="Resource Id" dataDxfId="6">
+    <tableColumn id="3" name="Resource" dataDxfId="45"/>
+    <tableColumn id="4" name="Relate Resource" dataDxfId="44"/>
+    <tableColumn id="2" name="Resource Id" dataDxfId="43">
       <calculatedColumnFormula>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Name" dataDxfId="5"/>
-    <tableColumn id="6" name="Description" dataDxfId="4"/>
-    <tableColumn id="7" name="Method" dataDxfId="3"/>
-    <tableColumn id="8" name="Type" dataDxfId="2"/>
-    <tableColumn id="10" name="Relate Id" dataDxfId="1">
+    <tableColumn id="5" name="Name" dataDxfId="42"/>
+    <tableColumn id="6" name="Description" dataDxfId="41"/>
+    <tableColumn id="7" name="Method" dataDxfId="40"/>
+    <tableColumn id="8" name="Type" dataDxfId="39"/>
+    <tableColumn id="10" name="Relate Id" dataDxfId="38">
       <calculatedColumnFormula>VLOOKUP([Relate Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4598,47 +4598,47 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="ResourceForms" displayName="ResourceForms" ref="A1:G9" totalsRowShown="0" dataDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="ResourceForms" displayName="ResourceForms" ref="A1:G9" totalsRowShown="0" dataDxfId="37">
   <autoFilter ref="A1:G9"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="No" dataDxfId="59">
+    <tableColumn id="1" name="No" dataDxfId="36">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Resource ID" dataDxfId="58"/>
-    <tableColumn id="3" name="Resource Name" dataDxfId="57">
+    <tableColumn id="2" name="Resource ID" dataDxfId="35"/>
+    <tableColumn id="3" name="Resource Name" dataDxfId="34">
       <calculatedColumnFormula>VLOOKUP([Resource ID],ResourceTable[],2,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Form Name" dataDxfId="56"/>
-    <tableColumn id="6" name="Title" dataDxfId="55"/>
-    <tableColumn id="7" name="Action Text" dataDxfId="54"/>
-    <tableColumn id="8" name="Description" dataDxfId="53"/>
+    <tableColumn id="4" name="Form Name" dataDxfId="33"/>
+    <tableColumn id="6" name="Title" dataDxfId="32"/>
+    <tableColumn id="7" name="Action Text" dataDxfId="31"/>
+    <tableColumn id="8" name="Description" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="FormFields" displayName="FormFields" ref="A1:L33" totalsRowShown="0" dataDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="FormFields" displayName="FormFields" ref="A1:L33" totalsRowShown="0" dataDxfId="29">
   <autoFilter ref="A1:L33"/>
   <tableColumns count="12">
-    <tableColumn id="9" name="No" dataDxfId="51">
+    <tableColumn id="9" name="No" dataDxfId="28">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Form Id" dataDxfId="50"/>
-    <tableColumn id="7" name="Form Name" dataDxfId="49">
+    <tableColumn id="1" name="Form Id" dataDxfId="27"/>
+    <tableColumn id="7" name="Form Name" dataDxfId="26">
       <calculatedColumnFormula>VLOOKUP([Form Id],ResourceForms[],4,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Name" dataDxfId="48"/>
-    <tableColumn id="2" name="Type" dataDxfId="47"/>
-    <tableColumn id="5" name="Label" dataDxfId="46"/>
-    <tableColumn id="6" name="Collection" dataDxfId="45"/>
-    <tableColumn id="14" name="Attribute" dataDxfId="44">
+    <tableColumn id="4" name="Name" dataDxfId="25"/>
+    <tableColumn id="2" name="Type" dataDxfId="24"/>
+    <tableColumn id="5" name="Label" dataDxfId="23"/>
+    <tableColumn id="6" name="Collection" dataDxfId="22"/>
+    <tableColumn id="14" name="Attribute" dataDxfId="21">
       <calculatedColumnFormula>[Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Relation" dataDxfId="43"/>
-    <tableColumn id="11" name="Deep 1" dataDxfId="42"/>
-    <tableColumn id="12" name="Deep 2" dataDxfId="41"/>
-    <tableColumn id="13" name="Deep 3" dataDxfId="40"/>
+    <tableColumn id="10" name="Relation" dataDxfId="20"/>
+    <tableColumn id="11" name="Deep 1" dataDxfId="19"/>
+    <tableColumn id="12" name="Deep 2" dataDxfId="18"/>
+    <tableColumn id="13" name="Deep 3" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5678,7 +5678,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="4" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B19" s="7" t="str">
         <f>"__"&amp;[Name]</f>
@@ -6293,7 +6293,7 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="2" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B34" s="7" t="str">
         <f>"__"&amp;[Name]</f>
@@ -6304,7 +6304,7 @@
         <v>resource_form_field_depend</v>
       </c>
       <c r="D34" s="7" t="str">
-        <f>"Milestone\Appframe\Model"</f>
+        <f t="shared" ref="D34:D40" si="1">"Milestone\Appframe\Model"</f>
         <v>Milestone\Appframe\Model</v>
       </c>
       <c r="E34" s="8" t="str">
@@ -6345,7 +6345,7 @@
         <v>resource_form_layout</v>
       </c>
       <c r="D35" s="7" t="str">
-        <f>"Milestone\Appframe\Model"</f>
+        <f t="shared" si="1"/>
         <v>Milestone\Appframe\Model</v>
       </c>
       <c r="E35" s="8" t="str">
@@ -6375,7 +6375,7 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="2" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B36" s="7" t="str">
         <f>"__"&amp;[Name]</f>
@@ -6386,7 +6386,7 @@
         <v>resource_form_collection</v>
       </c>
       <c r="D36" s="7" t="str">
-        <f>"Milestone\Appframe\Model"</f>
+        <f t="shared" si="1"/>
         <v>Milestone\Appframe\Model</v>
       </c>
       <c r="E36" s="8" t="str">
@@ -6416,7 +6416,7 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="4" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B37" s="7" t="str">
         <f>"__"&amp;[Name]</f>
@@ -6427,7 +6427,7 @@
         <v>resource_dashboard</v>
       </c>
       <c r="D37" s="7" t="str">
-        <f>"Milestone\Appframe\Model"</f>
+        <f t="shared" si="1"/>
         <v>Milestone\Appframe\Model</v>
       </c>
       <c r="E37" s="8" t="str">
@@ -6457,7 +6457,7 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="4" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B38" s="7" t="str">
         <f>"__"&amp;[Name]</f>
@@ -6468,7 +6468,7 @@
         <v>resource_dashboard_section</v>
       </c>
       <c r="D38" s="7" t="str">
-        <f>"Milestone\Appframe\Model"</f>
+        <f t="shared" si="1"/>
         <v>Milestone\Appframe\Model</v>
       </c>
       <c r="E38" s="8" t="str">
@@ -6498,7 +6498,7 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="4" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B39" s="7" t="str">
         <f>"__"&amp;[Name]</f>
@@ -6509,7 +6509,7 @@
         <v>resource_dashboard_section_item</v>
       </c>
       <c r="D39" s="7" t="str">
-        <f>"Milestone\Appframe\Model"</f>
+        <f t="shared" si="1"/>
         <v>Milestone\Appframe\Model</v>
       </c>
       <c r="E39" s="8" t="str">
@@ -6539,7 +6539,7 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="4" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B40" s="7" t="str">
         <f>"__"&amp;[Name]</f>
@@ -6550,7 +6550,7 @@
         <v>resource_metric</v>
       </c>
       <c r="D40" s="7" t="str">
-        <f>"Milestone\Appframe\Model"</f>
+        <f t="shared" si="1"/>
         <v>Milestone\Appframe\Model</v>
       </c>
       <c r="E40" s="8" t="str">
@@ -8243,8 +8243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I157"/>
   <sheetViews>
-    <sheetView topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="D156" sqref="D156"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="D100" sqref="D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="15"/>
@@ -8266,7 +8266,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="E1" t="s">
         <v>16</v>
@@ -10401,7 +10401,7 @@
         <v>49</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>642</v>
+        <v>768</v>
       </c>
       <c r="E100" s="4" t="s">
         <v>245</v>
@@ -10560,7 +10560,7 @@
     </row>
     <row r="108" spans="1:9">
       <c r="A108" s="4" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B108" s="4" t="s">
         <v>48</v>
@@ -10572,7 +10572,7 @@
         <v>460</v>
       </c>
       <c r="E108" s="4" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="F108" s="4"/>
       <c r="G108" s="4"/>
@@ -11008,7 +11008,7 @@
     </row>
     <row r="128" spans="1:9">
       <c r="A128" s="4" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B128" s="4" t="s">
         <v>24</v>
@@ -11029,7 +11029,7 @@
     </row>
     <row r="129" spans="1:9">
       <c r="A129" s="4" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B129" s="4" t="s">
         <v>42</v>
@@ -11054,13 +11054,13 @@
     </row>
     <row r="130" spans="1:9">
       <c r="A130" s="4" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B130" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C130" s="5" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D130" s="5"/>
       <c r="E130" s="5" t="s">
@@ -11073,13 +11073,13 @@
     </row>
     <row r="131" spans="1:9">
       <c r="A131" s="4" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B131" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D131" s="4"/>
       <c r="E131" s="4" t="s">
@@ -11098,7 +11098,7 @@
     </row>
     <row r="132" spans="1:9">
       <c r="A132" s="4" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B132" s="4" t="s">
         <v>48</v>
@@ -11107,10 +11107,10 @@
         <v>49</v>
       </c>
       <c r="D132" s="4" t="s">
+        <v>662</v>
+      </c>
+      <c r="E132" s="4" t="s">
         <v>663</v>
-      </c>
-      <c r="E132" s="4" t="s">
-        <v>664</v>
       </c>
       <c r="F132" s="4"/>
       <c r="G132" s="4"/>
@@ -11119,7 +11119,7 @@
     </row>
     <row r="133" spans="1:9">
       <c r="A133" s="4" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B133" s="4" t="s">
         <v>269</v>
@@ -11140,13 +11140,13 @@
     </row>
     <row r="134" spans="1:9">
       <c r="A134" s="4" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B134" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="D134" s="4"/>
       <c r="E134" s="4" t="s">
@@ -11161,13 +11161,13 @@
     </row>
     <row r="135" spans="1:9">
       <c r="A135" s="4" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B135" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="D135" s="4"/>
       <c r="E135" s="4" t="s">
@@ -11186,13 +11186,13 @@
     </row>
     <row r="136" spans="1:9">
       <c r="A136" s="4" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B136" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="D136" s="4">
         <v>64</v>
@@ -11209,13 +11209,13 @@
     </row>
     <row r="137" spans="1:9">
       <c r="A137" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B137" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C137" s="4" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D137" s="4">
         <v>64</v>
@@ -11230,19 +11230,19 @@
     </row>
     <row r="138" spans="1:9">
       <c r="A138" s="4" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B138" s="4" t="s">
         <v>48</v>
       </c>
       <c r="C138" s="4" t="s">
+        <v>684</v>
+      </c>
+      <c r="D138" s="4" t="s">
         <v>685</v>
       </c>
-      <c r="D138" s="4" t="s">
+      <c r="E138" s="4" t="s">
         <v>686</v>
-      </c>
-      <c r="E138" s="4" t="s">
-        <v>687</v>
       </c>
       <c r="F138" s="4"/>
       <c r="G138" s="4"/>
@@ -11251,13 +11251,13 @@
     </row>
     <row r="139" spans="1:9">
       <c r="A139" s="4" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B139" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="D139" s="4">
         <v>128</v>
@@ -11272,13 +11272,13 @@
     </row>
     <row r="140" spans="1:9">
       <c r="A140" s="4" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B140" s="4" t="s">
         <v>48</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="D140" s="4" t="s">
         <v>460</v>
@@ -11293,13 +11293,13 @@
     </row>
     <row r="141" spans="1:9">
       <c r="A141" s="4" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B141" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="D141" s="4">
         <v>64</v>
@@ -11314,19 +11314,19 @@
     </row>
     <row r="142" spans="1:9">
       <c r="A142" s="4" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B142" s="4" t="s">
         <v>48</v>
       </c>
       <c r="C142" s="4" t="s">
+        <v>703</v>
+      </c>
+      <c r="D142" s="4" t="s">
+        <v>705</v>
+      </c>
+      <c r="E142" s="4" t="s">
         <v>704</v>
-      </c>
-      <c r="D142" s="4" t="s">
-        <v>706</v>
-      </c>
-      <c r="E142" s="4" t="s">
-        <v>705</v>
       </c>
       <c r="F142" s="4"/>
       <c r="G142" s="4"/>
@@ -11335,13 +11335,13 @@
     </row>
     <row r="143" spans="1:9">
       <c r="A143" s="4" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B143" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="D143" s="4">
         <v>64</v>
@@ -11356,19 +11356,19 @@
     </row>
     <row r="144" spans="1:9">
       <c r="A144" s="4" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B144" s="4" t="s">
         <v>48</v>
       </c>
       <c r="C144" s="4" t="s">
+        <v>709</v>
+      </c>
+      <c r="D144" s="4" t="s">
         <v>710</v>
       </c>
-      <c r="D144" s="4" t="s">
-        <v>711</v>
-      </c>
       <c r="E144" s="4" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="F144" s="4"/>
       <c r="G144" s="4"/>
@@ -11377,19 +11377,19 @@
     </row>
     <row r="145" spans="1:9">
       <c r="A145" s="4" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="B145" s="4" t="s">
         <v>48</v>
       </c>
       <c r="C145" s="4" t="s">
+        <v>712</v>
+      </c>
+      <c r="D145" s="4" t="s">
         <v>713</v>
       </c>
-      <c r="D145" s="4" t="s">
+      <c r="E145" s="4" t="s">
         <v>714</v>
-      </c>
-      <c r="E145" s="4" t="s">
-        <v>715</v>
       </c>
       <c r="F145" s="4"/>
       <c r="G145" s="4"/>
@@ -11398,19 +11398,19 @@
     </row>
     <row r="146" spans="1:9">
       <c r="A146" s="4" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B146" s="4" t="s">
         <v>48</v>
       </c>
       <c r="C146" s="4" t="s">
+        <v>716</v>
+      </c>
+      <c r="D146" s="4" t="s">
         <v>717</v>
       </c>
-      <c r="D146" s="4" t="s">
+      <c r="E146" s="4" t="s">
         <v>718</v>
-      </c>
-      <c r="E146" s="4" t="s">
-        <v>719</v>
       </c>
       <c r="F146" s="4"/>
       <c r="G146" s="4"/>
@@ -11419,17 +11419,17 @@
     </row>
     <row r="147" spans="1:9">
       <c r="A147" s="4" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B147" s="4" t="s">
         <v>590</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="D147" s="4"/>
       <c r="E147" s="4" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="F147" s="4"/>
       <c r="G147" s="4"/>
@@ -11438,13 +11438,13 @@
     </row>
     <row r="148" spans="1:9">
       <c r="A148" s="4" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B148" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="D148" s="4">
         <v>64</v>
@@ -11459,17 +11459,17 @@
     </row>
     <row r="149" spans="1:9">
       <c r="A149" s="4" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B149" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="D149" s="4"/>
       <c r="E149" s="4" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="F149" s="4"/>
       <c r="G149" s="4"/>
@@ -11478,13 +11478,13 @@
     </row>
     <row r="150" spans="1:9">
       <c r="A150" s="4" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B150" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="D150" s="4"/>
       <c r="E150" s="4" t="s">
@@ -11497,20 +11497,20 @@
     </row>
     <row r="151" spans="1:9">
       <c r="A151" s="4" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B151" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="D151" s="4"/>
       <c r="E151" s="4" t="s">
         <v>43</v>
       </c>
       <c r="F151" s="4" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="G151" s="4" t="s">
         <v>45</v>
@@ -11522,7 +11522,7 @@
     </row>
     <row r="152" spans="1:9">
       <c r="A152" s="4" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B152" s="5" t="s">
         <v>24</v>
@@ -11541,7 +11541,7 @@
     </row>
     <row r="153" spans="1:9">
       <c r="A153" s="4" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B153" s="4" t="s">
         <v>42</v>
@@ -11554,7 +11554,7 @@
         <v>43</v>
       </c>
       <c r="F153" s="4" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="G153" s="4" t="s">
         <v>45</v>
@@ -11566,7 +11566,7 @@
     </row>
     <row r="154" spans="1:9">
       <c r="A154" s="4" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B154" s="4" t="s">
         <v>590</v>
@@ -11585,19 +11585,19 @@
     </row>
     <row r="155" spans="1:9">
       <c r="A155" s="4" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B155" s="4" t="s">
         <v>48</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D155" s="4" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="E155" s="4" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="F155" s="4"/>
       <c r="G155" s="4"/>
@@ -11606,13 +11606,13 @@
     </row>
     <row r="156" spans="1:9">
       <c r="A156" s="4" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B156" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="D156" s="4">
         <v>64</v>
@@ -11627,13 +11627,13 @@
     </row>
     <row r="157" spans="1:9">
       <c r="A157" s="4" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B157" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="D157" s="4">
         <v>64</v>
@@ -11666,7 +11666,7 @@
     <cfRule type="duplicateValues" dxfId="107" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A152:A153">
-    <cfRule type="duplicateValues" dxfId="22" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="106" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -17332,7 +17332,7 @@
       </c>
       <c r="E129" s="7" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>, ['Method','Form','List','Data','FormWithData','ListRelation','AddRelation','ManageRelation'])</v>
+        <v>, ['Method','Dashboard','Form','List','Data','FormWithData','ListRelation','AddRelation','ManageRelation'])</v>
       </c>
       <c r="F129" s="4" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
@@ -17356,7 +17356,7 @@
       </c>
       <c r="K129" s="4" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;enum('type', ['Method','Form','List','Data','FormWithData','ListRelation','AddRelation','ManageRelation'])-&gt;default('Method');</v>
+        <v>$table-&gt;enum('type', ['Method','Dashboard','Form','List','Data','FormWithData','ListRelation','AddRelation','ManageRelation'])-&gt;default('Method');</v>
       </c>
     </row>
     <row r="130" spans="1:11" hidden="1">
@@ -22732,7 +22732,7 @@
         <v>453</v>
       </c>
       <c r="B252" s="4" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C252" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -22776,7 +22776,7 @@
         <v>453</v>
       </c>
       <c r="B253" s="4" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C253" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -24885,7 +24885,7 @@
     </row>
     <row r="301" spans="1:11" hidden="1">
       <c r="A301" s="4" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B301" s="4" t="s">
         <v>21</v>
@@ -24929,7 +24929,7 @@
     </row>
     <row r="302" spans="1:11" hidden="1">
       <c r="A302" s="4" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B302" s="4" t="s">
         <v>117</v>
@@ -24973,10 +24973,10 @@
     </row>
     <row r="303" spans="1:11" hidden="1">
       <c r="A303" s="4" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B303" s="4" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C303" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -25017,7 +25017,7 @@
     </row>
     <row r="304" spans="1:11" hidden="1">
       <c r="A304" s="4" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B304" s="4" t="s">
         <v>572</v>
@@ -25061,10 +25061,10 @@
     </row>
     <row r="305" spans="1:11" s="26" customFormat="1" hidden="1">
       <c r="A305" s="4" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B305" s="4" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="C305" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -25105,7 +25105,7 @@
     </row>
     <row r="306" spans="1:11" hidden="1">
       <c r="A306" s="4" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B306" s="4" t="s">
         <v>40</v>
@@ -25149,7 +25149,7 @@
     </row>
     <row r="307" spans="1:11" hidden="1">
       <c r="A307" s="4" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B307" s="4" t="s">
         <v>118</v>
@@ -25193,10 +25193,10 @@
     </row>
     <row r="308" spans="1:11" hidden="1">
       <c r="A308" s="4" t="s">
+        <v>646</v>
+      </c>
+      <c r="B308" s="4" t="s">
         <v>647</v>
-      </c>
-      <c r="B308" s="4" t="s">
-        <v>648</v>
       </c>
       <c r="C308" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -25237,7 +25237,7 @@
     </row>
     <row r="309" spans="1:11" hidden="1">
       <c r="A309" s="4" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B309" s="4" t="s">
         <v>573</v>
@@ -25281,10 +25281,10 @@
     </row>
     <row r="310" spans="1:11" hidden="1">
       <c r="A310" s="4" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B310" s="4" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C310" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -25325,7 +25325,7 @@
     </row>
     <row r="311" spans="1:11" hidden="1">
       <c r="A311" s="4" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B311" s="4" t="s">
         <v>21</v>
@@ -25369,7 +25369,7 @@
     </row>
     <row r="312" spans="1:11" hidden="1">
       <c r="A312" s="4" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B312" s="4" t="s">
         <v>94</v>
@@ -25413,7 +25413,7 @@
     </row>
     <row r="313" spans="1:11" hidden="1">
       <c r="A313" s="4" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B313" s="4" t="s">
         <v>560</v>
@@ -25457,7 +25457,7 @@
     </row>
     <row r="314" spans="1:11" hidden="1">
       <c r="A314" s="4" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B314" s="4" t="s">
         <v>572</v>
@@ -25501,7 +25501,7 @@
     </row>
     <row r="315" spans="1:11" hidden="1">
       <c r="A315" s="4" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B315" s="4" t="s">
         <v>574</v>
@@ -25545,7 +25545,7 @@
     </row>
     <row r="316" spans="1:11" hidden="1">
       <c r="A316" s="4" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B316" s="4" t="s">
         <v>575</v>
@@ -25589,7 +25589,7 @@
     </row>
     <row r="317" spans="1:11" hidden="1">
       <c r="A317" s="4" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B317" s="4" t="s">
         <v>576</v>
@@ -25633,7 +25633,7 @@
     </row>
     <row r="318" spans="1:11" hidden="1">
       <c r="A318" s="4" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B318" s="4" t="s">
         <v>40</v>
@@ -25677,7 +25677,7 @@
     </row>
     <row r="319" spans="1:11" hidden="1">
       <c r="A319" s="4" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B319" s="4" t="s">
         <v>95</v>
@@ -25721,7 +25721,7 @@
     </row>
     <row r="320" spans="1:11" hidden="1">
       <c r="A320" s="4" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B320" s="4" t="s">
         <v>573</v>
@@ -25765,7 +25765,7 @@
     </row>
     <row r="321" spans="1:11" hidden="1">
       <c r="A321" s="4" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B321" s="4" t="s">
         <v>579</v>
@@ -25809,7 +25809,7 @@
     </row>
     <row r="322" spans="1:11" hidden="1">
       <c r="A322" s="4" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B322" s="4" t="s">
         <v>580</v>
@@ -25853,7 +25853,7 @@
     </row>
     <row r="323" spans="1:11" hidden="1">
       <c r="A323" s="4" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B323" s="4" t="s">
         <v>581</v>
@@ -25897,7 +25897,7 @@
     </row>
     <row r="324" spans="1:11">
       <c r="A324" s="4" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B324" s="4" t="s">
         <v>21</v>
@@ -25941,7 +25941,7 @@
     </row>
     <row r="325" spans="1:11">
       <c r="A325" s="4" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B325" s="4" t="s">
         <v>122</v>
@@ -25985,10 +25985,10 @@
     </row>
     <row r="326" spans="1:11">
       <c r="A326" s="4" t="s">
+        <v>678</v>
+      </c>
+      <c r="B326" s="4" t="s">
         <v>679</v>
-      </c>
-      <c r="B326" s="4" t="s">
-        <v>680</v>
       </c>
       <c r="C326" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -26029,10 +26029,10 @@
     </row>
     <row r="327" spans="1:11">
       <c r="A327" s="4" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B327" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="C327" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -26073,10 +26073,10 @@
     </row>
     <row r="328" spans="1:11">
       <c r="A328" s="4" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B328" s="4" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="C328" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -26117,10 +26117,10 @@
     </row>
     <row r="329" spans="1:11">
       <c r="A329" s="4" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B329" s="4" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="C329" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -26161,7 +26161,7 @@
     </row>
     <row r="330" spans="1:11">
       <c r="A330" s="4" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B330" s="4" t="s">
         <v>36</v>
@@ -26205,10 +26205,10 @@
     </row>
     <row r="331" spans="1:11" s="26" customFormat="1">
       <c r="A331" s="4" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B331" s="4" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C331" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -26249,10 +26249,10 @@
     </row>
     <row r="332" spans="1:11" s="26" customFormat="1">
       <c r="A332" s="4" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B332" s="4" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="C332" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -26293,7 +26293,7 @@
     </row>
     <row r="333" spans="1:11">
       <c r="A333" s="4" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B333" s="4" t="s">
         <v>40</v>
@@ -26337,7 +26337,7 @@
     </row>
     <row r="334" spans="1:11">
       <c r="A334" s="4" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B334" s="4" t="s">
         <v>123</v>
@@ -26381,7 +26381,7 @@
     </row>
     <row r="335" spans="1:11">
       <c r="A335" s="4" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B335" s="4" t="s">
         <v>21</v>
@@ -26425,7 +26425,7 @@
     </row>
     <row r="336" spans="1:11">
       <c r="A336" s="4" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B336" s="4" t="s">
         <v>23</v>
@@ -26469,7 +26469,7 @@
     </row>
     <row r="337" spans="1:11">
       <c r="A337" s="4" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B337" s="4" t="s">
         <v>26</v>
@@ -26513,7 +26513,7 @@
     </row>
     <row r="338" spans="1:11">
       <c r="A338" s="4" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B338" s="4" t="s">
         <v>94</v>
@@ -26557,10 +26557,10 @@
     </row>
     <row r="339" spans="1:11">
       <c r="A339" s="4" t="s">
+        <v>701</v>
+      </c>
+      <c r="B339" s="4" t="s">
         <v>702</v>
-      </c>
-      <c r="B339" s="4" t="s">
-        <v>703</v>
       </c>
       <c r="C339" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -26601,10 +26601,10 @@
     </row>
     <row r="340" spans="1:11">
       <c r="A340" s="4" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B340" s="4" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="C340" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -26645,10 +26645,10 @@
     </row>
     <row r="341" spans="1:11">
       <c r="A341" s="4" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B341" s="5" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="C341" s="5" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -26689,10 +26689,10 @@
     </row>
     <row r="342" spans="1:11">
       <c r="A342" s="4" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B342" s="5" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="C342" s="5" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -26733,10 +26733,10 @@
     </row>
     <row r="343" spans="1:11">
       <c r="A343" s="4" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B343" s="5" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C343" s="5" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -26777,10 +26777,10 @@
     </row>
     <row r="344" spans="1:11">
       <c r="A344" s="4" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B344" s="5" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="C344" s="5" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -26821,10 +26821,10 @@
     </row>
     <row r="345" spans="1:11">
       <c r="A345" s="4" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B345" s="4" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="C345" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -26865,7 +26865,7 @@
     </row>
     <row r="346" spans="1:11" s="26" customFormat="1">
       <c r="A346" s="4" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B346" s="4" t="s">
         <v>36</v>
@@ -26909,7 +26909,7 @@
     </row>
     <row r="347" spans="1:11">
       <c r="A347" s="4" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B347" s="4" t="s">
         <v>40</v>
@@ -26953,7 +26953,7 @@
     </row>
     <row r="348" spans="1:11">
       <c r="A348" s="4" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B348" s="4" t="s">
         <v>41</v>
@@ -26997,7 +26997,7 @@
     </row>
     <row r="349" spans="1:11">
       <c r="A349" s="4" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B349" s="4" t="s">
         <v>95</v>
@@ -27041,7 +27041,7 @@
     </row>
     <row r="350" spans="1:11">
       <c r="A350" s="4" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B350" s="4" t="s">
         <v>21</v>
@@ -27085,7 +27085,7 @@
     </row>
     <row r="351" spans="1:11">
       <c r="A351" s="4" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B351" s="4" t="s">
         <v>23</v>
@@ -27129,7 +27129,7 @@
     </row>
     <row r="352" spans="1:11">
       <c r="A352" s="4" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B352" s="4" t="s">
         <v>26</v>
@@ -27173,7 +27173,7 @@
     </row>
     <row r="353" spans="1:11">
       <c r="A353" s="4" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B353" s="4" t="s">
         <v>28</v>
@@ -27217,7 +27217,7 @@
     </row>
     <row r="354" spans="1:11">
       <c r="A354" s="4" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B354" s="4" t="s">
         <v>30</v>
@@ -27261,7 +27261,7 @@
     </row>
     <row r="355" spans="1:11">
       <c r="A355" s="4" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B355" s="4" t="s">
         <v>36</v>
@@ -27305,7 +27305,7 @@
     </row>
     <row r="356" spans="1:11">
       <c r="A356" s="4" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B356" s="4" t="s">
         <v>40</v>
@@ -27349,7 +27349,7 @@
     </row>
     <row r="357" spans="1:11">
       <c r="A357" s="4" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B357" s="4" t="s">
         <v>41</v>
@@ -27393,7 +27393,7 @@
     </row>
     <row r="358" spans="1:11">
       <c r="A358" s="4" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B358" s="4" t="s">
         <v>21</v>
@@ -27437,10 +27437,10 @@
     </row>
     <row r="359" spans="1:11" s="26" customFormat="1">
       <c r="A359" s="4" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B359" s="4" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="C359" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -27481,7 +27481,7 @@
     </row>
     <row r="360" spans="1:11">
       <c r="A360" s="4" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B360" s="4" t="s">
         <v>26</v>
@@ -27525,7 +27525,7 @@
     </row>
     <row r="361" spans="1:11">
       <c r="A361" s="4" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B361" s="4" t="s">
         <v>30</v>
@@ -27569,10 +27569,10 @@
     </row>
     <row r="362" spans="1:11">
       <c r="A362" s="4" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B362" s="4" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="C362" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -27613,7 +27613,7 @@
     </row>
     <row r="363" spans="1:11">
       <c r="A363" s="4" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B363" s="4" t="s">
         <v>40</v>
@@ -27657,10 +27657,10 @@
     </row>
     <row r="364" spans="1:11">
       <c r="A364" s="4" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B364" s="4" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C364" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -27701,7 +27701,7 @@
     </row>
     <row r="365" spans="1:11">
       <c r="A365" s="4" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B365" s="4" t="s">
         <v>21</v>
@@ -27745,10 +27745,10 @@
     </row>
     <row r="366" spans="1:11">
       <c r="A366" s="4" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B366" s="4" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C366" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -27789,10 +27789,10 @@
     </row>
     <row r="367" spans="1:11">
       <c r="A367" s="4" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B367" s="4" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C367" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -27833,7 +27833,7 @@
     </row>
     <row r="368" spans="1:11">
       <c r="A368" s="4" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B368" s="4" t="s">
         <v>30</v>
@@ -27877,10 +27877,10 @@
     </row>
     <row r="369" spans="1:11">
       <c r="A369" s="4" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B369" s="4" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="C369" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -27921,10 +27921,10 @@
     </row>
     <row r="370" spans="1:11">
       <c r="A370" s="4" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B370" s="4" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="C370" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -27965,10 +27965,10 @@
     </row>
     <row r="371" spans="1:11">
       <c r="A371" s="4" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B371" s="4" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="C371" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -28009,7 +28009,7 @@
     </row>
     <row r="372" spans="1:11">
       <c r="A372" s="4" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B372" s="4" t="s">
         <v>40</v>
@@ -28053,10 +28053,10 @@
     </row>
     <row r="373" spans="1:11">
       <c r="A373" s="4" t="s">
+        <v>731</v>
+      </c>
+      <c r="B373" s="4" t="s">
         <v>732</v>
-      </c>
-      <c r="B373" s="4" t="s">
-        <v>733</v>
       </c>
       <c r="C373" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -28117,8 +28117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R322"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B247" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView topLeftCell="B301" workbookViewId="0">
+      <selection activeCell="E317" sqref="E317"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -34555,10 +34555,10 @@
         <v>18</v>
       </c>
       <c r="E175" s="43" t="s">
+        <v>659</v>
+      </c>
+      <c r="F175" s="43" t="s">
         <v>660</v>
-      </c>
-      <c r="F175" s="43" t="s">
-        <v>661</v>
       </c>
       <c r="G175" s="43" t="s">
         <v>303</v>
@@ -38078,19 +38078,19 @@
         <v>30</v>
       </c>
       <c r="D272" s="40" t="s">
+        <v>649</v>
+      </c>
+      <c r="E272" s="40" t="s">
         <v>650</v>
       </c>
-      <c r="E272" s="40" t="s">
+      <c r="F272" s="40" t="s">
         <v>651</v>
-      </c>
-      <c r="F272" s="40" t="s">
-        <v>652</v>
       </c>
       <c r="G272" s="40" t="s">
         <v>558</v>
       </c>
       <c r="H272" s="40" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="I272" s="40" t="s">
         <v>21</v>
@@ -38121,13 +38121,13 @@
         <v>12</v>
       </c>
       <c r="E273" s="40" t="s">
+        <v>653</v>
+      </c>
+      <c r="F273" s="40" t="s">
         <v>654</v>
       </c>
-      <c r="F273" s="40" t="s">
-        <v>655</v>
-      </c>
       <c r="G273" s="40" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="H273" s="40" t="s">
         <v>310</v>
@@ -38161,10 +38161,10 @@
         <v>30</v>
       </c>
       <c r="E274" s="40" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="F274" s="40" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="G274" s="40" t="s">
         <v>349</v>
@@ -38204,7 +38204,7 @@
         <v>303</v>
       </c>
       <c r="F275" s="40" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="G275" s="40" t="s">
         <v>303</v>
@@ -38244,7 +38244,7 @@
         <v>13</v>
       </c>
       <c r="F276" s="43" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="G276" s="43" t="s">
         <v>13</v>
@@ -38284,7 +38284,7 @@
         <v>349</v>
       </c>
       <c r="F277" s="40" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="G277" s="40" t="s">
         <v>349</v>
@@ -38377,7 +38377,7 @@
         <v>Form Collection-0</v>
       </c>
       <c r="B280" s="40" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="C280" s="22">
         <f>COUNTIF($B$1:$B279,[Table Name])</f>
@@ -38387,13 +38387,13 @@
         <v>117</v>
       </c>
       <c r="E280" s="40" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="F280" s="40" t="s">
         <v>56</v>
       </c>
       <c r="G280" s="40" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="H280" s="40"/>
       <c r="I280" s="40"/>
@@ -38413,7 +38413,7 @@
         <v>Data Scopes-0</v>
       </c>
       <c r="B281" s="40" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C281" s="22">
         <f>COUNTIF($B$1:$B280,[Table Name])</f>
@@ -39181,7 +39181,7 @@
         <v>Resource List Search-0</v>
       </c>
       <c r="B305" s="40" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C305" s="22">
         <f>COUNTIF($B$1:$B304,[Table Name])</f>
@@ -39228,19 +39228,19 @@
         <v>31</v>
       </c>
       <c r="D306" s="40" t="s">
+        <v>672</v>
+      </c>
+      <c r="E306" s="40" t="s">
         <v>673</v>
       </c>
-      <c r="E306" s="40" t="s">
+      <c r="F306" s="40" t="s">
         <v>674</v>
-      </c>
-      <c r="F306" s="40" t="s">
-        <v>675</v>
       </c>
       <c r="G306" s="40" t="s">
         <v>558</v>
       </c>
       <c r="H306" s="40" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="I306" s="40" t="s">
         <v>21</v>
@@ -39271,13 +39271,13 @@
         <v>19</v>
       </c>
       <c r="E307" s="40" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="F307" s="40" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="G307" s="40" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="H307" s="40" t="s">
         <v>310</v>
@@ -39301,7 +39301,7 @@
         <v>Field Depends-0</v>
       </c>
       <c r="B308" s="40" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C308" s="22">
         <f>COUNTIF($B$1:$B307,[Table Name])</f>
@@ -39311,25 +39311,25 @@
         <v>122</v>
       </c>
       <c r="E308" s="40" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="F308" s="40" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="G308" s="40" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="H308" s="40" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="I308" s="40" t="s">
         <v>36</v>
       </c>
       <c r="J308" s="40" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="K308" s="40" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="L308" s="40"/>
       <c r="M308" s="40"/>
@@ -39352,19 +39352,19 @@
         <v>32</v>
       </c>
       <c r="D309" s="40" t="s">
+        <v>690</v>
+      </c>
+      <c r="E309" s="40" t="s">
         <v>691</v>
       </c>
-      <c r="E309" s="40" t="s">
+      <c r="F309" s="40" t="s">
         <v>692</v>
-      </c>
-      <c r="F309" s="40" t="s">
-        <v>693</v>
       </c>
       <c r="G309" s="40" t="s">
         <v>558</v>
       </c>
       <c r="H309" s="40" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="I309" s="40" t="s">
         <v>21</v>
@@ -39395,13 +39395,13 @@
         <v>13</v>
       </c>
       <c r="E310" s="40" t="s">
+        <v>694</v>
+      </c>
+      <c r="F310" s="40" t="s">
         <v>695</v>
       </c>
-      <c r="F310" s="40" t="s">
+      <c r="G310" s="40" t="s">
         <v>696</v>
-      </c>
-      <c r="G310" s="40" t="s">
-        <v>697</v>
       </c>
       <c r="H310" s="40" t="s">
         <v>310</v>
@@ -39425,7 +39425,7 @@
         <v>Dashboard-0</v>
       </c>
       <c r="B311" s="43" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C311" s="42">
         <f>COUNTIF($B$1:$B310,[Table Name])</f>
@@ -39463,14 +39463,14 @@
         <v>Dashboard Sections-0</v>
       </c>
       <c r="B312" s="43" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="C312" s="42">
         <f>COUNTIF($B$1:$B311,[Table Name])</f>
         <v>0</v>
       </c>
       <c r="D312" s="43" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="E312" s="43" t="s">
         <v>26</v>
@@ -39479,7 +39479,7 @@
         <v>30</v>
       </c>
       <c r="G312" s="43" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="H312" s="43"/>
       <c r="I312" s="43"/>
@@ -39499,7 +39499,7 @@
         <v>Dashboard Section Items-0</v>
       </c>
       <c r="B313" s="43" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="C313" s="42">
         <f>COUNTIF($B$1:$B312,[Table Name])</f>
@@ -39515,13 +39515,13 @@
         <v>30</v>
       </c>
       <c r="G313" s="43" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="H313" s="43" t="s">
+        <v>739</v>
+      </c>
+      <c r="I313" s="43" t="s">
         <v>740</v>
-      </c>
-      <c r="I313" s="43" t="s">
-        <v>741</v>
       </c>
       <c r="J313" s="43"/>
       <c r="K313" s="43"/>
@@ -39539,7 +39539,7 @@
         <v>Resource Metrics-0</v>
       </c>
       <c r="B314" s="40" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C314" s="22">
         <f>COUNTIF($B$1:$B313,[Table Name])</f>
@@ -39555,25 +39555,25 @@
         <v>94</v>
       </c>
       <c r="G314" s="40" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="H314" s="40" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="I314" s="40" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="J314" s="40" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="K314" s="40" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="L314" s="40" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="M314" s="40" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="N314" s="40" t="s">
         <v>36</v>
@@ -39596,19 +39596,19 @@
         <v>33</v>
       </c>
       <c r="D315" s="43" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="E315" s="43" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="F315" s="43" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="G315" s="43" t="s">
         <v>558</v>
       </c>
       <c r="H315" s="43" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="I315" s="43" t="s">
         <v>21</v>
@@ -39636,19 +39636,19 @@
         <v>34</v>
       </c>
       <c r="D316" s="43" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E316" s="43" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="F316" s="43" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="G316" s="43" t="s">
         <v>558</v>
       </c>
       <c r="H316" s="43" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="I316" s="43" t="s">
         <v>21</v>
@@ -39676,19 +39676,19 @@
         <v>35</v>
       </c>
       <c r="D317" s="43" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="E317" s="43" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="F317" s="43" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="G317" s="43" t="s">
         <v>558</v>
       </c>
       <c r="H317" s="43" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="I317" s="43" t="s">
         <v>21</v>
@@ -39716,19 +39716,19 @@
         <v>36</v>
       </c>
       <c r="D318" s="40" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="E318" s="40" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="F318" s="40" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="G318" s="40" t="s">
         <v>558</v>
       </c>
       <c r="H318" s="40" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="I318" s="40" t="s">
         <v>21</v>
@@ -39759,13 +39759,13 @@
         <v>4</v>
       </c>
       <c r="E319" s="43" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="F319" s="43" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="G319" s="43" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="H319" s="43" t="s">
         <v>310</v>
@@ -39799,10 +39799,10 @@
         <v>33</v>
       </c>
       <c r="E320" s="43" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="F320" s="43" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="G320" s="43" t="s">
         <v>609</v>
@@ -39839,10 +39839,10 @@
         <v>34</v>
       </c>
       <c r="E321" s="43" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="F321" s="43" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="G321" s="43" t="s">
         <v>616</v>
@@ -39879,10 +39879,10 @@
         <v>33</v>
       </c>
       <c r="E322" s="40" t="s">
+        <v>766</v>
+      </c>
+      <c r="F322" s="40" t="s">
         <v>767</v>
-      </c>
-      <c r="F322" s="40" t="s">
-        <v>768</v>
       </c>
       <c r="G322" s="40" t="s">
         <v>208</v>
@@ -40450,10 +40450,10 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="4" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C27" s="4" t="str">
         <f>VLOOKUP([FW Table Name],Tables[],4,0)</f>
@@ -40510,7 +40510,7 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="4" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>567</v>
@@ -40530,10 +40530,10 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="4" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="C31" s="4" t="str">
         <f>VLOOKUP([FW Table Name],Tables[],4,0)</f>
@@ -40544,16 +40544,16 @@
         <v>ResourceListSearch</v>
       </c>
       <c r="E31" s="7" t="str">
-        <f>"truncate"</f>
+        <f t="shared" ref="E31:E36" si="3">"truncate"</f>
         <v>truncate</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="4" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="C32" s="4" t="str">
         <f>VLOOKUP([FW Table Name],Tables[],4,0)</f>
@@ -40564,16 +40564,16 @@
         <v>ResourceFormFieldDepend</v>
       </c>
       <c r="E32" s="7" t="str">
-        <f>"truncate"</f>
+        <f t="shared" si="3"/>
         <v>truncate</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="5" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="C33" s="5" t="str">
         <f>VLOOKUP([FW Table Name],Tables[],4,0)</f>
@@ -40584,16 +40584,16 @@
         <v>ResourceDashboard</v>
       </c>
       <c r="E33" s="8" t="str">
-        <f>"truncate"</f>
+        <f t="shared" si="3"/>
         <v>truncate</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="5" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C34" s="5" t="str">
         <f>VLOOKUP([FW Table Name],Tables[],4,0)</f>
@@ -40604,16 +40604,16 @@
         <v>ResourceDashboardSection</v>
       </c>
       <c r="E34" s="8" t="str">
-        <f>"truncate"</f>
+        <f t="shared" si="3"/>
         <v>truncate</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="5" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C35" s="5" t="str">
         <f>VLOOKUP([FW Table Name],Tables[],4,0)</f>
@@ -40624,16 +40624,16 @@
         <v>ResourceDashboardSectionItem</v>
       </c>
       <c r="E35" s="8" t="str">
-        <f>"truncate"</f>
+        <f t="shared" si="3"/>
         <v>truncate</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="4" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C36" s="4" t="str">
         <f>VLOOKUP([FW Table Name],Tables[],4,0)</f>
@@ -40644,7 +40644,7 @@
         <v>ResourceMetric</v>
       </c>
       <c r="E36" s="7" t="str">
-        <f>"truncate"</f>
+        <f t="shared" si="3"/>
         <v>truncate</v>
       </c>
     </row>
@@ -41527,24 +41527,24 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="20">
-        <f>IFERROR($A30+1,1)</f>
+        <f t="shared" ref="A31:A37" si="11">IFERROR($A30+1,1)</f>
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>650</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="D31" s="4" t="s">
         <v>651</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>652</v>
       </c>
       <c r="E31" s="7" t="str">
         <f t="shared" si="9"/>
         <v>Milestone\Appframe\Model</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="G31" s="21" t="str">
         <f t="shared" si="10"/>
@@ -41555,24 +41555,24 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="20">
-        <f>IFERROR($A31+1,1)</f>
+        <f t="shared" si="11"/>
         <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
+        <v>672</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>673</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="D32" s="4" t="s">
         <v>674</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>675</v>
       </c>
       <c r="E32" s="7" t="str">
         <f t="shared" si="9"/>
         <v>Milestone\Appframe\Model</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="G32" s="21" t="str">
         <f t="shared" si="10"/>
@@ -41583,24 +41583,24 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="20">
-        <f>IFERROR($A32+1,1)</f>
+        <f t="shared" si="11"/>
         <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
+        <v>690</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>691</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="D33" s="4" t="s">
         <v>692</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>693</v>
       </c>
       <c r="E33" s="7" t="str">
         <f>"Milestone\Appframe\Model"</f>
         <v>Milestone\Appframe\Model</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="G33" s="21" t="str">
         <f>"id"</f>
@@ -41610,27 +41610,27 @@
       <c r="I33" s="4"/>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="51">
-        <f>IFERROR($A33+1,1)</f>
+      <c r="A34" s="45">
+        <f t="shared" si="11"/>
         <v>33</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="E34" s="8" t="str">
         <f>"Milestone\Appframe\Model"</f>
         <v>Milestone\Appframe\Model</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>756</v>
-      </c>
-      <c r="G34" s="52" t="str">
+        <v>755</v>
+      </c>
+      <c r="G34" s="46" t="str">
         <f>"id"</f>
         <v>id</v>
       </c>
@@ -41638,27 +41638,27 @@
       <c r="I34" s="5"/>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="51">
-        <f>IFERROR($A34+1,1)</f>
+      <c r="A35" s="45">
+        <f t="shared" si="11"/>
         <v>34</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="E35" s="8" t="str">
         <f>"Milestone\Appframe\Model"</f>
         <v>Milestone\Appframe\Model</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>757</v>
-      </c>
-      <c r="G35" s="52" t="str">
+        <v>756</v>
+      </c>
+      <c r="G35" s="46" t="str">
         <f>"id"</f>
         <v>id</v>
       </c>
@@ -41666,27 +41666,27 @@
       <c r="I35" s="5"/>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="51">
-        <f>IFERROR($A35+1,1)</f>
+      <c r="A36" s="45">
+        <f t="shared" si="11"/>
         <v>35</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E36" s="8" t="str">
         <f>"Milestone\Appframe\Model"</f>
         <v>Milestone\Appframe\Model</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>758</v>
-      </c>
-      <c r="G36" s="52" t="str">
+        <v>757</v>
+      </c>
+      <c r="G36" s="46" t="str">
         <f>"id"</f>
         <v>id</v>
       </c>
@@ -41695,24 +41695,24 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="20">
-        <f>IFERROR($A36+1,1)</f>
+        <f t="shared" si="11"/>
         <v>36</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="E37" s="7" t="str">
         <f>"Milestone\Appframe\Model"</f>
         <v>Milestone\Appframe\Model</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="G37" s="21" t="str">
         <f>"id"</f>
@@ -42475,10 +42475,10 @@
         <v>18</v>
       </c>
       <c r="E23" s="7" t="s">
+        <v>659</v>
+      </c>
+      <c r="F23" s="7" t="s">
         <v>660</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>661</v>
       </c>
       <c r="G23" s="22" t="s">
         <v>303</v>
@@ -43012,20 +43012,20 @@
         <v>402</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="D40" s="7">
         <f>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</f>
         <v>12</v>
       </c>
       <c r="E40" s="7" t="s">
+        <v>653</v>
+      </c>
+      <c r="F40" s="7" t="s">
         <v>654</v>
       </c>
-      <c r="F40" s="7" t="s">
-        <v>655</v>
-      </c>
       <c r="G40" s="22" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="H40" s="7" t="s">
         <v>310</v>
@@ -43041,7 +43041,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>402</v>
@@ -43051,10 +43051,10 @@
         <v>30</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="G41" s="22" t="s">
         <v>349</v>
@@ -43073,7 +43073,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>568</v>
@@ -43086,7 +43086,7 @@
         <v>303</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="G42" s="22" t="s">
         <v>303</v>
@@ -43101,7 +43101,7 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="20">
-        <f>IFERROR($A42+1,1)</f>
+        <f t="shared" ref="A43:A50" si="7">IFERROR($A42+1,1)</f>
         <v>42</v>
       </c>
       <c r="B43" s="7" t="s">
@@ -43118,7 +43118,7 @@
         <v>13</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="G43" s="22" t="s">
         <v>13</v>
@@ -43133,7 +43133,7 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="20">
-        <f>IFERROR($A43+1,1)</f>
+        <f t="shared" si="7"/>
         <v>43</v>
       </c>
       <c r="B44" s="7" t="s">
@@ -43150,7 +43150,7 @@
         <v>349</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="G44" s="22" t="s">
         <v>349</v>
@@ -43165,27 +43165,27 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="20">
-        <f>IFERROR($A44+1,1)</f>
+        <f t="shared" si="7"/>
         <v>44</v>
       </c>
       <c r="B45" s="7" t="s">
         <v>515</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="D45" s="7">
         <f>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</f>
         <v>19</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="G45" s="22" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="H45" s="7" t="s">
         <v>310</v>
@@ -43197,27 +43197,27 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="20">
-        <f>IFERROR($A45+1,1)</f>
+        <f t="shared" si="7"/>
         <v>45</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>406</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D46" s="7">
         <f>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</f>
         <v>13</v>
       </c>
       <c r="E46" s="7" t="s">
+        <v>694</v>
+      </c>
+      <c r="F46" s="7" t="s">
         <v>695</v>
       </c>
-      <c r="F46" s="7" t="s">
+      <c r="G46" s="22" t="s">
         <v>696</v>
-      </c>
-      <c r="G46" s="22" t="s">
-        <v>697</v>
       </c>
       <c r="H46" s="7" t="s">
         <v>310</v>
@@ -43229,27 +43229,27 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="20">
-        <f>IFERROR($A46+1,1)</f>
+        <f t="shared" si="7"/>
         <v>46</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>208</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="D47" s="7">
         <f>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</f>
         <v>4</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="G47" s="22" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="H47" s="7" t="s">
         <v>310</v>
@@ -43261,24 +43261,24 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="20">
-        <f>IFERROR($A47+1,1)</f>
+        <f t="shared" si="7"/>
         <v>47</v>
       </c>
       <c r="B48" s="7" t="s">
+        <v>747</v>
+      </c>
+      <c r="C48" s="7" t="s">
         <v>748</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>749</v>
       </c>
       <c r="D48" s="7">
         <f>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</f>
         <v>33</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="G48" s="22" t="s">
         <v>609</v>
@@ -43293,24 +43293,24 @@
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="20">
-        <f>IFERROR($A48+1,1)</f>
+        <f t="shared" si="7"/>
         <v>48</v>
       </c>
       <c r="B49" s="7" t="s">
+        <v>748</v>
+      </c>
+      <c r="C49" s="7" t="s">
         <v>749</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>750</v>
       </c>
       <c r="D49" s="7">
         <f>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</f>
         <v>34</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="G49" s="22" t="s">
         <v>616</v>
@@ -43325,11 +43325,11 @@
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="20">
-        <f>IFERROR($A49+1,1)</f>
+        <f t="shared" si="7"/>
         <v>49</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>208</v>
@@ -43339,10 +43339,10 @@
         <v>33</v>
       </c>
       <c r="E50" s="7" t="s">
+        <v>766</v>
+      </c>
+      <c r="F50" s="7" t="s">
         <v>767</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>768</v>
       </c>
       <c r="G50" s="22" t="s">
         <v>208</v>
@@ -43383,31 +43383,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="38" customFormat="1" ht="15" customHeight="1">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="50" t="s">
         <v>441</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="49" t="str">
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="51" t="str">
         <f>"\"&amp;VLOOKUP($A$1,SeedMap[],3,0)&amp;"\"&amp;VLOOKUP($A$1,SeedMap[],4,0)&amp;"::"&amp;VLOOKUP($A$1,SeedMap[],5,0)&amp;"()"</f>
         <v>\Milestone\Appframe\Model\ResourceRelation::truncate()</v>
       </c>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="50" t="s">
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="52" t="s">
         <v>176</v>
       </c>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="50"/>
-      <c r="R1" s="50"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
+      <c r="N1" s="52"/>
+      <c r="O1" s="52"/>
+      <c r="P1" s="52"/>
+      <c r="Q1" s="52"/>
+      <c r="R1" s="52"/>
       <c r="S1" s="31" t="str">
         <f>""</f>
         <v/>
@@ -43415,28 +43415,28 @@
       <c r="T1" s="10"/>
     </row>
     <row r="2" spans="1:20" s="38" customFormat="1" ht="15" customHeight="1">
-      <c r="A2" s="48"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="49" t="s">
+      <c r="A2" s="50"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="51" t="s">
         <v>436</v>
       </c>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="50" t="s">
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="52" t="s">
         <v>175</v>
       </c>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="50"/>
-      <c r="N2" s="50"/>
-      <c r="O2" s="50"/>
-      <c r="P2" s="50"/>
-      <c r="Q2" s="50"/>
-      <c r="R2" s="50"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="52"/>
+      <c r="P2" s="52"/>
+      <c r="Q2" s="52"/>
+      <c r="R2" s="52"/>
       <c r="S2" s="31" t="str">
         <f>";"</f>
         <v>;</v>
@@ -43444,26 +43444,26 @@
       <c r="T2" s="10"/>
     </row>
     <row r="3" spans="1:20" s="38" customFormat="1" ht="15" customHeight="1">
-      <c r="A3" s="48"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="50" t="s">
+      <c r="A3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="52" t="s">
         <v>430</v>
       </c>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="50"/>
-      <c r="R3" s="50"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="52"/>
+      <c r="O3" s="52"/>
+      <c r="P3" s="52"/>
+      <c r="Q3" s="52"/>
+      <c r="R3" s="52"/>
       <c r="S3" s="31" t="str">
         <f>$I$3</f>
         <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
@@ -43599,74 +43599,74 @@
     </row>
     <row r="6" spans="1:20">
       <c r="A6" s="32"/>
-      <c r="B6" s="45" t="str">
+      <c r="B6" s="47" t="str">
         <f>$I$1</f>
         <v>$_ = \DB::statement('SELECT @@GLOBAL.foreign_key_checks');</v>
       </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="45"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="45"/>
-      <c r="M6" s="45"/>
-      <c r="N6" s="45"/>
-      <c r="O6" s="45"/>
-      <c r="P6" s="45"/>
-      <c r="Q6" s="45"/>
-      <c r="R6" s="45"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="47"/>
+      <c r="O6" s="47"/>
+      <c r="P6" s="47"/>
+      <c r="Q6" s="47"/>
+      <c r="R6" s="47"/>
       <c r="S6" s="10"/>
       <c r="T6" s="10"/>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" s="32"/>
-      <c r="B7" s="46" t="str">
+      <c r="B7" s="48" t="str">
         <f>$I$2</f>
         <v>\DB::statement('set foreign_key_checks = 0');</v>
       </c>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
-      <c r="K7" s="46"/>
-      <c r="L7" s="46"/>
-      <c r="M7" s="46"/>
-      <c r="N7" s="46"/>
-      <c r="O7" s="46"/>
-      <c r="P7" s="46"/>
-      <c r="Q7" s="46"/>
-      <c r="R7" s="46"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="48"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="48"/>
+      <c r="M7" s="48"/>
+      <c r="N7" s="48"/>
+      <c r="O7" s="48"/>
+      <c r="P7" s="48"/>
+      <c r="Q7" s="48"/>
+      <c r="R7" s="48"/>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" s="32"/>
-      <c r="B8" s="47" t="str">
+      <c r="B8" s="49" t="str">
         <f>$E$1</f>
         <v>\Milestone\Appframe\Model\ResourceRelation::truncate()</v>
       </c>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="47"/>
-      <c r="K8" s="47"/>
-      <c r="L8" s="47"/>
-      <c r="M8" s="47"/>
-      <c r="N8" s="47"/>
-      <c r="O8" s="47"/>
-      <c r="P8" s="47"/>
-      <c r="Q8" s="47"/>
-      <c r="R8" s="47"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="49"/>
+      <c r="L8" s="49"/>
+      <c r="M8" s="49"/>
+      <c r="N8" s="49"/>
+      <c r="O8" s="49"/>
+      <c r="P8" s="49"/>
+      <c r="Q8" s="49"/>
+      <c r="R8" s="49"/>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" s="29">

</xml_diff>

<commit_message>
Resource Metric table modified
</commit_message>
<xml_diff>
--- a/Helper.xlsx
+++ b/Helper.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Tables" sheetId="1" r:id="rId1"/>
@@ -2149,9 +2149,6 @@
     <t>eloquent_aggregates</t>
   </si>
   <si>
-    <t>aggregates</t>
-  </si>
-  <si>
     <t>default('COUNT')</t>
   </si>
   <si>
@@ -2372,6 +2369,9 @@
   </si>
   <si>
     <t>default('value')</t>
+  </si>
+  <si>
+    <t>aggregate</t>
   </si>
 </sst>
 </file>
@@ -2607,55 +2607,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="128">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="124">
     <dxf>
       <font>
         <strike val="0"/>
@@ -4441,35 +4393,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tables" displayName="Tables" ref="A1:J42" totalsRowShown="0" dataDxfId="127">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tables" displayName="Tables" ref="A1:J42" totalsRowShown="0" dataDxfId="123">
   <autoFilter ref="A1:J42"/>
   <tableColumns count="10">
-    <tableColumn id="2" name="Name" dataDxfId="126"/>
-    <tableColumn id="10" name="Table" dataDxfId="125">
+    <tableColumn id="2" name="Name" dataDxfId="122"/>
+    <tableColumn id="10" name="Table" dataDxfId="121">
       <calculatedColumnFormula>"__"&amp;[Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Singular Name" dataDxfId="124">
+    <tableColumn id="5" name="Singular Name" dataDxfId="120">
       <calculatedColumnFormula>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Model NS" dataDxfId="123">
+    <tableColumn id="8" name="Model NS" dataDxfId="119">
       <calculatedColumnFormula>"Milestone\Appframe\Model"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Class Name" dataDxfId="122">
+    <tableColumn id="4" name="Class Name" dataDxfId="118">
       <calculatedColumnFormula>SUBSTITUTE(PROPER([Singular Name]),"_","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Migration Artisan" dataDxfId="121">
+    <tableColumn id="1" name="Migration Artisan" dataDxfId="117">
       <calculatedColumnFormula>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Model Artisan" dataDxfId="120">
+    <tableColumn id="6" name="Model Artisan" dataDxfId="116">
       <calculatedColumnFormula>"php artisan make:model "&amp;[Class Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Model Statement" dataDxfId="119">
+    <tableColumn id="3" name="Model Statement" dataDxfId="115">
       <calculatedColumnFormula>"protected $table = '"&amp;[Table]&amp;"';"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Seeder Artisan" dataDxfId="118">
+    <tableColumn id="7" name="Seeder Artisan" dataDxfId="114">
       <calculatedColumnFormula>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Seeder Class" dataDxfId="117">
+    <tableColumn id="9" name="Seeder Class" dataDxfId="113">
       <calculatedColumnFormula>[Class Name]&amp;"TableSeeder"&amp;"::class,"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4478,56 +4430,56 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="ResourceActions" displayName="ResourceActions" ref="A1:P9" totalsRowShown="0" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="ResourceActions" displayName="ResourceActions" ref="A1:P9" totalsRowShown="0" dataDxfId="16">
   <autoFilter ref="A1:P9"/>
   <tableColumns count="16">
-    <tableColumn id="1" name="No" dataDxfId="19">
+    <tableColumn id="1" name="No" dataDxfId="15">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Resource" dataDxfId="18"/>
-    <tableColumn id="13" name="Resource Id" dataDxfId="17">
+    <tableColumn id="2" name="Resource" dataDxfId="14"/>
+    <tableColumn id="13" name="Resource Id" dataDxfId="13">
       <calculatedColumnFormula>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Action Name" dataDxfId="16"/>
-    <tableColumn id="4" name="Description" dataDxfId="15"/>
-    <tableColumn id="5" name="Action Title" dataDxfId="14"/>
-    <tableColumn id="6" name="Button Type" dataDxfId="13"/>
-    <tableColumn id="7" name="Menu" dataDxfId="12"/>
-    <tableColumn id="8" name="Icon" dataDxfId="11"/>
-    <tableColumn id="9" name="Set" dataDxfId="10"/>
-    <tableColumn id="14" name="Action Type" dataDxfId="9"/>
-    <tableColumn id="15" name="ID1" dataDxfId="8"/>
-    <tableColumn id="16" name="ID2" dataDxfId="7"/>
-    <tableColumn id="10" name="On" dataDxfId="6"/>
-    <tableColumn id="11" name="Confirm" dataDxfId="5"/>
-    <tableColumn id="12" name="handler" dataDxfId="4"/>
+    <tableColumn id="3" name="Action Name" dataDxfId="12"/>
+    <tableColumn id="4" name="Description" dataDxfId="11"/>
+    <tableColumn id="5" name="Action Title" dataDxfId="10"/>
+    <tableColumn id="6" name="Button Type" dataDxfId="9"/>
+    <tableColumn id="7" name="Menu" dataDxfId="8"/>
+    <tableColumn id="8" name="Icon" dataDxfId="7"/>
+    <tableColumn id="9" name="Set" dataDxfId="6"/>
+    <tableColumn id="14" name="Action Type" dataDxfId="5"/>
+    <tableColumn id="15" name="ID1" dataDxfId="4"/>
+    <tableColumn id="16" name="ID2" dataDxfId="3"/>
+    <tableColumn id="10" name="On" dataDxfId="2"/>
+    <tableColumn id="11" name="Confirm" dataDxfId="1"/>
+    <tableColumn id="12" name="handler" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Columns" displayName="Columns" ref="A1:I161" totalsRowShown="0" dataDxfId="109">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Columns" displayName="Columns" ref="A1:I161" totalsRowShown="0" dataDxfId="105">
   <autoFilter ref="A1:I161">
     <filterColumn colId="0"/>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" name="Column" dataDxfId="108"/>
-    <tableColumn id="2" name="Type" dataDxfId="107"/>
-    <tableColumn id="3" name="Name" dataDxfId="106"/>
-    <tableColumn id="4" name="Length/Enum" dataDxfId="105"/>
-    <tableColumn id="5" name="Method1" dataDxfId="104"/>
-    <tableColumn id="6" name="Method2" dataDxfId="103"/>
-    <tableColumn id="7" name="Method3" dataDxfId="102"/>
-    <tableColumn id="8" name="Method4" dataDxfId="101"/>
-    <tableColumn id="9" name="Method5" dataDxfId="100"/>
+    <tableColumn id="1" name="Column" dataDxfId="104"/>
+    <tableColumn id="2" name="Type" dataDxfId="103"/>
+    <tableColumn id="3" name="Name" dataDxfId="102"/>
+    <tableColumn id="4" name="Length/Enum" dataDxfId="101"/>
+    <tableColumn id="5" name="Method1" dataDxfId="100"/>
+    <tableColumn id="6" name="Method2" dataDxfId="99"/>
+    <tableColumn id="7" name="Method3" dataDxfId="98"/>
+    <tableColumn id="8" name="Method4" dataDxfId="97"/>
+    <tableColumn id="9" name="Method5" dataDxfId="96"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TableFields" displayName="TableFields" ref="A1:K373" totalsRowShown="0" dataDxfId="99">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TableFields" displayName="TableFields" ref="A1:K373" totalsRowShown="0" dataDxfId="95">
   <autoFilter ref="A1:K373">
     <filterColumn colId="0">
       <filters>
@@ -4537,33 +4489,33 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="11">
-    <tableColumn id="2" name="Table" dataDxfId="98"/>
-    <tableColumn id="3" name="Field" dataDxfId="97"/>
-    <tableColumn id="5" name="Type" dataDxfId="96">
+    <tableColumn id="2" name="Table" dataDxfId="94"/>
+    <tableColumn id="3" name="Field" dataDxfId="93"/>
+    <tableColumn id="5" name="Type" dataDxfId="92">
       <calculatedColumnFormula>VLOOKUP([Field],Columns[],2,0)&amp;"("</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Name" dataDxfId="95">
+    <tableColumn id="4" name="Name" dataDxfId="91">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Arg2" dataDxfId="94">
+    <tableColumn id="6" name="Arg2" dataDxfId="90">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Method1" dataDxfId="93">
+    <tableColumn id="7" name="Method1" dataDxfId="89">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Method2" dataDxfId="92">
+    <tableColumn id="8" name="Method2" dataDxfId="88">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Method3" dataDxfId="91">
+    <tableColumn id="9" name="Method3" dataDxfId="87">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Method4" dataDxfId="90">
+    <tableColumn id="10" name="Method4" dataDxfId="86">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Method5" dataDxfId="89">
+    <tableColumn id="11" name="Method5" dataDxfId="85">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Statement" dataDxfId="88">
+    <tableColumn id="12" name="Statement" dataDxfId="84">
       <calculatedColumnFormula>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4572,51 +4524,51 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R322" totalsRowShown="0" headerRowDxfId="87" dataDxfId="86">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R322" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
   <autoFilter ref="A1:R322">
     <filterColumn colId="1"/>
   </autoFilter>
   <tableColumns count="18">
-    <tableColumn id="19" name="TRCode" dataDxfId="85">
+    <tableColumn id="19" name="TRCode" dataDxfId="81">
       <calculatedColumnFormula>[Table Name]&amp;"-"&amp;[Record No]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Table Name" dataDxfId="84"/>
-    <tableColumn id="2" name="Record No" dataDxfId="83">
+    <tableColumn id="1" name="Table Name" dataDxfId="80"/>
+    <tableColumn id="2" name="Record No" dataDxfId="79">
       <calculatedColumnFormula>COUNTIF($B$1:$B1,[Table Name])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="1" dataDxfId="82"/>
-    <tableColumn id="4" name="2" dataDxfId="81"/>
-    <tableColumn id="5" name="3" dataDxfId="80"/>
-    <tableColumn id="6" name="4" dataDxfId="79"/>
-    <tableColumn id="7" name="5" dataDxfId="78"/>
-    <tableColumn id="8" name="6" dataDxfId="77"/>
-    <tableColumn id="9" name="7" dataDxfId="76"/>
-    <tableColumn id="10" name="8" dataDxfId="75"/>
-    <tableColumn id="11" name="9" dataDxfId="74"/>
-    <tableColumn id="12" name="10" dataDxfId="73"/>
-    <tableColumn id="13" name="11" dataDxfId="72"/>
-    <tableColumn id="14" name="12" dataDxfId="71"/>
-    <tableColumn id="15" name="13" dataDxfId="70"/>
-    <tableColumn id="16" name="14" dataDxfId="69"/>
-    <tableColumn id="17" name="15" dataDxfId="68"/>
+    <tableColumn id="3" name="1" dataDxfId="78"/>
+    <tableColumn id="4" name="2" dataDxfId="77"/>
+    <tableColumn id="5" name="3" dataDxfId="76"/>
+    <tableColumn id="6" name="4" dataDxfId="75"/>
+    <tableColumn id="7" name="5" dataDxfId="74"/>
+    <tableColumn id="8" name="6" dataDxfId="73"/>
+    <tableColumn id="9" name="7" dataDxfId="72"/>
+    <tableColumn id="10" name="8" dataDxfId="71"/>
+    <tableColumn id="11" name="9" dataDxfId="70"/>
+    <tableColumn id="12" name="10" dataDxfId="69"/>
+    <tableColumn id="13" name="11" dataDxfId="68"/>
+    <tableColumn id="14" name="12" dataDxfId="67"/>
+    <tableColumn id="15" name="13" dataDxfId="66"/>
+    <tableColumn id="16" name="14" dataDxfId="65"/>
+    <tableColumn id="17" name="15" dataDxfId="64"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SeedMap" displayName="SeedMap" ref="A1:E36" totalsRowShown="0" dataDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SeedMap" displayName="SeedMap" ref="A1:E36" totalsRowShown="0" dataDxfId="63">
   <autoFilter ref="A1:E36"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Name" dataDxfId="66"/>
-    <tableColumn id="3" name="FW Table Name" dataDxfId="65"/>
-    <tableColumn id="20" name="NS" dataDxfId="64">
+    <tableColumn id="1" name="Name" dataDxfId="62"/>
+    <tableColumn id="3" name="FW Table Name" dataDxfId="61"/>
+    <tableColumn id="20" name="NS" dataDxfId="60">
       <calculatedColumnFormula>VLOOKUP([FW Table Name],Tables[],4,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="Model" dataDxfId="63">
+    <tableColumn id="21" name="Model" dataDxfId="59">
       <calculatedColumnFormula>VLOOKUP([FW Table Name],Tables[],5,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Query Method" dataDxfId="62">
+    <tableColumn id="4" name="Query Method" dataDxfId="58">
       <calculatedColumnFormula>"truncate"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4625,46 +4577,46 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="ResourceTable" displayName="ResourceTable" ref="A1:I37" totalsRowShown="0" dataDxfId="61">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="ResourceTable" displayName="ResourceTable" ref="A1:I37" totalsRowShown="0" dataDxfId="57">
   <autoFilter ref="A1:I37"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="No" dataDxfId="60">
+    <tableColumn id="1" name="No" dataDxfId="56">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Name" dataDxfId="59"/>
-    <tableColumn id="3" name="Description" dataDxfId="58"/>
-    <tableColumn id="4" name="Title" dataDxfId="57"/>
-    <tableColumn id="5" name="NS" dataDxfId="56">
+    <tableColumn id="2" name="Name" dataDxfId="55"/>
+    <tableColumn id="3" name="Description" dataDxfId="54"/>
+    <tableColumn id="4" name="Title" dataDxfId="53"/>
+    <tableColumn id="5" name="NS" dataDxfId="52">
       <calculatedColumnFormula>"Milestone\Appframe\Model"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Table" dataDxfId="55"/>
-    <tableColumn id="7" name="Key" dataDxfId="54">
+    <tableColumn id="6" name="Table" dataDxfId="51"/>
+    <tableColumn id="7" name="Key" dataDxfId="50">
       <calculatedColumnFormula>"id"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Controller" dataDxfId="53"/>
-    <tableColumn id="9" name="Controller NS" dataDxfId="52"/>
+    <tableColumn id="8" name="Controller" dataDxfId="49"/>
+    <tableColumn id="9" name="Controller NS" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RelationTable" displayName="RelationTable" ref="A1:I50" totalsRowShown="0" dataDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RelationTable" displayName="RelationTable" ref="A1:I50" totalsRowShown="0" dataDxfId="47">
   <autoFilter ref="A1:I50"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="No" dataDxfId="50">
+    <tableColumn id="1" name="No" dataDxfId="46">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Resource" dataDxfId="49"/>
-    <tableColumn id="4" name="Relate Resource" dataDxfId="48"/>
-    <tableColumn id="2" name="Resource Id" dataDxfId="47">
+    <tableColumn id="3" name="Resource" dataDxfId="45"/>
+    <tableColumn id="4" name="Relate Resource" dataDxfId="44"/>
+    <tableColumn id="2" name="Resource Id" dataDxfId="43">
       <calculatedColumnFormula>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Name" dataDxfId="46"/>
-    <tableColumn id="6" name="Description" dataDxfId="45"/>
-    <tableColumn id="7" name="Method" dataDxfId="44"/>
-    <tableColumn id="8" name="Type" dataDxfId="43"/>
-    <tableColumn id="10" name="Relate Id" dataDxfId="42">
+    <tableColumn id="5" name="Name" dataDxfId="42"/>
+    <tableColumn id="6" name="Description" dataDxfId="41"/>
+    <tableColumn id="7" name="Method" dataDxfId="40"/>
+    <tableColumn id="8" name="Type" dataDxfId="39"/>
+    <tableColumn id="10" name="Relate Id" dataDxfId="38">
       <calculatedColumnFormula>VLOOKUP([Relate Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4673,47 +4625,47 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="ResourceForms" displayName="ResourceForms" ref="A1:G9" totalsRowShown="0" dataDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="ResourceForms" displayName="ResourceForms" ref="A1:G9" totalsRowShown="0" dataDxfId="37">
   <autoFilter ref="A1:G9"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="No" dataDxfId="40">
+    <tableColumn id="1" name="No" dataDxfId="36">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Resource ID" dataDxfId="39"/>
-    <tableColumn id="3" name="Resource Name" dataDxfId="38">
+    <tableColumn id="2" name="Resource ID" dataDxfId="35"/>
+    <tableColumn id="3" name="Resource Name" dataDxfId="34">
       <calculatedColumnFormula>VLOOKUP([Resource ID],ResourceTable[],2,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Form Name" dataDxfId="37"/>
-    <tableColumn id="6" name="Title" dataDxfId="36"/>
-    <tableColumn id="7" name="Action Text" dataDxfId="35"/>
-    <tableColumn id="8" name="Description" dataDxfId="34"/>
+    <tableColumn id="4" name="Form Name" dataDxfId="33"/>
+    <tableColumn id="6" name="Title" dataDxfId="32"/>
+    <tableColumn id="7" name="Action Text" dataDxfId="31"/>
+    <tableColumn id="8" name="Description" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="FormFields" displayName="FormFields" ref="A1:L33" totalsRowShown="0" dataDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="FormFields" displayName="FormFields" ref="A1:L33" totalsRowShown="0" dataDxfId="29">
   <autoFilter ref="A1:L33"/>
   <tableColumns count="12">
-    <tableColumn id="9" name="No" dataDxfId="32">
+    <tableColumn id="9" name="No" dataDxfId="28">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Form Id" dataDxfId="31"/>
-    <tableColumn id="7" name="Form Name" dataDxfId="30">
+    <tableColumn id="1" name="Form Id" dataDxfId="27"/>
+    <tableColumn id="7" name="Form Name" dataDxfId="26">
       <calculatedColumnFormula>VLOOKUP([Form Id],ResourceForms[],4,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Name" dataDxfId="29"/>
-    <tableColumn id="2" name="Type" dataDxfId="28"/>
-    <tableColumn id="5" name="Label" dataDxfId="27"/>
-    <tableColumn id="6" name="Collection" dataDxfId="26"/>
-    <tableColumn id="14" name="Attribute" dataDxfId="25">
+    <tableColumn id="4" name="Name" dataDxfId="25"/>
+    <tableColumn id="2" name="Type" dataDxfId="24"/>
+    <tableColumn id="5" name="Label" dataDxfId="23"/>
+    <tableColumn id="6" name="Collection" dataDxfId="22"/>
+    <tableColumn id="14" name="Attribute" dataDxfId="21">
       <calculatedColumnFormula>[Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Relation" dataDxfId="24"/>
-    <tableColumn id="11" name="Deep 1" dataDxfId="23"/>
-    <tableColumn id="12" name="Deep 2" dataDxfId="22"/>
-    <tableColumn id="13" name="Deep 3" dataDxfId="21"/>
+    <tableColumn id="10" name="Relation" dataDxfId="20"/>
+    <tableColumn id="11" name="Deep 1" dataDxfId="19"/>
+    <tableColumn id="12" name="Deep 2" dataDxfId="18"/>
+    <tableColumn id="13" name="Deep 3" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6491,7 +6443,7 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="4" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B37" s="7" t="str">
         <f>"__"&amp;[Name]</f>
@@ -6532,7 +6484,7 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="4" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B38" s="7" t="str">
         <f>"__"&amp;[Name]</f>
@@ -6573,7 +6525,7 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="4" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B39" s="7" t="str">
         <f>"__"&amp;[Name]</f>
@@ -8319,7 +8271,7 @@
   <dimension ref="A1:I161"/>
   <sheetViews>
     <sheetView topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="A161" sqref="A161"/>
+      <selection activeCell="C143" sqref="C143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="15"/>
@@ -10476,7 +10428,7 @@
         <v>49</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="E100" s="4" t="s">
         <v>245</v>
@@ -11395,13 +11347,13 @@
         <v>48</v>
       </c>
       <c r="C142" s="4" t="s">
+        <v>777</v>
+      </c>
+      <c r="D142" s="4" t="s">
+        <v>704</v>
+      </c>
+      <c r="E142" s="4" t="s">
         <v>703</v>
-      </c>
-      <c r="D142" s="4" t="s">
-        <v>705</v>
-      </c>
-      <c r="E142" s="4" t="s">
-        <v>704</v>
       </c>
       <c r="F142" s="4"/>
       <c r="G142" s="4"/>
@@ -11410,13 +11362,13 @@
     </row>
     <row r="143" spans="1:9">
       <c r="A143" s="4" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B143" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D143" s="4">
         <v>64</v>
@@ -11431,16 +11383,16 @@
     </row>
     <row r="144" spans="1:9">
       <c r="A144" s="4" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B144" s="4" t="s">
         <v>48</v>
       </c>
       <c r="C144" s="4" t="s">
+        <v>708</v>
+      </c>
+      <c r="D144" s="4" t="s">
         <v>709</v>
-      </c>
-      <c r="D144" s="4" t="s">
-        <v>710</v>
       </c>
       <c r="E144" s="4" t="s">
         <v>643</v>
@@ -11452,19 +11404,19 @@
     </row>
     <row r="145" spans="1:9">
       <c r="A145" s="4" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B145" s="4" t="s">
         <v>48</v>
       </c>
       <c r="C145" s="4" t="s">
+        <v>711</v>
+      </c>
+      <c r="D145" s="4" t="s">
         <v>712</v>
       </c>
-      <c r="D145" s="4" t="s">
+      <c r="E145" s="4" t="s">
         <v>713</v>
-      </c>
-      <c r="E145" s="4" t="s">
-        <v>714</v>
       </c>
       <c r="F145" s="4"/>
       <c r="G145" s="4"/>
@@ -11473,19 +11425,19 @@
     </row>
     <row r="146" spans="1:9">
       <c r="A146" s="4" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="B146" s="4" t="s">
         <v>48</v>
       </c>
       <c r="C146" s="4" t="s">
+        <v>715</v>
+      </c>
+      <c r="D146" s="4" t="s">
         <v>716</v>
       </c>
-      <c r="D146" s="4" t="s">
+      <c r="E146" s="4" t="s">
         <v>717</v>
-      </c>
-      <c r="E146" s="4" t="s">
-        <v>718</v>
       </c>
       <c r="F146" s="4"/>
       <c r="G146" s="4"/>
@@ -11494,17 +11446,17 @@
     </row>
     <row r="147" spans="1:9">
       <c r="A147" s="4" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B147" s="4" t="s">
         <v>590</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="D147" s="4"/>
       <c r="E147" s="4" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="F147" s="4"/>
       <c r="G147" s="4"/>
@@ -11513,13 +11465,13 @@
     </row>
     <row r="148" spans="1:9">
       <c r="A148" s="4" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B148" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="D148" s="4">
         <v>64</v>
@@ -11534,17 +11486,17 @@
     </row>
     <row r="149" spans="1:9">
       <c r="A149" s="4" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B149" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="D149" s="4"/>
       <c r="E149" s="4" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="F149" s="4"/>
       <c r="G149" s="4"/>
@@ -11553,13 +11505,13 @@
     </row>
     <row r="150" spans="1:9">
       <c r="A150" s="4" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B150" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="D150" s="4"/>
       <c r="E150" s="4" t="s">
@@ -11572,20 +11524,20 @@
     </row>
     <row r="151" spans="1:9">
       <c r="A151" s="4" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B151" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="D151" s="4"/>
       <c r="E151" s="4" t="s">
         <v>43</v>
       </c>
       <c r="F151" s="4" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="G151" s="4" t="s">
         <v>45</v>
@@ -11597,7 +11549,7 @@
     </row>
     <row r="152" spans="1:9">
       <c r="A152" s="4" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B152" s="5" t="s">
         <v>24</v>
@@ -11616,7 +11568,7 @@
     </row>
     <row r="153" spans="1:9">
       <c r="A153" s="4" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B153" s="4" t="s">
         <v>42</v>
@@ -11629,7 +11581,7 @@
         <v>43</v>
       </c>
       <c r="F153" s="4" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="G153" s="4" t="s">
         <v>45</v>
@@ -11641,7 +11593,7 @@
     </row>
     <row r="154" spans="1:9">
       <c r="A154" s="4" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B154" s="4" t="s">
         <v>590</v>
@@ -11660,19 +11612,19 @@
     </row>
     <row r="155" spans="1:9">
       <c r="A155" s="4" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B155" s="4" t="s">
         <v>48</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="D155" s="4" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E155" s="4" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="F155" s="4"/>
       <c r="G155" s="4"/>
@@ -11681,13 +11633,13 @@
     </row>
     <row r="156" spans="1:9">
       <c r="A156" s="4" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B156" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="D156" s="4">
         <v>64</v>
@@ -11702,13 +11654,13 @@
     </row>
     <row r="157" spans="1:9">
       <c r="A157" s="4" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B157" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="D157" s="4">
         <v>64</v>
@@ -11723,7 +11675,7 @@
     </row>
     <row r="158" spans="1:9">
       <c r="A158" s="4" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="B158" s="4" t="s">
         <v>27</v>
@@ -11744,13 +11696,13 @@
     </row>
     <row r="159" spans="1:9">
       <c r="A159" s="4" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="B159" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="D159" s="4">
         <v>64</v>
@@ -11765,17 +11717,17 @@
     </row>
     <row r="160" spans="1:9">
       <c r="A160" s="4" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="B160" s="4" t="s">
         <v>590</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="D160" s="4"/>
       <c r="E160" s="4" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="F160" s="4"/>
       <c r="G160" s="4"/>
@@ -11784,7 +11736,7 @@
     </row>
     <row r="161" spans="1:9">
       <c r="A161" s="4" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="B161" s="4" t="s">
         <v>48</v>
@@ -11793,10 +11745,10 @@
         <v>49</v>
       </c>
       <c r="D161" s="4" t="s">
+        <v>775</v>
+      </c>
+      <c r="E161" s="4" t="s">
         <v>776</v>
-      </c>
-      <c r="E161" s="4" t="s">
-        <v>777</v>
       </c>
       <c r="F161" s="4"/>
       <c r="G161" s="4"/>
@@ -11805,25 +11757,25 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A43:A46">
-    <cfRule type="duplicateValues" dxfId="116" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="112" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56:A59">
-    <cfRule type="duplicateValues" dxfId="115" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="111" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A161">
-    <cfRule type="duplicateValues" dxfId="114" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="110" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A128:A129">
-    <cfRule type="duplicateValues" dxfId="113" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="109" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A128:A129">
-    <cfRule type="duplicateValues" dxfId="112" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="108" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A130:A131">
-    <cfRule type="duplicateValues" dxfId="111" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="107" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A152:A153">
-    <cfRule type="duplicateValues" dxfId="110" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="106" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -11837,8 +11789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K373"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A327" workbookViewId="0">
-      <selection activeCell="B344" sqref="B344"/>
+    <sheetView topLeftCell="A327" workbookViewId="0">
+      <selection activeCell="B340" sqref="B340"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="15"/>
@@ -26673,7 +26625,7 @@
         <v>701</v>
       </c>
       <c r="B338" s="4" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="C338" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -26769,7 +26721,7 @@
       </c>
       <c r="D340" s="4" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'aggregates'</v>
+        <v>'aggregate'</v>
       </c>
       <c r="E340" s="7" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
@@ -26797,7 +26749,7 @@
       </c>
       <c r="K340" s="4" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;enum('aggregates', ['COUNT','SUM','AVG','MAX','MIN'])-&gt;default('COUNT');</v>
+        <v>$table-&gt;enum('aggregate', ['COUNT','SUM','AVG','MAX','MIN'])-&gt;default('COUNT');</v>
       </c>
     </row>
     <row r="341" spans="1:11">
@@ -26805,7 +26757,7 @@
         <v>701</v>
       </c>
       <c r="B341" s="4" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C341" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -26849,7 +26801,7 @@
         <v>701</v>
       </c>
       <c r="B342" s="5" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="C342" s="5" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -26893,7 +26845,7 @@
         <v>701</v>
       </c>
       <c r="B343" s="5" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="C343" s="5" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -26937,7 +26889,7 @@
         <v>701</v>
       </c>
       <c r="B344" s="5" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="C344" s="5" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -26981,7 +26933,7 @@
         <v>701</v>
       </c>
       <c r="B345" s="5" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="C345" s="5" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -27198,7 +27150,7 @@
     </row>
     <row r="350" spans="1:11">
       <c r="A350" s="4" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B350" s="4" t="s">
         <v>21</v>
@@ -27242,7 +27194,7 @@
     </row>
     <row r="351" spans="1:11">
       <c r="A351" s="4" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B351" s="4" t="s">
         <v>23</v>
@@ -27286,7 +27238,7 @@
     </row>
     <row r="352" spans="1:11">
       <c r="A352" s="4" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B352" s="4" t="s">
         <v>26</v>
@@ -27330,7 +27282,7 @@
     </row>
     <row r="353" spans="1:11">
       <c r="A353" s="4" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B353" s="4" t="s">
         <v>28</v>
@@ -27374,7 +27326,7 @@
     </row>
     <row r="354" spans="1:11">
       <c r="A354" s="4" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B354" s="4" t="s">
         <v>30</v>
@@ -27418,7 +27370,7 @@
     </row>
     <row r="355" spans="1:11">
       <c r="A355" s="4" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B355" s="4" t="s">
         <v>36</v>
@@ -27462,7 +27414,7 @@
     </row>
     <row r="356" spans="1:11">
       <c r="A356" s="4" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B356" s="4" t="s">
         <v>40</v>
@@ -27506,7 +27458,7 @@
     </row>
     <row r="357" spans="1:11">
       <c r="A357" s="4" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B357" s="4" t="s">
         <v>41</v>
@@ -27550,7 +27502,7 @@
     </row>
     <row r="358" spans="1:11">
       <c r="A358" s="4" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B358" s="4" t="s">
         <v>21</v>
@@ -27594,10 +27546,10 @@
     </row>
     <row r="359" spans="1:11" s="26" customFormat="1">
       <c r="A359" s="4" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B359" s="4" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="C359" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -27638,7 +27590,7 @@
     </row>
     <row r="360" spans="1:11">
       <c r="A360" s="4" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B360" s="4" t="s">
         <v>26</v>
@@ -27682,7 +27634,7 @@
     </row>
     <row r="361" spans="1:11">
       <c r="A361" s="4" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B361" s="4" t="s">
         <v>30</v>
@@ -27726,10 +27678,10 @@
     </row>
     <row r="362" spans="1:11">
       <c r="A362" s="4" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B362" s="4" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C362" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -27770,7 +27722,7 @@
     </row>
     <row r="363" spans="1:11">
       <c r="A363" s="4" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B363" s="4" t="s">
         <v>40</v>
@@ -27814,10 +27766,10 @@
     </row>
     <row r="364" spans="1:11">
       <c r="A364" s="4" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B364" s="4" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C364" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -27858,7 +27810,7 @@
     </row>
     <row r="365" spans="1:11">
       <c r="A365" s="4" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B365" s="4" t="s">
         <v>21</v>
@@ -27902,10 +27854,10 @@
     </row>
     <row r="366" spans="1:11">
       <c r="A366" s="4" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B366" s="4" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C366" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -27946,10 +27898,10 @@
     </row>
     <row r="367" spans="1:11">
       <c r="A367" s="4" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B367" s="4" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C367" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -27990,7 +27942,7 @@
     </row>
     <row r="368" spans="1:11">
       <c r="A368" s="4" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B368" s="4" t="s">
         <v>30</v>
@@ -28034,10 +27986,10 @@
     </row>
     <row r="369" spans="1:11">
       <c r="A369" s="4" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B369" s="4" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="C369" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -28078,10 +28030,10 @@
     </row>
     <row r="370" spans="1:11">
       <c r="A370" s="4" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B370" s="4" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="C370" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -28122,10 +28074,10 @@
     </row>
     <row r="371" spans="1:11">
       <c r="A371" s="4" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B371" s="4" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="C371" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -28166,7 +28118,7 @@
     </row>
     <row r="372" spans="1:11">
       <c r="A372" s="4" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B372" s="4" t="s">
         <v>40</v>
@@ -28210,10 +28162,10 @@
     </row>
     <row r="373" spans="1:11">
       <c r="A373" s="4" t="s">
+        <v>730</v>
+      </c>
+      <c r="B373" s="4" t="s">
         <v>731</v>
-      </c>
-      <c r="B373" s="4" t="s">
-        <v>732</v>
       </c>
       <c r="C373" s="4" t="str">
         <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
@@ -28274,8 +28226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R322"/>
   <sheetViews>
-    <sheetView topLeftCell="B301" workbookViewId="0">
-      <selection activeCell="B314" sqref="B314"/>
+    <sheetView tabSelected="1" topLeftCell="B301" workbookViewId="0">
+      <selection activeCell="G314" sqref="G314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -39582,7 +39534,7 @@
         <v>Dashboard-0</v>
       </c>
       <c r="B311" s="43" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="C311" s="42">
         <f>COUNTIF($B$1:$B310,[Table Name])</f>
@@ -39620,14 +39572,14 @@
         <v>Dashboard Sections-0</v>
       </c>
       <c r="B312" s="43" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C312" s="42">
         <f>COUNTIF($B$1:$B311,[Table Name])</f>
         <v>0</v>
       </c>
       <c r="D312" s="43" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E312" s="43" t="s">
         <v>26</v>
@@ -39636,7 +39588,7 @@
         <v>30</v>
       </c>
       <c r="G312" s="43" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="H312" s="43"/>
       <c r="I312" s="43"/>
@@ -39656,7 +39608,7 @@
         <v>Dashboard Section Items-0</v>
       </c>
       <c r="B313" s="43" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="C313" s="42">
         <f>COUNTIF($B$1:$B312,[Table Name])</f>
@@ -39672,13 +39624,13 @@
         <v>30</v>
       </c>
       <c r="G313" s="43" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="H313" s="43" t="s">
+        <v>738</v>
+      </c>
+      <c r="I313" s="43" t="s">
         <v>739</v>
-      </c>
-      <c r="I313" s="43" t="s">
-        <v>740</v>
       </c>
       <c r="J313" s="43"/>
       <c r="K313" s="43"/>
@@ -39696,7 +39648,7 @@
         <v>Resource Metrics-0</v>
       </c>
       <c r="B314" s="40" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="C314" s="22">
         <f>COUNTIF($B$1:$B313,[Table Name])</f>
@@ -39715,22 +39667,22 @@
         <v>94</v>
       </c>
       <c r="H314" s="40" t="s">
-        <v>703</v>
+        <v>777</v>
       </c>
       <c r="I314" s="40" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="J314" s="40" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="K314" s="40" t="s">
         <v>560</v>
       </c>
       <c r="L314" s="40" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="M314" s="40" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="N314" s="40" t="s">
         <v>36</v>
@@ -39753,19 +39705,19 @@
         <v>33</v>
       </c>
       <c r="D315" s="43" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="E315" s="43" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="F315" s="43" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="G315" s="43" t="s">
         <v>558</v>
       </c>
       <c r="H315" s="43" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="I315" s="43" t="s">
         <v>21</v>
@@ -39793,19 +39745,19 @@
         <v>34</v>
       </c>
       <c r="D316" s="43" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="E316" s="43" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="F316" s="43" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="G316" s="43" t="s">
         <v>558</v>
       </c>
       <c r="H316" s="43" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="I316" s="43" t="s">
         <v>21</v>
@@ -39833,19 +39785,19 @@
         <v>35</v>
       </c>
       <c r="D317" s="43" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E317" s="43" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="F317" s="43" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="G317" s="43" t="s">
         <v>558</v>
       </c>
       <c r="H317" s="43" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="I317" s="43" t="s">
         <v>21</v>
@@ -39873,19 +39825,19 @@
         <v>36</v>
       </c>
       <c r="D318" s="40" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="E318" s="40" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="F318" s="40" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="G318" s="40" t="s">
         <v>558</v>
       </c>
       <c r="H318" s="40" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="I318" s="40" t="s">
         <v>21</v>
@@ -39916,13 +39868,13 @@
         <v>4</v>
       </c>
       <c r="E319" s="43" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="F319" s="43" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="G319" s="43" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="H319" s="43" t="s">
         <v>310</v>
@@ -39956,10 +39908,10 @@
         <v>33</v>
       </c>
       <c r="E320" s="43" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="F320" s="43" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="G320" s="43" t="s">
         <v>609</v>
@@ -39996,10 +39948,10 @@
         <v>34</v>
       </c>
       <c r="E321" s="43" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="F321" s="43" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="G321" s="43" t="s">
         <v>616</v>
@@ -40036,10 +39988,10 @@
         <v>33</v>
       </c>
       <c r="E322" s="40" t="s">
+        <v>765</v>
+      </c>
+      <c r="F322" s="40" t="s">
         <v>766</v>
-      </c>
-      <c r="F322" s="40" t="s">
-        <v>767</v>
       </c>
       <c r="G322" s="40" t="s">
         <v>208</v>
@@ -40727,10 +40679,10 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="5" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="C33" s="5" t="str">
         <f>VLOOKUP([FW Table Name],Tables[],4,0)</f>
@@ -40747,10 +40699,10 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="5" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="C34" s="5" t="str">
         <f>VLOOKUP([FW Table Name],Tables[],4,0)</f>
@@ -40767,10 +40719,10 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="5" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C35" s="5" t="str">
         <f>VLOOKUP([FW Table Name],Tables[],4,0)</f>
@@ -40787,7 +40739,7 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="4" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>701</v>
@@ -41772,20 +41724,20 @@
         <v>33</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="E34" s="8" t="str">
         <f>"Milestone\Appframe\Model"</f>
         <v>Milestone\Appframe\Model</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="G34" s="46" t="str">
         <f>"id"</f>
@@ -41800,20 +41752,20 @@
         <v>34</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E35" s="8" t="str">
         <f>"Milestone\Appframe\Model"</f>
         <v>Milestone\Appframe\Model</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="G35" s="46" t="str">
         <f>"id"</f>
@@ -41828,20 +41780,20 @@
         <v>35</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="E36" s="8" t="str">
         <f>"Milestone\Appframe\Model"</f>
         <v>Milestone\Appframe\Model</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="G36" s="46" t="str">
         <f>"id"</f>
@@ -41856,20 +41808,20 @@
         <v>36</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E37" s="7" t="str">
         <f>"Milestone\Appframe\Model"</f>
         <v>Milestone\Appframe\Model</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="G37" s="21" t="str">
         <f>"id"</f>
@@ -43393,20 +43345,20 @@
         <v>208</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="D47" s="7">
         <f>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</f>
         <v>4</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="G47" s="22" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="H47" s="7" t="s">
         <v>310</v>
@@ -43422,20 +43374,20 @@
         <v>47</v>
       </c>
       <c r="B48" s="7" t="s">
+        <v>746</v>
+      </c>
+      <c r="C48" s="7" t="s">
         <v>747</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>748</v>
       </c>
       <c r="D48" s="7">
         <f>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</f>
         <v>33</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="G48" s="22" t="s">
         <v>609</v>
@@ -43454,20 +43406,20 @@
         <v>48</v>
       </c>
       <c r="B49" s="7" t="s">
+        <v>747</v>
+      </c>
+      <c r="C49" s="7" t="s">
         <v>748</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>749</v>
       </c>
       <c r="D49" s="7">
         <f>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</f>
         <v>34</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="G49" s="22" t="s">
         <v>616</v>
@@ -43486,7 +43438,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>208</v>
@@ -43496,10 +43448,10 @@
         <v>33</v>
       </c>
       <c r="E50" s="7" t="s">
+        <v>765</v>
+      </c>
+      <c r="F50" s="7" t="s">
         <v>766</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>767</v>
       </c>
       <c r="G50" s="22" t="s">
         <v>208</v>
@@ -43541,7 +43493,7 @@
   <sheetData>
     <row r="1" spans="1:20" s="38" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="50" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="50"/>
@@ -43708,7 +43660,7 @@
       </c>
       <c r="G5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0))</f>
-        <v>aggregates</v>
+        <v>aggregate</v>
       </c>
       <c r="H5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],H$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],H$4+$B$4,0))</f>

</xml_diff>

<commit_message>
For dynamic form field, db table created
</commit_message>
<xml_diff>
--- a/Helper.xlsx
+++ b/Helper.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Tables" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3722" uniqueCount="778">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3779" uniqueCount="794">
   <si>
     <t>resource_scopes</t>
   </si>
@@ -2372,6 +2372,54 @@
   </si>
   <si>
     <t>aggregate</t>
+  </si>
+  <si>
+    <t>resource_form_field_dynamic</t>
+  </si>
+  <si>
+    <t>field_dynamic_type</t>
+  </si>
+  <si>
+    <t>default('disabled-enabled')</t>
+  </si>
+  <si>
+    <t>['disabled-enabled','enabled-disabled','hidden-visible','visible-hidden','readonly-editable','editable-readonly']</t>
+  </si>
+  <si>
+    <t>field_dynamic_alter_on</t>
+  </si>
+  <si>
+    <t>alter_on</t>
+  </si>
+  <si>
+    <t>['not null','value','null']</t>
+  </si>
+  <si>
+    <t>default('not null')</t>
+  </si>
+  <si>
+    <t>field_dynamic_value</t>
+  </si>
+  <si>
+    <t>field_dynamic_value_array</t>
+  </si>
+  <si>
+    <t>value_array</t>
+  </si>
+  <si>
+    <t>field_dynamic_multiple_comparison</t>
+  </si>
+  <si>
+    <t>on_multiple</t>
+  </si>
+  <si>
+    <t>['and','or']</t>
+  </si>
+  <si>
+    <t>default('and')</t>
+  </si>
+  <si>
+    <t>Field Dynamic</t>
   </si>
 </sst>
 </file>
@@ -2607,7 +2655,209 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="124">
+  <dxfs count="129">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -3995,148 +4245,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <condense val="0"/>
         <extend val="0"/>
         <color rgb="FF9C0006"/>
@@ -4393,35 +4501,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tables" displayName="Tables" ref="A1:J42" totalsRowShown="0" dataDxfId="123">
-  <autoFilter ref="A1:J42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tables" displayName="Tables" ref="A1:J43" totalsRowShown="0" dataDxfId="128">
+  <autoFilter ref="A1:J43"/>
   <tableColumns count="10">
-    <tableColumn id="2" name="Name" dataDxfId="122"/>
-    <tableColumn id="10" name="Table" dataDxfId="121">
+    <tableColumn id="2" name="Name" dataDxfId="127"/>
+    <tableColumn id="10" name="Table" dataDxfId="126">
       <calculatedColumnFormula>"__"&amp;[Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Singular Name" dataDxfId="120">
+    <tableColumn id="5" name="Singular Name" dataDxfId="125">
       <calculatedColumnFormula>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Model NS" dataDxfId="119">
+    <tableColumn id="8" name="Model NS" dataDxfId="124">
       <calculatedColumnFormula>"Milestone\Appframe\Model"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Class Name" dataDxfId="118">
+    <tableColumn id="4" name="Class Name" dataDxfId="123">
       <calculatedColumnFormula>SUBSTITUTE(PROPER([Singular Name]),"_","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Migration Artisan" dataDxfId="117">
+    <tableColumn id="1" name="Migration Artisan" dataDxfId="122">
       <calculatedColumnFormula>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Model Artisan" dataDxfId="116">
+    <tableColumn id="6" name="Model Artisan" dataDxfId="121">
       <calculatedColumnFormula>"php artisan make:model "&amp;[Class Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Model Statement" dataDxfId="115">
+    <tableColumn id="3" name="Model Statement" dataDxfId="120">
       <calculatedColumnFormula>"protected $table = '"&amp;[Table]&amp;"';"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Seeder Artisan" dataDxfId="114">
+    <tableColumn id="7" name="Seeder Artisan" dataDxfId="119">
       <calculatedColumnFormula>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Seeder Class" dataDxfId="113">
+    <tableColumn id="9" name="Seeder Class" dataDxfId="118">
       <calculatedColumnFormula>[Class Name]&amp;"TableSeeder"&amp;"::class,"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4430,57 +4538,57 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="ResourceActions" displayName="ResourceActions" ref="A1:P9" totalsRowShown="0" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="ResourceActions" displayName="ResourceActions" ref="A1:P9" totalsRowShown="0" dataDxfId="32">
   <autoFilter ref="A1:P9"/>
   <tableColumns count="16">
-    <tableColumn id="1" name="No" dataDxfId="15">
+    <tableColumn id="1" name="No" dataDxfId="31">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Resource" dataDxfId="14"/>
-    <tableColumn id="13" name="Resource Id" dataDxfId="13">
+    <tableColumn id="2" name="Resource" dataDxfId="30"/>
+    <tableColumn id="13" name="Resource Id" dataDxfId="29">
       <calculatedColumnFormula>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Action Name" dataDxfId="12"/>
-    <tableColumn id="4" name="Description" dataDxfId="11"/>
-    <tableColumn id="5" name="Action Title" dataDxfId="10"/>
-    <tableColumn id="6" name="Button Type" dataDxfId="9"/>
-    <tableColumn id="7" name="Menu" dataDxfId="8"/>
-    <tableColumn id="8" name="Icon" dataDxfId="7"/>
-    <tableColumn id="9" name="Set" dataDxfId="6"/>
-    <tableColumn id="14" name="Action Type" dataDxfId="5"/>
-    <tableColumn id="15" name="ID1" dataDxfId="4"/>
-    <tableColumn id="16" name="ID2" dataDxfId="3"/>
-    <tableColumn id="10" name="On" dataDxfId="2"/>
-    <tableColumn id="11" name="Confirm" dataDxfId="1"/>
-    <tableColumn id="12" name="handler" dataDxfId="0"/>
+    <tableColumn id="3" name="Action Name" dataDxfId="28"/>
+    <tableColumn id="4" name="Description" dataDxfId="27"/>
+    <tableColumn id="5" name="Action Title" dataDxfId="26"/>
+    <tableColumn id="6" name="Button Type" dataDxfId="25"/>
+    <tableColumn id="7" name="Menu" dataDxfId="24"/>
+    <tableColumn id="8" name="Icon" dataDxfId="23"/>
+    <tableColumn id="9" name="Set" dataDxfId="22"/>
+    <tableColumn id="14" name="Action Type" dataDxfId="21"/>
+    <tableColumn id="15" name="ID1" dataDxfId="20"/>
+    <tableColumn id="16" name="ID2" dataDxfId="19"/>
+    <tableColumn id="10" name="On" dataDxfId="18"/>
+    <tableColumn id="11" name="Confirm" dataDxfId="17"/>
+    <tableColumn id="12" name="handler" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Columns" displayName="Columns" ref="A1:I161" totalsRowShown="0" dataDxfId="105">
-  <autoFilter ref="A1:I161">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Columns" displayName="Columns" ref="A1:I166" totalsRowShown="0" dataDxfId="1">
+  <autoFilter ref="A1:I166">
     <filterColumn colId="0"/>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" name="Column" dataDxfId="104"/>
-    <tableColumn id="2" name="Type" dataDxfId="103"/>
-    <tableColumn id="3" name="Name" dataDxfId="102"/>
-    <tableColumn id="4" name="Length/Enum" dataDxfId="101"/>
-    <tableColumn id="5" name="Method1" dataDxfId="100"/>
-    <tableColumn id="6" name="Method2" dataDxfId="99"/>
-    <tableColumn id="7" name="Method3" dataDxfId="98"/>
-    <tableColumn id="8" name="Method4" dataDxfId="97"/>
-    <tableColumn id="9" name="Method5" dataDxfId="96"/>
+    <tableColumn id="1" name="Column" dataDxfId="10"/>
+    <tableColumn id="2" name="Type" dataDxfId="9"/>
+    <tableColumn id="3" name="Name" dataDxfId="8"/>
+    <tableColumn id="4" name="Length/Enum" dataDxfId="7"/>
+    <tableColumn id="5" name="Method1" dataDxfId="6"/>
+    <tableColumn id="6" name="Method2" dataDxfId="5"/>
+    <tableColumn id="7" name="Method3" dataDxfId="4"/>
+    <tableColumn id="8" name="Method4" dataDxfId="3"/>
+    <tableColumn id="9" name="Method5" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TableFields" displayName="TableFields" ref="A1:K373" totalsRowShown="0" dataDxfId="95">
-  <autoFilter ref="A1:K373">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TableFields" displayName="TableFields" ref="A1:K384" totalsRowShown="0" dataDxfId="111">
+  <autoFilter ref="A1:K384">
     <filterColumn colId="0">
       <filters>
         <filter val="resource_form_field_depends"/>
@@ -4489,33 +4597,33 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="11">
-    <tableColumn id="2" name="Table" dataDxfId="94"/>
-    <tableColumn id="3" name="Field" dataDxfId="93"/>
-    <tableColumn id="5" name="Type" dataDxfId="92">
+    <tableColumn id="2" name="Table" dataDxfId="110"/>
+    <tableColumn id="3" name="Field" dataDxfId="109"/>
+    <tableColumn id="5" name="Type" dataDxfId="108">
       <calculatedColumnFormula>VLOOKUP([Field],Columns[],2,0)&amp;"("</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Name" dataDxfId="91">
+    <tableColumn id="4" name="Name" dataDxfId="107">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Arg2" dataDxfId="90">
+    <tableColumn id="6" name="Arg2" dataDxfId="106">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Method1" dataDxfId="89">
+    <tableColumn id="7" name="Method1" dataDxfId="105">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Method2" dataDxfId="88">
+    <tableColumn id="8" name="Method2" dataDxfId="104">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Method3" dataDxfId="87">
+    <tableColumn id="9" name="Method3" dataDxfId="103">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Method4" dataDxfId="86">
+    <tableColumn id="10" name="Method4" dataDxfId="102">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Method5" dataDxfId="85">
+    <tableColumn id="11" name="Method5" dataDxfId="101">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Statement" dataDxfId="84">
+    <tableColumn id="12" name="Statement" dataDxfId="100">
       <calculatedColumnFormula>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4524,51 +4632,51 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R322" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
-  <autoFilter ref="A1:R322">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R323" totalsRowShown="0" headerRowDxfId="99" dataDxfId="98">
+  <autoFilter ref="A1:R323">
     <filterColumn colId="1"/>
   </autoFilter>
   <tableColumns count="18">
-    <tableColumn id="19" name="TRCode" dataDxfId="81">
+    <tableColumn id="19" name="TRCode" dataDxfId="97">
       <calculatedColumnFormula>[Table Name]&amp;"-"&amp;[Record No]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Table Name" dataDxfId="80"/>
-    <tableColumn id="2" name="Record No" dataDxfId="79">
+    <tableColumn id="1" name="Table Name" dataDxfId="96"/>
+    <tableColumn id="2" name="Record No" dataDxfId="95">
       <calculatedColumnFormula>COUNTIF($B$1:$B1,[Table Name])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="1" dataDxfId="78"/>
-    <tableColumn id="4" name="2" dataDxfId="77"/>
-    <tableColumn id="5" name="3" dataDxfId="76"/>
-    <tableColumn id="6" name="4" dataDxfId="75"/>
-    <tableColumn id="7" name="5" dataDxfId="74"/>
-    <tableColumn id="8" name="6" dataDxfId="73"/>
-    <tableColumn id="9" name="7" dataDxfId="72"/>
-    <tableColumn id="10" name="8" dataDxfId="71"/>
-    <tableColumn id="11" name="9" dataDxfId="70"/>
-    <tableColumn id="12" name="10" dataDxfId="69"/>
-    <tableColumn id="13" name="11" dataDxfId="68"/>
-    <tableColumn id="14" name="12" dataDxfId="67"/>
-    <tableColumn id="15" name="13" dataDxfId="66"/>
-    <tableColumn id="16" name="14" dataDxfId="65"/>
-    <tableColumn id="17" name="15" dataDxfId="64"/>
+    <tableColumn id="3" name="1" dataDxfId="94"/>
+    <tableColumn id="4" name="2" dataDxfId="93"/>
+    <tableColumn id="5" name="3" dataDxfId="92"/>
+    <tableColumn id="6" name="4" dataDxfId="91"/>
+    <tableColumn id="7" name="5" dataDxfId="90"/>
+    <tableColumn id="8" name="6" dataDxfId="89"/>
+    <tableColumn id="9" name="7" dataDxfId="88"/>
+    <tableColumn id="10" name="8" dataDxfId="87"/>
+    <tableColumn id="11" name="9" dataDxfId="86"/>
+    <tableColumn id="12" name="10" dataDxfId="85"/>
+    <tableColumn id="13" name="11" dataDxfId="84"/>
+    <tableColumn id="14" name="12" dataDxfId="83"/>
+    <tableColumn id="15" name="13" dataDxfId="82"/>
+    <tableColumn id="16" name="14" dataDxfId="81"/>
+    <tableColumn id="17" name="15" dataDxfId="80"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SeedMap" displayName="SeedMap" ref="A1:E36" totalsRowShown="0" dataDxfId="63">
-  <autoFilter ref="A1:E36"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SeedMap" displayName="SeedMap" ref="A1:E37" totalsRowShown="0" dataDxfId="79">
+  <autoFilter ref="A1:E37"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Name" dataDxfId="62"/>
-    <tableColumn id="3" name="FW Table Name" dataDxfId="61"/>
-    <tableColumn id="20" name="NS" dataDxfId="60">
+    <tableColumn id="1" name="Name" dataDxfId="78"/>
+    <tableColumn id="3" name="FW Table Name" dataDxfId="77"/>
+    <tableColumn id="20" name="NS" dataDxfId="76">
       <calculatedColumnFormula>VLOOKUP([FW Table Name],Tables[],4,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="Model" dataDxfId="59">
+    <tableColumn id="21" name="Model" dataDxfId="75">
       <calculatedColumnFormula>VLOOKUP([FW Table Name],Tables[],5,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Query Method" dataDxfId="58">
+    <tableColumn id="4" name="Query Method" dataDxfId="74">
       <calculatedColumnFormula>"truncate"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4577,46 +4685,46 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="ResourceTable" displayName="ResourceTable" ref="A1:I37" totalsRowShown="0" dataDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="ResourceTable" displayName="ResourceTable" ref="A1:I37" totalsRowShown="0" dataDxfId="73">
   <autoFilter ref="A1:I37"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="No" dataDxfId="56">
+    <tableColumn id="1" name="No" dataDxfId="72">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Name" dataDxfId="55"/>
-    <tableColumn id="3" name="Description" dataDxfId="54"/>
-    <tableColumn id="4" name="Title" dataDxfId="53"/>
-    <tableColumn id="5" name="NS" dataDxfId="52">
+    <tableColumn id="2" name="Name" dataDxfId="71"/>
+    <tableColumn id="3" name="Description" dataDxfId="70"/>
+    <tableColumn id="4" name="Title" dataDxfId="69"/>
+    <tableColumn id="5" name="NS" dataDxfId="68">
       <calculatedColumnFormula>"Milestone\Appframe\Model"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Table" dataDxfId="51"/>
-    <tableColumn id="7" name="Key" dataDxfId="50">
+    <tableColumn id="6" name="Table" dataDxfId="67"/>
+    <tableColumn id="7" name="Key" dataDxfId="66">
       <calculatedColumnFormula>"id"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Controller" dataDxfId="49"/>
-    <tableColumn id="9" name="Controller NS" dataDxfId="48"/>
+    <tableColumn id="8" name="Controller" dataDxfId="65"/>
+    <tableColumn id="9" name="Controller NS" dataDxfId="64"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RelationTable" displayName="RelationTable" ref="A1:I50" totalsRowShown="0" dataDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RelationTable" displayName="RelationTable" ref="A1:I50" totalsRowShown="0" dataDxfId="63">
   <autoFilter ref="A1:I50"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="No" dataDxfId="46">
+    <tableColumn id="1" name="No" dataDxfId="62">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Resource" dataDxfId="45"/>
-    <tableColumn id="4" name="Relate Resource" dataDxfId="44"/>
-    <tableColumn id="2" name="Resource Id" dataDxfId="43">
+    <tableColumn id="3" name="Resource" dataDxfId="61"/>
+    <tableColumn id="4" name="Relate Resource" dataDxfId="60"/>
+    <tableColumn id="2" name="Resource Id" dataDxfId="59">
       <calculatedColumnFormula>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Name" dataDxfId="42"/>
-    <tableColumn id="6" name="Description" dataDxfId="41"/>
-    <tableColumn id="7" name="Method" dataDxfId="40"/>
-    <tableColumn id="8" name="Type" dataDxfId="39"/>
-    <tableColumn id="10" name="Relate Id" dataDxfId="38">
+    <tableColumn id="5" name="Name" dataDxfId="58"/>
+    <tableColumn id="6" name="Description" dataDxfId="57"/>
+    <tableColumn id="7" name="Method" dataDxfId="56"/>
+    <tableColumn id="8" name="Type" dataDxfId="55"/>
+    <tableColumn id="10" name="Relate Id" dataDxfId="54">
       <calculatedColumnFormula>VLOOKUP([Relate Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4625,47 +4733,47 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="ResourceForms" displayName="ResourceForms" ref="A1:G9" totalsRowShown="0" dataDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="ResourceForms" displayName="ResourceForms" ref="A1:G9" totalsRowShown="0" dataDxfId="53">
   <autoFilter ref="A1:G9"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="No" dataDxfId="36">
+    <tableColumn id="1" name="No" dataDxfId="52">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Resource ID" dataDxfId="35"/>
-    <tableColumn id="3" name="Resource Name" dataDxfId="34">
+    <tableColumn id="2" name="Resource ID" dataDxfId="51"/>
+    <tableColumn id="3" name="Resource Name" dataDxfId="50">
       <calculatedColumnFormula>VLOOKUP([Resource ID],ResourceTable[],2,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Form Name" dataDxfId="33"/>
-    <tableColumn id="6" name="Title" dataDxfId="32"/>
-    <tableColumn id="7" name="Action Text" dataDxfId="31"/>
-    <tableColumn id="8" name="Description" dataDxfId="30"/>
+    <tableColumn id="4" name="Form Name" dataDxfId="49"/>
+    <tableColumn id="6" name="Title" dataDxfId="48"/>
+    <tableColumn id="7" name="Action Text" dataDxfId="47"/>
+    <tableColumn id="8" name="Description" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="FormFields" displayName="FormFields" ref="A1:L33" totalsRowShown="0" dataDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="FormFields" displayName="FormFields" ref="A1:L33" totalsRowShown="0" dataDxfId="45">
   <autoFilter ref="A1:L33"/>
   <tableColumns count="12">
-    <tableColumn id="9" name="No" dataDxfId="28">
+    <tableColumn id="9" name="No" dataDxfId="44">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Form Id" dataDxfId="27"/>
-    <tableColumn id="7" name="Form Name" dataDxfId="26">
+    <tableColumn id="1" name="Form Id" dataDxfId="43"/>
+    <tableColumn id="7" name="Form Name" dataDxfId="42">
       <calculatedColumnFormula>VLOOKUP([Form Id],ResourceForms[],4,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Name" dataDxfId="25"/>
-    <tableColumn id="2" name="Type" dataDxfId="24"/>
-    <tableColumn id="5" name="Label" dataDxfId="23"/>
-    <tableColumn id="6" name="Collection" dataDxfId="22"/>
-    <tableColumn id="14" name="Attribute" dataDxfId="21">
+    <tableColumn id="4" name="Name" dataDxfId="41"/>
+    <tableColumn id="2" name="Type" dataDxfId="40"/>
+    <tableColumn id="5" name="Label" dataDxfId="39"/>
+    <tableColumn id="6" name="Collection" dataDxfId="38"/>
+    <tableColumn id="14" name="Attribute" dataDxfId="37">
       <calculatedColumnFormula>[Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Relation" dataDxfId="20"/>
-    <tableColumn id="11" name="Deep 1" dataDxfId="19"/>
-    <tableColumn id="12" name="Deep 2" dataDxfId="18"/>
-    <tableColumn id="13" name="Deep 3" dataDxfId="17"/>
+    <tableColumn id="10" name="Relation" dataDxfId="36"/>
+    <tableColumn id="11" name="Deep 1" dataDxfId="35"/>
+    <tableColumn id="12" name="Deep 2" dataDxfId="34"/>
+    <tableColumn id="13" name="Deep 3" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4956,10 +5064,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5019,7 +5127,7 @@
         <v>user</v>
       </c>
       <c r="D2" s="8" t="str">
-        <f t="shared" ref="D2:D42" si="0">"Milestone\Appframe\Model"</f>
+        <f t="shared" ref="D2:D43" si="0">"Milestone\Appframe\Model"</f>
         <v>Milestone\Appframe\Model</v>
       </c>
       <c r="E2" s="8" t="str">
@@ -6331,7 +6439,7 @@
         <v>resource_form_field_depend</v>
       </c>
       <c r="D34" s="7" t="str">
-        <f t="shared" ref="D34:D40" si="1">"Milestone\Appframe\Model"</f>
+        <f t="shared" ref="D34:D41" si="1">"Milestone\Appframe\Model"</f>
         <v>Milestone\Appframe\Model</v>
       </c>
       <c r="E34" s="8" t="str">
@@ -6361,56 +6469,56 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="2" t="s">
-        <v>589</v>
+        <v>778</v>
       </c>
       <c r="B35" s="7" t="str">
         <f>"__"&amp;[Name]</f>
-        <v>__resource_form_layout</v>
+        <v>__resource_form_field_dynamic</v>
       </c>
       <c r="C35" s="7" t="str">
         <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
-        <v>resource_form_layout</v>
+        <v>resource_form_field_dynamic</v>
       </c>
       <c r="D35" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f>"Milestone\Appframe\Model"</f>
         <v>Milestone\Appframe\Model</v>
       </c>
       <c r="E35" s="8" t="str">
         <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
-        <v>ResourceFormLayout</v>
+        <v>ResourceFormFieldDynamic</v>
       </c>
       <c r="F35" s="8" t="str">
         <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
-        <v>php artisan make:migration create___resource_form_layout_table --create=__resource_form_layout</v>
+        <v>php artisan make:migration create___resource_form_field_dynamic_table --create=__resource_form_field_dynamic</v>
       </c>
       <c r="G35" s="8" t="str">
         <f>"php artisan make:model "&amp;[Class Name]</f>
-        <v>php artisan make:model ResourceFormLayout</v>
+        <v>php artisan make:model ResourceFormFieldDynamic</v>
       </c>
       <c r="H35" s="8" t="str">
         <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
-        <v>protected $table = '__resource_form_layout';</v>
+        <v>protected $table = '__resource_form_field_dynamic';</v>
       </c>
       <c r="I35" s="8" t="str">
         <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
-        <v>php artisan make:seed ResourceFormLayoutTableSeeder</v>
+        <v>php artisan make:seed ResourceFormFieldDynamicTableSeeder</v>
       </c>
       <c r="J35" s="8" t="str">
         <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
-        <v>ResourceFormLayoutTableSeeder::class,</v>
+        <v>ResourceFormFieldDynamicTableSeeder::class,</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="2" t="s">
-        <v>646</v>
+        <v>589</v>
       </c>
       <c r="B36" s="7" t="str">
         <f>"__"&amp;[Name]</f>
-        <v>__resource_form_collection</v>
+        <v>__resource_form_layout</v>
       </c>
       <c r="C36" s="7" t="str">
         <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
-        <v>resource_form_collection</v>
+        <v>resource_form_layout</v>
       </c>
       <c r="D36" s="7" t="str">
         <f t="shared" si="1"/>
@@ -6418,40 +6526,40 @@
       </c>
       <c r="E36" s="8" t="str">
         <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
-        <v>ResourceFormCollection</v>
+        <v>ResourceFormLayout</v>
       </c>
       <c r="F36" s="8" t="str">
         <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
-        <v>php artisan make:migration create___resource_form_collection_table --create=__resource_form_collection</v>
+        <v>php artisan make:migration create___resource_form_layout_table --create=__resource_form_layout</v>
       </c>
       <c r="G36" s="8" t="str">
         <f>"php artisan make:model "&amp;[Class Name]</f>
-        <v>php artisan make:model ResourceFormCollection</v>
+        <v>php artisan make:model ResourceFormLayout</v>
       </c>
       <c r="H36" s="8" t="str">
         <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
-        <v>protected $table = '__resource_form_collection';</v>
+        <v>protected $table = '__resource_form_layout';</v>
       </c>
       <c r="I36" s="8" t="str">
         <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
-        <v>php artisan make:seed ResourceFormCollectionTableSeeder</v>
+        <v>php artisan make:seed ResourceFormLayoutTableSeeder</v>
       </c>
       <c r="J36" s="8" t="str">
         <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
-        <v>ResourceFormCollectionTableSeeder::class,</v>
+        <v>ResourceFormLayoutTableSeeder::class,</v>
       </c>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="4" t="s">
-        <v>723</v>
+      <c r="A37" s="2" t="s">
+        <v>646</v>
       </c>
       <c r="B37" s="7" t="str">
         <f>"__"&amp;[Name]</f>
-        <v>__resource_dashboard</v>
+        <v>__resource_form_collection</v>
       </c>
       <c r="C37" s="7" t="str">
         <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
-        <v>resource_dashboard</v>
+        <v>resource_form_collection</v>
       </c>
       <c r="D37" s="7" t="str">
         <f t="shared" si="1"/>
@@ -6459,40 +6567,40 @@
       </c>
       <c r="E37" s="8" t="str">
         <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
-        <v>ResourceDashboard</v>
+        <v>ResourceFormCollection</v>
       </c>
       <c r="F37" s="8" t="str">
         <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
-        <v>php artisan make:migration create___resource_dashboard_table --create=__resource_dashboard</v>
+        <v>php artisan make:migration create___resource_form_collection_table --create=__resource_form_collection</v>
       </c>
       <c r="G37" s="8" t="str">
         <f>"php artisan make:model "&amp;[Class Name]</f>
-        <v>php artisan make:model ResourceDashboard</v>
+        <v>php artisan make:model ResourceFormCollection</v>
       </c>
       <c r="H37" s="8" t="str">
         <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
-        <v>protected $table = '__resource_dashboard';</v>
+        <v>protected $table = '__resource_form_collection';</v>
       </c>
       <c r="I37" s="8" t="str">
         <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
-        <v>php artisan make:seed ResourceDashboardTableSeeder</v>
+        <v>php artisan make:seed ResourceFormCollectionTableSeeder</v>
       </c>
       <c r="J37" s="8" t="str">
         <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
-        <v>ResourceDashboardTableSeeder::class,</v>
+        <v>ResourceFormCollectionTableSeeder::class,</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="4" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B38" s="7" t="str">
         <f>"__"&amp;[Name]</f>
-        <v>__resource_dashboard_sections</v>
+        <v>__resource_dashboard</v>
       </c>
       <c r="C38" s="7" t="str">
         <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
-        <v>resource_dashboard_section</v>
+        <v>resource_dashboard</v>
       </c>
       <c r="D38" s="7" t="str">
         <f t="shared" si="1"/>
@@ -6500,40 +6608,40 @@
       </c>
       <c r="E38" s="8" t="str">
         <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
-        <v>ResourceDashboardSection</v>
+        <v>ResourceDashboard</v>
       </c>
       <c r="F38" s="8" t="str">
         <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
-        <v>php artisan make:migration create___resource_dashboard_sections_table --create=__resource_dashboard_sections</v>
+        <v>php artisan make:migration create___resource_dashboard_table --create=__resource_dashboard</v>
       </c>
       <c r="G38" s="8" t="str">
         <f>"php artisan make:model "&amp;[Class Name]</f>
-        <v>php artisan make:model ResourceDashboardSection</v>
+        <v>php artisan make:model ResourceDashboard</v>
       </c>
       <c r="H38" s="8" t="str">
         <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
-        <v>protected $table = '__resource_dashboard_sections';</v>
+        <v>protected $table = '__resource_dashboard';</v>
       </c>
       <c r="I38" s="8" t="str">
         <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
-        <v>php artisan make:seed ResourceDashboardSectionTableSeeder</v>
+        <v>php artisan make:seed ResourceDashboardTableSeeder</v>
       </c>
       <c r="J38" s="8" t="str">
         <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
-        <v>ResourceDashboardSectionTableSeeder::class,</v>
+        <v>ResourceDashboardTableSeeder::class,</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="4" t="s">
-        <v>730</v>
+        <v>724</v>
       </c>
       <c r="B39" s="7" t="str">
         <f>"__"&amp;[Name]</f>
-        <v>__resource_dashboard_section_items</v>
+        <v>__resource_dashboard_sections</v>
       </c>
       <c r="C39" s="7" t="str">
         <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
-        <v>resource_dashboard_section_item</v>
+        <v>resource_dashboard_section</v>
       </c>
       <c r="D39" s="7" t="str">
         <f t="shared" si="1"/>
@@ -6541,40 +6649,40 @@
       </c>
       <c r="E39" s="8" t="str">
         <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
-        <v>ResourceDashboardSectionItem</v>
+        <v>ResourceDashboardSection</v>
       </c>
       <c r="F39" s="8" t="str">
         <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
-        <v>php artisan make:migration create___resource_dashboard_section_items_table --create=__resource_dashboard_section_items</v>
+        <v>php artisan make:migration create___resource_dashboard_sections_table --create=__resource_dashboard_sections</v>
       </c>
       <c r="G39" s="8" t="str">
         <f>"php artisan make:model "&amp;[Class Name]</f>
-        <v>php artisan make:model ResourceDashboardSectionItem</v>
+        <v>php artisan make:model ResourceDashboardSection</v>
       </c>
       <c r="H39" s="8" t="str">
         <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
-        <v>protected $table = '__resource_dashboard_section_items';</v>
+        <v>protected $table = '__resource_dashboard_sections';</v>
       </c>
       <c r="I39" s="8" t="str">
         <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
-        <v>php artisan make:seed ResourceDashboardSectionItemTableSeeder</v>
+        <v>php artisan make:seed ResourceDashboardSectionTableSeeder</v>
       </c>
       <c r="J39" s="8" t="str">
         <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
-        <v>ResourceDashboardSectionItemTableSeeder::class,</v>
+        <v>ResourceDashboardSectionTableSeeder::class,</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="4" t="s">
-        <v>701</v>
+        <v>730</v>
       </c>
       <c r="B40" s="7" t="str">
         <f>"__"&amp;[Name]</f>
-        <v>__resource_metrics</v>
+        <v>__resource_dashboard_section_items</v>
       </c>
       <c r="C40" s="7" t="str">
         <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
-        <v>resource_metric</v>
+        <v>resource_dashboard_section_item</v>
       </c>
       <c r="D40" s="7" t="str">
         <f t="shared" si="1"/>
@@ -6582,81 +6690,81 @@
       </c>
       <c r="E40" s="8" t="str">
         <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
-        <v>ResourceMetric</v>
+        <v>ResourceDashboardSectionItem</v>
       </c>
       <c r="F40" s="8" t="str">
         <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
-        <v>php artisan make:migration create___resource_metrics_table --create=__resource_metrics</v>
+        <v>php artisan make:migration create___resource_dashboard_section_items_table --create=__resource_dashboard_section_items</v>
       </c>
       <c r="G40" s="8" t="str">
         <f>"php artisan make:model "&amp;[Class Name]</f>
-        <v>php artisan make:model ResourceMetric</v>
+        <v>php artisan make:model ResourceDashboardSectionItem</v>
       </c>
       <c r="H40" s="8" t="str">
         <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
-        <v>protected $table = '__resource_metrics';</v>
+        <v>protected $table = '__resource_dashboard_section_items';</v>
       </c>
       <c r="I40" s="8" t="str">
         <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
-        <v>php artisan make:seed ResourceMetricTableSeeder</v>
+        <v>php artisan make:seed ResourceDashboardSectionItemTableSeeder</v>
       </c>
       <c r="J40" s="8" t="str">
         <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
+        <v>ResourceDashboardSectionItemTableSeeder::class,</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="4" t="s">
+        <v>701</v>
+      </c>
+      <c r="B41" s="7" t="str">
+        <f>"__"&amp;[Name]</f>
+        <v>__resource_metrics</v>
+      </c>
+      <c r="C41" s="7" t="str">
+        <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
+        <v>resource_metric</v>
+      </c>
+      <c r="D41" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>Milestone\Appframe\Model</v>
+      </c>
+      <c r="E41" s="8" t="str">
+        <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
+        <v>ResourceMetric</v>
+      </c>
+      <c r="F41" s="8" t="str">
+        <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
+        <v>php artisan make:migration create___resource_metrics_table --create=__resource_metrics</v>
+      </c>
+      <c r="G41" s="8" t="str">
+        <f>"php artisan make:model "&amp;[Class Name]</f>
+        <v>php artisan make:model ResourceMetric</v>
+      </c>
+      <c r="H41" s="8" t="str">
+        <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
+        <v>protected $table = '__resource_metrics';</v>
+      </c>
+      <c r="I41" s="8" t="str">
+        <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
+        <v>php artisan make:seed ResourceMetricTableSeeder</v>
+      </c>
+      <c r="J41" s="8" t="str">
+        <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
         <v>ResourceMetricTableSeeder::class,</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
-      <c r="A41" s="2" t="s">
+    <row r="42" spans="1:10">
+      <c r="A42" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B41" s="9" t="str">
+      <c r="B42" s="9" t="str">
         <f>"__"&amp;[Name]</f>
         <v>__organisation</v>
       </c>
-      <c r="C41" s="9" t="str">
+      <c r="C42" s="9" t="str">
         <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
         <v>organisation</v>
-      </c>
-      <c r="D41" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>Milestone\Appframe\Model</v>
-      </c>
-      <c r="E41" s="9" t="str">
-        <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
-        <v>Organisation</v>
-      </c>
-      <c r="F41" s="9" t="str">
-        <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
-        <v>php artisan make:migration create___organisation_table --create=__organisation</v>
-      </c>
-      <c r="G41" s="9" t="str">
-        <f>"php artisan make:model "&amp;[Class Name]</f>
-        <v>php artisan make:model Organisation</v>
-      </c>
-      <c r="H41" s="9" t="str">
-        <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
-        <v>protected $table = '__organisation';</v>
-      </c>
-      <c r="I41" s="9" t="str">
-        <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
-        <v>php artisan make:seed OrganisationTableSeeder</v>
-      </c>
-      <c r="J41" s="9" t="str">
-        <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
-        <v>OrganisationTableSeeder::class,</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10">
-      <c r="A42" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="B42" s="9" t="str">
-        <f>"__"&amp;[Name]</f>
-        <v>__organisation_contacts</v>
-      </c>
-      <c r="C42" s="9" t="str">
-        <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
-        <v>organisation_contact</v>
       </c>
       <c r="D42" s="9" t="str">
         <f t="shared" si="0"/>
@@ -6664,25 +6772,66 @@
       </c>
       <c r="E42" s="9" t="str">
         <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
-        <v>OrganisationContact</v>
+        <v>Organisation</v>
       </c>
       <c r="F42" s="9" t="str">
         <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
-        <v>php artisan make:migration create___organisation_contacts_table --create=__organisation_contacts</v>
+        <v>php artisan make:migration create___organisation_table --create=__organisation</v>
       </c>
       <c r="G42" s="9" t="str">
         <f>"php artisan make:model "&amp;[Class Name]</f>
-        <v>php artisan make:model OrganisationContact</v>
+        <v>php artisan make:model Organisation</v>
       </c>
       <c r="H42" s="9" t="str">
         <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
-        <v>protected $table = '__organisation_contacts';</v>
+        <v>protected $table = '__organisation';</v>
       </c>
       <c r="I42" s="9" t="str">
         <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
+        <v>php artisan make:seed OrganisationTableSeeder</v>
+      </c>
+      <c r="J42" s="9" t="str">
+        <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
+        <v>OrganisationTableSeeder::class,</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B43" s="9" t="str">
+        <f>"__"&amp;[Name]</f>
+        <v>__organisation_contacts</v>
+      </c>
+      <c r="C43" s="9" t="str">
+        <f>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</f>
+        <v>organisation_contact</v>
+      </c>
+      <c r="D43" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>Milestone\Appframe\Model</v>
+      </c>
+      <c r="E43" s="9" t="str">
+        <f>SUBSTITUTE(PROPER([Singular Name]),"_","")</f>
+        <v>OrganisationContact</v>
+      </c>
+      <c r="F43" s="9" t="str">
+        <f>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</f>
+        <v>php artisan make:migration create___organisation_contacts_table --create=__organisation_contacts</v>
+      </c>
+      <c r="G43" s="9" t="str">
+        <f>"php artisan make:model "&amp;[Class Name]</f>
+        <v>php artisan make:model OrganisationContact</v>
+      </c>
+      <c r="H43" s="9" t="str">
+        <f>"protected $table = '"&amp;[Table]&amp;"';"</f>
+        <v>protected $table = '__organisation_contacts';</v>
+      </c>
+      <c r="I43" s="9" t="str">
+        <f>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</f>
         <v>php artisan make:seed OrganisationContactTableSeeder</v>
       </c>
-      <c r="J42" s="9" t="str">
+      <c r="J43" s="9" t="str">
         <f>[Class Name]&amp;"TableSeeder"&amp;"::class,"</f>
         <v>OrganisationContactTableSeeder::class,</v>
       </c>
@@ -8268,10 +8417,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I161"/>
+  <dimension ref="A1:I166"/>
   <sheetViews>
-    <sheetView topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="C143" sqref="C143"/>
+    <sheetView topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="A166" sqref="A166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="15"/>
@@ -11755,27 +11904,132 @@
       <c r="H161" s="4"/>
       <c r="I161" s="4"/>
     </row>
+    <row r="162" spans="1:9">
+      <c r="A162" s="4" t="s">
+        <v>779</v>
+      </c>
+      <c r="B162" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C162" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D162" s="4" t="s">
+        <v>781</v>
+      </c>
+      <c r="E162" s="4" t="s">
+        <v>780</v>
+      </c>
+      <c r="F162" s="4"/>
+      <c r="G162" s="4"/>
+      <c r="H162" s="4"/>
+      <c r="I162" s="4"/>
+    </row>
+    <row r="163" spans="1:9">
+      <c r="A163" s="4" t="s">
+        <v>782</v>
+      </c>
+      <c r="B163" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C163" s="4" t="s">
+        <v>783</v>
+      </c>
+      <c r="D163" s="4" t="s">
+        <v>784</v>
+      </c>
+      <c r="E163" s="4" t="s">
+        <v>785</v>
+      </c>
+      <c r="F163" s="4"/>
+      <c r="G163" s="4"/>
+      <c r="H163" s="4"/>
+      <c r="I163" s="4"/>
+    </row>
+    <row r="164" spans="1:9">
+      <c r="A164" s="4" t="s">
+        <v>786</v>
+      </c>
+      <c r="B164" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C164" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D164" s="4">
+        <v>128</v>
+      </c>
+      <c r="E164" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F164" s="4"/>
+      <c r="G164" s="4"/>
+      <c r="H164" s="4"/>
+      <c r="I164" s="4"/>
+    </row>
+    <row r="165" spans="1:9">
+      <c r="A165" s="4" t="s">
+        <v>787</v>
+      </c>
+      <c r="B165" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C165" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="D165" s="4">
+        <v>512</v>
+      </c>
+      <c r="E165" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F165" s="4"/>
+      <c r="G165" s="4"/>
+      <c r="H165" s="4"/>
+      <c r="I165" s="4"/>
+    </row>
+    <row r="166" spans="1:9">
+      <c r="A166" s="4" t="s">
+        <v>789</v>
+      </c>
+      <c r="B166" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C166" s="4" t="s">
+        <v>790</v>
+      </c>
+      <c r="D166" s="4" t="s">
+        <v>791</v>
+      </c>
+      <c r="E166" s="4" t="s">
+        <v>792</v>
+      </c>
+      <c r="F166" s="4"/>
+      <c r="G166" s="4"/>
+      <c r="H166" s="4"/>
+      <c r="I166" s="4"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A43:A46">
-    <cfRule type="duplicateValues" dxfId="112" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="117" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56:A59">
-    <cfRule type="duplicateValues" dxfId="111" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="116" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A161">
-    <cfRule type="duplicateValues" dxfId="110" priority="25"/>
+  <conditionalFormatting sqref="A2:A166">
+    <cfRule type="duplicateValues" dxfId="11" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A128:A129">
-    <cfRule type="duplicateValues" dxfId="109" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="115" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A128:A129">
-    <cfRule type="duplicateValues" dxfId="108" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="114" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A130:A131">
-    <cfRule type="duplicateValues" dxfId="107" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="113" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A152:A153">
-    <cfRule type="duplicateValues" dxfId="106" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="112" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -11787,10 +12041,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K373"/>
+  <dimension ref="A1:K384"/>
   <sheetViews>
-    <sheetView topLeftCell="A327" workbookViewId="0">
-      <selection activeCell="B340" sqref="B340"/>
+    <sheetView topLeftCell="A366" workbookViewId="0">
+      <selection activeCell="K375" sqref="K375"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="15"/>
@@ -28204,13 +28458,497 @@
         <v>$table-&gt;foreign('section')-&gt;references('id')-&gt;on('__resource_dashboard_sections')-&gt;onUpdate('cascade')-&gt;onDelete('cascade');</v>
       </c>
     </row>
+    <row r="374" spans="1:11">
+      <c r="A374" s="4" t="s">
+        <v>778</v>
+      </c>
+      <c r="B374" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C374" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>increments(</v>
+      </c>
+      <c r="D374" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'id'</v>
+      </c>
+      <c r="E374" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>)</v>
+      </c>
+      <c r="F374" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v/>
+      </c>
+      <c r="G374" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v/>
+      </c>
+      <c r="H374" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v/>
+      </c>
+      <c r="I374" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v/>
+      </c>
+      <c r="J374" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K374" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;increments('id');</v>
+      </c>
+    </row>
+    <row r="375" spans="1:11">
+      <c r="A375" s="4" t="s">
+        <v>778</v>
+      </c>
+      <c r="B375" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C375" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>unsignedInteger(</v>
+      </c>
+      <c r="D375" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'form_field'</v>
+      </c>
+      <c r="E375" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>)</v>
+      </c>
+      <c r="F375" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>-&gt;index()</v>
+      </c>
+      <c r="G375" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v/>
+      </c>
+      <c r="H375" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v/>
+      </c>
+      <c r="I375" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v/>
+      </c>
+      <c r="J375" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K375" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;unsignedInteger('form_field')-&gt;index();</v>
+      </c>
+    </row>
+    <row r="376" spans="1:11">
+      <c r="A376" s="4" t="s">
+        <v>778</v>
+      </c>
+      <c r="B376" s="4" t="s">
+        <v>779</v>
+      </c>
+      <c r="C376" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>enum(</v>
+      </c>
+      <c r="D376" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'type'</v>
+      </c>
+      <c r="E376" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>, ['disabled-enabled','enabled-disabled','hidden-visible','visible-hidden','readonly-editable','editable-readonly'])</v>
+      </c>
+      <c r="F376" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>-&gt;default('disabled-enabled')</v>
+      </c>
+      <c r="G376" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v/>
+      </c>
+      <c r="H376" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v/>
+      </c>
+      <c r="I376" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v/>
+      </c>
+      <c r="J376" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K376" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;enum('type', ['disabled-enabled','enabled-disabled','hidden-visible','visible-hidden','readonly-editable','editable-readonly'])-&gt;default('disabled-enabled');</v>
+      </c>
+    </row>
+    <row r="377" spans="1:11">
+      <c r="A377" s="4" t="s">
+        <v>778</v>
+      </c>
+      <c r="B377" s="4" t="s">
+        <v>679</v>
+      </c>
+      <c r="C377" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>string(</v>
+      </c>
+      <c r="D377" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'depend_field'</v>
+      </c>
+      <c r="E377" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>, 64)</v>
+      </c>
+      <c r="F377" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>-&gt;index()</v>
+      </c>
+      <c r="G377" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v>-&gt;nullable()</v>
+      </c>
+      <c r="H377" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v/>
+      </c>
+      <c r="I377" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v/>
+      </c>
+      <c r="J377" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K377" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;string('depend_field', 64)-&gt;index()-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="378" spans="1:11">
+      <c r="A378" s="4" t="s">
+        <v>778</v>
+      </c>
+      <c r="B378" s="4" t="s">
+        <v>782</v>
+      </c>
+      <c r="C378" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>enum(</v>
+      </c>
+      <c r="D378" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'alter_on'</v>
+      </c>
+      <c r="E378" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>, ['not null','value','null'])</v>
+      </c>
+      <c r="F378" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>-&gt;default('not null')</v>
+      </c>
+      <c r="G378" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v/>
+      </c>
+      <c r="H378" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v/>
+      </c>
+      <c r="I378" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v/>
+      </c>
+      <c r="J378" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K378" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;enum('alter_on', ['not null','value','null'])-&gt;default('not null');</v>
+      </c>
+    </row>
+    <row r="379" spans="1:11">
+      <c r="A379" s="4" t="s">
+        <v>778</v>
+      </c>
+      <c r="B379" s="4" t="s">
+        <v>786</v>
+      </c>
+      <c r="C379" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>string(</v>
+      </c>
+      <c r="D379" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'value'</v>
+      </c>
+      <c r="E379" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>, 128)</v>
+      </c>
+      <c r="F379" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>-&gt;nullable()</v>
+      </c>
+      <c r="G379" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v/>
+      </c>
+      <c r="H379" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v/>
+      </c>
+      <c r="I379" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v/>
+      </c>
+      <c r="J379" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K379" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;string('value', 128)-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="380" spans="1:11">
+      <c r="A380" s="4" t="s">
+        <v>778</v>
+      </c>
+      <c r="B380" s="5" t="s">
+        <v>787</v>
+      </c>
+      <c r="C380" s="5" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>string(</v>
+      </c>
+      <c r="D380" s="5" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'value_array'</v>
+      </c>
+      <c r="E380" s="8" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>, 512)</v>
+      </c>
+      <c r="F380" s="5" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>-&gt;nullable()</v>
+      </c>
+      <c r="G380" s="5" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v/>
+      </c>
+      <c r="H380" s="5" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v/>
+      </c>
+      <c r="I380" s="5" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v/>
+      </c>
+      <c r="J380" s="5" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K380" s="5" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;string('value_array', 512)-&gt;nullable();</v>
+      </c>
+    </row>
+    <row r="381" spans="1:11">
+      <c r="A381" s="4" t="s">
+        <v>778</v>
+      </c>
+      <c r="B381" s="4" t="s">
+        <v>683</v>
+      </c>
+      <c r="C381" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>enum(</v>
+      </c>
+      <c r="D381" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'operator'</v>
+      </c>
+      <c r="E381" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>, ['=','&lt;','&gt;','&lt;=','&gt;=','&lt;&gt;','In','NotIn','like'])</v>
+      </c>
+      <c r="F381" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>-&gt;default('=')</v>
+      </c>
+      <c r="G381" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v/>
+      </c>
+      <c r="H381" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v/>
+      </c>
+      <c r="I381" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v/>
+      </c>
+      <c r="J381" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K381" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;enum('operator', ['=','&lt;','&gt;','&lt;=','&gt;=','&lt;&gt;','In','NotIn','like'])-&gt;default('=');</v>
+      </c>
+    </row>
+    <row r="382" spans="1:11">
+      <c r="A382" s="4" t="s">
+        <v>778</v>
+      </c>
+      <c r="B382" s="4" t="s">
+        <v>789</v>
+      </c>
+      <c r="C382" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>enum(</v>
+      </c>
+      <c r="D382" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'on_multiple'</v>
+      </c>
+      <c r="E382" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>, ['and','or'])</v>
+      </c>
+      <c r="F382" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>-&gt;default('and')</v>
+      </c>
+      <c r="G382" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v/>
+      </c>
+      <c r="H382" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v/>
+      </c>
+      <c r="I382" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v/>
+      </c>
+      <c r="J382" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K382" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;enum('on_multiple', ['and','or'])-&gt;default('and');</v>
+      </c>
+    </row>
+    <row r="383" spans="1:11">
+      <c r="A383" s="4" t="s">
+        <v>778</v>
+      </c>
+      <c r="B383" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C383" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>timestamps(</v>
+      </c>
+      <c r="D383" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v/>
+      </c>
+      <c r="E383" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>)</v>
+      </c>
+      <c r="F383" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v/>
+      </c>
+      <c r="G383" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v/>
+      </c>
+      <c r="H383" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v/>
+      </c>
+      <c r="I383" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v/>
+      </c>
+      <c r="J383" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K383" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;timestamps();</v>
+      </c>
+    </row>
+    <row r="384" spans="1:11">
+      <c r="A384" s="4" t="s">
+        <v>778</v>
+      </c>
+      <c r="B384" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C384" s="4" t="str">
+        <f>VLOOKUP([Field],Columns[],2,0)&amp;"("</f>
+        <v>foreign(</v>
+      </c>
+      <c r="D384" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
+        <v>'form_field'</v>
+      </c>
+      <c r="E384" s="7" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
+        <v>)</v>
+      </c>
+      <c r="F384" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
+        <v>-&gt;references('id')</v>
+      </c>
+      <c r="G384" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</f>
+        <v>-&gt;on('__resource_form_fields')</v>
+      </c>
+      <c r="H384" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</f>
+        <v>-&gt;onUpdate('cascade')</v>
+      </c>
+      <c r="I384" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</f>
+        <v>-&gt;onDelete('cascade')</v>
+      </c>
+      <c r="J384" s="4" t="str">
+        <f>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</f>
+        <v/>
+      </c>
+      <c r="K384" s="4" t="str">
+        <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
+        <v>$table-&gt;foreign('form_field')-&gt;references('id')-&gt;on('__resource_form_fields')-&gt;onUpdate('cascade')-&gt;onDelete('cascade');</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B373">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B384">
       <formula1>AvailableFields</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A373">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A384">
       <formula1>TableNames</formula1>
     </dataValidation>
   </dataValidations>
@@ -28224,10 +28962,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R322"/>
+  <dimension ref="A1:R323"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B301" workbookViewId="0">
-      <selection activeCell="G314" sqref="G314"/>
+    <sheetView topLeftCell="G301" workbookViewId="0">
+      <selection activeCell="J324" sqref="J324"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -40012,6 +40750,50 @@
       <c r="Q322" s="40"/>
       <c r="R322" s="40"/>
     </row>
+    <row r="323" spans="1:18">
+      <c r="A323" s="22" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Field Dynamic-0</v>
+      </c>
+      <c r="B323" s="40" t="s">
+        <v>793</v>
+      </c>
+      <c r="C323" s="22">
+        <f>COUNTIF($B$1:$B322,[Table Name])</f>
+        <v>0</v>
+      </c>
+      <c r="D323" s="40" t="s">
+        <v>122</v>
+      </c>
+      <c r="E323" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="F323" s="40" t="s">
+        <v>680</v>
+      </c>
+      <c r="G323" s="40" t="s">
+        <v>783</v>
+      </c>
+      <c r="H323" s="40" t="s">
+        <v>96</v>
+      </c>
+      <c r="I323" s="40" t="s">
+        <v>788</v>
+      </c>
+      <c r="J323" s="40" t="s">
+        <v>684</v>
+      </c>
+      <c r="K323" s="40" t="s">
+        <v>790</v>
+      </c>
+      <c r="L323" s="40"/>
+      <c r="M323" s="40"/>
+      <c r="N323" s="40"/>
+      <c r="O323" s="40"/>
+      <c r="P323" s="40"/>
+      <c r="Q323" s="40"/>
+      <c r="R323" s="40"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
@@ -40023,10 +40805,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -40757,12 +41539,32 @@
         <v>truncate</v>
       </c>
     </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="4" t="s">
+        <v>793</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>778</v>
+      </c>
+      <c r="C37" s="4" t="str">
+        <f>VLOOKUP([FW Table Name],Tables[],4,0)</f>
+        <v>Milestone\Appframe\Model</v>
+      </c>
+      <c r="D37" s="4" t="str">
+        <f>VLOOKUP([FW Table Name],Tables[],5,0)</f>
+        <v>ResourceFormFieldDynamic</v>
+      </c>
+      <c r="E37" s="7" t="str">
+        <f>"truncate"</f>
+        <v>truncate</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E36">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E37">
       <formula1>"truncate,query"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B36">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B37">
       <formula1>TableNames</formula1>
     </dataValidation>
   </dataValidations>
@@ -40778,8 +41580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34:G37"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Model created For dynamic field, and seeders added
</commit_message>
<xml_diff>
--- a/Helper.xlsx
+++ b/Helper.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Tables" sheetId="1" r:id="rId1"/>
@@ -5066,8 +5066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -41580,7 +41580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -44285,7 +44285,7 @@
   <dimension ref="A1:T109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D3"/>
+      <selection activeCell="B6" sqref="B6:R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -44295,14 +44295,14 @@
   <sheetData>
     <row r="1" spans="1:20" s="38" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="50" t="s">
-        <v>745</v>
+        <v>793</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="50"/>
       <c r="D1" s="50"/>
       <c r="E1" s="51" t="str">
         <f>"\"&amp;VLOOKUP($A$1,SeedMap[],3,0)&amp;"\"&amp;VLOOKUP($A$1,SeedMap[],4,0)&amp;"::"&amp;VLOOKUP($A$1,SeedMap[],5,0)&amp;"()"</f>
-        <v>\Milestone\Appframe\Model\ResourceMetric::truncate()</v>
+        <v>\Milestone\Appframe\Model\ResourceFormFieldDynamic::truncate()</v>
       </c>
       <c r="F1" s="51"/>
       <c r="G1" s="51"/>
@@ -44446,47 +44446,47 @@
       <c r="B5" s="28"/>
       <c r="C5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],C$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],C$4+$B$4,0))</f>
-        <v>resource</v>
+        <v>form_field</v>
       </c>
       <c r="D5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],D$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],D$4+$B$4,0))</f>
-        <v>name</v>
+        <v>type</v>
       </c>
       <c r="E5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0))</f>
-        <v>type</v>
+        <v>depend_field</v>
       </c>
       <c r="F5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0))</f>
-        <v>resource_list</v>
+        <v>alter_on</v>
       </c>
       <c r="G5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0))</f>
-        <v>aggregate</v>
+        <v>value</v>
       </c>
       <c r="H5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],H$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],H$4+$B$4,0))</f>
-        <v>aggregate_field</v>
+        <v>value_array</v>
       </c>
       <c r="I5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],I$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],I$4+$B$4,0))</f>
-        <v>aggregate_distinct</v>
+        <v>operator</v>
       </c>
       <c r="J5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],J$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],J$4+$B$4,0))</f>
-        <v>field</v>
+        <v>on_multiple</v>
       </c>
       <c r="K5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],K$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],K$4+$B$4,0))</f>
-        <v>field_sub</v>
+        <v/>
       </c>
       <c r="L5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],L$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],L$4+$B$4,0))</f>
-        <v>cache</v>
+        <v/>
       </c>
       <c r="M5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],M$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],M$4+$B$4,0))</f>
-        <v>method</v>
+        <v/>
       </c>
       <c r="N5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],N$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],N$4+$B$4,0))</f>
@@ -44560,7 +44560,7 @@
       <c r="A8" s="32"/>
       <c r="B8" s="49" t="str">
         <f>$E$1</f>
-        <v>\Milestone\Appframe\Model\ResourceMetric::truncate()</v>
+        <v>\Milestone\Appframe\Model\ResourceFormFieldDynamic::truncate()</v>
       </c>
       <c r="C8" s="49"/>
       <c r="D8" s="49"/>

</xml_diff>

<commit_message>
Dynamic field, resource and relations added
</commit_message>
<xml_diff>
--- a/Helper.xlsx
+++ b/Helper.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Tables" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3779" uniqueCount="794">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3801" uniqueCount="800">
   <si>
     <t>resource_scopes</t>
   </si>
@@ -2420,6 +2420,24 @@
   </si>
   <si>
     <t>Field Dynamic</t>
+  </si>
+  <si>
+    <t>ResourceFormFieldDynamic</t>
+  </si>
+  <si>
+    <t>Dynamic field details</t>
+  </si>
+  <si>
+    <t>Dynamic Field</t>
+  </si>
+  <si>
+    <t>__resource_form_field_dynamic</t>
+  </si>
+  <si>
+    <t>Dynamics</t>
+  </si>
+  <si>
+    <t>Field Dynamics</t>
   </si>
 </sst>
 </file>
@@ -4632,8 +4650,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R323" totalsRowShown="0" headerRowDxfId="99" dataDxfId="98">
-  <autoFilter ref="A1:R323">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R325" totalsRowShown="0" headerRowDxfId="99" dataDxfId="98">
+  <autoFilter ref="A1:R325">
     <filterColumn colId="1"/>
   </autoFilter>
   <tableColumns count="18">
@@ -4685,8 +4703,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="ResourceTable" displayName="ResourceTable" ref="A1:I37" totalsRowShown="0" dataDxfId="73">
-  <autoFilter ref="A1:I37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="ResourceTable" displayName="ResourceTable" ref="A1:I38" totalsRowShown="0" dataDxfId="73">
+  <autoFilter ref="A1:I38"/>
   <tableColumns count="9">
     <tableColumn id="1" name="No" dataDxfId="72">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
@@ -4709,8 +4727,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RelationTable" displayName="RelationTable" ref="A1:I50" totalsRowShown="0" dataDxfId="63">
-  <autoFilter ref="A1:I50"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RelationTable" displayName="RelationTable" ref="A1:I51" totalsRowShown="0" dataDxfId="63">
+  <autoFilter ref="A1:I51"/>
   <tableColumns count="9">
     <tableColumn id="1" name="No" dataDxfId="62">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
@@ -5066,8 +5084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView topLeftCell="D28" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -28962,10 +28980,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R323"/>
+  <dimension ref="A1:R325"/>
   <sheetViews>
-    <sheetView topLeftCell="G301" workbookViewId="0">
-      <selection activeCell="J324" sqref="J324"/>
+    <sheetView topLeftCell="B316" workbookViewId="0">
+      <selection activeCell="D325" sqref="D325:I325"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -40793,6 +40811,86 @@
       <c r="P323" s="40"/>
       <c r="Q323" s="40"/>
       <c r="R323" s="40"/>
+    </row>
+    <row r="324" spans="1:18">
+      <c r="A324" s="22" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resources-37</v>
+      </c>
+      <c r="B324" s="40" t="s">
+        <v>220</v>
+      </c>
+      <c r="C324" s="22">
+        <f>COUNTIF($B$1:$B323,[Table Name])</f>
+        <v>37</v>
+      </c>
+      <c r="D324" s="40" t="s">
+        <v>794</v>
+      </c>
+      <c r="E324" s="40" t="s">
+        <v>795</v>
+      </c>
+      <c r="F324" s="40" t="s">
+        <v>796</v>
+      </c>
+      <c r="G324" s="40" t="s">
+        <v>558</v>
+      </c>
+      <c r="H324" s="40" t="s">
+        <v>797</v>
+      </c>
+      <c r="I324" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="J324" s="40"/>
+      <c r="K324" s="40"/>
+      <c r="L324" s="40"/>
+      <c r="M324" s="40"/>
+      <c r="N324" s="40"/>
+      <c r="O324" s="40"/>
+      <c r="P324" s="40"/>
+      <c r="Q324" s="40"/>
+      <c r="R324" s="40"/>
+    </row>
+    <row r="325" spans="1:18">
+      <c r="A325" s="22" t="str">
+        <f>[Table Name]&amp;"-"&amp;[Record No]</f>
+        <v>Resource Relations-50</v>
+      </c>
+      <c r="B325" s="40" t="s">
+        <v>441</v>
+      </c>
+      <c r="C325" s="22">
+        <f>COUNTIF($B$1:$B324,[Table Name])</f>
+        <v>50</v>
+      </c>
+      <c r="D325" s="40">
+        <v>13</v>
+      </c>
+      <c r="E325" s="40" t="s">
+        <v>799</v>
+      </c>
+      <c r="F325" s="40" t="s">
+        <v>795</v>
+      </c>
+      <c r="G325" s="40" t="s">
+        <v>798</v>
+      </c>
+      <c r="H325" s="40" t="s">
+        <v>401</v>
+      </c>
+      <c r="I325" s="40">
+        <v>37</v>
+      </c>
+      <c r="J325" s="40"/>
+      <c r="K325" s="40"/>
+      <c r="L325" s="40"/>
+      <c r="M325" s="40"/>
+      <c r="N325" s="40"/>
+      <c r="O325" s="40"/>
+      <c r="P325" s="40"/>
+      <c r="Q325" s="40"/>
+      <c r="R325" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -41578,10 +41676,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="B38" sqref="B38:G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -42632,9 +42730,37 @@
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
     </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="20">
+        <f>IFERROR($A37+1,1)</f>
+        <v>37</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>794</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>795</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>796</v>
+      </c>
+      <c r="E38" s="7" t="str">
+        <f>"Milestone\Appframe\Model"</f>
+        <v>Milestone\Appframe\Model</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>797</v>
+      </c>
+      <c r="G38" s="21" t="str">
+        <f>"id"</f>
+        <v>id</v>
+      </c>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F37">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F38">
       <formula1>ActualTableNames</formula1>
     </dataValidation>
   </dataValidations>
@@ -42647,10 +42773,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47:I50"/>
+      <selection activeCell="D51" sqref="D51:I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -44266,9 +44392,41 @@
         <v>4</v>
       </c>
     </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="20">
+        <f>IFERROR($A50+1,1)</f>
+        <v>50</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>794</v>
+      </c>
+      <c r="D51" s="7">
+        <f>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</f>
+        <v>13</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>799</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>795</v>
+      </c>
+      <c r="G51" s="22" t="s">
+        <v>798</v>
+      </c>
+      <c r="H51" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="I51" s="41">
+        <f>VLOOKUP([Relate Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</f>
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C50">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C51">
       <formula1>Resources</formula1>
     </dataValidation>
   </dataValidations>
@@ -44284,8 +44442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T109"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:R10"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -44295,14 +44453,14 @@
   <sheetData>
     <row r="1" spans="1:20" s="38" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="50" t="s">
-        <v>793</v>
+        <v>441</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="50"/>
       <c r="D1" s="50"/>
       <c r="E1" s="51" t="str">
         <f>"\"&amp;VLOOKUP($A$1,SeedMap[],3,0)&amp;"\"&amp;VLOOKUP($A$1,SeedMap[],4,0)&amp;"::"&amp;VLOOKUP($A$1,SeedMap[],5,0)&amp;"()"</f>
-        <v>\Milestone\Appframe\Model\ResourceFormFieldDynamic::truncate()</v>
+        <v>\Milestone\Appframe\Model\ResourceRelation::truncate()</v>
       </c>
       <c r="F1" s="51"/>
       <c r="G1" s="51"/>
@@ -44446,35 +44604,35 @@
       <c r="B5" s="28"/>
       <c r="C5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],C$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],C$4+$B$4,0))</f>
-        <v>form_field</v>
+        <v>resource</v>
       </c>
       <c r="D5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],D$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],D$4+$B$4,0))</f>
-        <v>type</v>
+        <v>name</v>
       </c>
       <c r="E5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],E$4+$B$4,0))</f>
-        <v>depend_field</v>
+        <v>description</v>
       </c>
       <c r="F5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],F$4+$B$4,0))</f>
-        <v>alter_on</v>
+        <v>method</v>
       </c>
       <c r="G5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],G$4+$B$4,0))</f>
-        <v>value</v>
+        <v>type</v>
       </c>
       <c r="H5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],H$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],H$4+$B$4,0))</f>
-        <v>value_array</v>
+        <v>relate_resource</v>
       </c>
       <c r="I5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],I$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],I$4+$B$4,0))</f>
-        <v>operator</v>
+        <v/>
       </c>
       <c r="J5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],J$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],J$4+$B$4,0))</f>
-        <v>on_multiple</v>
+        <v/>
       </c>
       <c r="K5" s="34" t="str">
         <f>IF(VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],K$4+$B$4,0)=0,"",VLOOKUP($A$1&amp;"-0",TableData[[TRCode]:[15]],K$4+$B$4,0))</f>
@@ -44560,7 +44718,7 @@
       <c r="A8" s="32"/>
       <c r="B8" s="49" t="str">
         <f>$E$1</f>
-        <v>\Milestone\Appframe\Model\ResourceFormFieldDynamic::truncate()</v>
+        <v>\Milestone\Appframe\Model\ResourceRelation::truncate()</v>
       </c>
       <c r="C8" s="49"/>
       <c r="D8" s="49"/>
@@ -44585,31 +44743,31 @@
       </c>
       <c r="B9" s="30" t="str">
         <f ca="1">IF($B8="","",IF($B8=";",$I$3,IF($B8=$I$3,"",IF(ISNA(VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),1,0)),";",$S$4))))</f>
-        <v>;</v>
+        <v>-&gt;create([</v>
       </c>
       <c r="C9" s="33" t="str">
         <f ca="1">IF(AND($B9=$S$4,C$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),C$4+$B$4,0)="","","'"&amp;C$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),C$4+$B$4,0)&amp;"', "),"")</f>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '1', </v>
       </c>
       <c r="D9" s="33" t="str">
         <f t="shared" ref="D9:Q24" ca="1" si="0">IF(AND($B9=$S$4,D$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),D$4+$B$4,0)="","","'"&amp;D$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A9,INDIRECT($E$2),D$4+$B$4,0)&amp;"', "),"")</f>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'User Groups', </v>
       </c>
       <c r="E9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Which groups this user belongs to', </v>
       </c>
       <c r="F9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Groups', </v>
       </c>
       <c r="G9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
       </c>
       <c r="H9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '2', </v>
       </c>
       <c r="I9" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44649,7 +44807,7 @@
       </c>
       <c r="R9" s="33" t="str">
         <f ca="1">IF(B9=$S$4,$T$4,"")</f>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="10" spans="1:20">
@@ -44658,31 +44816,31 @@
       </c>
       <c r="B10" s="30" t="str">
         <f t="shared" ref="B10:B73" ca="1" si="1">IF($B9="","",IF($B9=";",$I$3,IF($B9=$I$3,"",IF(ISNA(VLOOKUP($A$1&amp;"-"&amp;$A10,INDIRECT($E$2),1,0)),";",$S$4))))</f>
-        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
+        <v>-&gt;create([</v>
       </c>
       <c r="C10" s="33" t="str">
         <f ca="1">IF(AND($B10=$S$4,C$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A10,INDIRECT($E$2),C$4+$B$4,0)="","","'"&amp;C$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A10,INDIRECT($E$2),C$4+$B$4,0)&amp;"', "),"")</f>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '2', </v>
       </c>
       <c r="D10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Group Users', </v>
       </c>
       <c r="E10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'List of users belongs to this group', </v>
       </c>
       <c r="F10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Users', </v>
       </c>
       <c r="G10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
       </c>
       <c r="H10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '1', </v>
       </c>
       <c r="I10" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44722,7 +44880,7 @@
       </c>
       <c r="R10" s="33" t="str">
         <f t="shared" ref="R10:R73" ca="1" si="2">IF(B10=$S$4,$T$4,"")</f>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -44731,31 +44889,31 @@
       </c>
       <c r="B11" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C11" s="33" t="str">
         <f t="shared" ref="C11:G74" ca="1" si="3">IF(AND($B11=$S$4,C$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A11,INDIRECT($E$2),C$4+$B$4,0)="","","'"&amp;C$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A11,INDIRECT($E$2),C$4+$B$4,0)&amp;"', "),"")</f>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '2', </v>
       </c>
       <c r="D11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Group Roles', </v>
       </c>
       <c r="E11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Roles assigneed to this group', </v>
       </c>
       <c r="F11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Roles', </v>
       </c>
       <c r="G11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
       </c>
       <c r="H11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '3', </v>
       </c>
       <c r="I11" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44795,7 +44953,7 @@
       </c>
       <c r="R11" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -44804,31 +44962,31 @@
       </c>
       <c r="B12" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C12" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '3', </v>
       </c>
       <c r="D12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Role Groups', </v>
       </c>
       <c r="E12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Details of groups this role assigned to', </v>
       </c>
       <c r="F12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Groups', </v>
       </c>
       <c r="G12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
       </c>
       <c r="H12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '2', </v>
       </c>
       <c r="I12" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44868,7 +45026,7 @@
       </c>
       <c r="R12" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -44877,31 +45035,31 @@
       </c>
       <c r="B13" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C13" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '3', </v>
       </c>
       <c r="D13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Role Resource', </v>
       </c>
       <c r="E13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Resources assigned to a role', </v>
       </c>
       <c r="F13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Resources', </v>
       </c>
       <c r="G13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '11', </v>
       </c>
       <c r="I13" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -44941,7 +45099,7 @@
       </c>
       <c r="R13" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -44950,31 +45108,31 @@
       </c>
       <c r="B14" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C14" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '4', </v>
       </c>
       <c r="D14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Resource Roles', </v>
       </c>
       <c r="E14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'The details of roles who have access to this resource', </v>
       </c>
       <c r="F14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Roles', </v>
       </c>
       <c r="G14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
       </c>
       <c r="H14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '3', </v>
       </c>
       <c r="I14" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -45014,7 +45172,7 @@
       </c>
       <c r="R14" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -45023,31 +45181,31 @@
       </c>
       <c r="B15" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C15" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '4', </v>
       </c>
       <c r="D15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Resource Actions', </v>
       </c>
       <c r="E15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Get actions available for the resource', </v>
       </c>
       <c r="F15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Actions', </v>
       </c>
       <c r="G15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '7', </v>
       </c>
       <c r="I15" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -45087,7 +45245,7 @@
       </c>
       <c r="R15" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="16" spans="1:20">
@@ -45096,31 +45254,31 @@
       </c>
       <c r="B16" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C16" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '7', </v>
       </c>
       <c r="D16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Resource Action Methods', </v>
       </c>
       <c r="E16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Handler details of an action', </v>
       </c>
       <c r="F16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Method', </v>
       </c>
       <c r="G16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasOne', </v>
       </c>
       <c r="H16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '8', </v>
       </c>
       <c r="I16" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -45160,7 +45318,7 @@
       </c>
       <c r="R16" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="17" spans="1:18">
@@ -45169,31 +45327,31 @@
       </c>
       <c r="B17" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C17" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '7', </v>
       </c>
       <c r="D17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Resource Action Lists', </v>
       </c>
       <c r="E17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Lists where action available', </v>
       </c>
       <c r="F17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Lists', </v>
       </c>
       <c r="G17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '9', </v>
       </c>
       <c r="I17" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -45233,7 +45391,7 @@
       </c>
       <c r="R17" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="18" spans="1:18">
@@ -45242,31 +45400,31 @@
       </c>
       <c r="B18" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C18" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '7', </v>
       </c>
       <c r="D18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Resource Action Data', </v>
       </c>
       <c r="E18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Resource data where action available', </v>
       </c>
       <c r="F18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Data', </v>
       </c>
       <c r="G18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '10', </v>
       </c>
       <c r="I18" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -45306,7 +45464,7 @@
       </c>
       <c r="R18" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="19" spans="1:18">
@@ -45315,31 +45473,31 @@
       </c>
       <c r="B19" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C19" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '5', </v>
       </c>
       <c r="D19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Organisation Contacts', </v>
       </c>
       <c r="E19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Contact details of organisation', </v>
       </c>
       <c r="F19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Contacts', </v>
       </c>
       <c r="G19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '6', </v>
       </c>
       <c r="I19" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -45379,7 +45537,7 @@
       </c>
       <c r="R19" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="20" spans="1:18">
@@ -45388,31 +45546,31 @@
       </c>
       <c r="B20" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C20" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '11', </v>
       </c>
       <c r="D20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Resource Details', </v>
       </c>
       <c r="E20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Resource details', </v>
       </c>
       <c r="F20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Resource', </v>
       </c>
       <c r="G20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
       </c>
       <c r="I20" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -45452,7 +45610,7 @@
       </c>
       <c r="R20" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="21" spans="1:18">
@@ -45461,31 +45619,31 @@
       </c>
       <c r="B21" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C21" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '4', </v>
       </c>
       <c r="D21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Resource Forms', </v>
       </c>
       <c r="E21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Forms available for a resource', </v>
       </c>
       <c r="F21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Forms', </v>
       </c>
       <c r="G21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '12', </v>
       </c>
       <c r="I21" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -45525,7 +45683,7 @@
       </c>
       <c r="R21" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="22" spans="1:18">
@@ -45534,31 +45692,31 @@
       </c>
       <c r="B22" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C22" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '12', </v>
       </c>
       <c r="D22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Form Fields', </v>
       </c>
       <c r="E22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Fields associated with a form', </v>
       </c>
       <c r="F22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Fields', </v>
       </c>
       <c r="G22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '13', </v>
       </c>
       <c r="I22" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -45598,7 +45756,7 @@
       </c>
       <c r="R22" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="23" spans="1:18">
@@ -45607,31 +45765,31 @@
       </c>
       <c r="B23" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C23" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '13', </v>
       </c>
       <c r="D23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Field Attributes', </v>
       </c>
       <c r="E23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Attributes of Field', </v>
       </c>
       <c r="F23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Attributes', </v>
       </c>
       <c r="G23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '14', </v>
       </c>
       <c r="I23" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -45671,7 +45829,7 @@
       </c>
       <c r="R23" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="24" spans="1:18">
@@ -45680,31 +45838,31 @@
       </c>
       <c r="B24" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C24" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '13', </v>
       </c>
       <c r="D24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Field Options', </v>
       </c>
       <c r="E24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Options of Field', </v>
       </c>
       <c r="F24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Options', </v>
       </c>
       <c r="G24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasOne', </v>
       </c>
       <c r="H24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '15', </v>
       </c>
       <c r="I24" s="33" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -45744,7 +45902,7 @@
       </c>
       <c r="R24" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="25" spans="1:18">
@@ -45753,31 +45911,31 @@
       </c>
       <c r="B25" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '13', </v>
       </c>
       <c r="D25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Field Validations', </v>
       </c>
       <c r="E25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Validation details of field', </v>
       </c>
       <c r="F25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Validations', </v>
       </c>
       <c r="G25" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H25" s="33" t="str">
         <f t="shared" ref="H25:K88" ca="1" si="4">IF(AND($B25=$S$4,H$5&lt;&gt;""),IF(VLOOKUP($A$1&amp;"-"&amp;$A25,INDIRECT($E$2),H$4+$B$4,0)="","","'"&amp;H$5&amp;"' =&gt; '"&amp;VLOOKUP($A$1&amp;"-"&amp;$A25,INDIRECT($E$2),H$4+$B$4,0)&amp;"', "),"")</f>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '16', </v>
       </c>
       <c r="I25" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -45817,7 +45975,7 @@
       </c>
       <c r="R25" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="26" spans="1:18">
@@ -45826,31 +45984,31 @@
       </c>
       <c r="B26" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '12', </v>
       </c>
       <c r="D26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'From Resource', </v>
       </c>
       <c r="E26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Resource this form belongs to', </v>
       </c>
       <c r="F26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Resource', </v>
       </c>
       <c r="G26" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H26" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
       </c>
       <c r="I26" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -45890,7 +46048,7 @@
       </c>
       <c r="R26" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="27" spans="1:18">
@@ -45899,31 +46057,31 @@
       </c>
       <c r="B27" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '12', </v>
       </c>
       <c r="D27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Form Defaults', </v>
       </c>
       <c r="E27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Predefined values for a form', </v>
       </c>
       <c r="F27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Defaults', </v>
       </c>
       <c r="G27" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H27" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '17', </v>
       </c>
       <c r="I27" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -45963,7 +46121,7 @@
       </c>
       <c r="R27" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="28" spans="1:18">
@@ -45972,31 +46130,31 @@
       </c>
       <c r="B28" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '13', </v>
       </c>
       <c r="D28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Field Data', </v>
       </c>
       <c r="E28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Fields Database binding details', </v>
       </c>
       <c r="F28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Data', </v>
       </c>
       <c r="G28" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasOne', </v>
       </c>
       <c r="H28" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '18', </v>
       </c>
       <c r="I28" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -46036,7 +46194,7 @@
       </c>
       <c r="R28" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="29" spans="1:18">
@@ -46045,31 +46203,31 @@
       </c>
       <c r="B29" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '4', </v>
       </c>
       <c r="D29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Resource Relations', </v>
       </c>
       <c r="E29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Relation of  a resource to another resource', </v>
       </c>
       <c r="F29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Relations', </v>
       </c>
       <c r="G29" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H29" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
       </c>
       <c r="I29" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -46109,7 +46267,7 @@
       </c>
       <c r="R29" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="30" spans="1:18">
@@ -46118,31 +46276,31 @@
       </c>
       <c r="B30" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '18', </v>
       </c>
       <c r="D30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Bind Data Relation', </v>
       </c>
       <c r="E30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Relation to which the data to be bind', </v>
       </c>
       <c r="F30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
       </c>
       <c r="G30" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H30" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
       </c>
       <c r="I30" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -46182,7 +46340,7 @@
       </c>
       <c r="R30" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="31" spans="1:18">
@@ -46191,31 +46349,31 @@
       </c>
       <c r="B31" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '17', </v>
       </c>
       <c r="D31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Default Data Resource', </v>
       </c>
       <c r="E31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Resource to which the forms predefined data to be bind', </v>
       </c>
       <c r="F31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
       </c>
       <c r="G31" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H31" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
       </c>
       <c r="I31" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -46255,7 +46413,7 @@
       </c>
       <c r="R31" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="32" spans="1:18">
@@ -46264,31 +46422,31 @@
       </c>
       <c r="B32" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '19', </v>
       </c>
       <c r="D32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Resource Details', </v>
       </c>
       <c r="E32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Resource details of a list', </v>
       </c>
       <c r="F32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Resource', </v>
       </c>
       <c r="G32" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H32" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
       </c>
       <c r="I32" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -46328,7 +46486,7 @@
       </c>
       <c r="R32" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="33" spans="1:18">
@@ -46337,31 +46495,31 @@
       </c>
       <c r="B33" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '19', </v>
       </c>
       <c r="D33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'List Relations', </v>
       </c>
       <c r="E33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Relations to be loaded on accessing list', </v>
       </c>
       <c r="F33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Relations', </v>
       </c>
       <c r="G33" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H33" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '20', </v>
       </c>
       <c r="I33" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -46401,7 +46559,7 @@
       </c>
       <c r="R33" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="34" spans="1:18">
@@ -46410,31 +46568,31 @@
       </c>
       <c r="B34" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '4', </v>
       </c>
       <c r="D34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Resource Scopes', </v>
       </c>
       <c r="E34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Scopes available on a Resource', </v>
       </c>
       <c r="F34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Scopes', </v>
       </c>
       <c r="G34" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H34" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '21', </v>
       </c>
       <c r="I34" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -46474,7 +46632,7 @@
       </c>
       <c r="R34" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="35" spans="1:18">
@@ -46483,31 +46641,31 @@
       </c>
       <c r="B35" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '19', </v>
       </c>
       <c r="D35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'List Scopes', </v>
       </c>
       <c r="E35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Scopes by which a list to be filtered', </v>
       </c>
       <c r="F35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Scopes', </v>
       </c>
       <c r="G35" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsToMany', </v>
       </c>
       <c r="H35" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '21', </v>
       </c>
       <c r="I35" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -46547,7 +46705,7 @@
       </c>
       <c r="R35" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="36" spans="1:18">
@@ -46556,31 +46714,31 @@
       </c>
       <c r="B36" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '23', </v>
       </c>
       <c r="D36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Data Relation', </v>
       </c>
       <c r="E36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Relations to be loaded on a data view', </v>
       </c>
       <c r="F36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Relations', </v>
       </c>
       <c r="G36" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H36" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '24', </v>
       </c>
       <c r="I36" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -46620,7 +46778,7 @@
       </c>
       <c r="R36" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="37" spans="1:18">
@@ -46629,31 +46787,31 @@
       </c>
       <c r="B37" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '23', </v>
       </c>
       <c r="D37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Resource Details', </v>
       </c>
       <c r="E37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Details of resource of a record', </v>
       </c>
       <c r="F37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Resource', </v>
       </c>
       <c r="G37" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H37" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
       </c>
       <c r="I37" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -46693,7 +46851,7 @@
       </c>
       <c r="R37" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="38" spans="1:18">
@@ -46702,31 +46860,31 @@
       </c>
       <c r="B38" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '19', </v>
       </c>
       <c r="D38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'List Layout', </v>
       </c>
       <c r="E38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Layout of a list', </v>
       </c>
       <c r="F38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Layout', </v>
       </c>
       <c r="G38" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H38" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '25', </v>
       </c>
       <c r="I38" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -46766,7 +46924,7 @@
       </c>
       <c r="R38" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="39" spans="1:18">
@@ -46775,31 +46933,31 @@
       </c>
       <c r="B39" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C39" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '26', </v>
       </c>
       <c r="D39" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Nested Relation', </v>
       </c>
       <c r="E39" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Nested Relation', </v>
       </c>
       <c r="F39" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Nest', </v>
       </c>
       <c r="G39" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H39" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
       </c>
       <c r="I39" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -46839,7 +46997,7 @@
       </c>
       <c r="R39" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="40" spans="1:18">
@@ -46848,31 +47006,31 @@
       </c>
       <c r="B40" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C40" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '26', </v>
       </c>
       <c r="D40" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Related Resource', </v>
       </c>
       <c r="E40" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Related Resource Details', </v>
       </c>
       <c r="F40" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
       </c>
       <c r="G40" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H40" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
       </c>
       <c r="I40" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -46912,7 +47070,7 @@
       </c>
       <c r="R40" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="41" spans="1:18">
@@ -46921,31 +47079,31 @@
       </c>
       <c r="B41" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C41" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '26', </v>
       </c>
       <c r="D41" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Form Layout', </v>
       </c>
       <c r="E41" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Layout details', </v>
       </c>
       <c r="F41" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Layout', </v>
       </c>
       <c r="G41" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H41" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '27', </v>
       </c>
       <c r="I41" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -46985,7 +47143,7 @@
       </c>
       <c r="R41" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="42" spans="1:18">
@@ -46994,31 +47152,31 @@
       </c>
       <c r="B42" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C42" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '23', </v>
       </c>
       <c r="D42" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Data View Section', </v>
       </c>
       <c r="E42" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Section details of data view', </v>
       </c>
       <c r="F42" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Sections', </v>
       </c>
       <c r="G42" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H42" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '28', </v>
       </c>
       <c r="I42" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -47058,7 +47216,7 @@
       </c>
       <c r="R42" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="43" spans="1:18">
@@ -47067,31 +47225,31 @@
       </c>
       <c r="B43" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C43" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '26', </v>
       </c>
       <c r="D43" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Data View Section Items', </v>
       </c>
       <c r="E43" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Items of a data view section', </v>
       </c>
       <c r="F43" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Items', </v>
       </c>
       <c r="G43" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H43" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '29', </v>
       </c>
       <c r="I43" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -47131,7 +47289,7 @@
       </c>
       <c r="R43" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="44" spans="1:18">
@@ -47140,31 +47298,31 @@
       </c>
       <c r="B44" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C44" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '28', </v>
       </c>
       <c r="D44" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Data Relation', </v>
       </c>
       <c r="E44" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'View relation of a data', </v>
       </c>
       <c r="F44" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
       </c>
       <c r="G44" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H44" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
       </c>
       <c r="I44" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -47204,7 +47362,7 @@
       </c>
       <c r="R44" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="45" spans="1:18">
@@ -47213,31 +47371,31 @@
       </c>
       <c r="B45" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C45" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '29', </v>
       </c>
       <c r="D45" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Data item relation', </v>
       </c>
       <c r="E45" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'View relation of a data item', </v>
       </c>
       <c r="F45" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
       </c>
       <c r="G45" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H45" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
       </c>
       <c r="I45" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -47277,7 +47435,7 @@
       </c>
       <c r="R45" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="46" spans="1:18">
@@ -47286,31 +47444,31 @@
       </c>
       <c r="B46" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C46" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '26', </v>
       </c>
       <c r="D46" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Owner Relation', </v>
       </c>
       <c r="E46" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'View the owner resource', </v>
       </c>
       <c r="F46" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Owner', </v>
       </c>
       <c r="G46" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H46" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
       </c>
       <c r="I46" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -47350,7 +47508,7 @@
       </c>
       <c r="R46" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="47" spans="1:18">
@@ -47359,31 +47517,31 @@
       </c>
       <c r="B47" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C47" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '12', </v>
       </c>
       <c r="D47" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Collections', </v>
       </c>
       <c r="E47" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Collection/Detail form', </v>
       </c>
       <c r="F47" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Collections', </v>
       </c>
       <c r="G47" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H47" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '30', </v>
       </c>
       <c r="I47" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -47423,7 +47581,7 @@
       </c>
       <c r="R47" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="48" spans="1:18">
@@ -47432,31 +47590,31 @@
       </c>
       <c r="B48" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C48" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '30', </v>
       </c>
       <c r="D48" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Collection Form', </v>
       </c>
       <c r="E48" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Collection Form', </v>
       </c>
       <c r="F48" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Form', </v>
       </c>
       <c r="G48" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H48" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '12', </v>
       </c>
       <c r="I48" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -47496,7 +47654,7 @@
       </c>
       <c r="R48" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="49" spans="1:18">
@@ -47505,31 +47663,31 @@
       </c>
       <c r="B49" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C49" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '30', </v>
       </c>
       <c r="D49" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Relation', </v>
       </c>
       <c r="E49" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Details of Relation', </v>
       </c>
       <c r="F49" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Relation', </v>
       </c>
       <c r="G49" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H49" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '26', </v>
       </c>
       <c r="I49" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -47569,7 +47727,7 @@
       </c>
       <c r="R49" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="50" spans="1:18">
@@ -47578,31 +47736,31 @@
       </c>
       <c r="B50" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C50" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '15', </v>
       </c>
       <c r="D50" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Field', </v>
       </c>
       <c r="E50" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Field details', </v>
       </c>
       <c r="F50" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Field', </v>
       </c>
       <c r="G50" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H50" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '13', </v>
       </c>
       <c r="I50" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -47642,7 +47800,7 @@
       </c>
       <c r="R50" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="51" spans="1:18">
@@ -47651,31 +47809,31 @@
       </c>
       <c r="B51" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C51" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '13', </v>
       </c>
       <c r="D51" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Form', </v>
       </c>
       <c r="E51" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Form details', </v>
       </c>
       <c r="F51" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Form', </v>
       </c>
       <c r="G51" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H51" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '12', </v>
       </c>
       <c r="I51" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -47715,7 +47873,7 @@
       </c>
       <c r="R51" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="52" spans="1:18">
@@ -47724,31 +47882,31 @@
       </c>
       <c r="B52" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C52" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '19', </v>
       </c>
       <c r="D52" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'List Search', </v>
       </c>
       <c r="E52" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Search fields for a list', </v>
       </c>
       <c r="F52" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Search', </v>
       </c>
       <c r="G52" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H52" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '31', </v>
       </c>
       <c r="I52" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -47788,7 +47946,7 @@
       </c>
       <c r="R52" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="53" spans="1:18">
@@ -47797,31 +47955,31 @@
       </c>
       <c r="B53" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C53" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '13', </v>
       </c>
       <c r="D53" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Depending Fields', </v>
       </c>
       <c r="E53" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Dependent fields', </v>
       </c>
       <c r="F53" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Depends', </v>
       </c>
       <c r="G53" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H53" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '32', </v>
       </c>
       <c r="I53" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -47861,7 +48019,7 @@
       </c>
       <c r="R53" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="54" spans="1:18">
@@ -47870,31 +48028,31 @@
       </c>
       <c r="B54" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C54" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '4', </v>
       </c>
       <c r="D54" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Resource Dashboards', </v>
       </c>
       <c r="E54" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Dashboards of a Resource', </v>
       </c>
       <c r="F54" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Dashboards', </v>
       </c>
       <c r="G54" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H54" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '33', </v>
       </c>
       <c r="I54" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -47934,7 +48092,7 @@
       </c>
       <c r="R54" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="55" spans="1:18">
@@ -47943,31 +48101,31 @@
       </c>
       <c r="B55" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C55" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '33', </v>
       </c>
       <c r="D55" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Dashboard Sections', </v>
       </c>
       <c r="E55" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Sections of a dashboard', </v>
       </c>
       <c r="F55" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Sections', </v>
       </c>
       <c r="G55" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H55" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '34', </v>
       </c>
       <c r="I55" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -48007,7 +48165,7 @@
       </c>
       <c r="R55" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="56" spans="1:18">
@@ -48016,31 +48174,31 @@
       </c>
       <c r="B56" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C56" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '34', </v>
       </c>
       <c r="D56" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Dashboard Section Items', </v>
       </c>
       <c r="E56" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Items of a dashboard section', </v>
       </c>
       <c r="F56" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Items', </v>
       </c>
       <c r="G56" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'hasMany', </v>
       </c>
       <c r="H56" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '35', </v>
       </c>
       <c r="I56" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -48080,7 +48238,7 @@
       </c>
       <c r="R56" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="57" spans="1:18">
@@ -48089,31 +48247,31 @@
       </c>
       <c r="B57" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C57" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '33', </v>
       </c>
       <c r="D57" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Dashboard Resource', </v>
       </c>
       <c r="E57" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Resource details of a dashboard', </v>
       </c>
       <c r="F57" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Resource', </v>
       </c>
       <c r="G57" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H57" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '4', </v>
       </c>
       <c r="I57" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -48153,7 +48311,7 @@
       </c>
       <c r="R57" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="58" spans="1:18">
@@ -48162,31 +48320,31 @@
       </c>
       <c r="B58" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>-&gt;create([</v>
       </c>
       <c r="C58" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'resource' =&gt; '13', </v>
       </c>
       <c r="D58" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'name' =&gt; 'Field Dynamics', </v>
       </c>
       <c r="E58" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'description' =&gt; 'Dynamic field details', </v>
       </c>
       <c r="F58" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'method' =&gt; 'Dynamics', </v>
       </c>
       <c r="G58" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v xml:space="preserve">'type' =&gt; 'belongsTo', </v>
       </c>
       <c r="H58" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">'relate_resource' =&gt; '37', </v>
       </c>
       <c r="I58" s="33" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -48226,7 +48384,7 @@
       </c>
       <c r="R58" s="33" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>])</v>
       </c>
     </row>
     <row r="59" spans="1:18">
@@ -48235,7 +48393,7 @@
       </c>
       <c r="B59" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>;</v>
       </c>
       <c r="C59" s="33" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -48308,7 +48466,7 @@
       </c>
       <c r="B60" s="30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>\DB::statement('set foreign_key_checks = ' . $_);</v>
       </c>
       <c r="C60" s="33" t="str">
         <f t="shared" ca="1" si="3"/>

</xml_diff>

<commit_message>
field dynamic table modified
</commit_message>
<xml_diff>
--- a/Helper.xlsx
+++ b/Helper.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" tabRatio="912" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Framework Tables" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3801" uniqueCount="800">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3801" uniqueCount="801">
   <si>
     <t>resource_scopes</t>
   </si>
@@ -2438,6 +2438,9 @@
   </si>
   <si>
     <t>Field Dynamics</t>
+  </si>
+  <si>
+    <t>values</t>
   </si>
 </sst>
 </file>
@@ -2673,209 +2676,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="129">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="124">
     <dxf>
       <font>
         <strike val="0"/>
@@ -4263,6 +4064,148 @@
     </dxf>
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <condense val="0"/>
         <extend val="0"/>
         <color rgb="FF9C0006"/>
@@ -4519,35 +4462,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tables" displayName="Tables" ref="A1:J43" totalsRowShown="0" dataDxfId="128">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tables" displayName="Tables" ref="A1:J43" totalsRowShown="0" dataDxfId="123">
   <autoFilter ref="A1:J43"/>
   <tableColumns count="10">
-    <tableColumn id="2" name="Name" dataDxfId="127"/>
-    <tableColumn id="10" name="Table" dataDxfId="126">
+    <tableColumn id="2" name="Name" dataDxfId="122"/>
+    <tableColumn id="10" name="Table" dataDxfId="121">
       <calculatedColumnFormula>"__"&amp;[Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Singular Name" dataDxfId="125">
+    <tableColumn id="5" name="Singular Name" dataDxfId="120">
       <calculatedColumnFormula>IF(RIGHT([Name],3)="ies",MID([Name],1,LEN([Name])-3)&amp;"y",IF(RIGHT([Name],1)="s",MID([Name],1,LEN([Name])-1),[Name]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Model NS" dataDxfId="124">
+    <tableColumn id="8" name="Model NS" dataDxfId="119">
       <calculatedColumnFormula>"Milestone\Appframe\Model"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Class Name" dataDxfId="123">
+    <tableColumn id="4" name="Class Name" dataDxfId="118">
       <calculatedColumnFormula>SUBSTITUTE(PROPER([Singular Name]),"_","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Migration Artisan" dataDxfId="122">
+    <tableColumn id="1" name="Migration Artisan" dataDxfId="117">
       <calculatedColumnFormula>"php artisan make:migration create_"&amp;[Table]&amp;"_table --create=__"&amp;[Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Model Artisan" dataDxfId="121">
+    <tableColumn id="6" name="Model Artisan" dataDxfId="116">
       <calculatedColumnFormula>"php artisan make:model "&amp;[Class Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Model Statement" dataDxfId="120">
+    <tableColumn id="3" name="Model Statement" dataDxfId="115">
       <calculatedColumnFormula>"protected $table = '"&amp;[Table]&amp;"';"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Seeder Artisan" dataDxfId="119">
+    <tableColumn id="7" name="Seeder Artisan" dataDxfId="114">
       <calculatedColumnFormula>"php artisan make:seed "&amp;[Class Name]&amp;"TableSeeder"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Seeder Class" dataDxfId="118">
+    <tableColumn id="9" name="Seeder Class" dataDxfId="113">
       <calculatedColumnFormula>[Class Name]&amp;"TableSeeder"&amp;"::class,"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4556,56 +4499,56 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="ResourceActions" displayName="ResourceActions" ref="A1:P9" totalsRowShown="0" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="ResourceActions" displayName="ResourceActions" ref="A1:P9" totalsRowShown="0" dataDxfId="16">
   <autoFilter ref="A1:P9"/>
   <tableColumns count="16">
-    <tableColumn id="1" name="No" dataDxfId="31">
+    <tableColumn id="1" name="No" dataDxfId="15">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Resource" dataDxfId="30"/>
-    <tableColumn id="13" name="Resource Id" dataDxfId="29">
+    <tableColumn id="2" name="Resource" dataDxfId="14"/>
+    <tableColumn id="13" name="Resource Id" dataDxfId="13">
       <calculatedColumnFormula>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Action Name" dataDxfId="28"/>
-    <tableColumn id="4" name="Description" dataDxfId="27"/>
-    <tableColumn id="5" name="Action Title" dataDxfId="26"/>
-    <tableColumn id="6" name="Button Type" dataDxfId="25"/>
-    <tableColumn id="7" name="Menu" dataDxfId="24"/>
-    <tableColumn id="8" name="Icon" dataDxfId="23"/>
-    <tableColumn id="9" name="Set" dataDxfId="22"/>
-    <tableColumn id="14" name="Action Type" dataDxfId="21"/>
-    <tableColumn id="15" name="ID1" dataDxfId="20"/>
-    <tableColumn id="16" name="ID2" dataDxfId="19"/>
-    <tableColumn id="10" name="On" dataDxfId="18"/>
-    <tableColumn id="11" name="Confirm" dataDxfId="17"/>
-    <tableColumn id="12" name="handler" dataDxfId="16"/>
+    <tableColumn id="3" name="Action Name" dataDxfId="12"/>
+    <tableColumn id="4" name="Description" dataDxfId="11"/>
+    <tableColumn id="5" name="Action Title" dataDxfId="10"/>
+    <tableColumn id="6" name="Button Type" dataDxfId="9"/>
+    <tableColumn id="7" name="Menu" dataDxfId="8"/>
+    <tableColumn id="8" name="Icon" dataDxfId="7"/>
+    <tableColumn id="9" name="Set" dataDxfId="6"/>
+    <tableColumn id="14" name="Action Type" dataDxfId="5"/>
+    <tableColumn id="15" name="ID1" dataDxfId="4"/>
+    <tableColumn id="16" name="ID2" dataDxfId="3"/>
+    <tableColumn id="10" name="On" dataDxfId="2"/>
+    <tableColumn id="11" name="Confirm" dataDxfId="1"/>
+    <tableColumn id="12" name="handler" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Columns" displayName="Columns" ref="A1:I166" totalsRowShown="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Columns" displayName="Columns" ref="A1:I166" totalsRowShown="0" dataDxfId="105">
   <autoFilter ref="A1:I166">
     <filterColumn colId="0"/>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" name="Column" dataDxfId="10"/>
-    <tableColumn id="2" name="Type" dataDxfId="9"/>
-    <tableColumn id="3" name="Name" dataDxfId="8"/>
-    <tableColumn id="4" name="Length/Enum" dataDxfId="7"/>
-    <tableColumn id="5" name="Method1" dataDxfId="6"/>
-    <tableColumn id="6" name="Method2" dataDxfId="5"/>
-    <tableColumn id="7" name="Method3" dataDxfId="4"/>
-    <tableColumn id="8" name="Method4" dataDxfId="3"/>
-    <tableColumn id="9" name="Method5" dataDxfId="2"/>
+    <tableColumn id="1" name="Column" dataDxfId="104"/>
+    <tableColumn id="2" name="Type" dataDxfId="103"/>
+    <tableColumn id="3" name="Name" dataDxfId="102"/>
+    <tableColumn id="4" name="Length/Enum" dataDxfId="101"/>
+    <tableColumn id="5" name="Method1" dataDxfId="100"/>
+    <tableColumn id="6" name="Method2" dataDxfId="99"/>
+    <tableColumn id="7" name="Method3" dataDxfId="98"/>
+    <tableColumn id="8" name="Method4" dataDxfId="97"/>
+    <tableColumn id="9" name="Method5" dataDxfId="96"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TableFields" displayName="TableFields" ref="A1:K384" totalsRowShown="0" dataDxfId="111">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TableFields" displayName="TableFields" ref="A1:K384" totalsRowShown="0" dataDxfId="95">
   <autoFilter ref="A1:K384">
     <filterColumn colId="0">
       <filters>
@@ -4615,33 +4558,33 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="11">
-    <tableColumn id="2" name="Table" dataDxfId="110"/>
-    <tableColumn id="3" name="Field" dataDxfId="109"/>
-    <tableColumn id="5" name="Type" dataDxfId="108">
+    <tableColumn id="2" name="Table" dataDxfId="94"/>
+    <tableColumn id="3" name="Field" dataDxfId="93"/>
+    <tableColumn id="5" name="Type" dataDxfId="92">
       <calculatedColumnFormula>VLOOKUP([Field],Columns[],2,0)&amp;"("</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Name" dataDxfId="107">
+    <tableColumn id="4" name="Name" dataDxfId="91">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Arg2" dataDxfId="106">
+    <tableColumn id="6" name="Arg2" dataDxfId="90">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Method1" dataDxfId="105">
+    <tableColumn id="7" name="Method1" dataDxfId="89">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Method2" dataDxfId="104">
+    <tableColumn id="8" name="Method2" dataDxfId="88">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],6,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],6,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Method3" dataDxfId="103">
+    <tableColumn id="9" name="Method3" dataDxfId="87">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],7,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],7,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Method4" dataDxfId="102">
+    <tableColumn id="10" name="Method4" dataDxfId="86">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],8,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],8,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Method5" dataDxfId="101">
+    <tableColumn id="11" name="Method5" dataDxfId="85">
       <calculatedColumnFormula>IF(VLOOKUP([Field],Columns[],9,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],9,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Statement" dataDxfId="100">
+    <tableColumn id="12" name="Statement" dataDxfId="84">
       <calculatedColumnFormula>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4650,51 +4593,51 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R325" totalsRowShown="0" headerRowDxfId="99" dataDxfId="98">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="TableData" displayName="TableData" ref="A1:R325" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
   <autoFilter ref="A1:R325">
     <filterColumn colId="1"/>
   </autoFilter>
   <tableColumns count="18">
-    <tableColumn id="19" name="TRCode" dataDxfId="97">
+    <tableColumn id="19" name="TRCode" dataDxfId="81">
       <calculatedColumnFormula>[Table Name]&amp;"-"&amp;[Record No]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Table Name" dataDxfId="96"/>
-    <tableColumn id="2" name="Record No" dataDxfId="95">
+    <tableColumn id="1" name="Table Name" dataDxfId="80"/>
+    <tableColumn id="2" name="Record No" dataDxfId="79">
       <calculatedColumnFormula>COUNTIF($B$1:$B1,[Table Name])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="1" dataDxfId="94"/>
-    <tableColumn id="4" name="2" dataDxfId="93"/>
-    <tableColumn id="5" name="3" dataDxfId="92"/>
-    <tableColumn id="6" name="4" dataDxfId="91"/>
-    <tableColumn id="7" name="5" dataDxfId="90"/>
-    <tableColumn id="8" name="6" dataDxfId="89"/>
-    <tableColumn id="9" name="7" dataDxfId="88"/>
-    <tableColumn id="10" name="8" dataDxfId="87"/>
-    <tableColumn id="11" name="9" dataDxfId="86"/>
-    <tableColumn id="12" name="10" dataDxfId="85"/>
-    <tableColumn id="13" name="11" dataDxfId="84"/>
-    <tableColumn id="14" name="12" dataDxfId="83"/>
-    <tableColumn id="15" name="13" dataDxfId="82"/>
-    <tableColumn id="16" name="14" dataDxfId="81"/>
-    <tableColumn id="17" name="15" dataDxfId="80"/>
+    <tableColumn id="3" name="1" dataDxfId="78"/>
+    <tableColumn id="4" name="2" dataDxfId="77"/>
+    <tableColumn id="5" name="3" dataDxfId="76"/>
+    <tableColumn id="6" name="4" dataDxfId="75"/>
+    <tableColumn id="7" name="5" dataDxfId="74"/>
+    <tableColumn id="8" name="6" dataDxfId="73"/>
+    <tableColumn id="9" name="7" dataDxfId="72"/>
+    <tableColumn id="10" name="8" dataDxfId="71"/>
+    <tableColumn id="11" name="9" dataDxfId="70"/>
+    <tableColumn id="12" name="10" dataDxfId="69"/>
+    <tableColumn id="13" name="11" dataDxfId="68"/>
+    <tableColumn id="14" name="12" dataDxfId="67"/>
+    <tableColumn id="15" name="13" dataDxfId="66"/>
+    <tableColumn id="16" name="14" dataDxfId="65"/>
+    <tableColumn id="17" name="15" dataDxfId="64"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SeedMap" displayName="SeedMap" ref="A1:E37" totalsRowShown="0" dataDxfId="79">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SeedMap" displayName="SeedMap" ref="A1:E37" totalsRowShown="0" dataDxfId="63">
   <autoFilter ref="A1:E37"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Name" dataDxfId="78"/>
-    <tableColumn id="3" name="FW Table Name" dataDxfId="77"/>
-    <tableColumn id="20" name="NS" dataDxfId="76">
+    <tableColumn id="1" name="Name" dataDxfId="62"/>
+    <tableColumn id="3" name="FW Table Name" dataDxfId="61"/>
+    <tableColumn id="20" name="NS" dataDxfId="60">
       <calculatedColumnFormula>VLOOKUP([FW Table Name],Tables[],4,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="Model" dataDxfId="75">
+    <tableColumn id="21" name="Model" dataDxfId="59">
       <calculatedColumnFormula>VLOOKUP([FW Table Name],Tables[],5,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Query Method" dataDxfId="74">
+    <tableColumn id="4" name="Query Method" dataDxfId="58">
       <calculatedColumnFormula>"truncate"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4703,46 +4646,46 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="ResourceTable" displayName="ResourceTable" ref="A1:I38" totalsRowShown="0" dataDxfId="73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="ResourceTable" displayName="ResourceTable" ref="A1:I38" totalsRowShown="0" dataDxfId="57">
   <autoFilter ref="A1:I38"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="No" dataDxfId="72">
+    <tableColumn id="1" name="No" dataDxfId="56">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Name" dataDxfId="71"/>
-    <tableColumn id="3" name="Description" dataDxfId="70"/>
-    <tableColumn id="4" name="Title" dataDxfId="69"/>
-    <tableColumn id="5" name="NS" dataDxfId="68">
+    <tableColumn id="2" name="Name" dataDxfId="55"/>
+    <tableColumn id="3" name="Description" dataDxfId="54"/>
+    <tableColumn id="4" name="Title" dataDxfId="53"/>
+    <tableColumn id="5" name="NS" dataDxfId="52">
       <calculatedColumnFormula>"Milestone\Appframe\Model"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Table" dataDxfId="67"/>
-    <tableColumn id="7" name="Key" dataDxfId="66">
+    <tableColumn id="6" name="Table" dataDxfId="51"/>
+    <tableColumn id="7" name="Key" dataDxfId="50">
       <calculatedColumnFormula>"id"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Controller" dataDxfId="65"/>
-    <tableColumn id="9" name="Controller NS" dataDxfId="64"/>
+    <tableColumn id="8" name="Controller" dataDxfId="49"/>
+    <tableColumn id="9" name="Controller NS" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RelationTable" displayName="RelationTable" ref="A1:I51" totalsRowShown="0" dataDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RelationTable" displayName="RelationTable" ref="A1:I51" totalsRowShown="0" dataDxfId="47">
   <autoFilter ref="A1:I51"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="No" dataDxfId="62">
+    <tableColumn id="1" name="No" dataDxfId="46">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Resource" dataDxfId="61"/>
-    <tableColumn id="4" name="Relate Resource" dataDxfId="60"/>
-    <tableColumn id="2" name="Resource Id" dataDxfId="59">
+    <tableColumn id="3" name="Resource" dataDxfId="45"/>
+    <tableColumn id="4" name="Relate Resource" dataDxfId="44"/>
+    <tableColumn id="2" name="Resource Id" dataDxfId="43">
       <calculatedColumnFormula>VLOOKUP([Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Name" dataDxfId="58"/>
-    <tableColumn id="6" name="Description" dataDxfId="57"/>
-    <tableColumn id="7" name="Method" dataDxfId="56"/>
-    <tableColumn id="8" name="Type" dataDxfId="55"/>
-    <tableColumn id="10" name="Relate Id" dataDxfId="54">
+    <tableColumn id="5" name="Name" dataDxfId="42"/>
+    <tableColumn id="6" name="Description" dataDxfId="41"/>
+    <tableColumn id="7" name="Method" dataDxfId="40"/>
+    <tableColumn id="8" name="Type" dataDxfId="39"/>
+    <tableColumn id="10" name="Relate Id" dataDxfId="38">
       <calculatedColumnFormula>VLOOKUP([Relate Resource],CHOOSE({1,2},ResourceTable[Name],ResourceTable[No]),2,0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4751,47 +4694,47 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="ResourceForms" displayName="ResourceForms" ref="A1:G9" totalsRowShown="0" dataDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="ResourceForms" displayName="ResourceForms" ref="A1:G9" totalsRowShown="0" dataDxfId="37">
   <autoFilter ref="A1:G9"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="No" dataDxfId="52">
+    <tableColumn id="1" name="No" dataDxfId="36">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Resource ID" dataDxfId="51"/>
-    <tableColumn id="3" name="Resource Name" dataDxfId="50">
+    <tableColumn id="2" name="Resource ID" dataDxfId="35"/>
+    <tableColumn id="3" name="Resource Name" dataDxfId="34">
       <calculatedColumnFormula>VLOOKUP([Resource ID],ResourceTable[],2,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Form Name" dataDxfId="49"/>
-    <tableColumn id="6" name="Title" dataDxfId="48"/>
-    <tableColumn id="7" name="Action Text" dataDxfId="47"/>
-    <tableColumn id="8" name="Description" dataDxfId="46"/>
+    <tableColumn id="4" name="Form Name" dataDxfId="33"/>
+    <tableColumn id="6" name="Title" dataDxfId="32"/>
+    <tableColumn id="7" name="Action Text" dataDxfId="31"/>
+    <tableColumn id="8" name="Description" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="FormFields" displayName="FormFields" ref="A1:L33" totalsRowShown="0" dataDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="FormFields" displayName="FormFields" ref="A1:L33" totalsRowShown="0" dataDxfId="29">
   <autoFilter ref="A1:L33"/>
   <tableColumns count="12">
-    <tableColumn id="9" name="No" dataDxfId="44">
+    <tableColumn id="9" name="No" dataDxfId="28">
       <calculatedColumnFormula>IFERROR($A1+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Form Id" dataDxfId="43"/>
-    <tableColumn id="7" name="Form Name" dataDxfId="42">
+    <tableColumn id="1" name="Form Id" dataDxfId="27"/>
+    <tableColumn id="7" name="Form Name" dataDxfId="26">
       <calculatedColumnFormula>VLOOKUP([Form Id],ResourceForms[],4,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Name" dataDxfId="41"/>
-    <tableColumn id="2" name="Type" dataDxfId="40"/>
-    <tableColumn id="5" name="Label" dataDxfId="39"/>
-    <tableColumn id="6" name="Collection" dataDxfId="38"/>
-    <tableColumn id="14" name="Attribute" dataDxfId="37">
+    <tableColumn id="4" name="Name" dataDxfId="25"/>
+    <tableColumn id="2" name="Type" dataDxfId="24"/>
+    <tableColumn id="5" name="Label" dataDxfId="23"/>
+    <tableColumn id="6" name="Collection" dataDxfId="22"/>
+    <tableColumn id="14" name="Attribute" dataDxfId="21">
       <calculatedColumnFormula>[Name]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Relation" dataDxfId="36"/>
-    <tableColumn id="11" name="Deep 1" dataDxfId="35"/>
-    <tableColumn id="12" name="Deep 2" dataDxfId="34"/>
-    <tableColumn id="13" name="Deep 3" dataDxfId="33"/>
+    <tableColumn id="10" name="Relation" dataDxfId="20"/>
+    <tableColumn id="11" name="Deep 1" dataDxfId="19"/>
+    <tableColumn id="12" name="Deep 2" dataDxfId="18"/>
+    <tableColumn id="13" name="Deep 3" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5085,7 +5028,7 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView topLeftCell="D28" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8438,7 +8381,7 @@
   <dimension ref="A1:I166"/>
   <sheetViews>
     <sheetView topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="A166" sqref="A166"/>
+      <selection activeCell="D165" sqref="D165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="15"/>
@@ -11993,10 +11936,10 @@
         <v>27</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>788</v>
+        <v>800</v>
       </c>
       <c r="D165" s="4">
-        <v>512</v>
+        <v>1024</v>
       </c>
       <c r="E165" s="4" t="s">
         <v>29</v>
@@ -12029,25 +11972,25 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A43:A46">
-    <cfRule type="duplicateValues" dxfId="117" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="112" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56:A59">
-    <cfRule type="duplicateValues" dxfId="116" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="111" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A166">
-    <cfRule type="duplicateValues" dxfId="11" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="110" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A128:A129">
-    <cfRule type="duplicateValues" dxfId="115" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="109" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A128:A129">
-    <cfRule type="duplicateValues" dxfId="114" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="108" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A130:A131">
-    <cfRule type="duplicateValues" dxfId="113" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="107" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A152:A153">
-    <cfRule type="duplicateValues" dxfId="112" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="106" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -12061,8 +12004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K384"/>
   <sheetViews>
-    <sheetView topLeftCell="A366" workbookViewId="0">
-      <selection activeCell="K375" sqref="K375"/>
+    <sheetView tabSelected="1" topLeftCell="A366" workbookViewId="0">
+      <selection activeCell="K379" sqref="K379"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="15"/>
@@ -28753,11 +28696,11 @@
       </c>
       <c r="D380" s="5" t="str">
         <f>IF(VLOOKUP([Field],Columns[],3,0)&lt;&gt;"","'"&amp;VLOOKUP([Field],Columns[],3,0)&amp;"'","")</f>
-        <v>'value_array'</v>
+        <v>'values'</v>
       </c>
       <c r="E380" s="8" t="str">
         <f>IF(VLOOKUP([Field],Columns[],4,0)&lt;&gt;0,", "&amp;VLOOKUP([Field],Columns[],4,0)&amp;")",")")</f>
-        <v>, 512)</v>
+        <v>, 1024)</v>
       </c>
       <c r="F380" s="5" t="str">
         <f>IF(VLOOKUP([Field],Columns[],5,0)=0,"","-&gt;"&amp;VLOOKUP([Field],Columns[],5,0))</f>
@@ -28781,7 +28724,7 @@
       </c>
       <c r="K380" s="5" t="str">
         <f>"$table-&gt;"&amp;[Type]&amp;[Name]&amp;[Arg2]&amp;[Method1]&amp;[Method2]&amp;[Method3]&amp;[Method4]&amp;[Method5]&amp;";"</f>
-        <v>$table-&gt;string('value_array', 512)-&gt;nullable();</v>
+        <v>$table-&gt;string('values', 1024)-&gt;nullable();</v>
       </c>
     </row>
     <row r="381" spans="1:11">
@@ -42605,14 +42548,14 @@
         <v>692</v>
       </c>
       <c r="E33" s="7" t="str">
-        <f>"Milestone\Appframe\Model"</f>
+        <f t="shared" ref="E33:E38" si="12">"Milestone\Appframe\Model"</f>
         <v>Milestone\Appframe\Model</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>693</v>
       </c>
       <c r="G33" s="21" t="str">
-        <f>"id"</f>
+        <f t="shared" ref="G33:G38" si="13">"id"</f>
         <v>id</v>
       </c>
       <c r="H33" s="4"/>
@@ -42633,14 +42576,14 @@
         <v>753</v>
       </c>
       <c r="E34" s="8" t="str">
-        <f>"Milestone\Appframe\Model"</f>
+        <f t="shared" si="12"/>
         <v>Milestone\Appframe\Model</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>754</v>
       </c>
       <c r="G34" s="46" t="str">
-        <f>"id"</f>
+        <f t="shared" si="13"/>
         <v>id</v>
       </c>
       <c r="H34" s="5"/>
@@ -42661,14 +42604,14 @@
         <v>758</v>
       </c>
       <c r="E35" s="8" t="str">
-        <f>"Milestone\Appframe\Model"</f>
+        <f t="shared" si="12"/>
         <v>Milestone\Appframe\Model</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>755</v>
       </c>
       <c r="G35" s="46" t="str">
-        <f>"id"</f>
+        <f t="shared" si="13"/>
         <v>id</v>
       </c>
       <c r="H35" s="5"/>
@@ -42689,14 +42632,14 @@
         <v>744</v>
       </c>
       <c r="E36" s="8" t="str">
-        <f>"Milestone\Appframe\Model"</f>
+        <f t="shared" si="12"/>
         <v>Milestone\Appframe\Model</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>756</v>
       </c>
       <c r="G36" s="46" t="str">
-        <f>"id"</f>
+        <f t="shared" si="13"/>
         <v>id</v>
       </c>
       <c r="H36" s="5"/>
@@ -42717,14 +42660,14 @@
         <v>745</v>
       </c>
       <c r="E37" s="7" t="str">
-        <f>"Milestone\Appframe\Model"</f>
+        <f t="shared" si="12"/>
         <v>Milestone\Appframe\Model</v>
       </c>
       <c r="F37" s="4" t="s">
         <v>757</v>
       </c>
       <c r="G37" s="21" t="str">
-        <f>"id"</f>
+        <f t="shared" si="13"/>
         <v>id</v>
       </c>
       <c r="H37" s="4"/>
@@ -42745,14 +42688,14 @@
         <v>796</v>
       </c>
       <c r="E38" s="7" t="str">
-        <f>"Milestone\Appframe\Model"</f>
+        <f t="shared" si="12"/>
         <v>Milestone\Appframe\Model</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>797</v>
       </c>
       <c r="G38" s="21" t="str">
-        <f>"id"</f>
+        <f t="shared" si="13"/>
         <v>id</v>
       </c>
       <c r="H38" s="4"/>
@@ -44442,7 +44385,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+    <sheetView topLeftCell="A42" workbookViewId="0">
       <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>

</xml_diff>